<commit_message>
instruction decoder almost done...?
</commit_message>
<xml_diff>
--- a/doc/RiscyInstSet32Bit.xlsx
+++ b/doc/RiscyInstSet32Bit.xlsx
@@ -27,14 +27,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="200">
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>H</t>
-  </si>
-  <si>
     <t>16 MB</t>
   </si>
   <si>
@@ -314,9 +311,6 @@
     <t>Destination register must contain the argument (stored as Int32)</t>
   </si>
   <si>
-    <t>C: 0-Read, 1-Write</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
@@ -527,9 +521,6 @@
     <t>Load word immediate</t>
   </si>
   <si>
-    <t>H: 0-Low, 1-High</t>
-  </si>
-  <si>
     <t>Halfword</t>
   </si>
   <si>
@@ -605,9 +596,6 @@
     <t>Mode</t>
   </si>
   <si>
-    <t>Rperi: register to peripheral # (Store 0 at Rperi to MEMCPY to main mem); C: 0-Read, 1-Write; Mode: 0-Byte, 1-Halfword, 2-Word</t>
-  </si>
-  <si>
     <t>Rs/Rd: device (see Rperi); Rlen: length</t>
   </si>
   <si>
@@ -626,10 +614,19 @@
     <t>IntOffset (address = 4 * offset) (only for PUSHWORDI, POPWORDI)</t>
   </si>
   <si>
-    <t>C: 0-Read, 1-Write; IntOffset: set to 0 if not used; popped value will go to LR register</t>
-  </si>
-  <si>
     <t>Memory size of the peripheral, returned in Int32; IRQ 0 for the main memory</t>
+  </si>
+  <si>
+    <t>Rperi: register to peripheral # (Store 0 at Rperi to MEMCPY to main mem); C: 0-Load, 1-Store; Mode: 0-Byte, 1-Halfword, 2-Word</t>
+  </si>
+  <si>
+    <t>M: 0-Low, 1-High</t>
+  </si>
+  <si>
+    <t>C: 0-Load, 1-Store</t>
+  </si>
+  <si>
+    <t>C: 0-Push 1-Pop; IntOffset: set to 0 if not used; popped value will go to LR register if IntOffset is non-zero</t>
   </si>
 </sst>
 </file>
@@ -824,7 +821,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="5" applyFont="1"/>
@@ -860,6 +857,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -890,6 +890,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1181,7 +1184,7 @@
   <dimension ref="A1:AK46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="AJ25" sqref="AJ25"/>
+      <selection activeCell="AJ19" sqref="AJ19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1196,7 +1199,7 @@
   <sheetData>
     <row r="1" spans="1:37" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1235,11 +1238,11 @@
     <row r="2" spans="1:37" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -1273,12 +1276,12 @@
       <c r="AG3" s="5"/>
       <c r="AH3" s="5"/>
       <c r="AJ3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="12">
@@ -1316,16 +1319,16 @@
       <c r="AG4" s="5"/>
       <c r="AH4" s="5"/>
       <c r="AJ4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -1359,7 +1362,7 @@
       <c r="AG5" s="5"/>
       <c r="AH5" s="5"/>
       <c r="AJ5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1466,7 +1469,7 @@
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="13">
         <v>0</v>
@@ -1490,17 +1493,17 @@
         <v>0</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K8" s="11"/>
       <c r="L8" s="11"/>
       <c r="M8" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N8" s="11"/>
       <c r="O8" s="11"/>
       <c r="P8" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q8" s="11"/>
       <c r="R8" s="11"/>
@@ -1535,7 +1538,7 @@
         <v>0</v>
       </c>
       <c r="AC8" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AD8" s="11"/>
       <c r="AE8" s="11"/>
@@ -1543,49 +1546,49 @@
       <c r="AG8" s="11"/>
       <c r="AH8" s="11"/>
       <c r="AJ8" s="12" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C9" s="20">
-        <v>0</v>
-      </c>
-      <c r="D9" s="20">
-        <v>0</v>
-      </c>
-      <c r="E9" s="20">
-        <v>0</v>
-      </c>
-      <c r="F9" s="20">
-        <v>0</v>
-      </c>
-      <c r="G9" s="20">
-        <v>0</v>
-      </c>
-      <c r="H9" s="20">
-        <v>0</v>
-      </c>
-      <c r="I9" s="20">
-        <v>0</v>
-      </c>
-      <c r="J9" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="N9" s="21"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="22" t="s">
-        <v>172</v>
-      </c>
-      <c r="Q9" s="22"/>
-      <c r="R9" s="22"/>
+        <v>97</v>
+      </c>
+      <c r="C9" s="21">
+        <v>0</v>
+      </c>
+      <c r="D9" s="21">
+        <v>0</v>
+      </c>
+      <c r="E9" s="21">
+        <v>0</v>
+      </c>
+      <c r="F9" s="21">
+        <v>0</v>
+      </c>
+      <c r="G9" s="21">
+        <v>0</v>
+      </c>
+      <c r="H9" s="21">
+        <v>0</v>
+      </c>
+      <c r="I9" s="21">
+        <v>0</v>
+      </c>
+      <c r="J9" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q9" s="23"/>
+      <c r="R9" s="23"/>
       <c r="S9" s="14">
         <v>0</v>
       </c>
@@ -1616,119 +1619,121 @@
       <c r="AB9" s="6">
         <v>0</v>
       </c>
-      <c r="AC9" s="20">
-        <v>1</v>
-      </c>
-      <c r="AD9" s="20">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="20">
-        <v>0</v>
-      </c>
-      <c r="AF9" s="20">
-        <v>1</v>
-      </c>
-      <c r="AG9" s="20">
-        <v>0</v>
-      </c>
-      <c r="AH9" s="20" t="s">
-        <v>149</v>
+      <c r="AC9" s="21">
+        <v>1</v>
+      </c>
+      <c r="AD9" s="21">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="21">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="21">
+        <v>1</v>
+      </c>
+      <c r="AG9" s="21">
+        <v>0</v>
+      </c>
+      <c r="AH9" s="21" t="s">
+        <v>147</v>
       </c>
       <c r="AJ9" s="12" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="C10" s="20">
-        <v>0</v>
-      </c>
-      <c r="D10" s="20">
-        <v>0</v>
-      </c>
-      <c r="E10" s="20">
-        <v>0</v>
-      </c>
-      <c r="F10" s="20">
-        <v>0</v>
-      </c>
-      <c r="G10" s="20">
-        <v>0</v>
-      </c>
-      <c r="H10" s="20">
-        <v>0</v>
-      </c>
-      <c r="I10" s="20">
-        <v>0</v>
-      </c>
-      <c r="J10" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="C10" s="21">
+        <v>0</v>
+      </c>
+      <c r="D10" s="21">
+        <v>0</v>
+      </c>
+      <c r="E10" s="21">
+        <v>0</v>
+      </c>
+      <c r="F10" s="21">
+        <v>0</v>
+      </c>
+      <c r="G10" s="21">
+        <v>0</v>
+      </c>
+      <c r="H10" s="21">
+        <v>0</v>
+      </c>
+      <c r="I10" s="21">
+        <v>0</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="28"/>
+      <c r="R10" s="28"/>
+      <c r="S10" s="14">
+        <v>0</v>
+      </c>
+      <c r="T10" s="6">
+        <v>0</v>
+      </c>
+      <c r="U10" s="6">
+        <v>0</v>
+      </c>
+      <c r="V10" s="6">
+        <v>0</v>
+      </c>
+      <c r="W10" s="6">
+        <v>0</v>
+      </c>
+      <c r="X10" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="21">
+        <v>1</v>
+      </c>
+      <c r="AD10" s="21">
+        <v>1</v>
+      </c>
+      <c r="AE10" s="21">
+        <v>1</v>
+      </c>
+      <c r="AF10" s="21">
+        <v>1</v>
+      </c>
+      <c r="AG10" s="21">
+        <v>1</v>
+      </c>
+      <c r="AH10" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ10" s="12" t="s">
         <v>172</v>
-      </c>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="22"/>
-      <c r="R10" s="22"/>
-      <c r="S10" s="14">
-        <v>0</v>
-      </c>
-      <c r="T10" s="6">
-        <v>0</v>
-      </c>
-      <c r="U10" s="6">
-        <v>0</v>
-      </c>
-      <c r="V10" s="6">
-        <v>0</v>
-      </c>
-      <c r="W10" s="6">
-        <v>0</v>
-      </c>
-      <c r="X10" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="6">
-        <v>0</v>
-      </c>
-      <c r="AB10" s="6">
-        <v>0</v>
-      </c>
-      <c r="AC10" s="20">
-        <v>1</v>
-      </c>
-      <c r="AD10" s="20">
-        <v>1</v>
-      </c>
-      <c r="AE10" s="20">
-        <v>1</v>
-      </c>
-      <c r="AF10" s="20">
-        <v>1</v>
-      </c>
-      <c r="AG10" s="20">
-        <v>1</v>
-      </c>
-      <c r="AH10" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="AJ10" s="12" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C11" s="6">
         <v>0</v>
@@ -1752,17 +1757,17 @@
         <v>0</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
       <c r="M11" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N11" s="10"/>
       <c r="O11" s="10"/>
       <c r="P11" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="Q11" s="10"/>
       <c r="R11" s="10"/>
@@ -1806,22 +1811,22 @@
         <v>0</v>
       </c>
       <c r="AF11" s="10" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="AG11" s="10"/>
       <c r="AH11" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AJ11" s="12" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="AK11" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C12" s="6">
         <v>0</v>
@@ -1845,27 +1850,27 @@
         <v>0</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
       <c r="M12" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N12" s="10"/>
       <c r="O12" s="10"/>
       <c r="P12" s="10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="Q12" s="10"/>
       <c r="R12" s="10"/>
       <c r="S12" s="10" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="T12" s="10"/>
       <c r="U12" s="10"/>
       <c r="V12" s="10" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="W12" s="10"/>
       <c r="X12" s="10"/>
@@ -1900,12 +1905,12 @@
         <v>0</v>
       </c>
       <c r="AJ12" s="12" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C13" s="6">
         <v>0</v>
@@ -1929,12 +1934,12 @@
         <v>1</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
       <c r="M13" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
@@ -1990,18 +1995,18 @@
         <v>0</v>
       </c>
       <c r="AG13" s="6" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="AH13" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AJ13" s="12" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C14" s="6">
         <v>0</v>
@@ -2025,7 +2030,7 @@
         <v>1</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K14" s="10"/>
       <c r="L14" s="10"/>
@@ -2045,7 +2050,7 @@
         <v>1</v>
       </c>
       <c r="R14" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="S14" s="6">
         <v>0</v>
@@ -2072,7 +2077,7 @@
         <v>0</v>
       </c>
       <c r="AA14" s="10" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AB14" s="10"/>
       <c r="AC14" s="10"/>
@@ -2082,12 +2087,12 @@
       <c r="AG14" s="10"/>
       <c r="AH14" s="10"/>
       <c r="AJ14" s="12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C15" s="6">
         <v>0</v>
@@ -2111,7 +2116,7 @@
         <v>1</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
@@ -2131,10 +2136,10 @@
         <v>0</v>
       </c>
       <c r="R15" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="S15" s="10" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="T15" s="10"/>
       <c r="U15" s="10"/>
@@ -2152,12 +2157,12 @@
       <c r="AG15" s="10"/>
       <c r="AH15" s="10"/>
       <c r="AJ15" s="12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C16" s="6">
         <v>0</v>
@@ -2181,7 +2186,7 @@
         <v>1</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
@@ -2201,10 +2206,10 @@
         <v>1</v>
       </c>
       <c r="R16" s="6" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="S16" s="10" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="T16" s="10"/>
       <c r="U16" s="10"/>
@@ -2222,12 +2227,12 @@
       <c r="AG16" s="10"/>
       <c r="AH16" s="10"/>
       <c r="AJ16" s="12" t="s">
-        <v>166</v>
+        <v>197</v>
       </c>
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C17" s="6">
         <v>0</v>
@@ -2248,15 +2253,15 @@
         <v>1</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
       <c r="M17" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
@@ -2280,12 +2285,12 @@
       <c r="AG17" s="10"/>
       <c r="AH17" s="10"/>
       <c r="AJ17" s="12" t="s">
-        <v>95</v>
+        <v>198</v>
       </c>
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C18" s="6">
         <v>0</v>
@@ -2306,15 +2311,15 @@
         <v>0</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K18" s="10"/>
       <c r="L18" s="10"/>
       <c r="M18" s="10" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="N18" s="10"/>
       <c r="O18" s="10"/>
@@ -2343,36 +2348,36 @@
     </row>
     <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="6">
+        <v>0</v>
+      </c>
+      <c r="D19" s="6">
+        <v>0</v>
+      </c>
+      <c r="E19" s="6">
+        <v>0</v>
+      </c>
+      <c r="F19" s="6">
+        <v>0</v>
+      </c>
+      <c r="G19" s="14">
+        <v>1</v>
+      </c>
+      <c r="H19" s="14">
+        <v>1</v>
+      </c>
+      <c r="I19" s="14">
+        <v>0</v>
+      </c>
+      <c r="J19" s="10" t="s">
         <v>6</v>
-      </c>
-      <c r="C19" s="6">
-        <v>0</v>
-      </c>
-      <c r="D19" s="6">
-        <v>0</v>
-      </c>
-      <c r="E19" s="6">
-        <v>0</v>
-      </c>
-      <c r="F19" s="6">
-        <v>0</v>
-      </c>
-      <c r="G19" s="14">
-        <v>1</v>
-      </c>
-      <c r="H19" s="14">
-        <v>1</v>
-      </c>
-      <c r="I19" s="14">
-        <v>0</v>
-      </c>
-      <c r="J19" s="10" t="s">
-        <v>7</v>
       </c>
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
       <c r="M19" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N19" s="10"/>
       <c r="O19" s="10"/>
@@ -2396,12 +2401,12 @@
       <c r="AG19" s="10"/>
       <c r="AH19" s="10"/>
       <c r="AJ19" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C20" s="6">
         <v>1</v>
@@ -2425,7 +2430,7 @@
         <v>1</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K20" s="10"/>
       <c r="L20" s="10"/>
@@ -2472,7 +2477,7 @@
         <v>0</v>
       </c>
       <c r="AA20" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AB20" s="10"/>
       <c r="AC20" s="10"/>
@@ -2482,12 +2487,12 @@
       <c r="AG20" s="10"/>
       <c r="AH20" s="10"/>
       <c r="AJ20" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C21" s="6">
         <v>1</v>
@@ -2511,7 +2516,7 @@
         <v>1</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K21" s="10"/>
       <c r="L21" s="10"/>
@@ -2558,7 +2563,7 @@
         <v>1</v>
       </c>
       <c r="AA21" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AB21" s="10"/>
       <c r="AC21" s="10"/>
@@ -2568,12 +2573,12 @@
       <c r="AG21" s="10"/>
       <c r="AH21" s="10"/>
       <c r="AJ21" s="12" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C22" s="6">
         <v>1</v>
@@ -2597,7 +2602,7 @@
         <v>1</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K22" s="10"/>
       <c r="L22" s="10"/>
@@ -2671,7 +2676,7 @@
     </row>
     <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C23" s="6">
         <v>1</v>
@@ -2746,7 +2751,7 @@
         <v>1</v>
       </c>
       <c r="AA23" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AB23" s="10"/>
       <c r="AC23" s="10"/>
@@ -3375,13 +3380,14 @@
       <c r="A46" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="37">
+  <mergeCells count="38">
     <mergeCell ref="J9:L9"/>
     <mergeCell ref="M9:O9"/>
     <mergeCell ref="P9:R9"/>
-    <mergeCell ref="J10:R10"/>
     <mergeCell ref="AF11:AG11"/>
     <mergeCell ref="V12:X12"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="M10:R10"/>
     <mergeCell ref="J21:L21"/>
     <mergeCell ref="AA21:AH21"/>
     <mergeCell ref="J22:L22"/>
@@ -3437,12 +3443,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="A1" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
@@ -3452,20 +3458,20 @@
       <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
-        <v>178</v>
-      </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="23" t="s">
-        <v>177</v>
+      <c r="A2" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="24" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3493,18 +3499,18 @@
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6">
@@ -3526,18 +3532,18 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6">
@@ -3559,18 +3565,18 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="L5" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6">
@@ -3592,18 +3598,18 @@
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="L6" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6">
@@ -3625,18 +3631,18 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L7" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6">
@@ -3658,15 +3664,15 @@
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6">
@@ -3688,18 +3694,18 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="K9" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="L9" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6">
@@ -3721,18 +3727,18 @@
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="K10" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L10" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6">
@@ -3754,12 +3760,12 @@
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6">
@@ -3781,12 +3787,12 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6">
@@ -3808,18 +3814,18 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="L13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6">
@@ -3841,18 +3847,18 @@
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K14" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L14" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6">
@@ -3874,18 +3880,18 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="L15" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6">
@@ -3907,18 +3913,18 @@
         <v>0</v>
       </c>
       <c r="J16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K16" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L16" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6">
@@ -3940,18 +3946,18 @@
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K17" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L17" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6">
@@ -3973,18 +3979,18 @@
         <v>0</v>
       </c>
       <c r="J18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K18" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="L18" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6">
@@ -4006,18 +4012,18 @@
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K19" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L19" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6">
@@ -4039,18 +4045,18 @@
         <v>0</v>
       </c>
       <c r="J20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K20" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L20" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="6">
@@ -4072,18 +4078,18 @@
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K21" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L21" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="6">
@@ -4105,18 +4111,18 @@
         <v>0</v>
       </c>
       <c r="J22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K22" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="L22" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="6">
@@ -4138,18 +4144,18 @@
         <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K23" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L23" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="6">
@@ -4171,18 +4177,18 @@
         <v>0</v>
       </c>
       <c r="J24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="L24" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="6">
@@ -4204,18 +4210,18 @@
         <v>0</v>
       </c>
       <c r="J25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K25" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="L25" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="6">
@@ -4237,18 +4243,18 @@
         <v>1</v>
       </c>
       <c r="J26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K26" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L26" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="6">
@@ -4270,18 +4276,18 @@
         <v>0</v>
       </c>
       <c r="J27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L27" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="6">
@@ -4303,18 +4309,18 @@
         <v>1</v>
       </c>
       <c r="J28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K28" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="L28" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="6">
@@ -4336,18 +4342,18 @@
         <v>0</v>
       </c>
       <c r="J29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K29" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L29" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="6">
@@ -4369,18 +4375,18 @@
         <v>1</v>
       </c>
       <c r="J30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K30" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="L30" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="6">
@@ -4402,18 +4408,18 @@
         <v>0</v>
       </c>
       <c r="J31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K31" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="L31" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="6">
@@ -4435,18 +4441,18 @@
         <v>1</v>
       </c>
       <c r="J32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K32" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="L32" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="6">
@@ -4468,18 +4474,18 @@
         <v>0</v>
       </c>
       <c r="J33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K33" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L33" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="6">
@@ -4501,18 +4507,18 @@
         <v>1</v>
       </c>
       <c r="J34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K34" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="L34" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="6">
@@ -4534,18 +4540,18 @@
         <v>0</v>
       </c>
       <c r="J35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K35" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="L35" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="6">
@@ -4567,18 +4573,18 @@
         <v>1</v>
       </c>
       <c r="J36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K36" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="L36" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="6">
@@ -4600,18 +4606,18 @@
         <v>0</v>
       </c>
       <c r="J37" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K37" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="L37" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B38" s="6"/>
       <c r="C38" s="6">
@@ -4633,18 +4639,18 @@
         <v>1</v>
       </c>
       <c r="J38" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K38" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="L38" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="6">
@@ -4666,18 +4672,18 @@
         <v>0</v>
       </c>
       <c r="J39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K39" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L39" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B40" s="6"/>
       <c r="C40" s="6">
@@ -4699,44 +4705,44 @@
         <v>1</v>
       </c>
       <c r="J40" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K40" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="L40" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="18" t="s">
+      <c r="A41" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41" s="16"/>
+      <c r="C41" s="16">
+        <v>0</v>
+      </c>
+      <c r="D41" s="16">
+        <v>0</v>
+      </c>
+      <c r="E41" s="16">
+        <v>0</v>
+      </c>
+      <c r="F41" s="16">
+        <v>0</v>
+      </c>
+      <c r="G41" s="16">
+        <v>0</v>
+      </c>
+      <c r="H41" s="16">
+        <v>0</v>
+      </c>
+      <c r="I41" s="20"/>
+      <c r="J41" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15">
-        <v>0</v>
-      </c>
-      <c r="D41" s="15">
-        <v>0</v>
-      </c>
-      <c r="E41" s="15">
-        <v>0</v>
-      </c>
-      <c r="F41" s="15">
-        <v>0</v>
-      </c>
-      <c r="G41" s="15">
-        <v>0</v>
-      </c>
-      <c r="H41" s="15">
-        <v>0</v>
-      </c>
-      <c r="I41" s="19"/>
-      <c r="J41" s="19" t="s">
-        <v>90</v>
-      </c>
       <c r="K41" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -4777,7 +4783,7 @@
   <sheetData>
     <row r="1" spans="1:36" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -4954,7 +4960,7 @@
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C5" s="6">
         <v>0</v>
@@ -4981,7 +4987,7 @@
         <v>1</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L5" s="10"/>
       <c r="M5" s="10"/>
@@ -5010,7 +5016,7 @@
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C6" s="6">
         <v>0</v>
@@ -5037,7 +5043,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
@@ -5047,7 +5053,7 @@
       <c r="Q6" s="10"/>
       <c r="R6" s="10"/>
       <c r="S6" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="T6" s="10"/>
       <c r="U6" s="10"/>
@@ -5057,7 +5063,7 @@
       <c r="Y6" s="10"/>
       <c r="Z6" s="10"/>
       <c r="AA6" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="AB6" s="10"/>
       <c r="AC6" s="10"/>
@@ -5220,8 +5226,8 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="14"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
       <c r="J11" s="6"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
@@ -6231,7 +6237,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -6306,7 +6312,7 @@
         <v>0</v>
       </c>
       <c r="T3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -6328,68 +6334,68 @@
       <c r="Q4" s="11"/>
       <c r="R4" s="11"/>
       <c r="T4" s="12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0</v>
+      </c>
+      <c r="J5" s="6">
+        <v>0</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0</v>
+      </c>
+      <c r="L5" s="6">
+        <v>0</v>
+      </c>
+      <c r="M5" s="6">
+        <v>0</v>
+      </c>
+      <c r="N5" s="6">
+        <v>0</v>
+      </c>
+      <c r="O5" s="6">
+        <v>0</v>
+      </c>
+      <c r="P5" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>0</v>
+      </c>
+      <c r="R5" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="C5" s="6">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6">
-        <v>0</v>
-      </c>
-      <c r="G5" s="6">
-        <v>0</v>
-      </c>
-      <c r="H5" s="6">
-        <v>0</v>
-      </c>
-      <c r="I5" s="6">
-        <v>0</v>
-      </c>
-      <c r="J5" s="6">
-        <v>0</v>
-      </c>
-      <c r="K5" s="6">
-        <v>0</v>
-      </c>
-      <c r="L5" s="6">
-        <v>0</v>
-      </c>
-      <c r="M5" s="6">
-        <v>0</v>
-      </c>
-      <c r="N5" s="6">
-        <v>0</v>
-      </c>
-      <c r="O5" s="6">
-        <v>0</v>
-      </c>
-      <c r="P5" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="6">
-        <v>0</v>
-      </c>
-      <c r="R5" s="6" t="s">
-        <v>149</v>
-      </c>
       <c r="T5" s="12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C6" s="6">
         <v>0</v>
@@ -6416,7 +6422,7 @@
         <v>1</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
@@ -6429,7 +6435,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C7" s="6">
         <v>0</v>
@@ -6453,10 +6459,10 @@
         <v>1</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
@@ -6469,7 +6475,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C8" s="6">
         <v>0</v>
@@ -6493,10 +6499,10 @@
         <v>0</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
@@ -6509,7 +6515,7 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C9" s="6">
         <v>0</v>
@@ -6533,10 +6539,10 @@
         <v>1</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>

</xml_diff>

<commit_message>
conditional in every instruction (except CMP)
</commit_message>
<xml_diff>
--- a/doc/RiscyInstSet32Bit.xlsx
+++ b/doc/RiscyInstSet32Bit.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="215">
   <si>
     <t>Description</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Registers key:</t>
   </si>
   <si>
-    <t>Jump</t>
-  </si>
-  <si>
     <t>Cond</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
     <t>Push and Pop</t>
   </si>
   <si>
-    <t>Cond: 0-Un, 1-m1 == zero, 2-m1 != nonzero, 3-m1 &gt; 0, 4-m1 &lt; 0, 5-fwd, 6-bwd</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -627,13 +621,64 @@
   </si>
   <si>
     <t>C: 0-Push 1-Pop; IntOffset: set to 0 if not used; popped value will go to LR register if IntOffset is non-zero</t>
+  </si>
+  <si>
+    <t>Conditional jump</t>
+  </si>
+  <si>
+    <t>Conditional suffix</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>NZ</t>
+  </si>
+  <si>
+    <t>GT</t>
+  </si>
+  <si>
+    <t>LS</t>
+  </si>
+  <si>
+    <t>m1 == 0</t>
+  </si>
+  <si>
+    <t>m1 != 0</t>
+  </si>
+  <si>
+    <t>m1 &gt; 0</t>
+  </si>
+  <si>
+    <t>m1 &lt; 0</t>
+  </si>
+  <si>
+    <t>e.g. RETURNGT</t>
+  </si>
+  <si>
+    <t>e.g. XORLS</t>
+  </si>
+  <si>
+    <t>Cond: 0-Un, 1-m1==zero, 2-m1 != zero, 3-m1 &gt; 0, 4-m1 &lt; 0</t>
+  </si>
+  <si>
+    <t>Cond: 5-fwd, 6-bwd</t>
+  </si>
+  <si>
+    <t>e.g. MOVZ</t>
+  </si>
+  <si>
+    <t>e.g. GOSUBNZ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -674,6 +719,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -696,12 +748,17 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -812,19 +869,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -860,50 +918,68 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="5" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="6" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="Explanatory Text" xfId="6" builtinId="53" customBuiltin="1"/>
+  <cellStyles count="8">
+    <cellStyle name="Explanatory Text" xfId="7" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
     <cellStyle name="Heading 3" xfId="3" builtinId="18"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="5" builtinId="10"/>
-    <cellStyle name="Warning Text" xfId="4" builtinId="11"/>
+    <cellStyle name="Note" xfId="6" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="5" builtinId="11"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1183,8 +1259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="AJ19" sqref="AJ19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20:L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1238,7 +1314,7 @@
     <row r="2" spans="1:37" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5" t="s">
@@ -1281,7 +1357,7 @@
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="12">
@@ -1319,12 +1395,12 @@
       <c r="AG4" s="5"/>
       <c r="AH4" s="5"/>
       <c r="AJ4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
@@ -1362,7 +1438,12 @@
       <c r="AG5" s="5"/>
       <c r="AH5" s="5"/>
       <c r="AJ5" t="s">
-        <v>161</v>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AJ6" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1469,17 +1550,13 @@
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="13">
-        <v>0</v>
-      </c>
-      <c r="D8" s="13">
-        <v>0</v>
-      </c>
-      <c r="E8" s="13">
-        <v>0</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
       <c r="F8" s="13">
         <v>0</v>
       </c>
@@ -1493,17 +1570,17 @@
         <v>0</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K8" s="11"/>
       <c r="L8" s="11"/>
       <c r="M8" s="11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="N8" s="11"/>
       <c r="O8" s="11"/>
       <c r="P8" s="11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="Q8" s="11"/>
       <c r="R8" s="11"/>
@@ -1538,7 +1615,7 @@
         <v>0</v>
       </c>
       <c r="AC8" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="AD8" s="11"/>
       <c r="AE8" s="11"/>
@@ -1546,22 +1623,18 @@
       <c r="AG8" s="11"/>
       <c r="AH8" s="11"/>
       <c r="AJ8" s="12" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C9" s="21">
-        <v>0</v>
-      </c>
-      <c r="D9" s="21">
-        <v>0</v>
-      </c>
-      <c r="E9" s="21">
-        <v>0</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
       <c r="F9" s="21">
         <v>0</v>
       </c>
@@ -1574,21 +1647,19 @@
       <c r="I9" s="21">
         <v>0</v>
       </c>
-      <c r="J9" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22" t="s">
-        <v>168</v>
-      </c>
-      <c r="N9" s="22"/>
-      <c r="O9" s="22"/>
-      <c r="P9" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="Q9" s="23"/>
-      <c r="R9" s="23"/>
+      <c r="J9" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="29"/>
       <c r="S9" s="14">
         <v>0</v>
       </c>
@@ -1623,127 +1694,121 @@
         <v>1</v>
       </c>
       <c r="AD9" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE9" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF9" s="21">
         <v>1</v>
       </c>
       <c r="AG9" s="21">
-        <v>0</v>
-      </c>
-      <c r="AH9" s="21" t="s">
-        <v>147</v>
+        <v>1</v>
+      </c>
+      <c r="AH9" s="32" t="s">
+        <v>10</v>
       </c>
       <c r="AJ9" s="12" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="21">
+        <v>0</v>
+      </c>
+      <c r="G10" s="21">
+        <v>0</v>
+      </c>
+      <c r="H10" s="21">
+        <v>0</v>
+      </c>
+      <c r="I10" s="21">
+        <v>0</v>
+      </c>
+      <c r="J10" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q10" s="23"/>
+      <c r="R10" s="23"/>
+      <c r="S10" s="14">
+        <v>0</v>
+      </c>
+      <c r="T10" s="6">
+        <v>0</v>
+      </c>
+      <c r="U10" s="6">
+        <v>0</v>
+      </c>
+      <c r="V10" s="6">
+        <v>0</v>
+      </c>
+      <c r="W10" s="6">
+        <v>0</v>
+      </c>
+      <c r="X10" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="21">
+        <v>1</v>
+      </c>
+      <c r="AD10" s="21">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="21">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="21">
+        <v>1</v>
+      </c>
+      <c r="AG10" s="21">
+        <v>0</v>
+      </c>
+      <c r="AH10" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="AJ10" s="12" t="s">
         <v>171</v>
-      </c>
-      <c r="C10" s="21">
-        <v>0</v>
-      </c>
-      <c r="D10" s="21">
-        <v>0</v>
-      </c>
-      <c r="E10" s="21">
-        <v>0</v>
-      </c>
-      <c r="F10" s="21">
-        <v>0</v>
-      </c>
-      <c r="G10" s="21">
-        <v>0</v>
-      </c>
-      <c r="H10" s="21">
-        <v>0</v>
-      </c>
-      <c r="I10" s="21">
-        <v>0</v>
-      </c>
-      <c r="J10" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="28" t="s">
-        <v>169</v>
-      </c>
-      <c r="N10" s="28"/>
-      <c r="O10" s="28"/>
-      <c r="P10" s="28"/>
-      <c r="Q10" s="28"/>
-      <c r="R10" s="28"/>
-      <c r="S10" s="14">
-        <v>0</v>
-      </c>
-      <c r="T10" s="6">
-        <v>0</v>
-      </c>
-      <c r="U10" s="6">
-        <v>0</v>
-      </c>
-      <c r="V10" s="6">
-        <v>0</v>
-      </c>
-      <c r="W10" s="6">
-        <v>0</v>
-      </c>
-      <c r="X10" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="6">
-        <v>0</v>
-      </c>
-      <c r="AB10" s="6">
-        <v>0</v>
-      </c>
-      <c r="AC10" s="21">
-        <v>1</v>
-      </c>
-      <c r="AD10" s="21">
-        <v>1</v>
-      </c>
-      <c r="AE10" s="21">
-        <v>1</v>
-      </c>
-      <c r="AF10" s="21">
-        <v>1</v>
-      </c>
-      <c r="AG10" s="21">
-        <v>1</v>
-      </c>
-      <c r="AH10" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="AJ10" s="12" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="C11" s="6">
-        <v>0</v>
-      </c>
-      <c r="D11" s="6">
-        <v>0</v>
-      </c>
-      <c r="E11" s="6">
-        <v>0</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
       <c r="F11" s="6">
         <v>0</v>
       </c>
@@ -1757,17 +1822,17 @@
         <v>0</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
       <c r="M11" s="10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="N11" s="10"/>
       <c r="O11" s="10"/>
       <c r="P11" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="Q11" s="10"/>
       <c r="R11" s="10"/>
@@ -1810,33 +1875,29 @@
       <c r="AE11" s="6">
         <v>0</v>
       </c>
-      <c r="AF11" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="AG11" s="10"/>
-      <c r="AH11" s="6" t="s">
-        <v>94</v>
+      <c r="AF11" s="30" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG11" s="30"/>
+      <c r="AH11" s="33" t="s">
+        <v>92</v>
       </c>
       <c r="AJ11" s="12" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="AK11" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C12" s="6">
-        <v>0</v>
-      </c>
-      <c r="D12" s="6">
-        <v>0</v>
-      </c>
-      <c r="E12" s="6">
-        <v>0</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="6">
         <v>0</v>
       </c>
@@ -1850,27 +1911,27 @@
         <v>0</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
       <c r="M12" s="10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="N12" s="10"/>
       <c r="O12" s="10"/>
       <c r="P12" s="10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="Q12" s="10"/>
       <c r="R12" s="10"/>
       <c r="S12" s="10" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="T12" s="10"/>
       <c r="U12" s="10"/>
       <c r="V12" s="10" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="W12" s="10"/>
       <c r="X12" s="10"/>
@@ -1905,22 +1966,18 @@
         <v>0</v>
       </c>
       <c r="AJ12" s="12" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C13" s="6">
-        <v>0</v>
-      </c>
-      <c r="D13" s="6">
-        <v>0</v>
-      </c>
-      <c r="E13" s="6">
-        <v>0</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>167</v>
+      </c>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
       <c r="F13" s="6">
         <v>0</v>
       </c>
@@ -1934,12 +1991,12 @@
         <v>1</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
       <c r="M13" s="10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
@@ -1994,29 +2051,25 @@
       <c r="AF13" s="6">
         <v>0</v>
       </c>
-      <c r="AG13" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="AH13" s="6" t="s">
-        <v>109</v>
+      <c r="AG13" s="33" t="s">
+        <v>190</v>
+      </c>
+      <c r="AH13" s="33" t="s">
+        <v>107</v>
       </c>
       <c r="AJ13" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="C14" s="6">
-        <v>0</v>
-      </c>
-      <c r="D14" s="6">
-        <v>0</v>
-      </c>
-      <c r="E14" s="6">
-        <v>0</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
       <c r="F14" s="6">
         <v>0</v>
       </c>
@@ -2030,7 +2083,7 @@
         <v>1</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K14" s="10"/>
       <c r="L14" s="10"/>
@@ -2049,8 +2102,8 @@
       <c r="Q14" s="6">
         <v>1</v>
       </c>
-      <c r="R14" s="6" t="s">
-        <v>12</v>
+      <c r="R14" s="33" t="s">
+        <v>10</v>
       </c>
       <c r="S14" s="6">
         <v>0</v>
@@ -2077,7 +2130,7 @@
         <v>0</v>
       </c>
       <c r="AA14" s="10" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="AB14" s="10"/>
       <c r="AC14" s="10"/>
@@ -2087,22 +2140,18 @@
       <c r="AG14" s="10"/>
       <c r="AH14" s="10"/>
       <c r="AJ14" s="12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="C15" s="6">
-        <v>0</v>
-      </c>
-      <c r="D15" s="6">
-        <v>0</v>
-      </c>
-      <c r="E15" s="6">
-        <v>0</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
       <c r="F15" s="6">
         <v>0</v>
       </c>
@@ -2116,7 +2165,7 @@
         <v>1</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
@@ -2135,11 +2184,11 @@
       <c r="Q15" s="6">
         <v>0</v>
       </c>
-      <c r="R15" s="6" t="s">
-        <v>12</v>
+      <c r="R15" s="33" t="s">
+        <v>10</v>
       </c>
       <c r="S15" s="10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="T15" s="10"/>
       <c r="U15" s="10"/>
@@ -2157,22 +2206,18 @@
       <c r="AG15" s="10"/>
       <c r="AH15" s="10"/>
       <c r="AJ15" s="12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="C16" s="6">
-        <v>0</v>
-      </c>
-      <c r="D16" s="6">
-        <v>0</v>
-      </c>
-      <c r="E16" s="6">
-        <v>0</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
       <c r="F16" s="6">
         <v>0</v>
       </c>
@@ -2186,7 +2231,7 @@
         <v>1</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
@@ -2205,11 +2250,11 @@
       <c r="Q16" s="6">
         <v>1</v>
       </c>
-      <c r="R16" s="6" t="s">
-        <v>12</v>
+      <c r="R16" s="33" t="s">
+        <v>10</v>
       </c>
       <c r="S16" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="T16" s="10"/>
       <c r="U16" s="10"/>
@@ -2227,22 +2272,18 @@
       <c r="AG16" s="10"/>
       <c r="AH16" s="10"/>
       <c r="AJ16" s="12" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="C17" s="6">
-        <v>0</v>
-      </c>
-      <c r="D17" s="6">
-        <v>0</v>
-      </c>
-      <c r="E17" s="6">
-        <v>0</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
       <c r="F17" s="6">
         <v>0</v>
       </c>
@@ -2253,15 +2294,15 @@
         <v>1</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
       <c r="M17" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
@@ -2285,22 +2326,18 @@
       <c r="AG17" s="10"/>
       <c r="AH17" s="10"/>
       <c r="AJ17" s="12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="6">
-        <v>0</v>
-      </c>
-      <c r="D18" s="6">
-        <v>0</v>
-      </c>
-      <c r="E18" s="6">
-        <v>0</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
       <c r="F18" s="6">
         <v>0</v>
       </c>
@@ -2311,15 +2348,15 @@
         <v>0</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K18" s="10"/>
       <c r="L18" s="10"/>
       <c r="M18" s="10" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="N18" s="10"/>
       <c r="O18" s="10"/>
@@ -2343,22 +2380,18 @@
       <c r="AG18" s="10"/>
       <c r="AH18" s="10"/>
       <c r="AJ18" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C19" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="6">
-        <v>0</v>
-      </c>
-      <c r="D19" s="6">
-        <v>0</v>
-      </c>
-      <c r="E19" s="6">
-        <v>0</v>
-      </c>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
       <c r="F19" s="6">
         <v>0</v>
       </c>
@@ -2371,13 +2404,13 @@
       <c r="I19" s="14">
         <v>0</v>
       </c>
-      <c r="J19" s="10" t="s">
+      <c r="J19" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="K19" s="29"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="10" t="s">
         <v>6</v>
-      </c>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10" t="s">
-        <v>7</v>
       </c>
       <c r="N19" s="10"/>
       <c r="O19" s="10"/>
@@ -2401,22 +2434,18 @@
       <c r="AG19" s="10"/>
       <c r="AH19" s="10"/>
       <c r="AJ19" s="12" t="s">
-        <v>11</v>
+        <v>212</v>
       </c>
     </row>
     <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C20" s="6">
-        <v>1</v>
-      </c>
-      <c r="D20" s="6">
-        <v>1</v>
-      </c>
-      <c r="E20" s="6">
-        <v>1</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
       <c r="F20" s="6">
         <v>1</v>
       </c>
@@ -2430,7 +2459,7 @@
         <v>1</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K20" s="10"/>
       <c r="L20" s="10"/>
@@ -2477,7 +2506,7 @@
         <v>0</v>
       </c>
       <c r="AA20" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AB20" s="10"/>
       <c r="AC20" s="10"/>
@@ -2487,22 +2516,18 @@
       <c r="AG20" s="10"/>
       <c r="AH20" s="10"/>
       <c r="AJ20" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C21" s="6">
-        <v>1</v>
-      </c>
-      <c r="D21" s="6">
-        <v>1</v>
-      </c>
-      <c r="E21" s="6">
-        <v>1</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
       <c r="F21" s="6">
         <v>1</v>
       </c>
@@ -2516,7 +2541,7 @@
         <v>1</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K21" s="10"/>
       <c r="L21" s="10"/>
@@ -2563,7 +2588,7 @@
         <v>1</v>
       </c>
       <c r="AA21" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AB21" s="10"/>
       <c r="AC21" s="10"/>
@@ -2573,22 +2598,18 @@
       <c r="AG21" s="10"/>
       <c r="AH21" s="10"/>
       <c r="AJ21" s="12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C22" s="6">
-        <v>1</v>
-      </c>
-      <c r="D22" s="6">
-        <v>1</v>
-      </c>
-      <c r="E22" s="6">
-        <v>1</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
       <c r="F22" s="6">
         <v>1</v>
       </c>
@@ -2602,7 +2623,7 @@
         <v>1</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K22" s="10"/>
       <c r="L22" s="10"/>
@@ -2676,17 +2697,13 @@
     </row>
     <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C23" s="6">
-        <v>1</v>
-      </c>
-      <c r="D23" s="6">
-        <v>1</v>
-      </c>
-      <c r="E23" s="6">
-        <v>1</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
       <c r="F23" s="6">
         <v>1</v>
       </c>
@@ -2751,7 +2768,7 @@
         <v>1</v>
       </c>
       <c r="AA23" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AB23" s="10"/>
       <c r="AC23" s="10"/>
@@ -2760,42 +2777,6 @@
       <c r="AF23" s="10"/>
       <c r="AG23" s="10"/>
       <c r="AH23" s="10"/>
-    </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
-      <c r="O25" s="6"/>
-      <c r="P25" s="6"/>
-      <c r="Q25" s="6"/>
-      <c r="R25" s="6"/>
-      <c r="S25" s="6"/>
-      <c r="T25" s="6"/>
-      <c r="U25" s="6"/>
-      <c r="V25" s="6"/>
-      <c r="W25" s="6"/>
-      <c r="X25" s="6"/>
-      <c r="Y25" s="6"/>
-      <c r="Z25" s="6"/>
-      <c r="AA25" s="6"/>
-      <c r="AB25" s="6"/>
-      <c r="AC25" s="6"/>
-      <c r="AD25" s="6"/>
-      <c r="AE25" s="6"/>
-      <c r="AF25" s="6"/>
-      <c r="AG25" s="6"/>
-      <c r="AH25" s="6"/>
-      <c r="AJ25" s="12"/>
     </row>
     <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
@@ -3380,14 +3361,29 @@
       <c r="A46" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="38">
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="P9:R9"/>
+  <mergeCells count="54">
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="P10:R10"/>
     <mergeCell ref="AF11:AG11"/>
     <mergeCell ref="V12:X12"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="M10:R10"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="M9:R9"/>
     <mergeCell ref="J21:L21"/>
     <mergeCell ref="AA21:AH21"/>
     <mergeCell ref="J22:L22"/>
@@ -3400,7 +3396,7 @@
     <mergeCell ref="M12:O12"/>
     <mergeCell ref="P12:R12"/>
     <mergeCell ref="S12:U12"/>
-    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="C19:E19"/>
     <mergeCell ref="J15:L15"/>
     <mergeCell ref="S15:AH15"/>
     <mergeCell ref="AA23:AH23"/>
@@ -3414,6 +3410,7 @@
     <mergeCell ref="J18:L18"/>
     <mergeCell ref="J20:L20"/>
     <mergeCell ref="S16:AH16"/>
+    <mergeCell ref="J19:L19"/>
     <mergeCell ref="AC8:AH8"/>
     <mergeCell ref="J8:L8"/>
     <mergeCell ref="M8:O8"/>
@@ -3427,10 +3424,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L42"/>
+  <dimension ref="A1:O42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3440,11 +3437,14 @@
     <col min="3" max="8" width="3.42578125" customWidth="1"/>
     <col min="9" max="9" width="2.5703125" customWidth="1"/>
     <col min="11" max="11" width="45.7109375" customWidth="1"/>
+    <col min="13" max="13" width="3.42578125" customWidth="1"/>
+    <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -3457,24 +3457,24 @@
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
     </row>
-    <row r="2" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="24" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="25" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -3499,18 +3499,24 @@
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="O3" s="34" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6">
@@ -3532,18 +3538,24 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" t="s">
+        <v>103</v>
+      </c>
+      <c r="L4" t="s">
+        <v>175</v>
+      </c>
+      <c r="N4" t="s">
+        <v>201</v>
+      </c>
+      <c r="O4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="K4" t="s">
-        <v>105</v>
-      </c>
-      <c r="L4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>22</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6">
@@ -3565,18 +3577,24 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="L5" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+      <c r="N5" t="s">
+        <v>202</v>
+      </c>
+      <c r="O5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6">
@@ -3598,18 +3616,24 @@
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L6" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+      <c r="N6" t="s">
+        <v>203</v>
+      </c>
+      <c r="O6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6">
@@ -3631,18 +3655,24 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="L7" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+      <c r="N7" t="s">
+        <v>204</v>
+      </c>
+      <c r="O7" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6">
@@ -3664,15 +3694,15 @@
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6">
@@ -3694,18 +3724,21 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
+        <v>178</v>
+      </c>
+      <c r="K9" t="s">
         <v>180</v>
       </c>
-      <c r="K9" t="s">
-        <v>182</v>
-      </c>
       <c r="L9" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+      <c r="N9" s="24" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6">
@@ -3727,18 +3760,21 @@
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K10" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="L10" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+      <c r="N10" s="24" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6">
@@ -3760,12 +3796,15 @@
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="N11" s="24" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6">
@@ -3787,12 +3826,15 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="N12" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6">
@@ -3814,18 +3856,18 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="L13" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6">
@@ -3847,18 +3889,18 @@
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="L14" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6">
@@ -3880,18 +3922,18 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="L15" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6">
@@ -3913,18 +3955,18 @@
         <v>0</v>
       </c>
       <c r="J16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L16" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6">
@@ -3946,18 +3988,18 @@
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K17" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="L17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6">
@@ -3979,18 +4021,18 @@
         <v>0</v>
       </c>
       <c r="J18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L18" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6">
@@ -4012,18 +4054,18 @@
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K19" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L19" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6">
@@ -4045,18 +4087,18 @@
         <v>0</v>
       </c>
       <c r="J20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K20" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="L20" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="6">
@@ -4078,18 +4120,18 @@
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K21" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L21" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="6">
@@ -4111,18 +4153,18 @@
         <v>0</v>
       </c>
       <c r="J22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K22" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L22" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="6">
@@ -4144,18 +4186,18 @@
         <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K23" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L23" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="6">
@@ -4177,18 +4219,18 @@
         <v>0</v>
       </c>
       <c r="J24" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K24" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="L24" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="6">
@@ -4210,18 +4252,18 @@
         <v>0</v>
       </c>
       <c r="J25" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K25" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="L25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="6">
@@ -4243,18 +4285,18 @@
         <v>1</v>
       </c>
       <c r="J26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K26" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L26" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="6">
@@ -4276,18 +4318,18 @@
         <v>0</v>
       </c>
       <c r="J27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L27" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="6">
@@ -4309,18 +4351,18 @@
         <v>1</v>
       </c>
       <c r="J28" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K28" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="L28" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="6">
@@ -4342,18 +4384,18 @@
         <v>0</v>
       </c>
       <c r="J29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K29" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L29" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="6">
@@ -4375,18 +4417,18 @@
         <v>1</v>
       </c>
       <c r="J30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K30" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="L30" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="6">
@@ -4408,18 +4450,18 @@
         <v>0</v>
       </c>
       <c r="J31" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K31" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L31" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="6">
@@ -4441,18 +4483,18 @@
         <v>1</v>
       </c>
       <c r="J32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K32" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="L32" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="6">
@@ -4474,18 +4516,18 @@
         <v>0</v>
       </c>
       <c r="J33" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K33" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="L33" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="6">
@@ -4507,18 +4549,18 @@
         <v>1</v>
       </c>
       <c r="J34" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K34" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="L34" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="6">
@@ -4540,18 +4582,18 @@
         <v>0</v>
       </c>
       <c r="J35" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K35" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="L35" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="6">
@@ -4573,18 +4615,18 @@
         <v>1</v>
       </c>
       <c r="J36" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K36" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L36" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="6">
@@ -4606,18 +4648,18 @@
         <v>0</v>
       </c>
       <c r="J37" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K37" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="L37" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B38" s="6"/>
       <c r="C38" s="6">
@@ -4639,18 +4681,18 @@
         <v>1</v>
       </c>
       <c r="J38" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K38" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L38" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="6">
@@ -4672,18 +4714,18 @@
         <v>0</v>
       </c>
       <c r="J39" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K39" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="L39" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B40" s="6"/>
       <c r="C40" s="6">
@@ -4705,18 +4747,18 @@
         <v>1</v>
       </c>
       <c r="J40" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K40" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="L40" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B41" s="16"/>
       <c r="C41" s="16">
@@ -4739,10 +4781,10 @@
       </c>
       <c r="I41" s="20"/>
       <c r="J41" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K41" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -4783,7 +4825,7 @@
   <sheetData>
     <row r="1" spans="1:36" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -4960,7 +5002,7 @@
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C5" s="6">
         <v>0</v>
@@ -4987,7 +5029,7 @@
         <v>1</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L5" s="10"/>
       <c r="M5" s="10"/>
@@ -5016,7 +5058,7 @@
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C6" s="6">
         <v>0</v>
@@ -5043,7 +5085,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
@@ -5053,7 +5095,7 @@
       <c r="Q6" s="10"/>
       <c r="R6" s="10"/>
       <c r="S6" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="T6" s="10"/>
       <c r="U6" s="10"/>
@@ -5063,7 +5105,7 @@
       <c r="Y6" s="10"/>
       <c r="Z6" s="10"/>
       <c r="AA6" s="10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="AB6" s="10"/>
       <c r="AC6" s="10"/>
@@ -6237,7 +6279,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -6312,7 +6354,7 @@
         <v>0</v>
       </c>
       <c r="T3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -6334,68 +6376,68 @@
       <c r="Q4" s="11"/>
       <c r="R4" s="11"/>
       <c r="T4" s="12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0</v>
+      </c>
+      <c r="J5" s="6">
+        <v>0</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0</v>
+      </c>
+      <c r="L5" s="6">
+        <v>0</v>
+      </c>
+      <c r="M5" s="6">
+        <v>0</v>
+      </c>
+      <c r="N5" s="6">
+        <v>0</v>
+      </c>
+      <c r="O5" s="6">
+        <v>0</v>
+      </c>
+      <c r="P5" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>0</v>
+      </c>
+      <c r="R5" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="C5" s="6">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6">
-        <v>0</v>
-      </c>
-      <c r="G5" s="6">
-        <v>0</v>
-      </c>
-      <c r="H5" s="6">
-        <v>0</v>
-      </c>
-      <c r="I5" s="6">
-        <v>0</v>
-      </c>
-      <c r="J5" s="6">
-        <v>0</v>
-      </c>
-      <c r="K5" s="6">
-        <v>0</v>
-      </c>
-      <c r="L5" s="6">
-        <v>0</v>
-      </c>
-      <c r="M5" s="6">
-        <v>0</v>
-      </c>
-      <c r="N5" s="6">
-        <v>0</v>
-      </c>
-      <c r="O5" s="6">
-        <v>0</v>
-      </c>
-      <c r="P5" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="6">
-        <v>0</v>
-      </c>
-      <c r="R5" s="6" t="s">
-        <v>147</v>
-      </c>
       <c r="T5" s="12" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C6" s="6">
         <v>0</v>
@@ -6422,7 +6464,7 @@
         <v>1</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
@@ -6435,7 +6477,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C7" s="6">
         <v>0</v>
@@ -6459,10 +6501,10 @@
         <v>1</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
@@ -6475,7 +6517,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C8" s="6">
         <v>0</v>
@@ -6499,10 +6541,10 @@
         <v>0</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
@@ -6515,7 +6557,7 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C9" s="6">
         <v>0</v>
@@ -6539,10 +6581,10 @@
         <v>1</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>

</xml_diff>

<commit_message>
going RISCy with assembler
</commit_message>
<xml_diff>
--- a/doc/RiscyInstSet32Bit.xlsx
+++ b/doc/RiscyInstSet32Bit.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="214">
   <si>
     <t>Description</t>
   </si>
@@ -152,9 +152,6 @@
     <t>Log</t>
   </si>
   <si>
-    <t>Int-ify</t>
-  </si>
-  <si>
     <t>Random</t>
   </si>
   <si>
@@ -239,9 +236,6 @@
     <t>LOG</t>
   </si>
   <si>
-    <t>INT</t>
-  </si>
-  <si>
     <t>RND</t>
   </si>
   <si>
@@ -410,9 +404,6 @@
     <t>Rd = Log(Rs)</t>
   </si>
   <si>
-    <t>Rd = Int(Rs)</t>
-  </si>
-  <si>
     <t>Rd = Sgn(Rs)</t>
   </si>
   <si>
@@ -542,9 +533,6 @@
     <t>M: 0-GOSUB, 1-RETURN</t>
   </si>
   <si>
-    <t>Rsize must contain size of memory, in T: 0-Int32, 1-Float</t>
-  </si>
-  <si>
     <t>Unused registers are ignored</t>
   </si>
   <si>
@@ -569,21 +557,12 @@
     <t>ITOF</t>
   </si>
   <si>
-    <t>Rd = Rs.toInt</t>
-  </si>
-  <si>
-    <t>Rd = Rs.</t>
-  </si>
-  <si>
     <t>Float to Int</t>
   </si>
   <si>
     <t>Int to Float</t>
   </si>
   <si>
-    <t>Rd = Rs.toFloat</t>
-  </si>
-  <si>
     <t>memory[Rd] = Rs, only the low 8 bits of Rs are used</t>
   </si>
   <si>
@@ -620,9 +599,6 @@
     <t>C: 0-Load, 1-Store</t>
   </si>
   <si>
-    <t>C: 0-Push 1-Pop; IntOffset: set to 0 if not used; popped value will go to LR register if IntOffset is non-zero</t>
-  </si>
-  <si>
     <t>Conditional jump</t>
   </si>
   <si>
@@ -672,6 +648,27 @@
   </si>
   <si>
     <t>e.g. GOSUBNZ</t>
+  </si>
+  <si>
+    <t>Rd = (int) Rs</t>
+  </si>
+  <si>
+    <t>Rd = (float) Rs</t>
+  </si>
+  <si>
+    <t>RNDI</t>
+  </si>
+  <si>
+    <t>Rd = Rndint()</t>
+  </si>
+  <si>
+    <t>Random integer</t>
+  </si>
+  <si>
+    <t>Rsize must contain size of memory, in Int32</t>
+  </si>
+  <si>
+    <t>M: 0-push reg, 1-pushword; C: 0-Push 1-Pop; IntOffset: set to 0 if not used; popped value will go to LR register if IntOffset is non-zero</t>
   </si>
 </sst>
 </file>
@@ -879,7 +876,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="6" applyFont="1"/>
@@ -901,12 +898,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -921,9 +912,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -932,15 +920,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="7"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="6" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -950,25 +969,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="7" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="7" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1259,8 +1259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20:L20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="AJ19" sqref="AJ19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1314,7 +1314,7 @@
     <row r="2" spans="1:37" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5" t="s">
@@ -1360,7 +1360,7 @@
         <v>16</v>
       </c>
       <c r="B4" s="5"/>
-      <c r="C4" s="12">
+      <c r="C4" s="10">
         <v>8</v>
       </c>
       <c r="D4" s="5"/>
@@ -1400,7 +1400,7 @@
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
@@ -1438,12 +1438,12 @@
       <c r="AG5" s="5"/>
       <c r="AH5" s="5"/>
       <c r="AJ5" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="AJ6" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1552,39 +1552,39 @@
       <c r="A8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="13">
-        <v>0</v>
-      </c>
-      <c r="G8" s="13">
-        <v>0</v>
-      </c>
-      <c r="H8" s="13">
-        <v>0</v>
-      </c>
-      <c r="I8" s="13">
-        <v>0</v>
-      </c>
-      <c r="J8" s="11" t="s">
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="11">
+        <v>0</v>
+      </c>
+      <c r="G8" s="11">
+        <v>0</v>
+      </c>
+      <c r="H8" s="11">
+        <v>0</v>
+      </c>
+      <c r="I8" s="11">
+        <v>0</v>
+      </c>
+      <c r="J8" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11" t="s">
+      <c r="K8" s="32"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11" t="s">
+      <c r="N8" s="32"/>
+      <c r="O8" s="32"/>
+      <c r="P8" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="14">
+      <c r="Q8" s="32"/>
+      <c r="R8" s="32"/>
+      <c r="S8" s="12">
         <v>0</v>
       </c>
       <c r="T8" s="6">
@@ -1614,141 +1614,141 @@
       <c r="AB8" s="6">
         <v>0</v>
       </c>
-      <c r="AC8" s="11" t="s">
+      <c r="AC8" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="AD8" s="11"/>
-      <c r="AE8" s="11"/>
-      <c r="AF8" s="11"/>
-      <c r="AG8" s="11"/>
-      <c r="AH8" s="11"/>
-      <c r="AJ8" s="12" t="s">
-        <v>168</v>
+      <c r="AD8" s="32"/>
+      <c r="AE8" s="32"/>
+      <c r="AF8" s="32"/>
+      <c r="AG8" s="32"/>
+      <c r="AH8" s="32"/>
+      <c r="AJ8" s="10" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="C9" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="C9" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="21">
-        <v>0</v>
-      </c>
-      <c r="G9" s="21">
-        <v>0</v>
-      </c>
-      <c r="H9" s="21">
-        <v>0</v>
-      </c>
-      <c r="I9" s="21">
-        <v>0</v>
-      </c>
-      <c r="J9" s="15" t="s">
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="18">
+        <v>0</v>
+      </c>
+      <c r="G9" s="18">
+        <v>0</v>
+      </c>
+      <c r="H9" s="18">
+        <v>0</v>
+      </c>
+      <c r="I9" s="18">
+        <v>0</v>
+      </c>
+      <c r="J9" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="29" t="s">
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="N9" s="31"/>
+      <c r="O9" s="31"/>
+      <c r="P9" s="31"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="31"/>
+      <c r="S9" s="12">
+        <v>0</v>
+      </c>
+      <c r="T9" s="6">
+        <v>0</v>
+      </c>
+      <c r="U9" s="6">
+        <v>0</v>
+      </c>
+      <c r="V9" s="6">
+        <v>0</v>
+      </c>
+      <c r="W9" s="6">
+        <v>0</v>
+      </c>
+      <c r="X9" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="18">
+        <v>1</v>
+      </c>
+      <c r="AD9" s="18">
+        <v>1</v>
+      </c>
+      <c r="AE9" s="18">
+        <v>1</v>
+      </c>
+      <c r="AF9" s="18">
+        <v>1</v>
+      </c>
+      <c r="AG9" s="18">
+        <v>1</v>
+      </c>
+      <c r="AH9" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="AJ9" s="10" t="s">
         <v>167</v>
-      </c>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="29"/>
-      <c r="S9" s="14">
-        <v>0</v>
-      </c>
-      <c r="T9" s="6">
-        <v>0</v>
-      </c>
-      <c r="U9" s="6">
-        <v>0</v>
-      </c>
-      <c r="V9" s="6">
-        <v>0</v>
-      </c>
-      <c r="W9" s="6">
-        <v>0</v>
-      </c>
-      <c r="X9" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="6">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="6">
-        <v>0</v>
-      </c>
-      <c r="AC9" s="21">
-        <v>1</v>
-      </c>
-      <c r="AD9" s="21">
-        <v>1</v>
-      </c>
-      <c r="AE9" s="21">
-        <v>1</v>
-      </c>
-      <c r="AF9" s="21">
-        <v>1</v>
-      </c>
-      <c r="AG9" s="21">
-        <v>1</v>
-      </c>
-      <c r="AH9" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="AJ9" s="12" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C10" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="21">
-        <v>0</v>
-      </c>
-      <c r="G10" s="21">
-        <v>0</v>
-      </c>
-      <c r="H10" s="21">
-        <v>0</v>
-      </c>
-      <c r="I10" s="21">
-        <v>0</v>
-      </c>
-      <c r="J10" s="22" t="s">
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="18">
+        <v>0</v>
+      </c>
+      <c r="G10" s="18">
+        <v>0</v>
+      </c>
+      <c r="H10" s="18">
+        <v>0</v>
+      </c>
+      <c r="I10" s="18">
+        <v>0</v>
+      </c>
+      <c r="J10" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="23" t="s">
-        <v>167</v>
-      </c>
-      <c r="Q10" s="23"/>
-      <c r="R10" s="23"/>
-      <c r="S10" s="14">
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="N10" s="27"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q10" s="28"/>
+      <c r="R10" s="28"/>
+      <c r="S10" s="12">
         <v>0</v>
       </c>
       <c r="T10" s="6">
@@ -1778,64 +1778,64 @@
       <c r="AB10" s="6">
         <v>0</v>
       </c>
-      <c r="AC10" s="21">
-        <v>1</v>
-      </c>
-      <c r="AD10" s="21">
-        <v>0</v>
-      </c>
-      <c r="AE10" s="21">
-        <v>0</v>
-      </c>
-      <c r="AF10" s="21">
-        <v>1</v>
-      </c>
-      <c r="AG10" s="21">
-        <v>0</v>
-      </c>
-      <c r="AH10" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="AJ10" s="12" t="s">
-        <v>171</v>
+      <c r="AC10" s="18">
+        <v>1</v>
+      </c>
+      <c r="AD10" s="18">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="18">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="18">
+        <v>1</v>
+      </c>
+      <c r="AG10" s="18">
+        <v>0</v>
+      </c>
+      <c r="AH10" s="13">
+        <v>0</v>
+      </c>
+      <c r="AJ10" s="10" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="C11" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="C11" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
       <c r="F11" s="6">
         <v>0</v>
       </c>
-      <c r="G11" s="14">
-        <v>0</v>
-      </c>
-      <c r="H11" s="14">
-        <v>0</v>
-      </c>
-      <c r="I11" s="14">
-        <v>0</v>
-      </c>
-      <c r="J11" s="10" t="s">
+      <c r="G11" s="12">
+        <v>0</v>
+      </c>
+      <c r="H11" s="12">
+        <v>0</v>
+      </c>
+      <c r="I11" s="12">
+        <v>0</v>
+      </c>
+      <c r="J11" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10" t="s">
+      <c r="K11" s="29"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="10"/>
+      <c r="N11" s="29"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q11" s="29"/>
+      <c r="R11" s="29"/>
       <c r="S11" s="6">
         <v>0</v>
       </c>
@@ -1875,66 +1875,66 @@
       <c r="AE11" s="6">
         <v>0</v>
       </c>
-      <c r="AF11" s="30" t="s">
-        <v>186</v>
-      </c>
-      <c r="AG11" s="30"/>
-      <c r="AH11" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="AJ11" s="12" t="s">
-        <v>194</v>
+      <c r="AF11" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="AG11" s="24"/>
+      <c r="AH11" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="AJ11" s="10" t="s">
+        <v>187</v>
       </c>
       <c r="AK11" s="2" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C12" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
       <c r="F12" s="6">
         <v>0</v>
       </c>
-      <c r="G12" s="14">
-        <v>0</v>
-      </c>
-      <c r="H12" s="14">
-        <v>0</v>
-      </c>
-      <c r="I12" s="14">
-        <v>0</v>
-      </c>
-      <c r="J12" s="10" t="s">
+      <c r="G12" s="12">
+        <v>0</v>
+      </c>
+      <c r="H12" s="12">
+        <v>0</v>
+      </c>
+      <c r="I12" s="12">
+        <v>0</v>
+      </c>
+      <c r="J12" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10" t="s">
+      <c r="K12" s="29"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="Q12" s="10"/>
-      <c r="R12" s="10"/>
-      <c r="S12" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="T12" s="10"/>
-      <c r="U12" s="10"/>
-      <c r="V12" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="W12" s="10"/>
-      <c r="X12" s="10"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q12" s="29"/>
+      <c r="R12" s="29"/>
+      <c r="S12" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="T12" s="29"/>
+      <c r="U12" s="29"/>
+      <c r="V12" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="W12" s="29"/>
+      <c r="X12" s="29"/>
       <c r="Y12" s="6">
         <v>0</v>
       </c>
@@ -1965,41 +1965,41 @@
       <c r="AH12" s="6">
         <v>0</v>
       </c>
-      <c r="AJ12" s="12" t="s">
-        <v>187</v>
+      <c r="AJ12" s="10" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="C13" s="35" t="s">
-        <v>167</v>
-      </c>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
+        <v>153</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
       <c r="F13" s="6">
         <v>0</v>
       </c>
-      <c r="G13" s="14">
-        <v>0</v>
-      </c>
-      <c r="H13" s="14">
-        <v>0</v>
-      </c>
-      <c r="I13" s="14">
-        <v>1</v>
-      </c>
-      <c r="J13" s="10" t="s">
+      <c r="G13" s="12">
+        <v>0</v>
+      </c>
+      <c r="H13" s="12">
+        <v>0</v>
+      </c>
+      <c r="I13" s="12">
+        <v>1</v>
+      </c>
+      <c r="J13" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10" t="s">
+      <c r="K13" s="29"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
+      <c r="N13" s="29"/>
+      <c r="O13" s="29"/>
       <c r="P13" s="6">
         <v>0</v>
       </c>
@@ -2051,42 +2051,42 @@
       <c r="AF13" s="6">
         <v>0</v>
       </c>
-      <c r="AG13" s="33" t="s">
-        <v>190</v>
-      </c>
-      <c r="AH13" s="33" t="s">
-        <v>107</v>
-      </c>
-      <c r="AJ13" s="12" t="s">
-        <v>191</v>
+      <c r="AG13" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="AH13" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="AJ13" s="10" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="C14" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="C14" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
       <c r="F14" s="6">
         <v>0</v>
       </c>
-      <c r="G14" s="14">
-        <v>0</v>
-      </c>
-      <c r="H14" s="14">
-        <v>0</v>
-      </c>
-      <c r="I14" s="14">
-        <v>1</v>
-      </c>
-      <c r="J14" s="10" t="s">
+      <c r="G14" s="12">
+        <v>0</v>
+      </c>
+      <c r="H14" s="12">
+        <v>0</v>
+      </c>
+      <c r="I14" s="12">
+        <v>1</v>
+      </c>
+      <c r="J14" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
       <c r="M14" s="6">
         <v>0</v>
       </c>
@@ -2102,7 +2102,7 @@
       <c r="Q14" s="6">
         <v>1</v>
       </c>
-      <c r="R14" s="33" t="s">
+      <c r="R14" s="22" t="s">
         <v>10</v>
       </c>
       <c r="S14" s="6">
@@ -2129,46 +2129,46 @@
       <c r="Z14" s="6">
         <v>0</v>
       </c>
-      <c r="AA14" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="AB14" s="10"/>
-      <c r="AC14" s="10"/>
-      <c r="AD14" s="10"/>
-      <c r="AE14" s="10"/>
-      <c r="AF14" s="10"/>
-      <c r="AG14" s="10"/>
-      <c r="AH14" s="10"/>
-      <c r="AJ14" s="12" t="s">
-        <v>157</v>
+      <c r="AA14" s="29" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB14" s="29"/>
+      <c r="AC14" s="29"/>
+      <c r="AD14" s="29"/>
+      <c r="AE14" s="29"/>
+      <c r="AF14" s="29"/>
+      <c r="AG14" s="29"/>
+      <c r="AH14" s="29"/>
+      <c r="AJ14" s="10" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C15" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="C15" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
       <c r="F15" s="6">
         <v>0</v>
       </c>
-      <c r="G15" s="14">
-        <v>0</v>
-      </c>
-      <c r="H15" s="14">
-        <v>0</v>
-      </c>
-      <c r="I15" s="14">
-        <v>1</v>
-      </c>
-      <c r="J15" s="10" t="s">
+      <c r="G15" s="12">
+        <v>0</v>
+      </c>
+      <c r="H15" s="12">
+        <v>0</v>
+      </c>
+      <c r="I15" s="12">
+        <v>1</v>
+      </c>
+      <c r="J15" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
       <c r="M15" s="6">
         <v>0</v>
       </c>
@@ -2184,57 +2184,57 @@
       <c r="Q15" s="6">
         <v>0</v>
       </c>
-      <c r="R15" s="33" t="s">
+      <c r="R15" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="S15" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="T15" s="10"/>
-      <c r="U15" s="10"/>
-      <c r="V15" s="10"/>
-      <c r="W15" s="10"/>
-      <c r="X15" s="10"/>
-      <c r="Y15" s="10"/>
-      <c r="Z15" s="10"/>
-      <c r="AA15" s="10"/>
-      <c r="AB15" s="10"/>
-      <c r="AC15" s="10"/>
-      <c r="AD15" s="10"/>
-      <c r="AE15" s="10"/>
-      <c r="AF15" s="10"/>
-      <c r="AG15" s="10"/>
-      <c r="AH15" s="10"/>
-      <c r="AJ15" s="12" t="s">
-        <v>157</v>
+      <c r="S15" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="T15" s="29"/>
+      <c r="U15" s="29"/>
+      <c r="V15" s="29"/>
+      <c r="W15" s="29"/>
+      <c r="X15" s="29"/>
+      <c r="Y15" s="29"/>
+      <c r="Z15" s="29"/>
+      <c r="AA15" s="29"/>
+      <c r="AB15" s="29"/>
+      <c r="AC15" s="29"/>
+      <c r="AD15" s="29"/>
+      <c r="AE15" s="29"/>
+      <c r="AF15" s="29"/>
+      <c r="AG15" s="29"/>
+      <c r="AH15" s="29"/>
+      <c r="AJ15" s="10" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="C16" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="C16" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
       <c r="F16" s="6">
         <v>0</v>
       </c>
-      <c r="G16" s="14">
-        <v>0</v>
-      </c>
-      <c r="H16" s="14">
-        <v>0</v>
-      </c>
-      <c r="I16" s="14">
-        <v>1</v>
-      </c>
-      <c r="J16" s="10" t="s">
+      <c r="G16" s="12">
+        <v>0</v>
+      </c>
+      <c r="H16" s="12">
+        <v>0</v>
+      </c>
+      <c r="I16" s="12">
+        <v>1</v>
+      </c>
+      <c r="J16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="29"/>
       <c r="M16" s="6">
         <v>0</v>
       </c>
@@ -2250,202 +2250,202 @@
       <c r="Q16" s="6">
         <v>1</v>
       </c>
-      <c r="R16" s="33" t="s">
+      <c r="R16" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="S16" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="T16" s="10"/>
-      <c r="U16" s="10"/>
-      <c r="V16" s="10"/>
-      <c r="W16" s="10"/>
-      <c r="X16" s="10"/>
-      <c r="Y16" s="10"/>
-      <c r="Z16" s="10"/>
-      <c r="AA16" s="10"/>
-      <c r="AB16" s="10"/>
-      <c r="AC16" s="10"/>
-      <c r="AD16" s="10"/>
-      <c r="AE16" s="10"/>
-      <c r="AF16" s="10"/>
-      <c r="AG16" s="10"/>
-      <c r="AH16" s="10"/>
-      <c r="AJ16" s="12" t="s">
-        <v>195</v>
+      <c r="S16" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="T16" s="29"/>
+      <c r="U16" s="29"/>
+      <c r="V16" s="29"/>
+      <c r="W16" s="29"/>
+      <c r="X16" s="29"/>
+      <c r="Y16" s="29"/>
+      <c r="Z16" s="29"/>
+      <c r="AA16" s="29"/>
+      <c r="AB16" s="29"/>
+      <c r="AC16" s="29"/>
+      <c r="AD16" s="29"/>
+      <c r="AE16" s="29"/>
+      <c r="AF16" s="29"/>
+      <c r="AG16" s="29"/>
+      <c r="AH16" s="29"/>
+      <c r="AJ16" s="10" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="C17" s="30" t="s">
+        <v>162</v>
+      </c>
+      <c r="C17" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
       <c r="F17" s="6">
         <v>0</v>
       </c>
-      <c r="G17" s="14">
-        <v>0</v>
-      </c>
-      <c r="H17" s="14">
-        <v>1</v>
-      </c>
-      <c r="I17" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="J17" s="10" t="s">
+      <c r="G17" s="12">
+        <v>0</v>
+      </c>
+      <c r="H17" s="12">
+        <v>1</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="J17" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10" t="s">
+      <c r="K17" s="29"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="10"/>
-      <c r="R17" s="10"/>
-      <c r="S17" s="10"/>
-      <c r="T17" s="10"/>
-      <c r="U17" s="10"/>
-      <c r="V17" s="10"/>
-      <c r="W17" s="10"/>
-      <c r="X17" s="10"/>
-      <c r="Y17" s="10"/>
-      <c r="Z17" s="10"/>
-      <c r="AA17" s="10"/>
-      <c r="AB17" s="10"/>
-      <c r="AC17" s="10"/>
-      <c r="AD17" s="10"/>
-      <c r="AE17" s="10"/>
-      <c r="AF17" s="10"/>
-      <c r="AG17" s="10"/>
-      <c r="AH17" s="10"/>
-      <c r="AJ17" s="12" t="s">
-        <v>196</v>
+      <c r="N17" s="29"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="29"/>
+      <c r="Q17" s="29"/>
+      <c r="R17" s="29"/>
+      <c r="S17" s="29"/>
+      <c r="T17" s="29"/>
+      <c r="U17" s="29"/>
+      <c r="V17" s="29"/>
+      <c r="W17" s="29"/>
+      <c r="X17" s="29"/>
+      <c r="Y17" s="29"/>
+      <c r="Z17" s="29"/>
+      <c r="AA17" s="29"/>
+      <c r="AB17" s="29"/>
+      <c r="AC17" s="29"/>
+      <c r="AD17" s="29"/>
+      <c r="AE17" s="29"/>
+      <c r="AF17" s="29"/>
+      <c r="AG17" s="29"/>
+      <c r="AH17" s="29"/>
+      <c r="AJ17" s="10" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="30" t="s">
+      <c r="C18" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
       <c r="F18" s="6">
         <v>0</v>
       </c>
-      <c r="G18" s="14">
-        <v>1</v>
-      </c>
-      <c r="H18" s="14">
-        <v>0</v>
-      </c>
-      <c r="I18" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="J18" s="10" t="s">
+      <c r="G18" s="12">
+        <v>1</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="J18" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="10"/>
-      <c r="S18" s="10"/>
-      <c r="T18" s="10"/>
-      <c r="U18" s="10"/>
-      <c r="V18" s="10"/>
-      <c r="W18" s="10"/>
-      <c r="X18" s="10"/>
-      <c r="Y18" s="10"/>
-      <c r="Z18" s="10"/>
-      <c r="AA18" s="10"/>
-      <c r="AB18" s="10"/>
-      <c r="AC18" s="10"/>
-      <c r="AD18" s="10"/>
-      <c r="AE18" s="10"/>
-      <c r="AF18" s="10"/>
-      <c r="AG18" s="10"/>
-      <c r="AH18" s="10"/>
-      <c r="AJ18" s="12" t="s">
-        <v>197</v>
+      <c r="K18" s="29"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="N18" s="29"/>
+      <c r="O18" s="29"/>
+      <c r="P18" s="29"/>
+      <c r="Q18" s="29"/>
+      <c r="R18" s="29"/>
+      <c r="S18" s="29"/>
+      <c r="T18" s="29"/>
+      <c r="U18" s="29"/>
+      <c r="V18" s="29"/>
+      <c r="W18" s="29"/>
+      <c r="X18" s="29"/>
+      <c r="Y18" s="29"/>
+      <c r="Z18" s="29"/>
+      <c r="AA18" s="29"/>
+      <c r="AB18" s="29"/>
+      <c r="AC18" s="29"/>
+      <c r="AD18" s="29"/>
+      <c r="AE18" s="29"/>
+      <c r="AF18" s="29"/>
+      <c r="AG18" s="29"/>
+      <c r="AH18" s="29"/>
+      <c r="AJ18" s="10" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="C19" s="30" t="s">
+        <v>190</v>
+      </c>
+      <c r="C19" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
       <c r="F19" s="6">
-        <v>0</v>
-      </c>
-      <c r="G19" s="14">
-        <v>1</v>
-      </c>
-      <c r="H19" s="14">
-        <v>1</v>
-      </c>
-      <c r="I19" s="14">
-        <v>0</v>
-      </c>
-      <c r="J19" s="29" t="s">
-        <v>167</v>
-      </c>
-      <c r="K19" s="29"/>
-      <c r="L19" s="29"/>
-      <c r="M19" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="12">
+        <v>0</v>
+      </c>
+      <c r="H19" s="12">
+        <v>0</v>
+      </c>
+      <c r="I19" s="12">
+        <v>0</v>
+      </c>
+      <c r="J19" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="K19" s="31"/>
+      <c r="L19" s="31"/>
+      <c r="M19" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
-      <c r="Q19" s="10"/>
-      <c r="R19" s="10"/>
-      <c r="S19" s="10"/>
-      <c r="T19" s="10"/>
-      <c r="U19" s="10"/>
-      <c r="V19" s="10"/>
-      <c r="W19" s="10"/>
-      <c r="X19" s="10"/>
-      <c r="Y19" s="10"/>
-      <c r="Z19" s="10"/>
-      <c r="AA19" s="10"/>
-      <c r="AB19" s="10"/>
-      <c r="AC19" s="10"/>
-      <c r="AD19" s="10"/>
-      <c r="AE19" s="10"/>
-      <c r="AF19" s="10"/>
-      <c r="AG19" s="10"/>
-      <c r="AH19" s="10"/>
-      <c r="AJ19" s="12" t="s">
-        <v>212</v>
+      <c r="N19" s="29"/>
+      <c r="O19" s="29"/>
+      <c r="P19" s="29"/>
+      <c r="Q19" s="29"/>
+      <c r="R19" s="29"/>
+      <c r="S19" s="29"/>
+      <c r="T19" s="29"/>
+      <c r="U19" s="29"/>
+      <c r="V19" s="29"/>
+      <c r="W19" s="29"/>
+      <c r="X19" s="29"/>
+      <c r="Y19" s="29"/>
+      <c r="Z19" s="29"/>
+      <c r="AA19" s="29"/>
+      <c r="AB19" s="29"/>
+      <c r="AC19" s="29"/>
+      <c r="AD19" s="29"/>
+      <c r="AE19" s="29"/>
+      <c r="AF19" s="29"/>
+      <c r="AG19" s="29"/>
+      <c r="AH19" s="29"/>
+      <c r="AJ19" s="10" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C20" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
       <c r="F20" s="6">
         <v>1</v>
       </c>
@@ -2458,11 +2458,11 @@
       <c r="I20" s="6">
         <v>1</v>
       </c>
-      <c r="J20" s="10" t="s">
+      <c r="J20" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="29"/>
       <c r="M20" s="6">
         <v>0</v>
       </c>
@@ -2505,29 +2505,29 @@
       <c r="Z20" s="6">
         <v>0</v>
       </c>
-      <c r="AA20" s="10" t="s">
+      <c r="AA20" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB20" s="29"/>
+      <c r="AC20" s="29"/>
+      <c r="AD20" s="29"/>
+      <c r="AE20" s="29"/>
+      <c r="AF20" s="29"/>
+      <c r="AG20" s="29"/>
+      <c r="AH20" s="29"/>
+      <c r="AJ20" s="10" t="s">
         <v>89</v>
-      </c>
-      <c r="AB20" s="10"/>
-      <c r="AC20" s="10"/>
-      <c r="AD20" s="10"/>
-      <c r="AE20" s="10"/>
-      <c r="AF20" s="10"/>
-      <c r="AG20" s="10"/>
-      <c r="AH20" s="10"/>
-      <c r="AJ20" s="12" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C21" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
       <c r="F21" s="6">
         <v>1</v>
       </c>
@@ -2540,11 +2540,11 @@
       <c r="I21" s="6">
         <v>1</v>
       </c>
-      <c r="J21" s="10" t="s">
+      <c r="J21" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
+      <c r="K21" s="29"/>
+      <c r="L21" s="29"/>
       <c r="M21" s="6">
         <v>0</v>
       </c>
@@ -2587,29 +2587,29 @@
       <c r="Z21" s="6">
         <v>1</v>
       </c>
-      <c r="AA21" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="AB21" s="10"/>
-      <c r="AC21" s="10"/>
-      <c r="AD21" s="10"/>
-      <c r="AE21" s="10"/>
-      <c r="AF21" s="10"/>
-      <c r="AG21" s="10"/>
-      <c r="AH21" s="10"/>
-      <c r="AJ21" s="12" t="s">
-        <v>193</v>
+      <c r="AA21" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB21" s="29"/>
+      <c r="AC21" s="29"/>
+      <c r="AD21" s="29"/>
+      <c r="AE21" s="29"/>
+      <c r="AF21" s="29"/>
+      <c r="AG21" s="29"/>
+      <c r="AH21" s="29"/>
+      <c r="AJ21" s="10" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C22" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
       <c r="F22" s="6">
         <v>1</v>
       </c>
@@ -2622,11 +2622,11 @@
       <c r="I22" s="6">
         <v>1</v>
       </c>
-      <c r="J22" s="10" t="s">
+      <c r="J22" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="29"/>
       <c r="M22" s="6">
         <v>0</v>
       </c>
@@ -2693,17 +2693,17 @@
       <c r="AH22" s="6">
         <v>1</v>
       </c>
-      <c r="AJ22" s="12"/>
+      <c r="AJ22" s="10"/>
     </row>
     <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="C23" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
       <c r="F23" s="6">
         <v>1</v>
       </c>
@@ -2767,16 +2767,16 @@
       <c r="Z23" s="6">
         <v>1</v>
       </c>
-      <c r="AA23" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="AB23" s="10"/>
-      <c r="AC23" s="10"/>
-      <c r="AD23" s="10"/>
-      <c r="AE23" s="10"/>
-      <c r="AF23" s="10"/>
-      <c r="AG23" s="10"/>
-      <c r="AH23" s="10"/>
+      <c r="AA23" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB23" s="29"/>
+      <c r="AC23" s="29"/>
+      <c r="AD23" s="29"/>
+      <c r="AE23" s="29"/>
+      <c r="AF23" s="29"/>
+      <c r="AG23" s="29"/>
+      <c r="AH23" s="29"/>
     </row>
     <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
@@ -2813,7 +2813,7 @@
       <c r="AF30" s="6"/>
       <c r="AG30" s="6"/>
       <c r="AH30" s="6"/>
-      <c r="AJ30" s="12"/>
+      <c r="AJ30" s="10"/>
     </row>
     <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
@@ -2850,7 +2850,7 @@
       <c r="AF31" s="6"/>
       <c r="AG31" s="6"/>
       <c r="AH31" s="6"/>
-      <c r="AJ31" s="12"/>
+      <c r="AJ31" s="10"/>
     </row>
     <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
@@ -2887,7 +2887,7 @@
       <c r="AF32" s="6"/>
       <c r="AG32" s="6"/>
       <c r="AH32" s="6"/>
-      <c r="AJ32" s="12"/>
+      <c r="AJ32" s="10"/>
     </row>
     <row r="33" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
@@ -2924,7 +2924,7 @@
       <c r="AF33" s="6"/>
       <c r="AG33" s="6"/>
       <c r="AH33" s="6"/>
-      <c r="AJ33" s="12"/>
+      <c r="AJ33" s="10"/>
     </row>
     <row r="34" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
@@ -2960,7 +2960,7 @@
       <c r="AF34" s="6"/>
       <c r="AG34" s="6"/>
       <c r="AH34" s="6"/>
-      <c r="AJ34" s="12"/>
+      <c r="AJ34" s="10"/>
     </row>
     <row r="35" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
@@ -2996,7 +2996,7 @@
       <c r="AF35" s="6"/>
       <c r="AG35" s="6"/>
       <c r="AH35" s="6"/>
-      <c r="AJ35" s="12"/>
+      <c r="AJ35" s="10"/>
     </row>
     <row r="36" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
@@ -3032,7 +3032,7 @@
       <c r="AF36" s="6"/>
       <c r="AG36" s="6"/>
       <c r="AH36" s="6"/>
-      <c r="AJ36" s="12"/>
+      <c r="AJ36" s="10"/>
     </row>
     <row r="37" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
@@ -3068,7 +3068,7 @@
       <c r="AF37" s="6"/>
       <c r="AG37" s="6"/>
       <c r="AH37" s="6"/>
-      <c r="AJ37" s="12"/>
+      <c r="AJ37" s="10"/>
     </row>
     <row r="38" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
@@ -3104,7 +3104,7 @@
       <c r="AF38" s="6"/>
       <c r="AG38" s="6"/>
       <c r="AH38" s="6"/>
-      <c r="AJ38" s="12"/>
+      <c r="AJ38" s="10"/>
     </row>
     <row r="39" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
@@ -3140,7 +3140,7 @@
       <c r="AF39" s="6"/>
       <c r="AG39" s="6"/>
       <c r="AH39" s="6"/>
-      <c r="AJ39" s="12"/>
+      <c r="AJ39" s="10"/>
     </row>
     <row r="40" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
@@ -3176,7 +3176,7 @@
       <c r="AF40" s="6"/>
       <c r="AG40" s="6"/>
       <c r="AH40" s="6"/>
-      <c r="AJ40" s="12"/>
+      <c r="AJ40" s="10"/>
     </row>
     <row r="41" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
@@ -3212,7 +3212,7 @@
       <c r="AF41" s="6"/>
       <c r="AG41" s="6"/>
       <c r="AH41" s="6"/>
-      <c r="AJ41" s="12"/>
+      <c r="AJ41" s="10"/>
     </row>
     <row r="42" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
@@ -3248,7 +3248,7 @@
       <c r="AF42" s="6"/>
       <c r="AG42" s="6"/>
       <c r="AH42" s="6"/>
-      <c r="AJ42" s="12"/>
+      <c r="AJ42" s="10"/>
     </row>
     <row r="43" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
@@ -3284,7 +3284,7 @@
       <c r="AF43" s="6"/>
       <c r="AG43" s="6"/>
       <c r="AH43" s="6"/>
-      <c r="AJ43" s="12"/>
+      <c r="AJ43" s="10"/>
     </row>
     <row r="44" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
@@ -3320,7 +3320,7 @@
       <c r="AF44" s="6"/>
       <c r="AG44" s="6"/>
       <c r="AH44" s="6"/>
-      <c r="AJ44" s="12"/>
+      <c r="AJ44" s="10"/>
     </row>
     <row r="45" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
@@ -3362,26 +3362,23 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="P10:R10"/>
-    <mergeCell ref="AF11:AG11"/>
-    <mergeCell ref="V12:X12"/>
+    <mergeCell ref="AC8:AH8"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="P8:R8"/>
+    <mergeCell ref="AA20:AH20"/>
+    <mergeCell ref="AA23:AH23"/>
+    <mergeCell ref="M17:AH17"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="P11:R11"/>
+    <mergeCell ref="M19:AH19"/>
+    <mergeCell ref="M18:AH18"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="S16:AH16"/>
+    <mergeCell ref="J19:L19"/>
     <mergeCell ref="J9:L9"/>
     <mergeCell ref="M9:R9"/>
     <mergeCell ref="J21:L21"/>
@@ -3396,26 +3393,29 @@
     <mergeCell ref="M12:O12"/>
     <mergeCell ref="P12:R12"/>
     <mergeCell ref="S12:U12"/>
-    <mergeCell ref="C19:E19"/>
     <mergeCell ref="J15:L15"/>
     <mergeCell ref="S15:AH15"/>
-    <mergeCell ref="AA23:AH23"/>
-    <mergeCell ref="M17:AH17"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="M11:O11"/>
-    <mergeCell ref="P11:R11"/>
-    <mergeCell ref="M19:AH19"/>
-    <mergeCell ref="M18:AH18"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="S16:AH16"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="AC8:AH8"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="P8:R8"/>
-    <mergeCell ref="AA20:AH20"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="P10:R10"/>
+    <mergeCell ref="AF11:AG11"/>
+    <mergeCell ref="V12:X12"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C19:E19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3427,7 +3427,7 @@
   <dimension ref="A1:O42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3443,12 +3443,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
@@ -3458,20 +3458,20 @@
       <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="25" t="s">
-        <v>172</v>
+      <c r="A2" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="20" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3502,16 +3502,16 @@
         <v>14</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="O3" s="34" t="s">
-        <v>200</v>
+        <v>191</v>
+      </c>
+      <c r="O3" s="23" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -3541,16 +3541,16 @@
         <v>18</v>
       </c>
       <c r="K4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="N4" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="O4" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -3577,24 +3577,24 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="N5" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="O5" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6">
@@ -3616,24 +3616,24 @@
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L6" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="N6" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="O6" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6">
@@ -3655,24 +3655,24 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="L7" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="N7" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="O7" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6">
@@ -3694,15 +3694,15 @@
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6">
@@ -3724,21 +3724,21 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="K9" t="s">
-        <v>180</v>
+        <v>207</v>
       </c>
       <c r="L9" t="s">
-        <v>176</v>
-      </c>
-      <c r="N9" s="24" t="s">
-        <v>213</v>
+        <v>172</v>
+      </c>
+      <c r="N9" s="19" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6">
@@ -3760,21 +3760,21 @@
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="K10" t="s">
-        <v>184</v>
+        <v>208</v>
       </c>
       <c r="L10" t="s">
-        <v>175</v>
-      </c>
-      <c r="N10" s="24" t="s">
-        <v>214</v>
+        <v>171</v>
+      </c>
+      <c r="N10" s="19" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6">
@@ -3796,15 +3796,15 @@
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>83</v>
-      </c>
-      <c r="N11" s="24" t="s">
-        <v>209</v>
+        <v>81</v>
+      </c>
+      <c r="N11" s="19" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6">
@@ -3826,10 +3826,10 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>85</v>
-      </c>
-      <c r="N12" s="24" t="s">
-        <v>210</v>
+        <v>83</v>
+      </c>
+      <c r="N12" s="19" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -3856,13 +3856,13 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K13" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="L13" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -3889,13 +3889,13 @@
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K14" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L14" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -3922,13 +3922,13 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="L15" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -3955,13 +3955,13 @@
         <v>0</v>
       </c>
       <c r="J16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="L16" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -3988,13 +3988,13 @@
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K17" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="L17" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -4021,13 +4021,13 @@
         <v>0</v>
       </c>
       <c r="J18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K18" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L18" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -4054,13 +4054,13 @@
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K19" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="L19" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -4087,13 +4087,13 @@
         <v>0</v>
       </c>
       <c r="J20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L20" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -4120,13 +4120,13 @@
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K21" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L21" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -4153,13 +4153,13 @@
         <v>0</v>
       </c>
       <c r="J22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K22" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="L22" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -4186,13 +4186,13 @@
         <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K23" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L23" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -4219,13 +4219,13 @@
         <v>0</v>
       </c>
       <c r="J24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K24" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L24" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -4252,13 +4252,13 @@
         <v>0</v>
       </c>
       <c r="J25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K25" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="L25" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -4285,13 +4285,13 @@
         <v>1</v>
       </c>
       <c r="J26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K26" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="L26" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -4318,13 +4318,13 @@
         <v>0</v>
       </c>
       <c r="J27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K27" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L27" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -4351,13 +4351,13 @@
         <v>1</v>
       </c>
       <c r="J28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K28" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="L28" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -4384,13 +4384,13 @@
         <v>0</v>
       </c>
       <c r="J29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K29" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L29" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -4417,13 +4417,13 @@
         <v>1</v>
       </c>
       <c r="J30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K30" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="L30" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -4450,13 +4450,13 @@
         <v>0</v>
       </c>
       <c r="J31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K31" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L31" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -4483,18 +4483,18 @@
         <v>1</v>
       </c>
       <c r="J32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K32" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="L32" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>41</v>
+        <v>211</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="6">
@@ -4516,18 +4516,18 @@
         <v>0</v>
       </c>
       <c r="J33" t="s">
-        <v>70</v>
+        <v>209</v>
       </c>
       <c r="K33" t="s">
-        <v>127</v>
+        <v>210</v>
       </c>
       <c r="L33" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="6">
@@ -4549,18 +4549,18 @@
         <v>1</v>
       </c>
       <c r="J34" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K34" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="L34" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="6">
@@ -4582,18 +4582,18 @@
         <v>0</v>
       </c>
       <c r="J35" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K35" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="L35" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="6">
@@ -4615,18 +4615,18 @@
         <v>1</v>
       </c>
       <c r="J36" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K36" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="L36" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="6">
@@ -4648,18 +4648,18 @@
         <v>0</v>
       </c>
       <c r="J37" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K37" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="L37" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B38" s="6"/>
       <c r="C38" s="6">
@@ -4681,18 +4681,18 @@
         <v>1</v>
       </c>
       <c r="J38" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K38" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="L38" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="6">
@@ -4714,18 +4714,18 @@
         <v>0</v>
       </c>
       <c r="J39" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K39" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="L39" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B40" s="6"/>
       <c r="C40" s="6">
@@ -4747,44 +4747,41 @@
         <v>1</v>
       </c>
       <c r="J40" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K40" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L40" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="B41" s="16"/>
-      <c r="C41" s="16">
-        <v>0</v>
-      </c>
-      <c r="D41" s="16">
-        <v>0</v>
-      </c>
-      <c r="E41" s="16">
-        <v>0</v>
-      </c>
-      <c r="F41" s="16">
-        <v>0</v>
-      </c>
-      <c r="G41" s="16">
-        <v>0</v>
-      </c>
-      <c r="H41" s="16">
-        <v>0</v>
-      </c>
-      <c r="I41" s="20"/>
-      <c r="J41" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="K41" t="s">
-        <v>181</v>
+      <c r="A41" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" s="14"/>
+      <c r="C41" s="14">
+        <v>0</v>
+      </c>
+      <c r="D41" s="14">
+        <v>0</v>
+      </c>
+      <c r="E41" s="14">
+        <v>0</v>
+      </c>
+      <c r="F41" s="14">
+        <v>0</v>
+      </c>
+      <c r="G41" s="14">
+        <v>0</v>
+      </c>
+      <c r="H41" s="14">
+        <v>0</v>
+      </c>
+      <c r="I41" s="17"/>
+      <c r="J41" s="17" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -4825,7 +4822,7 @@
   <sheetData>
     <row r="1" spans="1:36" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -4966,43 +4963,43 @@
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
-      <c r="U4" s="11"/>
-      <c r="V4" s="11"/>
-      <c r="W4" s="11"/>
-      <c r="X4" s="11"/>
-      <c r="Y4" s="11"/>
-      <c r="Z4" s="11"/>
-      <c r="AA4" s="11"/>
-      <c r="AB4" s="11"/>
-      <c r="AC4" s="11"/>
-      <c r="AD4" s="11"/>
-      <c r="AE4" s="11"/>
-      <c r="AF4" s="11"/>
-      <c r="AG4" s="11"/>
-      <c r="AH4" s="11"/>
-      <c r="AJ4" s="12"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="32"/>
+      <c r="S4" s="32"/>
+      <c r="T4" s="32"/>
+      <c r="U4" s="32"/>
+      <c r="V4" s="32"/>
+      <c r="W4" s="32"/>
+      <c r="X4" s="32"/>
+      <c r="Y4" s="32"/>
+      <c r="Z4" s="32"/>
+      <c r="AA4" s="32"/>
+      <c r="AB4" s="32"/>
+      <c r="AC4" s="32"/>
+      <c r="AD4" s="32"/>
+      <c r="AE4" s="32"/>
+      <c r="AF4" s="32"/>
+      <c r="AG4" s="32"/>
+      <c r="AH4" s="32"/>
+      <c r="AJ4" s="10"/>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C5" s="6">
         <v>0</v>
@@ -5016,106 +5013,106 @@
       <c r="F5" s="6">
         <v>0</v>
       </c>
-      <c r="G5" s="14">
-        <v>0</v>
-      </c>
-      <c r="H5" s="14">
-        <v>0</v>
-      </c>
-      <c r="I5" s="14">
+      <c r="G5" s="12">
+        <v>0</v>
+      </c>
+      <c r="H5" s="12">
+        <v>0</v>
+      </c>
+      <c r="I5" s="12">
         <v>0</v>
       </c>
       <c r="J5" s="6">
         <v>1</v>
       </c>
-      <c r="K5" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
-      <c r="U5" s="10"/>
-      <c r="V5" s="10"/>
-      <c r="W5" s="10"/>
-      <c r="X5" s="10"/>
-      <c r="Y5" s="10"/>
-      <c r="Z5" s="10"/>
-      <c r="AA5" s="10"/>
-      <c r="AB5" s="10"/>
-      <c r="AC5" s="10"/>
-      <c r="AD5" s="10"/>
-      <c r="AE5" s="10"/>
-      <c r="AF5" s="10"/>
-      <c r="AG5" s="10"/>
-      <c r="AH5" s="10"/>
-      <c r="AJ5" s="12"/>
+      <c r="K5" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="29"/>
+      <c r="U5" s="29"/>
+      <c r="V5" s="29"/>
+      <c r="W5" s="29"/>
+      <c r="X5" s="29"/>
+      <c r="Y5" s="29"/>
+      <c r="Z5" s="29"/>
+      <c r="AA5" s="29"/>
+      <c r="AB5" s="29"/>
+      <c r="AC5" s="29"/>
+      <c r="AD5" s="29"/>
+      <c r="AE5" s="29"/>
+      <c r="AF5" s="29"/>
+      <c r="AG5" s="29"/>
+      <c r="AH5" s="29"/>
+      <c r="AJ5" s="10"/>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="12">
+        <v>0</v>
+      </c>
+      <c r="I6" s="12">
+        <v>1</v>
+      </c>
+      <c r="J6" s="6">
+        <v>0</v>
+      </c>
+      <c r="K6" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="C6" s="6">
-        <v>0</v>
-      </c>
-      <c r="D6" s="6">
-        <v>0</v>
-      </c>
-      <c r="E6" s="6">
-        <v>0</v>
-      </c>
-      <c r="F6" s="6">
-        <v>0</v>
-      </c>
-      <c r="G6" s="6">
-        <v>0</v>
-      </c>
-      <c r="H6" s="14">
-        <v>0</v>
-      </c>
-      <c r="I6" s="14">
-        <v>1</v>
-      </c>
-      <c r="J6" s="6">
-        <v>0</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
-      <c r="V6" s="10"/>
-      <c r="W6" s="10"/>
-      <c r="X6" s="10"/>
-      <c r="Y6" s="10"/>
-      <c r="Z6" s="10"/>
-      <c r="AA6" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="AB6" s="10"/>
-      <c r="AC6" s="10"/>
-      <c r="AD6" s="10"/>
-      <c r="AE6" s="10"/>
-      <c r="AF6" s="10"/>
-      <c r="AG6" s="10"/>
-      <c r="AH6" s="10"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="29"/>
+      <c r="S6" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="T6" s="29"/>
+      <c r="U6" s="29"/>
+      <c r="V6" s="29"/>
+      <c r="W6" s="29"/>
+      <c r="X6" s="29"/>
+      <c r="Y6" s="29"/>
+      <c r="Z6" s="29"/>
+      <c r="AA6" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB6" s="29"/>
+      <c r="AC6" s="29"/>
+      <c r="AD6" s="29"/>
+      <c r="AE6" s="29"/>
+      <c r="AF6" s="29"/>
+      <c r="AG6" s="29"/>
+      <c r="AH6" s="29"/>
       <c r="AI6" s="6"/>
-      <c r="AJ6" s="12"/>
+      <c r="AJ6" s="10"/>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
@@ -5123,9 +5120,9 @@
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
       <c r="J7" s="6"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
@@ -5151,7 +5148,7 @@
       <c r="AF7" s="5"/>
       <c r="AG7" s="5"/>
       <c r="AH7" s="5"/>
-      <c r="AJ7" s="12"/>
+      <c r="AJ7" s="10"/>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
@@ -5159,9 +5156,9 @@
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
       <c r="J8" s="6"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -5187,7 +5184,7 @@
       <c r="AF8" s="5"/>
       <c r="AG8" s="5"/>
       <c r="AH8" s="5"/>
-      <c r="AJ8" s="12"/>
+      <c r="AJ8" s="10"/>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
@@ -5195,9 +5192,9 @@
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
       <c r="J9" s="6"/>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
@@ -5223,7 +5220,7 @@
       <c r="AF9" s="5"/>
       <c r="AG9" s="5"/>
       <c r="AH9" s="5"/>
-      <c r="AJ9" s="12"/>
+      <c r="AJ9" s="10"/>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
@@ -5231,9 +5228,9 @@
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
       <c r="J10" s="6"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -5259,7 +5256,7 @@
       <c r="AF10" s="5"/>
       <c r="AG10" s="5"/>
       <c r="AH10" s="5"/>
-      <c r="AJ10" s="12"/>
+      <c r="AJ10" s="10"/>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
@@ -5267,9 +5264,9 @@
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
       <c r="J11" s="6"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
@@ -5295,7 +5292,7 @@
       <c r="AF11" s="5"/>
       <c r="AG11" s="5"/>
       <c r="AH11" s="5"/>
-      <c r="AJ11" s="12"/>
+      <c r="AJ11" s="10"/>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
@@ -5303,9 +5300,9 @@
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
@@ -5331,7 +5328,7 @@
       <c r="AF12" s="6"/>
       <c r="AG12" s="6"/>
       <c r="AH12" s="6"/>
-      <c r="AJ12" s="12"/>
+      <c r="AJ12" s="10"/>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
@@ -5339,9 +5336,9 @@
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
@@ -5367,7 +5364,7 @@
       <c r="AF13" s="6"/>
       <c r="AG13" s="6"/>
       <c r="AH13" s="6"/>
-      <c r="AJ13" s="12"/>
+      <c r="AJ13" s="10"/>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
@@ -5403,7 +5400,7 @@
       <c r="AF14" s="5"/>
       <c r="AG14" s="5"/>
       <c r="AH14" s="5"/>
-      <c r="AJ14" s="12"/>
+      <c r="AJ14" s="10"/>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
@@ -5439,7 +5436,7 @@
       <c r="AF15" s="5"/>
       <c r="AG15" s="5"/>
       <c r="AH15" s="5"/>
-      <c r="AJ15" s="12"/>
+      <c r="AJ15" s="10"/>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
@@ -5475,7 +5472,7 @@
       <c r="AF16" s="6"/>
       <c r="AG16" s="6"/>
       <c r="AH16" s="6"/>
-      <c r="AJ16" s="12"/>
+      <c r="AJ16" s="10"/>
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
@@ -5549,7 +5546,7 @@
       <c r="AF19" s="6"/>
       <c r="AG19" s="6"/>
       <c r="AH19" s="6"/>
-      <c r="AJ19" s="12"/>
+      <c r="AJ19" s="10"/>
     </row>
     <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="J20" s="6"/>
@@ -5589,7 +5586,7 @@
       <c r="AF21" s="6"/>
       <c r="AG21" s="6"/>
       <c r="AH21" s="6"/>
-      <c r="AJ21" s="12"/>
+      <c r="AJ21" s="10"/>
     </row>
     <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
@@ -5626,7 +5623,7 @@
       <c r="AF22" s="6"/>
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
-      <c r="AJ22" s="12"/>
+      <c r="AJ22" s="10"/>
     </row>
     <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
@@ -5663,7 +5660,7 @@
       <c r="AF23" s="6"/>
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
-      <c r="AJ23" s="12"/>
+      <c r="AJ23" s="10"/>
     </row>
     <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
@@ -5700,7 +5697,7 @@
       <c r="AF24" s="6"/>
       <c r="AG24" s="6"/>
       <c r="AH24" s="6"/>
-      <c r="AJ24" s="12"/>
+      <c r="AJ24" s="10"/>
     </row>
     <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
@@ -5737,7 +5734,7 @@
       <c r="AF25" s="6"/>
       <c r="AG25" s="6"/>
       <c r="AH25" s="6"/>
-      <c r="AJ25" s="12"/>
+      <c r="AJ25" s="10"/>
     </row>
     <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
@@ -5774,7 +5771,7 @@
       <c r="AF26" s="6"/>
       <c r="AG26" s="6"/>
       <c r="AH26" s="6"/>
-      <c r="AJ26" s="12"/>
+      <c r="AJ26" s="10"/>
     </row>
     <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
@@ -5811,7 +5808,7 @@
       <c r="AF27" s="6"/>
       <c r="AG27" s="6"/>
       <c r="AH27" s="6"/>
-      <c r="AJ27" s="12"/>
+      <c r="AJ27" s="10"/>
     </row>
     <row r="28" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
@@ -5847,7 +5844,7 @@
       <c r="AF28" s="6"/>
       <c r="AG28" s="6"/>
       <c r="AH28" s="6"/>
-      <c r="AJ28" s="12"/>
+      <c r="AJ28" s="10"/>
     </row>
     <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
@@ -5883,7 +5880,7 @@
       <c r="AF29" s="6"/>
       <c r="AG29" s="6"/>
       <c r="AH29" s="6"/>
-      <c r="AJ29" s="12"/>
+      <c r="AJ29" s="10"/>
     </row>
     <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
@@ -5919,7 +5916,7 @@
       <c r="AF30" s="6"/>
       <c r="AG30" s="6"/>
       <c r="AH30" s="6"/>
-      <c r="AJ30" s="12"/>
+      <c r="AJ30" s="10"/>
     </row>
     <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
@@ -5955,7 +5952,7 @@
       <c r="AF31" s="6"/>
       <c r="AG31" s="6"/>
       <c r="AH31" s="6"/>
-      <c r="AJ31" s="12"/>
+      <c r="AJ31" s="10"/>
     </row>
     <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
@@ -5991,7 +5988,7 @@
       <c r="AF32" s="6"/>
       <c r="AG32" s="6"/>
       <c r="AH32" s="6"/>
-      <c r="AJ32" s="12"/>
+      <c r="AJ32" s="10"/>
     </row>
     <row r="33" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
@@ -6027,7 +6024,7 @@
       <c r="AF33" s="6"/>
       <c r="AG33" s="6"/>
       <c r="AH33" s="6"/>
-      <c r="AJ33" s="12"/>
+      <c r="AJ33" s="10"/>
     </row>
     <row r="34" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
@@ -6063,7 +6060,7 @@
       <c r="AF34" s="6"/>
       <c r="AG34" s="6"/>
       <c r="AH34" s="6"/>
-      <c r="AJ34" s="12"/>
+      <c r="AJ34" s="10"/>
     </row>
     <row r="35" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
@@ -6099,7 +6096,7 @@
       <c r="AF35" s="6"/>
       <c r="AG35" s="6"/>
       <c r="AH35" s="6"/>
-      <c r="AJ35" s="12"/>
+      <c r="AJ35" s="10"/>
     </row>
     <row r="36" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
@@ -6135,7 +6132,7 @@
       <c r="AF36" s="6"/>
       <c r="AG36" s="6"/>
       <c r="AH36" s="6"/>
-      <c r="AJ36" s="12"/>
+      <c r="AJ36" s="10"/>
     </row>
     <row r="37" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
@@ -6171,7 +6168,7 @@
       <c r="AF37" s="6"/>
       <c r="AG37" s="6"/>
       <c r="AH37" s="6"/>
-      <c r="AJ37" s="12"/>
+      <c r="AJ37" s="10"/>
     </row>
     <row r="38" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
@@ -6207,7 +6204,7 @@
       <c r="AF38" s="6"/>
       <c r="AG38" s="6"/>
       <c r="AH38" s="6"/>
-      <c r="AJ38" s="12"/>
+      <c r="AJ38" s="10"/>
     </row>
     <row r="39" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
@@ -6279,7 +6276,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -6354,34 +6351,34 @@
         <v>0</v>
       </c>
       <c r="T3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="T4" s="12" t="s">
-        <v>146</v>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="32"/>
+      <c r="T4" s="10" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C5" s="6">
         <v>0</v>
@@ -6429,15 +6426,15 @@
         <v>0</v>
       </c>
       <c r="R5" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="T5" s="12" t="s">
-        <v>153</v>
+        <v>142</v>
+      </c>
+      <c r="T5" s="10" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C6" s="6">
         <v>0</v>
@@ -6463,21 +6460,21 @@
       <c r="J6" s="6">
         <v>1</v>
       </c>
-      <c r="K6" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="T6" s="12"/>
+      <c r="K6" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="29"/>
+      <c r="T6" s="10"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C7" s="6">
         <v>0</v>
@@ -6501,23 +6498,23 @@
         <v>1</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="K7" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="10"/>
-      <c r="T7" s="12"/>
+        <v>145</v>
+      </c>
+      <c r="K7" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="29"/>
+      <c r="T7" s="10"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C8" s="6">
         <v>0</v>
@@ -6541,23 +6538,23 @@
         <v>0</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="K8" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
-      <c r="T8" s="12"/>
+        <v>145</v>
+      </c>
+      <c r="K8" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="29"/>
+      <c r="R8" s="29"/>
+      <c r="T8" s="10"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C9" s="6">
         <v>0</v>
@@ -6581,19 +6578,19 @@
         <v>1</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="K9" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
-      <c r="T9" s="12"/>
+        <v>145</v>
+      </c>
+      <c r="K9" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="29"/>
+      <c r="T9" s="10"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
@@ -6613,7 +6610,7 @@
       <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
-      <c r="T10" s="12"/>
+      <c r="T10" s="10"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
@@ -6633,7 +6630,7 @@
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
       <c r="R11" s="6"/>
-      <c r="T11" s="12"/>
+      <c r="T11" s="10"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
@@ -6653,7 +6650,7 @@
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>
-      <c r="T12" s="12"/>
+      <c r="T12" s="10"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
@@ -6673,7 +6670,7 @@
       <c r="P13" s="6"/>
       <c r="Q13" s="6"/>
       <c r="R13" s="6"/>
-      <c r="T13" s="12"/>
+      <c r="T13" s="10"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
@@ -6693,7 +6690,7 @@
       <c r="P14" s="6"/>
       <c r="Q14" s="6"/>
       <c r="R14" s="6"/>
-      <c r="T14" s="12"/>
+      <c r="T14" s="10"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
@@ -6713,7 +6710,7 @@
       <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
       <c r="R15" s="6"/>
-      <c r="T15" s="12"/>
+      <c r="T15" s="10"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
@@ -6733,7 +6730,7 @@
       <c r="P16" s="6"/>
       <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
-      <c r="T16" s="12"/>
+      <c r="T16" s="10"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
@@ -6753,7 +6750,7 @@
       <c r="P17" s="6"/>
       <c r="Q17" s="6"/>
       <c r="R17" s="6"/>
-      <c r="T17" s="12"/>
+      <c r="T17" s="10"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
@@ -6775,22 +6772,22 @@
       <c r="R18" s="6"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="14"/>
-      <c r="Q19" s="14"/>
-      <c r="R19" s="14"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="12"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
@@ -6810,25 +6807,25 @@
       <c r="P20" s="6"/>
       <c r="Q20" s="6"/>
       <c r="R20" s="6"/>
-      <c r="T20" s="12"/>
+      <c r="T20" s="10"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="14"/>
-      <c r="R21" s="14"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="12"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
@@ -6849,7 +6846,7 @@
       <c r="P22" s="6"/>
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
-      <c r="T22" s="12"/>
+      <c r="T22" s="10"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
@@ -6870,7 +6867,7 @@
       <c r="P23" s="6"/>
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
-      <c r="T23" s="12"/>
+      <c r="T23" s="10"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
@@ -6891,7 +6888,7 @@
       <c r="P24" s="6"/>
       <c r="Q24" s="6"/>
       <c r="R24" s="6"/>
-      <c r="T24" s="12"/>
+      <c r="T24" s="10"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
@@ -6912,7 +6909,7 @@
       <c r="P25" s="6"/>
       <c r="Q25" s="6"/>
       <c r="R25" s="6"/>
-      <c r="T25" s="12"/>
+      <c r="T25" s="10"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
@@ -6933,7 +6930,7 @@
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
       <c r="R26" s="6"/>
-      <c r="T26" s="12"/>
+      <c r="T26" s="10"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
@@ -6954,7 +6951,7 @@
       <c r="P27" s="6"/>
       <c r="Q27" s="6"/>
       <c r="R27" s="6"/>
-      <c r="T27" s="12"/>
+      <c r="T27" s="10"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
@@ -6975,7 +6972,7 @@
       <c r="P28" s="6"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="6"/>
-      <c r="T28" s="12"/>
+      <c r="T28" s="10"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
@@ -6995,7 +6992,7 @@
       <c r="P29" s="6"/>
       <c r="Q29" s="6"/>
       <c r="R29" s="6"/>
-      <c r="T29" s="12"/>
+      <c r="T29" s="10"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
@@ -7015,7 +7012,7 @@
       <c r="P30" s="6"/>
       <c r="Q30" s="6"/>
       <c r="R30" s="6"/>
-      <c r="T30" s="12"/>
+      <c r="T30" s="10"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
@@ -7035,7 +7032,7 @@
       <c r="P31" s="6"/>
       <c r="Q31" s="6"/>
       <c r="R31" s="6"/>
-      <c r="T31" s="12"/>
+      <c r="T31" s="10"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
@@ -7055,7 +7052,7 @@
       <c r="P32" s="6"/>
       <c r="Q32" s="6"/>
       <c r="R32" s="6"/>
-      <c r="T32" s="12"/>
+      <c r="T32" s="10"/>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
@@ -7075,7 +7072,7 @@
       <c r="P33" s="6"/>
       <c r="Q33" s="6"/>
       <c r="R33" s="6"/>
-      <c r="T33" s="12"/>
+      <c r="T33" s="10"/>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
@@ -7095,7 +7092,7 @@
       <c r="P34" s="6"/>
       <c r="Q34" s="6"/>
       <c r="R34" s="6"/>
-      <c r="T34" s="12"/>
+      <c r="T34" s="10"/>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
@@ -7115,7 +7112,7 @@
       <c r="P35" s="6"/>
       <c r="Q35" s="6"/>
       <c r="R35" s="6"/>
-      <c r="T35" s="12"/>
+      <c r="T35" s="10"/>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
@@ -7135,7 +7132,7 @@
       <c r="P36" s="6"/>
       <c r="Q36" s="6"/>
       <c r="R36" s="6"/>
-      <c r="T36" s="12"/>
+      <c r="T36" s="10"/>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
@@ -7155,7 +7152,7 @@
       <c r="P37" s="6"/>
       <c r="Q37" s="6"/>
       <c r="R37" s="6"/>
-      <c r="T37" s="12"/>
+      <c r="T37" s="10"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
@@ -7175,7 +7172,7 @@
       <c r="P38" s="6"/>
       <c r="Q38" s="6"/>
       <c r="R38" s="6"/>
-      <c r="T38" s="12"/>
+      <c r="T38" s="10"/>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
@@ -7195,7 +7192,7 @@
       <c r="P39" s="6"/>
       <c r="Q39" s="6"/>
       <c r="R39" s="6"/>
-      <c r="T39" s="12"/>
+      <c r="T39" s="10"/>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>

</xml_diff>

<commit_message>
CMP now takes conditions
</commit_message>
<xml_diff>
--- a/doc/RiscyInstSet32Bit.xlsx
+++ b/doc/RiscyInstSet32Bit.xlsx
@@ -876,7 +876,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="6" applyFont="1"/>
@@ -932,9 +932,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
@@ -1259,8 +1256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="AJ19" sqref="AJ19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1552,11 +1549,11 @@
       <c r="A8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
       <c r="F8" s="11">
         <v>0</v>
       </c>
@@ -1569,21 +1566,21 @@
       <c r="I8" s="11">
         <v>0</v>
       </c>
-      <c r="J8" s="32" t="s">
+      <c r="J8" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="32"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32" t="s">
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="N8" s="32"/>
-      <c r="O8" s="32"/>
-      <c r="P8" s="32" t="s">
+      <c r="N8" s="31"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="Q8" s="32"/>
-      <c r="R8" s="32"/>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="31"/>
       <c r="S8" s="12">
         <v>0</v>
       </c>
@@ -1614,14 +1611,14 @@
       <c r="AB8" s="6">
         <v>0</v>
       </c>
-      <c r="AC8" s="32" t="s">
+      <c r="AC8" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="AD8" s="32"/>
-      <c r="AE8" s="32"/>
-      <c r="AF8" s="32"/>
-      <c r="AG8" s="32"/>
-      <c r="AH8" s="32"/>
+      <c r="AD8" s="31"/>
+      <c r="AE8" s="31"/>
+      <c r="AF8" s="31"/>
+      <c r="AG8" s="31"/>
+      <c r="AH8" s="31"/>
       <c r="AJ8" s="10" t="s">
         <v>165</v>
       </c>
@@ -1647,19 +1644,19 @@
       <c r="I9" s="18">
         <v>0</v>
       </c>
-      <c r="J9" s="30" t="s">
+      <c r="J9" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="31" t="s">
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="30" t="s">
         <v>164</v>
       </c>
-      <c r="N9" s="31"/>
-      <c r="O9" s="31"/>
-      <c r="P9" s="31"/>
-      <c r="Q9" s="31"/>
-      <c r="R9" s="31"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="30"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="30"/>
+      <c r="R9" s="30"/>
       <c r="S9" s="12">
         <v>0</v>
       </c>
@@ -1733,21 +1730,21 @@
       <c r="I10" s="18">
         <v>0</v>
       </c>
-      <c r="J10" s="27" t="s">
+      <c r="J10" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="27" t="s">
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="N10" s="27"/>
-      <c r="O10" s="27"/>
-      <c r="P10" s="28" t="s">
+      <c r="N10" s="26"/>
+      <c r="O10" s="26"/>
+      <c r="P10" s="27" t="s">
         <v>164</v>
       </c>
-      <c r="Q10" s="28"/>
-      <c r="R10" s="28"/>
+      <c r="Q10" s="27"/>
+      <c r="R10" s="27"/>
       <c r="S10" s="12">
         <v>0</v>
       </c>
@@ -1821,21 +1818,21 @@
       <c r="I11" s="12">
         <v>0</v>
       </c>
-      <c r="J11" s="29" t="s">
+      <c r="J11" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="K11" s="29"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="29" t="s">
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="N11" s="29"/>
-      <c r="O11" s="29"/>
-      <c r="P11" s="29" t="s">
+      <c r="N11" s="28"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="Q11" s="29"/>
-      <c r="R11" s="29"/>
+      <c r="Q11" s="28"/>
+      <c r="R11" s="28"/>
       <c r="S11" s="6">
         <v>0</v>
       </c>
@@ -1910,31 +1907,31 @@
       <c r="I12" s="12">
         <v>0</v>
       </c>
-      <c r="J12" s="29" t="s">
+      <c r="J12" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29" t="s">
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29" t="s">
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="Q12" s="29"/>
-      <c r="R12" s="29"/>
-      <c r="S12" s="29" t="s">
+      <c r="Q12" s="28"/>
+      <c r="R12" s="28"/>
+      <c r="S12" s="28" t="s">
         <v>181</v>
       </c>
-      <c r="T12" s="29"/>
-      <c r="U12" s="29"/>
-      <c r="V12" s="29" t="s">
+      <c r="T12" s="28"/>
+      <c r="U12" s="28"/>
+      <c r="V12" s="28" t="s">
         <v>182</v>
       </c>
-      <c r="W12" s="29"/>
-      <c r="X12" s="29"/>
+      <c r="W12" s="28"/>
+      <c r="X12" s="28"/>
       <c r="Y12" s="6">
         <v>0</v>
       </c>
@@ -1973,11 +1970,11 @@
       <c r="A13" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="C13" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
+      <c r="C13" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
       <c r="F13" s="6">
         <v>0</v>
       </c>
@@ -1990,16 +1987,16 @@
       <c r="I13" s="12">
         <v>1</v>
       </c>
-      <c r="J13" s="29" t="s">
+      <c r="J13" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29" t="s">
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="N13" s="29"/>
-      <c r="O13" s="29"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
       <c r="P13" s="6">
         <v>0</v>
       </c>
@@ -2082,11 +2079,11 @@
       <c r="I14" s="12">
         <v>1</v>
       </c>
-      <c r="J14" s="29" t="s">
+      <c r="J14" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
       <c r="M14" s="6">
         <v>0</v>
       </c>
@@ -2129,16 +2126,16 @@
       <c r="Z14" s="6">
         <v>0</v>
       </c>
-      <c r="AA14" s="29" t="s">
+      <c r="AA14" s="28" t="s">
         <v>161</v>
       </c>
-      <c r="AB14" s="29"/>
-      <c r="AC14" s="29"/>
-      <c r="AD14" s="29"/>
-      <c r="AE14" s="29"/>
-      <c r="AF14" s="29"/>
-      <c r="AG14" s="29"/>
-      <c r="AH14" s="29"/>
+      <c r="AB14" s="28"/>
+      <c r="AC14" s="28"/>
+      <c r="AD14" s="28"/>
+      <c r="AE14" s="28"/>
+      <c r="AF14" s="28"/>
+      <c r="AG14" s="28"/>
+      <c r="AH14" s="28"/>
       <c r="AJ14" s="10" t="s">
         <v>154</v>
       </c>
@@ -2164,11 +2161,11 @@
       <c r="I15" s="12">
         <v>1</v>
       </c>
-      <c r="J15" s="29" t="s">
+      <c r="J15" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
       <c r="M15" s="6">
         <v>0</v>
       </c>
@@ -2187,24 +2184,24 @@
       <c r="R15" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="S15" s="29" t="s">
+      <c r="S15" s="28" t="s">
         <v>159</v>
       </c>
-      <c r="T15" s="29"/>
-      <c r="U15" s="29"/>
-      <c r="V15" s="29"/>
-      <c r="W15" s="29"/>
-      <c r="X15" s="29"/>
-      <c r="Y15" s="29"/>
-      <c r="Z15" s="29"/>
-      <c r="AA15" s="29"/>
-      <c r="AB15" s="29"/>
-      <c r="AC15" s="29"/>
-      <c r="AD15" s="29"/>
-      <c r="AE15" s="29"/>
-      <c r="AF15" s="29"/>
-      <c r="AG15" s="29"/>
-      <c r="AH15" s="29"/>
+      <c r="T15" s="28"/>
+      <c r="U15" s="28"/>
+      <c r="V15" s="28"/>
+      <c r="W15" s="28"/>
+      <c r="X15" s="28"/>
+      <c r="Y15" s="28"/>
+      <c r="Z15" s="28"/>
+      <c r="AA15" s="28"/>
+      <c r="AB15" s="28"/>
+      <c r="AC15" s="28"/>
+      <c r="AD15" s="28"/>
+      <c r="AE15" s="28"/>
+      <c r="AF15" s="28"/>
+      <c r="AG15" s="28"/>
+      <c r="AH15" s="28"/>
       <c r="AJ15" s="10" t="s">
         <v>154</v>
       </c>
@@ -2230,11 +2227,11 @@
       <c r="I16" s="12">
         <v>1</v>
       </c>
-      <c r="J16" s="29" t="s">
+      <c r="J16" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
       <c r="M16" s="6">
         <v>0</v>
       </c>
@@ -2253,24 +2250,24 @@
       <c r="R16" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="S16" s="29" t="s">
+      <c r="S16" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="T16" s="29"/>
-      <c r="U16" s="29"/>
-      <c r="V16" s="29"/>
-      <c r="W16" s="29"/>
-      <c r="X16" s="29"/>
-      <c r="Y16" s="29"/>
-      <c r="Z16" s="29"/>
-      <c r="AA16" s="29"/>
-      <c r="AB16" s="29"/>
-      <c r="AC16" s="29"/>
-      <c r="AD16" s="29"/>
-      <c r="AE16" s="29"/>
-      <c r="AF16" s="29"/>
-      <c r="AG16" s="29"/>
-      <c r="AH16" s="29"/>
+      <c r="T16" s="28"/>
+      <c r="U16" s="28"/>
+      <c r="V16" s="28"/>
+      <c r="W16" s="28"/>
+      <c r="X16" s="28"/>
+      <c r="Y16" s="28"/>
+      <c r="Z16" s="28"/>
+      <c r="AA16" s="28"/>
+      <c r="AB16" s="28"/>
+      <c r="AC16" s="28"/>
+      <c r="AD16" s="28"/>
+      <c r="AE16" s="28"/>
+      <c r="AF16" s="28"/>
+      <c r="AG16" s="28"/>
+      <c r="AH16" s="28"/>
       <c r="AJ16" s="10" t="s">
         <v>188</v>
       </c>
@@ -2296,35 +2293,35 @@
       <c r="I17" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="J17" s="29" t="s">
+      <c r="J17" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="K17" s="29"/>
-      <c r="L17" s="29"/>
-      <c r="M17" s="29" t="s">
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="N17" s="29"/>
-      <c r="O17" s="29"/>
-      <c r="P17" s="29"/>
-      <c r="Q17" s="29"/>
-      <c r="R17" s="29"/>
-      <c r="S17" s="29"/>
-      <c r="T17" s="29"/>
-      <c r="U17" s="29"/>
-      <c r="V17" s="29"/>
-      <c r="W17" s="29"/>
-      <c r="X17" s="29"/>
-      <c r="Y17" s="29"/>
-      <c r="Z17" s="29"/>
-      <c r="AA17" s="29"/>
-      <c r="AB17" s="29"/>
-      <c r="AC17" s="29"/>
-      <c r="AD17" s="29"/>
-      <c r="AE17" s="29"/>
-      <c r="AF17" s="29"/>
-      <c r="AG17" s="29"/>
-      <c r="AH17" s="29"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="28"/>
+      <c r="P17" s="28"/>
+      <c r="Q17" s="28"/>
+      <c r="R17" s="28"/>
+      <c r="S17" s="28"/>
+      <c r="T17" s="28"/>
+      <c r="U17" s="28"/>
+      <c r="V17" s="28"/>
+      <c r="W17" s="28"/>
+      <c r="X17" s="28"/>
+      <c r="Y17" s="28"/>
+      <c r="Z17" s="28"/>
+      <c r="AA17" s="28"/>
+      <c r="AB17" s="28"/>
+      <c r="AC17" s="28"/>
+      <c r="AD17" s="28"/>
+      <c r="AE17" s="28"/>
+      <c r="AF17" s="28"/>
+      <c r="AG17" s="28"/>
+      <c r="AH17" s="28"/>
       <c r="AJ17" s="10" t="s">
         <v>189</v>
       </c>
@@ -2350,35 +2347,35 @@
       <c r="I18" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="J18" s="29" t="s">
+      <c r="J18" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="K18" s="29"/>
-      <c r="L18" s="29"/>
-      <c r="M18" s="29" t="s">
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28" t="s">
         <v>185</v>
       </c>
-      <c r="N18" s="29"/>
-      <c r="O18" s="29"/>
-      <c r="P18" s="29"/>
-      <c r="Q18" s="29"/>
-      <c r="R18" s="29"/>
-      <c r="S18" s="29"/>
-      <c r="T18" s="29"/>
-      <c r="U18" s="29"/>
-      <c r="V18" s="29"/>
-      <c r="W18" s="29"/>
-      <c r="X18" s="29"/>
-      <c r="Y18" s="29"/>
-      <c r="Z18" s="29"/>
-      <c r="AA18" s="29"/>
-      <c r="AB18" s="29"/>
-      <c r="AC18" s="29"/>
-      <c r="AD18" s="29"/>
-      <c r="AE18" s="29"/>
-      <c r="AF18" s="29"/>
-      <c r="AG18" s="29"/>
-      <c r="AH18" s="29"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="28"/>
+      <c r="P18" s="28"/>
+      <c r="Q18" s="28"/>
+      <c r="R18" s="28"/>
+      <c r="S18" s="28"/>
+      <c r="T18" s="28"/>
+      <c r="U18" s="28"/>
+      <c r="V18" s="28"/>
+      <c r="W18" s="28"/>
+      <c r="X18" s="28"/>
+      <c r="Y18" s="28"/>
+      <c r="Z18" s="28"/>
+      <c r="AA18" s="28"/>
+      <c r="AB18" s="28"/>
+      <c r="AC18" s="28"/>
+      <c r="AD18" s="28"/>
+      <c r="AE18" s="28"/>
+      <c r="AF18" s="28"/>
+      <c r="AG18" s="28"/>
+      <c r="AH18" s="28"/>
       <c r="AJ18" s="10" t="s">
         <v>213</v>
       </c>
@@ -2404,35 +2401,35 @@
       <c r="I19" s="12">
         <v>0</v>
       </c>
-      <c r="J19" s="31" t="s">
+      <c r="J19" s="30" t="s">
         <v>164</v>
       </c>
-      <c r="K19" s="31"/>
-      <c r="L19" s="31"/>
-      <c r="M19" s="29" t="s">
+      <c r="K19" s="30"/>
+      <c r="L19" s="30"/>
+      <c r="M19" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="N19" s="29"/>
-      <c r="O19" s="29"/>
-      <c r="P19" s="29"/>
-      <c r="Q19" s="29"/>
-      <c r="R19" s="29"/>
-      <c r="S19" s="29"/>
-      <c r="T19" s="29"/>
-      <c r="U19" s="29"/>
-      <c r="V19" s="29"/>
-      <c r="W19" s="29"/>
-      <c r="X19" s="29"/>
-      <c r="Y19" s="29"/>
-      <c r="Z19" s="29"/>
-      <c r="AA19" s="29"/>
-      <c r="AB19" s="29"/>
-      <c r="AC19" s="29"/>
-      <c r="AD19" s="29"/>
-      <c r="AE19" s="29"/>
-      <c r="AF19" s="29"/>
-      <c r="AG19" s="29"/>
-      <c r="AH19" s="29"/>
+      <c r="N19" s="28"/>
+      <c r="O19" s="28"/>
+      <c r="P19" s="28"/>
+      <c r="Q19" s="28"/>
+      <c r="R19" s="28"/>
+      <c r="S19" s="28"/>
+      <c r="T19" s="28"/>
+      <c r="U19" s="28"/>
+      <c r="V19" s="28"/>
+      <c r="W19" s="28"/>
+      <c r="X19" s="28"/>
+      <c r="Y19" s="28"/>
+      <c r="Z19" s="28"/>
+      <c r="AA19" s="28"/>
+      <c r="AB19" s="28"/>
+      <c r="AC19" s="28"/>
+      <c r="AD19" s="28"/>
+      <c r="AE19" s="28"/>
+      <c r="AF19" s="28"/>
+      <c r="AG19" s="28"/>
+      <c r="AH19" s="28"/>
       <c r="AJ19" s="10" t="s">
         <v>204</v>
       </c>
@@ -2458,11 +2455,11 @@
       <c r="I20" s="6">
         <v>1</v>
       </c>
-      <c r="J20" s="29" t="s">
+      <c r="J20" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="K20" s="29"/>
-      <c r="L20" s="29"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
       <c r="M20" s="6">
         <v>0</v>
       </c>
@@ -2505,16 +2502,16 @@
       <c r="Z20" s="6">
         <v>0</v>
       </c>
-      <c r="AA20" s="29" t="s">
+      <c r="AA20" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="AB20" s="29"/>
-      <c r="AC20" s="29"/>
-      <c r="AD20" s="29"/>
-      <c r="AE20" s="29"/>
-      <c r="AF20" s="29"/>
-      <c r="AG20" s="29"/>
-      <c r="AH20" s="29"/>
+      <c r="AB20" s="28"/>
+      <c r="AC20" s="28"/>
+      <c r="AD20" s="28"/>
+      <c r="AE20" s="28"/>
+      <c r="AF20" s="28"/>
+      <c r="AG20" s="28"/>
+      <c r="AH20" s="28"/>
       <c r="AJ20" s="10" t="s">
         <v>89</v>
       </c>
@@ -2540,11 +2537,11 @@
       <c r="I21" s="6">
         <v>1</v>
       </c>
-      <c r="J21" s="29" t="s">
+      <c r="J21" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="K21" s="29"/>
-      <c r="L21" s="29"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
       <c r="M21" s="6">
         <v>0</v>
       </c>
@@ -2587,16 +2584,16 @@
       <c r="Z21" s="6">
         <v>1</v>
       </c>
-      <c r="AA21" s="29" t="s">
+      <c r="AA21" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="AB21" s="29"/>
-      <c r="AC21" s="29"/>
-      <c r="AD21" s="29"/>
-      <c r="AE21" s="29"/>
-      <c r="AF21" s="29"/>
-      <c r="AG21" s="29"/>
-      <c r="AH21" s="29"/>
+      <c r="AB21" s="28"/>
+      <c r="AC21" s="28"/>
+      <c r="AD21" s="28"/>
+      <c r="AE21" s="28"/>
+      <c r="AF21" s="28"/>
+      <c r="AG21" s="28"/>
+      <c r="AH21" s="28"/>
       <c r="AJ21" s="10" t="s">
         <v>186</v>
       </c>
@@ -2622,11 +2619,11 @@
       <c r="I22" s="6">
         <v>1</v>
       </c>
-      <c r="J22" s="29" t="s">
+      <c r="J22" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="K22" s="29"/>
-      <c r="L22" s="29"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="28"/>
       <c r="M22" s="6">
         <v>0</v>
       </c>
@@ -2767,16 +2764,16 @@
       <c r="Z23" s="6">
         <v>1</v>
       </c>
-      <c r="AA23" s="29" t="s">
+      <c r="AA23" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="AB23" s="29"/>
-      <c r="AC23" s="29"/>
-      <c r="AD23" s="29"/>
-      <c r="AE23" s="29"/>
-      <c r="AF23" s="29"/>
-      <c r="AG23" s="29"/>
-      <c r="AH23" s="29"/>
+      <c r="AB23" s="28"/>
+      <c r="AC23" s="28"/>
+      <c r="AD23" s="28"/>
+      <c r="AE23" s="28"/>
+      <c r="AF23" s="28"/>
+      <c r="AG23" s="28"/>
+      <c r="AH23" s="28"/>
     </row>
     <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
@@ -3427,7 +3424,7 @@
   <dimension ref="A1:O42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K41" sqref="K41"/>
+      <selection activeCell="Z38" sqref="Z38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3443,12 +3440,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
@@ -3458,18 +3455,18 @@
       <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="36"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="35"/>
       <c r="K2" s="20" t="s">
         <v>168</v>
       </c>
@@ -4808,7 +4805,7 @@
   <dimension ref="A1:AJ40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4971,30 +4968,30 @@
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="32"/>
-      <c r="O4" s="32"/>
-      <c r="P4" s="32"/>
-      <c r="Q4" s="32"/>
-      <c r="R4" s="32"/>
-      <c r="S4" s="32"/>
-      <c r="T4" s="32"/>
-      <c r="U4" s="32"/>
-      <c r="V4" s="32"/>
-      <c r="W4" s="32"/>
-      <c r="X4" s="32"/>
-      <c r="Y4" s="32"/>
-      <c r="Z4" s="32"/>
-      <c r="AA4" s="32"/>
-      <c r="AB4" s="32"/>
-      <c r="AC4" s="32"/>
-      <c r="AD4" s="32"/>
-      <c r="AE4" s="32"/>
-      <c r="AF4" s="32"/>
-      <c r="AG4" s="32"/>
-      <c r="AH4" s="32"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="31"/>
+      <c r="T4" s="31"/>
+      <c r="U4" s="31"/>
+      <c r="V4" s="31"/>
+      <c r="W4" s="31"/>
+      <c r="X4" s="31"/>
+      <c r="Y4" s="31"/>
+      <c r="Z4" s="31"/>
+      <c r="AA4" s="31"/>
+      <c r="AB4" s="31"/>
+      <c r="AC4" s="31"/>
+      <c r="AD4" s="31"/>
+      <c r="AE4" s="31"/>
+      <c r="AF4" s="31"/>
+      <c r="AG4" s="31"/>
+      <c r="AH4" s="31"/>
       <c r="AJ4" s="10"/>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
@@ -5025,32 +5022,32 @@
       <c r="J5" s="6">
         <v>1</v>
       </c>
-      <c r="K5" s="29" t="s">
+      <c r="K5" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="29"/>
-      <c r="T5" s="29"/>
-      <c r="U5" s="29"/>
-      <c r="V5" s="29"/>
-      <c r="W5" s="29"/>
-      <c r="X5" s="29"/>
-      <c r="Y5" s="29"/>
-      <c r="Z5" s="29"/>
-      <c r="AA5" s="29"/>
-      <c r="AB5" s="29"/>
-      <c r="AC5" s="29"/>
-      <c r="AD5" s="29"/>
-      <c r="AE5" s="29"/>
-      <c r="AF5" s="29"/>
-      <c r="AG5" s="29"/>
-      <c r="AH5" s="29"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="28"/>
+      <c r="Q5" s="28"/>
+      <c r="R5" s="28"/>
+      <c r="S5" s="28"/>
+      <c r="T5" s="28"/>
+      <c r="U5" s="28"/>
+      <c r="V5" s="28"/>
+      <c r="W5" s="28"/>
+      <c r="X5" s="28"/>
+      <c r="Y5" s="28"/>
+      <c r="Z5" s="28"/>
+      <c r="AA5" s="28"/>
+      <c r="AB5" s="28"/>
+      <c r="AC5" s="28"/>
+      <c r="AD5" s="28"/>
+      <c r="AE5" s="28"/>
+      <c r="AF5" s="28"/>
+      <c r="AG5" s="28"/>
+      <c r="AH5" s="28"/>
       <c r="AJ5" s="10"/>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
@@ -5081,36 +5078,36 @@
       <c r="J6" s="6">
         <v>0</v>
       </c>
-      <c r="K6" s="29" t="s">
+      <c r="K6" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="29"/>
-      <c r="S6" s="29" t="s">
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="28"/>
+      <c r="R6" s="28"/>
+      <c r="S6" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="T6" s="29"/>
-      <c r="U6" s="29"/>
-      <c r="V6" s="29"/>
-      <c r="W6" s="29"/>
-      <c r="X6" s="29"/>
-      <c r="Y6" s="29"/>
-      <c r="Z6" s="29"/>
-      <c r="AA6" s="29" t="s">
+      <c r="T6" s="28"/>
+      <c r="U6" s="28"/>
+      <c r="V6" s="28"/>
+      <c r="W6" s="28"/>
+      <c r="X6" s="28"/>
+      <c r="Y6" s="28"/>
+      <c r="Z6" s="28"/>
+      <c r="AA6" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="AB6" s="29"/>
-      <c r="AC6" s="29"/>
-      <c r="AD6" s="29"/>
-      <c r="AE6" s="29"/>
-      <c r="AF6" s="29"/>
-      <c r="AG6" s="29"/>
-      <c r="AH6" s="29"/>
+      <c r="AB6" s="28"/>
+      <c r="AC6" s="28"/>
+      <c r="AD6" s="28"/>
+      <c r="AE6" s="28"/>
+      <c r="AF6" s="28"/>
+      <c r="AG6" s="28"/>
+      <c r="AH6" s="28"/>
       <c r="AI6" s="6"/>
       <c r="AJ6" s="10"/>
     </row>
@@ -6356,22 +6353,22 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="32"/>
-      <c r="O4" s="32"/>
-      <c r="P4" s="32"/>
-      <c r="Q4" s="32"/>
-      <c r="R4" s="32"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="31"/>
       <c r="T4" s="10" t="s">
         <v>143</v>
       </c>
@@ -6460,16 +6457,16 @@
       <c r="J6" s="6">
         <v>1</v>
       </c>
-      <c r="K6" s="29" t="s">
+      <c r="K6" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="29"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="28"/>
+      <c r="R6" s="28"/>
       <c r="T6" s="10"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -6500,16 +6497,16 @@
       <c r="J7" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="K7" s="29" t="s">
+      <c r="K7" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29"/>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="29"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="28"/>
+      <c r="R7" s="28"/>
       <c r="T7" s="10"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -6540,16 +6537,16 @@
       <c r="J8" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="K8" s="29" t="s">
+      <c r="K8" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="29"/>
-      <c r="R8" s="29"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="28"/>
       <c r="T8" s="10"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -6580,16 +6577,16 @@
       <c r="J9" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="K9" s="29" t="s">
+      <c r="K9" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="29"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
+      <c r="Q9" s="28"/>
+      <c r="R9" s="28"/>
       <c r="T9" s="10"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
quick disassembler for easier debugging
</commit_message>
<xml_diff>
--- a/doc/RiscyInstSet32Bit.xlsx
+++ b/doc/RiscyInstSet32Bit.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="14715"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="14715" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="Instructions" sheetId="6" r:id="rId2"/>
-    <sheet name="Math Opcodes" sheetId="2" r:id="rId3"/>
+    <sheet name="Chapter 1. Math Opcodes" sheetId="2" r:id="rId2"/>
+    <sheet name="Instructions" sheetId="6" r:id="rId3"/>
     <sheet name="BIOS Call" sheetId="4" r:id="rId4"/>
     <sheet name="StdGrAd Call" sheetId="5" r:id="rId5"/>
   </sheets>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="271">
   <si>
     <t>Description</t>
   </si>
@@ -832,6 +832,15 @@
   </si>
   <si>
     <t>Inquire feature support</t>
+  </si>
+  <si>
+    <t>Chapter</t>
+  </si>
+  <si>
+    <t>Load and Store</t>
+  </si>
+  <si>
+    <t>Memory Copy</t>
   </si>
 </sst>
 </file>
@@ -1039,7 +1048,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="6" applyFont="1"/>
@@ -1141,6 +1150,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1430,23 +1460,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK48"/>
+  <dimension ref="A1:AL48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.7109375" customWidth="1"/>
-    <col min="2" max="2" width="2.5703125" customWidth="1"/>
-    <col min="3" max="34" width="3.42578125" customWidth="1"/>
-    <col min="35" max="35" width="2.5703125" customWidth="1"/>
-    <col min="36" max="36" width="116.85546875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" customWidth="1"/>
+    <col min="3" max="3" width="2.5703125" customWidth="1"/>
+    <col min="4" max="35" width="3.42578125" customWidth="1"/>
+    <col min="36" max="36" width="2.5703125" customWidth="1"/>
+    <col min="37" max="37" width="116.85546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:38" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1483,17 +1514,17 @@
       <c r="AF1" s="1"/>
       <c r="AG1" s="1"/>
       <c r="AH1" s="1"/>
-    </row>
-    <row r="2" spans="1:37" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="AI1" s="1"/>
+    </row>
+    <row r="2" spans="1:38" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
@@ -1524,19 +1555,19 @@
       <c r="AF3" s="5"/>
       <c r="AG3" s="5"/>
       <c r="AH3" s="5"/>
-      <c r="AJ3" t="s">
+      <c r="AI3" s="5"/>
+      <c r="AK3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="10">
+      <c r="C4" s="5"/>
+      <c r="D4" s="10">
         <v>8</v>
       </c>
-      <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
@@ -1567,19 +1598,19 @@
       <c r="AF4" s="5"/>
       <c r="AG4" s="5"/>
       <c r="AH4" s="5"/>
-      <c r="AJ4" t="s">
+      <c r="AI4" s="5"/>
+      <c r="AK4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5" t="s">
+        <v>1</v>
+      </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
@@ -1610,129 +1641,133 @@
       <c r="AF5" s="5"/>
       <c r="AG5" s="5"/>
       <c r="AH5" s="5"/>
-      <c r="AJ5" t="s">
+      <c r="AI5" s="5"/>
+      <c r="AK5" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="AJ6" t="s">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AK6" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="7" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4">
+    <row r="7" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="27" t="s">
+        <v>268</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4">
         <v>31</v>
       </c>
-      <c r="D7" s="4">
+      <c r="E7" s="4">
         <v>30</v>
       </c>
-      <c r="E7" s="4">
+      <c r="F7" s="4">
         <v>29</v>
       </c>
-      <c r="F7" s="4">
+      <c r="G7" s="4">
         <v>28</v>
       </c>
-      <c r="G7" s="4">
+      <c r="H7" s="4">
         <v>27</v>
       </c>
-      <c r="H7" s="4">
+      <c r="I7" s="4">
         <v>26</v>
       </c>
-      <c r="I7" s="4">
+      <c r="J7" s="4">
         <v>25</v>
       </c>
-      <c r="J7" s="4">
+      <c r="K7" s="4">
         <v>24</v>
       </c>
-      <c r="K7" s="4">
+      <c r="L7" s="4">
         <v>23</v>
       </c>
-      <c r="L7" s="4">
+      <c r="M7" s="4">
         <v>22</v>
       </c>
-      <c r="M7" s="4">
+      <c r="N7" s="4">
         <v>21</v>
       </c>
-      <c r="N7" s="4">
+      <c r="O7" s="4">
         <v>20</v>
       </c>
-      <c r="O7" s="4">
+      <c r="P7" s="4">
         <v>19</v>
       </c>
-      <c r="P7" s="4">
+      <c r="Q7" s="4">
         <v>18</v>
       </c>
-      <c r="Q7" s="4">
+      <c r="R7" s="4">
         <v>17</v>
       </c>
-      <c r="R7" s="4">
+      <c r="S7" s="4">
         <v>16</v>
       </c>
-      <c r="S7" s="4">
+      <c r="T7" s="4">
         <v>15</v>
       </c>
-      <c r="T7" s="4">
+      <c r="U7" s="4">
         <v>14</v>
       </c>
-      <c r="U7" s="4">
+      <c r="V7" s="4">
         <v>13</v>
       </c>
-      <c r="V7" s="4">
+      <c r="W7" s="4">
         <v>12</v>
       </c>
-      <c r="W7" s="4">
+      <c r="X7" s="4">
         <v>11</v>
       </c>
-      <c r="X7" s="4">
+      <c r="Y7" s="4">
         <v>10</v>
       </c>
-      <c r="Y7" s="4">
+      <c r="Z7" s="4">
         <v>9</v>
       </c>
-      <c r="Z7" s="4">
+      <c r="AA7" s="4">
         <v>8</v>
       </c>
-      <c r="AA7" s="4">
+      <c r="AB7" s="4">
         <v>7</v>
       </c>
-      <c r="AB7" s="4">
+      <c r="AC7" s="4">
         <v>6</v>
       </c>
-      <c r="AC7" s="4">
+      <c r="AD7" s="4">
         <v>5</v>
       </c>
-      <c r="AD7" s="4">
+      <c r="AE7" s="4">
         <v>4</v>
       </c>
-      <c r="AE7" s="4">
+      <c r="AF7" s="4">
         <v>3</v>
       </c>
-      <c r="AF7" s="4">
+      <c r="AG7" s="4">
         <v>2</v>
       </c>
-      <c r="AG7" s="4">
-        <v>1</v>
-      </c>
       <c r="AH7" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A8" s="42">
+        <v>1</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="D8" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="31"/>
       <c r="E8" s="31"/>
-      <c r="F8" s="11">
-        <v>0</v>
-      </c>
+      <c r="F8" s="31"/>
       <c r="G8" s="11">
         <v>0</v>
       </c>
@@ -1742,25 +1777,25 @@
       <c r="I8" s="11">
         <v>0</v>
       </c>
-      <c r="J8" s="35" t="s">
+      <c r="J8" s="11">
+        <v>0</v>
+      </c>
+      <c r="K8" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="35"/>
       <c r="L8" s="35"/>
-      <c r="M8" s="35" t="s">
+      <c r="M8" s="35"/>
+      <c r="N8" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="N8" s="35"/>
       <c r="O8" s="35"/>
-      <c r="P8" s="35" t="s">
+      <c r="P8" s="35"/>
+      <c r="Q8" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="Q8" s="35"/>
       <c r="R8" s="35"/>
-      <c r="S8" s="12">
-        <v>0</v>
-      </c>
-      <c r="T8" s="6">
+      <c r="S8" s="35"/>
+      <c r="T8" s="12">
         <v>0</v>
       </c>
       <c r="U8" s="6">
@@ -1787,30 +1822,31 @@
       <c r="AB8" s="6">
         <v>0</v>
       </c>
-      <c r="AC8" s="35" t="s">
+      <c r="AC8" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="AD8" s="35"/>
       <c r="AE8" s="35"/>
       <c r="AF8" s="35"/>
       <c r="AG8" s="35"/>
       <c r="AH8" s="35"/>
-      <c r="AJ8" s="10" t="s">
+      <c r="AI8" s="35"/>
+      <c r="AK8" s="10" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A9" s="41"/>
+      <c r="B9" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="D9" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="30"/>
       <c r="E9" s="30"/>
-      <c r="F9" s="18">
-        <v>0</v>
-      </c>
+      <c r="F9" s="30"/>
       <c r="G9" s="18">
         <v>0</v>
       </c>
@@ -1820,23 +1856,23 @@
       <c r="I9" s="18">
         <v>0</v>
       </c>
-      <c r="J9" s="36" t="s">
+      <c r="J9" s="18">
+        <v>0</v>
+      </c>
+      <c r="K9" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="K9" s="36"/>
       <c r="L9" s="36"/>
-      <c r="M9" s="34" t="s">
+      <c r="M9" s="36"/>
+      <c r="N9" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="N9" s="34"/>
       <c r="O9" s="34"/>
       <c r="P9" s="34"/>
       <c r="Q9" s="34"/>
       <c r="R9" s="34"/>
-      <c r="S9" s="12">
-        <v>0</v>
-      </c>
-      <c r="T9" s="6">
+      <c r="S9" s="34"/>
+      <c r="T9" s="12">
         <v>0</v>
       </c>
       <c r="U9" s="6">
@@ -1863,8 +1899,8 @@
       <c r="AB9" s="6">
         <v>0</v>
       </c>
-      <c r="AC9" s="18">
-        <v>1</v>
+      <c r="AC9" s="6">
+        <v>0</v>
       </c>
       <c r="AD9" s="18">
         <v>1</v>
@@ -1878,25 +1914,26 @@
       <c r="AG9" s="18">
         <v>1</v>
       </c>
-      <c r="AH9" s="21" t="s">
+      <c r="AH9" s="18">
+        <v>1</v>
+      </c>
+      <c r="AI9" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="AJ9" s="10" t="s">
+      <c r="AK9" s="10" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A10" s="41"/>
+      <c r="B10" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="D10" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="30"/>
       <c r="E10" s="30"/>
-      <c r="F10" s="18">
-        <v>0</v>
-      </c>
+      <c r="F10" s="30"/>
       <c r="G10" s="18">
         <v>0</v>
       </c>
@@ -1906,25 +1943,25 @@
       <c r="I10" s="18">
         <v>0</v>
       </c>
-      <c r="J10" s="32" t="s">
+      <c r="J10" s="18">
+        <v>0</v>
+      </c>
+      <c r="K10" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="K10" s="32"/>
       <c r="L10" s="32"/>
-      <c r="M10" s="32" t="s">
+      <c r="M10" s="32"/>
+      <c r="N10" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="N10" s="32"/>
       <c r="O10" s="32"/>
-      <c r="P10" s="33" t="s">
+      <c r="P10" s="32"/>
+      <c r="Q10" s="33" t="s">
         <v>163</v>
       </c>
-      <c r="Q10" s="33"/>
       <c r="R10" s="33"/>
-      <c r="S10" s="12">
-        <v>0</v>
-      </c>
-      <c r="T10" s="6">
+      <c r="S10" s="33"/>
+      <c r="T10" s="12">
         <v>0</v>
       </c>
       <c r="U10" s="6">
@@ -1951,41 +1988,44 @@
       <c r="AB10" s="6">
         <v>0</v>
       </c>
-      <c r="AC10" s="18">
-        <v>1</v>
+      <c r="AC10" s="6">
+        <v>0</v>
       </c>
       <c r="AD10" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE10" s="18">
         <v>0</v>
       </c>
       <c r="AF10" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG10" s="18">
-        <v>0</v>
-      </c>
-      <c r="AH10" s="13">
-        <v>0</v>
-      </c>
-      <c r="AJ10" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH10" s="18">
+        <v>0</v>
+      </c>
+      <c r="AI10" s="13">
+        <v>0</v>
+      </c>
+      <c r="AK10" s="10" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="D11" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="30"/>
       <c r="E11" s="30"/>
-      <c r="F11" s="6">
-        <v>0</v>
-      </c>
-      <c r="G11" s="12">
+      <c r="F11" s="30"/>
+      <c r="G11" s="6">
         <v>0</v>
       </c>
       <c r="H11" s="12">
@@ -1994,24 +2034,24 @@
       <c r="I11" s="12">
         <v>0</v>
       </c>
-      <c r="J11" s="29" t="s">
+      <c r="J11" s="12">
+        <v>0</v>
+      </c>
+      <c r="K11" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="K11" s="29"/>
       <c r="L11" s="29"/>
-      <c r="M11" s="29" t="s">
+      <c r="M11" s="29"/>
+      <c r="N11" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="N11" s="29"/>
       <c r="O11" s="29"/>
-      <c r="P11" s="29" t="s">
+      <c r="P11" s="29"/>
+      <c r="Q11" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="Q11" s="29"/>
       <c r="R11" s="29"/>
-      <c r="S11" s="6">
-        <v>0</v>
-      </c>
+      <c r="S11" s="29"/>
       <c r="T11" s="6">
         <v>0</v>
       </c>
@@ -2037,10 +2077,10 @@
         <v>0</v>
       </c>
       <c r="AB11" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC11" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD11" s="6">
         <v>0</v>
@@ -2048,33 +2088,36 @@
       <c r="AE11" s="6">
         <v>0</v>
       </c>
-      <c r="AF11" s="30" t="s">
+      <c r="AF11" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="AG11" s="30"/>
-      <c r="AH11" s="22" t="s">
+      <c r="AH11" s="30"/>
+      <c r="AI11" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="AJ11" s="10" t="s">
+      <c r="AK11" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="AK11" s="2" t="s">
+      <c r="AL11" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="D12" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="30"/>
       <c r="E12" s="30"/>
-      <c r="F12" s="6">
-        <v>0</v>
-      </c>
-      <c r="G12" s="12">
+      <c r="F12" s="30"/>
+      <c r="G12" s="6">
         <v>0</v>
       </c>
       <c r="H12" s="12">
@@ -2083,34 +2126,34 @@
       <c r="I12" s="12">
         <v>0</v>
       </c>
-      <c r="J12" s="29" t="s">
+      <c r="J12" s="12">
+        <v>0</v>
+      </c>
+      <c r="K12" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="K12" s="29"/>
       <c r="L12" s="29"/>
-      <c r="M12" s="29" t="s">
+      <c r="M12" s="29"/>
+      <c r="N12" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="N12" s="29"/>
       <c r="O12" s="29"/>
-      <c r="P12" s="29" t="s">
+      <c r="P12" s="29"/>
+      <c r="Q12" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="Q12" s="29"/>
       <c r="R12" s="29"/>
-      <c r="S12" s="29" t="s">
+      <c r="S12" s="29"/>
+      <c r="T12" s="29" t="s">
         <v>180</v>
       </c>
-      <c r="T12" s="29"/>
       <c r="U12" s="29"/>
-      <c r="V12" s="29" t="s">
+      <c r="V12" s="29"/>
+      <c r="W12" s="29" t="s">
         <v>181</v>
       </c>
-      <c r="W12" s="29"/>
       <c r="X12" s="29"/>
-      <c r="Y12" s="6">
-        <v>0</v>
-      </c>
+      <c r="Y12" s="29"/>
       <c r="Z12" s="6">
         <v>0</v>
       </c>
@@ -2118,19 +2161,19 @@
         <v>0</v>
       </c>
       <c r="AB12" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC12" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD12" s="6">
         <v>0</v>
       </c>
       <c r="AE12" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF12" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG12" s="6">
         <v>0</v>
@@ -2138,44 +2181,47 @@
       <c r="AH12" s="6">
         <v>0</v>
       </c>
-      <c r="AJ12" s="10" t="s">
+      <c r="AI12" s="6">
+        <v>0</v>
+      </c>
+      <c r="AK12" s="10" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="D13" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="30"/>
       <c r="E13" s="30"/>
-      <c r="F13" s="6">
-        <v>0</v>
-      </c>
-      <c r="G13" s="12">
+      <c r="F13" s="30"/>
+      <c r="G13" s="6">
         <v>0</v>
       </c>
       <c r="H13" s="12">
         <v>0</v>
       </c>
       <c r="I13" s="12">
-        <v>1</v>
-      </c>
-      <c r="J13" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="J13" s="12">
+        <v>1</v>
+      </c>
+      <c r="K13" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="K13" s="29"/>
       <c r="L13" s="29"/>
-      <c r="M13" s="29" t="s">
+      <c r="M13" s="29"/>
+      <c r="N13" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="N13" s="29"/>
       <c r="O13" s="29"/>
-      <c r="P13" s="6">
-        <v>0</v>
-      </c>
+      <c r="P13" s="29"/>
       <c r="Q13" s="6">
         <v>0</v>
       </c>
@@ -2224,59 +2270,62 @@
       <c r="AF13" s="6">
         <v>0</v>
       </c>
-      <c r="AG13" s="22" t="s">
+      <c r="AG13" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH13" s="22" t="s">
         <v>182</v>
       </c>
-      <c r="AH13" s="22" t="s">
+      <c r="AI13" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="AJ13" s="10" t="s">
+      <c r="AK13" s="10" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A14" s="41">
+        <v>2</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="D14" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="30"/>
       <c r="E14" s="30"/>
-      <c r="F14" s="6">
-        <v>0</v>
-      </c>
-      <c r="G14" s="12">
+      <c r="F14" s="30"/>
+      <c r="G14" s="6">
         <v>0</v>
       </c>
       <c r="H14" s="12">
         <v>0</v>
       </c>
       <c r="I14" s="12">
-        <v>1</v>
-      </c>
-      <c r="J14" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="J14" s="12">
+        <v>1</v>
+      </c>
+      <c r="K14" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="K14" s="29"/>
       <c r="L14" s="29"/>
-      <c r="M14" s="29" t="s">
+      <c r="M14" s="29"/>
+      <c r="N14" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="N14" s="29"/>
       <c r="O14" s="29"/>
-      <c r="P14" s="6">
-        <v>0</v>
-      </c>
+      <c r="P14" s="29"/>
       <c r="Q14" s="6">
-        <v>1</v>
-      </c>
-      <c r="R14" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="R14" s="6">
+        <v>1</v>
+      </c>
+      <c r="S14" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="S14" s="6">
-        <v>0</v>
-      </c>
       <c r="T14" s="6">
         <v>0</v>
       </c>
@@ -2298,64 +2347,67 @@
       <c r="Z14" s="6">
         <v>0</v>
       </c>
-      <c r="AA14" s="29" t="s">
+      <c r="AA14" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="29" t="s">
         <v>160</v>
       </c>
-      <c r="AB14" s="29"/>
       <c r="AC14" s="29"/>
       <c r="AD14" s="29"/>
       <c r="AE14" s="29"/>
       <c r="AF14" s="29"/>
       <c r="AG14" s="29"/>
       <c r="AH14" s="29"/>
-      <c r="AJ14" s="10" t="s">
+      <c r="AI14" s="29"/>
+      <c r="AK14" s="10" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A15" s="41"/>
+      <c r="B15" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="D15" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="30"/>
       <c r="E15" s="30"/>
-      <c r="F15" s="6">
-        <v>0</v>
-      </c>
-      <c r="G15" s="12">
+      <c r="F15" s="30"/>
+      <c r="G15" s="6">
         <v>0</v>
       </c>
       <c r="H15" s="12">
         <v>0</v>
       </c>
       <c r="I15" s="12">
-        <v>1</v>
-      </c>
-      <c r="J15" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="J15" s="12">
+        <v>1</v>
+      </c>
+      <c r="K15" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="K15" s="29"/>
       <c r="L15" s="29"/>
-      <c r="M15" s="29" t="s">
+      <c r="M15" s="29"/>
+      <c r="N15" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="N15" s="29"/>
       <c r="O15" s="29"/>
-      <c r="P15" s="6">
-        <v>1</v>
-      </c>
+      <c r="P15" s="29"/>
       <c r="Q15" s="6">
-        <v>0</v>
-      </c>
-      <c r="R15" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="R15" s="6">
+        <v>0</v>
+      </c>
+      <c r="S15" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="S15" s="29" t="s">
+      <c r="T15" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="T15" s="29"/>
       <c r="U15" s="29"/>
       <c r="V15" s="29"/>
       <c r="W15" s="29"/>
@@ -2370,54 +2422,55 @@
       <c r="AF15" s="29"/>
       <c r="AG15" s="29"/>
       <c r="AH15" s="29"/>
-      <c r="AJ15" s="10" t="s">
+      <c r="AI15" s="29"/>
+      <c r="AK15" s="10" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A16" s="41"/>
+      <c r="B16" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="D16" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="30"/>
       <c r="E16" s="30"/>
-      <c r="F16" s="6">
-        <v>0</v>
-      </c>
-      <c r="G16" s="12">
+      <c r="F16" s="30"/>
+      <c r="G16" s="6">
         <v>0</v>
       </c>
       <c r="H16" s="12">
         <v>0</v>
       </c>
       <c r="I16" s="12">
-        <v>1</v>
-      </c>
-      <c r="J16" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="J16" s="12">
+        <v>1</v>
+      </c>
+      <c r="K16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="K16" s="29"/>
       <c r="L16" s="29"/>
-      <c r="M16" s="29" t="s">
+      <c r="M16" s="29"/>
+      <c r="N16" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="N16" s="29"/>
       <c r="O16" s="29"/>
-      <c r="P16" s="6">
-        <v>1</v>
-      </c>
+      <c r="P16" s="29"/>
       <c r="Q16" s="6">
         <v>1</v>
       </c>
-      <c r="R16" s="22" t="s">
+      <c r="R16" s="6">
+        <v>1</v>
+      </c>
+      <c r="S16" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="S16" s="29" t="s">
+      <c r="T16" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="T16" s="29"/>
       <c r="U16" s="29"/>
       <c r="V16" s="29"/>
       <c r="W16" s="29"/>
@@ -2432,40 +2485,41 @@
       <c r="AF16" s="29"/>
       <c r="AG16" s="29"/>
       <c r="AH16" s="29"/>
-      <c r="AJ16" s="10" t="s">
+      <c r="AI16" s="29"/>
+      <c r="AK16" s="10" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A17" s="41"/>
+      <c r="B17" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="D17" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="30"/>
       <c r="E17" s="30"/>
-      <c r="F17" s="6">
-        <v>0</v>
-      </c>
-      <c r="G17" s="12">
+      <c r="F17" s="30"/>
+      <c r="G17" s="6">
         <v>0</v>
       </c>
       <c r="H17" s="12">
-        <v>1</v>
-      </c>
-      <c r="I17" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="I17" s="12">
+        <v>1</v>
+      </c>
+      <c r="J17" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="J17" s="29" t="s">
+      <c r="K17" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="K17" s="29"/>
       <c r="L17" s="29"/>
-      <c r="M17" s="29" t="s">
+      <c r="M17" s="29"/>
+      <c r="N17" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="N17" s="29"/>
       <c r="O17" s="29"/>
       <c r="P17" s="29"/>
       <c r="Q17" s="29"/>
@@ -2486,40 +2540,43 @@
       <c r="AF17" s="29"/>
       <c r="AG17" s="29"/>
       <c r="AH17" s="29"/>
-      <c r="AJ17" s="10" t="s">
+      <c r="AI17" s="29"/>
+      <c r="AK17" s="10" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="30" t="s">
+      <c r="D18" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="30"/>
       <c r="E18" s="30"/>
-      <c r="F18" s="6">
-        <v>0</v>
-      </c>
-      <c r="G18" s="12">
-        <v>1</v>
-      </c>
-      <c r="H18" s="12" t="s">
+      <c r="F18" s="30"/>
+      <c r="G18" s="6">
+        <v>0</v>
+      </c>
+      <c r="H18" s="12">
+        <v>1</v>
+      </c>
+      <c r="I18" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="I18" s="12" t="s">
+      <c r="J18" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="J18" s="29" t="s">
+      <c r="K18" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="K18" s="29"/>
       <c r="L18" s="29"/>
-      <c r="M18" s="29" t="s">
+      <c r="M18" s="29"/>
+      <c r="N18" s="29" t="s">
         <v>184</v>
       </c>
-      <c r="N18" s="29"/>
       <c r="O18" s="29"/>
       <c r="P18" s="29"/>
       <c r="Q18" s="29"/>
@@ -2540,24 +2597,25 @@
       <c r="AF18" s="29"/>
       <c r="AG18" s="29"/>
       <c r="AH18" s="29"/>
-      <c r="AJ18" s="10" t="s">
+      <c r="AI18" s="29"/>
+      <c r="AK18" s="10" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="C19" s="30" t="s">
+      <c r="D19" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="30"/>
       <c r="E19" s="30"/>
-      <c r="F19" s="6">
-        <v>1</v>
-      </c>
-      <c r="G19" s="12">
-        <v>0</v>
+      <c r="F19" s="30"/>
+      <c r="G19" s="6">
+        <v>1</v>
       </c>
       <c r="H19" s="12">
         <v>0</v>
@@ -2565,15 +2623,17 @@
       <c r="I19" s="12">
         <v>0</v>
       </c>
-      <c r="J19" s="34" t="s">
+      <c r="J19" s="12">
+        <v>0</v>
+      </c>
+      <c r="K19" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="K19" s="34"/>
       <c r="L19" s="34"/>
-      <c r="M19" s="29" t="s">
+      <c r="M19" s="34"/>
+      <c r="N19" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="N19" s="29"/>
       <c r="O19" s="29"/>
       <c r="P19" s="29"/>
       <c r="Q19" s="29"/>
@@ -2594,57 +2654,60 @@
       <c r="AF19" s="29"/>
       <c r="AG19" s="29"/>
       <c r="AH19" s="29"/>
-      <c r="AJ19" s="10" t="s">
+      <c r="AI19" s="29"/>
+      <c r="AK19" s="10" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>7</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="C20" s="30" t="s">
+      <c r="D20" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="30"/>
       <c r="E20" s="30"/>
-      <c r="F20" s="24">
-        <v>1</v>
-      </c>
-      <c r="G20" s="25">
-        <v>0</v>
+      <c r="F20" s="30"/>
+      <c r="G20" s="24">
+        <v>1</v>
       </c>
       <c r="H20" s="25">
         <v>0</v>
       </c>
       <c r="I20" s="25">
-        <v>1</v>
-      </c>
-      <c r="J20" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="J20" s="25">
+        <v>1</v>
+      </c>
+      <c r="K20" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="K20" s="34"/>
       <c r="L20" s="34"/>
-      <c r="M20" s="25">
-        <v>0</v>
-      </c>
+      <c r="M20" s="34"/>
       <c r="N20" s="25">
         <v>0</v>
       </c>
       <c r="O20" s="25">
         <v>0</v>
       </c>
-      <c r="P20" s="36" t="s">
+      <c r="P20" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="36" t="s">
         <v>262</v>
       </c>
-      <c r="Q20" s="36"/>
       <c r="R20" s="36"/>
       <c r="S20" s="36"/>
       <c r="T20" s="36"/>
       <c r="U20" s="36"/>
-      <c r="V20" s="29" t="s">
+      <c r="V20" s="36"/>
+      <c r="W20" s="29" t="s">
         <v>261</v>
       </c>
-      <c r="W20" s="29"/>
       <c r="X20" s="29"/>
       <c r="Y20" s="29"/>
       <c r="Z20" s="29"/>
@@ -2656,52 +2719,53 @@
       <c r="AF20" s="29"/>
       <c r="AG20" s="29"/>
       <c r="AH20" s="29"/>
-      <c r="AJ20" s="10" t="s">
+      <c r="AI20" s="29"/>
+      <c r="AK20" s="10" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>8</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>267</v>
       </c>
-      <c r="C21" s="30" t="s">
+      <c r="D21" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="30"/>
       <c r="E21" s="30"/>
-      <c r="F21" s="24">
-        <v>1</v>
-      </c>
-      <c r="G21" s="25">
-        <v>0</v>
+      <c r="F21" s="30"/>
+      <c r="G21" s="24">
+        <v>1</v>
       </c>
       <c r="H21" s="25">
         <v>0</v>
       </c>
       <c r="I21" s="25">
-        <v>1</v>
-      </c>
-      <c r="J21" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="J21" s="25">
+        <v>1</v>
+      </c>
+      <c r="K21" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="K21" s="36"/>
       <c r="L21" s="36"/>
-      <c r="M21" s="25">
-        <v>0</v>
-      </c>
+      <c r="M21" s="36"/>
       <c r="N21" s="25">
         <v>0</v>
       </c>
       <c r="O21" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P21" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q21" s="25">
         <v>0</v>
       </c>
-      <c r="R21" s="24">
+      <c r="R21" s="25">
         <v>0</v>
       </c>
       <c r="S21" s="24">
@@ -2728,32 +2792,35 @@
       <c r="Z21" s="24">
         <v>0</v>
       </c>
-      <c r="AA21" s="29" t="s">
+      <c r="AA21" s="24">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="29" t="s">
         <v>264</v>
       </c>
-      <c r="AB21" s="29"/>
       <c r="AC21" s="29"/>
       <c r="AD21" s="29"/>
       <c r="AE21" s="29"/>
       <c r="AF21" s="29"/>
       <c r="AG21" s="29"/>
       <c r="AH21" s="29"/>
-      <c r="AJ21" s="10" t="s">
+      <c r="AI21" s="29"/>
+      <c r="AK21" s="10" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>9</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C22" s="30" t="s">
+      <c r="D22" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="30"/>
       <c r="E22" s="30"/>
-      <c r="F22" s="6">
-        <v>1</v>
-      </c>
+      <c r="F22" s="30"/>
       <c r="G22" s="6">
         <v>1</v>
       </c>
@@ -2763,14 +2830,14 @@
       <c r="I22" s="6">
         <v>1</v>
       </c>
-      <c r="J22" s="29" t="s">
+      <c r="J22" s="6">
+        <v>1</v>
+      </c>
+      <c r="K22" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="K22" s="29"/>
       <c r="L22" s="29"/>
-      <c r="M22" s="6">
-        <v>0</v>
-      </c>
+      <c r="M22" s="29"/>
       <c r="N22" s="6">
         <v>0</v>
       </c>
@@ -2810,32 +2877,35 @@
       <c r="Z22" s="6">
         <v>0</v>
       </c>
-      <c r="AA22" s="29" t="s">
+      <c r="AA22" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="AB22" s="29"/>
       <c r="AC22" s="29"/>
       <c r="AD22" s="29"/>
       <c r="AE22" s="29"/>
       <c r="AF22" s="29"/>
       <c r="AG22" s="29"/>
       <c r="AH22" s="29"/>
-      <c r="AJ22" s="10" t="s">
+      <c r="AI22" s="29"/>
+      <c r="AK22" s="10" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>10</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C23" s="30" t="s">
+      <c r="D23" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="30"/>
       <c r="E23" s="30"/>
-      <c r="F23" s="6">
-        <v>1</v>
-      </c>
+      <c r="F23" s="30"/>
       <c r="G23" s="6">
         <v>1</v>
       </c>
@@ -2845,14 +2915,14 @@
       <c r="I23" s="6">
         <v>1</v>
       </c>
-      <c r="J23" s="29" t="s">
+      <c r="J23" s="6">
+        <v>1</v>
+      </c>
+      <c r="K23" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="K23" s="29"/>
       <c r="L23" s="29"/>
-      <c r="M23" s="6">
-        <v>0</v>
-      </c>
+      <c r="M23" s="29"/>
       <c r="N23" s="6">
         <v>0</v>
       </c>
@@ -2890,34 +2960,37 @@
         <v>0</v>
       </c>
       <c r="Z23" s="6">
-        <v>1</v>
-      </c>
-      <c r="AA23" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="6">
+        <v>1</v>
+      </c>
+      <c r="AB23" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="AB23" s="29"/>
       <c r="AC23" s="29"/>
       <c r="AD23" s="29"/>
       <c r="AE23" s="29"/>
       <c r="AF23" s="29"/>
       <c r="AG23" s="29"/>
       <c r="AH23" s="29"/>
-      <c r="AJ23" s="10" t="s">
+      <c r="AI23" s="29"/>
+      <c r="AK23" s="10" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>11</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="C24" s="30" t="s">
+      <c r="D24" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D24" s="30"/>
       <c r="E24" s="30"/>
-      <c r="F24" s="6">
-        <v>1</v>
-      </c>
+      <c r="F24" s="30"/>
       <c r="G24" s="6">
         <v>1</v>
       </c>
@@ -2927,14 +3000,14 @@
       <c r="I24" s="6">
         <v>1</v>
       </c>
-      <c r="J24" s="29" t="s">
+      <c r="J24" s="6">
+        <v>1</v>
+      </c>
+      <c r="K24" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="K24" s="29"/>
       <c r="L24" s="29"/>
-      <c r="M24" s="6">
-        <v>0</v>
-      </c>
+      <c r="M24" s="29"/>
       <c r="N24" s="6">
         <v>0</v>
       </c>
@@ -2972,7 +3045,7 @@
         <v>0</v>
       </c>
       <c r="Z24" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA24" s="6">
         <v>1</v>
@@ -2998,20 +3071,23 @@
       <c r="AH24" s="6">
         <v>1</v>
       </c>
-      <c r="AJ24" s="10"/>
-    </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+      <c r="AI24" s="6">
+        <v>1</v>
+      </c>
+      <c r="AK24" s="10"/>
+    </row>
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>12</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C25" s="30" t="s">
+      <c r="D25" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="30"/>
       <c r="E25" s="30"/>
-      <c r="F25" s="6">
-        <v>1</v>
-      </c>
+      <c r="F25" s="30"/>
       <c r="G25" s="6">
         <v>1</v>
       </c>
@@ -3072,20 +3148,22 @@
       <c r="Z25" s="6">
         <v>1</v>
       </c>
-      <c r="AA25" s="29" t="s">
+      <c r="AA25" s="6">
+        <v>1</v>
+      </c>
+      <c r="AB25" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="AB25" s="29"/>
       <c r="AC25" s="29"/>
       <c r="AD25" s="29"/>
       <c r="AE25" s="29"/>
       <c r="AF25" s="29"/>
       <c r="AG25" s="29"/>
       <c r="AH25" s="29"/>
-    </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="6"/>
+      <c r="AI25" s="29"/>
+    </row>
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B32" s="7"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
@@ -3118,11 +3196,11 @@
       <c r="AF32" s="6"/>
       <c r="AG32" s="6"/>
       <c r="AH32" s="6"/>
-      <c r="AJ32" s="10"/>
-    </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
-      <c r="B33" s="6"/>
+      <c r="AI32" s="6"/>
+      <c r="AK32" s="10"/>
+    </row>
+    <row r="33" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B33" s="7"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
@@ -3155,11 +3233,11 @@
       <c r="AF33" s="6"/>
       <c r="AG33" s="6"/>
       <c r="AH33" s="6"/>
-      <c r="AJ33" s="10"/>
-    </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
-      <c r="B34" s="6"/>
+      <c r="AI33" s="6"/>
+      <c r="AK33" s="10"/>
+    </row>
+    <row r="34" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B34" s="7"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
@@ -3192,11 +3270,11 @@
       <c r="AF34" s="6"/>
       <c r="AG34" s="6"/>
       <c r="AH34" s="6"/>
-      <c r="AJ34" s="10"/>
-    </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
-      <c r="B35" s="6"/>
+      <c r="AI34" s="6"/>
+      <c r="AK34" s="10"/>
+    </row>
+    <row r="35" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B35" s="7"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
@@ -3229,11 +3307,11 @@
       <c r="AF35" s="6"/>
       <c r="AG35" s="6"/>
       <c r="AH35" s="6"/>
-      <c r="AJ35" s="10"/>
-    </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
-      <c r="C36" s="6"/>
+      <c r="AI35" s="6"/>
+      <c r="AK35" s="10"/>
+    </row>
+    <row r="36" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B36" s="7"/>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
@@ -3265,11 +3343,11 @@
       <c r="AF36" s="6"/>
       <c r="AG36" s="6"/>
       <c r="AH36" s="6"/>
-      <c r="AJ36" s="10"/>
-    </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
-      <c r="C37" s="6"/>
+      <c r="AI36" s="6"/>
+      <c r="AK36" s="10"/>
+    </row>
+    <row r="37" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B37" s="7"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
@@ -3301,11 +3379,11 @@
       <c r="AF37" s="6"/>
       <c r="AG37" s="6"/>
       <c r="AH37" s="6"/>
-      <c r="AJ37" s="10"/>
-    </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A38" s="7"/>
-      <c r="C38" s="6"/>
+      <c r="AI37" s="6"/>
+      <c r="AK37" s="10"/>
+    </row>
+    <row r="38" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B38" s="7"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
@@ -3337,11 +3415,11 @@
       <c r="AF38" s="6"/>
       <c r="AG38" s="6"/>
       <c r="AH38" s="6"/>
-      <c r="AJ38" s="10"/>
-    </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="C39" s="6"/>
+      <c r="AI38" s="6"/>
+      <c r="AK38" s="10"/>
+    </row>
+    <row r="39" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B39" s="7"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
@@ -3373,11 +3451,11 @@
       <c r="AF39" s="6"/>
       <c r="AG39" s="6"/>
       <c r="AH39" s="6"/>
-      <c r="AJ39" s="10"/>
-    </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
-      <c r="C40" s="6"/>
+      <c r="AI39" s="6"/>
+      <c r="AK39" s="10"/>
+    </row>
+    <row r="40" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B40" s="7"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
@@ -3409,11 +3487,11 @@
       <c r="AF40" s="6"/>
       <c r="AG40" s="6"/>
       <c r="AH40" s="6"/>
-      <c r="AJ40" s="10"/>
-    </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A41" s="7"/>
-      <c r="C41" s="6"/>
+      <c r="AI40" s="6"/>
+      <c r="AK40" s="10"/>
+    </row>
+    <row r="41" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B41" s="7"/>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
@@ -3445,11 +3523,11 @@
       <c r="AF41" s="6"/>
       <c r="AG41" s="6"/>
       <c r="AH41" s="6"/>
-      <c r="AJ41" s="10"/>
-    </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A42" s="7"/>
-      <c r="C42" s="6"/>
+      <c r="AI41" s="6"/>
+      <c r="AK41" s="10"/>
+    </row>
+    <row r="42" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B42" s="7"/>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
@@ -3481,11 +3559,11 @@
       <c r="AF42" s="6"/>
       <c r="AG42" s="6"/>
       <c r="AH42" s="6"/>
-      <c r="AJ42" s="10"/>
-    </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
-      <c r="C43" s="6"/>
+      <c r="AI42" s="6"/>
+      <c r="AK42" s="10"/>
+    </row>
+    <row r="43" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B43" s="7"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
@@ -3517,11 +3595,11 @@
       <c r="AF43" s="6"/>
       <c r="AG43" s="6"/>
       <c r="AH43" s="6"/>
-      <c r="AJ43" s="10"/>
-    </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A44" s="7"/>
-      <c r="C44" s="6"/>
+      <c r="AI43" s="6"/>
+      <c r="AK43" s="10"/>
+    </row>
+    <row r="44" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B44" s="7"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
@@ -3553,11 +3631,11 @@
       <c r="AF44" s="6"/>
       <c r="AG44" s="6"/>
       <c r="AH44" s="6"/>
-      <c r="AJ44" s="10"/>
-    </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A45" s="7"/>
-      <c r="C45" s="6"/>
+      <c r="AI44" s="6"/>
+      <c r="AK44" s="10"/>
+    </row>
+    <row r="45" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B45" s="7"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
@@ -3589,11 +3667,11 @@
       <c r="AF45" s="6"/>
       <c r="AG45" s="6"/>
       <c r="AH45" s="6"/>
-      <c r="AJ45" s="10"/>
-    </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A46" s="7"/>
-      <c r="C46" s="6"/>
+      <c r="AI45" s="6"/>
+      <c r="AK45" s="10"/>
+    </row>
+    <row r="46" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B46" s="7"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
@@ -3625,11 +3703,11 @@
       <c r="AF46" s="6"/>
       <c r="AG46" s="6"/>
       <c r="AH46" s="6"/>
-      <c r="AJ46" s="10"/>
-    </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A47" s="7"/>
-      <c r="C47" s="6"/>
+      <c r="AI46" s="6"/>
+      <c r="AK46" s="10"/>
+    </row>
+    <row r="47" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B47" s="7"/>
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
@@ -3661,76 +3739,79 @@
       <c r="AF47" s="6"/>
       <c r="AG47" s="6"/>
       <c r="AH47" s="6"/>
-    </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A48" s="7"/>
+      <c r="AI47" s="6"/>
+    </row>
+    <row r="48" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B48" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="64">
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="P20:U20"/>
-    <mergeCell ref="V20:AH20"/>
-    <mergeCell ref="AA21:AH21"/>
-    <mergeCell ref="J21:L21"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="AC8:AH8"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="P8:R8"/>
-    <mergeCell ref="AA22:AH22"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="M9:R9"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="AA14:AH14"/>
-    <mergeCell ref="J16:L16"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="P12:R12"/>
-    <mergeCell ref="S12:U12"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="AA25:AH25"/>
-    <mergeCell ref="M17:AH17"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="M11:O11"/>
-    <mergeCell ref="P11:R11"/>
-    <mergeCell ref="M19:AH19"/>
-    <mergeCell ref="M18:AH18"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="S16:AH16"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="J23:L23"/>
-    <mergeCell ref="AA23:AH23"/>
-    <mergeCell ref="J24:L24"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="S15:AH15"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="P10:R10"/>
-    <mergeCell ref="AF11:AG11"/>
-    <mergeCell ref="V12:X12"/>
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C24:E24"/>
+  <mergeCells count="66">
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="Q20:V20"/>
+    <mergeCell ref="W20:AI20"/>
+    <mergeCell ref="AB21:AI21"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="AD8:AI8"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="N8:P8"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="AB22:AI22"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="N9:S9"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="AB14:AI14"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="N12:P12"/>
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="T12:V12"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="AB25:AI25"/>
+    <mergeCell ref="N17:AI17"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="N19:AI19"/>
+    <mergeCell ref="N18:AI18"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="T16:AI16"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="AB23:AI23"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="T15:AI15"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="AG11:AH11"/>
+    <mergeCell ref="W12:Y12"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="N15:P15"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="N16:P16"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D24:F24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3738,276 +3819,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20" style="26" customWidth="1"/>
-    <col min="2" max="2" width="3.42578125" customWidth="1"/>
-    <col min="3" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="141" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="108.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="28" t="s">
-        <v>221</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="8"/>
-    </row>
-    <row r="2" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
-        <v>214</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="23" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>213</v>
-      </c>
-      <c r="C3" t="s">
-        <v>251</v>
-      </c>
-      <c r="D3" t="s">
-        <v>230</v>
-      </c>
-      <c r="E3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>215</v>
-      </c>
-      <c r="C4" t="s">
-        <v>251</v>
-      </c>
-      <c r="D4" t="s">
-        <v>230</v>
-      </c>
-      <c r="E4" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>216</v>
-      </c>
-      <c r="C5" t="s">
-        <v>251</v>
-      </c>
-      <c r="D5" t="s">
-        <v>230</v>
-      </c>
-      <c r="E5" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
-        <v>218</v>
-      </c>
-      <c r="C6" t="s">
-        <v>252</v>
-      </c>
-      <c r="D6" t="s">
-        <v>231</v>
-      </c>
-      <c r="E6" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
-        <v>219</v>
-      </c>
-      <c r="C7" t="s">
-        <v>252</v>
-      </c>
-      <c r="D7" t="s">
-        <v>232</v>
-      </c>
-      <c r="E7" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
-        <v>220</v>
-      </c>
-      <c r="C8" t="s">
-        <v>252</v>
-      </c>
-      <c r="D8" t="s">
-        <v>233</v>
-      </c>
-      <c r="E8" t="s">
-        <v>242</v>
-      </c>
-      <c r="F8" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
-        <v>228</v>
-      </c>
-      <c r="C9" t="s">
-        <v>258</v>
-      </c>
-      <c r="D9" t="s">
-        <v>236</v>
-      </c>
-      <c r="E9" t="s">
-        <v>243</v>
-      </c>
-      <c r="F9" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="28" t="s">
-        <v>222</v>
-      </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="8"/>
-    </row>
-    <row r="11" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="27" t="s">
-        <v>214</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F11" s="23" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
-        <v>223</v>
-      </c>
-      <c r="C12" t="s">
-        <v>253</v>
-      </c>
-      <c r="D12" t="s">
-        <v>230</v>
-      </c>
-      <c r="E12" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
-        <v>224</v>
-      </c>
-      <c r="C13" t="s">
-        <v>253</v>
-      </c>
-      <c r="D13" t="s">
-        <v>230</v>
-      </c>
-      <c r="E13" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
-        <v>225</v>
-      </c>
-      <c r="C14" t="s">
-        <v>253</v>
-      </c>
-      <c r="D14" t="s">
-        <v>230</v>
-      </c>
-      <c r="E14" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
-        <v>226</v>
-      </c>
-      <c r="C15" t="s">
-        <v>257</v>
-      </c>
-      <c r="D15" t="s">
-        <v>254</v>
-      </c>
-      <c r="E15" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
-        <v>227</v>
-      </c>
-      <c r="C16" t="s">
-        <v>257</v>
-      </c>
-      <c r="D16" t="s">
-        <v>255</v>
-      </c>
-      <c r="E16" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="C17" t="s">
-        <v>256</v>
-      </c>
-      <c r="D17" t="s">
-        <v>236</v>
-      </c>
-      <c r="E17" t="s">
-        <v>250</v>
-      </c>
-      <c r="F17" t="s">
-        <v>244</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O42"/>
   <sheetViews>
@@ -5384,6 +5195,305 @@
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:J2"/>
   </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" style="26" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" style="25" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="141" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="108.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="44" t="s">
+        <v>268</v>
+      </c>
+      <c r="B1" s="45">
+        <v>2</v>
+      </c>
+      <c r="C1" s="43" t="s">
+        <v>269</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="B2" s="46"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="B3" s="47"/>
+      <c r="C3" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>213</v>
+      </c>
+      <c r="C4" t="s">
+        <v>251</v>
+      </c>
+      <c r="D4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="C5" t="s">
+        <v>251</v>
+      </c>
+      <c r="D5" t="s">
+        <v>230</v>
+      </c>
+      <c r="E5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>216</v>
+      </c>
+      <c r="C6" t="s">
+        <v>251</v>
+      </c>
+      <c r="D6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E6" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
+        <v>218</v>
+      </c>
+      <c r="C7" t="s">
+        <v>252</v>
+      </c>
+      <c r="D7" t="s">
+        <v>231</v>
+      </c>
+      <c r="E7" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
+        <v>219</v>
+      </c>
+      <c r="C8" t="s">
+        <v>252</v>
+      </c>
+      <c r="D8" t="s">
+        <v>232</v>
+      </c>
+      <c r="E8" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="C9" t="s">
+        <v>252</v>
+      </c>
+      <c r="D9" t="s">
+        <v>233</v>
+      </c>
+      <c r="E9" t="s">
+        <v>242</v>
+      </c>
+      <c r="F9" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="s">
+        <v>228</v>
+      </c>
+      <c r="C10" t="s">
+        <v>258</v>
+      </c>
+      <c r="D10" t="s">
+        <v>236</v>
+      </c>
+      <c r="E10" t="s">
+        <v>243</v>
+      </c>
+      <c r="F10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="B11" s="46"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="B12" s="47"/>
+      <c r="C12" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="C13" t="s">
+        <v>253</v>
+      </c>
+      <c r="D13" t="s">
+        <v>230</v>
+      </c>
+      <c r="E13" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="C14" t="s">
+        <v>253</v>
+      </c>
+      <c r="D14" t="s">
+        <v>230</v>
+      </c>
+      <c r="E14" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="C15" t="s">
+        <v>253</v>
+      </c>
+      <c r="D15" t="s">
+        <v>230</v>
+      </c>
+      <c r="E15" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
+        <v>226</v>
+      </c>
+      <c r="C16" t="s">
+        <v>257</v>
+      </c>
+      <c r="D16" t="s">
+        <v>254</v>
+      </c>
+      <c r="E16" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C17" t="s">
+        <v>257</v>
+      </c>
+      <c r="D17" t="s">
+        <v>255</v>
+      </c>
+      <c r="E17" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="26" t="s">
+        <v>229</v>
+      </c>
+      <c r="C18" t="s">
+        <v>256</v>
+      </c>
+      <c r="D18" t="s">
+        <v>236</v>
+      </c>
+      <c r="E18" t="s">
+        <v>250</v>
+      </c>
+      <c r="F18" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="44" t="s">
+        <v>268</v>
+      </c>
+      <c r="B19" s="45">
+        <v>3</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
adjusted order of tree traverse for IF statement
</commit_message>
<xml_diff>
--- a/doc/RiscyInstSet32Bit.xlsx
+++ b/doc/RiscyInstSet32Bit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="14715" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="14715" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="301">
   <si>
     <t>Description</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Number of Registers</t>
   </si>
   <si>
-    <t>Mathematical opcodes</t>
-  </si>
-  <si>
     <t>MOV</t>
   </si>
   <si>
@@ -841,6 +838,99 @@
   </si>
   <si>
     <t>Memory Copy</t>
+  </si>
+  <si>
+    <t>MEMCPY</t>
+  </si>
+  <si>
+    <t>destination, source, length, from, to</t>
+  </si>
+  <si>
+    <t>dev[to].mem[dest] = dev[from].mem[src]</t>
+  </si>
+  <si>
+    <t>CMP/CMPII</t>
+  </si>
+  <si>
+    <t>lhand, rhand</t>
+  </si>
+  <si>
+    <t>rCMP = rHand - lHand</t>
+  </si>
+  <si>
+    <t>Two arguments are both integer</t>
+  </si>
+  <si>
+    <t>CMPFI</t>
+  </si>
+  <si>
+    <t>CMPIF</t>
+  </si>
+  <si>
+    <t>CMPFF</t>
+  </si>
+  <si>
+    <t>Lhand is float, Rhand is integer</t>
+  </si>
+  <si>
+    <t>Lhand is integer, Rhand is float</t>
+  </si>
+  <si>
+    <t>Two arguments are both float</t>
+  </si>
+  <si>
+    <t>PUSH</t>
+  </si>
+  <si>
+    <t>PUSHINT</t>
+  </si>
+  <si>
+    <t>POP</t>
+  </si>
+  <si>
+    <t>POPINT</t>
+  </si>
+  <si>
+    <t>Conditional Jump</t>
+  </si>
+  <si>
+    <t>JMP</t>
+  </si>
+  <si>
+    <t>JZ</t>
+  </si>
+  <si>
+    <t>JNZ</t>
+  </si>
+  <si>
+    <t>JGT</t>
+  </si>
+  <si>
+    <t>JLS</t>
+  </si>
+  <si>
+    <t>JFW</t>
+  </si>
+  <si>
+    <t>JBW</t>
+  </si>
+  <si>
+    <t>Memory Bank Operation</t>
+  </si>
+  <si>
+    <t>Supported Feature Inquiry</t>
+  </si>
+  <si>
+    <t>Calling Peripheral</t>
+  </si>
+  <si>
+    <t>Memory Size Inquiry</t>
+  </si>
+  <si>
+    <t>System Uptime Inquiry</t>
+  </si>
+  <si>
+    <t>Mathematical Opcodes</t>
   </si>
 </sst>
 </file>
@@ -1048,7 +1138,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="6" applyFont="1"/>
@@ -1139,9 +1229,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1463,7 +1550,7 @@
   <dimension ref="A1:AL48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1519,7 +1606,7 @@
     <row r="2" spans="1:38" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5" t="s">
@@ -1605,7 +1692,7 @@
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
@@ -1643,17 +1730,17 @@
       <c r="AH5" s="5"/>
       <c r="AI5" s="5"/>
       <c r="AK5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="AK6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>0</v>
@@ -1757,7 +1844,7 @@
       </c>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A8" s="42">
+      <c r="A8" s="41">
         <v>1</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -1834,13 +1921,13 @@
       <c r="AH8" s="35"/>
       <c r="AI8" s="35"/>
       <c r="AK8" s="10" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A9" s="40"/>
+      <c r="B9" s="7" t="s">
         <v>164</v>
-      </c>
-    </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
-      <c r="B9" s="7" t="s">
-        <v>165</v>
       </c>
       <c r="D9" s="30" t="s">
         <v>5</v>
@@ -1865,7 +1952,7 @@
       <c r="L9" s="36"/>
       <c r="M9" s="36"/>
       <c r="N9" s="34" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O9" s="34"/>
       <c r="P9" s="34"/>
@@ -1921,13 +2008,13 @@
         <v>10</v>
       </c>
       <c r="AK9" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D10" s="30" t="s">
         <v>5</v>
@@ -1952,12 +2039,12 @@
       <c r="L10" s="32"/>
       <c r="M10" s="32"/>
       <c r="N10" s="32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O10" s="32"/>
       <c r="P10" s="32"/>
       <c r="Q10" s="33" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="R10" s="33"/>
       <c r="S10" s="33"/>
@@ -2010,7 +2097,7 @@
         <v>0</v>
       </c>
       <c r="AK10" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
@@ -2018,7 +2105,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D11" s="30" t="s">
         <v>5</v>
@@ -2048,7 +2135,7 @@
       <c r="O11" s="29"/>
       <c r="P11" s="29"/>
       <c r="Q11" s="29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="R11" s="29"/>
       <c r="S11" s="29"/>
@@ -2092,17 +2179,17 @@
         <v>0</v>
       </c>
       <c r="AG11" s="30" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AH11" s="30"/>
       <c r="AI11" s="22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AK11" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AL11" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.25">
@@ -2110,7 +2197,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D12" s="30" t="s">
         <v>5</v>
@@ -2140,17 +2227,17 @@
       <c r="O12" s="29"/>
       <c r="P12" s="29"/>
       <c r="Q12" s="29" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="R12" s="29"/>
       <c r="S12" s="29"/>
       <c r="T12" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="U12" s="29"/>
       <c r="V12" s="29"/>
       <c r="W12" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="X12" s="29"/>
       <c r="Y12" s="29"/>
@@ -2185,7 +2272,7 @@
         <v>0</v>
       </c>
       <c r="AK12" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
@@ -2193,7 +2280,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D13" s="30" t="s">
         <v>5</v>
@@ -2274,21 +2361,21 @@
         <v>0</v>
       </c>
       <c r="AH13" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="AI13" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="AK13" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="AI13" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="AK13" s="10" t="s">
-        <v>183</v>
-      </c>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A14" s="41">
+      <c r="A14" s="40">
         <v>2</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D14" s="30" t="s">
         <v>5</v>
@@ -2313,7 +2400,7 @@
       <c r="L14" s="29"/>
       <c r="M14" s="29"/>
       <c r="N14" s="29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O14" s="29"/>
       <c r="P14" s="29"/>
@@ -2351,7 +2438,7 @@
         <v>0</v>
       </c>
       <c r="AB14" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AC14" s="29"/>
       <c r="AD14" s="29"/>
@@ -2361,13 +2448,13 @@
       <c r="AH14" s="29"/>
       <c r="AI14" s="29"/>
       <c r="AK14" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A15" s="40"/>
+      <c r="B15" s="7" t="s">
         <v>153</v>
-      </c>
-    </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A15" s="41"/>
-      <c r="B15" s="7" t="s">
-        <v>154</v>
       </c>
       <c r="D15" s="30" t="s">
         <v>5</v>
@@ -2392,7 +2479,7 @@
       <c r="L15" s="29"/>
       <c r="M15" s="29"/>
       <c r="N15" s="29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O15" s="29"/>
       <c r="P15" s="29"/>
@@ -2406,7 +2493,7 @@
         <v>10</v>
       </c>
       <c r="T15" s="29" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="U15" s="29"/>
       <c r="V15" s="29"/>
@@ -2424,13 +2511,13 @@
       <c r="AH15" s="29"/>
       <c r="AI15" s="29"/>
       <c r="AK15" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
+      <c r="A16" s="40"/>
       <c r="B16" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D16" s="30" t="s">
         <v>5</v>
@@ -2455,7 +2542,7 @@
       <c r="L16" s="29"/>
       <c r="M16" s="29"/>
       <c r="N16" s="29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O16" s="29"/>
       <c r="P16" s="29"/>
@@ -2469,7 +2556,7 @@
         <v>10</v>
       </c>
       <c r="T16" s="29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="U16" s="29"/>
       <c r="V16" s="29"/>
@@ -2487,13 +2574,13 @@
       <c r="AH16" s="29"/>
       <c r="AI16" s="29"/>
       <c r="AK16" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A17" s="41"/>
+      <c r="A17" s="40"/>
       <c r="B17" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D17" s="30" t="s">
         <v>5</v>
@@ -2510,7 +2597,7 @@
         <v>1</v>
       </c>
       <c r="J17" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K17" s="29" t="s">
         <v>7</v>
@@ -2542,7 +2629,7 @@
       <c r="AH17" s="29"/>
       <c r="AI17" s="29"/>
       <c r="AK17" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
@@ -2567,7 +2654,7 @@
         <v>10</v>
       </c>
       <c r="J18" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K18" s="29" t="s">
         <v>7</v>
@@ -2575,7 +2662,7 @@
       <c r="L18" s="29"/>
       <c r="M18" s="29"/>
       <c r="N18" s="29" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O18" s="29"/>
       <c r="P18" s="29"/>
@@ -2599,7 +2686,7 @@
       <c r="AH18" s="29"/>
       <c r="AI18" s="29"/>
       <c r="AK18" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
@@ -2607,7 +2694,7 @@
         <v>6</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D19" s="30" t="s">
         <v>5</v>
@@ -2627,7 +2714,7 @@
         <v>0</v>
       </c>
       <c r="K19" s="34" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L19" s="34"/>
       <c r="M19" s="34"/>
@@ -2656,7 +2743,7 @@
       <c r="AH19" s="29"/>
       <c r="AI19" s="29"/>
       <c r="AK19" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.25">
@@ -2664,7 +2751,7 @@
         <v>7</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D20" s="30" t="s">
         <v>5</v>
@@ -2684,7 +2771,7 @@
         <v>1</v>
       </c>
       <c r="K20" s="34" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L20" s="34"/>
       <c r="M20" s="34"/>
@@ -2698,7 +2785,7 @@
         <v>0</v>
       </c>
       <c r="Q20" s="36" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="R20" s="36"/>
       <c r="S20" s="36"/>
@@ -2706,7 +2793,7 @@
       <c r="U20" s="36"/>
       <c r="V20" s="36"/>
       <c r="W20" s="29" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="X20" s="29"/>
       <c r="Y20" s="29"/>
@@ -2721,7 +2808,7 @@
       <c r="AH20" s="29"/>
       <c r="AI20" s="29"/>
       <c r="AK20" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
@@ -2729,7 +2816,7 @@
         <v>8</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D21" s="30" t="s">
         <v>5</v>
@@ -2796,7 +2883,7 @@
         <v>0</v>
       </c>
       <c r="AB21" s="29" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AC21" s="29"/>
       <c r="AD21" s="29"/>
@@ -2806,7 +2893,7 @@
       <c r="AH21" s="29"/>
       <c r="AI21" s="29"/>
       <c r="AK21" s="10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.25">
@@ -2814,7 +2901,7 @@
         <v>9</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D22" s="30" t="s">
         <v>5</v>
@@ -2881,7 +2968,7 @@
         <v>0</v>
       </c>
       <c r="AB22" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AC22" s="29"/>
       <c r="AD22" s="29"/>
@@ -2891,7 +2978,7 @@
       <c r="AH22" s="29"/>
       <c r="AI22" s="29"/>
       <c r="AK22" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
@@ -2899,7 +2986,7 @@
         <v>10</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D23" s="30" t="s">
         <v>5</v>
@@ -2966,7 +3053,7 @@
         <v>1</v>
       </c>
       <c r="AB23" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AC23" s="29"/>
       <c r="AD23" s="29"/>
@@ -2976,7 +3063,7 @@
       <c r="AH23" s="29"/>
       <c r="AI23" s="29"/>
       <c r="AK23" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
@@ -2984,7 +3071,7 @@
         <v>11</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D24" s="30" t="s">
         <v>5</v>
@@ -3081,7 +3168,7 @@
         <v>12</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D25" s="30" t="s">
         <v>5</v>
@@ -3152,7 +3239,7 @@
         <v>1</v>
       </c>
       <c r="AB25" s="29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AC25" s="29"/>
       <c r="AD25" s="29"/>
@@ -3822,13 +3909,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.5703125" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.5703125" customWidth="1"/>
     <col min="3" max="8" width="3.42578125" customWidth="1"/>
     <col min="9" max="9" width="2.5703125" customWidth="1"/>
@@ -3838,36 +3925,35 @@
     <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
+    <row r="1" spans="1:15" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="43" t="s">
+        <v>267</v>
+      </c>
+      <c r="B1" s="44">
+        <v>1</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>300</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
-        <v>168</v>
-      </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="40"/>
+      <c r="A2" s="37" t="s">
+        <v>167</v>
+      </c>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="39"/>
       <c r="K2" s="20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3898,21 +3984,21 @@
         <v>14</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="N3" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="O3" s="23" t="s">
         <v>190</v>
-      </c>
-      <c r="O3" s="23" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6">
@@ -3934,24 +4020,24 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="N4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6">
@@ -3973,24 +4059,24 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="N5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6">
@@ -4012,24 +4098,24 @@
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="N6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6">
@@ -4051,24 +4137,24 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="N7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6">
@@ -4090,15 +4176,15 @@
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6">
@@ -4120,21 +4206,21 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="N9" s="19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6">
@@ -4156,21 +4242,21 @@
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="N10" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6">
@@ -4192,15 +4278,15 @@
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N11" s="19" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6">
@@ -4222,15 +4308,15 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N12" s="19" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6">
@@ -4252,18 +4338,18 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6">
@@ -4285,18 +4371,18 @@
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6">
@@ -4318,18 +4404,18 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6">
@@ -4351,18 +4437,18 @@
         <v>0</v>
       </c>
       <c r="J16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6">
@@ -4384,18 +4470,18 @@
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L17" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6">
@@ -4417,18 +4503,18 @@
         <v>0</v>
       </c>
       <c r="J18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6">
@@ -4450,18 +4536,18 @@
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6">
@@ -4483,18 +4569,18 @@
         <v>0</v>
       </c>
       <c r="J20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="6">
@@ -4516,18 +4602,18 @@
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="6">
@@ -4549,18 +4635,18 @@
         <v>0</v>
       </c>
       <c r="J22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="6">
@@ -4582,18 +4668,18 @@
         <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="6">
@@ -4615,18 +4701,18 @@
         <v>0</v>
       </c>
       <c r="J24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L24" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="6">
@@ -4648,18 +4734,18 @@
         <v>0</v>
       </c>
       <c r="J25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="6">
@@ -4681,18 +4767,18 @@
         <v>1</v>
       </c>
       <c r="J26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L26" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="6">
@@ -4714,18 +4800,18 @@
         <v>0</v>
       </c>
       <c r="J27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="6">
@@ -4747,18 +4833,18 @@
         <v>1</v>
       </c>
       <c r="J28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L28" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="6">
@@ -4780,18 +4866,18 @@
         <v>0</v>
       </c>
       <c r="J29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K29" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="6">
@@ -4813,18 +4899,18 @@
         <v>1</v>
       </c>
       <c r="J30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K30" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L30" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="6">
@@ -4846,18 +4932,18 @@
         <v>0</v>
       </c>
       <c r="J31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K31" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L31" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="6">
@@ -4879,18 +4965,18 @@
         <v>1</v>
       </c>
       <c r="J32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L32" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="6">
@@ -4912,18 +4998,18 @@
         <v>0</v>
       </c>
       <c r="J33" t="s">
+        <v>207</v>
+      </c>
+      <c r="K33" t="s">
         <v>208</v>
       </c>
-      <c r="K33" t="s">
-        <v>209</v>
-      </c>
       <c r="L33" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="6">
@@ -4945,18 +5031,18 @@
         <v>1</v>
       </c>
       <c r="J34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K34" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L34" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="6">
@@ -4978,18 +5064,18 @@
         <v>0</v>
       </c>
       <c r="J35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K35" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L35" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="6">
@@ -5011,18 +5097,18 @@
         <v>1</v>
       </c>
       <c r="J36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L36" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="6">
@@ -5044,18 +5130,18 @@
         <v>0</v>
       </c>
       <c r="J37" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K37" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L37" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B38" s="6"/>
       <c r="C38" s="6">
@@ -5077,18 +5163,18 @@
         <v>1</v>
       </c>
       <c r="J38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K38" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L38" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="6">
@@ -5110,18 +5196,18 @@
         <v>0</v>
       </c>
       <c r="J39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L39" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B40" s="6"/>
       <c r="C40" s="6">
@@ -5143,18 +5229,18 @@
         <v>1</v>
       </c>
       <c r="J40" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K40" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L40" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B41" s="14"/>
       <c r="C41" s="14">
@@ -5177,7 +5263,7 @@
       </c>
       <c r="I41" s="17"/>
       <c r="J41" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -5191,8 +5277,7 @@
       <c r="H42" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:D1"/>
+  <mergeCells count="1">
     <mergeCell ref="A2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5201,31 +5286,31 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="26" customWidth="1"/>
-    <col min="2" max="2" width="3.42578125" style="25" customWidth="1"/>
-    <col min="3" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="41.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="141" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="108.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="43" t="s">
+        <v>267</v>
+      </c>
+      <c r="B1" s="44">
+        <v>2</v>
+      </c>
+      <c r="C1" s="42" t="s">
         <v>268</v>
-      </c>
-      <c r="B1" s="45">
-        <v>2</v>
-      </c>
-      <c r="C1" s="43" t="s">
-        <v>269</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -5233,9 +5318,9 @@
     </row>
     <row r="2" spans="1:6" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="28" t="s">
-        <v>221</v>
-      </c>
-      <c r="B2" s="46"/>
+        <v>220</v>
+      </c>
+      <c r="B2" s="45"/>
       <c r="C2" s="28"/>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
@@ -5243,131 +5328,131 @@
     </row>
     <row r="3" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
-        <v>214</v>
-      </c>
-      <c r="B3" s="47"/>
+        <v>213</v>
+      </c>
+      <c r="B3" s="46"/>
       <c r="C3" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E10" t="s">
+        <v>242</v>
+      </c>
+      <c r="F10" t="s">
         <v>243</v>
-      </c>
-      <c r="F10" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="28" t="s">
-        <v>222</v>
-      </c>
-      <c r="B11" s="46"/>
+        <v>221</v>
+      </c>
+      <c r="B11" s="45"/>
       <c r="C11" s="28"/>
       <c r="D11" s="28"/>
       <c r="E11" s="28"/>
@@ -5375,124 +5460,551 @@
     </row>
     <row r="12" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="27" t="s">
-        <v>214</v>
-      </c>
-      <c r="B12" s="47"/>
+        <v>213</v>
+      </c>
+      <c r="B12" s="46"/>
       <c r="C12" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C13" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E14" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C15" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E15" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D16" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="26" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C17" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D17" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C18" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D18" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="44" t="s">
-        <v>268</v>
-      </c>
-      <c r="B19" s="45">
+      <c r="A19" s="43" t="s">
+        <v>267</v>
+      </c>
+      <c r="B19" s="44">
         <v>3</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="B20" s="46"/>
+      <c r="C20" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="26" t="s">
+        <v>270</v>
+      </c>
+      <c r="C21" t="s">
+        <v>272</v>
+      </c>
+      <c r="D21" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="43" t="s">
+        <v>267</v>
+      </c>
+      <c r="B22" s="44">
+        <v>4</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="B23" s="46"/>
+      <c r="C23" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="26" t="s">
+        <v>273</v>
+      </c>
+      <c r="C24" t="s">
+        <v>275</v>
+      </c>
+      <c r="D24" t="s">
+        <v>274</v>
+      </c>
+      <c r="E24" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="26" t="s">
+        <v>277</v>
+      </c>
+      <c r="C25" t="s">
+        <v>275</v>
+      </c>
+      <c r="D25" t="s">
+        <v>274</v>
+      </c>
+      <c r="E25" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="C26" t="s">
+        <v>275</v>
+      </c>
+      <c r="D26" t="s">
+        <v>274</v>
+      </c>
+      <c r="E26" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="26" t="s">
+        <v>279</v>
+      </c>
+      <c r="C27" t="s">
+        <v>275</v>
+      </c>
+      <c r="D27" t="s">
+        <v>274</v>
+      </c>
+      <c r="E27" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="43" t="s">
+        <v>267</v>
+      </c>
+      <c r="B28" s="44">
+        <v>5</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="B29" s="46"/>
+      <c r="C29" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F29" s="23" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="26" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="26" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="26" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="26" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="43" t="s">
+        <v>267</v>
+      </c>
+      <c r="B34" s="44">
+        <v>6</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+    </row>
+    <row r="35" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="B35" s="46"/>
+      <c r="C35" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F35" s="23" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="26" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="26" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="26" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="26" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="26" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="26" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="26" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="43" t="s">
+        <v>267</v>
+      </c>
+      <c r="B43" s="44">
+        <v>7</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+    </row>
+    <row r="44" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="B44" s="46"/>
+      <c r="C44" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F44" s="23" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="43" t="s">
+        <v>267</v>
+      </c>
+      <c r="B46" s="44">
+        <v>8</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+    </row>
+    <row r="47" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="B47" s="46"/>
+      <c r="C47" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F47" s="23" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="43" t="s">
+        <v>267</v>
+      </c>
+      <c r="B49" s="44">
+        <v>9</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+    </row>
+    <row r="50" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="B50" s="46"/>
+      <c r="C50" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F50" s="23" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="43" t="s">
+        <v>267</v>
+      </c>
+      <c r="B52" s="44">
+        <v>10</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+    </row>
+    <row r="53" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="B53" s="46"/>
+      <c r="C53" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F53" s="23" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="43" t="s">
+        <v>267</v>
+      </c>
+      <c r="B55" s="44">
+        <v>11</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+    </row>
+    <row r="56" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="B56" s="46"/>
+      <c r="C56" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F56" s="23" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="43" t="s">
+        <v>267</v>
+      </c>
+      <c r="B58" s="44">
+        <v>12</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+    </row>
+    <row r="59" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="B59" s="46"/>
+      <c r="C59" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F59" s="23" t="s">
+        <v>233</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5517,7 +6029,7 @@
   <sheetData>
     <row r="1" spans="1:36" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -5694,34 +6206,34 @@
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0</v>
+      </c>
+      <c r="G5" s="12">
+        <v>0</v>
+      </c>
+      <c r="H5" s="12">
+        <v>0</v>
+      </c>
+      <c r="I5" s="12">
+        <v>0</v>
+      </c>
+      <c r="J5" s="6">
+        <v>1</v>
+      </c>
+      <c r="K5" s="29" t="s">
         <v>98</v>
-      </c>
-      <c r="C5" s="6">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6">
-        <v>0</v>
-      </c>
-      <c r="G5" s="12">
-        <v>0</v>
-      </c>
-      <c r="H5" s="12">
-        <v>0</v>
-      </c>
-      <c r="I5" s="12">
-        <v>0</v>
-      </c>
-      <c r="J5" s="6">
-        <v>1</v>
-      </c>
-      <c r="K5" s="29" t="s">
-        <v>99</v>
       </c>
       <c r="L5" s="29"/>
       <c r="M5" s="29"/>
@@ -5750,7 +6262,7 @@
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C6" s="6">
         <v>0</v>
@@ -5777,7 +6289,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L6" s="29"/>
       <c r="M6" s="29"/>
@@ -5787,7 +6299,7 @@
       <c r="Q6" s="29"/>
       <c r="R6" s="29"/>
       <c r="S6" s="29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="T6" s="29"/>
       <c r="U6" s="29"/>
@@ -5797,7 +6309,7 @@
       <c r="Y6" s="29"/>
       <c r="Z6" s="29"/>
       <c r="AA6" s="29" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AB6" s="29"/>
       <c r="AC6" s="29"/>
@@ -6971,7 +7483,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -7046,7 +7558,7 @@
         <v>0</v>
       </c>
       <c r="T3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -7068,12 +7580,12 @@
       <c r="Q4" s="35"/>
       <c r="R4" s="35"/>
       <c r="T4" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C5" s="6">
         <v>0</v>
@@ -7121,15 +7633,15 @@
         <v>1</v>
       </c>
       <c r="R5" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="T5" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C6" s="24">
         <v>0</v>
@@ -7177,13 +7689,13 @@
         <v>0</v>
       </c>
       <c r="R6" s="24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="T6" s="10"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C7" s="6">
         <v>0</v>
@@ -7210,7 +7722,7 @@
         <v>1</v>
       </c>
       <c r="K7" s="29" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L7" s="29"/>
       <c r="M7" s="29"/>
@@ -7223,7 +7735,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C8" s="6">
         <v>0</v>
@@ -7247,10 +7759,10 @@
         <v>1</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K8" s="29" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L8" s="29"/>
       <c r="M8" s="29"/>
@@ -7263,7 +7775,7 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C9" s="6">
         <v>0</v>
@@ -7287,10 +7799,10 @@
         <v>0</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K9" s="29" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L9" s="29"/>
       <c r="M9" s="29"/>
@@ -7303,7 +7815,7 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C10" s="6">
         <v>0</v>
@@ -7327,10 +7839,10 @@
         <v>1</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K10" s="29" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L10" s="29"/>
       <c r="M10" s="29"/>

</xml_diff>

<commit_message>
Instruction set doc: added dec/hex lookup for math opcodes
</commit_message>
<xml_diff>
--- a/doc/RiscyInstSet32Bit.xlsx
+++ b/doc/RiscyInstSet32Bit.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="14715" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="14715"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
     <sheet name="Chapter 1. Math Opcodes" sheetId="2" r:id="rId2"/>
     <sheet name="Instructions" sheetId="6" r:id="rId3"/>
-    <sheet name="BIOS Call" sheetId="4" r:id="rId4"/>
-    <sheet name="StdGrAd Call" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId4"/>
+    <sheet name="BIOS Call" sheetId="4" r:id="rId5"/>
+    <sheet name="StdGrAd Call" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="309">
   <si>
     <t>Description</t>
   </si>
@@ -594,9 +595,6 @@
     <t>C: 0-Load, 1-Store</t>
   </si>
   <si>
-    <t>Conditional jump</t>
-  </si>
-  <si>
     <t>Conditional suffix</t>
   </si>
   <si>
@@ -931,6 +929,33 @@
   </si>
   <si>
     <t>Mathematical Opcodes</t>
+  </si>
+  <si>
+    <t>32 Bits; 8 General, 4 Special</t>
+  </si>
+  <si>
+    <t>(Un)Conditional jump</t>
+  </si>
+  <si>
+    <t>Feature Identifier</t>
+  </si>
+  <si>
+    <t>Always return TRUE</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
+  <si>
+    <t>Memory Banking: 16 Slots</t>
+  </si>
+  <si>
+    <t>Memory Banking: 32 Slots</t>
+  </si>
+  <si>
+    <t>Memory Banking: 64 Slots</t>
+  </si>
+  <si>
+    <t>Hex</t>
   </si>
 </sst>
 </file>
@@ -1138,7 +1163,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="6" applyFont="1"/>
@@ -1259,6 +1284,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1549,8 +1577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1652,8 +1680,8 @@
         <v>16</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="10">
-        <v>8</v>
+      <c r="D4" s="10" t="s">
+        <v>300</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -1692,7 +1720,7 @@
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
@@ -1735,12 +1763,12 @@
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="AK6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>0</v>
@@ -2097,7 +2125,7 @@
         <v>0</v>
       </c>
       <c r="AK10" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
@@ -2686,7 +2714,7 @@
       <c r="AH18" s="29"/>
       <c r="AI18" s="29"/>
       <c r="AK18" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
@@ -2694,7 +2722,7 @@
         <v>6</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>188</v>
+        <v>301</v>
       </c>
       <c r="D19" s="30" t="s">
         <v>5</v>
@@ -2743,7 +2771,7 @@
       <c r="AH19" s="29"/>
       <c r="AI19" s="29"/>
       <c r="AK19" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.25">
@@ -2751,7 +2779,7 @@
         <v>7</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D20" s="30" t="s">
         <v>5</v>
@@ -2785,7 +2813,7 @@
         <v>0</v>
       </c>
       <c r="Q20" s="36" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="R20" s="36"/>
       <c r="S20" s="36"/>
@@ -2793,7 +2821,7 @@
       <c r="U20" s="36"/>
       <c r="V20" s="36"/>
       <c r="W20" s="29" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="X20" s="29"/>
       <c r="Y20" s="29"/>
@@ -2808,7 +2836,7 @@
       <c r="AH20" s="29"/>
       <c r="AI20" s="29"/>
       <c r="AK20" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
@@ -2816,7 +2844,7 @@
         <v>8</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D21" s="30" t="s">
         <v>5</v>
@@ -2883,7 +2911,7 @@
         <v>0</v>
       </c>
       <c r="AB21" s="29" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AC21" s="29"/>
       <c r="AD21" s="29"/>
@@ -2893,7 +2921,7 @@
       <c r="AH21" s="29"/>
       <c r="AI21" s="29"/>
       <c r="AK21" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.25">
@@ -3907,10 +3935,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O42"/>
+  <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3918,28 +3946,29 @@
     <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.5703125" customWidth="1"/>
     <col min="3" max="8" width="3.42578125" customWidth="1"/>
-    <col min="9" max="9" width="2.5703125" customWidth="1"/>
-    <col min="11" max="11" width="45.7109375" customWidth="1"/>
-    <col min="13" max="13" width="3.42578125" customWidth="1"/>
-    <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="6" customWidth="1"/>
+    <col min="11" max="11" width="2.5703125" customWidth="1"/>
+    <col min="13" max="13" width="45.7109375" customWidth="1"/>
+    <col min="15" max="15" width="3.42578125" customWidth="1"/>
+    <col min="16" max="16" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="43" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B1" s="44">
         <v>1</v>
       </c>
       <c r="C1" s="42" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
         <v>167</v>
       </c>
@@ -3951,12 +3980,14 @@
       <c r="G2" s="38"/>
       <c r="H2" s="38"/>
       <c r="I2" s="38"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="20" t="s">
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="20" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -3979,24 +4010,30 @@
       <c r="H3" s="4">
         <v>0</v>
       </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3" t="s">
+      <c r="I3" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="P3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q3" s="23" t="s">
         <v>189</v>
       </c>
-      <c r="O3" s="23" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>18</v>
       </c>
@@ -4019,23 +4056,31 @@
       <c r="H4" s="6">
         <v>0</v>
       </c>
-      <c r="J4" t="s">
+      <c r="I4" s="24">
+        <f>_xlfn.DECIMAL(CONCATENATE(C4,D4,E4,F4,G4,H4),2)</f>
+        <v>32</v>
+      </c>
+      <c r="J4" s="24" t="str">
+        <f>DEC2HEX(I4,2)&amp;"h"</f>
+        <v>20h</v>
+      </c>
+      <c r="L4" t="s">
         <v>17</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>100</v>
       </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>169</v>
       </c>
-      <c r="N4" t="s">
-        <v>191</v>
-      </c>
-      <c r="O4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>19</v>
       </c>
@@ -4058,23 +4103,31 @@
       <c r="H5" s="6">
         <v>1</v>
       </c>
-      <c r="J5" t="s">
+      <c r="I5" s="24">
+        <f t="shared" ref="I5:I41" si="0">_xlfn.DECIMAL(CONCATENATE(C5,D5,E5,F5,G5,H5),2)</f>
+        <v>33</v>
+      </c>
+      <c r="J5" s="24" t="str">
+        <f t="shared" ref="J5:J41" si="1">DEC2HEX(I5,2)&amp;"h"</f>
+        <v>21h</v>
+      </c>
+      <c r="L5" t="s">
         <v>47</v>
       </c>
-      <c r="K5" t="s">
+      <c r="M5" t="s">
         <v>101</v>
       </c>
-      <c r="L5" t="s">
+      <c r="N5" t="s">
         <v>169</v>
       </c>
-      <c r="N5" t="s">
-        <v>192</v>
-      </c>
-      <c r="O5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>75</v>
       </c>
@@ -4097,23 +4150,31 @@
       <c r="H6" s="6">
         <v>0</v>
       </c>
-      <c r="J6" t="s">
+      <c r="I6" s="24">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="J6" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>22h</v>
+      </c>
+      <c r="L6" t="s">
         <v>77</v>
       </c>
-      <c r="K6" t="s">
+      <c r="M6" t="s">
         <v>102</v>
       </c>
-      <c r="L6" t="s">
+      <c r="N6" t="s">
         <v>169</v>
       </c>
-      <c r="N6" t="s">
-        <v>193</v>
-      </c>
-      <c r="O6" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P6" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>76</v>
       </c>
@@ -4136,23 +4197,31 @@
       <c r="H7" s="6">
         <v>1</v>
       </c>
-      <c r="J7" t="s">
+      <c r="I7" s="24">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="J7" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>23h</v>
+      </c>
+      <c r="L7" t="s">
         <v>78</v>
       </c>
-      <c r="K7" t="s">
+      <c r="M7" t="s">
         <v>103</v>
       </c>
-      <c r="L7" t="s">
+      <c r="N7" t="s">
         <v>169</v>
       </c>
-      <c r="N7" t="s">
-        <v>194</v>
-      </c>
-      <c r="O7" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P7" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>92</v>
       </c>
@@ -4175,14 +4244,22 @@
       <c r="H8" s="6">
         <v>0</v>
       </c>
-      <c r="J8" t="s">
+      <c r="I8" s="24">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="J8" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>24h</v>
+      </c>
+      <c r="L8" t="s">
         <v>93</v>
       </c>
-      <c r="K8" t="s">
+      <c r="M8" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>174</v>
       </c>
@@ -4205,20 +4282,28 @@
       <c r="H9" s="6">
         <v>1</v>
       </c>
-      <c r="J9" t="s">
+      <c r="I9" s="24">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="J9" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>25h</v>
+      </c>
+      <c r="L9" t="s">
         <v>172</v>
       </c>
-      <c r="K9" t="s">
-        <v>205</v>
-      </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
+        <v>204</v>
+      </c>
+      <c r="N9" t="s">
         <v>170</v>
       </c>
-      <c r="N9" s="19" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P9" s="19" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>175</v>
       </c>
@@ -4241,20 +4326,28 @@
       <c r="H10" s="6">
         <v>0</v>
       </c>
-      <c r="J10" t="s">
+      <c r="I10" s="24">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="J10" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>26h</v>
+      </c>
+      <c r="L10" t="s">
         <v>173</v>
       </c>
-      <c r="K10" t="s">
-        <v>206</v>
-      </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
+        <v>205</v>
+      </c>
+      <c r="N10" t="s">
         <v>169</v>
       </c>
-      <c r="N10" s="19" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P10" s="19" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>79</v>
       </c>
@@ -4277,14 +4370,22 @@
       <c r="H11" s="6">
         <v>0</v>
       </c>
-      <c r="J11" t="s">
+      <c r="I11" s="24">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="J11" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>3Eh</v>
+      </c>
+      <c r="L11" t="s">
         <v>80</v>
       </c>
-      <c r="N11" s="19" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P11" s="19" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>81</v>
       </c>
@@ -4307,14 +4408,22 @@
       <c r="H12" s="6">
         <v>1</v>
       </c>
-      <c r="J12" t="s">
+      <c r="I12" s="24">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="J12" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>3Fh</v>
+      </c>
+      <c r="L12" t="s">
         <v>82</v>
       </c>
-      <c r="N12" s="19" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P12" s="19" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>20</v>
       </c>
@@ -4337,17 +4446,25 @@
       <c r="H13" s="6">
         <v>1</v>
       </c>
-      <c r="J13" t="s">
+      <c r="I13" s="24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J13" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>01h</v>
+      </c>
+      <c r="L13" t="s">
         <v>48</v>
       </c>
-      <c r="K13" t="s">
+      <c r="M13" t="s">
         <v>106</v>
       </c>
-      <c r="L13" t="s">
+      <c r="N13" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>21</v>
       </c>
@@ -4370,17 +4487,25 @@
       <c r="H14" s="6">
         <v>0</v>
       </c>
-      <c r="J14" t="s">
+      <c r="I14" s="24">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J14" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>02h</v>
+      </c>
+      <c r="L14" t="s">
         <v>49</v>
       </c>
-      <c r="K14" t="s">
+      <c r="M14" t="s">
         <v>107</v>
       </c>
-      <c r="L14" t="s">
+      <c r="N14" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>22</v>
       </c>
@@ -4403,17 +4528,25 @@
       <c r="H15" s="6">
         <v>1</v>
       </c>
-      <c r="J15" t="s">
+      <c r="I15" s="24">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J15" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>03h</v>
+      </c>
+      <c r="L15" t="s">
         <v>50</v>
       </c>
-      <c r="K15" t="s">
+      <c r="M15" t="s">
         <v>108</v>
       </c>
-      <c r="L15" t="s">
+      <c r="N15" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>23</v>
       </c>
@@ -4436,17 +4569,25 @@
       <c r="H16" s="6">
         <v>0</v>
       </c>
-      <c r="J16" t="s">
+      <c r="I16" s="24">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J16" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>04h</v>
+      </c>
+      <c r="L16" t="s">
         <v>51</v>
       </c>
-      <c r="K16" t="s">
+      <c r="M16" t="s">
         <v>109</v>
       </c>
-      <c r="L16" t="s">
+      <c r="N16" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>24</v>
       </c>
@@ -4469,17 +4610,25 @@
       <c r="H17" s="6">
         <v>1</v>
       </c>
-      <c r="J17" t="s">
+      <c r="I17" s="24">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="J17" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>05h</v>
+      </c>
+      <c r="L17" t="s">
         <v>52</v>
       </c>
-      <c r="K17" t="s">
+      <c r="M17" t="s">
         <v>110</v>
       </c>
-      <c r="L17" t="s">
+      <c r="N17" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>25</v>
       </c>
@@ -4502,17 +4651,25 @@
       <c r="H18" s="6">
         <v>0</v>
       </c>
-      <c r="J18" t="s">
+      <c r="I18" s="24">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="J18" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>06h</v>
+      </c>
+      <c r="L18" t="s">
         <v>53</v>
       </c>
-      <c r="K18" t="s">
+      <c r="M18" t="s">
         <v>111</v>
       </c>
-      <c r="L18" t="s">
+      <c r="N18" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>26</v>
       </c>
@@ -4535,17 +4692,25 @@
       <c r="H19" s="6">
         <v>1</v>
       </c>
-      <c r="J19" t="s">
+      <c r="I19" s="24">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J19" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>07h</v>
+      </c>
+      <c r="L19" t="s">
         <v>54</v>
       </c>
-      <c r="K19" t="s">
+      <c r="M19" t="s">
         <v>112</v>
       </c>
-      <c r="L19" t="s">
+      <c r="N19" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>27</v>
       </c>
@@ -4568,17 +4733,25 @@
       <c r="H20" s="6">
         <v>0</v>
       </c>
-      <c r="J20" t="s">
+      <c r="I20" s="24">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J20" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>08h</v>
+      </c>
+      <c r="L20" t="s">
         <v>55</v>
       </c>
-      <c r="K20" t="s">
+      <c r="M20" t="s">
         <v>113</v>
       </c>
-      <c r="L20" t="s">
+      <c r="N20" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>28</v>
       </c>
@@ -4601,17 +4774,25 @@
       <c r="H21" s="6">
         <v>1</v>
       </c>
-      <c r="J21" t="s">
+      <c r="I21" s="24">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J21" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>09h</v>
+      </c>
+      <c r="L21" t="s">
         <v>56</v>
       </c>
-      <c r="K21" t="s">
+      <c r="M21" t="s">
         <v>114</v>
       </c>
-      <c r="L21" t="s">
+      <c r="N21" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>29</v>
       </c>
@@ -4634,17 +4815,25 @@
       <c r="H22" s="6">
         <v>0</v>
       </c>
-      <c r="J22" t="s">
+      <c r="I22" s="24">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="J22" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>0Ah</v>
+      </c>
+      <c r="L22" t="s">
         <v>57</v>
       </c>
-      <c r="K22" t="s">
+      <c r="M22" t="s">
         <v>115</v>
       </c>
-      <c r="L22" t="s">
+      <c r="N22" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>30</v>
       </c>
@@ -4667,17 +4856,25 @@
       <c r="H23" s="6">
         <v>1</v>
       </c>
-      <c r="J23" t="s">
+      <c r="I23" s="24">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="J23" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>0Bh</v>
+      </c>
+      <c r="L23" t="s">
         <v>58</v>
       </c>
-      <c r="K23" t="s">
+      <c r="M23" t="s">
         <v>116</v>
       </c>
-      <c r="L23" t="s">
+      <c r="N23" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>31</v>
       </c>
@@ -4700,17 +4897,25 @@
       <c r="H24" s="6">
         <v>0</v>
       </c>
-      <c r="J24" t="s">
+      <c r="I24" s="24">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J24" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>0Ch</v>
+      </c>
+      <c r="L24" t="s">
         <v>59</v>
       </c>
-      <c r="K24" t="s">
+      <c r="M24" t="s">
         <v>117</v>
       </c>
-      <c r="L24" t="s">
+      <c r="N24" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>32</v>
       </c>
@@ -4733,17 +4938,25 @@
       <c r="H25" s="6">
         <v>0</v>
       </c>
-      <c r="J25" t="s">
+      <c r="I25" s="24">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="J25" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>10h</v>
+      </c>
+      <c r="L25" t="s">
         <v>60</v>
       </c>
-      <c r="K25" t="s">
+      <c r="M25" t="s">
         <v>128</v>
       </c>
-      <c r="L25" t="s">
+      <c r="N25" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>33</v>
       </c>
@@ -4766,17 +4979,25 @@
       <c r="H26" s="6">
         <v>1</v>
       </c>
-      <c r="J26" t="s">
+      <c r="I26" s="24">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="J26" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>11h</v>
+      </c>
+      <c r="L26" t="s">
         <v>61</v>
       </c>
-      <c r="K26" t="s">
+      <c r="M26" t="s">
         <v>129</v>
       </c>
-      <c r="L26" t="s">
+      <c r="N26" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>34</v>
       </c>
@@ -4799,17 +5020,25 @@
       <c r="H27" s="6">
         <v>0</v>
       </c>
-      <c r="J27" t="s">
+      <c r="I27" s="24">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="J27" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>12h</v>
+      </c>
+      <c r="L27" t="s">
         <v>62</v>
       </c>
-      <c r="K27" t="s">
+      <c r="M27" t="s">
         <v>118</v>
       </c>
-      <c r="L27" t="s">
+      <c r="N27" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>35</v>
       </c>
@@ -4832,17 +5061,25 @@
       <c r="H28" s="6">
         <v>1</v>
       </c>
-      <c r="J28" t="s">
+      <c r="I28" s="24">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="J28" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>13h</v>
+      </c>
+      <c r="L28" t="s">
         <v>63</v>
       </c>
-      <c r="K28" t="s">
+      <c r="M28" t="s">
         <v>119</v>
       </c>
-      <c r="L28" t="s">
+      <c r="N28" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>36</v>
       </c>
@@ -4865,17 +5102,25 @@
       <c r="H29" s="6">
         <v>0</v>
       </c>
-      <c r="J29" t="s">
+      <c r="I29" s="24">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="J29" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>14h</v>
+      </c>
+      <c r="L29" t="s">
         <v>64</v>
       </c>
-      <c r="K29" t="s">
+      <c r="M29" t="s">
         <v>120</v>
       </c>
-      <c r="L29" t="s">
+      <c r="N29" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>37</v>
       </c>
@@ -4898,17 +5143,25 @@
       <c r="H30" s="6">
         <v>1</v>
       </c>
-      <c r="J30" t="s">
+      <c r="I30" s="24">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="J30" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>15h</v>
+      </c>
+      <c r="L30" t="s">
         <v>65</v>
       </c>
-      <c r="K30" t="s">
+      <c r="M30" t="s">
         <v>121</v>
       </c>
-      <c r="L30" t="s">
+      <c r="N30" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>38</v>
       </c>
@@ -4931,17 +5184,25 @@
       <c r="H31" s="6">
         <v>0</v>
       </c>
-      <c r="J31" t="s">
+      <c r="I31" s="24">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="J31" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>16h</v>
+      </c>
+      <c r="L31" t="s">
         <v>66</v>
       </c>
-      <c r="K31" t="s">
+      <c r="M31" t="s">
         <v>122</v>
       </c>
-      <c r="L31" t="s">
+      <c r="N31" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>39</v>
       </c>
@@ -4964,19 +5225,27 @@
       <c r="H32" s="6">
         <v>1</v>
       </c>
-      <c r="J32" t="s">
+      <c r="I32" s="24">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="J32" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>17h</v>
+      </c>
+      <c r="L32" t="s">
         <v>67</v>
       </c>
-      <c r="K32" t="s">
+      <c r="M32" t="s">
         <v>123</v>
       </c>
-      <c r="L32" t="s">
+      <c r="N32" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="6">
@@ -4997,17 +5266,25 @@
       <c r="H33" s="6">
         <v>0</v>
       </c>
-      <c r="J33" t="s">
+      <c r="I33" s="24">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="J33" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>18h</v>
+      </c>
+      <c r="L33" t="s">
+        <v>206</v>
+      </c>
+      <c r="M33" t="s">
         <v>207</v>
       </c>
-      <c r="K33" t="s">
-        <v>208</v>
-      </c>
-      <c r="L33" t="s">
+      <c r="N33" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>40</v>
       </c>
@@ -5030,17 +5307,25 @@
       <c r="H34" s="6">
         <v>1</v>
       </c>
-      <c r="J34" t="s">
+      <c r="I34" s="24">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="J34" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>19h</v>
+      </c>
+      <c r="L34" t="s">
         <v>68</v>
       </c>
-      <c r="K34" t="s">
+      <c r="M34" t="s">
         <v>171</v>
       </c>
-      <c r="L34" t="s">
+      <c r="N34" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>41</v>
       </c>
@@ -5063,17 +5348,25 @@
       <c r="H35" s="6">
         <v>0</v>
       </c>
-      <c r="J35" t="s">
+      <c r="I35" s="24">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="J35" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>1Ah</v>
+      </c>
+      <c r="L35" t="s">
         <v>69</v>
       </c>
-      <c r="K35" t="s">
+      <c r="M35" t="s">
         <v>124</v>
       </c>
-      <c r="L35" t="s">
+      <c r="N35" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>42</v>
       </c>
@@ -5096,17 +5389,25 @@
       <c r="H36" s="6">
         <v>1</v>
       </c>
-      <c r="J36" t="s">
+      <c r="I36" s="24">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="J36" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>1Bh</v>
+      </c>
+      <c r="L36" t="s">
         <v>70</v>
       </c>
-      <c r="K36" t="s">
+      <c r="M36" t="s">
         <v>125</v>
       </c>
-      <c r="L36" t="s">
+      <c r="N36" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>43</v>
       </c>
@@ -5129,17 +5430,25 @@
       <c r="H37" s="6">
         <v>0</v>
       </c>
-      <c r="J37" t="s">
+      <c r="I37" s="24">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="J37" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>1Ch</v>
+      </c>
+      <c r="L37" t="s">
         <v>71</v>
       </c>
-      <c r="K37" t="s">
+      <c r="M37" t="s">
         <v>126</v>
       </c>
-      <c r="L37" t="s">
+      <c r="N37" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>44</v>
       </c>
@@ -5162,17 +5471,25 @@
       <c r="H38" s="6">
         <v>1</v>
       </c>
-      <c r="J38" t="s">
+      <c r="I38" s="24">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="J38" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>1Dh</v>
+      </c>
+      <c r="L38" t="s">
         <v>72</v>
       </c>
-      <c r="K38" t="s">
+      <c r="M38" t="s">
         <v>131</v>
       </c>
-      <c r="L38" t="s">
+      <c r="N38" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>45</v>
       </c>
@@ -5195,17 +5512,25 @@
       <c r="H39" s="6">
         <v>0</v>
       </c>
-      <c r="J39" t="s">
+      <c r="I39" s="24">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="J39" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>1Eh</v>
+      </c>
+      <c r="L39" t="s">
         <v>73</v>
       </c>
-      <c r="K39" t="s">
+      <c r="M39" t="s">
         <v>127</v>
       </c>
-      <c r="L39" t="s">
+      <c r="N39" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>46</v>
       </c>
@@ -5228,17 +5553,25 @@
       <c r="H40" s="6">
         <v>1</v>
       </c>
-      <c r="J40" t="s">
+      <c r="I40" s="24">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="J40" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>1Fh</v>
+      </c>
+      <c r="L40" t="s">
         <v>74</v>
       </c>
-      <c r="K40" t="s">
+      <c r="M40" t="s">
         <v>130</v>
       </c>
-      <c r="L40" t="s">
+      <c r="N40" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
         <v>83</v>
       </c>
@@ -5261,12 +5594,20 @@
       <c r="H41" s="14">
         <v>0</v>
       </c>
-      <c r="I41" s="17"/>
-      <c r="J41" s="17" t="s">
+      <c r="I41" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J41" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>00h</v>
+      </c>
+      <c r="K41" s="17"/>
+      <c r="L41" s="17" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -5275,10 +5616,12 @@
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
       <c r="H42" s="6"/>
+      <c r="I42" s="24"/>
+      <c r="J42" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5304,13 +5647,13 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="43" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B1" s="44">
         <v>2</v>
       </c>
       <c r="C1" s="42" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -5318,7 +5661,7 @@
     </row>
     <row r="2" spans="1:6" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="28" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B2" s="45"/>
       <c r="C2" s="28"/>
@@ -5328,129 +5671,129 @@
     </row>
     <row r="3" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B3" s="46"/>
       <c r="C3" s="3" t="s">
         <v>99</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E10" t="s">
+        <v>241</v>
+      </c>
+      <c r="F10" t="s">
         <v>242</v>
-      </c>
-      <c r="F10" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="28" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B11" s="45"/>
       <c r="C11" s="28"/>
@@ -5460,118 +5803,118 @@
     </row>
     <row r="12" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="27" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B12" s="46"/>
       <c r="C12" s="3" t="s">
         <v>99</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C15" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E15" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D16" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E16" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="26" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C17" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D17" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E17" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C18" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E18" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F18" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="43" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B19" s="44">
         <v>3</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -5579,36 +5922,36 @@
     </row>
     <row r="20" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="27" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B20" s="46"/>
       <c r="C20" s="3" t="s">
         <v>99</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F20" s="23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="26" t="s">
+        <v>269</v>
+      </c>
+      <c r="C21" t="s">
+        <v>271</v>
+      </c>
+      <c r="D21" t="s">
         <v>270</v>
-      </c>
-      <c r="C21" t="s">
-        <v>272</v>
-      </c>
-      <c r="D21" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="43" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B22" s="44">
         <v>4</v>
@@ -5622,81 +5965,81 @@
     </row>
     <row r="23" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="27" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B23" s="46"/>
       <c r="C23" s="3" t="s">
         <v>99</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F23" s="23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="C24" t="s">
+        <v>274</v>
+      </c>
+      <c r="D24" t="s">
         <v>273</v>
       </c>
-      <c r="C24" t="s">
+      <c r="E24" t="s">
         <v>275</v>
-      </c>
-      <c r="D24" t="s">
-        <v>274</v>
-      </c>
-      <c r="E24" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C25" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D25" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E25" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="26" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C26" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D26" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E26" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="26" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C27" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D27" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E27" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="43" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B28" s="44">
         <v>5</v>
@@ -5710,51 +6053,51 @@
     </row>
     <row r="29" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="27" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B29" s="46"/>
       <c r="C29" s="3" t="s">
         <v>99</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F29" s="23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="26" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="26" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="43" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B34" s="44">
         <v>6</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -5762,66 +6105,66 @@
     </row>
     <row r="35" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="27" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B35" s="46"/>
       <c r="C35" s="3" t="s">
         <v>99</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F35" s="23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="26" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="26" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="26" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="26" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="26" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="26" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="26" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="43" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B43" s="44">
         <v>7</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -5829,31 +6172,31 @@
     </row>
     <row r="44" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="27" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B44" s="46"/>
       <c r="C44" s="3" t="s">
         <v>99</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F44" s="23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="43" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B46" s="44">
         <v>8</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -5861,31 +6204,31 @@
     </row>
     <row r="47" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="27" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B47" s="46"/>
       <c r="C47" s="3" t="s">
         <v>99</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F47" s="23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="43" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B49" s="44">
         <v>9</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
@@ -5893,31 +6236,31 @@
     </row>
     <row r="50" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="27" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B50" s="46"/>
       <c r="C50" s="3" t="s">
         <v>99</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F50" s="23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="43" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B52" s="44">
         <v>10</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
@@ -5925,31 +6268,31 @@
     </row>
     <row r="53" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="27" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B53" s="46"/>
       <c r="C53" s="3" t="s">
         <v>99</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F53" s="23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="43" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B55" s="44">
         <v>11</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
@@ -5957,25 +6300,25 @@
     </row>
     <row r="56" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="27" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B56" s="46"/>
       <c r="C56" s="3" t="s">
         <v>99</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F56" s="23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="43" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B58" s="44">
         <v>12</v>
@@ -5989,20 +6332,20 @@
     </row>
     <row r="59" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="27" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B59" s="46"/>
       <c r="C59" s="3" t="s">
         <v>99</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F59" s="23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -6011,6 +6354,309 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="2.42578125" customWidth="1"/>
+    <col min="3" max="10" width="2.85546875" style="25" customWidth="1"/>
+    <col min="11" max="12" width="6" style="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="46">
+        <v>7</v>
+      </c>
+      <c r="D3" s="46">
+        <v>6</v>
+      </c>
+      <c r="E3" s="46">
+        <v>5</v>
+      </c>
+      <c r="F3" s="46">
+        <v>4</v>
+      </c>
+      <c r="G3" s="46">
+        <v>3</v>
+      </c>
+      <c r="H3" s="46">
+        <v>2</v>
+      </c>
+      <c r="I3" s="46">
+        <v>1</v>
+      </c>
+      <c r="J3" s="46">
+        <v>0</v>
+      </c>
+      <c r="K3" s="46" t="s">
+        <v>304</v>
+      </c>
+      <c r="L3" s="46" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>303</v>
+      </c>
+      <c r="C4" s="25">
+        <v>0</v>
+      </c>
+      <c r="D4" s="25">
+        <v>0</v>
+      </c>
+      <c r="E4" s="25">
+        <v>0</v>
+      </c>
+      <c r="F4" s="25">
+        <v>0</v>
+      </c>
+      <c r="G4" s="25">
+        <v>0</v>
+      </c>
+      <c r="H4" s="25">
+        <v>0</v>
+      </c>
+      <c r="I4" s="25">
+        <v>0</v>
+      </c>
+      <c r="J4" s="25">
+        <v>0</v>
+      </c>
+      <c r="K4" s="25">
+        <f>_xlfn.DECIMAL(CONCATENATE(C4,D4,E4,F4,G4,H4,I4,J4),2)</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="25" t="str">
+        <f>DEC2HEX(K4,2)&amp;"h"</f>
+        <v>00h</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>305</v>
+      </c>
+      <c r="C5" s="25">
+        <v>0</v>
+      </c>
+      <c r="D5" s="25">
+        <v>0</v>
+      </c>
+      <c r="E5" s="25">
+        <v>0</v>
+      </c>
+      <c r="F5" s="25">
+        <v>0</v>
+      </c>
+      <c r="G5" s="25">
+        <v>0</v>
+      </c>
+      <c r="H5" s="25">
+        <v>1</v>
+      </c>
+      <c r="I5" s="25">
+        <v>0</v>
+      </c>
+      <c r="J5" s="25">
+        <v>1</v>
+      </c>
+      <c r="K5" s="25">
+        <f t="shared" ref="K5:K7" si="0">_xlfn.DECIMAL(CONCATENATE(C5,D5,E5,F5,G5,H5,I5,J5),2)</f>
+        <v>5</v>
+      </c>
+      <c r="L5" s="25" t="str">
+        <f t="shared" ref="L5:L7" si="1">DEC2HEX(K5,2)&amp;"h"</f>
+        <v>05h</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>306</v>
+      </c>
+      <c r="C6" s="25">
+        <v>0</v>
+      </c>
+      <c r="D6" s="25">
+        <v>0</v>
+      </c>
+      <c r="E6" s="25">
+        <v>0</v>
+      </c>
+      <c r="F6" s="25">
+        <v>0</v>
+      </c>
+      <c r="G6" s="25">
+        <v>0</v>
+      </c>
+      <c r="H6" s="25">
+        <v>1</v>
+      </c>
+      <c r="I6" s="25">
+        <v>1</v>
+      </c>
+      <c r="J6" s="25">
+        <v>0</v>
+      </c>
+      <c r="K6" s="25">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="L6" s="25" t="str">
+        <f t="shared" si="1"/>
+        <v>06h</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
+        <v>307</v>
+      </c>
+      <c r="C7" s="25">
+        <v>0</v>
+      </c>
+      <c r="D7" s="25">
+        <v>0</v>
+      </c>
+      <c r="E7" s="25">
+        <v>0</v>
+      </c>
+      <c r="F7" s="25">
+        <v>0</v>
+      </c>
+      <c r="G7" s="25">
+        <v>0</v>
+      </c>
+      <c r="H7" s="25">
+        <v>1</v>
+      </c>
+      <c r="I7" s="25">
+        <v>1</v>
+      </c>
+      <c r="J7" s="25">
+        <v>1</v>
+      </c>
+      <c r="K7" s="25">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="L7" s="25" t="str">
+        <f t="shared" si="1"/>
+        <v>07h</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="26"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="26"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="26"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="26"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="26"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="26"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="26"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="26"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="26"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="26"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="26"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="26"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="26"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="26"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="26"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="26"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="26"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="26"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="26"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="26"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="26"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="26"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="26"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="26"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="26"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="26"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ40"/>
   <sheetViews>
@@ -7464,7 +8110,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T42"/>
   <sheetViews>
@@ -7641,7 +8287,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C6" s="24">
         <v>0</v>

</xml_diff>

<commit_message>
Assembler: fixed bunch of bad jumps; IF statement works!
</commit_message>
<xml_diff>
--- a/doc/RiscyInstSet32Bit.xlsx
+++ b/doc/RiscyInstSet32Bit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="14715"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="14715" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -850,9 +850,6 @@
     <t>CMP/CMPII</t>
   </si>
   <si>
-    <t>lhand, rhand</t>
-  </si>
-  <si>
     <t>rCMP = rHand - lHand</t>
   </si>
   <si>
@@ -940,9 +937,6 @@
     <t>Feature Identifier</t>
   </si>
   <si>
-    <t>Always return TRUE</t>
-  </si>
-  <si>
     <t>Dec</t>
   </si>
   <si>
@@ -956,6 +950,12 @@
   </si>
   <si>
     <t>Hex</t>
+  </si>
+  <si>
+    <t>lhand, rhand (registers)</t>
+  </si>
+  <si>
+    <t>Always return TRUE (FFFFFFFFh)</t>
   </si>
 </sst>
 </file>
@@ -1577,8 +1577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1681,7 +1681,7 @@
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -2722,7 +2722,7 @@
         <v>6</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D19" s="30" t="s">
         <v>5</v>
@@ -3962,7 +3962,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="42" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4011,10 +4011,10 @@
         <v>0</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3" t="s">
@@ -5632,7 +5632,7 @@
   <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5986,55 +5986,55 @@
         <v>272</v>
       </c>
       <c r="C24" t="s">
+        <v>273</v>
+      </c>
+      <c r="D24" t="s">
+        <v>307</v>
+      </c>
+      <c r="E24" t="s">
         <v>274</v>
-      </c>
-      <c r="D24" t="s">
-        <v>273</v>
-      </c>
-      <c r="E24" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C25" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D25" t="s">
-        <v>273</v>
+        <v>307</v>
       </c>
       <c r="E25" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="26" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C26" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D26" t="s">
-        <v>273</v>
+        <v>307</v>
       </c>
       <c r="E26" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="26" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C27" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D27" t="s">
-        <v>273</v>
+        <v>307</v>
       </c>
       <c r="E27" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -6071,22 +6071,22 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="26" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="26" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -6097,7 +6097,7 @@
         <v>6</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -6123,37 +6123,37 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="26" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="26" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="26" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="26" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="26" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="26" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="26" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -6164,7 +6164,7 @@
         <v>7</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -6196,7 +6196,7 @@
         <v>8</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -6228,7 +6228,7 @@
         <v>9</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
@@ -6260,7 +6260,7 @@
         <v>10</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
@@ -6292,7 +6292,7 @@
         <v>11</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
@@ -6357,8 +6357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6371,7 +6371,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="47" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B1" s="47"/>
       <c r="C1" s="47"/>
@@ -6416,15 +6416,15 @@
         <v>0</v>
       </c>
       <c r="K3" s="46" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="L3" s="46" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="C4" s="25">
         <v>0</v>
@@ -6461,7 +6461,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C5" s="25">
         <v>0</v>
@@ -6498,7 +6498,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C6" s="25">
         <v>0</v>
@@ -6535,7 +6535,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C7" s="25">
         <v>0</v>

</xml_diff>

<commit_message>
subroutine definition (function wo any args) works
</commit_message>
<xml_diff>
--- a/doc/RiscyInstSet32Bit.xlsx
+++ b/doc/RiscyInstSet32Bit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="14715" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="14715" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="311">
   <si>
     <t>Description</t>
   </si>
@@ -956,6 +956,12 @@
   </si>
   <si>
     <t>Always return TRUE (FFFFFFFFh)</t>
+  </si>
+  <si>
+    <t>pc = POPWORDI()</t>
+  </si>
+  <si>
+    <t>PUSHWORDI(pc); JMP(addr)</t>
   </si>
 </sst>
 </file>
@@ -1231,45 +1237,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="7" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1283,6 +1250,45 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
@@ -1872,17 +1878,17 @@
       </c>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A8" s="41">
+      <c r="A8" s="35">
         <v>1</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
       <c r="G8" s="11">
         <v>0</v>
       </c>
@@ -1895,21 +1901,21 @@
       <c r="J8" s="11">
         <v>0</v>
       </c>
-      <c r="K8" s="35" t="s">
+      <c r="K8" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="L8" s="35"/>
-      <c r="M8" s="35"/>
-      <c r="N8" s="35" t="s">
+      <c r="L8" s="40"/>
+      <c r="M8" s="40"/>
+      <c r="N8" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="O8" s="35"/>
-      <c r="P8" s="35"/>
-      <c r="Q8" s="35" t="s">
+      <c r="O8" s="40"/>
+      <c r="P8" s="40"/>
+      <c r="Q8" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="R8" s="35"/>
-      <c r="S8" s="35"/>
+      <c r="R8" s="40"/>
+      <c r="S8" s="40"/>
       <c r="T8" s="12">
         <v>0</v>
       </c>
@@ -1940,28 +1946,28 @@
       <c r="AC8" s="6">
         <v>0</v>
       </c>
-      <c r="AD8" s="35" t="s">
+      <c r="AD8" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="AE8" s="35"/>
-      <c r="AF8" s="35"/>
-      <c r="AG8" s="35"/>
-      <c r="AH8" s="35"/>
-      <c r="AI8" s="35"/>
+      <c r="AE8" s="40"/>
+      <c r="AF8" s="40"/>
+      <c r="AG8" s="40"/>
+      <c r="AH8" s="40"/>
+      <c r="AI8" s="40"/>
       <c r="AK8" s="10" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="18">
         <v>0</v>
       </c>
@@ -1974,19 +1980,19 @@
       <c r="J9" s="18">
         <v>0</v>
       </c>
-      <c r="K9" s="36" t="s">
+      <c r="K9" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="L9" s="36"/>
-      <c r="M9" s="36"/>
-      <c r="N9" s="34" t="s">
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="39" t="s">
         <v>162</v>
       </c>
-      <c r="O9" s="34"/>
-      <c r="P9" s="34"/>
-      <c r="Q9" s="34"/>
-      <c r="R9" s="34"/>
-      <c r="S9" s="34"/>
+      <c r="O9" s="39"/>
+      <c r="P9" s="39"/>
+      <c r="Q9" s="39"/>
+      <c r="R9" s="39"/>
+      <c r="S9" s="39"/>
       <c r="T9" s="12">
         <v>0</v>
       </c>
@@ -2040,15 +2046,15 @@
       </c>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="18">
         <v>0</v>
       </c>
@@ -2061,21 +2067,21 @@
       <c r="J10" s="18">
         <v>0</v>
       </c>
-      <c r="K10" s="32" t="s">
+      <c r="K10" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="32" t="s">
+      <c r="L10" s="41"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="41" t="s">
         <v>161</v>
       </c>
-      <c r="O10" s="32"/>
-      <c r="P10" s="32"/>
-      <c r="Q10" s="33" t="s">
+      <c r="O10" s="41"/>
+      <c r="P10" s="41"/>
+      <c r="Q10" s="42" t="s">
         <v>162</v>
       </c>
-      <c r="R10" s="33"/>
-      <c r="S10" s="33"/>
+      <c r="R10" s="42"/>
+      <c r="S10" s="42"/>
       <c r="T10" s="12">
         <v>0</v>
       </c>
@@ -2135,11 +2141,11 @@
       <c r="B11" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="6">
         <v>0</v>
       </c>
@@ -2152,21 +2158,21 @@
       <c r="J11" s="12">
         <v>0</v>
       </c>
-      <c r="K11" s="29" t="s">
+      <c r="K11" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="L11" s="29"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="29" t="s">
+      <c r="L11" s="38"/>
+      <c r="M11" s="38"/>
+      <c r="N11" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="O11" s="29"/>
-      <c r="P11" s="29"/>
-      <c r="Q11" s="29" t="s">
+      <c r="O11" s="38"/>
+      <c r="P11" s="38"/>
+      <c r="Q11" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="R11" s="29"/>
-      <c r="S11" s="29"/>
+      <c r="R11" s="38"/>
+      <c r="S11" s="38"/>
       <c r="T11" s="6">
         <v>0</v>
       </c>
@@ -2206,10 +2212,10 @@
       <c r="AF11" s="6">
         <v>0</v>
       </c>
-      <c r="AG11" s="30" t="s">
+      <c r="AG11" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="AH11" s="30"/>
+      <c r="AH11" s="36"/>
       <c r="AI11" s="22" t="s">
         <v>89</v>
       </c>
@@ -2227,11 +2233,11 @@
       <c r="B12" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
       <c r="G12" s="6">
         <v>0</v>
       </c>
@@ -2244,31 +2250,31 @@
       <c r="J12" s="12">
         <v>0</v>
       </c>
-      <c r="K12" s="29" t="s">
+      <c r="K12" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29" t="s">
+      <c r="L12" s="38"/>
+      <c r="M12" s="38"/>
+      <c r="N12" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="29" t="s">
+      <c r="O12" s="38"/>
+      <c r="P12" s="38"/>
+      <c r="Q12" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="R12" s="29"/>
-      <c r="S12" s="29"/>
-      <c r="T12" s="29" t="s">
+      <c r="R12" s="38"/>
+      <c r="S12" s="38"/>
+      <c r="T12" s="38" t="s">
         <v>179</v>
       </c>
-      <c r="U12" s="29"/>
-      <c r="V12" s="29"/>
-      <c r="W12" s="29" t="s">
+      <c r="U12" s="38"/>
+      <c r="V12" s="38"/>
+      <c r="W12" s="38" t="s">
         <v>180</v>
       </c>
-      <c r="X12" s="29"/>
-      <c r="Y12" s="29"/>
+      <c r="X12" s="38"/>
+      <c r="Y12" s="38"/>
       <c r="Z12" s="6">
         <v>0</v>
       </c>
@@ -2310,11 +2316,11 @@
       <c r="B13" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="D13" s="30" t="s">
+      <c r="D13" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
       <c r="G13" s="6">
         <v>0</v>
       </c>
@@ -2327,16 +2333,16 @@
       <c r="J13" s="12">
         <v>1</v>
       </c>
-      <c r="K13" s="29" t="s">
+      <c r="K13" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="29" t="s">
+      <c r="L13" s="38"/>
+      <c r="M13" s="38"/>
+      <c r="N13" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="O13" s="29"/>
-      <c r="P13" s="29"/>
+      <c r="O13" s="38"/>
+      <c r="P13" s="38"/>
       <c r="Q13" s="6">
         <v>0</v>
       </c>
@@ -2399,17 +2405,17 @@
       </c>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A14" s="40">
+      <c r="A14" s="34">
         <v>2</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
       <c r="G14" s="6">
         <v>0</v>
       </c>
@@ -2422,16 +2428,16 @@
       <c r="J14" s="12">
         <v>1</v>
       </c>
-      <c r="K14" s="29" t="s">
+      <c r="K14" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="29" t="s">
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
+      <c r="N14" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="O14" s="29"/>
-      <c r="P14" s="29"/>
+      <c r="O14" s="38"/>
+      <c r="P14" s="38"/>
       <c r="Q14" s="6">
         <v>0</v>
       </c>
@@ -2465,30 +2471,30 @@
       <c r="AA14" s="6">
         <v>0</v>
       </c>
-      <c r="AB14" s="29" t="s">
+      <c r="AB14" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="AC14" s="29"/>
-      <c r="AD14" s="29"/>
-      <c r="AE14" s="29"/>
-      <c r="AF14" s="29"/>
-      <c r="AG14" s="29"/>
-      <c r="AH14" s="29"/>
-      <c r="AI14" s="29"/>
+      <c r="AC14" s="38"/>
+      <c r="AD14" s="38"/>
+      <c r="AE14" s="38"/>
+      <c r="AF14" s="38"/>
+      <c r="AG14" s="38"/>
+      <c r="AH14" s="38"/>
+      <c r="AI14" s="38"/>
       <c r="AK14" s="10" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A15" s="40"/>
+      <c r="A15" s="34"/>
       <c r="B15" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="D15" s="30" t="s">
+      <c r="D15" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
       <c r="G15" s="6">
         <v>0</v>
       </c>
@@ -2501,16 +2507,16 @@
       <c r="J15" s="12">
         <v>1</v>
       </c>
-      <c r="K15" s="29" t="s">
+      <c r="K15" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="29" t="s">
+      <c r="L15" s="38"/>
+      <c r="M15" s="38"/>
+      <c r="N15" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="O15" s="29"/>
-      <c r="P15" s="29"/>
+      <c r="O15" s="38"/>
+      <c r="P15" s="38"/>
       <c r="Q15" s="6">
         <v>1</v>
       </c>
@@ -2520,38 +2526,38 @@
       <c r="S15" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="T15" s="29" t="s">
+      <c r="T15" s="38" t="s">
         <v>157</v>
       </c>
-      <c r="U15" s="29"/>
-      <c r="V15" s="29"/>
-      <c r="W15" s="29"/>
-      <c r="X15" s="29"/>
-      <c r="Y15" s="29"/>
-      <c r="Z15" s="29"/>
-      <c r="AA15" s="29"/>
-      <c r="AB15" s="29"/>
-      <c r="AC15" s="29"/>
-      <c r="AD15" s="29"/>
-      <c r="AE15" s="29"/>
-      <c r="AF15" s="29"/>
-      <c r="AG15" s="29"/>
-      <c r="AH15" s="29"/>
-      <c r="AI15" s="29"/>
+      <c r="U15" s="38"/>
+      <c r="V15" s="38"/>
+      <c r="W15" s="38"/>
+      <c r="X15" s="38"/>
+      <c r="Y15" s="38"/>
+      <c r="Z15" s="38"/>
+      <c r="AA15" s="38"/>
+      <c r="AB15" s="38"/>
+      <c r="AC15" s="38"/>
+      <c r="AD15" s="38"/>
+      <c r="AE15" s="38"/>
+      <c r="AF15" s="38"/>
+      <c r="AG15" s="38"/>
+      <c r="AH15" s="38"/>
+      <c r="AI15" s="38"/>
       <c r="AK15" s="10" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A16" s="40"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="D16" s="30" t="s">
+      <c r="D16" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
       <c r="G16" s="6">
         <v>0</v>
       </c>
@@ -2564,16 +2570,16 @@
       <c r="J16" s="12">
         <v>1</v>
       </c>
-      <c r="K16" s="29" t="s">
+      <c r="K16" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="29" t="s">
+      <c r="L16" s="38"/>
+      <c r="M16" s="38"/>
+      <c r="N16" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="O16" s="29"/>
-      <c r="P16" s="29"/>
+      <c r="O16" s="38"/>
+      <c r="P16" s="38"/>
       <c r="Q16" s="6">
         <v>1</v>
       </c>
@@ -2583,38 +2589,38 @@
       <c r="S16" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="T16" s="29" t="s">
+      <c r="T16" s="38" t="s">
         <v>158</v>
       </c>
-      <c r="U16" s="29"/>
-      <c r="V16" s="29"/>
-      <c r="W16" s="29"/>
-      <c r="X16" s="29"/>
-      <c r="Y16" s="29"/>
-      <c r="Z16" s="29"/>
-      <c r="AA16" s="29"/>
-      <c r="AB16" s="29"/>
-      <c r="AC16" s="29"/>
-      <c r="AD16" s="29"/>
-      <c r="AE16" s="29"/>
-      <c r="AF16" s="29"/>
-      <c r="AG16" s="29"/>
-      <c r="AH16" s="29"/>
-      <c r="AI16" s="29"/>
+      <c r="U16" s="38"/>
+      <c r="V16" s="38"/>
+      <c r="W16" s="38"/>
+      <c r="X16" s="38"/>
+      <c r="Y16" s="38"/>
+      <c r="Z16" s="38"/>
+      <c r="AA16" s="38"/>
+      <c r="AB16" s="38"/>
+      <c r="AC16" s="38"/>
+      <c r="AD16" s="38"/>
+      <c r="AE16" s="38"/>
+      <c r="AF16" s="38"/>
+      <c r="AG16" s="38"/>
+      <c r="AH16" s="38"/>
+      <c r="AI16" s="38"/>
       <c r="AK16" s="10" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A17" s="40"/>
+      <c r="A17" s="34"/>
       <c r="B17" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="D17" s="30" t="s">
+      <c r="D17" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
       <c r="G17" s="6">
         <v>0</v>
       </c>
@@ -2627,35 +2633,35 @@
       <c r="J17" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="K17" s="29" t="s">
+      <c r="K17" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="L17" s="29"/>
-      <c r="M17" s="29"/>
-      <c r="N17" s="29" t="s">
+      <c r="L17" s="38"/>
+      <c r="M17" s="38"/>
+      <c r="N17" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="O17" s="29"/>
-      <c r="P17" s="29"/>
-      <c r="Q17" s="29"/>
-      <c r="R17" s="29"/>
-      <c r="S17" s="29"/>
-      <c r="T17" s="29"/>
-      <c r="U17" s="29"/>
-      <c r="V17" s="29"/>
-      <c r="W17" s="29"/>
-      <c r="X17" s="29"/>
-      <c r="Y17" s="29"/>
-      <c r="Z17" s="29"/>
-      <c r="AA17" s="29"/>
-      <c r="AB17" s="29"/>
-      <c r="AC17" s="29"/>
-      <c r="AD17" s="29"/>
-      <c r="AE17" s="29"/>
-      <c r="AF17" s="29"/>
-      <c r="AG17" s="29"/>
-      <c r="AH17" s="29"/>
-      <c r="AI17" s="29"/>
+      <c r="O17" s="38"/>
+      <c r="P17" s="38"/>
+      <c r="Q17" s="38"/>
+      <c r="R17" s="38"/>
+      <c r="S17" s="38"/>
+      <c r="T17" s="38"/>
+      <c r="U17" s="38"/>
+      <c r="V17" s="38"/>
+      <c r="W17" s="38"/>
+      <c r="X17" s="38"/>
+      <c r="Y17" s="38"/>
+      <c r="Z17" s="38"/>
+      <c r="AA17" s="38"/>
+      <c r="AB17" s="38"/>
+      <c r="AC17" s="38"/>
+      <c r="AD17" s="38"/>
+      <c r="AE17" s="38"/>
+      <c r="AF17" s="38"/>
+      <c r="AG17" s="38"/>
+      <c r="AH17" s="38"/>
+      <c r="AI17" s="38"/>
       <c r="AK17" s="10" t="s">
         <v>187</v>
       </c>
@@ -2667,11 +2673,11 @@
       <c r="B18" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="30" t="s">
+      <c r="D18" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
       <c r="G18" s="6">
         <v>0</v>
       </c>
@@ -2684,35 +2690,35 @@
       <c r="J18" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="K18" s="29" t="s">
+      <c r="K18" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="L18" s="29"/>
-      <c r="M18" s="29"/>
-      <c r="N18" s="29" t="s">
+      <c r="L18" s="38"/>
+      <c r="M18" s="38"/>
+      <c r="N18" s="38" t="s">
         <v>183</v>
       </c>
-      <c r="O18" s="29"/>
-      <c r="P18" s="29"/>
-      <c r="Q18" s="29"/>
-      <c r="R18" s="29"/>
-      <c r="S18" s="29"/>
-      <c r="T18" s="29"/>
-      <c r="U18" s="29"/>
-      <c r="V18" s="29"/>
-      <c r="W18" s="29"/>
-      <c r="X18" s="29"/>
-      <c r="Y18" s="29"/>
-      <c r="Z18" s="29"/>
-      <c r="AA18" s="29"/>
-      <c r="AB18" s="29"/>
-      <c r="AC18" s="29"/>
-      <c r="AD18" s="29"/>
-      <c r="AE18" s="29"/>
-      <c r="AF18" s="29"/>
-      <c r="AG18" s="29"/>
-      <c r="AH18" s="29"/>
-      <c r="AI18" s="29"/>
+      <c r="O18" s="38"/>
+      <c r="P18" s="38"/>
+      <c r="Q18" s="38"/>
+      <c r="R18" s="38"/>
+      <c r="S18" s="38"/>
+      <c r="T18" s="38"/>
+      <c r="U18" s="38"/>
+      <c r="V18" s="38"/>
+      <c r="W18" s="38"/>
+      <c r="X18" s="38"/>
+      <c r="Y18" s="38"/>
+      <c r="Z18" s="38"/>
+      <c r="AA18" s="38"/>
+      <c r="AB18" s="38"/>
+      <c r="AC18" s="38"/>
+      <c r="AD18" s="38"/>
+      <c r="AE18" s="38"/>
+      <c r="AF18" s="38"/>
+      <c r="AG18" s="38"/>
+      <c r="AH18" s="38"/>
+      <c r="AI18" s="38"/>
       <c r="AK18" s="10" t="s">
         <v>210</v>
       </c>
@@ -2724,11 +2730,11 @@
       <c r="B19" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="D19" s="30" t="s">
+      <c r="D19" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
       <c r="G19" s="6">
         <v>1</v>
       </c>
@@ -2741,35 +2747,35 @@
       <c r="J19" s="12">
         <v>0</v>
       </c>
-      <c r="K19" s="34" t="s">
+      <c r="K19" s="39" t="s">
         <v>162</v>
       </c>
-      <c r="L19" s="34"/>
-      <c r="M19" s="34"/>
-      <c r="N19" s="29" t="s">
+      <c r="L19" s="39"/>
+      <c r="M19" s="39"/>
+      <c r="N19" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="O19" s="29"/>
-      <c r="P19" s="29"/>
-      <c r="Q19" s="29"/>
-      <c r="R19" s="29"/>
-      <c r="S19" s="29"/>
-      <c r="T19" s="29"/>
-      <c r="U19" s="29"/>
-      <c r="V19" s="29"/>
-      <c r="W19" s="29"/>
-      <c r="X19" s="29"/>
-      <c r="Y19" s="29"/>
-      <c r="Z19" s="29"/>
-      <c r="AA19" s="29"/>
-      <c r="AB19" s="29"/>
-      <c r="AC19" s="29"/>
-      <c r="AD19" s="29"/>
-      <c r="AE19" s="29"/>
-      <c r="AF19" s="29"/>
-      <c r="AG19" s="29"/>
-      <c r="AH19" s="29"/>
-      <c r="AI19" s="29"/>
+      <c r="O19" s="38"/>
+      <c r="P19" s="38"/>
+      <c r="Q19" s="38"/>
+      <c r="R19" s="38"/>
+      <c r="S19" s="38"/>
+      <c r="T19" s="38"/>
+      <c r="U19" s="38"/>
+      <c r="V19" s="38"/>
+      <c r="W19" s="38"/>
+      <c r="X19" s="38"/>
+      <c r="Y19" s="38"/>
+      <c r="Z19" s="38"/>
+      <c r="AA19" s="38"/>
+      <c r="AB19" s="38"/>
+      <c r="AC19" s="38"/>
+      <c r="AD19" s="38"/>
+      <c r="AE19" s="38"/>
+      <c r="AF19" s="38"/>
+      <c r="AG19" s="38"/>
+      <c r="AH19" s="38"/>
+      <c r="AI19" s="38"/>
       <c r="AK19" s="10" t="s">
         <v>201</v>
       </c>
@@ -2781,11 +2787,11 @@
       <c r="B20" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="D20" s="30" t="s">
+      <c r="D20" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
       <c r="G20" s="24">
         <v>1</v>
       </c>
@@ -2798,11 +2804,11 @@
       <c r="J20" s="25">
         <v>1</v>
       </c>
-      <c r="K20" s="34" t="s">
+      <c r="K20" s="39" t="s">
         <v>162</v>
       </c>
-      <c r="L20" s="34"/>
-      <c r="M20" s="34"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="39"/>
       <c r="N20" s="25">
         <v>0</v>
       </c>
@@ -2812,29 +2818,29 @@
       <c r="P20" s="25">
         <v>0</v>
       </c>
-      <c r="Q20" s="36" t="s">
+      <c r="Q20" s="37" t="s">
         <v>260</v>
       </c>
-      <c r="R20" s="36"/>
-      <c r="S20" s="36"/>
-      <c r="T20" s="36"/>
-      <c r="U20" s="36"/>
-      <c r="V20" s="36"/>
-      <c r="W20" s="29" t="s">
+      <c r="R20" s="37"/>
+      <c r="S20" s="37"/>
+      <c r="T20" s="37"/>
+      <c r="U20" s="37"/>
+      <c r="V20" s="37"/>
+      <c r="W20" s="38" t="s">
         <v>259</v>
       </c>
-      <c r="X20" s="29"/>
-      <c r="Y20" s="29"/>
-      <c r="Z20" s="29"/>
-      <c r="AA20" s="29"/>
-      <c r="AB20" s="29"/>
-      <c r="AC20" s="29"/>
-      <c r="AD20" s="29"/>
-      <c r="AE20" s="29"/>
-      <c r="AF20" s="29"/>
-      <c r="AG20" s="29"/>
-      <c r="AH20" s="29"/>
-      <c r="AI20" s="29"/>
+      <c r="X20" s="38"/>
+      <c r="Y20" s="38"/>
+      <c r="Z20" s="38"/>
+      <c r="AA20" s="38"/>
+      <c r="AB20" s="38"/>
+      <c r="AC20" s="38"/>
+      <c r="AD20" s="38"/>
+      <c r="AE20" s="38"/>
+      <c r="AF20" s="38"/>
+      <c r="AG20" s="38"/>
+      <c r="AH20" s="38"/>
+      <c r="AI20" s="38"/>
       <c r="AK20" s="10" t="s">
         <v>263</v>
       </c>
@@ -2846,11 +2852,11 @@
       <c r="B21" s="7" t="s">
         <v>265</v>
       </c>
-      <c r="D21" s="30" t="s">
+      <c r="D21" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
       <c r="G21" s="24">
         <v>1</v>
       </c>
@@ -2863,11 +2869,11 @@
       <c r="J21" s="25">
         <v>1</v>
       </c>
-      <c r="K21" s="36" t="s">
+      <c r="K21" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="L21" s="36"/>
-      <c r="M21" s="36"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="37"/>
       <c r="N21" s="25">
         <v>0</v>
       </c>
@@ -2910,16 +2916,16 @@
       <c r="AA21" s="24">
         <v>0</v>
       </c>
-      <c r="AB21" s="29" t="s">
+      <c r="AB21" s="38" t="s">
         <v>262</v>
       </c>
-      <c r="AC21" s="29"/>
-      <c r="AD21" s="29"/>
-      <c r="AE21" s="29"/>
-      <c r="AF21" s="29"/>
-      <c r="AG21" s="29"/>
-      <c r="AH21" s="29"/>
-      <c r="AI21" s="29"/>
+      <c r="AC21" s="38"/>
+      <c r="AD21" s="38"/>
+      <c r="AE21" s="38"/>
+      <c r="AF21" s="38"/>
+      <c r="AG21" s="38"/>
+      <c r="AH21" s="38"/>
+      <c r="AI21" s="38"/>
       <c r="AK21" s="10" t="s">
         <v>264</v>
       </c>
@@ -2931,11 +2937,11 @@
       <c r="B22" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D22" s="30" t="s">
+      <c r="D22" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
       <c r="G22" s="6">
         <v>1</v>
       </c>
@@ -2948,11 +2954,11 @@
       <c r="J22" s="6">
         <v>1</v>
       </c>
-      <c r="K22" s="29" t="s">
+      <c r="K22" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="L22" s="29"/>
-      <c r="M22" s="29"/>
+      <c r="L22" s="38"/>
+      <c r="M22" s="38"/>
       <c r="N22" s="6">
         <v>0</v>
       </c>
@@ -2995,16 +3001,16 @@
       <c r="AA22" s="6">
         <v>0</v>
       </c>
-      <c r="AB22" s="29" t="s">
+      <c r="AB22" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="AC22" s="29"/>
-      <c r="AD22" s="29"/>
-      <c r="AE22" s="29"/>
-      <c r="AF22" s="29"/>
-      <c r="AG22" s="29"/>
-      <c r="AH22" s="29"/>
-      <c r="AI22" s="29"/>
+      <c r="AC22" s="38"/>
+      <c r="AD22" s="38"/>
+      <c r="AE22" s="38"/>
+      <c r="AF22" s="38"/>
+      <c r="AG22" s="38"/>
+      <c r="AH22" s="38"/>
+      <c r="AI22" s="38"/>
       <c r="AK22" s="10" t="s">
         <v>88</v>
       </c>
@@ -3016,11 +3022,11 @@
       <c r="B23" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D23" s="30" t="s">
+      <c r="D23" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
       <c r="G23" s="6">
         <v>1</v>
       </c>
@@ -3033,11 +3039,11 @@
       <c r="J23" s="6">
         <v>1</v>
       </c>
-      <c r="K23" s="29" t="s">
+      <c r="K23" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="L23" s="29"/>
-      <c r="M23" s="29"/>
+      <c r="L23" s="38"/>
+      <c r="M23" s="38"/>
       <c r="N23" s="6">
         <v>0</v>
       </c>
@@ -3080,16 +3086,16 @@
       <c r="AA23" s="6">
         <v>1</v>
       </c>
-      <c r="AB23" s="29" t="s">
+      <c r="AB23" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="AC23" s="29"/>
-      <c r="AD23" s="29"/>
-      <c r="AE23" s="29"/>
-      <c r="AF23" s="29"/>
-      <c r="AG23" s="29"/>
-      <c r="AH23" s="29"/>
-      <c r="AI23" s="29"/>
+      <c r="AC23" s="38"/>
+      <c r="AD23" s="38"/>
+      <c r="AE23" s="38"/>
+      <c r="AF23" s="38"/>
+      <c r="AG23" s="38"/>
+      <c r="AH23" s="38"/>
+      <c r="AI23" s="38"/>
       <c r="AK23" s="10" t="s">
         <v>184</v>
       </c>
@@ -3101,11 +3107,11 @@
       <c r="B24" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="30" t="s">
+      <c r="D24" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
       <c r="G24" s="6">
         <v>1</v>
       </c>
@@ -3118,11 +3124,11 @@
       <c r="J24" s="6">
         <v>1</v>
       </c>
-      <c r="K24" s="29" t="s">
+      <c r="K24" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="L24" s="29"/>
-      <c r="M24" s="29"/>
+      <c r="L24" s="38"/>
+      <c r="M24" s="38"/>
       <c r="N24" s="6">
         <v>0</v>
       </c>
@@ -3198,11 +3204,11 @@
       <c r="B25" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D25" s="30" t="s">
+      <c r="D25" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="E25" s="30"/>
-      <c r="F25" s="30"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
       <c r="G25" s="6">
         <v>1</v>
       </c>
@@ -3266,16 +3272,16 @@
       <c r="AA25" s="6">
         <v>1</v>
       </c>
-      <c r="AB25" s="29" t="s">
+      <c r="AB25" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="AC25" s="29"/>
-      <c r="AD25" s="29"/>
-      <c r="AE25" s="29"/>
-      <c r="AF25" s="29"/>
-      <c r="AG25" s="29"/>
-      <c r="AH25" s="29"/>
-      <c r="AI25" s="29"/>
+      <c r="AC25" s="38"/>
+      <c r="AD25" s="38"/>
+      <c r="AE25" s="38"/>
+      <c r="AF25" s="38"/>
+      <c r="AG25" s="38"/>
+      <c r="AH25" s="38"/>
+      <c r="AI25" s="38"/>
     </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B32" s="7"/>
@@ -3861,30 +3867,24 @@
     </row>
   </sheetData>
   <mergeCells count="66">
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="Q20:V20"/>
-    <mergeCell ref="W20:AI20"/>
-    <mergeCell ref="AB21:AI21"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="AD8:AI8"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="N8:P8"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="AB22:AI22"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="N9:S9"/>
-    <mergeCell ref="N13:P13"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="AB14:AI14"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="N12:P12"/>
-    <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="T12:V12"/>
-    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="N16:P16"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D20:F20"/>
     <mergeCell ref="AB25:AI25"/>
     <mergeCell ref="N17:AI17"/>
     <mergeCell ref="K17:M17"/>
@@ -3901,32 +3901,38 @@
     <mergeCell ref="AB23:AI23"/>
     <mergeCell ref="K24:M24"/>
     <mergeCell ref="K13:M13"/>
+    <mergeCell ref="AB22:AI22"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="N9:S9"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="AB14:AI14"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="N12:P12"/>
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="T12:V12"/>
+    <mergeCell ref="K15:M15"/>
     <mergeCell ref="T15:AI15"/>
     <mergeCell ref="K10:M10"/>
     <mergeCell ref="N10:P10"/>
     <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="Q20:V20"/>
+    <mergeCell ref="W20:AI20"/>
+    <mergeCell ref="AB21:AI21"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="AD8:AI8"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="N8:P8"/>
+    <mergeCell ref="Q8:S8"/>
     <mergeCell ref="AG11:AH11"/>
     <mergeCell ref="W12:Y12"/>
     <mergeCell ref="N14:P14"/>
     <mergeCell ref="N15:P15"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="N16:P16"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D24:F24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3937,8 +3943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3955,13 +3961,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="30" t="s">
         <v>266</v>
       </c>
-      <c r="B1" s="44">
-        <v>1</v>
-      </c>
-      <c r="C1" s="42" t="s">
+      <c r="B1" s="31">
+        <v>1</v>
+      </c>
+      <c r="C1" s="29" t="s">
         <v>298</v>
       </c>
       <c r="D1" s="1"/>
@@ -3969,20 +3975,20 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="44" t="s">
         <v>167</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="39"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="46"/>
       <c r="M2" s="20" t="s">
         <v>166</v>
       </c>
@@ -4381,6 +4387,9 @@
       <c r="L11" t="s">
         <v>80</v>
       </c>
+      <c r="M11" t="s">
+        <v>310</v>
+      </c>
       <c r="P11" s="19" t="s">
         <v>198</v>
       </c>
@@ -4418,6 +4427,9 @@
       </c>
       <c r="L12" t="s">
         <v>82</v>
+      </c>
+      <c r="M12" t="s">
+        <v>309</v>
       </c>
       <c r="P12" s="19" t="s">
         <v>199</v>
@@ -5632,7 +5644,7 @@
   <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5646,13 +5658,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="30" t="s">
         <v>266</v>
       </c>
-      <c r="B1" s="44">
+      <c r="B1" s="31">
         <v>2</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="29" t="s">
         <v>267</v>
       </c>
       <c r="D1" s="1"/>
@@ -5663,7 +5675,7 @@
       <c r="A2" s="28" t="s">
         <v>219</v>
       </c>
-      <c r="B2" s="45"/>
+      <c r="B2" s="32"/>
       <c r="C2" s="28"/>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
@@ -5673,7 +5685,7 @@
       <c r="A3" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="B3" s="46"/>
+      <c r="B3" s="33"/>
       <c r="C3" s="3" t="s">
         <v>99</v>
       </c>
@@ -5795,7 +5807,7 @@
       <c r="A11" s="28" t="s">
         <v>220</v>
       </c>
-      <c r="B11" s="45"/>
+      <c r="B11" s="32"/>
       <c r="C11" s="28"/>
       <c r="D11" s="28"/>
       <c r="E11" s="28"/>
@@ -5805,7 +5817,7 @@
       <c r="A12" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="B12" s="46"/>
+      <c r="B12" s="33"/>
       <c r="C12" s="3" t="s">
         <v>99</v>
       </c>
@@ -5907,10 +5919,10 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="30" t="s">
         <v>266</v>
       </c>
-      <c r="B19" s="44">
+      <c r="B19" s="31">
         <v>3</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -5924,7 +5936,7 @@
       <c r="A20" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="B20" s="46"/>
+      <c r="B20" s="33"/>
       <c r="C20" s="3" t="s">
         <v>99</v>
       </c>
@@ -5950,10 +5962,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="43" t="s">
+      <c r="A22" s="30" t="s">
         <v>266</v>
       </c>
-      <c r="B22" s="44">
+      <c r="B22" s="31">
         <v>4</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -5967,7 +5979,7 @@
       <c r="A23" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="B23" s="46"/>
+      <c r="B23" s="33"/>
       <c r="C23" s="3" t="s">
         <v>99</v>
       </c>
@@ -6038,10 +6050,10 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="30" t="s">
         <v>266</v>
       </c>
-      <c r="B28" s="44">
+      <c r="B28" s="31">
         <v>5</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -6055,7 +6067,7 @@
       <c r="A29" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="B29" s="46"/>
+      <c r="B29" s="33"/>
       <c r="C29" s="3" t="s">
         <v>99</v>
       </c>
@@ -6090,10 +6102,10 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="43" t="s">
+      <c r="A34" s="30" t="s">
         <v>266</v>
       </c>
-      <c r="B34" s="44">
+      <c r="B34" s="31">
         <v>6</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -6107,7 +6119,7 @@
       <c r="A35" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="B35" s="46"/>
+      <c r="B35" s="33"/>
       <c r="C35" s="3" t="s">
         <v>99</v>
       </c>
@@ -6157,10 +6169,10 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="43" t="s">
+      <c r="A43" s="30" t="s">
         <v>266</v>
       </c>
-      <c r="B43" s="44">
+      <c r="B43" s="31">
         <v>7</v>
       </c>
       <c r="C43" s="1" t="s">
@@ -6174,7 +6186,7 @@
       <c r="A44" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="B44" s="46"/>
+      <c r="B44" s="33"/>
       <c r="C44" s="3" t="s">
         <v>99</v>
       </c>
@@ -6189,10 +6201,10 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="43" t="s">
+      <c r="A46" s="30" t="s">
         <v>266</v>
       </c>
-      <c r="B46" s="44">
+      <c r="B46" s="31">
         <v>8</v>
       </c>
       <c r="C46" s="1" t="s">
@@ -6206,7 +6218,7 @@
       <c r="A47" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="B47" s="46"/>
+      <c r="B47" s="33"/>
       <c r="C47" s="3" t="s">
         <v>99</v>
       </c>
@@ -6221,10 +6233,10 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="43" t="s">
+      <c r="A49" s="30" t="s">
         <v>266</v>
       </c>
-      <c r="B49" s="44">
+      <c r="B49" s="31">
         <v>9</v>
       </c>
       <c r="C49" s="1" t="s">
@@ -6238,7 +6250,7 @@
       <c r="A50" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="B50" s="46"/>
+      <c r="B50" s="33"/>
       <c r="C50" s="3" t="s">
         <v>99</v>
       </c>
@@ -6253,10 +6265,10 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="43" t="s">
+      <c r="A52" s="30" t="s">
         <v>266</v>
       </c>
-      <c r="B52" s="44">
+      <c r="B52" s="31">
         <v>10</v>
       </c>
       <c r="C52" s="1" t="s">
@@ -6270,7 +6282,7 @@
       <c r="A53" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="B53" s="46"/>
+      <c r="B53" s="33"/>
       <c r="C53" s="3" t="s">
         <v>99</v>
       </c>
@@ -6285,10 +6297,10 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="43" t="s">
+      <c r="A55" s="30" t="s">
         <v>266</v>
       </c>
-      <c r="B55" s="44">
+      <c r="B55" s="31">
         <v>11</v>
       </c>
       <c r="C55" s="1" t="s">
@@ -6302,7 +6314,7 @@
       <c r="A56" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="B56" s="46"/>
+      <c r="B56" s="33"/>
       <c r="C56" s="3" t="s">
         <v>99</v>
       </c>
@@ -6317,10 +6329,10 @@
       </c>
     </row>
     <row r="58" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="43" t="s">
+      <c r="A58" s="30" t="s">
         <v>266</v>
       </c>
-      <c r="B58" s="44">
+      <c r="B58" s="31">
         <v>12</v>
       </c>
       <c r="C58" s="1" t="s">
@@ -6334,7 +6346,7 @@
       <c r="A59" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="B59" s="46"/>
+      <c r="B59" s="33"/>
       <c r="C59" s="3" t="s">
         <v>99</v>
       </c>
@@ -6357,7 +6369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -6391,34 +6403,34 @@
         <v>0</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="46">
+      <c r="C3" s="33">
         <v>7</v>
       </c>
-      <c r="D3" s="46">
+      <c r="D3" s="33">
         <v>6</v>
       </c>
-      <c r="E3" s="46">
+      <c r="E3" s="33">
         <v>5</v>
       </c>
-      <c r="F3" s="46">
+      <c r="F3" s="33">
         <v>4</v>
       </c>
-      <c r="G3" s="46">
+      <c r="G3" s="33">
         <v>3</v>
       </c>
-      <c r="H3" s="46">
+      <c r="H3" s="33">
         <v>2</v>
       </c>
-      <c r="I3" s="46">
-        <v>1</v>
-      </c>
-      <c r="J3" s="46">
-        <v>0</v>
-      </c>
-      <c r="K3" s="46" t="s">
+      <c r="I3" s="33">
+        <v>1</v>
+      </c>
+      <c r="J3" s="33">
+        <v>0</v>
+      </c>
+      <c r="K3" s="33" t="s">
         <v>302</v>
       </c>
-      <c r="L3" s="46" t="s">
+      <c r="L3" s="33" t="s">
         <v>306</v>
       </c>
     </row>
@@ -6824,30 +6836,30 @@
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="35"/>
-      <c r="R4" s="35"/>
-      <c r="S4" s="35"/>
-      <c r="T4" s="35"/>
-      <c r="U4" s="35"/>
-      <c r="V4" s="35"/>
-      <c r="W4" s="35"/>
-      <c r="X4" s="35"/>
-      <c r="Y4" s="35"/>
-      <c r="Z4" s="35"/>
-      <c r="AA4" s="35"/>
-      <c r="AB4" s="35"/>
-      <c r="AC4" s="35"/>
-      <c r="AD4" s="35"/>
-      <c r="AE4" s="35"/>
-      <c r="AF4" s="35"/>
-      <c r="AG4" s="35"/>
-      <c r="AH4" s="35"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="40"/>
+      <c r="S4" s="40"/>
+      <c r="T4" s="40"/>
+      <c r="U4" s="40"/>
+      <c r="V4" s="40"/>
+      <c r="W4" s="40"/>
+      <c r="X4" s="40"/>
+      <c r="Y4" s="40"/>
+      <c r="Z4" s="40"/>
+      <c r="AA4" s="40"/>
+      <c r="AB4" s="40"/>
+      <c r="AC4" s="40"/>
+      <c r="AD4" s="40"/>
+      <c r="AE4" s="40"/>
+      <c r="AF4" s="40"/>
+      <c r="AG4" s="40"/>
+      <c r="AH4" s="40"/>
       <c r="AJ4" s="10"/>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
@@ -6878,32 +6890,32 @@
       <c r="J5" s="6">
         <v>1</v>
       </c>
-      <c r="K5" s="29" t="s">
+      <c r="K5" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="29"/>
-      <c r="T5" s="29"/>
-      <c r="U5" s="29"/>
-      <c r="V5" s="29"/>
-      <c r="W5" s="29"/>
-      <c r="X5" s="29"/>
-      <c r="Y5" s="29"/>
-      <c r="Z5" s="29"/>
-      <c r="AA5" s="29"/>
-      <c r="AB5" s="29"/>
-      <c r="AC5" s="29"/>
-      <c r="AD5" s="29"/>
-      <c r="AE5" s="29"/>
-      <c r="AF5" s="29"/>
-      <c r="AG5" s="29"/>
-      <c r="AH5" s="29"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="38"/>
+      <c r="N5" s="38"/>
+      <c r="O5" s="38"/>
+      <c r="P5" s="38"/>
+      <c r="Q5" s="38"/>
+      <c r="R5" s="38"/>
+      <c r="S5" s="38"/>
+      <c r="T5" s="38"/>
+      <c r="U5" s="38"/>
+      <c r="V5" s="38"/>
+      <c r="W5" s="38"/>
+      <c r="X5" s="38"/>
+      <c r="Y5" s="38"/>
+      <c r="Z5" s="38"/>
+      <c r="AA5" s="38"/>
+      <c r="AB5" s="38"/>
+      <c r="AC5" s="38"/>
+      <c r="AD5" s="38"/>
+      <c r="AE5" s="38"/>
+      <c r="AF5" s="38"/>
+      <c r="AG5" s="38"/>
+      <c r="AH5" s="38"/>
       <c r="AJ5" s="10"/>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
@@ -6934,36 +6946,36 @@
       <c r="J6" s="6">
         <v>0</v>
       </c>
-      <c r="K6" s="29" t="s">
+      <c r="K6" s="38" t="s">
         <v>138</v>
       </c>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="29"/>
-      <c r="S6" s="29" t="s">
+      <c r="L6" s="38"/>
+      <c r="M6" s="38"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="38"/>
+      <c r="P6" s="38"/>
+      <c r="Q6" s="38"/>
+      <c r="R6" s="38"/>
+      <c r="S6" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="T6" s="29"/>
-      <c r="U6" s="29"/>
-      <c r="V6" s="29"/>
-      <c r="W6" s="29"/>
-      <c r="X6" s="29"/>
-      <c r="Y6" s="29"/>
-      <c r="Z6" s="29"/>
-      <c r="AA6" s="29" t="s">
+      <c r="T6" s="38"/>
+      <c r="U6" s="38"/>
+      <c r="V6" s="38"/>
+      <c r="W6" s="38"/>
+      <c r="X6" s="38"/>
+      <c r="Y6" s="38"/>
+      <c r="Z6" s="38"/>
+      <c r="AA6" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="AB6" s="29"/>
-      <c r="AC6" s="29"/>
-      <c r="AD6" s="29"/>
-      <c r="AE6" s="29"/>
-      <c r="AF6" s="29"/>
-      <c r="AG6" s="29"/>
-      <c r="AH6" s="29"/>
+      <c r="AB6" s="38"/>
+      <c r="AC6" s="38"/>
+      <c r="AD6" s="38"/>
+      <c r="AE6" s="38"/>
+      <c r="AF6" s="38"/>
+      <c r="AG6" s="38"/>
+      <c r="AH6" s="38"/>
       <c r="AI6" s="6"/>
       <c r="AJ6" s="10"/>
     </row>
@@ -8209,22 +8221,22 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="35"/>
-      <c r="R4" s="35"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="40"/>
       <c r="T4" s="10" t="s">
         <v>142</v>
       </c>
@@ -8367,16 +8379,16 @@
       <c r="J7" s="6">
         <v>1</v>
       </c>
-      <c r="K7" s="29" t="s">
+      <c r="K7" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29"/>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="29"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="38"/>
+      <c r="P7" s="38"/>
+      <c r="Q7" s="38"/>
+      <c r="R7" s="38"/>
       <c r="T7" s="10"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -8407,16 +8419,16 @@
       <c r="J8" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="K8" s="29" t="s">
+      <c r="K8" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="29"/>
-      <c r="R8" s="29"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="38"/>
+      <c r="P8" s="38"/>
+      <c r="Q8" s="38"/>
+      <c r="R8" s="38"/>
       <c r="T8" s="10"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -8447,16 +8459,16 @@
       <c r="J9" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="K9" s="29" t="s">
+      <c r="K9" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="29"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="38"/>
+      <c r="N9" s="38"/>
+      <c r="O9" s="38"/>
+      <c r="P9" s="38"/>
+      <c r="Q9" s="38"/>
+      <c r="R9" s="38"/>
       <c r="T9" s="10"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -8487,16 +8499,16 @@
       <c r="J10" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="K10" s="29" t="s">
+      <c r="K10" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="L10" s="29"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="29"/>
-      <c r="O10" s="29"/>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="29"/>
-      <c r="R10" s="29"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="38"/>
+      <c r="P10" s="38"/>
+      <c r="Q10" s="38"/>
+      <c r="R10" s="38"/>
       <c r="T10" s="10"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
renamed GOSUB -> JSR
</commit_message>
<xml_diff>
--- a/doc/RiscyInstSet32Bit.xlsx
+++ b/doc/RiscyInstSet32Bit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="14715" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="14715"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -268,12 +268,6 @@
     <t>DEC</t>
   </si>
   <si>
-    <t>Gosub</t>
-  </si>
-  <si>
-    <t>GOSUB</t>
-  </si>
-  <si>
     <t>Return</t>
   </si>
   <si>
@@ -523,12 +517,6 @@
     <t>MathOpcode 0 for Halt</t>
   </si>
   <si>
-    <t>Gosub/Return</t>
-  </si>
-  <si>
-    <t>M: 0-GOSUB, 1-RETURN</t>
-  </si>
-  <si>
     <t>Unused registers are ignored</t>
   </si>
   <si>
@@ -640,9 +628,6 @@
     <t>e.g. MOVZ</t>
   </si>
   <si>
-    <t>e.g. GOSUBNZ</t>
-  </si>
-  <si>
     <t>Rd = (int) Rs</t>
   </si>
   <si>
@@ -962,6 +947,21 @@
   </si>
   <si>
     <t>PUSHWORDI(pc); JMP(addr)</t>
+  </si>
+  <si>
+    <t>Jump to Subroutine</t>
+  </si>
+  <si>
+    <t>JSR</t>
+  </si>
+  <si>
+    <t>e.g. JSRNZ</t>
+  </si>
+  <si>
+    <t>JSR/Return</t>
+  </si>
+  <si>
+    <t>M: 0-JSR, 1-RETURN</t>
   </si>
 </sst>
 </file>
@@ -1583,8 +1583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AK10" sqref="AK10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1640,7 +1640,7 @@
     <row r="2" spans="1:38" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5" t="s">
@@ -1687,7 +1687,7 @@
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="10" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -1726,7 +1726,7 @@
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
@@ -1764,17 +1764,17 @@
       <c r="AH5" s="5"/>
       <c r="AI5" s="5"/>
       <c r="AK5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="AK6" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>0</v>
@@ -1955,13 +1955,13 @@
       <c r="AH8" s="40"/>
       <c r="AI8" s="40"/>
       <c r="AK8" s="10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="34"/>
       <c r="B9" s="7" t="s">
-        <v>164</v>
+        <v>309</v>
       </c>
       <c r="D9" s="36" t="s">
         <v>5</v>
@@ -1986,7 +1986,7 @@
       <c r="L9" s="37"/>
       <c r="M9" s="37"/>
       <c r="N9" s="39" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="O9" s="39"/>
       <c r="P9" s="39"/>
@@ -2042,13 +2042,13 @@
         <v>10</v>
       </c>
       <c r="AK9" s="10" t="s">
-        <v>165</v>
+        <v>310</v>
       </c>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="34"/>
       <c r="B10" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D10" s="36" t="s">
         <v>5</v>
@@ -2073,12 +2073,12 @@
       <c r="L10" s="41"/>
       <c r="M10" s="41"/>
       <c r="N10" s="41" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O10" s="41"/>
       <c r="P10" s="41"/>
       <c r="Q10" s="42" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="R10" s="42"/>
       <c r="S10" s="42"/>
@@ -2131,7 +2131,7 @@
         <v>0</v>
       </c>
       <c r="AK10" s="10" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
@@ -2139,7 +2139,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D11" s="36" t="s">
         <v>5</v>
@@ -2169,7 +2169,7 @@
       <c r="O11" s="38"/>
       <c r="P11" s="38"/>
       <c r="Q11" s="38" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R11" s="38"/>
       <c r="S11" s="38"/>
@@ -2213,17 +2213,17 @@
         <v>0</v>
       </c>
       <c r="AG11" s="36" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="AH11" s="36"/>
       <c r="AI11" s="22" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AK11" s="10" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="AL11" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.25">
@@ -2231,7 +2231,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D12" s="36" t="s">
         <v>5</v>
@@ -2261,17 +2261,17 @@
       <c r="O12" s="38"/>
       <c r="P12" s="38"/>
       <c r="Q12" s="38" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="R12" s="38"/>
       <c r="S12" s="38"/>
       <c r="T12" s="38" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="U12" s="38"/>
       <c r="V12" s="38"/>
       <c r="W12" s="38" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="X12" s="38"/>
       <c r="Y12" s="38"/>
@@ -2306,7 +2306,7 @@
         <v>0</v>
       </c>
       <c r="AK12" s="10" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
@@ -2314,7 +2314,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D13" s="36" t="s">
         <v>5</v>
@@ -2395,13 +2395,13 @@
         <v>0</v>
       </c>
       <c r="AH13" s="22" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="AI13" s="22" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AK13" s="10" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
@@ -2409,7 +2409,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D14" s="36" t="s">
         <v>5</v>
@@ -2434,7 +2434,7 @@
       <c r="L14" s="38"/>
       <c r="M14" s="38"/>
       <c r="N14" s="38" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="O14" s="38"/>
       <c r="P14" s="38"/>
@@ -2472,7 +2472,7 @@
         <v>0</v>
       </c>
       <c r="AB14" s="38" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="AC14" s="38"/>
       <c r="AD14" s="38"/>
@@ -2482,13 +2482,13 @@
       <c r="AH14" s="38"/>
       <c r="AI14" s="38"/>
       <c r="AK14" s="10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="34"/>
       <c r="B15" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D15" s="36" t="s">
         <v>5</v>
@@ -2513,7 +2513,7 @@
       <c r="L15" s="38"/>
       <c r="M15" s="38"/>
       <c r="N15" s="38" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="O15" s="38"/>
       <c r="P15" s="38"/>
@@ -2527,7 +2527,7 @@
         <v>10</v>
       </c>
       <c r="T15" s="38" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="U15" s="38"/>
       <c r="V15" s="38"/>
@@ -2545,13 +2545,13 @@
       <c r="AH15" s="38"/>
       <c r="AI15" s="38"/>
       <c r="AK15" s="10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="34"/>
       <c r="B16" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D16" s="36" t="s">
         <v>5</v>
@@ -2576,7 +2576,7 @@
       <c r="L16" s="38"/>
       <c r="M16" s="38"/>
       <c r="N16" s="38" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="O16" s="38"/>
       <c r="P16" s="38"/>
@@ -2590,7 +2590,7 @@
         <v>10</v>
       </c>
       <c r="T16" s="38" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="U16" s="38"/>
       <c r="V16" s="38"/>
@@ -2608,13 +2608,13 @@
       <c r="AH16" s="38"/>
       <c r="AI16" s="38"/>
       <c r="AK16" s="10" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" s="34"/>
       <c r="B17" s="7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D17" s="36" t="s">
         <v>5</v>
@@ -2631,7 +2631,7 @@
         <v>1</v>
       </c>
       <c r="J17" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K17" s="38" t="s">
         <v>7</v>
@@ -2663,7 +2663,7 @@
       <c r="AH17" s="38"/>
       <c r="AI17" s="38"/>
       <c r="AK17" s="10" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
@@ -2688,7 +2688,7 @@
         <v>10</v>
       </c>
       <c r="J18" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K18" s="38" t="s">
         <v>7</v>
@@ -2696,7 +2696,7 @@
       <c r="L18" s="38"/>
       <c r="M18" s="38"/>
       <c r="N18" s="38" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="O18" s="38"/>
       <c r="P18" s="38"/>
@@ -2720,7 +2720,7 @@
       <c r="AH18" s="38"/>
       <c r="AI18" s="38"/>
       <c r="AK18" s="10" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
@@ -2728,7 +2728,7 @@
         <v>6</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="D19" s="36" t="s">
         <v>5</v>
@@ -2748,7 +2748,7 @@
         <v>0</v>
       </c>
       <c r="K19" s="39" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="L19" s="39"/>
       <c r="M19" s="39"/>
@@ -2777,7 +2777,7 @@
       <c r="AH19" s="38"/>
       <c r="AI19" s="38"/>
       <c r="AK19" s="10" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.25">
@@ -2785,7 +2785,7 @@
         <v>7</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="D20" s="36" t="s">
         <v>5</v>
@@ -2805,7 +2805,7 @@
         <v>1</v>
       </c>
       <c r="K20" s="39" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="L20" s="39"/>
       <c r="M20" s="39"/>
@@ -2819,7 +2819,7 @@
         <v>0</v>
       </c>
       <c r="Q20" s="37" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="R20" s="37"/>
       <c r="S20" s="37"/>
@@ -2827,7 +2827,7 @@
       <c r="U20" s="37"/>
       <c r="V20" s="37"/>
       <c r="W20" s="38" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="X20" s="38"/>
       <c r="Y20" s="38"/>
@@ -2842,7 +2842,7 @@
       <c r="AH20" s="38"/>
       <c r="AI20" s="38"/>
       <c r="AK20" s="10" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
@@ -2850,7 +2850,7 @@
         <v>8</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D21" s="36" t="s">
         <v>5</v>
@@ -2917,7 +2917,7 @@
         <v>0</v>
       </c>
       <c r="AB21" s="38" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="AC21" s="38"/>
       <c r="AD21" s="38"/>
@@ -2927,7 +2927,7 @@
       <c r="AH21" s="38"/>
       <c r="AI21" s="38"/>
       <c r="AK21" s="10" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.25">
@@ -2935,7 +2935,7 @@
         <v>9</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D22" s="36" t="s">
         <v>5</v>
@@ -3002,7 +3002,7 @@
         <v>0</v>
       </c>
       <c r="AB22" s="38" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AC22" s="38"/>
       <c r="AD22" s="38"/>
@@ -3012,7 +3012,7 @@
       <c r="AH22" s="38"/>
       <c r="AI22" s="38"/>
       <c r="AK22" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
@@ -3020,7 +3020,7 @@
         <v>10</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D23" s="36" t="s">
         <v>5</v>
@@ -3087,7 +3087,7 @@
         <v>1</v>
       </c>
       <c r="AB23" s="38" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AC23" s="38"/>
       <c r="AD23" s="38"/>
@@ -3097,7 +3097,7 @@
       <c r="AH23" s="38"/>
       <c r="AI23" s="38"/>
       <c r="AK23" s="10" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
@@ -3105,7 +3105,7 @@
         <v>11</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D24" s="36" t="s">
         <v>5</v>
@@ -3202,7 +3202,7 @@
         <v>12</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D25" s="36" t="s">
         <v>5</v>
@@ -3273,7 +3273,7 @@
         <v>1</v>
       </c>
       <c r="AB25" s="38" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="AC25" s="38"/>
       <c r="AD25" s="38"/>
@@ -3943,8 +3943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3962,13 +3962,13 @@
   <sheetData>
     <row r="1" spans="1:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="30" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B1" s="31">
         <v>1</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -3976,7 +3976,7 @@
     </row>
     <row r="2" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="44" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B2" s="45"/>
       <c r="C2" s="45"/>
@@ -3990,7 +3990,7 @@
       <c r="K2" s="45"/>
       <c r="L2" s="46"/>
       <c r="M2" s="20" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4017,26 +4017,26 @@
         <v>0</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="Q3" s="23" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -4074,16 +4074,16 @@
         <v>17</v>
       </c>
       <c r="M4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="N4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="P4" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q4" t="s">
         <v>190</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -4121,16 +4121,16 @@
         <v>47</v>
       </c>
       <c r="M5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="N5" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="P5" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q5" t="s">
         <v>191</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -4168,16 +4168,16 @@
         <v>77</v>
       </c>
       <c r="M6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="N6" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="P6" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q6" t="s">
         <v>192</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -4215,21 +4215,21 @@
         <v>78</v>
       </c>
       <c r="M7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="N7" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="P7" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q7" t="s">
         <v>193</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6">
@@ -4259,15 +4259,15 @@
         <v>24h</v>
       </c>
       <c r="L8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="M8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6">
@@ -4297,21 +4297,21 @@
         <v>25h</v>
       </c>
       <c r="L9" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="M9" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="N9" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="P9" s="19" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6">
@@ -4341,21 +4341,21 @@
         <v>26h</v>
       </c>
       <c r="L10" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="M10" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="N10" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="P10" s="19" t="s">
-        <v>203</v>
+        <v>308</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>79</v>
+        <v>306</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6">
@@ -4385,18 +4385,18 @@
         <v>3Eh</v>
       </c>
       <c r="L11" t="s">
-        <v>80</v>
+        <v>307</v>
       </c>
       <c r="M11" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="P11" s="19" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6">
@@ -4426,13 +4426,13 @@
         <v>3Fh</v>
       </c>
       <c r="L12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M12" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="P12" s="19" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -4470,10 +4470,10 @@
         <v>48</v>
       </c>
       <c r="M13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="N13" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -4511,10 +4511,10 @@
         <v>49</v>
       </c>
       <c r="M14" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N14" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -4552,10 +4552,10 @@
         <v>50</v>
       </c>
       <c r="M15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="N15" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -4593,10 +4593,10 @@
         <v>51</v>
       </c>
       <c r="M16" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="N16" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -4634,10 +4634,10 @@
         <v>52</v>
       </c>
       <c r="M17" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="N17" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -4675,10 +4675,10 @@
         <v>53</v>
       </c>
       <c r="M18" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N18" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -4716,10 +4716,10 @@
         <v>54</v>
       </c>
       <c r="M19" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="N19" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -4757,10 +4757,10 @@
         <v>55</v>
       </c>
       <c r="M20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="N20" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -4798,10 +4798,10 @@
         <v>56</v>
       </c>
       <c r="M21" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="N21" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -4839,10 +4839,10 @@
         <v>57</v>
       </c>
       <c r="M22" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="N22" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -4880,10 +4880,10 @@
         <v>58</v>
       </c>
       <c r="M23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="N23" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -4921,10 +4921,10 @@
         <v>59</v>
       </c>
       <c r="M24" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="N24" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -4962,10 +4962,10 @@
         <v>60</v>
       </c>
       <c r="M25" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="N25" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -5003,10 +5003,10 @@
         <v>61</v>
       </c>
       <c r="M26" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="N26" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -5044,10 +5044,10 @@
         <v>62</v>
       </c>
       <c r="M27" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="N27" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -5085,10 +5085,10 @@
         <v>63</v>
       </c>
       <c r="M28" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="N28" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -5126,10 +5126,10 @@
         <v>64</v>
       </c>
       <c r="M29" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="N29" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -5167,10 +5167,10 @@
         <v>65</v>
       </c>
       <c r="M30" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="N30" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -5208,10 +5208,10 @@
         <v>66</v>
       </c>
       <c r="M31" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="N31" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -5249,15 +5249,15 @@
         <v>67</v>
       </c>
       <c r="M32" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="N32" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="6">
@@ -5287,13 +5287,13 @@
         <v>18h</v>
       </c>
       <c r="L33" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="M33" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="N33" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -5331,10 +5331,10 @@
         <v>68</v>
       </c>
       <c r="M34" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="N34" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
@@ -5372,10 +5372,10 @@
         <v>69</v>
       </c>
       <c r="M35" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N35" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
@@ -5413,10 +5413,10 @@
         <v>70</v>
       </c>
       <c r="M36" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N36" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
@@ -5454,10 +5454,10 @@
         <v>71</v>
       </c>
       <c r="M37" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="N37" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -5495,10 +5495,10 @@
         <v>72</v>
       </c>
       <c r="M38" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N38" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
@@ -5536,10 +5536,10 @@
         <v>73</v>
       </c>
       <c r="M39" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="N39" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
@@ -5577,15 +5577,15 @@
         <v>74</v>
       </c>
       <c r="M40" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="N40" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B41" s="14"/>
       <c r="C41" s="14">
@@ -5616,7 +5616,7 @@
       </c>
       <c r="K41" s="17"/>
       <c r="L41" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
@@ -5659,13 +5659,13 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="30" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B1" s="31">
         <v>2</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -5673,7 +5673,7 @@
     </row>
     <row r="2" spans="1:6" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="28" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B2" s="32"/>
       <c r="C2" s="28"/>
@@ -5683,129 +5683,129 @@
     </row>
     <row r="3" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B3" s="33"/>
       <c r="C3" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C4" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="D4" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="E4" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C5" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="D5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="E5" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C6" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="D6" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="E6" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C7" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D7" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="E7" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C8" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D8" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="E8" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C9" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D9" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="E9" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="F9" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="C10" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="D10" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="E10" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="F10" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="28" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B11" s="32"/>
       <c r="C11" s="28"/>
@@ -5815,118 +5815,118 @@
     </row>
     <row r="12" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="27" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C13" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="D13" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="E13" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="C14" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="D14" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="E14" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
+        <v>218</v>
+      </c>
+      <c r="C15" t="s">
+        <v>246</v>
+      </c>
+      <c r="D15" t="s">
         <v>223</v>
       </c>
-      <c r="C15" t="s">
-        <v>251</v>
-      </c>
-      <c r="D15" t="s">
-        <v>228</v>
-      </c>
       <c r="E15" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C16" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="D16" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E16" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="26" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="C17" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="D17" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="E17" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="C18" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="D18" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="E18" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="F18" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="30" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B19" s="31">
         <v>3</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -5934,42 +5934,42 @@
     </row>
     <row r="20" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="27" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B20" s="33"/>
       <c r="C20" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F20" s="23" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="26" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C21" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D21" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="30" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B22" s="31">
         <v>4</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -5977,81 +5977,81 @@
     </row>
     <row r="23" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="27" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B23" s="33"/>
       <c r="C23" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F23" s="23" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="C24" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D24" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="E24" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="C25" t="s">
+        <v>268</v>
+      </c>
+      <c r="D25" t="s">
+        <v>302</v>
+      </c>
+      <c r="E25" t="s">
         <v>273</v>
-      </c>
-      <c r="D25" t="s">
-        <v>307</v>
-      </c>
-      <c r="E25" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="26" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C26" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D26" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="E26" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="26" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C27" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D27" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="E27" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="30" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B28" s="31">
         <v>5</v>
@@ -6065,51 +6065,51 @@
     </row>
     <row r="29" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="27" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B29" s="33"/>
       <c r="C29" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F29" s="23" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="26" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="26" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="30" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B34" s="31">
         <v>6</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -6117,66 +6117,66 @@
     </row>
     <row r="35" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="27" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B35" s="33"/>
       <c r="C35" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F35" s="23" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="26" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="26" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="26" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="26" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="26" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="26" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="26" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="30" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B43" s="31">
         <v>7</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -6184,31 +6184,31 @@
     </row>
     <row r="44" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="27" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B44" s="33"/>
       <c r="C44" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F44" s="23" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="30" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B46" s="31">
         <v>8</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -6216,31 +6216,31 @@
     </row>
     <row r="47" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="27" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B47" s="33"/>
       <c r="C47" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F47" s="23" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="30" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B49" s="31">
         <v>9</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
@@ -6248,31 +6248,31 @@
     </row>
     <row r="50" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="27" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B50" s="33"/>
       <c r="C50" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F50" s="23" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="30" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B52" s="31">
         <v>10</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
@@ -6280,31 +6280,31 @@
     </row>
     <row r="53" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="27" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B53" s="33"/>
       <c r="C53" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F53" s="23" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="30" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B55" s="31">
         <v>11</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
@@ -6312,31 +6312,31 @@
     </row>
     <row r="56" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="27" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B56" s="33"/>
       <c r="C56" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F56" s="23" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="30" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B58" s="31">
         <v>12</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
@@ -6344,20 +6344,20 @@
     </row>
     <row r="59" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="27" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B59" s="33"/>
       <c r="C59" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F59" s="23" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -6383,7 +6383,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="47" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="B1" s="47"/>
       <c r="C1" s="47"/>
@@ -6428,15 +6428,15 @@
         <v>0</v>
       </c>
       <c r="K3" s="33" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="L3" s="33" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="C4" s="25">
         <v>0</v>
@@ -6473,7 +6473,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="C5" s="25">
         <v>0</v>
@@ -6510,7 +6510,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="C6" s="25">
         <v>0</v>
@@ -6547,7 +6547,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C7" s="25">
         <v>0</v>
@@ -6687,7 +6687,7 @@
   <sheetData>
     <row r="1" spans="1:36" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -6864,7 +6864,7 @@
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C5" s="6">
         <v>0</v>
@@ -6891,7 +6891,7 @@
         <v>1</v>
       </c>
       <c r="K5" s="38" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="L5" s="38"/>
       <c r="M5" s="38"/>
@@ -6920,7 +6920,7 @@
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C6" s="6">
         <v>0</v>
@@ -6947,7 +6947,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="38" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="L6" s="38"/>
       <c r="M6" s="38"/>
@@ -6957,7 +6957,7 @@
       <c r="Q6" s="38"/>
       <c r="R6" s="38"/>
       <c r="S6" s="38" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="T6" s="38"/>
       <c r="U6" s="38"/>
@@ -6967,7 +6967,7 @@
       <c r="Y6" s="38"/>
       <c r="Z6" s="38"/>
       <c r="AA6" s="38" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="AB6" s="38"/>
       <c r="AC6" s="38"/>
@@ -8141,7 +8141,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -8216,7 +8216,7 @@
         <v>0</v>
       </c>
       <c r="T3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -8238,68 +8238,68 @@
       <c r="Q4" s="40"/>
       <c r="R4" s="40"/>
       <c r="T4" s="10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0</v>
+      </c>
+      <c r="J5" s="6">
+        <v>0</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0</v>
+      </c>
+      <c r="L5" s="6">
+        <v>0</v>
+      </c>
+      <c r="M5" s="6">
+        <v>0</v>
+      </c>
+      <c r="N5" s="6">
+        <v>0</v>
+      </c>
+      <c r="O5" s="6">
+        <v>0</v>
+      </c>
+      <c r="P5" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>1</v>
+      </c>
+      <c r="R5" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="C5" s="6">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6">
-        <v>0</v>
-      </c>
-      <c r="G5" s="6">
-        <v>0</v>
-      </c>
-      <c r="H5" s="6">
-        <v>0</v>
-      </c>
-      <c r="I5" s="6">
-        <v>0</v>
-      </c>
-      <c r="J5" s="6">
-        <v>0</v>
-      </c>
-      <c r="K5" s="6">
-        <v>0</v>
-      </c>
-      <c r="L5" s="6">
-        <v>0</v>
-      </c>
-      <c r="M5" s="6">
-        <v>0</v>
-      </c>
-      <c r="N5" s="6">
-        <v>0</v>
-      </c>
-      <c r="O5" s="6">
-        <v>0</v>
-      </c>
-      <c r="P5" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="6">
-        <v>1</v>
-      </c>
-      <c r="R5" s="6" t="s">
-        <v>141</v>
-      </c>
       <c r="T5" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="C6" s="24">
         <v>0</v>
@@ -8347,13 +8347,13 @@
         <v>0</v>
       </c>
       <c r="R6" s="24" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="T6" s="10"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C7" s="6">
         <v>0</v>
@@ -8380,7 +8380,7 @@
         <v>1</v>
       </c>
       <c r="K7" s="38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L7" s="38"/>
       <c r="M7" s="38"/>
@@ -8393,7 +8393,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C8" s="6">
         <v>0</v>
@@ -8417,10 +8417,10 @@
         <v>1</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K8" s="38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L8" s="38"/>
       <c r="M8" s="38"/>
@@ -8433,7 +8433,7 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C9" s="6">
         <v>0</v>
@@ -8457,10 +8457,10 @@
         <v>0</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K9" s="38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L9" s="38"/>
       <c r="M9" s="38"/>
@@ -8473,7 +8473,7 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C10" s="6">
         <v>0</v>
@@ -8497,10 +8497,10 @@
         <v>1</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K10" s="38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L10" s="38"/>
       <c r="M10" s="38"/>

</xml_diff>

<commit_message>
functions return value (goes to r8)
</commit_message>
<xml_diff>
--- a/doc/RiscyInstSet32Bit.xlsx
+++ b/doc/RiscyInstSet32Bit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="14715"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="14715" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -325,9 +325,6 @@
     <t>Expression</t>
   </si>
   <si>
-    <t>Rd = Rs</t>
-  </si>
-  <si>
     <t>Rd &lt;-&gt; Rs</t>
   </si>
   <si>
@@ -962,6 +959,9 @@
   </si>
   <si>
     <t>M: 0-JSR, 1-RETURN</t>
+  </si>
+  <si>
+    <t>Rd &lt;- Rs</t>
   </si>
 </sst>
 </file>
@@ -1583,7 +1583,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AK10" sqref="AK10"/>
     </sheetView>
   </sheetViews>
@@ -1640,7 +1640,7 @@
     <row r="2" spans="1:38" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5" t="s">
@@ -1687,7 +1687,7 @@
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="10" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -1726,7 +1726,7 @@
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
@@ -1764,17 +1764,17 @@
       <c r="AH5" s="5"/>
       <c r="AI5" s="5"/>
       <c r="AK5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="AK6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>0</v>
@@ -1955,13 +1955,13 @@
       <c r="AH8" s="40"/>
       <c r="AI8" s="40"/>
       <c r="AK8" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="34"/>
       <c r="B9" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D9" s="36" t="s">
         <v>5</v>
@@ -1986,7 +1986,7 @@
       <c r="L9" s="37"/>
       <c r="M9" s="37"/>
       <c r="N9" s="39" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="O9" s="39"/>
       <c r="P9" s="39"/>
@@ -2042,7 +2042,7 @@
         <v>10</v>
       </c>
       <c r="AK9" s="10" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
@@ -2073,12 +2073,12 @@
       <c r="L10" s="41"/>
       <c r="M10" s="41"/>
       <c r="N10" s="41" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="O10" s="41"/>
       <c r="P10" s="41"/>
       <c r="Q10" s="42" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="R10" s="42"/>
       <c r="S10" s="42"/>
@@ -2131,7 +2131,7 @@
         <v>0</v>
       </c>
       <c r="AK10" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
@@ -2139,7 +2139,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D11" s="36" t="s">
         <v>5</v>
@@ -2213,17 +2213,17 @@
         <v>0</v>
       </c>
       <c r="AG11" s="36" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AH11" s="36"/>
       <c r="AI11" s="22" t="s">
         <v>87</v>
       </c>
       <c r="AK11" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AL11" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.25">
@@ -2261,17 +2261,17 @@
       <c r="O12" s="38"/>
       <c r="P12" s="38"/>
       <c r="Q12" s="38" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="R12" s="38"/>
       <c r="S12" s="38"/>
       <c r="T12" s="38" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="U12" s="38"/>
       <c r="V12" s="38"/>
       <c r="W12" s="38" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="X12" s="38"/>
       <c r="Y12" s="38"/>
@@ -2306,7 +2306,7 @@
         <v>0</v>
       </c>
       <c r="AK12" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
@@ -2314,7 +2314,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D13" s="36" t="s">
         <v>5</v>
@@ -2395,13 +2395,13 @@
         <v>0</v>
       </c>
       <c r="AH13" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="AI13" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="AK13" s="10" t="s">
         <v>177</v>
-      </c>
-      <c r="AI13" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="AK13" s="10" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
@@ -2409,7 +2409,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D14" s="36" t="s">
         <v>5</v>
@@ -2472,7 +2472,7 @@
         <v>0</v>
       </c>
       <c r="AB14" s="38" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AC14" s="38"/>
       <c r="AD14" s="38"/>
@@ -2482,13 +2482,13 @@
       <c r="AH14" s="38"/>
       <c r="AI14" s="38"/>
       <c r="AK14" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="34"/>
       <c r="B15" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D15" s="36" t="s">
         <v>5</v>
@@ -2527,7 +2527,7 @@
         <v>10</v>
       </c>
       <c r="T15" s="38" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="U15" s="38"/>
       <c r="V15" s="38"/>
@@ -2545,13 +2545,13 @@
       <c r="AH15" s="38"/>
       <c r="AI15" s="38"/>
       <c r="AK15" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="34"/>
       <c r="B16" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D16" s="36" t="s">
         <v>5</v>
@@ -2590,7 +2590,7 @@
         <v>10</v>
       </c>
       <c r="T16" s="38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U16" s="38"/>
       <c r="V16" s="38"/>
@@ -2608,13 +2608,13 @@
       <c r="AH16" s="38"/>
       <c r="AI16" s="38"/>
       <c r="AK16" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" s="34"/>
       <c r="B17" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D17" s="36" t="s">
         <v>5</v>
@@ -2663,7 +2663,7 @@
       <c r="AH17" s="38"/>
       <c r="AI17" s="38"/>
       <c r="AK17" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
@@ -2696,7 +2696,7 @@
       <c r="L18" s="38"/>
       <c r="M18" s="38"/>
       <c r="N18" s="38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O18" s="38"/>
       <c r="P18" s="38"/>
@@ -2720,7 +2720,7 @@
       <c r="AH18" s="38"/>
       <c r="AI18" s="38"/>
       <c r="AK18" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
@@ -2728,7 +2728,7 @@
         <v>6</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D19" s="36" t="s">
         <v>5</v>
@@ -2748,7 +2748,7 @@
         <v>0</v>
       </c>
       <c r="K19" s="39" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L19" s="39"/>
       <c r="M19" s="39"/>
@@ -2777,7 +2777,7 @@
       <c r="AH19" s="38"/>
       <c r="AI19" s="38"/>
       <c r="AK19" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.25">
@@ -2785,7 +2785,7 @@
         <v>7</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D20" s="36" t="s">
         <v>5</v>
@@ -2805,7 +2805,7 @@
         <v>1</v>
       </c>
       <c r="K20" s="39" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L20" s="39"/>
       <c r="M20" s="39"/>
@@ -2819,7 +2819,7 @@
         <v>0</v>
       </c>
       <c r="Q20" s="37" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="R20" s="37"/>
       <c r="S20" s="37"/>
@@ -2827,7 +2827,7 @@
       <c r="U20" s="37"/>
       <c r="V20" s="37"/>
       <c r="W20" s="38" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="X20" s="38"/>
       <c r="Y20" s="38"/>
@@ -2842,7 +2842,7 @@
       <c r="AH20" s="38"/>
       <c r="AI20" s="38"/>
       <c r="AK20" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
@@ -2850,7 +2850,7 @@
         <v>8</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D21" s="36" t="s">
         <v>5</v>
@@ -2917,7 +2917,7 @@
         <v>0</v>
       </c>
       <c r="AB21" s="38" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="AC21" s="38"/>
       <c r="AD21" s="38"/>
@@ -2927,7 +2927,7 @@
       <c r="AH21" s="38"/>
       <c r="AI21" s="38"/>
       <c r="AK21" s="10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.25">
@@ -3097,7 +3097,7 @@
       <c r="AH23" s="38"/>
       <c r="AI23" s="38"/>
       <c r="AK23" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
@@ -3943,8 +3943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3962,13 +3962,13 @@
   <sheetData>
     <row r="1" spans="1:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="30" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B1" s="31">
         <v>1</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -3976,7 +3976,7 @@
     </row>
     <row r="2" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="44" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B2" s="45"/>
       <c r="C2" s="45"/>
@@ -3990,7 +3990,7 @@
       <c r="K2" s="45"/>
       <c r="L2" s="46"/>
       <c r="M2" s="20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4017,10 +4017,10 @@
         <v>0</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3" t="s">
@@ -4030,13 +4030,13 @@
         <v>97</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="P3" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q3" s="23" t="s">
         <v>184</v>
-      </c>
-      <c r="Q3" s="23" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -4074,16 +4074,16 @@
         <v>17</v>
       </c>
       <c r="M4" t="s">
-        <v>98</v>
+        <v>310</v>
       </c>
       <c r="N4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="Q4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -4121,16 +4121,16 @@
         <v>47</v>
       </c>
       <c r="M5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="Q5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -4168,16 +4168,16 @@
         <v>77</v>
       </c>
       <c r="M6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="Q6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -4215,16 +4215,16 @@
         <v>78</v>
       </c>
       <c r="M7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="Q7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -4262,12 +4262,12 @@
         <v>91</v>
       </c>
       <c r="M8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6">
@@ -4297,21 +4297,21 @@
         <v>25h</v>
       </c>
       <c r="L9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="M9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="N9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P9" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6">
@@ -4341,21 +4341,21 @@
         <v>26h</v>
       </c>
       <c r="L10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="N10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P10" s="19" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6">
@@ -4385,13 +4385,13 @@
         <v>3Eh</v>
       </c>
       <c r="L11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="M11" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="P11" s="19" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -4429,10 +4429,10 @@
         <v>80</v>
       </c>
       <c r="M12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="P12" s="19" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -4470,10 +4470,10 @@
         <v>48</v>
       </c>
       <c r="M13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -4511,10 +4511,10 @@
         <v>49</v>
       </c>
       <c r="M14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -4552,10 +4552,10 @@
         <v>50</v>
       </c>
       <c r="M15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -4593,10 +4593,10 @@
         <v>51</v>
       </c>
       <c r="M16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -4634,10 +4634,10 @@
         <v>52</v>
       </c>
       <c r="M17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -4675,10 +4675,10 @@
         <v>53</v>
       </c>
       <c r="M18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -4716,10 +4716,10 @@
         <v>54</v>
       </c>
       <c r="M19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N19" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -4757,10 +4757,10 @@
         <v>55</v>
       </c>
       <c r="M20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -4798,10 +4798,10 @@
         <v>56</v>
       </c>
       <c r="M21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -4839,10 +4839,10 @@
         <v>57</v>
       </c>
       <c r="M22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -4880,10 +4880,10 @@
         <v>58</v>
       </c>
       <c r="M23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N23" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -4921,10 +4921,10 @@
         <v>59</v>
       </c>
       <c r="M24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -4962,10 +4962,10 @@
         <v>60</v>
       </c>
       <c r="M25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -5003,10 +5003,10 @@
         <v>61</v>
       </c>
       <c r="M26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -5044,10 +5044,10 @@
         <v>62</v>
       </c>
       <c r="M27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N27" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -5085,10 +5085,10 @@
         <v>63</v>
       </c>
       <c r="M28" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N28" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -5126,10 +5126,10 @@
         <v>64</v>
       </c>
       <c r="M29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N29" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -5167,10 +5167,10 @@
         <v>65</v>
       </c>
       <c r="M30" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N30" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -5208,10 +5208,10 @@
         <v>66</v>
       </c>
       <c r="M31" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -5249,15 +5249,15 @@
         <v>67</v>
       </c>
       <c r="M32" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="N32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="6">
@@ -5287,13 +5287,13 @@
         <v>18h</v>
       </c>
       <c r="L33" t="s">
+        <v>200</v>
+      </c>
+      <c r="M33" t="s">
         <v>201</v>
       </c>
-      <c r="M33" t="s">
-        <v>202</v>
-      </c>
       <c r="N33" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -5331,10 +5331,10 @@
         <v>68</v>
       </c>
       <c r="M34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N34" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
@@ -5372,10 +5372,10 @@
         <v>69</v>
       </c>
       <c r="M35" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
@@ -5413,10 +5413,10 @@
         <v>70</v>
       </c>
       <c r="M36" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N36" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
@@ -5454,10 +5454,10 @@
         <v>71</v>
       </c>
       <c r="M37" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N37" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -5495,10 +5495,10 @@
         <v>72</v>
       </c>
       <c r="M38" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N38" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
@@ -5536,10 +5536,10 @@
         <v>73</v>
       </c>
       <c r="M39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N39" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
@@ -5577,10 +5577,10 @@
         <v>74</v>
       </c>
       <c r="M40" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N40" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
@@ -5659,13 +5659,13 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="30" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B1" s="31">
         <v>2</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -5673,7 +5673,7 @@
     </row>
     <row r="2" spans="1:6" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="28" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B2" s="32"/>
       <c r="C2" s="28"/>
@@ -5683,129 +5683,129 @@
     </row>
     <row r="3" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B3" s="33"/>
       <c r="C3" s="3" t="s">
         <v>97</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C10" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E10" t="s">
+        <v>235</v>
+      </c>
+      <c r="F10" t="s">
         <v>236</v>
-      </c>
-      <c r="F10" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="28" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B11" s="32"/>
       <c r="C11" s="28"/>
@@ -5815,118 +5815,118 @@
     </row>
     <row r="12" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="3" t="s">
         <v>97</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C14" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C15" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D15" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E15" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C16" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D16" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E16" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C17" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D17" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E17" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C18" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E18" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F18" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="30" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B19" s="31">
         <v>3</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -5934,42 +5934,42 @@
     </row>
     <row r="20" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B20" s="33"/>
       <c r="C20" s="3" t="s">
         <v>97</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F20" s="23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="26" t="s">
+        <v>263</v>
+      </c>
+      <c r="C21" t="s">
+        <v>265</v>
+      </c>
+      <c r="D21" t="s">
         <v>264</v>
-      </c>
-      <c r="C21" t="s">
-        <v>266</v>
-      </c>
-      <c r="D21" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="30" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B22" s="31">
         <v>4</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -5977,81 +5977,81 @@
     </row>
     <row r="23" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B23" s="33"/>
       <c r="C23" s="3" t="s">
         <v>97</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F23" s="23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
+        <v>266</v>
+      </c>
+      <c r="C24" t="s">
         <v>267</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
+        <v>301</v>
+      </c>
+      <c r="E24" t="s">
         <v>268</v>
-      </c>
-      <c r="D24" t="s">
-        <v>302</v>
-      </c>
-      <c r="E24" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C25" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D25" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E25" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="26" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C26" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E26" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="26" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C27" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D27" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E27" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="30" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B28" s="31">
         <v>5</v>
@@ -6065,51 +6065,51 @@
     </row>
     <row r="29" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B29" s="33"/>
       <c r="C29" s="3" t="s">
         <v>97</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F29" s="23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="26" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="26" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="30" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B34" s="31">
         <v>6</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -6117,66 +6117,66 @@
     </row>
     <row r="35" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B35" s="33"/>
       <c r="C35" s="3" t="s">
         <v>97</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F35" s="23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="26" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="26" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="26" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="26" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="26" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="26" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="26" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="30" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B43" s="31">
         <v>7</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -6184,31 +6184,31 @@
     </row>
     <row r="44" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B44" s="33"/>
       <c r="C44" s="3" t="s">
         <v>97</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F44" s="23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="30" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B46" s="31">
         <v>8</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -6216,31 +6216,31 @@
     </row>
     <row r="47" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B47" s="33"/>
       <c r="C47" s="3" t="s">
         <v>97</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F47" s="23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="30" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B49" s="31">
         <v>9</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
@@ -6248,31 +6248,31 @@
     </row>
     <row r="50" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B50" s="33"/>
       <c r="C50" s="3" t="s">
         <v>97</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F50" s="23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="30" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B52" s="31">
         <v>10</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
@@ -6280,31 +6280,31 @@
     </row>
     <row r="53" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B53" s="33"/>
       <c r="C53" s="3" t="s">
         <v>97</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F53" s="23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="30" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B55" s="31">
         <v>11</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
@@ -6312,25 +6312,25 @@
     </row>
     <row r="56" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B56" s="33"/>
       <c r="C56" s="3" t="s">
         <v>97</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F56" s="23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="30" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B58" s="31">
         <v>12</v>
@@ -6344,20 +6344,20 @@
     </row>
     <row r="59" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B59" s="33"/>
       <c r="C59" s="3" t="s">
         <v>97</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F59" s="23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -6383,7 +6383,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="47" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B1" s="47"/>
       <c r="C1" s="47"/>
@@ -6428,15 +6428,15 @@
         <v>0</v>
       </c>
       <c r="K3" s="33" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L3" s="33" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C4" s="25">
         <v>0</v>
@@ -6473,7 +6473,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C5" s="25">
         <v>0</v>
@@ -6510,7 +6510,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C6" s="25">
         <v>0</v>
@@ -6547,7 +6547,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C7" s="25">
         <v>0</v>
@@ -6920,7 +6920,7 @@
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C6" s="6">
         <v>0</v>
@@ -6947,7 +6947,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="38" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L6" s="38"/>
       <c r="M6" s="38"/>
@@ -6957,7 +6957,7 @@
       <c r="Q6" s="38"/>
       <c r="R6" s="38"/>
       <c r="S6" s="38" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="T6" s="38"/>
       <c r="U6" s="38"/>
@@ -6967,7 +6967,7 @@
       <c r="Y6" s="38"/>
       <c r="Z6" s="38"/>
       <c r="AA6" s="38" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AB6" s="38"/>
       <c r="AC6" s="38"/>
@@ -8141,7 +8141,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -8216,7 +8216,7 @@
         <v>0</v>
       </c>
       <c r="T3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -8238,12 +8238,12 @@
       <c r="Q4" s="40"/>
       <c r="R4" s="40"/>
       <c r="T4" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C5" s="6">
         <v>0</v>
@@ -8291,15 +8291,15 @@
         <v>1</v>
       </c>
       <c r="R5" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="T5" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C6" s="24">
         <v>0</v>
@@ -8347,13 +8347,13 @@
         <v>0</v>
       </c>
       <c r="R6" s="24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="T6" s="10"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C7" s="6">
         <v>0</v>
@@ -8380,7 +8380,7 @@
         <v>1</v>
       </c>
       <c r="K7" s="38" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L7" s="38"/>
       <c r="M7" s="38"/>
@@ -8393,7 +8393,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C8" s="6">
         <v>0</v>
@@ -8417,10 +8417,10 @@
         <v>1</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K8" s="38" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L8" s="38"/>
       <c r="M8" s="38"/>
@@ -8433,7 +8433,7 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C9" s="6">
         <v>0</v>
@@ -8457,10 +8457,10 @@
         <v>0</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K9" s="38" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L9" s="38"/>
       <c r="M9" s="38"/>
@@ -8473,7 +8473,7 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C10" s="6">
         <v>0</v>
@@ -8497,10 +8497,10 @@
         <v>1</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K10" s="38" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L10" s="38"/>
       <c r="M10" s="38"/>

</xml_diff>

<commit_message>
update instruction set - Added integer mathematics
</commit_message>
<xml_diff>
--- a/doc/RiscyInstSet32Bit.xlsx
+++ b/doc/RiscyInstSet32Bit.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="311">
   <si>
     <t>Description</t>
   </si>
@@ -1169,7 +1169,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="6" applyFont="1"/>
@@ -1237,6 +1237,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1878,17 +1884,17 @@
       </c>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A8" s="35">
+      <c r="A8" s="37">
         <v>1</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="43" t="s">
+      <c r="D8" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
       <c r="G8" s="11">
         <v>0</v>
       </c>
@@ -1901,21 +1907,21 @@
       <c r="J8" s="11">
         <v>0</v>
       </c>
-      <c r="K8" s="40" t="s">
+      <c r="K8" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="L8" s="40"/>
-      <c r="M8" s="40"/>
-      <c r="N8" s="40" t="s">
+      <c r="L8" s="42"/>
+      <c r="M8" s="42"/>
+      <c r="N8" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="O8" s="40"/>
-      <c r="P8" s="40"/>
-      <c r="Q8" s="40" t="s">
+      <c r="O8" s="42"/>
+      <c r="P8" s="42"/>
+      <c r="Q8" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="R8" s="40"/>
-      <c r="S8" s="40"/>
+      <c r="R8" s="42"/>
+      <c r="S8" s="42"/>
       <c r="T8" s="12">
         <v>0</v>
       </c>
@@ -1946,28 +1952,28 @@
       <c r="AC8" s="6">
         <v>0</v>
       </c>
-      <c r="AD8" s="40" t="s">
+      <c r="AD8" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="AE8" s="40"/>
-      <c r="AF8" s="40"/>
-      <c r="AG8" s="40"/>
-      <c r="AH8" s="40"/>
-      <c r="AI8" s="40"/>
+      <c r="AE8" s="42"/>
+      <c r="AF8" s="42"/>
+      <c r="AG8" s="42"/>
+      <c r="AH8" s="42"/>
+      <c r="AI8" s="42"/>
       <c r="AK8" s="10" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
+      <c r="A9" s="36"/>
       <c r="B9" s="7" t="s">
         <v>308</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
       <c r="G9" s="18">
         <v>0</v>
       </c>
@@ -1980,19 +1986,19 @@
       <c r="J9" s="18">
         <v>0</v>
       </c>
-      <c r="K9" s="37" t="s">
+      <c r="K9" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="L9" s="37"/>
-      <c r="M9" s="37"/>
-      <c r="N9" s="39" t="s">
+      <c r="L9" s="39"/>
+      <c r="M9" s="39"/>
+      <c r="N9" s="41" t="s">
         <v>159</v>
       </c>
-      <c r="O9" s="39"/>
-      <c r="P9" s="39"/>
-      <c r="Q9" s="39"/>
-      <c r="R9" s="39"/>
-      <c r="S9" s="39"/>
+      <c r="O9" s="41"/>
+      <c r="P9" s="41"/>
+      <c r="Q9" s="41"/>
+      <c r="R9" s="41"/>
+      <c r="S9" s="41"/>
       <c r="T9" s="12">
         <v>0</v>
       </c>
@@ -2046,15 +2052,15 @@
       </c>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
       <c r="G10" s="18">
         <v>0</v>
       </c>
@@ -2067,21 +2073,21 @@
       <c r="J10" s="18">
         <v>0</v>
       </c>
-      <c r="K10" s="41" t="s">
+      <c r="K10" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="L10" s="41"/>
-      <c r="M10" s="41"/>
-      <c r="N10" s="41" t="s">
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="43" t="s">
         <v>158</v>
       </c>
-      <c r="O10" s="41"/>
-      <c r="P10" s="41"/>
-      <c r="Q10" s="42" t="s">
+      <c r="O10" s="43"/>
+      <c r="P10" s="43"/>
+      <c r="Q10" s="44" t="s">
         <v>159</v>
       </c>
-      <c r="R10" s="42"/>
-      <c r="S10" s="42"/>
+      <c r="R10" s="44"/>
+      <c r="S10" s="44"/>
       <c r="T10" s="12">
         <v>0</v>
       </c>
@@ -2141,11 +2147,11 @@
       <c r="B11" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="D11" s="36" t="s">
+      <c r="D11" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
       <c r="G11" s="6">
         <v>0</v>
       </c>
@@ -2158,21 +2164,21 @@
       <c r="J11" s="12">
         <v>0</v>
       </c>
-      <c r="K11" s="38" t="s">
+      <c r="K11" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="L11" s="38"/>
-      <c r="M11" s="38"/>
-      <c r="N11" s="38" t="s">
+      <c r="L11" s="40"/>
+      <c r="M11" s="40"/>
+      <c r="N11" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="O11" s="38"/>
-      <c r="P11" s="38"/>
-      <c r="Q11" s="38" t="s">
+      <c r="O11" s="40"/>
+      <c r="P11" s="40"/>
+      <c r="Q11" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="R11" s="38"/>
-      <c r="S11" s="38"/>
+      <c r="R11" s="40"/>
+      <c r="S11" s="40"/>
       <c r="T11" s="6">
         <v>0</v>
       </c>
@@ -2212,10 +2218,10 @@
       <c r="AF11" s="6">
         <v>0</v>
       </c>
-      <c r="AG11" s="36" t="s">
+      <c r="AG11" s="38" t="s">
         <v>172</v>
       </c>
-      <c r="AH11" s="36"/>
+      <c r="AH11" s="38"/>
       <c r="AI11" s="22" t="s">
         <v>87</v>
       </c>
@@ -2233,11 +2239,11 @@
       <c r="B12" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D12" s="36" t="s">
+      <c r="D12" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
       <c r="G12" s="6">
         <v>0</v>
       </c>
@@ -2250,31 +2256,31 @@
       <c r="J12" s="12">
         <v>0</v>
       </c>
-      <c r="K12" s="38" t="s">
+      <c r="K12" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="L12" s="38"/>
-      <c r="M12" s="38"/>
-      <c r="N12" s="38" t="s">
+      <c r="L12" s="40"/>
+      <c r="M12" s="40"/>
+      <c r="N12" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="O12" s="38"/>
-      <c r="P12" s="38"/>
-      <c r="Q12" s="38" t="s">
+      <c r="O12" s="40"/>
+      <c r="P12" s="40"/>
+      <c r="Q12" s="40" t="s">
         <v>129</v>
       </c>
-      <c r="R12" s="38"/>
-      <c r="S12" s="38"/>
-      <c r="T12" s="38" t="s">
+      <c r="R12" s="40"/>
+      <c r="S12" s="40"/>
+      <c r="T12" s="40" t="s">
         <v>174</v>
       </c>
-      <c r="U12" s="38"/>
-      <c r="V12" s="38"/>
-      <c r="W12" s="38" t="s">
+      <c r="U12" s="40"/>
+      <c r="V12" s="40"/>
+      <c r="W12" s="40" t="s">
         <v>175</v>
       </c>
-      <c r="X12" s="38"/>
-      <c r="Y12" s="38"/>
+      <c r="X12" s="40"/>
+      <c r="Y12" s="40"/>
       <c r="Z12" s="6">
         <v>0</v>
       </c>
@@ -2316,11 +2322,11 @@
       <c r="B13" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="D13" s="36" t="s">
+      <c r="D13" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
       <c r="G13" s="6">
         <v>0</v>
       </c>
@@ -2333,16 +2339,16 @@
       <c r="J13" s="12">
         <v>1</v>
       </c>
-      <c r="K13" s="38" t="s">
+      <c r="K13" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="L13" s="38"/>
-      <c r="M13" s="38"/>
-      <c r="N13" s="38" t="s">
+      <c r="L13" s="40"/>
+      <c r="M13" s="40"/>
+      <c r="N13" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="O13" s="38"/>
-      <c r="P13" s="38"/>
+      <c r="O13" s="40"/>
+      <c r="P13" s="40"/>
       <c r="Q13" s="6">
         <v>0</v>
       </c>
@@ -2405,17 +2411,17 @@
       </c>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A14" s="34">
+      <c r="A14" s="36">
         <v>2</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="D14" s="36" t="s">
+      <c r="D14" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
       <c r="G14" s="6">
         <v>0</v>
       </c>
@@ -2428,16 +2434,16 @@
       <c r="J14" s="12">
         <v>1</v>
       </c>
-      <c r="K14" s="38" t="s">
+      <c r="K14" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="L14" s="38"/>
-      <c r="M14" s="38"/>
-      <c r="N14" s="38" t="s">
+      <c r="L14" s="40"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="O14" s="38"/>
-      <c r="P14" s="38"/>
+      <c r="O14" s="40"/>
+      <c r="P14" s="40"/>
       <c r="Q14" s="6">
         <v>0</v>
       </c>
@@ -2471,30 +2477,30 @@
       <c r="AA14" s="6">
         <v>0</v>
       </c>
-      <c r="AB14" s="38" t="s">
+      <c r="AB14" s="40" t="s">
         <v>156</v>
       </c>
-      <c r="AC14" s="38"/>
-      <c r="AD14" s="38"/>
-      <c r="AE14" s="38"/>
-      <c r="AF14" s="38"/>
-      <c r="AG14" s="38"/>
-      <c r="AH14" s="38"/>
-      <c r="AI14" s="38"/>
+      <c r="AC14" s="40"/>
+      <c r="AD14" s="40"/>
+      <c r="AE14" s="40"/>
+      <c r="AF14" s="40"/>
+      <c r="AG14" s="40"/>
+      <c r="AH14" s="40"/>
+      <c r="AI14" s="40"/>
       <c r="AK14" s="10" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
+      <c r="A15" s="36"/>
       <c r="B15" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="D15" s="36" t="s">
+      <c r="D15" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
       <c r="G15" s="6">
         <v>0</v>
       </c>
@@ -2507,16 +2513,16 @@
       <c r="J15" s="12">
         <v>1</v>
       </c>
-      <c r="K15" s="38" t="s">
+      <c r="K15" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="L15" s="38"/>
-      <c r="M15" s="38"/>
-      <c r="N15" s="38" t="s">
+      <c r="L15" s="40"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="O15" s="38"/>
-      <c r="P15" s="38"/>
+      <c r="O15" s="40"/>
+      <c r="P15" s="40"/>
       <c r="Q15" s="6">
         <v>1</v>
       </c>
@@ -2526,38 +2532,38 @@
       <c r="S15" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="T15" s="38" t="s">
+      <c r="T15" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="U15" s="38"/>
-      <c r="V15" s="38"/>
-      <c r="W15" s="38"/>
-      <c r="X15" s="38"/>
-      <c r="Y15" s="38"/>
-      <c r="Z15" s="38"/>
-      <c r="AA15" s="38"/>
-      <c r="AB15" s="38"/>
-      <c r="AC15" s="38"/>
-      <c r="AD15" s="38"/>
-      <c r="AE15" s="38"/>
-      <c r="AF15" s="38"/>
-      <c r="AG15" s="38"/>
-      <c r="AH15" s="38"/>
-      <c r="AI15" s="38"/>
+      <c r="U15" s="40"/>
+      <c r="V15" s="40"/>
+      <c r="W15" s="40"/>
+      <c r="X15" s="40"/>
+      <c r="Y15" s="40"/>
+      <c r="Z15" s="40"/>
+      <c r="AA15" s="40"/>
+      <c r="AB15" s="40"/>
+      <c r="AC15" s="40"/>
+      <c r="AD15" s="40"/>
+      <c r="AE15" s="40"/>
+      <c r="AF15" s="40"/>
+      <c r="AG15" s="40"/>
+      <c r="AH15" s="40"/>
+      <c r="AI15" s="40"/>
       <c r="AK15" s="10" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
+      <c r="A16" s="36"/>
       <c r="B16" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="D16" s="36" t="s">
+      <c r="D16" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
       <c r="G16" s="6">
         <v>0</v>
       </c>
@@ -2570,16 +2576,16 @@
       <c r="J16" s="12">
         <v>1</v>
       </c>
-      <c r="K16" s="38" t="s">
+      <c r="K16" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="L16" s="38"/>
-      <c r="M16" s="38"/>
-      <c r="N16" s="38" t="s">
+      <c r="L16" s="40"/>
+      <c r="M16" s="40"/>
+      <c r="N16" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="O16" s="38"/>
-      <c r="P16" s="38"/>
+      <c r="O16" s="40"/>
+      <c r="P16" s="40"/>
       <c r="Q16" s="6">
         <v>1</v>
       </c>
@@ -2589,38 +2595,38 @@
       <c r="S16" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="T16" s="38" t="s">
+      <c r="T16" s="40" t="s">
         <v>155</v>
       </c>
-      <c r="U16" s="38"/>
-      <c r="V16" s="38"/>
-      <c r="W16" s="38"/>
-      <c r="X16" s="38"/>
-      <c r="Y16" s="38"/>
-      <c r="Z16" s="38"/>
-      <c r="AA16" s="38"/>
-      <c r="AB16" s="38"/>
-      <c r="AC16" s="38"/>
-      <c r="AD16" s="38"/>
-      <c r="AE16" s="38"/>
-      <c r="AF16" s="38"/>
-      <c r="AG16" s="38"/>
-      <c r="AH16" s="38"/>
-      <c r="AI16" s="38"/>
+      <c r="U16" s="40"/>
+      <c r="V16" s="40"/>
+      <c r="W16" s="40"/>
+      <c r="X16" s="40"/>
+      <c r="Y16" s="40"/>
+      <c r="Z16" s="40"/>
+      <c r="AA16" s="40"/>
+      <c r="AB16" s="40"/>
+      <c r="AC16" s="40"/>
+      <c r="AD16" s="40"/>
+      <c r="AE16" s="40"/>
+      <c r="AF16" s="40"/>
+      <c r="AG16" s="40"/>
+      <c r="AH16" s="40"/>
+      <c r="AI16" s="40"/>
       <c r="AK16" s="10" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A17" s="34"/>
+      <c r="A17" s="36"/>
       <c r="B17" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="D17" s="36" t="s">
+      <c r="D17" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
       <c r="G17" s="6">
         <v>0</v>
       </c>
@@ -2633,35 +2639,35 @@
       <c r="J17" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="K17" s="38" t="s">
+      <c r="K17" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="L17" s="38"/>
-      <c r="M17" s="38"/>
-      <c r="N17" s="38" t="s">
+      <c r="L17" s="40"/>
+      <c r="M17" s="40"/>
+      <c r="N17" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="O17" s="38"/>
-      <c r="P17" s="38"/>
-      <c r="Q17" s="38"/>
-      <c r="R17" s="38"/>
-      <c r="S17" s="38"/>
-      <c r="T17" s="38"/>
-      <c r="U17" s="38"/>
-      <c r="V17" s="38"/>
-      <c r="W17" s="38"/>
-      <c r="X17" s="38"/>
-      <c r="Y17" s="38"/>
-      <c r="Z17" s="38"/>
-      <c r="AA17" s="38"/>
-      <c r="AB17" s="38"/>
-      <c r="AC17" s="38"/>
-      <c r="AD17" s="38"/>
-      <c r="AE17" s="38"/>
-      <c r="AF17" s="38"/>
-      <c r="AG17" s="38"/>
-      <c r="AH17" s="38"/>
-      <c r="AI17" s="38"/>
+      <c r="O17" s="40"/>
+      <c r="P17" s="40"/>
+      <c r="Q17" s="40"/>
+      <c r="R17" s="40"/>
+      <c r="S17" s="40"/>
+      <c r="T17" s="40"/>
+      <c r="U17" s="40"/>
+      <c r="V17" s="40"/>
+      <c r="W17" s="40"/>
+      <c r="X17" s="40"/>
+      <c r="Y17" s="40"/>
+      <c r="Z17" s="40"/>
+      <c r="AA17" s="40"/>
+      <c r="AB17" s="40"/>
+      <c r="AC17" s="40"/>
+      <c r="AD17" s="40"/>
+      <c r="AE17" s="40"/>
+      <c r="AF17" s="40"/>
+      <c r="AG17" s="40"/>
+      <c r="AH17" s="40"/>
+      <c r="AI17" s="40"/>
       <c r="AK17" s="10" t="s">
         <v>182</v>
       </c>
@@ -2673,11 +2679,11 @@
       <c r="B18" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="36" t="s">
+      <c r="D18" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
       <c r="G18" s="6">
         <v>0</v>
       </c>
@@ -2690,35 +2696,35 @@
       <c r="J18" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="K18" s="38" t="s">
+      <c r="K18" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="L18" s="38"/>
-      <c r="M18" s="38"/>
-      <c r="N18" s="38" t="s">
+      <c r="L18" s="40"/>
+      <c r="M18" s="40"/>
+      <c r="N18" s="40" t="s">
         <v>178</v>
       </c>
-      <c r="O18" s="38"/>
-      <c r="P18" s="38"/>
-      <c r="Q18" s="38"/>
-      <c r="R18" s="38"/>
-      <c r="S18" s="38"/>
-      <c r="T18" s="38"/>
-      <c r="U18" s="38"/>
-      <c r="V18" s="38"/>
-      <c r="W18" s="38"/>
-      <c r="X18" s="38"/>
-      <c r="Y18" s="38"/>
-      <c r="Z18" s="38"/>
-      <c r="AA18" s="38"/>
-      <c r="AB18" s="38"/>
-      <c r="AC18" s="38"/>
-      <c r="AD18" s="38"/>
-      <c r="AE18" s="38"/>
-      <c r="AF18" s="38"/>
-      <c r="AG18" s="38"/>
-      <c r="AH18" s="38"/>
-      <c r="AI18" s="38"/>
+      <c r="O18" s="40"/>
+      <c r="P18" s="40"/>
+      <c r="Q18" s="40"/>
+      <c r="R18" s="40"/>
+      <c r="S18" s="40"/>
+      <c r="T18" s="40"/>
+      <c r="U18" s="40"/>
+      <c r="V18" s="40"/>
+      <c r="W18" s="40"/>
+      <c r="X18" s="40"/>
+      <c r="Y18" s="40"/>
+      <c r="Z18" s="40"/>
+      <c r="AA18" s="40"/>
+      <c r="AB18" s="40"/>
+      <c r="AC18" s="40"/>
+      <c r="AD18" s="40"/>
+      <c r="AE18" s="40"/>
+      <c r="AF18" s="40"/>
+      <c r="AG18" s="40"/>
+      <c r="AH18" s="40"/>
+      <c r="AI18" s="40"/>
       <c r="AK18" s="10" t="s">
         <v>204</v>
       </c>
@@ -2730,11 +2736,11 @@
       <c r="B19" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="D19" s="36" t="s">
+      <c r="D19" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
       <c r="G19" s="6">
         <v>1</v>
       </c>
@@ -2747,35 +2753,35 @@
       <c r="J19" s="12">
         <v>0</v>
       </c>
-      <c r="K19" s="39" t="s">
+      <c r="K19" s="41" t="s">
         <v>159</v>
       </c>
-      <c r="L19" s="39"/>
-      <c r="M19" s="39"/>
-      <c r="N19" s="38" t="s">
+      <c r="L19" s="41"/>
+      <c r="M19" s="41"/>
+      <c r="N19" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="O19" s="38"/>
-      <c r="P19" s="38"/>
-      <c r="Q19" s="38"/>
-      <c r="R19" s="38"/>
-      <c r="S19" s="38"/>
-      <c r="T19" s="38"/>
-      <c r="U19" s="38"/>
-      <c r="V19" s="38"/>
-      <c r="W19" s="38"/>
-      <c r="X19" s="38"/>
-      <c r="Y19" s="38"/>
-      <c r="Z19" s="38"/>
-      <c r="AA19" s="38"/>
-      <c r="AB19" s="38"/>
-      <c r="AC19" s="38"/>
-      <c r="AD19" s="38"/>
-      <c r="AE19" s="38"/>
-      <c r="AF19" s="38"/>
-      <c r="AG19" s="38"/>
-      <c r="AH19" s="38"/>
-      <c r="AI19" s="38"/>
+      <c r="O19" s="40"/>
+      <c r="P19" s="40"/>
+      <c r="Q19" s="40"/>
+      <c r="R19" s="40"/>
+      <c r="S19" s="40"/>
+      <c r="T19" s="40"/>
+      <c r="U19" s="40"/>
+      <c r="V19" s="40"/>
+      <c r="W19" s="40"/>
+      <c r="X19" s="40"/>
+      <c r="Y19" s="40"/>
+      <c r="Z19" s="40"/>
+      <c r="AA19" s="40"/>
+      <c r="AB19" s="40"/>
+      <c r="AC19" s="40"/>
+      <c r="AD19" s="40"/>
+      <c r="AE19" s="40"/>
+      <c r="AF19" s="40"/>
+      <c r="AG19" s="40"/>
+      <c r="AH19" s="40"/>
+      <c r="AI19" s="40"/>
       <c r="AK19" s="10" t="s">
         <v>196</v>
       </c>
@@ -2787,11 +2793,11 @@
       <c r="B20" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="D20" s="36" t="s">
+      <c r="D20" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
       <c r="G20" s="24">
         <v>1</v>
       </c>
@@ -2804,11 +2810,11 @@
       <c r="J20" s="25">
         <v>1</v>
       </c>
-      <c r="K20" s="39" t="s">
+      <c r="K20" s="41" t="s">
         <v>159</v>
       </c>
-      <c r="L20" s="39"/>
-      <c r="M20" s="39"/>
+      <c r="L20" s="41"/>
+      <c r="M20" s="41"/>
       <c r="N20" s="25">
         <v>0</v>
       </c>
@@ -2818,29 +2824,29 @@
       <c r="P20" s="25">
         <v>0</v>
       </c>
-      <c r="Q20" s="37" t="s">
+      <c r="Q20" s="39" t="s">
         <v>254</v>
       </c>
-      <c r="R20" s="37"/>
-      <c r="S20" s="37"/>
-      <c r="T20" s="37"/>
-      <c r="U20" s="37"/>
-      <c r="V20" s="37"/>
-      <c r="W20" s="38" t="s">
+      <c r="R20" s="39"/>
+      <c r="S20" s="39"/>
+      <c r="T20" s="39"/>
+      <c r="U20" s="39"/>
+      <c r="V20" s="39"/>
+      <c r="W20" s="40" t="s">
         <v>253</v>
       </c>
-      <c r="X20" s="38"/>
-      <c r="Y20" s="38"/>
-      <c r="Z20" s="38"/>
-      <c r="AA20" s="38"/>
-      <c r="AB20" s="38"/>
-      <c r="AC20" s="38"/>
-      <c r="AD20" s="38"/>
-      <c r="AE20" s="38"/>
-      <c r="AF20" s="38"/>
-      <c r="AG20" s="38"/>
-      <c r="AH20" s="38"/>
-      <c r="AI20" s="38"/>
+      <c r="X20" s="40"/>
+      <c r="Y20" s="40"/>
+      <c r="Z20" s="40"/>
+      <c r="AA20" s="40"/>
+      <c r="AB20" s="40"/>
+      <c r="AC20" s="40"/>
+      <c r="AD20" s="40"/>
+      <c r="AE20" s="40"/>
+      <c r="AF20" s="40"/>
+      <c r="AG20" s="40"/>
+      <c r="AH20" s="40"/>
+      <c r="AI20" s="40"/>
       <c r="AK20" s="10" t="s">
         <v>257</v>
       </c>
@@ -2852,11 +2858,11 @@
       <c r="B21" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="D21" s="36" t="s">
+      <c r="D21" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
       <c r="G21" s="24">
         <v>1</v>
       </c>
@@ -2869,11 +2875,11 @@
       <c r="J21" s="25">
         <v>1</v>
       </c>
-      <c r="K21" s="37" t="s">
+      <c r="K21" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="L21" s="37"/>
-      <c r="M21" s="37"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="39"/>
       <c r="N21" s="25">
         <v>0</v>
       </c>
@@ -2916,16 +2922,16 @@
       <c r="AA21" s="24">
         <v>0</v>
       </c>
-      <c r="AB21" s="38" t="s">
+      <c r="AB21" s="40" t="s">
         <v>256</v>
       </c>
-      <c r="AC21" s="38"/>
-      <c r="AD21" s="38"/>
-      <c r="AE21" s="38"/>
-      <c r="AF21" s="38"/>
-      <c r="AG21" s="38"/>
-      <c r="AH21" s="38"/>
-      <c r="AI21" s="38"/>
+      <c r="AC21" s="40"/>
+      <c r="AD21" s="40"/>
+      <c r="AE21" s="40"/>
+      <c r="AF21" s="40"/>
+      <c r="AG21" s="40"/>
+      <c r="AH21" s="40"/>
+      <c r="AI21" s="40"/>
       <c r="AK21" s="10" t="s">
         <v>258</v>
       </c>
@@ -2937,11 +2943,11 @@
       <c r="B22" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D22" s="36" t="s">
+      <c r="D22" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
       <c r="G22" s="6">
         <v>1</v>
       </c>
@@ -2954,11 +2960,11 @@
       <c r="J22" s="6">
         <v>1</v>
       </c>
-      <c r="K22" s="38" t="s">
+      <c r="K22" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="L22" s="38"/>
-      <c r="M22" s="38"/>
+      <c r="L22" s="40"/>
+      <c r="M22" s="40"/>
       <c r="N22" s="6">
         <v>0</v>
       </c>
@@ -3001,16 +3007,16 @@
       <c r="AA22" s="6">
         <v>0</v>
       </c>
-      <c r="AB22" s="38" t="s">
+      <c r="AB22" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="AC22" s="38"/>
-      <c r="AD22" s="38"/>
-      <c r="AE22" s="38"/>
-      <c r="AF22" s="38"/>
-      <c r="AG22" s="38"/>
-      <c r="AH22" s="38"/>
-      <c r="AI22" s="38"/>
+      <c r="AC22" s="40"/>
+      <c r="AD22" s="40"/>
+      <c r="AE22" s="40"/>
+      <c r="AF22" s="40"/>
+      <c r="AG22" s="40"/>
+      <c r="AH22" s="40"/>
+      <c r="AI22" s="40"/>
       <c r="AK22" s="10" t="s">
         <v>86</v>
       </c>
@@ -3022,11 +3028,11 @@
       <c r="B23" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D23" s="36" t="s">
+      <c r="D23" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
       <c r="G23" s="6">
         <v>1</v>
       </c>
@@ -3039,11 +3045,11 @@
       <c r="J23" s="6">
         <v>1</v>
       </c>
-      <c r="K23" s="38" t="s">
+      <c r="K23" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="L23" s="38"/>
-      <c r="M23" s="38"/>
+      <c r="L23" s="40"/>
+      <c r="M23" s="40"/>
       <c r="N23" s="6">
         <v>0</v>
       </c>
@@ -3086,16 +3092,16 @@
       <c r="AA23" s="6">
         <v>1</v>
       </c>
-      <c r="AB23" s="38" t="s">
+      <c r="AB23" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="AC23" s="38"/>
-      <c r="AD23" s="38"/>
-      <c r="AE23" s="38"/>
-      <c r="AF23" s="38"/>
-      <c r="AG23" s="38"/>
-      <c r="AH23" s="38"/>
-      <c r="AI23" s="38"/>
+      <c r="AC23" s="40"/>
+      <c r="AD23" s="40"/>
+      <c r="AE23" s="40"/>
+      <c r="AF23" s="40"/>
+      <c r="AG23" s="40"/>
+      <c r="AH23" s="40"/>
+      <c r="AI23" s="40"/>
       <c r="AK23" s="10" t="s">
         <v>179</v>
       </c>
@@ -3107,11 +3113,11 @@
       <c r="B24" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D24" s="36" t="s">
+      <c r="D24" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
       <c r="G24" s="6">
         <v>1</v>
       </c>
@@ -3124,11 +3130,11 @@
       <c r="J24" s="6">
         <v>1</v>
       </c>
-      <c r="K24" s="38" t="s">
+      <c r="K24" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="L24" s="38"/>
-      <c r="M24" s="38"/>
+      <c r="L24" s="40"/>
+      <c r="M24" s="40"/>
       <c r="N24" s="6">
         <v>0</v>
       </c>
@@ -3204,11 +3210,11 @@
       <c r="B25" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="D25" s="36" t="s">
+      <c r="D25" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
       <c r="G25" s="6">
         <v>1</v>
       </c>
@@ -3272,16 +3278,16 @@
       <c r="AA25" s="6">
         <v>1</v>
       </c>
-      <c r="AB25" s="38" t="s">
+      <c r="AB25" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="AC25" s="38"/>
-      <c r="AD25" s="38"/>
-      <c r="AE25" s="38"/>
-      <c r="AF25" s="38"/>
-      <c r="AG25" s="38"/>
-      <c r="AH25" s="38"/>
-      <c r="AI25" s="38"/>
+      <c r="AC25" s="40"/>
+      <c r="AD25" s="40"/>
+      <c r="AE25" s="40"/>
+      <c r="AF25" s="40"/>
+      <c r="AG25" s="40"/>
+      <c r="AH25" s="40"/>
+      <c r="AI25" s="40"/>
     </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B32" s="7"/>
@@ -3941,10 +3947,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q42"/>
+  <dimension ref="A1:Q48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3961,13 +3967,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="B1" s="31">
-        <v>1</v>
-      </c>
-      <c r="C1" s="29" t="s">
+      <c r="B1" s="33">
+        <v>1</v>
+      </c>
+      <c r="C1" s="31" t="s">
         <v>292</v>
       </c>
       <c r="D1" s="1"/>
@@ -3975,20 +3981,20 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="46" t="s">
         <v>162</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="46"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="48"/>
       <c r="M2" s="20" t="s">
         <v>161</v>
       </c>
@@ -4048,7 +4054,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="6">
         <v>0</v>
@@ -4064,11 +4070,11 @@
       </c>
       <c r="I4" s="24">
         <f>_xlfn.DECIMAL(CONCATENATE(C4,D4,E4,F4,G4,H4),2)</f>
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="J4" s="24" t="str">
         <f>DEC2HEX(I4,2)&amp;"h"</f>
-        <v>20h</v>
+        <v>30h</v>
       </c>
       <c r="L4" t="s">
         <v>17</v>
@@ -4095,7 +4101,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="6">
         <v>0</v>
@@ -4110,12 +4116,12 @@
         <v>1</v>
       </c>
       <c r="I5" s="24">
-        <f t="shared" ref="I5:I41" si="0">_xlfn.DECIMAL(CONCATENATE(C5,D5,E5,F5,G5,H5),2)</f>
-        <v>33</v>
+        <f t="shared" ref="I5:I47" si="0">_xlfn.DECIMAL(CONCATENATE(C5,D5,E5,F5,G5,H5),2)</f>
+        <v>49</v>
       </c>
       <c r="J5" s="24" t="str">
-        <f t="shared" ref="J5:J41" si="1">DEC2HEX(I5,2)&amp;"h"</f>
-        <v>21h</v>
+        <f t="shared" ref="J5:J47" si="1">DEC2HEX(I5,2)&amp;"h"</f>
+        <v>31h</v>
       </c>
       <c r="L5" t="s">
         <v>47</v>
@@ -4142,7 +4148,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="6">
         <v>0</v>
@@ -4158,11 +4164,11 @@
       </c>
       <c r="I6" s="24">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="J6" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>22h</v>
+        <v>32h</v>
       </c>
       <c r="L6" t="s">
         <v>77</v>
@@ -4189,7 +4195,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="6">
         <v>0</v>
@@ -4205,11 +4211,11 @@
       </c>
       <c r="I7" s="24">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="J7" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>23h</v>
+        <v>33h</v>
       </c>
       <c r="L7" t="s">
         <v>78</v>
@@ -4236,7 +4242,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="6">
         <v>0</v>
@@ -4252,11 +4258,11 @@
       </c>
       <c r="I8" s="24">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="J8" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>24h</v>
+        <v>34h</v>
       </c>
       <c r="L8" t="s">
         <v>91</v>
@@ -4274,7 +4280,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="6">
         <v>0</v>
@@ -4283,18 +4289,18 @@
         <v>1</v>
       </c>
       <c r="G9" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9" s="24">
         <f t="shared" si="0"/>
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="J9" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>25h</v>
+        <v>36h</v>
       </c>
       <c r="L9" t="s">
         <v>167</v>
@@ -4318,7 +4324,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="6">
         <v>0</v>
@@ -4330,15 +4336,15 @@
         <v>1</v>
       </c>
       <c r="H10" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" s="24">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="J10" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>26h</v>
+        <v>37h</v>
       </c>
       <c r="L10" t="s">
         <v>168</v>
@@ -4682,954 +4688,1218 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="30" t="str">
+        <f>A13&amp;" integer"</f>
+        <v>Add integer</v>
+      </c>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29">
+        <v>1</v>
+      </c>
+      <c r="D19" s="29">
+        <v>0</v>
+      </c>
+      <c r="E19" s="29">
+        <v>0</v>
+      </c>
+      <c r="F19" s="29">
+        <v>0</v>
+      </c>
+      <c r="G19" s="29">
+        <v>0</v>
+      </c>
+      <c r="H19" s="29">
+        <v>1</v>
+      </c>
+      <c r="I19" s="29">
+        <f t="shared" ref="I19:I24" si="2">_xlfn.DECIMAL(CONCATENATE(C19,D19,E19,F19,G19,H19),2)</f>
+        <v>33</v>
+      </c>
+      <c r="J19" s="29" t="str">
+        <f t="shared" ref="J19:J24" si="3">DEC2HEX(I19,2)&amp;"h"</f>
+        <v>21h</v>
+      </c>
+      <c r="L19" t="str">
+        <f>L13&amp;"INT"</f>
+        <v>ADDINT</v>
+      </c>
+      <c r="M19" t="str">
+        <f>M13</f>
+        <v>Rd = Rs + Rm</v>
+      </c>
+      <c r="N19" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="30" t="str">
+        <f t="shared" ref="A20:A24" si="4">A14&amp;" integer"</f>
+        <v>Subtract integer</v>
+      </c>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29">
+        <v>1</v>
+      </c>
+      <c r="D20" s="29">
+        <v>0</v>
+      </c>
+      <c r="E20" s="29">
+        <v>0</v>
+      </c>
+      <c r="F20" s="29">
+        <v>0</v>
+      </c>
+      <c r="G20" s="29">
+        <v>1</v>
+      </c>
+      <c r="H20" s="29">
+        <v>0</v>
+      </c>
+      <c r="I20" s="29">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="J20" s="29" t="str">
+        <f t="shared" si="3"/>
+        <v>22h</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" ref="L20:L24" si="5">L14&amp;"INT"</f>
+        <v>SUBINT</v>
+      </c>
+      <c r="M20" t="str">
+        <f t="shared" ref="M20:M24" si="6">M14</f>
+        <v>Rd = Rs - Rm</v>
+      </c>
+      <c r="N20" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="30" t="str">
+        <f t="shared" si="4"/>
+        <v>Multiply integer</v>
+      </c>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29">
+        <v>1</v>
+      </c>
+      <c r="D21" s="29">
+        <v>0</v>
+      </c>
+      <c r="E21" s="29">
+        <v>0</v>
+      </c>
+      <c r="F21" s="29">
+        <v>0</v>
+      </c>
+      <c r="G21" s="29">
+        <v>1</v>
+      </c>
+      <c r="H21" s="29">
+        <v>1</v>
+      </c>
+      <c r="I21" s="29">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="J21" s="29" t="str">
+        <f t="shared" si="3"/>
+        <v>23h</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="5"/>
+        <v>MULINT</v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" si="6"/>
+        <v>Rd = Rs * Rm</v>
+      </c>
+      <c r="N21" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="30" t="str">
+        <f t="shared" si="4"/>
+        <v>Divide integer</v>
+      </c>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29">
+        <v>1</v>
+      </c>
+      <c r="D22" s="29">
+        <v>0</v>
+      </c>
+      <c r="E22" s="29">
+        <v>0</v>
+      </c>
+      <c r="F22" s="29">
+        <v>1</v>
+      </c>
+      <c r="G22" s="29">
+        <v>0</v>
+      </c>
+      <c r="H22" s="29">
+        <v>0</v>
+      </c>
+      <c r="I22" s="29">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="J22" s="29" t="str">
+        <f t="shared" si="3"/>
+        <v>24h</v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="5"/>
+        <v>DIVINT</v>
+      </c>
+      <c r="M22" t="str">
+        <f t="shared" si="6"/>
+        <v>Rd = Rs / Rm</v>
+      </c>
+      <c r="N22" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="30" t="str">
+        <f t="shared" si="4"/>
+        <v>Powerof integer</v>
+      </c>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29">
+        <v>1</v>
+      </c>
+      <c r="D23" s="29">
+        <v>0</v>
+      </c>
+      <c r="E23" s="29">
+        <v>0</v>
+      </c>
+      <c r="F23" s="29">
+        <v>1</v>
+      </c>
+      <c r="G23" s="29">
+        <v>0</v>
+      </c>
+      <c r="H23" s="29">
+        <v>1</v>
+      </c>
+      <c r="I23" s="29">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="J23" s="29" t="str">
+        <f t="shared" si="3"/>
+        <v>25h</v>
+      </c>
+      <c r="L23" t="str">
+        <f t="shared" si="5"/>
+        <v>POWINT</v>
+      </c>
+      <c r="M23" t="str">
+        <f t="shared" si="6"/>
+        <v>Rd = Rs ^ Rm</v>
+      </c>
+      <c r="N23" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="30" t="str">
+        <f t="shared" si="4"/>
+        <v>Modulo integer</v>
+      </c>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29">
+        <v>1</v>
+      </c>
+      <c r="D24" s="29">
+        <v>0</v>
+      </c>
+      <c r="E24" s="29">
+        <v>0</v>
+      </c>
+      <c r="F24" s="29">
+        <v>1</v>
+      </c>
+      <c r="G24" s="29">
+        <v>1</v>
+      </c>
+      <c r="H24" s="29">
+        <v>0</v>
+      </c>
+      <c r="I24" s="29">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="J24" s="29" t="str">
+        <f t="shared" si="3"/>
+        <v>26h</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" si="5"/>
+        <v>MODINT</v>
+      </c>
+      <c r="M24" t="str">
+        <f t="shared" si="6"/>
+        <v>Rd = Rs % Rm</v>
+      </c>
+      <c r="N24" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6">
-        <v>0</v>
-      </c>
-      <c r="D19" s="6">
-        <v>0</v>
-      </c>
-      <c r="E19" s="6">
-        <v>0</v>
-      </c>
-      <c r="F19" s="6">
-        <v>1</v>
-      </c>
-      <c r="G19" s="6">
-        <v>1</v>
-      </c>
-      <c r="H19" s="6">
-        <v>1</v>
-      </c>
-      <c r="I19" s="24">
+      <c r="B25" s="6"/>
+      <c r="C25" s="6">
+        <v>0</v>
+      </c>
+      <c r="D25" s="6">
+        <v>0</v>
+      </c>
+      <c r="E25" s="6">
+        <v>0</v>
+      </c>
+      <c r="F25" s="6">
+        <v>1</v>
+      </c>
+      <c r="G25" s="6">
+        <v>1</v>
+      </c>
+      <c r="H25" s="6">
+        <v>1</v>
+      </c>
+      <c r="I25" s="24">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="J19" s="24" t="str">
+      <c r="J25" s="24" t="str">
         <f t="shared" si="1"/>
         <v>07h</v>
       </c>
-      <c r="L19" t="s">
+      <c r="L25" t="s">
         <v>54</v>
       </c>
-      <c r="M19" t="s">
+      <c r="M25" t="s">
         <v>109</v>
       </c>
-      <c r="N19" t="s">
+      <c r="N25" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6">
-        <v>0</v>
-      </c>
-      <c r="D20" s="6">
-        <v>0</v>
-      </c>
-      <c r="E20" s="6">
-        <v>1</v>
-      </c>
-      <c r="F20" s="6">
-        <v>0</v>
-      </c>
-      <c r="G20" s="6">
-        <v>0</v>
-      </c>
-      <c r="H20" s="6">
-        <v>0</v>
-      </c>
-      <c r="I20" s="24">
+      <c r="B26" s="6"/>
+      <c r="C26" s="6">
+        <v>0</v>
+      </c>
+      <c r="D26" s="6">
+        <v>0</v>
+      </c>
+      <c r="E26" s="6">
+        <v>1</v>
+      </c>
+      <c r="F26" s="6">
+        <v>0</v>
+      </c>
+      <c r="G26" s="6">
+        <v>0</v>
+      </c>
+      <c r="H26" s="6">
+        <v>0</v>
+      </c>
+      <c r="I26" s="24">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="J20" s="24" t="str">
+      <c r="J26" s="24" t="str">
         <f t="shared" si="1"/>
         <v>08h</v>
       </c>
-      <c r="L20" t="s">
+      <c r="L26" t="s">
         <v>55</v>
       </c>
-      <c r="M20" t="s">
+      <c r="M26" t="s">
         <v>110</v>
       </c>
-      <c r="N20" t="s">
+      <c r="N26" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6">
-        <v>0</v>
-      </c>
-      <c r="D21" s="6">
-        <v>0</v>
-      </c>
-      <c r="E21" s="6">
-        <v>1</v>
-      </c>
-      <c r="F21" s="6">
-        <v>0</v>
-      </c>
-      <c r="G21" s="6">
-        <v>0</v>
-      </c>
-      <c r="H21" s="6">
-        <v>1</v>
-      </c>
-      <c r="I21" s="24">
+      <c r="B27" s="6"/>
+      <c r="C27" s="6">
+        <v>0</v>
+      </c>
+      <c r="D27" s="6">
+        <v>0</v>
+      </c>
+      <c r="E27" s="6">
+        <v>1</v>
+      </c>
+      <c r="F27" s="6">
+        <v>0</v>
+      </c>
+      <c r="G27" s="6">
+        <v>0</v>
+      </c>
+      <c r="H27" s="6">
+        <v>1</v>
+      </c>
+      <c r="I27" s="24">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="J21" s="24" t="str">
+      <c r="J27" s="24" t="str">
         <f t="shared" si="1"/>
         <v>09h</v>
       </c>
-      <c r="L21" t="s">
+      <c r="L27" t="s">
         <v>56</v>
       </c>
-      <c r="M21" t="s">
+      <c r="M27" t="s">
         <v>111</v>
       </c>
-      <c r="N21" t="s">
+      <c r="N27" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6">
-        <v>0</v>
-      </c>
-      <c r="D22" s="6">
-        <v>0</v>
-      </c>
-      <c r="E22" s="6">
-        <v>1</v>
-      </c>
-      <c r="F22" s="6">
-        <v>0</v>
-      </c>
-      <c r="G22" s="6">
-        <v>1</v>
-      </c>
-      <c r="H22" s="6">
-        <v>0</v>
-      </c>
-      <c r="I22" s="24">
+      <c r="B28" s="6"/>
+      <c r="C28" s="6">
+        <v>0</v>
+      </c>
+      <c r="D28" s="6">
+        <v>0</v>
+      </c>
+      <c r="E28" s="6">
+        <v>1</v>
+      </c>
+      <c r="F28" s="6">
+        <v>0</v>
+      </c>
+      <c r="G28" s="6">
+        <v>1</v>
+      </c>
+      <c r="H28" s="6">
+        <v>0</v>
+      </c>
+      <c r="I28" s="24">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="J22" s="24" t="str">
+      <c r="J28" s="24" t="str">
         <f t="shared" si="1"/>
         <v>0Ah</v>
       </c>
-      <c r="L22" t="s">
+      <c r="L28" t="s">
         <v>57</v>
       </c>
-      <c r="M22" t="s">
+      <c r="M28" t="s">
         <v>112</v>
       </c>
-      <c r="N22" t="s">
+      <c r="N28" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6">
-        <v>0</v>
-      </c>
-      <c r="D23" s="6">
-        <v>0</v>
-      </c>
-      <c r="E23" s="6">
-        <v>1</v>
-      </c>
-      <c r="F23" s="6">
-        <v>0</v>
-      </c>
-      <c r="G23" s="6">
-        <v>1</v>
-      </c>
-      <c r="H23" s="6">
-        <v>1</v>
-      </c>
-      <c r="I23" s="24">
+      <c r="B29" s="6"/>
+      <c r="C29" s="6">
+        <v>0</v>
+      </c>
+      <c r="D29" s="6">
+        <v>0</v>
+      </c>
+      <c r="E29" s="6">
+        <v>1</v>
+      </c>
+      <c r="F29" s="6">
+        <v>0</v>
+      </c>
+      <c r="G29" s="6">
+        <v>1</v>
+      </c>
+      <c r="H29" s="6">
+        <v>1</v>
+      </c>
+      <c r="I29" s="24">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="J23" s="24" t="str">
+      <c r="J29" s="24" t="str">
         <f t="shared" si="1"/>
         <v>0Bh</v>
       </c>
-      <c r="L23" t="s">
+      <c r="L29" t="s">
         <v>58</v>
       </c>
-      <c r="M23" t="s">
+      <c r="M29" t="s">
         <v>113</v>
       </c>
-      <c r="N23" t="s">
+      <c r="N29" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6">
-        <v>0</v>
-      </c>
-      <c r="D24" s="6">
-        <v>0</v>
-      </c>
-      <c r="E24" s="6">
-        <v>1</v>
-      </c>
-      <c r="F24" s="6">
-        <v>1</v>
-      </c>
-      <c r="G24" s="6">
-        <v>0</v>
-      </c>
-      <c r="H24" s="6">
-        <v>0</v>
-      </c>
-      <c r="I24" s="24">
+      <c r="B30" s="6"/>
+      <c r="C30" s="6">
+        <v>0</v>
+      </c>
+      <c r="D30" s="6">
+        <v>0</v>
+      </c>
+      <c r="E30" s="6">
+        <v>1</v>
+      </c>
+      <c r="F30" s="6">
+        <v>1</v>
+      </c>
+      <c r="G30" s="6">
+        <v>0</v>
+      </c>
+      <c r="H30" s="6">
+        <v>0</v>
+      </c>
+      <c r="I30" s="24">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="J24" s="24" t="str">
+      <c r="J30" s="24" t="str">
         <f t="shared" si="1"/>
         <v>0Ch</v>
       </c>
-      <c r="L24" t="s">
+      <c r="L30" t="s">
         <v>59</v>
       </c>
-      <c r="M24" t="s">
+      <c r="M30" t="s">
         <v>114</v>
       </c>
-      <c r="N24" t="s">
+      <c r="N30" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6">
-        <v>0</v>
-      </c>
-      <c r="D25" s="6">
-        <v>1</v>
-      </c>
-      <c r="E25" s="6">
-        <v>0</v>
-      </c>
-      <c r="F25" s="6">
-        <v>0</v>
-      </c>
-      <c r="G25" s="6">
-        <v>0</v>
-      </c>
-      <c r="H25" s="6">
-        <v>0</v>
-      </c>
-      <c r="I25" s="24">
+      <c r="B31" s="6"/>
+      <c r="C31" s="6">
+        <v>0</v>
+      </c>
+      <c r="D31" s="6">
+        <v>1</v>
+      </c>
+      <c r="E31" s="6">
+        <v>0</v>
+      </c>
+      <c r="F31" s="6">
+        <v>0</v>
+      </c>
+      <c r="G31" s="6">
+        <v>0</v>
+      </c>
+      <c r="H31" s="6">
+        <v>0</v>
+      </c>
+      <c r="I31" s="24">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="J25" s="24" t="str">
+      <c r="J31" s="24" t="str">
         <f t="shared" si="1"/>
         <v>10h</v>
       </c>
-      <c r="L25" t="s">
+      <c r="L31" t="s">
         <v>60</v>
       </c>
-      <c r="M25" t="s">
+      <c r="M31" t="s">
         <v>125</v>
       </c>
-      <c r="N25" t="s">
+      <c r="N31" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6">
-        <v>0</v>
-      </c>
-      <c r="D26" s="6">
-        <v>1</v>
-      </c>
-      <c r="E26" s="6">
-        <v>0</v>
-      </c>
-      <c r="F26" s="6">
-        <v>0</v>
-      </c>
-      <c r="G26" s="6">
-        <v>0</v>
-      </c>
-      <c r="H26" s="6">
-        <v>1</v>
-      </c>
-      <c r="I26" s="24">
+      <c r="B32" s="6"/>
+      <c r="C32" s="6">
+        <v>0</v>
+      </c>
+      <c r="D32" s="6">
+        <v>1</v>
+      </c>
+      <c r="E32" s="6">
+        <v>0</v>
+      </c>
+      <c r="F32" s="6">
+        <v>0</v>
+      </c>
+      <c r="G32" s="6">
+        <v>0</v>
+      </c>
+      <c r="H32" s="6">
+        <v>1</v>
+      </c>
+      <c r="I32" s="24">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="J26" s="24" t="str">
+      <c r="J32" s="24" t="str">
         <f t="shared" si="1"/>
         <v>11h</v>
       </c>
-      <c r="L26" t="s">
+      <c r="L32" t="s">
         <v>61</v>
       </c>
-      <c r="M26" t="s">
+      <c r="M32" t="s">
         <v>126</v>
       </c>
-      <c r="N26" t="s">
+      <c r="N32" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6">
-        <v>0</v>
-      </c>
-      <c r="D27" s="6">
-        <v>1</v>
-      </c>
-      <c r="E27" s="6">
-        <v>0</v>
-      </c>
-      <c r="F27" s="6">
-        <v>0</v>
-      </c>
-      <c r="G27" s="6">
-        <v>1</v>
-      </c>
-      <c r="H27" s="6">
-        <v>0</v>
-      </c>
-      <c r="I27" s="24">
+      <c r="B33" s="6"/>
+      <c r="C33" s="6">
+        <v>0</v>
+      </c>
+      <c r="D33" s="6">
+        <v>1</v>
+      </c>
+      <c r="E33" s="6">
+        <v>0</v>
+      </c>
+      <c r="F33" s="6">
+        <v>0</v>
+      </c>
+      <c r="G33" s="6">
+        <v>1</v>
+      </c>
+      <c r="H33" s="6">
+        <v>0</v>
+      </c>
+      <c r="I33" s="24">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="J27" s="24" t="str">
+      <c r="J33" s="24" t="str">
         <f t="shared" si="1"/>
         <v>12h</v>
       </c>
-      <c r="L27" t="s">
+      <c r="L33" t="s">
         <v>62</v>
       </c>
-      <c r="M27" t="s">
+      <c r="M33" t="s">
         <v>115</v>
       </c>
-      <c r="N27" t="s">
+      <c r="N33" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6">
-        <v>0</v>
-      </c>
-      <c r="D28" s="6">
-        <v>1</v>
-      </c>
-      <c r="E28" s="6">
-        <v>0</v>
-      </c>
-      <c r="F28" s="6">
-        <v>0</v>
-      </c>
-      <c r="G28" s="6">
-        <v>1</v>
-      </c>
-      <c r="H28" s="6">
-        <v>1</v>
-      </c>
-      <c r="I28" s="24">
+      <c r="B34" s="6"/>
+      <c r="C34" s="6">
+        <v>0</v>
+      </c>
+      <c r="D34" s="6">
+        <v>1</v>
+      </c>
+      <c r="E34" s="6">
+        <v>0</v>
+      </c>
+      <c r="F34" s="6">
+        <v>0</v>
+      </c>
+      <c r="G34" s="6">
+        <v>1</v>
+      </c>
+      <c r="H34" s="6">
+        <v>1</v>
+      </c>
+      <c r="I34" s="24">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="J28" s="24" t="str">
+      <c r="J34" s="24" t="str">
         <f t="shared" si="1"/>
         <v>13h</v>
       </c>
-      <c r="L28" t="s">
+      <c r="L34" t="s">
         <v>63</v>
       </c>
-      <c r="M28" t="s">
+      <c r="M34" t="s">
         <v>116</v>
       </c>
-      <c r="N28" t="s">
+      <c r="N34" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6">
-        <v>0</v>
-      </c>
-      <c r="D29" s="6">
-        <v>1</v>
-      </c>
-      <c r="E29" s="6">
-        <v>0</v>
-      </c>
-      <c r="F29" s="6">
-        <v>1</v>
-      </c>
-      <c r="G29" s="6">
-        <v>0</v>
-      </c>
-      <c r="H29" s="6">
-        <v>0</v>
-      </c>
-      <c r="I29" s="24">
+      <c r="B35" s="6"/>
+      <c r="C35" s="6">
+        <v>0</v>
+      </c>
+      <c r="D35" s="6">
+        <v>1</v>
+      </c>
+      <c r="E35" s="6">
+        <v>0</v>
+      </c>
+      <c r="F35" s="6">
+        <v>1</v>
+      </c>
+      <c r="G35" s="6">
+        <v>0</v>
+      </c>
+      <c r="H35" s="6">
+        <v>0</v>
+      </c>
+      <c r="I35" s="24">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="J29" s="24" t="str">
+      <c r="J35" s="24" t="str">
         <f t="shared" si="1"/>
         <v>14h</v>
       </c>
-      <c r="L29" t="s">
+      <c r="L35" t="s">
         <v>64</v>
       </c>
-      <c r="M29" t="s">
+      <c r="M35" t="s">
         <v>117</v>
       </c>
-      <c r="N29" t="s">
+      <c r="N35" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6">
-        <v>0</v>
-      </c>
-      <c r="D30" s="6">
-        <v>1</v>
-      </c>
-      <c r="E30" s="6">
-        <v>0</v>
-      </c>
-      <c r="F30" s="6">
-        <v>1</v>
-      </c>
-      <c r="G30" s="6">
-        <v>0</v>
-      </c>
-      <c r="H30" s="6">
-        <v>1</v>
-      </c>
-      <c r="I30" s="24">
+      <c r="B36" s="6"/>
+      <c r="C36" s="6">
+        <v>0</v>
+      </c>
+      <c r="D36" s="6">
+        <v>1</v>
+      </c>
+      <c r="E36" s="6">
+        <v>0</v>
+      </c>
+      <c r="F36" s="6">
+        <v>1</v>
+      </c>
+      <c r="G36" s="6">
+        <v>0</v>
+      </c>
+      <c r="H36" s="6">
+        <v>1</v>
+      </c>
+      <c r="I36" s="24">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="J30" s="24" t="str">
+      <c r="J36" s="24" t="str">
         <f t="shared" si="1"/>
         <v>15h</v>
       </c>
-      <c r="L30" t="s">
+      <c r="L36" t="s">
         <v>65</v>
       </c>
-      <c r="M30" t="s">
+      <c r="M36" t="s">
         <v>118</v>
       </c>
-      <c r="N30" t="s">
+      <c r="N36" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6">
-        <v>0</v>
-      </c>
-      <c r="D31" s="6">
-        <v>1</v>
-      </c>
-      <c r="E31" s="6">
-        <v>0</v>
-      </c>
-      <c r="F31" s="6">
-        <v>1</v>
-      </c>
-      <c r="G31" s="6">
-        <v>1</v>
-      </c>
-      <c r="H31" s="6">
-        <v>0</v>
-      </c>
-      <c r="I31" s="24">
+      <c r="B37" s="6"/>
+      <c r="C37" s="6">
+        <v>0</v>
+      </c>
+      <c r="D37" s="6">
+        <v>1</v>
+      </c>
+      <c r="E37" s="6">
+        <v>0</v>
+      </c>
+      <c r="F37" s="6">
+        <v>1</v>
+      </c>
+      <c r="G37" s="6">
+        <v>1</v>
+      </c>
+      <c r="H37" s="6">
+        <v>0</v>
+      </c>
+      <c r="I37" s="24">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="J31" s="24" t="str">
+      <c r="J37" s="24" t="str">
         <f t="shared" si="1"/>
         <v>16h</v>
       </c>
-      <c r="L31" t="s">
+      <c r="L37" t="s">
         <v>66</v>
       </c>
-      <c r="M31" t="s">
+      <c r="M37" t="s">
         <v>119</v>
       </c>
-      <c r="N31" t="s">
+      <c r="N37" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6">
-        <v>0</v>
-      </c>
-      <c r="D32" s="6">
-        <v>1</v>
-      </c>
-      <c r="E32" s="6">
-        <v>0</v>
-      </c>
-      <c r="F32" s="6">
-        <v>1</v>
-      </c>
-      <c r="G32" s="6">
-        <v>1</v>
-      </c>
-      <c r="H32" s="6">
-        <v>1</v>
-      </c>
-      <c r="I32" s="24">
+      <c r="B38" s="6"/>
+      <c r="C38" s="6">
+        <v>0</v>
+      </c>
+      <c r="D38" s="6">
+        <v>1</v>
+      </c>
+      <c r="E38" s="6">
+        <v>0</v>
+      </c>
+      <c r="F38" s="6">
+        <v>1</v>
+      </c>
+      <c r="G38" s="6">
+        <v>1</v>
+      </c>
+      <c r="H38" s="6">
+        <v>1</v>
+      </c>
+      <c r="I38" s="24">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="J32" s="24" t="str">
+      <c r="J38" s="24" t="str">
         <f t="shared" si="1"/>
         <v>17h</v>
       </c>
-      <c r="L32" t="s">
+      <c r="L38" t="s">
         <v>67</v>
       </c>
-      <c r="M32" t="s">
+      <c r="M38" t="s">
         <v>120</v>
       </c>
-      <c r="N32" t="s">
+      <c r="N38" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6">
-        <v>0</v>
-      </c>
-      <c r="D33" s="6">
-        <v>1</v>
-      </c>
-      <c r="E33" s="6">
-        <v>1</v>
-      </c>
-      <c r="F33" s="6">
-        <v>0</v>
-      </c>
-      <c r="G33" s="6">
-        <v>0</v>
-      </c>
-      <c r="H33" s="6">
-        <v>0</v>
-      </c>
-      <c r="I33" s="24">
+      <c r="B39" s="6"/>
+      <c r="C39" s="6">
+        <v>0</v>
+      </c>
+      <c r="D39" s="6">
+        <v>1</v>
+      </c>
+      <c r="E39" s="6">
+        <v>1</v>
+      </c>
+      <c r="F39" s="6">
+        <v>0</v>
+      </c>
+      <c r="G39" s="6">
+        <v>0</v>
+      </c>
+      <c r="H39" s="6">
+        <v>0</v>
+      </c>
+      <c r="I39" s="24">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="J33" s="24" t="str">
+      <c r="J39" s="24" t="str">
         <f t="shared" si="1"/>
         <v>18h</v>
       </c>
-      <c r="L33" t="s">
+      <c r="L39" t="s">
         <v>200</v>
       </c>
-      <c r="M33" t="s">
+      <c r="M39" t="s">
         <v>201</v>
       </c>
-      <c r="N33" t="s">
+      <c r="N39" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6">
-        <v>0</v>
-      </c>
-      <c r="D34" s="6">
-        <v>1</v>
-      </c>
-      <c r="E34" s="6">
-        <v>1</v>
-      </c>
-      <c r="F34" s="6">
-        <v>0</v>
-      </c>
-      <c r="G34" s="6">
-        <v>0</v>
-      </c>
-      <c r="H34" s="6">
-        <v>1</v>
-      </c>
-      <c r="I34" s="24">
+      <c r="B40" s="6"/>
+      <c r="C40" s="6">
+        <v>0</v>
+      </c>
+      <c r="D40" s="6">
+        <v>1</v>
+      </c>
+      <c r="E40" s="6">
+        <v>1</v>
+      </c>
+      <c r="F40" s="6">
+        <v>0</v>
+      </c>
+      <c r="G40" s="6">
+        <v>0</v>
+      </c>
+      <c r="H40" s="6">
+        <v>1</v>
+      </c>
+      <c r="I40" s="24">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="J34" s="24" t="str">
+      <c r="J40" s="24" t="str">
         <f t="shared" si="1"/>
         <v>19h</v>
       </c>
-      <c r="L34" t="s">
+      <c r="L40" t="s">
         <v>68</v>
       </c>
-      <c r="M34" t="s">
+      <c r="M40" t="s">
         <v>166</v>
       </c>
-      <c r="N34" t="s">
+      <c r="N40" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6">
-        <v>0</v>
-      </c>
-      <c r="D35" s="6">
-        <v>1</v>
-      </c>
-      <c r="E35" s="6">
-        <v>1</v>
-      </c>
-      <c r="F35" s="6">
-        <v>0</v>
-      </c>
-      <c r="G35" s="6">
-        <v>1</v>
-      </c>
-      <c r="H35" s="6">
-        <v>0</v>
-      </c>
-      <c r="I35" s="24">
+      <c r="B41" s="6"/>
+      <c r="C41" s="6">
+        <v>0</v>
+      </c>
+      <c r="D41" s="6">
+        <v>1</v>
+      </c>
+      <c r="E41" s="6">
+        <v>1</v>
+      </c>
+      <c r="F41" s="6">
+        <v>0</v>
+      </c>
+      <c r="G41" s="6">
+        <v>1</v>
+      </c>
+      <c r="H41" s="6">
+        <v>0</v>
+      </c>
+      <c r="I41" s="24">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="J35" s="24" t="str">
+      <c r="J41" s="24" t="str">
         <f t="shared" si="1"/>
         <v>1Ah</v>
       </c>
-      <c r="L35" t="s">
+      <c r="L41" t="s">
         <v>69</v>
       </c>
-      <c r="M35" t="s">
+      <c r="M41" t="s">
         <v>121</v>
       </c>
-      <c r="N35" t="s">
+      <c r="N41" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6">
-        <v>0</v>
-      </c>
-      <c r="D36" s="6">
-        <v>1</v>
-      </c>
-      <c r="E36" s="6">
-        <v>1</v>
-      </c>
-      <c r="F36" s="6">
-        <v>0</v>
-      </c>
-      <c r="G36" s="6">
-        <v>1</v>
-      </c>
-      <c r="H36" s="6">
-        <v>1</v>
-      </c>
-      <c r="I36" s="24">
+      <c r="B42" s="6"/>
+      <c r="C42" s="6">
+        <v>0</v>
+      </c>
+      <c r="D42" s="6">
+        <v>1</v>
+      </c>
+      <c r="E42" s="6">
+        <v>1</v>
+      </c>
+      <c r="F42" s="6">
+        <v>0</v>
+      </c>
+      <c r="G42" s="6">
+        <v>1</v>
+      </c>
+      <c r="H42" s="6">
+        <v>1</v>
+      </c>
+      <c r="I42" s="24">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="J36" s="24" t="str">
+      <c r="J42" s="24" t="str">
         <f t="shared" si="1"/>
         <v>1Bh</v>
       </c>
-      <c r="L36" t="s">
+      <c r="L42" t="s">
         <v>70</v>
       </c>
-      <c r="M36" t="s">
+      <c r="M42" t="s">
         <v>122</v>
       </c>
-      <c r="N36" t="s">
+      <c r="N42" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6">
-        <v>0</v>
-      </c>
-      <c r="D37" s="6">
-        <v>1</v>
-      </c>
-      <c r="E37" s="6">
-        <v>1</v>
-      </c>
-      <c r="F37" s="6">
-        <v>1</v>
-      </c>
-      <c r="G37" s="6">
-        <v>0</v>
-      </c>
-      <c r="H37" s="6">
-        <v>0</v>
-      </c>
-      <c r="I37" s="24">
+      <c r="B43" s="6"/>
+      <c r="C43" s="6">
+        <v>0</v>
+      </c>
+      <c r="D43" s="6">
+        <v>1</v>
+      </c>
+      <c r="E43" s="6">
+        <v>1</v>
+      </c>
+      <c r="F43" s="6">
+        <v>1</v>
+      </c>
+      <c r="G43" s="6">
+        <v>0</v>
+      </c>
+      <c r="H43" s="6">
+        <v>0</v>
+      </c>
+      <c r="I43" s="24">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="J37" s="24" t="str">
+      <c r="J43" s="24" t="str">
         <f t="shared" si="1"/>
         <v>1Ch</v>
       </c>
-      <c r="L37" t="s">
+      <c r="L43" t="s">
         <v>71</v>
       </c>
-      <c r="M37" t="s">
+      <c r="M43" t="s">
         <v>123</v>
       </c>
-      <c r="N37" t="s">
+      <c r="N43" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6">
-        <v>0</v>
-      </c>
-      <c r="D38" s="6">
-        <v>1</v>
-      </c>
-      <c r="E38" s="6">
-        <v>1</v>
-      </c>
-      <c r="F38" s="6">
-        <v>1</v>
-      </c>
-      <c r="G38" s="6">
-        <v>0</v>
-      </c>
-      <c r="H38" s="6">
-        <v>1</v>
-      </c>
-      <c r="I38" s="24">
+      <c r="B44" s="6"/>
+      <c r="C44" s="6">
+        <v>0</v>
+      </c>
+      <c r="D44" s="6">
+        <v>1</v>
+      </c>
+      <c r="E44" s="6">
+        <v>1</v>
+      </c>
+      <c r="F44" s="6">
+        <v>1</v>
+      </c>
+      <c r="G44" s="6">
+        <v>0</v>
+      </c>
+      <c r="H44" s="6">
+        <v>1</v>
+      </c>
+      <c r="I44" s="24">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="J38" s="24" t="str">
+      <c r="J44" s="24" t="str">
         <f t="shared" si="1"/>
         <v>1Dh</v>
       </c>
-      <c r="L38" t="s">
+      <c r="L44" t="s">
         <v>72</v>
       </c>
-      <c r="M38" t="s">
+      <c r="M44" t="s">
         <v>128</v>
       </c>
-      <c r="N38" t="s">
+      <c r="N44" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6">
-        <v>0</v>
-      </c>
-      <c r="D39" s="6">
-        <v>1</v>
-      </c>
-      <c r="E39" s="6">
-        <v>1</v>
-      </c>
-      <c r="F39" s="6">
-        <v>1</v>
-      </c>
-      <c r="G39" s="6">
-        <v>1</v>
-      </c>
-      <c r="H39" s="6">
-        <v>0</v>
-      </c>
-      <c r="I39" s="24">
+      <c r="B45" s="6"/>
+      <c r="C45" s="6">
+        <v>0</v>
+      </c>
+      <c r="D45" s="6">
+        <v>1</v>
+      </c>
+      <c r="E45" s="6">
+        <v>1</v>
+      </c>
+      <c r="F45" s="6">
+        <v>1</v>
+      </c>
+      <c r="G45" s="6">
+        <v>1</v>
+      </c>
+      <c r="H45" s="6">
+        <v>0</v>
+      </c>
+      <c r="I45" s="24">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="J39" s="24" t="str">
+      <c r="J45" s="24" t="str">
         <f t="shared" si="1"/>
         <v>1Eh</v>
       </c>
-      <c r="L39" t="s">
+      <c r="L45" t="s">
         <v>73</v>
       </c>
-      <c r="M39" t="s">
+      <c r="M45" t="s">
         <v>124</v>
       </c>
-      <c r="N39" t="s">
+      <c r="N45" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6">
-        <v>0</v>
-      </c>
-      <c r="D40" s="6">
-        <v>1</v>
-      </c>
-      <c r="E40" s="6">
-        <v>1</v>
-      </c>
-      <c r="F40" s="6">
-        <v>1</v>
-      </c>
-      <c r="G40" s="6">
-        <v>1</v>
-      </c>
-      <c r="H40" s="6">
-        <v>1</v>
-      </c>
-      <c r="I40" s="24">
+      <c r="B46" s="6"/>
+      <c r="C46" s="6">
+        <v>0</v>
+      </c>
+      <c r="D46" s="6">
+        <v>1</v>
+      </c>
+      <c r="E46" s="6">
+        <v>1</v>
+      </c>
+      <c r="F46" s="6">
+        <v>1</v>
+      </c>
+      <c r="G46" s="6">
+        <v>1</v>
+      </c>
+      <c r="H46" s="6">
+        <v>1</v>
+      </c>
+      <c r="I46" s="24">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="J40" s="24" t="str">
+      <c r="J46" s="24" t="str">
         <f t="shared" si="1"/>
         <v>1Fh</v>
       </c>
-      <c r="L40" t="s">
+      <c r="L46" t="s">
         <v>74</v>
       </c>
-      <c r="M40" t="s">
+      <c r="M46" t="s">
         <v>127</v>
       </c>
-      <c r="N40" t="s">
+      <c r="N46" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="16" t="s">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14">
-        <v>0</v>
-      </c>
-      <c r="D41" s="14">
-        <v>0</v>
-      </c>
-      <c r="E41" s="14">
-        <v>0</v>
-      </c>
-      <c r="F41" s="14">
-        <v>0</v>
-      </c>
-      <c r="G41" s="14">
-        <v>0</v>
-      </c>
-      <c r="H41" s="14">
-        <v>0</v>
-      </c>
-      <c r="I41" s="24">
+      <c r="B47" s="14"/>
+      <c r="C47" s="14">
+        <v>0</v>
+      </c>
+      <c r="D47" s="14">
+        <v>0</v>
+      </c>
+      <c r="E47" s="14">
+        <v>0</v>
+      </c>
+      <c r="F47" s="14">
+        <v>0</v>
+      </c>
+      <c r="G47" s="14">
+        <v>0</v>
+      </c>
+      <c r="H47" s="14">
+        <v>0</v>
+      </c>
+      <c r="I47" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J41" s="24" t="str">
+      <c r="J47" s="24" t="str">
         <f t="shared" si="1"/>
         <v>00h</v>
       </c>
-      <c r="K41" s="17"/>
-      <c r="L41" s="17" t="s">
+      <c r="K47" s="17"/>
+      <c r="L47" s="17" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="7"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="24"/>
-      <c r="J42" s="24"/>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" s="7"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="24"/>
+      <c r="J48" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5658,13 +5928,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="B1" s="31">
+      <c r="B1" s="33">
         <v>2</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="31" t="s">
         <v>261</v>
       </c>
       <c r="D1" s="1"/>
@@ -5675,7 +5945,7 @@
       <c r="A2" s="28" t="s">
         <v>213</v>
       </c>
-      <c r="B2" s="32"/>
+      <c r="B2" s="34"/>
       <c r="C2" s="28"/>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
@@ -5685,7 +5955,7 @@
       <c r="A3" s="27" t="s">
         <v>206</v>
       </c>
-      <c r="B3" s="33"/>
+      <c r="B3" s="35"/>
       <c r="C3" s="3" t="s">
         <v>97</v>
       </c>
@@ -5807,7 +6077,7 @@
       <c r="A11" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="B11" s="32"/>
+      <c r="B11" s="34"/>
       <c r="C11" s="28"/>
       <c r="D11" s="28"/>
       <c r="E11" s="28"/>
@@ -5817,7 +6087,7 @@
       <c r="A12" s="27" t="s">
         <v>206</v>
       </c>
-      <c r="B12" s="33"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="3" t="s">
         <v>97</v>
       </c>
@@ -5919,10 +6189,10 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="B19" s="31">
+      <c r="B19" s="33">
         <v>3</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -5936,7 +6206,7 @@
       <c r="A20" s="27" t="s">
         <v>206</v>
       </c>
-      <c r="B20" s="33"/>
+      <c r="B20" s="35"/>
       <c r="C20" s="3" t="s">
         <v>97</v>
       </c>
@@ -5962,10 +6232,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="B22" s="31">
+      <c r="B22" s="33">
         <v>4</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -5979,7 +6249,7 @@
       <c r="A23" s="27" t="s">
         <v>206</v>
       </c>
-      <c r="B23" s="33"/>
+      <c r="B23" s="35"/>
       <c r="C23" s="3" t="s">
         <v>97</v>
       </c>
@@ -6050,10 +6320,10 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="30" t="s">
+      <c r="A28" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="B28" s="31">
+      <c r="B28" s="33">
         <v>5</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -6067,7 +6337,7 @@
       <c r="A29" s="27" t="s">
         <v>206</v>
       </c>
-      <c r="B29" s="33"/>
+      <c r="B29" s="35"/>
       <c r="C29" s="3" t="s">
         <v>97</v>
       </c>
@@ -6102,10 +6372,10 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="30" t="s">
+      <c r="A34" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="B34" s="31">
+      <c r="B34" s="33">
         <v>6</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -6119,7 +6389,7 @@
       <c r="A35" s="27" t="s">
         <v>206</v>
       </c>
-      <c r="B35" s="33"/>
+      <c r="B35" s="35"/>
       <c r="C35" s="3" t="s">
         <v>97</v>
       </c>
@@ -6169,10 +6439,10 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="30" t="s">
+      <c r="A43" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="B43" s="31">
+      <c r="B43" s="33">
         <v>7</v>
       </c>
       <c r="C43" s="1" t="s">
@@ -6186,7 +6456,7 @@
       <c r="A44" s="27" t="s">
         <v>206</v>
       </c>
-      <c r="B44" s="33"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="3" t="s">
         <v>97</v>
       </c>
@@ -6201,10 +6471,10 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="30" t="s">
+      <c r="A46" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="B46" s="31">
+      <c r="B46" s="33">
         <v>8</v>
       </c>
       <c r="C46" s="1" t="s">
@@ -6218,7 +6488,7 @@
       <c r="A47" s="27" t="s">
         <v>206</v>
       </c>
-      <c r="B47" s="33"/>
+      <c r="B47" s="35"/>
       <c r="C47" s="3" t="s">
         <v>97</v>
       </c>
@@ -6233,10 +6503,10 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="30" t="s">
+      <c r="A49" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="B49" s="31">
+      <c r="B49" s="33">
         <v>9</v>
       </c>
       <c r="C49" s="1" t="s">
@@ -6250,7 +6520,7 @@
       <c r="A50" s="27" t="s">
         <v>206</v>
       </c>
-      <c r="B50" s="33"/>
+      <c r="B50" s="35"/>
       <c r="C50" s="3" t="s">
         <v>97</v>
       </c>
@@ -6265,10 +6535,10 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="30" t="s">
+      <c r="A52" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="B52" s="31">
+      <c r="B52" s="33">
         <v>10</v>
       </c>
       <c r="C52" s="1" t="s">
@@ -6282,7 +6552,7 @@
       <c r="A53" s="27" t="s">
         <v>206</v>
       </c>
-      <c r="B53" s="33"/>
+      <c r="B53" s="35"/>
       <c r="C53" s="3" t="s">
         <v>97</v>
       </c>
@@ -6297,10 +6567,10 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="30" t="s">
+      <c r="A55" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="B55" s="31">
+      <c r="B55" s="33">
         <v>11</v>
       </c>
       <c r="C55" s="1" t="s">
@@ -6314,7 +6584,7 @@
       <c r="A56" s="27" t="s">
         <v>206</v>
       </c>
-      <c r="B56" s="33"/>
+      <c r="B56" s="35"/>
       <c r="C56" s="3" t="s">
         <v>97</v>
       </c>
@@ -6329,10 +6599,10 @@
       </c>
     </row>
     <row r="58" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="30" t="s">
+      <c r="A58" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="B58" s="31">
+      <c r="B58" s="33">
         <v>12</v>
       </c>
       <c r="C58" s="1" t="s">
@@ -6346,7 +6616,7 @@
       <c r="A59" s="27" t="s">
         <v>206</v>
       </c>
-      <c r="B59" s="33"/>
+      <c r="B59" s="35"/>
       <c r="C59" s="3" t="s">
         <v>97</v>
       </c>
@@ -6382,20 +6652,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="49" t="s">
         <v>295</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6403,34 +6673,34 @@
         <v>0</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="33">
+      <c r="C3" s="35">
         <v>7</v>
       </c>
-      <c r="D3" s="33">
+      <c r="D3" s="35">
         <v>6</v>
       </c>
-      <c r="E3" s="33">
+      <c r="E3" s="35">
         <v>5</v>
       </c>
-      <c r="F3" s="33">
+      <c r="F3" s="35">
         <v>4</v>
       </c>
-      <c r="G3" s="33">
+      <c r="G3" s="35">
         <v>3</v>
       </c>
-      <c r="H3" s="33">
+      <c r="H3" s="35">
         <v>2</v>
       </c>
-      <c r="I3" s="33">
-        <v>1</v>
-      </c>
-      <c r="J3" s="33">
-        <v>0</v>
-      </c>
-      <c r="K3" s="33" t="s">
+      <c r="I3" s="35">
+        <v>1</v>
+      </c>
+      <c r="J3" s="35">
+        <v>0</v>
+      </c>
+      <c r="K3" s="35" t="s">
         <v>296</v>
       </c>
-      <c r="L3" s="33" t="s">
+      <c r="L3" s="35" t="s">
         <v>300</v>
       </c>
     </row>
@@ -6836,30 +7106,30 @@
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
-      <c r="O4" s="40"/>
-      <c r="P4" s="40"/>
-      <c r="Q4" s="40"/>
-      <c r="R4" s="40"/>
-      <c r="S4" s="40"/>
-      <c r="T4" s="40"/>
-      <c r="U4" s="40"/>
-      <c r="V4" s="40"/>
-      <c r="W4" s="40"/>
-      <c r="X4" s="40"/>
-      <c r="Y4" s="40"/>
-      <c r="Z4" s="40"/>
-      <c r="AA4" s="40"/>
-      <c r="AB4" s="40"/>
-      <c r="AC4" s="40"/>
-      <c r="AD4" s="40"/>
-      <c r="AE4" s="40"/>
-      <c r="AF4" s="40"/>
-      <c r="AG4" s="40"/>
-      <c r="AH4" s="40"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="42"/>
+      <c r="P4" s="42"/>
+      <c r="Q4" s="42"/>
+      <c r="R4" s="42"/>
+      <c r="S4" s="42"/>
+      <c r="T4" s="42"/>
+      <c r="U4" s="42"/>
+      <c r="V4" s="42"/>
+      <c r="W4" s="42"/>
+      <c r="X4" s="42"/>
+      <c r="Y4" s="42"/>
+      <c r="Z4" s="42"/>
+      <c r="AA4" s="42"/>
+      <c r="AB4" s="42"/>
+      <c r="AC4" s="42"/>
+      <c r="AD4" s="42"/>
+      <c r="AE4" s="42"/>
+      <c r="AF4" s="42"/>
+      <c r="AG4" s="42"/>
+      <c r="AH4" s="42"/>
       <c r="AJ4" s="10"/>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
@@ -6890,32 +7160,32 @@
       <c r="J5" s="6">
         <v>1</v>
       </c>
-      <c r="K5" s="38" t="s">
+      <c r="K5" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="L5" s="38"/>
-      <c r="M5" s="38"/>
-      <c r="N5" s="38"/>
-      <c r="O5" s="38"/>
-      <c r="P5" s="38"/>
-      <c r="Q5" s="38"/>
-      <c r="R5" s="38"/>
-      <c r="S5" s="38"/>
-      <c r="T5" s="38"/>
-      <c r="U5" s="38"/>
-      <c r="V5" s="38"/>
-      <c r="W5" s="38"/>
-      <c r="X5" s="38"/>
-      <c r="Y5" s="38"/>
-      <c r="Z5" s="38"/>
-      <c r="AA5" s="38"/>
-      <c r="AB5" s="38"/>
-      <c r="AC5" s="38"/>
-      <c r="AD5" s="38"/>
-      <c r="AE5" s="38"/>
-      <c r="AF5" s="38"/>
-      <c r="AG5" s="38"/>
-      <c r="AH5" s="38"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="40"/>
+      <c r="O5" s="40"/>
+      <c r="P5" s="40"/>
+      <c r="Q5" s="40"/>
+      <c r="R5" s="40"/>
+      <c r="S5" s="40"/>
+      <c r="T5" s="40"/>
+      <c r="U5" s="40"/>
+      <c r="V5" s="40"/>
+      <c r="W5" s="40"/>
+      <c r="X5" s="40"/>
+      <c r="Y5" s="40"/>
+      <c r="Z5" s="40"/>
+      <c r="AA5" s="40"/>
+      <c r="AB5" s="40"/>
+      <c r="AC5" s="40"/>
+      <c r="AD5" s="40"/>
+      <c r="AE5" s="40"/>
+      <c r="AF5" s="40"/>
+      <c r="AG5" s="40"/>
+      <c r="AH5" s="40"/>
       <c r="AJ5" s="10"/>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
@@ -6946,36 +7216,36 @@
       <c r="J6" s="6">
         <v>0</v>
       </c>
-      <c r="K6" s="38" t="s">
+      <c r="K6" s="40" t="s">
         <v>135</v>
       </c>
-      <c r="L6" s="38"/>
-      <c r="M6" s="38"/>
-      <c r="N6" s="38"/>
-      <c r="O6" s="38"/>
-      <c r="P6" s="38"/>
-      <c r="Q6" s="38"/>
-      <c r="R6" s="38"/>
-      <c r="S6" s="38" t="s">
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="40"/>
+      <c r="Q6" s="40"/>
+      <c r="R6" s="40"/>
+      <c r="S6" s="40" t="s">
         <v>134</v>
       </c>
-      <c r="T6" s="38"/>
-      <c r="U6" s="38"/>
-      <c r="V6" s="38"/>
-      <c r="W6" s="38"/>
-      <c r="X6" s="38"/>
-      <c r="Y6" s="38"/>
-      <c r="Z6" s="38"/>
-      <c r="AA6" s="38" t="s">
+      <c r="T6" s="40"/>
+      <c r="U6" s="40"/>
+      <c r="V6" s="40"/>
+      <c r="W6" s="40"/>
+      <c r="X6" s="40"/>
+      <c r="Y6" s="40"/>
+      <c r="Z6" s="40"/>
+      <c r="AA6" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="AB6" s="38"/>
-      <c r="AC6" s="38"/>
-      <c r="AD6" s="38"/>
-      <c r="AE6" s="38"/>
-      <c r="AF6" s="38"/>
-      <c r="AG6" s="38"/>
-      <c r="AH6" s="38"/>
+      <c r="AB6" s="40"/>
+      <c r="AC6" s="40"/>
+      <c r="AD6" s="40"/>
+      <c r="AE6" s="40"/>
+      <c r="AF6" s="40"/>
+      <c r="AG6" s="40"/>
+      <c r="AH6" s="40"/>
       <c r="AI6" s="6"/>
       <c r="AJ6" s="10"/>
     </row>
@@ -8221,22 +8491,22 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
-      <c r="O4" s="40"/>
-      <c r="P4" s="40"/>
-      <c r="Q4" s="40"/>
-      <c r="R4" s="40"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="42"/>
+      <c r="P4" s="42"/>
+      <c r="Q4" s="42"/>
+      <c r="R4" s="42"/>
       <c r="T4" s="10" t="s">
         <v>139</v>
       </c>
@@ -8379,16 +8649,16 @@
       <c r="J7" s="6">
         <v>1</v>
       </c>
-      <c r="K7" s="38" t="s">
+      <c r="K7" s="40" t="s">
         <v>140</v>
       </c>
-      <c r="L7" s="38"/>
-      <c r="M7" s="38"/>
-      <c r="N7" s="38"/>
-      <c r="O7" s="38"/>
-      <c r="P7" s="38"/>
-      <c r="Q7" s="38"/>
-      <c r="R7" s="38"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="40"/>
+      <c r="O7" s="40"/>
+      <c r="P7" s="40"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="40"/>
       <c r="T7" s="10"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -8419,16 +8689,16 @@
       <c r="J8" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="K8" s="38" t="s">
+      <c r="K8" s="40" t="s">
         <v>140</v>
       </c>
-      <c r="L8" s="38"/>
-      <c r="M8" s="38"/>
-      <c r="N8" s="38"/>
-      <c r="O8" s="38"/>
-      <c r="P8" s="38"/>
-      <c r="Q8" s="38"/>
-      <c r="R8" s="38"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="40"/>
+      <c r="N8" s="40"/>
+      <c r="O8" s="40"/>
+      <c r="P8" s="40"/>
+      <c r="Q8" s="40"/>
+      <c r="R8" s="40"/>
       <c r="T8" s="10"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -8459,16 +8729,16 @@
       <c r="J9" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="K9" s="38" t="s">
+      <c r="K9" s="40" t="s">
         <v>140</v>
       </c>
-      <c r="L9" s="38"/>
-      <c r="M9" s="38"/>
-      <c r="N9" s="38"/>
-      <c r="O9" s="38"/>
-      <c r="P9" s="38"/>
-      <c r="Q9" s="38"/>
-      <c r="R9" s="38"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="40"/>
+      <c r="O9" s="40"/>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="40"/>
       <c r="T9" s="10"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -8499,16 +8769,16 @@
       <c r="J10" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="K10" s="38" t="s">
+      <c r="K10" s="40" t="s">
         <v>140</v>
       </c>
-      <c r="L10" s="38"/>
-      <c r="M10" s="38"/>
-      <c r="N10" s="38"/>
-      <c r="O10" s="38"/>
-      <c r="P10" s="38"/>
-      <c r="Q10" s="38"/>
-      <c r="R10" s="38"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="40"/>
+      <c r="N10" s="40"/>
+      <c r="O10" s="40"/>
+      <c r="P10" s="40"/>
+      <c r="Q10" s="40"/>
+      <c r="R10" s="40"/>
       <c r="T10" s="10"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
new inst for reading from special registers
</commit_message>
<xml_diff>
--- a/doc/RiscyInstSet32Bit.xlsx
+++ b/doc/RiscyInstSet32Bit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25410" windowHeight="12690" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25410" windowHeight="12690"/>
   </bookViews>
   <sheets>
     <sheet name="Summary - Terra" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="349">
   <si>
     <t>Description</t>
   </si>
@@ -1068,6 +1068,15 @@
   </si>
   <si>
     <t>Unconditionally decrement program counter</t>
+  </si>
+  <si>
+    <t>Reg: 0-pc, 1-sp, 2-lr</t>
+  </si>
+  <si>
+    <t>Special Register MOV (SMOV)</t>
+  </si>
+  <si>
+    <t>SpReg</t>
   </si>
 </sst>
 </file>
@@ -1275,7 +1284,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="6" applyFont="1"/>
@@ -1422,6 +1431,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Explanatory Text" xfId="7" builtinId="53" customBuiltin="1"/>
@@ -1709,10 +1721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL49"/>
+  <dimension ref="A1:AL50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13:P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2127,7 +2139,7 @@
       </c>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
+      <c r="A10" s="56"/>
       <c r="B10" s="7" t="s">
         <v>304</v>
       </c>
@@ -2214,7 +2226,7 @@
       </c>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A11" s="40"/>
+      <c r="A11" s="56"/>
       <c r="B11" s="7" t="s">
         <v>89</v>
       </c>
@@ -2303,27 +2315,25 @@
       </c>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>2</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>129</v>
+      <c r="A12" s="56"/>
+      <c r="B12" s="34" t="s">
+        <v>347</v>
       </c>
       <c r="D12" s="42" t="s">
         <v>4</v>
       </c>
       <c r="E12" s="42"/>
       <c r="F12" s="42"/>
-      <c r="G12" s="6">
-        <v>0</v>
-      </c>
-      <c r="H12" s="12">
-        <v>0</v>
-      </c>
-      <c r="I12" s="12">
-        <v>0</v>
-      </c>
-      <c r="J12" s="12">
+      <c r="G12" s="31">
+        <v>0</v>
+      </c>
+      <c r="H12" s="31">
+        <v>0</v>
+      </c>
+      <c r="I12" s="31">
+        <v>0</v>
+      </c>
+      <c r="J12" s="31">
         <v>0</v>
       </c>
       <c r="K12" s="44" t="s">
@@ -2332,74 +2342,63 @@
       <c r="L12" s="44"/>
       <c r="M12" s="44"/>
       <c r="N12" s="44" t="s">
-        <v>10</v>
+        <v>348</v>
       </c>
       <c r="O12" s="44"/>
       <c r="P12" s="44"/>
-      <c r="Q12" s="44" t="s">
-        <v>88</v>
-      </c>
-      <c r="R12" s="44"/>
-      <c r="S12" s="44"/>
-      <c r="T12" s="6">
-        <v>0</v>
-      </c>
-      <c r="U12" s="6">
-        <v>0</v>
-      </c>
-      <c r="V12" s="6">
-        <v>0</v>
-      </c>
-      <c r="W12" s="6">
-        <v>0</v>
-      </c>
-      <c r="X12" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y12" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z12" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA12" s="6">
-        <v>0</v>
-      </c>
-      <c r="AB12" s="6">
-        <v>0</v>
-      </c>
-      <c r="AC12" s="6">
-        <v>1</v>
-      </c>
-      <c r="AD12" s="6">
-        <v>0</v>
-      </c>
-      <c r="AE12" s="6">
-        <v>0</v>
-      </c>
-      <c r="AF12" s="6">
-        <v>0</v>
-      </c>
-      <c r="AG12" s="42" t="s">
-        <v>171</v>
-      </c>
-      <c r="AH12" s="42"/>
-      <c r="AI12" s="22" t="s">
-        <v>86</v>
-      </c>
+      <c r="Q12" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="R12" s="48"/>
+      <c r="S12" s="48"/>
+      <c r="T12" s="33">
+        <v>0</v>
+      </c>
+      <c r="U12" s="29">
+        <v>0</v>
+      </c>
+      <c r="V12" s="29">
+        <v>0</v>
+      </c>
+      <c r="W12" s="29">
+        <v>0</v>
+      </c>
+      <c r="X12" s="29">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="29">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="29">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="29">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="29">
+        <v>1</v>
+      </c>
+      <c r="AC12" s="29">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE12" s="47"/>
+      <c r="AF12" s="47"/>
+      <c r="AG12" s="47"/>
+      <c r="AH12" s="47"/>
+      <c r="AI12" s="47"/>
       <c r="AK12" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="AL12" s="2" t="s">
-        <v>170</v>
+        <v>346</v>
       </c>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>87</v>
+        <v>129</v>
       </c>
       <c r="D13" s="42" t="s">
         <v>4</v>
@@ -2429,20 +2428,28 @@
       <c r="O13" s="44"/>
       <c r="P13" s="44"/>
       <c r="Q13" s="44" t="s">
-        <v>128</v>
+        <v>88</v>
       </c>
       <c r="R13" s="44"/>
       <c r="S13" s="44"/>
-      <c r="T13" s="44" t="s">
-        <v>173</v>
-      </c>
-      <c r="U13" s="44"/>
-      <c r="V13" s="44"/>
-      <c r="W13" s="44" t="s">
-        <v>174</v>
-      </c>
-      <c r="X13" s="44"/>
-      <c r="Y13" s="44"/>
+      <c r="T13" s="6">
+        <v>0</v>
+      </c>
+      <c r="U13" s="6">
+        <v>0</v>
+      </c>
+      <c r="V13" s="6">
+        <v>0</v>
+      </c>
+      <c r="W13" s="6">
+        <v>0</v>
+      </c>
+      <c r="X13" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="6">
+        <v>0</v>
+      </c>
       <c r="Z13" s="6">
         <v>0</v>
       </c>
@@ -2462,27 +2469,28 @@
         <v>0</v>
       </c>
       <c r="AF13" s="6">
-        <v>1</v>
-      </c>
-      <c r="AG13" s="6">
-        <v>0</v>
-      </c>
-      <c r="AH13" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI13" s="6">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="AG13" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="AH13" s="42"/>
+      <c r="AI13" s="22" t="s">
+        <v>86</v>
       </c>
       <c r="AK13" s="10" t="s">
-        <v>172</v>
+        <v>179</v>
+      </c>
+      <c r="AL13" s="2" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>147</v>
+        <v>87</v>
       </c>
       <c r="D14" s="42" t="s">
         <v>4</v>
@@ -2499,7 +2507,7 @@
         <v>0</v>
       </c>
       <c r="J14" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14" s="44" t="s">
         <v>6</v>
@@ -2511,33 +2519,21 @@
       </c>
       <c r="O14" s="44"/>
       <c r="P14" s="44"/>
-      <c r="Q14" s="6">
-        <v>0</v>
-      </c>
-      <c r="R14" s="6">
-        <v>0</v>
-      </c>
-      <c r="S14" s="6">
-        <v>0</v>
-      </c>
-      <c r="T14" s="6">
-        <v>0</v>
-      </c>
-      <c r="U14" s="6">
-        <v>0</v>
-      </c>
-      <c r="V14" s="6">
-        <v>0</v>
-      </c>
-      <c r="W14" s="6">
-        <v>0</v>
-      </c>
-      <c r="X14" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="6">
-        <v>0</v>
-      </c>
+      <c r="Q14" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="R14" s="44"/>
+      <c r="S14" s="44"/>
+      <c r="T14" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="U14" s="44"/>
+      <c r="V14" s="44"/>
+      <c r="W14" s="44" t="s">
+        <v>174</v>
+      </c>
+      <c r="X14" s="44"/>
+      <c r="Y14" s="44"/>
       <c r="Z14" s="6">
         <v>0</v>
       </c>
@@ -2548,7 +2544,7 @@
         <v>0</v>
       </c>
       <c r="AC14" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD14" s="6">
         <v>0</v>
@@ -2557,27 +2553,27 @@
         <v>0</v>
       </c>
       <c r="AF14" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG14" s="6">
         <v>0</v>
       </c>
-      <c r="AH14" s="22" t="s">
-        <v>175</v>
-      </c>
-      <c r="AI14" s="22" t="s">
-        <v>100</v>
+      <c r="AH14" s="6">
+        <v>0</v>
+      </c>
+      <c r="AI14" s="6">
+        <v>0</v>
       </c>
       <c r="AK14" s="10" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A15" s="40">
-        <v>2</v>
+      <c r="A15">
+        <v>4</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D15" s="42" t="s">
         <v>4</v>
@@ -2602,7 +2598,7 @@
       <c r="L15" s="44"/>
       <c r="M15" s="44"/>
       <c r="N15" s="44" t="s">
-        <v>88</v>
+        <v>10</v>
       </c>
       <c r="O15" s="44"/>
       <c r="P15" s="44"/>
@@ -2610,10 +2606,10 @@
         <v>0</v>
       </c>
       <c r="R15" s="6">
-        <v>1</v>
-      </c>
-      <c r="S15" s="22" t="s">
-        <v>9</v>
+        <v>0</v>
+      </c>
+      <c r="S15" s="6">
+        <v>0</v>
       </c>
       <c r="T15" s="6">
         <v>0</v>
@@ -2639,24 +2635,40 @@
       <c r="AA15" s="6">
         <v>0</v>
       </c>
-      <c r="AB15" s="44" t="s">
-        <v>155</v>
-      </c>
-      <c r="AC15" s="44"/>
-      <c r="AD15" s="44"/>
-      <c r="AE15" s="44"/>
-      <c r="AF15" s="44"/>
-      <c r="AG15" s="44"/>
-      <c r="AH15" s="44"/>
-      <c r="AI15" s="44"/>
+      <c r="AB15" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD15" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF15" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG15" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH15" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="AI15" s="22" t="s">
+        <v>100</v>
+      </c>
       <c r="AK15" s="10" t="s">
-        <v>148</v>
+        <v>176</v>
       </c>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A16" s="40"/>
+      <c r="A16" s="40">
+        <v>2</v>
+      </c>
       <c r="B16" s="7" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D16" s="42" t="s">
         <v>4</v>
@@ -2686,25 +2698,41 @@
       <c r="O16" s="44"/>
       <c r="P16" s="44"/>
       <c r="Q16" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R16" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S16" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="T16" s="44" t="s">
-        <v>153</v>
-      </c>
-      <c r="U16" s="44"/>
-      <c r="V16" s="44"/>
-      <c r="W16" s="44"/>
-      <c r="X16" s="44"/>
-      <c r="Y16" s="44"/>
-      <c r="Z16" s="44"/>
-      <c r="AA16" s="44"/>
-      <c r="AB16" s="44"/>
+      <c r="T16" s="6">
+        <v>0</v>
+      </c>
+      <c r="U16" s="6">
+        <v>0</v>
+      </c>
+      <c r="V16" s="6">
+        <v>0</v>
+      </c>
+      <c r="W16" s="6">
+        <v>0</v>
+      </c>
+      <c r="X16" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="44" t="s">
+        <v>155</v>
+      </c>
       <c r="AC16" s="44"/>
       <c r="AD16" s="44"/>
       <c r="AE16" s="44"/>
@@ -2719,7 +2747,7 @@
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" s="40"/>
       <c r="B17" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D17" s="42" t="s">
         <v>4</v>
@@ -2752,13 +2780,13 @@
         <v>1</v>
       </c>
       <c r="R17" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S17" s="22" t="s">
         <v>9</v>
       </c>
       <c r="T17" s="44" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="U17" s="44"/>
       <c r="V17" s="44"/>
@@ -2776,13 +2804,13 @@
       <c r="AH17" s="44"/>
       <c r="AI17" s="44"/>
       <c r="AK17" s="10" t="s">
-        <v>180</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" s="40"/>
       <c r="B18" s="7" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D18" s="42" t="s">
         <v>4</v>
@@ -2796,10 +2824,10 @@
         <v>0</v>
       </c>
       <c r="I18" s="12">
-        <v>1</v>
-      </c>
-      <c r="J18" s="12" t="s">
-        <v>86</v>
+        <v>0</v>
+      </c>
+      <c r="J18" s="12">
+        <v>1</v>
       </c>
       <c r="K18" s="44" t="s">
         <v>6</v>
@@ -2807,14 +2835,22 @@
       <c r="L18" s="44"/>
       <c r="M18" s="44"/>
       <c r="N18" s="44" t="s">
-        <v>5</v>
+        <v>88</v>
       </c>
       <c r="O18" s="44"/>
       <c r="P18" s="44"/>
-      <c r="Q18" s="44"/>
-      <c r="R18" s="44"/>
-      <c r="S18" s="44"/>
-      <c r="T18" s="44"/>
+      <c r="Q18" s="6">
+        <v>1</v>
+      </c>
+      <c r="R18" s="6">
+        <v>1</v>
+      </c>
+      <c r="S18" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="T18" s="44" t="s">
+        <v>154</v>
+      </c>
       <c r="U18" s="44"/>
       <c r="V18" s="44"/>
       <c r="W18" s="44"/>
@@ -2831,15 +2867,13 @@
       <c r="AH18" s="44"/>
       <c r="AI18" s="44"/>
       <c r="AK18" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>5</v>
-      </c>
+      <c r="A19" s="40"/>
       <c r="B19" s="7" t="s">
-        <v>8</v>
+        <v>156</v>
       </c>
       <c r="D19" s="42" t="s">
         <v>4</v>
@@ -2850,10 +2884,10 @@
         <v>0</v>
       </c>
       <c r="H19" s="12">
-        <v>1</v>
-      </c>
-      <c r="I19" s="12" t="s">
-        <v>9</v>
+        <v>0</v>
+      </c>
+      <c r="I19" s="12">
+        <v>1</v>
       </c>
       <c r="J19" s="12" t="s">
         <v>86</v>
@@ -2864,7 +2898,7 @@
       <c r="L19" s="44"/>
       <c r="M19" s="44"/>
       <c r="N19" s="44" t="s">
-        <v>177</v>
+        <v>5</v>
       </c>
       <c r="O19" s="44"/>
       <c r="P19" s="44"/>
@@ -2888,15 +2922,15 @@
       <c r="AH19" s="44"/>
       <c r="AI19" s="44"/>
       <c r="AK19" s="10" t="s">
-        <v>203</v>
+        <v>181</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>290</v>
+        <v>8</v>
       </c>
       <c r="D20" s="42" t="s">
         <v>4</v>
@@ -2904,24 +2938,24 @@
       <c r="E20" s="42"/>
       <c r="F20" s="42"/>
       <c r="G20" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20" s="12">
-        <v>0</v>
-      </c>
-      <c r="I20" s="12">
-        <v>0</v>
-      </c>
-      <c r="J20" s="12">
-        <v>0</v>
-      </c>
-      <c r="K20" s="45" t="s">
-        <v>158</v>
-      </c>
-      <c r="L20" s="45"/>
-      <c r="M20" s="45"/>
+        <v>1</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="K20" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="L20" s="44"/>
+      <c r="M20" s="44"/>
       <c r="N20" s="44" t="s">
-        <v>5</v>
+        <v>177</v>
       </c>
       <c r="O20" s="44"/>
       <c r="P20" s="44"/>
@@ -2945,58 +2979,50 @@
       <c r="AH20" s="44"/>
       <c r="AI20" s="44"/>
       <c r="AK20" s="10" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>251</v>
+        <v>290</v>
       </c>
       <c r="D21" s="42" t="s">
         <v>4</v>
       </c>
       <c r="E21" s="42"/>
       <c r="F21" s="42"/>
-      <c r="G21" s="24">
-        <v>1</v>
-      </c>
-      <c r="H21" s="25">
-        <v>0</v>
-      </c>
-      <c r="I21" s="25">
-        <v>0</v>
-      </c>
-      <c r="J21" s="25">
-        <v>1</v>
+      <c r="G21" s="6">
+        <v>1</v>
+      </c>
+      <c r="H21" s="12">
+        <v>0</v>
+      </c>
+      <c r="I21" s="12">
+        <v>0</v>
+      </c>
+      <c r="J21" s="12">
+        <v>0</v>
       </c>
       <c r="K21" s="45" t="s">
         <v>158</v>
       </c>
       <c r="L21" s="45"/>
       <c r="M21" s="45"/>
-      <c r="N21" s="25">
-        <v>0</v>
-      </c>
-      <c r="O21" s="25">
-        <v>0</v>
-      </c>
-      <c r="P21" s="25">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="43" t="s">
-        <v>253</v>
-      </c>
-      <c r="R21" s="43"/>
-      <c r="S21" s="43"/>
-      <c r="T21" s="43"/>
-      <c r="U21" s="43"/>
-      <c r="V21" s="43"/>
-      <c r="W21" s="44" t="s">
-        <v>252</v>
-      </c>
+      <c r="N21" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="O21" s="44"/>
+      <c r="P21" s="44"/>
+      <c r="Q21" s="44"/>
+      <c r="R21" s="44"/>
+      <c r="S21" s="44"/>
+      <c r="T21" s="44"/>
+      <c r="U21" s="44"/>
+      <c r="V21" s="44"/>
+      <c r="W21" s="44"/>
       <c r="X21" s="44"/>
       <c r="Y21" s="44"/>
       <c r="Z21" s="44"/>
@@ -3010,15 +3036,15 @@
       <c r="AH21" s="44"/>
       <c r="AI21" s="44"/>
       <c r="AK21" s="10" t="s">
-        <v>256</v>
+        <v>195</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="D22" s="42" t="s">
         <v>4</v>
@@ -3037,11 +3063,11 @@
       <c r="J22" s="25">
         <v>1</v>
       </c>
-      <c r="K22" s="43" t="s">
-        <v>6</v>
-      </c>
-      <c r="L22" s="43"/>
-      <c r="M22" s="43"/>
+      <c r="K22" s="45" t="s">
+        <v>158</v>
+      </c>
+      <c r="L22" s="45"/>
+      <c r="M22" s="45"/>
       <c r="N22" s="25">
         <v>0</v>
       </c>
@@ -3049,44 +3075,24 @@
         <v>0</v>
       </c>
       <c r="P22" s="25">
-        <v>1</v>
-      </c>
-      <c r="Q22" s="25">
-        <v>0</v>
-      </c>
-      <c r="R22" s="25">
-        <v>0</v>
-      </c>
-      <c r="S22" s="24">
-        <v>0</v>
-      </c>
-      <c r="T22" s="24">
-        <v>0</v>
-      </c>
-      <c r="U22" s="24">
-        <v>0</v>
-      </c>
-      <c r="V22" s="24">
-        <v>0</v>
-      </c>
-      <c r="W22" s="24">
-        <v>0</v>
-      </c>
-      <c r="X22" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y22" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z22" s="24">
-        <v>0</v>
-      </c>
-      <c r="AA22" s="24">
-        <v>0</v>
-      </c>
-      <c r="AB22" s="44" t="s">
-        <v>255</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="Q22" s="43" t="s">
+        <v>253</v>
+      </c>
+      <c r="R22" s="43"/>
+      <c r="S22" s="43"/>
+      <c r="T22" s="43"/>
+      <c r="U22" s="43"/>
+      <c r="V22" s="43"/>
+      <c r="W22" s="44" t="s">
+        <v>252</v>
+      </c>
+      <c r="X22" s="44"/>
+      <c r="Y22" s="44"/>
+      <c r="Z22" s="44"/>
+      <c r="AA22" s="44"/>
+      <c r="AB22" s="44"/>
       <c r="AC22" s="44"/>
       <c r="AD22" s="44"/>
       <c r="AE22" s="44"/>
@@ -3095,82 +3101,82 @@
       <c r="AH22" s="44"/>
       <c r="AI22" s="44"/>
       <c r="AK22" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>84</v>
+        <v>258</v>
       </c>
       <c r="D23" s="42" t="s">
         <v>4</v>
       </c>
       <c r="E23" s="42"/>
       <c r="F23" s="42"/>
-      <c r="G23" s="6">
-        <v>1</v>
-      </c>
-      <c r="H23" s="6">
-        <v>1</v>
-      </c>
-      <c r="I23" s="6">
-        <v>1</v>
-      </c>
-      <c r="J23" s="6">
-        <v>1</v>
-      </c>
-      <c r="K23" s="44" t="s">
+      <c r="G23" s="24">
+        <v>1</v>
+      </c>
+      <c r="H23" s="25">
+        <v>0</v>
+      </c>
+      <c r="I23" s="25">
+        <v>0</v>
+      </c>
+      <c r="J23" s="25">
+        <v>1</v>
+      </c>
+      <c r="K23" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="L23" s="44"/>
-      <c r="M23" s="44"/>
-      <c r="N23" s="6">
-        <v>0</v>
-      </c>
-      <c r="O23" s="6">
-        <v>0</v>
-      </c>
-      <c r="P23" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="6">
-        <v>0</v>
-      </c>
-      <c r="R23" s="6">
-        <v>0</v>
-      </c>
-      <c r="S23" s="6">
-        <v>0</v>
-      </c>
-      <c r="T23" s="6">
-        <v>0</v>
-      </c>
-      <c r="U23" s="6">
-        <v>0</v>
-      </c>
-      <c r="V23" s="6">
-        <v>0</v>
-      </c>
-      <c r="W23" s="6">
-        <v>0</v>
-      </c>
-      <c r="X23" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y23" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z23" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA23" s="6">
+      <c r="L23" s="43"/>
+      <c r="M23" s="43"/>
+      <c r="N23" s="25">
+        <v>0</v>
+      </c>
+      <c r="O23" s="25">
+        <v>0</v>
+      </c>
+      <c r="P23" s="25">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="25">
+        <v>0</v>
+      </c>
+      <c r="R23" s="25">
+        <v>0</v>
+      </c>
+      <c r="S23" s="24">
+        <v>0</v>
+      </c>
+      <c r="T23" s="24">
+        <v>0</v>
+      </c>
+      <c r="U23" s="24">
+        <v>0</v>
+      </c>
+      <c r="V23" s="24">
+        <v>0</v>
+      </c>
+      <c r="W23" s="24">
+        <v>0</v>
+      </c>
+      <c r="X23" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="24">
         <v>0</v>
       </c>
       <c r="AB23" s="44" t="s">
-        <v>83</v>
+        <v>255</v>
       </c>
       <c r="AC23" s="44"/>
       <c r="AD23" s="44"/>
@@ -3180,15 +3186,15 @@
       <c r="AH23" s="44"/>
       <c r="AI23" s="44"/>
       <c r="AK23" s="10" t="s">
-        <v>85</v>
+        <v>257</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D24" s="42" t="s">
         <v>4</v>
@@ -3252,7 +3258,7 @@
         <v>0</v>
       </c>
       <c r="AA24" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB24" s="44" t="s">
         <v>83</v>
@@ -3265,15 +3271,15 @@
       <c r="AH24" s="44"/>
       <c r="AI24" s="44"/>
       <c r="AK24" s="10" t="s">
-        <v>178</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D25" s="42" t="s">
         <v>4</v>
@@ -3339,38 +3345,26 @@
       <c r="AA25" s="6">
         <v>1</v>
       </c>
-      <c r="AB25" s="6">
-        <v>1</v>
-      </c>
-      <c r="AC25" s="6">
-        <v>1</v>
-      </c>
-      <c r="AD25" s="6">
-        <v>1</v>
-      </c>
-      <c r="AE25" s="6">
-        <v>1</v>
-      </c>
-      <c r="AF25" s="6">
-        <v>1</v>
-      </c>
-      <c r="AG25" s="6">
-        <v>1</v>
-      </c>
-      <c r="AH25" s="6">
-        <v>1</v>
-      </c>
-      <c r="AI25" s="6">
-        <v>1</v>
-      </c>
-      <c r="AK25" s="10"/>
+      <c r="AB25" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC25" s="44"/>
+      <c r="AD25" s="44"/>
+      <c r="AE25" s="44"/>
+      <c r="AF25" s="44"/>
+      <c r="AG25" s="44"/>
+      <c r="AH25" s="44"/>
+      <c r="AI25" s="44"/>
+      <c r="AK25" s="10" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="D26" s="42" t="s">
         <v>4</v>
@@ -3389,104 +3383,164 @@
       <c r="J26" s="6">
         <v>1</v>
       </c>
-      <c r="K26" s="6">
-        <v>1</v>
-      </c>
-      <c r="L26" s="6">
-        <v>1</v>
-      </c>
-      <c r="M26" s="6">
-        <v>1</v>
-      </c>
+      <c r="K26" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="L26" s="44"/>
+      <c r="M26" s="44"/>
       <c r="N26" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O26" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P26" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q26" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R26" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S26" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T26" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U26" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V26" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W26" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X26" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y26" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z26" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA26" s="6">
         <v>1</v>
       </c>
-      <c r="AB26" s="44" t="s">
+      <c r="AB26" s="6">
+        <v>1</v>
+      </c>
+      <c r="AC26" s="6">
+        <v>1</v>
+      </c>
+      <c r="AD26" s="6">
+        <v>1</v>
+      </c>
+      <c r="AE26" s="6">
+        <v>1</v>
+      </c>
+      <c r="AF26" s="6">
+        <v>1</v>
+      </c>
+      <c r="AG26" s="6">
+        <v>1</v>
+      </c>
+      <c r="AH26" s="6">
+        <v>1</v>
+      </c>
+      <c r="AI26" s="6">
+        <v>1</v>
+      </c>
+      <c r="AK26" s="10"/>
+    </row>
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>12</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="AC26" s="44"/>
-      <c r="AD26" s="44"/>
-      <c r="AE26" s="44"/>
-      <c r="AF26" s="44"/>
-      <c r="AG26" s="44"/>
-      <c r="AH26" s="44"/>
-      <c r="AI26" s="44"/>
-    </row>
-    <row r="33" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B33" s="7"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
-      <c r="M33" s="6"/>
-      <c r="N33" s="6"/>
-      <c r="O33" s="6"/>
-      <c r="P33" s="6"/>
-      <c r="Q33" s="6"/>
-      <c r="R33" s="6"/>
-      <c r="S33" s="6"/>
-      <c r="T33" s="6"/>
-      <c r="U33" s="6"/>
-      <c r="V33" s="6"/>
-      <c r="W33" s="6"/>
-      <c r="X33" s="6"/>
-      <c r="Y33" s="6"/>
-      <c r="Z33" s="6"/>
-      <c r="AA33" s="6"/>
-      <c r="AB33" s="6"/>
-      <c r="AC33" s="6"/>
-      <c r="AD33" s="6"/>
-      <c r="AE33" s="6"/>
-      <c r="AF33" s="6"/>
-      <c r="AG33" s="6"/>
-      <c r="AH33" s="6"/>
-      <c r="AI33" s="6"/>
-      <c r="AK33" s="10"/>
+      <c r="D27" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="6">
+        <v>1</v>
+      </c>
+      <c r="H27" s="6">
+        <v>1</v>
+      </c>
+      <c r="I27" s="6">
+        <v>1</v>
+      </c>
+      <c r="J27" s="6">
+        <v>1</v>
+      </c>
+      <c r="K27" s="6">
+        <v>1</v>
+      </c>
+      <c r="L27" s="6">
+        <v>1</v>
+      </c>
+      <c r="M27" s="6">
+        <v>1</v>
+      </c>
+      <c r="N27" s="6">
+        <v>1</v>
+      </c>
+      <c r="O27" s="6">
+        <v>1</v>
+      </c>
+      <c r="P27" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="6">
+        <v>1</v>
+      </c>
+      <c r="R27" s="6">
+        <v>1</v>
+      </c>
+      <c r="S27" s="6">
+        <v>1</v>
+      </c>
+      <c r="T27" s="6">
+        <v>1</v>
+      </c>
+      <c r="U27" s="6">
+        <v>1</v>
+      </c>
+      <c r="V27" s="6">
+        <v>1</v>
+      </c>
+      <c r="W27" s="6">
+        <v>1</v>
+      </c>
+      <c r="X27" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y27" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z27" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA27" s="6">
+        <v>1</v>
+      </c>
+      <c r="AB27" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC27" s="44"/>
+      <c r="AD27" s="44"/>
+      <c r="AE27" s="44"/>
+      <c r="AF27" s="44"/>
+      <c r="AG27" s="44"/>
+      <c r="AH27" s="44"/>
+      <c r="AI27" s="44"/>
     </row>
     <row r="34" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B34" s="7"/>
@@ -3601,6 +3655,7 @@
     </row>
     <row r="37" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B37" s="7"/>
+      <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
@@ -4029,78 +4084,119 @@
       <c r="AG48" s="6"/>
       <c r="AH48" s="6"/>
       <c r="AI48" s="6"/>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="AK48" s="10"/>
+    </row>
+    <row r="49" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="6"/>
+      <c r="J49" s="6"/>
+      <c r="K49" s="6"/>
+      <c r="L49" s="6"/>
+      <c r="M49" s="6"/>
+      <c r="N49" s="6"/>
+      <c r="O49" s="6"/>
+      <c r="P49" s="6"/>
+      <c r="Q49" s="6"/>
+      <c r="R49" s="6"/>
+      <c r="S49" s="6"/>
+      <c r="T49" s="6"/>
+      <c r="U49" s="6"/>
+      <c r="V49" s="6"/>
+      <c r="W49" s="6"/>
+      <c r="X49" s="6"/>
+      <c r="Y49" s="6"/>
+      <c r="Z49" s="6"/>
+      <c r="AA49" s="6"/>
+      <c r="AB49" s="6"/>
+      <c r="AC49" s="6"/>
+      <c r="AD49" s="6"/>
+      <c r="AE49" s="6"/>
+      <c r="AF49" s="6"/>
+      <c r="AG49" s="6"/>
+      <c r="AH49" s="6"/>
+      <c r="AI49" s="6"/>
+    </row>
+    <row r="50" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B50" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="66">
-    <mergeCell ref="N17:P17"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D23:F23"/>
+  <mergeCells count="71">
+    <mergeCell ref="AD12:AI12"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="N12:P12"/>
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="D20:F20"/>
     <mergeCell ref="D24:F24"/>
     <mergeCell ref="D25:F25"/>
     <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D21:F21"/>
     <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:F19"/>
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:F13"/>
     <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D13:F13"/>
     <mergeCell ref="D14:F14"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="AB26:AI26"/>
-    <mergeCell ref="N18:AI18"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="N12:P12"/>
-    <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="N20:AI20"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="AB27:AI27"/>
     <mergeCell ref="N19:AI19"/>
     <mergeCell ref="K19:M19"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="T17:AI17"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="K24:M24"/>
-    <mergeCell ref="AB24:AI24"/>
-    <mergeCell ref="K25:M25"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="AB23:AI23"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="N10:S10"/>
-    <mergeCell ref="N14:P14"/>
-    <mergeCell ref="K15:M15"/>
-    <mergeCell ref="AB15:AI15"/>
-    <mergeCell ref="K17:M17"/>
     <mergeCell ref="K13:M13"/>
     <mergeCell ref="N13:P13"/>
     <mergeCell ref="Q13:S13"/>
-    <mergeCell ref="T13:V13"/>
+    <mergeCell ref="N21:AI21"/>
+    <mergeCell ref="N20:AI20"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="T18:AI18"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="AB25:AI25"/>
+    <mergeCell ref="K26:M26"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="AB24:AI24"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="N10:S10"/>
+    <mergeCell ref="N15:P15"/>
     <mergeCell ref="K16:M16"/>
-    <mergeCell ref="T16:AI16"/>
+    <mergeCell ref="AB16:AI16"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="Q14:S14"/>
+    <mergeCell ref="T14:V14"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="T17:AI17"/>
     <mergeCell ref="K11:M11"/>
     <mergeCell ref="N11:P11"/>
     <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="Q21:V21"/>
-    <mergeCell ref="W21:AI21"/>
-    <mergeCell ref="AB22:AI22"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="Q22:V22"/>
+    <mergeCell ref="W22:AI22"/>
+    <mergeCell ref="AB23:AI23"/>
+    <mergeCell ref="K23:M23"/>
     <mergeCell ref="K22:M22"/>
-    <mergeCell ref="K21:M21"/>
     <mergeCell ref="AD9:AI9"/>
     <mergeCell ref="K9:M9"/>
     <mergeCell ref="N9:P9"/>
     <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="AG12:AH12"/>
-    <mergeCell ref="W13:Y13"/>
-    <mergeCell ref="N15:P15"/>
+    <mergeCell ref="AG13:AH13"/>
+    <mergeCell ref="W14:Y14"/>
     <mergeCell ref="N16:P16"/>
+    <mergeCell ref="N17:P17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6817,7 +6913,7 @@
   <dimension ref="A1:Q48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8781,7 +8877,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
labels in assembler, call stacks, etc. must contain OFFSET, not actual address
</commit_message>
<xml_diff>
--- a/doc/RiscyInstSet32Bit.xlsx
+++ b/doc/RiscyInstSet32Bit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25410" windowHeight="12690"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25410" windowHeight="12690" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Summary - Terra" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="412">
   <si>
     <t>Description</t>
   </si>
@@ -309,9 +309,6 @@
     <t>Print string</t>
   </si>
   <si>
-    <t>Database address</t>
-  </si>
-  <si>
     <t>Expression</t>
   </si>
   <si>
@@ -1264,6 +1261,12 @@
   </si>
   <si>
     <t>Jump to Subroutine, immediate</t>
+  </si>
+  <si>
+    <t>Tips: You can get extra speed if you directly memcpy the texts instead of calling BIOS</t>
+  </si>
+  <si>
+    <t>Database address (offset)</t>
   </si>
 </sst>
 </file>
@@ -2074,8 +2077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21:F21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23:AI23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2091,7 +2094,7 @@
   <sheetData>
     <row r="1" spans="1:38" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2131,16 +2134,16 @@
     <row r="2" spans="1:38" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -2179,11 +2182,11 @@
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B5" s="33" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -2226,7 +2229,7 @@
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="10" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -2260,12 +2263,12 @@
       <c r="AH6" s="5"/>
       <c r="AI6" s="5"/>
       <c r="AK6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
@@ -2303,12 +2306,12 @@
       <c r="AH7" s="5"/>
       <c r="AI7" s="5"/>
       <c r="AK7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>0</v>
@@ -2481,7 +2484,7 @@
         <v>0</v>
       </c>
       <c r="AD10" s="57" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AE10" s="57"/>
       <c r="AF10" s="57"/>
@@ -2489,13 +2492,13 @@
       <c r="AH10" s="57"/>
       <c r="AI10" s="57"/>
       <c r="AK10" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="56"/>
       <c r="B11" s="7" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D11" s="51" t="s">
         <v>3</v>
@@ -2520,7 +2523,7 @@
       <c r="L11" s="49"/>
       <c r="M11" s="49"/>
       <c r="N11" s="50" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O11" s="50"/>
       <c r="P11" s="50"/>
@@ -2576,7 +2579,7 @@
         <v>8</v>
       </c>
       <c r="AK11" s="10" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.25">
@@ -2607,12 +2610,12 @@
       <c r="L12" s="52"/>
       <c r="M12" s="52"/>
       <c r="N12" s="52" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O12" s="52"/>
       <c r="P12" s="52"/>
       <c r="Q12" s="53" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="R12" s="53"/>
       <c r="S12" s="53"/>
@@ -2665,13 +2668,13 @@
         <v>0</v>
       </c>
       <c r="AK12" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="56"/>
       <c r="B13" s="33" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D13" s="51" t="s">
         <v>3</v>
@@ -2696,12 +2699,12 @@
       <c r="L13" s="48"/>
       <c r="M13" s="48"/>
       <c r="N13" s="48" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="O13" s="48"/>
       <c r="P13" s="48"/>
       <c r="Q13" s="53" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="R13" s="53"/>
       <c r="S13" s="53"/>
@@ -2736,7 +2739,7 @@
         <v>0</v>
       </c>
       <c r="AD13" s="52" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AE13" s="52"/>
       <c r="AF13" s="52"/>
@@ -2744,7 +2747,7 @@
       <c r="AH13" s="52"/>
       <c r="AI13" s="52"/>
       <c r="AK13" s="10" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
@@ -2752,7 +2755,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D14" s="51" t="s">
         <v>3</v>
@@ -2826,17 +2829,17 @@
         <v>0</v>
       </c>
       <c r="AG14" s="51" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AH14" s="51"/>
       <c r="AI14" s="22" t="s">
         <v>84</v>
       </c>
       <c r="AK14" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AL14" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
@@ -2874,17 +2877,17 @@
       <c r="O15" s="48"/>
       <c r="P15" s="48"/>
       <c r="Q15" s="48" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="R15" s="48"/>
       <c r="S15" s="48"/>
       <c r="T15" s="48" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="U15" s="48"/>
       <c r="V15" s="48"/>
       <c r="W15" s="48" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="X15" s="48"/>
       <c r="Y15" s="48"/>
@@ -2919,7 +2922,7 @@
         <v>0</v>
       </c>
       <c r="AK15" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
@@ -2927,7 +2930,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D16" s="51" t="s">
         <v>3</v>
@@ -3008,13 +3011,13 @@
         <v>0</v>
       </c>
       <c r="AH16" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="AI16" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="AK16" s="10" t="s">
         <v>168</v>
-      </c>
-      <c r="AI16" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="AK16" s="10" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
@@ -3022,7 +3025,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D17" s="51" t="s">
         <v>3</v>
@@ -3085,7 +3088,7 @@
         <v>0</v>
       </c>
       <c r="AB17" s="48" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AC17" s="48"/>
       <c r="AD17" s="48"/>
@@ -3095,13 +3098,13 @@
       <c r="AH17" s="48"/>
       <c r="AI17" s="48"/>
       <c r="AK17" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" s="47"/>
       <c r="B18" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D18" s="51" t="s">
         <v>3</v>
@@ -3140,7 +3143,7 @@
         <v>8</v>
       </c>
       <c r="T18" s="48" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="U18" s="48"/>
       <c r="V18" s="48"/>
@@ -3158,13 +3161,13 @@
       <c r="AH18" s="48"/>
       <c r="AI18" s="48"/>
       <c r="AK18" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" s="47"/>
       <c r="B19" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D19" s="51" t="s">
         <v>3</v>
@@ -3203,7 +3206,7 @@
         <v>8</v>
       </c>
       <c r="T19" s="48" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="U19" s="48"/>
       <c r="V19" s="48"/>
@@ -3221,13 +3224,13 @@
       <c r="AH19" s="48"/>
       <c r="AI19" s="48"/>
       <c r="AK19" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" s="47"/>
       <c r="B20" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D20" s="51" t="s">
         <v>3</v>
@@ -3276,7 +3279,7 @@
       <c r="AH20" s="48"/>
       <c r="AI20" s="48"/>
       <c r="AK20" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
@@ -3309,7 +3312,7 @@
       <c r="L21" s="48"/>
       <c r="M21" s="48"/>
       <c r="N21" s="48" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O21" s="48"/>
       <c r="P21" s="48"/>
@@ -3333,7 +3336,7 @@
       <c r="AH21" s="48"/>
       <c r="AI21" s="48"/>
       <c r="AK21" s="10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.25">
@@ -3341,7 +3344,7 @@
         <v>6</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D22" s="51" t="s">
         <v>3</v>
@@ -3361,7 +3364,7 @@
         <v>0</v>
       </c>
       <c r="K22" s="50" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L22" s="50"/>
       <c r="M22" s="50"/>
@@ -3390,13 +3393,13 @@
       <c r="AH22" s="48"/>
       <c r="AI22" s="48"/>
       <c r="AK22" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" s="78"/>
       <c r="B23" s="46" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D23" s="51" t="s">
         <v>3</v>
@@ -3416,7 +3419,7 @@
         <v>1</v>
       </c>
       <c r="K23" s="66" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L23" s="67"/>
       <c r="M23" s="68"/>
@@ -3451,7 +3454,7 @@
         <v>7</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D24" s="51" t="s">
         <v>3</v>
@@ -3471,7 +3474,7 @@
         <v>0</v>
       </c>
       <c r="K24" s="50" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L24" s="50"/>
       <c r="M24" s="50"/>
@@ -3485,7 +3488,7 @@
         <v>0</v>
       </c>
       <c r="Q24" s="49" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="R24" s="49"/>
       <c r="S24" s="49"/>
@@ -3493,7 +3496,7 @@
       <c r="U24" s="49"/>
       <c r="V24" s="49"/>
       <c r="W24" s="48" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="X24" s="48"/>
       <c r="Y24" s="48"/>
@@ -3508,7 +3511,7 @@
       <c r="AH24" s="48"/>
       <c r="AI24" s="48"/>
       <c r="AK24" s="10" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
@@ -3516,7 +3519,7 @@
         <v>8</v>
       </c>
       <c r="B25" s="46" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D25" s="75" t="s">
         <v>3</v>
@@ -3583,7 +3586,7 @@
         <v>0</v>
       </c>
       <c r="AB25" s="69" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AC25" s="70"/>
       <c r="AD25" s="70"/>
@@ -3593,7 +3596,7 @@
       <c r="AH25" s="70"/>
       <c r="AI25" s="71"/>
       <c r="AK25" s="10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
@@ -3763,7 +3766,7 @@
       <c r="AH27" s="48"/>
       <c r="AI27" s="48"/>
       <c r="AK27" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" spans="1:37" x14ac:dyDescent="0.25">
@@ -4635,7 +4638,7 @@
   <sheetData>
     <row r="1" spans="1:21" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -4659,16 +4662,16 @@
     <row r="2" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B4" s="33" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -4691,11 +4694,11 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B5" s="33" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -4722,7 +4725,7 @@
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -4742,11 +4745,11 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B7" s="33" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -4764,12 +4767,12 @@
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
       <c r="U7" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>0</v>
@@ -4841,7 +4844,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="48" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H10" s="48"/>
       <c r="I10" s="48"/>
@@ -4871,7 +4874,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D11" s="32">
         <v>0</v>
@@ -4923,7 +4926,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C12" s="29"/>
       <c r="D12" s="32">
@@ -4977,7 +4980,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C13" s="29"/>
       <c r="D13" s="32">
@@ -5003,7 +5006,7 @@
         <v>1</v>
       </c>
       <c r="L13" s="49" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="M13" s="49"/>
       <c r="N13" s="49"/>
@@ -5019,7 +5022,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="33" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C14" s="29"/>
       <c r="D14" s="32">
@@ -5045,7 +5048,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="49" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="M14" s="49"/>
       <c r="N14" s="49"/>
@@ -5087,7 +5090,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="49" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="M15" s="49"/>
       <c r="N15" s="49"/>
@@ -5103,7 +5106,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="33" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D16" s="32">
         <v>0</v>
@@ -5126,7 +5129,7 @@
         <v>1</v>
       </c>
       <c r="L16" s="49" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="M16" s="49"/>
       <c r="N16" s="49"/>
@@ -5136,7 +5139,7 @@
       <c r="R16" s="49"/>
       <c r="S16" s="49"/>
       <c r="U16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
@@ -5144,7 +5147,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D17" s="32">
         <v>1</v>
@@ -5159,11 +5162,11 @@
         <v>0</v>
       </c>
       <c r="H17" s="49" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I17" s="49"/>
       <c r="J17" s="49" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K17" s="49"/>
       <c r="L17" s="32">
@@ -5191,13 +5194,13 @@
         <v>8</v>
       </c>
       <c r="U17" s="10" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="47"/>
       <c r="B18" s="33" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D18" s="32">
         <v>1</v>
@@ -5212,11 +5215,11 @@
         <v>0</v>
       </c>
       <c r="H18" s="49" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I18" s="49"/>
       <c r="J18" s="49" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K18" s="49"/>
       <c r="L18" s="32">
@@ -5244,13 +5247,13 @@
         <v>8</v>
       </c>
       <c r="U18" s="10" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="47"/>
       <c r="B19" s="33" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D19" s="32">
         <v>1</v>
@@ -5265,7 +5268,7 @@
         <v>0</v>
       </c>
       <c r="H19" s="50" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="I19" s="50"/>
       <c r="J19" s="50"/>
@@ -5295,7 +5298,7 @@
         <v>0</v>
       </c>
       <c r="U19" s="10" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
@@ -5527,7 +5530,7 @@
   <dimension ref="A1:Q48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5545,13 +5548,13 @@
   <sheetData>
     <row r="1" spans="1:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="35" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" s="36">
         <v>1</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -5559,7 +5562,7 @@
     </row>
     <row r="2" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="59" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B2" s="60"/>
       <c r="C2" s="60"/>
@@ -5573,7 +5576,7 @@
       <c r="K2" s="60"/>
       <c r="L2" s="61"/>
       <c r="M2" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5600,26 +5603,26 @@
         <v>0</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="P3" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q3" s="23" t="s">
         <v>175</v>
-      </c>
-      <c r="Q3" s="23" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -5657,16 +5660,16 @@
         <v>14</v>
       </c>
       <c r="M4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="N4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="Q4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -5704,16 +5707,16 @@
         <v>44</v>
       </c>
       <c r="M5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="Q5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -5751,16 +5754,16 @@
         <v>74</v>
       </c>
       <c r="M6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Q6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -5798,16 +5801,16 @@
         <v>75</v>
       </c>
       <c r="M7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="Q7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -5845,12 +5848,12 @@
         <v>88</v>
       </c>
       <c r="M8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6">
@@ -5880,21 +5883,21 @@
         <v>36h</v>
       </c>
       <c r="L9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="N9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="P9" s="19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6">
@@ -5924,21 +5927,21 @@
         <v>37h</v>
       </c>
       <c r="L10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="N10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P10" s="19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6">
@@ -5968,13 +5971,13 @@
         <v>3Eh</v>
       </c>
       <c r="L11" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="M11" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="P11" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -6012,10 +6015,10 @@
         <v>77</v>
       </c>
       <c r="M12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="P12" s="19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -6053,10 +6056,10 @@
         <v>45</v>
       </c>
       <c r="M13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -6094,10 +6097,10 @@
         <v>46</v>
       </c>
       <c r="M14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -6135,10 +6138,10 @@
         <v>47</v>
       </c>
       <c r="M15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -6176,10 +6179,10 @@
         <v>48</v>
       </c>
       <c r="M16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -6217,10 +6220,10 @@
         <v>49</v>
       </c>
       <c r="M17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -6258,10 +6261,10 @@
         <v>50</v>
       </c>
       <c r="M18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -6305,7 +6308,7 @@
         <v>Rd = Rs + Rm</v>
       </c>
       <c r="N19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -6349,7 +6352,7 @@
         <v>Rd = Rs - Rm</v>
       </c>
       <c r="N20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -6393,7 +6396,7 @@
         <v>Rd = Rs * Rm</v>
       </c>
       <c r="N21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -6437,7 +6440,7 @@
         <v>Rd = Rs / Rm</v>
       </c>
       <c r="N22" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -6481,7 +6484,7 @@
         <v>Rd = Rs ^ Rm</v>
       </c>
       <c r="N23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -6525,7 +6528,7 @@
         <v>Rd = Rs % Rm</v>
       </c>
       <c r="N24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -6563,10 +6566,10 @@
         <v>51</v>
       </c>
       <c r="M25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -6604,10 +6607,10 @@
         <v>52</v>
       </c>
       <c r="M26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -6645,10 +6648,10 @@
         <v>53</v>
       </c>
       <c r="M27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -6686,10 +6689,10 @@
         <v>54</v>
       </c>
       <c r="M28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -6727,10 +6730,10 @@
         <v>55</v>
       </c>
       <c r="M29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -6768,10 +6771,10 @@
         <v>56</v>
       </c>
       <c r="M30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -6809,10 +6812,10 @@
         <v>57</v>
       </c>
       <c r="M31" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="N31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -6850,10 +6853,10 @@
         <v>58</v>
       </c>
       <c r="M32" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N32" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -6891,10 +6894,10 @@
         <v>59</v>
       </c>
       <c r="M33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N33" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -6932,10 +6935,10 @@
         <v>60</v>
       </c>
       <c r="M34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
@@ -6973,10 +6976,10 @@
         <v>61</v>
       </c>
       <c r="M35" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N35" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
@@ -7014,10 +7017,10 @@
         <v>62</v>
       </c>
       <c r="M36" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N36" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
@@ -7055,10 +7058,10 @@
         <v>63</v>
       </c>
       <c r="M37" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N37" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -7096,15 +7099,15 @@
         <v>64</v>
       </c>
       <c r="M38" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N38" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="6">
@@ -7134,13 +7137,13 @@
         <v>18h</v>
       </c>
       <c r="L39" t="s">
+        <v>191</v>
+      </c>
+      <c r="M39" t="s">
         <v>192</v>
       </c>
-      <c r="M39" t="s">
-        <v>193</v>
-      </c>
       <c r="N39" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
@@ -7178,10 +7181,10 @@
         <v>65</v>
       </c>
       <c r="M40" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N40" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
@@ -7219,10 +7222,10 @@
         <v>66</v>
       </c>
       <c r="M41" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N41" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
@@ -7260,10 +7263,10 @@
         <v>67</v>
       </c>
       <c r="M42" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N42" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
@@ -7301,10 +7304,10 @@
         <v>68</v>
       </c>
       <c r="M43" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N43" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
@@ -7342,10 +7345,10 @@
         <v>69</v>
       </c>
       <c r="M44" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N44" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
@@ -7383,10 +7386,10 @@
         <v>70</v>
       </c>
       <c r="M45" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N45" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
@@ -7424,10 +7427,10 @@
         <v>71</v>
       </c>
       <c r="M46" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N46" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
@@ -7508,7 +7511,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="35" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" s="36">
         <v>1</v>
@@ -7519,7 +7522,7 @@
     </row>
     <row r="2" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="59" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B2" s="60"/>
       <c r="C2" s="60"/>
@@ -7532,7 +7535,7 @@
       <c r="J2" s="60"/>
       <c r="K2" s="61"/>
       <c r="L2" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7556,20 +7559,20 @@
         <v>0</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -7604,10 +7607,10 @@
         <v>14</v>
       </c>
       <c r="L4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="M4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -7642,10 +7645,10 @@
         <v>44</v>
       </c>
       <c r="L5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -7680,10 +7683,10 @@
         <v>74</v>
       </c>
       <c r="L6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -7718,15 +7721,15 @@
         <v>75</v>
       </c>
       <c r="L7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B8" s="29"/>
       <c r="C8" s="29">
@@ -7753,10 +7756,10 @@
         <v>1Eh</v>
       </c>
       <c r="K8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="L8" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -7791,7 +7794,7 @@
         <v>77</v>
       </c>
       <c r="L9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -7826,10 +7829,10 @@
         <v>45</v>
       </c>
       <c r="L10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -7864,10 +7867,10 @@
         <v>46</v>
       </c>
       <c r="L11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -7902,10 +7905,10 @@
         <v>47</v>
       </c>
       <c r="L12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -7940,10 +7943,10 @@
         <v>48</v>
       </c>
       <c r="L13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -7978,10 +7981,10 @@
         <v>49</v>
       </c>
       <c r="L14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -8016,10 +8019,10 @@
         <v>50</v>
       </c>
       <c r="L15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -8054,10 +8057,10 @@
         <v>51</v>
       </c>
       <c r="L16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -8092,10 +8095,10 @@
         <v>52</v>
       </c>
       <c r="L17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -8130,10 +8133,10 @@
         <v>53</v>
       </c>
       <c r="L18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -8168,10 +8171,10 @@
         <v>54</v>
       </c>
       <c r="L19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="M19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -8206,10 +8209,10 @@
         <v>55</v>
       </c>
       <c r="L20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -8244,10 +8247,10 @@
         <v>56</v>
       </c>
       <c r="L21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -8282,10 +8285,10 @@
         <v>71</v>
       </c>
       <c r="L22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="M22" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -8345,8 +8348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8361,13 +8364,13 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="35" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" s="36">
         <v>2</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -8375,7 +8378,7 @@
     </row>
     <row r="2" spans="1:6" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="28" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B2" s="37"/>
       <c r="C2" s="28"/>
@@ -8385,129 +8388,129 @@
     </row>
     <row r="3" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B3" s="38"/>
       <c r="C3" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E10" t="s">
+        <v>226</v>
+      </c>
+      <c r="F10" t="s">
         <v>227</v>
-      </c>
-      <c r="F10" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="28" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B11" s="37"/>
       <c r="C11" s="28"/>
@@ -8517,118 +8520,118 @@
     </row>
     <row r="12" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="27" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B12" s="38"/>
       <c r="C12" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D15" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C16" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D16" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E16" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="26" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C17" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D17" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E17" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C18" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="35" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B19" s="36">
         <v>3</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -8636,42 +8639,42 @@
     </row>
     <row r="20" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="27" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B20" s="38"/>
       <c r="C20" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F20" s="23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="C21" t="s">
+        <v>256</v>
+      </c>
+      <c r="D21" t="s">
         <v>255</v>
-      </c>
-      <c r="C21" t="s">
-        <v>257</v>
-      </c>
-      <c r="D21" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="35" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B22" s="36">
         <v>4</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -8679,81 +8682,81 @@
     </row>
     <row r="23" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="27" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B23" s="38"/>
       <c r="C23" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F23" s="23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
+        <v>257</v>
+      </c>
+      <c r="C24" t="s">
         <v>258</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
+        <v>289</v>
+      </c>
+      <c r="E24" t="s">
         <v>259</v>
-      </c>
-      <c r="D24" t="s">
-        <v>290</v>
-      </c>
-      <c r="E24" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C25" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D25" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E25" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="26" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C26" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D26" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E26" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="26" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C27" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D27" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E27" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="35" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B28" s="36">
         <v>5</v>
@@ -8767,78 +8770,78 @@
     </row>
     <row r="29" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="27" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B29" s="38"/>
       <c r="C29" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F29" s="23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D31" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E31" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F31" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="26" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D32" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E32" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="26" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E33" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="35" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B34" s="36">
         <v>6</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -8846,144 +8849,144 @@
     </row>
     <row r="35" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="27" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B35" s="38"/>
       <c r="C35" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F35" s="23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="26" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C36" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D36" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E36" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F36" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="26" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C37" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D37" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E37" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F37" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="26" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C38" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D38" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E38" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F38" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="26" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C39" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D39" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E39" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F39" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="26" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C40" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D40" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E40" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F40" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="26" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C41" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D41" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E41" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="26" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C42" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D42" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E42" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="35" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B43" s="36">
         <v>7</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -8991,31 +8994,31 @@
     </row>
     <row r="44" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="27" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B44" s="38"/>
       <c r="C44" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F44" s="23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="35" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B46" s="36">
         <v>8</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -9023,31 +9026,31 @@
     </row>
     <row r="47" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="27" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B47" s="38"/>
       <c r="C47" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F47" s="23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="35" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B49" s="36">
         <v>9</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
@@ -9055,31 +9058,31 @@
     </row>
     <row r="50" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="27" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B50" s="38"/>
       <c r="C50" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F50" s="23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="35" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B52" s="36">
         <v>10</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
@@ -9087,31 +9090,31 @@
     </row>
     <row r="53" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="27" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B53" s="38"/>
       <c r="C53" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F53" s="23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="35" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B55" s="36">
         <v>11</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
@@ -9119,25 +9122,25 @@
     </row>
     <row r="56" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="27" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B56" s="38"/>
       <c r="C56" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F56" s="23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="35" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B58" s="36">
         <v>12</v>
@@ -9151,20 +9154,20 @@
     </row>
     <row r="59" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="27" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B59" s="38"/>
       <c r="C59" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F59" s="23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -9176,8 +9179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AJ6" sqref="AJ6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9191,7 +9194,7 @@
   <sheetData>
     <row r="1" spans="1:36" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -9229,7 +9232,7 @@
     </row>
     <row r="2" spans="1:36" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="4" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9336,7 +9339,7 @@
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="39" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C5" s="41">
         <v>0</v>
@@ -9421,12 +9424,12 @@
       <c r="AG5" s="52"/>
       <c r="AH5" s="52"/>
       <c r="AJ5" s="10" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="46" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C6" s="43">
         <v>0</v>
@@ -9501,99 +9504,99 @@
         <v>1</v>
       </c>
       <c r="AA6" s="53" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AB6" s="53"/>
       <c r="AC6" s="53"/>
       <c r="AD6" s="53"/>
       <c r="AE6" s="53"/>
       <c r="AF6" s="52" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="AG6" s="52"/>
       <c r="AH6" s="52"/>
       <c r="AJ6" s="10" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="46" t="s">
+        <v>405</v>
+      </c>
+      <c r="C7" s="43">
+        <v>0</v>
+      </c>
+      <c r="D7" s="43">
+        <v>0</v>
+      </c>
+      <c r="E7" s="43">
+        <v>0</v>
+      </c>
+      <c r="F7" s="43">
+        <v>0</v>
+      </c>
+      <c r="G7" s="43">
+        <v>0</v>
+      </c>
+      <c r="H7" s="43">
+        <v>0</v>
+      </c>
+      <c r="I7" s="43">
+        <v>0</v>
+      </c>
+      <c r="J7" s="43">
+        <v>0</v>
+      </c>
+      <c r="K7" s="43">
+        <v>0</v>
+      </c>
+      <c r="L7" s="43">
+        <v>0</v>
+      </c>
+      <c r="M7" s="43">
+        <v>0</v>
+      </c>
+      <c r="N7" s="43">
+        <v>0</v>
+      </c>
+      <c r="O7" s="43">
+        <v>0</v>
+      </c>
+      <c r="P7" s="43">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="43">
+        <v>0</v>
+      </c>
+      <c r="R7" s="43">
+        <v>0</v>
+      </c>
+      <c r="S7" s="43">
+        <v>0</v>
+      </c>
+      <c r="T7" s="43">
+        <v>0</v>
+      </c>
+      <c r="U7" s="43">
+        <v>0</v>
+      </c>
+      <c r="V7" s="43">
+        <v>0</v>
+      </c>
+      <c r="W7" s="43">
+        <v>0</v>
+      </c>
+      <c r="X7" s="43">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="43">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="AA7" s="63" t="s">
         <v>406</v>
-      </c>
-      <c r="C7" s="43">
-        <v>0</v>
-      </c>
-      <c r="D7" s="43">
-        <v>0</v>
-      </c>
-      <c r="E7" s="43">
-        <v>0</v>
-      </c>
-      <c r="F7" s="43">
-        <v>0</v>
-      </c>
-      <c r="G7" s="43">
-        <v>0</v>
-      </c>
-      <c r="H7" s="43">
-        <v>0</v>
-      </c>
-      <c r="I7" s="43">
-        <v>0</v>
-      </c>
-      <c r="J7" s="43">
-        <v>0</v>
-      </c>
-      <c r="K7" s="43">
-        <v>0</v>
-      </c>
-      <c r="L7" s="43">
-        <v>0</v>
-      </c>
-      <c r="M7" s="43">
-        <v>0</v>
-      </c>
-      <c r="N7" s="43">
-        <v>0</v>
-      </c>
-      <c r="O7" s="43">
-        <v>0</v>
-      </c>
-      <c r="P7" s="43">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="43">
-        <v>0</v>
-      </c>
-      <c r="R7" s="43">
-        <v>0</v>
-      </c>
-      <c r="S7" s="43">
-        <v>0</v>
-      </c>
-      <c r="T7" s="43">
-        <v>0</v>
-      </c>
-      <c r="U7" s="43">
-        <v>0</v>
-      </c>
-      <c r="V7" s="43">
-        <v>0</v>
-      </c>
-      <c r="W7" s="43">
-        <v>0</v>
-      </c>
-      <c r="X7" s="43">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="43">
-        <v>1</v>
-      </c>
-      <c r="Z7" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="AA7" s="63" t="s">
-        <v>407</v>
       </c>
       <c r="AB7" s="64"/>
       <c r="AC7" s="64"/>
@@ -9603,12 +9606,12 @@
       <c r="AG7" s="64"/>
       <c r="AH7" s="65"/>
       <c r="AJ7" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="39" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C8" s="41">
         <v>0</v>
@@ -9635,19 +9638,19 @@
         <v>1</v>
       </c>
       <c r="K8" s="52" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="L8" s="52"/>
       <c r="M8" s="52"/>
       <c r="N8" s="52"/>
       <c r="O8" s="52"/>
       <c r="P8" s="52" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="Q8" s="52"/>
       <c r="R8" s="52"/>
       <c r="S8" s="52" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="T8" s="52"/>
       <c r="U8" s="52"/>
@@ -9667,7 +9670,7 @@
       <c r="AG8" s="52"/>
       <c r="AH8" s="52"/>
       <c r="AJ8" s="10" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.25">
@@ -9699,7 +9702,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="48" t="s">
-        <v>92</v>
+        <v>411</v>
       </c>
       <c r="L9" s="48"/>
       <c r="M9" s="48"/>
@@ -9725,7 +9728,7 @@
       <c r="AG9" s="48"/>
       <c r="AH9" s="48"/>
       <c r="AJ9" s="10" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
@@ -9766,7 +9769,7 @@
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C11" s="6">
         <v>1</v>
@@ -9803,7 +9806,7 @@
       <c r="AG11" s="48"/>
       <c r="AH11" s="48"/>
       <c r="AJ11" s="10" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.25">
@@ -9948,7 +9951,9 @@
       <c r="AF15" s="6"/>
       <c r="AG15" s="6"/>
       <c r="AH15" s="6"/>
-      <c r="AJ15" s="10"/>
+      <c r="AJ15" s="10" t="s">
+        <v>410</v>
+      </c>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
@@ -10321,7 +10326,7 @@
     </row>
     <row r="28" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4">
@@ -10370,7 +10375,7 @@
     </row>
     <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="45">
@@ -10390,7 +10395,7 @@
       </c>
       <c r="H29" s="6"/>
       <c r="I29" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
@@ -10421,7 +10426,7 @@
     </row>
     <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="45">
@@ -10467,12 +10472,12 @@
       <c r="AG30" s="6"/>
       <c r="AH30" s="6"/>
       <c r="AJ30" s="10" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C31" s="45">
         <v>0</v>
@@ -10491,7 +10496,7 @@
       </c>
       <c r="H31" s="6"/>
       <c r="I31" s="10" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
@@ -10522,7 +10527,7 @@
     </row>
     <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C32" s="45">
         <v>0</v>
@@ -10541,7 +10546,7 @@
       </c>
       <c r="H32" s="6"/>
       <c r="I32" s="10" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="J32" s="6"/>
       <c r="K32" s="6"/>
@@ -10572,7 +10577,7 @@
     </row>
     <row r="33" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C33" s="45">
         <v>0</v>
@@ -10591,7 +10596,7 @@
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="10" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="J33" s="6"/>
       <c r="K33" s="6"/>
@@ -10619,12 +10624,12 @@
       <c r="AG33" s="6"/>
       <c r="AH33" s="6"/>
       <c r="AJ33" s="10" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="34" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C34" s="45">
         <v>0</v>
@@ -10643,7 +10648,7 @@
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="10" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="J34" s="6"/>
       <c r="K34" s="6"/>
@@ -10674,7 +10679,7 @@
     </row>
     <row r="35" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A35" s="46" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C35" s="45">
         <v>0</v>
@@ -10693,7 +10698,7 @@
       </c>
       <c r="H35" s="44"/>
       <c r="I35" s="10" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="J35" s="44"/>
       <c r="K35" s="44"/>
@@ -10724,7 +10729,7 @@
     </row>
     <row r="36" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C36" s="45">
         <v>0</v>
@@ -10743,7 +10748,7 @@
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="10" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="J36" s="6"/>
       <c r="K36" s="6"/>
@@ -10774,7 +10779,7 @@
     </row>
     <row r="37" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C37" s="45">
         <v>0</v>
@@ -10793,7 +10798,7 @@
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="J37" s="6"/>
       <c r="K37" s="6"/>
@@ -10824,7 +10829,7 @@
     </row>
     <row r="38" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C38" s="45">
         <v>0</v>
@@ -10843,7 +10848,7 @@
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="10" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="J38" s="6"/>
       <c r="K38" s="6"/>
@@ -10874,7 +10879,7 @@
     </row>
     <row r="39" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C39" s="45">
         <v>0</v>
@@ -10893,7 +10898,7 @@
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="10" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J39" s="6"/>
       <c r="K39" s="6"/>
@@ -10924,7 +10929,7 @@
     </row>
     <row r="40" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C40" s="45">
         <v>0</v>
@@ -10943,7 +10948,7 @@
       </c>
       <c r="H40" s="6"/>
       <c r="I40" s="10" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="J40" s="6"/>
       <c r="K40" s="6"/>
@@ -10973,30 +10978,30 @@
     </row>
     <row r="41" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="C41" s="45">
+        <v>0</v>
+      </c>
+      <c r="D41" s="44">
+        <v>1</v>
+      </c>
+      <c r="E41" s="44">
+        <v>1</v>
+      </c>
+      <c r="F41" s="6">
+        <v>0</v>
+      </c>
+      <c r="G41" s="6">
+        <v>0</v>
+      </c>
+      <c r="I41" s="10" t="s">
         <v>387</v>
-      </c>
-      <c r="C41" s="45">
-        <v>0</v>
-      </c>
-      <c r="D41" s="44">
-        <v>1</v>
-      </c>
-      <c r="E41" s="44">
-        <v>1</v>
-      </c>
-      <c r="F41" s="6">
-        <v>0</v>
-      </c>
-      <c r="G41" s="6">
-        <v>0</v>
-      </c>
-      <c r="I41" s="10" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="42" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A42" s="46" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C42" s="45">
         <v>0</v>
@@ -11017,7 +11022,7 @@
     </row>
     <row r="43" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C43" s="45">
         <v>0</v>
@@ -11036,7 +11041,7 @@
       </c>
       <c r="H43" s="6"/>
       <c r="I43" s="10" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="J43" s="6"/>
       <c r="K43" s="6"/>
@@ -11067,30 +11072,30 @@
     </row>
     <row r="44" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A44" s="46" t="s">
+        <v>391</v>
+      </c>
+      <c r="C44" s="45">
+        <v>0</v>
+      </c>
+      <c r="D44" s="44">
+        <v>1</v>
+      </c>
+      <c r="E44" s="44">
+        <v>1</v>
+      </c>
+      <c r="F44" s="44">
+        <v>1</v>
+      </c>
+      <c r="G44" s="44">
+        <v>1</v>
+      </c>
+      <c r="I44" s="10" t="s">
         <v>392</v>
-      </c>
-      <c r="C44" s="45">
-        <v>0</v>
-      </c>
-      <c r="D44" s="44">
-        <v>1</v>
-      </c>
-      <c r="E44" s="44">
-        <v>1</v>
-      </c>
-      <c r="F44" s="44">
-        <v>1</v>
-      </c>
-      <c r="G44" s="44">
-        <v>1</v>
-      </c>
-      <c r="I44" s="10" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="45" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A45" s="46" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C45" s="45">
         <v>1</v>
@@ -11108,36 +11113,36 @@
         <v>0</v>
       </c>
       <c r="I45" s="10" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="AJ45" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="46" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A46" s="46" t="s">
+        <v>400</v>
+      </c>
+      <c r="C46" s="45">
+        <v>1</v>
+      </c>
+      <c r="D46" s="44">
+        <v>0</v>
+      </c>
+      <c r="E46" s="44">
+        <v>0</v>
+      </c>
+      <c r="F46" s="44">
+        <v>1</v>
+      </c>
+      <c r="G46" s="44">
+        <v>1</v>
+      </c>
+      <c r="I46" s="10" t="s">
+        <v>402</v>
+      </c>
+      <c r="AJ46" t="s">
         <v>401</v>
-      </c>
-      <c r="C46" s="45">
-        <v>1</v>
-      </c>
-      <c r="D46" s="44">
-        <v>0</v>
-      </c>
-      <c r="E46" s="44">
-        <v>0</v>
-      </c>
-      <c r="F46" s="44">
-        <v>1</v>
-      </c>
-      <c r="G46" s="44">
-        <v>1</v>
-      </c>
-      <c r="I46" s="10" t="s">
-        <v>403</v>
-      </c>
-      <c r="AJ46" t="s">
-        <v>402</v>
       </c>
     </row>
   </sheetData>
@@ -11176,7 +11181,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="62" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B1" s="62"/>
       <c r="C1" s="62"/>
@@ -11221,15 +11226,15 @@
         <v>0</v>
       </c>
       <c r="K3" s="38" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L3" s="38" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C4" s="25">
         <v>0</v>
@@ -11266,7 +11271,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C5" s="25">
         <v>0</v>
@@ -11303,7 +11308,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C6" s="25">
         <v>0</v>
@@ -11340,7 +11345,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C7" s="25">
         <v>0</v>
@@ -11480,7 +11485,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -11555,68 +11560,68 @@
         <v>0</v>
       </c>
       <c r="T3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="39" t="s">
+        <v>307</v>
+      </c>
+      <c r="C4" s="41">
+        <v>0</v>
+      </c>
+      <c r="D4" s="41">
+        <v>0</v>
+      </c>
+      <c r="E4" s="41">
+        <v>0</v>
+      </c>
+      <c r="F4" s="41">
+        <v>0</v>
+      </c>
+      <c r="G4" s="41">
+        <v>0</v>
+      </c>
+      <c r="H4" s="41">
+        <v>0</v>
+      </c>
+      <c r="I4" s="41">
+        <v>0</v>
+      </c>
+      <c r="J4" s="41">
+        <v>0</v>
+      </c>
+      <c r="K4" s="41">
+        <v>0</v>
+      </c>
+      <c r="L4" s="41">
+        <v>0</v>
+      </c>
+      <c r="M4" s="41">
+        <v>0</v>
+      </c>
+      <c r="N4" s="41">
+        <v>0</v>
+      </c>
+      <c r="O4" s="41">
+        <v>0</v>
+      </c>
+      <c r="P4" s="41">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="41">
+        <v>0</v>
+      </c>
+      <c r="R4" s="41" t="s">
         <v>308</v>
       </c>
-      <c r="C4" s="41">
-        <v>0</v>
-      </c>
-      <c r="D4" s="41">
-        <v>0</v>
-      </c>
-      <c r="E4" s="41">
-        <v>0</v>
-      </c>
-      <c r="F4" s="41">
-        <v>0</v>
-      </c>
-      <c r="G4" s="41">
-        <v>0</v>
-      </c>
-      <c r="H4" s="41">
-        <v>0</v>
-      </c>
-      <c r="I4" s="41">
-        <v>0</v>
-      </c>
-      <c r="J4" s="41">
-        <v>0</v>
-      </c>
-      <c r="K4" s="41">
-        <v>0</v>
-      </c>
-      <c r="L4" s="41">
-        <v>0</v>
-      </c>
-      <c r="M4" s="41">
-        <v>0</v>
-      </c>
-      <c r="N4" s="41">
-        <v>0</v>
-      </c>
-      <c r="O4" s="41">
-        <v>0</v>
-      </c>
-      <c r="P4" s="41">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="41">
-        <v>0</v>
-      </c>
-      <c r="R4" s="41" t="s">
-        <v>309</v>
-      </c>
       <c r="T4" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C5" s="40">
         <v>0</v>
@@ -11664,15 +11669,15 @@
         <v>1</v>
       </c>
       <c r="R5" s="40" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="T5" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="39" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C6" s="40">
         <v>0</v>
@@ -11720,52 +11725,52 @@
         <v>0</v>
       </c>
       <c r="R6" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="T6" s="10"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="39" t="s">
+        <v>305</v>
+      </c>
+      <c r="C7" s="40">
+        <v>0</v>
+      </c>
+      <c r="D7" s="40">
+        <v>0</v>
+      </c>
+      <c r="E7" s="40">
+        <v>0</v>
+      </c>
+      <c r="F7" s="40">
+        <v>0</v>
+      </c>
+      <c r="G7" s="40">
+        <v>0</v>
+      </c>
+      <c r="H7" s="40">
+        <v>0</v>
+      </c>
+      <c r="I7" s="40">
+        <v>0</v>
+      </c>
+      <c r="J7" s="40">
+        <v>0</v>
+      </c>
+      <c r="K7" s="40">
+        <v>0</v>
+      </c>
+      <c r="L7" s="40">
+        <v>0</v>
+      </c>
+      <c r="M7" s="40">
+        <v>0</v>
+      </c>
+      <c r="N7" s="40">
+        <v>1</v>
+      </c>
+      <c r="O7" s="48" t="s">
         <v>306</v>
-      </c>
-      <c r="C7" s="40">
-        <v>0</v>
-      </c>
-      <c r="D7" s="40">
-        <v>0</v>
-      </c>
-      <c r="E7" s="40">
-        <v>0</v>
-      </c>
-      <c r="F7" s="40">
-        <v>0</v>
-      </c>
-      <c r="G7" s="40">
-        <v>0</v>
-      </c>
-      <c r="H7" s="40">
-        <v>0</v>
-      </c>
-      <c r="I7" s="40">
-        <v>0</v>
-      </c>
-      <c r="J7" s="40">
-        <v>0</v>
-      </c>
-      <c r="K7" s="40">
-        <v>0</v>
-      </c>
-      <c r="L7" s="40">
-        <v>0</v>
-      </c>
-      <c r="M7" s="40">
-        <v>0</v>
-      </c>
-      <c r="N7" s="40">
-        <v>1</v>
-      </c>
-      <c r="O7" s="48" t="s">
-        <v>307</v>
       </c>
       <c r="P7" s="48"/>
       <c r="Q7" s="48"/>
@@ -11774,7 +11779,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="39" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C8" s="40">
         <v>0</v>
@@ -11801,7 +11806,7 @@
         <v>1</v>
       </c>
       <c r="K8" s="48" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L8" s="48"/>
       <c r="M8" s="48"/>
@@ -11814,7 +11819,7 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="39" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C9" s="40">
         <v>0</v>
@@ -11838,10 +11843,10 @@
         <v>1</v>
       </c>
       <c r="J9" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K9" s="48" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L9" s="48"/>
       <c r="M9" s="48"/>
@@ -11854,7 +11859,7 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="39" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C10" s="40">
         <v>0</v>
@@ -11878,10 +11883,10 @@
         <v>0</v>
       </c>
       <c r="J10" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K10" s="48" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L10" s="48"/>
       <c r="M10" s="48"/>
@@ -11894,7 +11899,7 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="39" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C11" s="40">
         <v>0</v>
@@ -11918,10 +11923,10 @@
         <v>1</v>
       </c>
       <c r="J11" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K11" s="48" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L11" s="48"/>
       <c r="M11" s="48"/>
@@ -11934,34 +11939,34 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0</v>
+      </c>
+      <c r="G12" s="6">
+        <v>1</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0</v>
+      </c>
+      <c r="J12" s="6">
+        <v>0</v>
+      </c>
+      <c r="K12" s="48" t="s">
         <v>304</v>
-      </c>
-      <c r="C12" s="6">
-        <v>0</v>
-      </c>
-      <c r="D12" s="6">
-        <v>0</v>
-      </c>
-      <c r="E12" s="6">
-        <v>0</v>
-      </c>
-      <c r="F12" s="6">
-        <v>0</v>
-      </c>
-      <c r="G12" s="6">
-        <v>1</v>
-      </c>
-      <c r="H12" s="6">
-        <v>0</v>
-      </c>
-      <c r="I12" s="6">
-        <v>0</v>
-      </c>
-      <c r="J12" s="6">
-        <v>0</v>
-      </c>
-      <c r="K12" s="48" t="s">
-        <v>305</v>
       </c>
       <c r="L12" s="48"/>
       <c r="M12" s="48"/>

</xml_diff>

<commit_message>
fixing assembler not recognising LOADWORDI(option) astwo-liner at pass #1
</commit_message>
<xml_diff>
--- a/doc/RiscyInstSet32Bit.xlsx
+++ b/doc/RiscyInstSet32Bit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25410" windowHeight="12690" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25410" windowHeight="12690" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Summary - Terra" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="417">
   <si>
     <t>Description</t>
   </si>
@@ -693,9 +693,6 @@
     <t>destination, memory address offset</t>
   </si>
   <si>
-    <t>Loads destination register with a byte from address stored in source register, in the device (IRQ) stored in peripheral register</t>
-  </si>
-  <si>
     <t>Loads destination register with a halfword (two consecutive bytes) from address stored in source register, in the device (IRQ) stored in peripheral register</t>
   </si>
   <si>
@@ -717,24 +714,15 @@
     <t>You can only address xxx0h, xxx4h, xxx8h, xxxCh addresses; offset is a forementioned memory address divided by four</t>
   </si>
   <si>
-    <t>Stores a byte from destination register to address stored in source register, in the device (IRQ) stored in peripheral register</t>
-  </si>
-  <si>
     <t>Stores a halfword (two consecutive bytes) from destination register to address stored in source register, in the device (IRQ) stored in peripheral register</t>
   </si>
   <si>
     <t>Stores a full word (four consecutive bytes) from destination register to address stored in source register, in the device (IRQ) stored in peripheral register</t>
   </si>
   <si>
-    <t>Stores a byte immediate from address stored in destination register</t>
-  </si>
-  <si>
     <t>Stores a halfword immediate from address stored in destination register</t>
   </si>
   <si>
-    <t>Stores a full word from destination register to specified memory address</t>
-  </si>
-  <si>
     <t>rDest = dev[rPeri].mem[rSrc]</t>
   </si>
   <si>
@@ -1267,6 +1255,33 @@
   </si>
   <si>
     <t>Database address (offset)</t>
+  </si>
+  <si>
+    <t>Search for file by path</t>
+  </si>
+  <si>
+    <t>rDest</t>
+  </si>
+  <si>
+    <t>rDest must contain the IRQ of drive, and will be overwritten with file handle</t>
+  </si>
+  <si>
+    <t>Rd += 1h</t>
+  </si>
+  <si>
+    <t>Rd -= 1h</t>
+  </si>
+  <si>
+    <t>Stores a byte from destination register to address (NOT an offset) stored in source register, in the device (IRQ) stored in peripheral register</t>
+  </si>
+  <si>
+    <t>Loads destination register with a byte from address (NOT at offset) stored in source register, in the device (IRQ) stored in peripheral register</t>
+  </si>
+  <si>
+    <t>Stores a byte immediate from address (NOT an offset) stored in destination register</t>
+  </si>
+  <si>
+    <t>Stores a full word from destination register to specified memory address offset</t>
   </si>
 </sst>
 </file>
@@ -1367,7 +1382,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -1559,6 +1574,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9"/>
@@ -1570,7 +1607,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="6" applyFont="1"/>
@@ -1787,6 +1824,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -2078,7 +2121,7 @@
   <dimension ref="A1:AL52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23:AI23"/>
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2094,7 +2137,7 @@
   <sheetData>
     <row r="1" spans="1:38" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2134,7 +2177,7 @@
     <row r="2" spans="1:38" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.25">
@@ -2143,7 +2186,7 @@
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -2182,11 +2225,11 @@
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B5" s="33" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -2229,7 +2272,7 @@
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="10" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -2268,7 +2311,7 @@
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
@@ -2311,7 +2354,7 @@
     </row>
     <row r="9" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>0</v>
@@ -2484,7 +2527,7 @@
         <v>0</v>
       </c>
       <c r="AD10" s="57" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="AE10" s="57"/>
       <c r="AF10" s="57"/>
@@ -2498,7 +2541,7 @@
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="56"/>
       <c r="B11" s="7" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D11" s="51" t="s">
         <v>3</v>
@@ -2579,7 +2622,7 @@
         <v>8</v>
       </c>
       <c r="AK11" s="10" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.25">
@@ -2674,7 +2717,7 @@
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="56"/>
       <c r="B13" s="33" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D13" s="51" t="s">
         <v>3</v>
@@ -2699,7 +2742,7 @@
       <c r="L13" s="48"/>
       <c r="M13" s="48"/>
       <c r="N13" s="48" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="O13" s="48"/>
       <c r="P13" s="48"/>
@@ -2739,7 +2782,7 @@
         <v>0</v>
       </c>
       <c r="AD13" s="52" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="AE13" s="52"/>
       <c r="AF13" s="52"/>
@@ -2747,7 +2790,7 @@
       <c r="AH13" s="52"/>
       <c r="AI13" s="52"/>
       <c r="AK13" s="10" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
@@ -3344,7 +3387,7 @@
         <v>6</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="D22" s="51" t="s">
         <v>3</v>
@@ -3399,7 +3442,7 @@
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" s="78"/>
       <c r="B23" s="46" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="D23" s="51" t="s">
         <v>3</v>
@@ -3454,7 +3497,7 @@
         <v>7</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D24" s="51" t="s">
         <v>3</v>
@@ -3488,7 +3531,7 @@
         <v>0</v>
       </c>
       <c r="Q24" s="49" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="R24" s="49"/>
       <c r="S24" s="49"/>
@@ -3496,7 +3539,7 @@
       <c r="U24" s="49"/>
       <c r="V24" s="49"/>
       <c r="W24" s="48" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="X24" s="48"/>
       <c r="Y24" s="48"/>
@@ -3511,7 +3554,7 @@
       <c r="AH24" s="48"/>
       <c r="AI24" s="48"/>
       <c r="AK24" s="10" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
@@ -3519,7 +3562,7 @@
         <v>8</v>
       </c>
       <c r="B25" s="46" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D25" s="75" t="s">
         <v>3</v>
@@ -3586,7 +3629,7 @@
         <v>0</v>
       </c>
       <c r="AB25" s="69" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="AC25" s="70"/>
       <c r="AD25" s="70"/>
@@ -3596,7 +3639,7 @@
       <c r="AH25" s="70"/>
       <c r="AI25" s="71"/>
       <c r="AK25" s="10" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
@@ -4638,7 +4681,7 @@
   <sheetData>
     <row r="1" spans="1:21" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -4662,7 +4705,7 @@
     <row r="2" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -4671,7 +4714,7 @@
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -4694,11 +4737,11 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B5" s="33" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -4725,7 +4768,7 @@
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -4745,11 +4788,11 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B7" s="33" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -4767,12 +4810,12 @@
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
       <c r="U7" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>0</v>
@@ -4844,7 +4887,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="48" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="H10" s="48"/>
       <c r="I10" s="48"/>
@@ -4874,7 +4917,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="D11" s="32">
         <v>0</v>
@@ -5048,7 +5091,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="49" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="M14" s="49"/>
       <c r="N14" s="49"/>
@@ -5090,7 +5133,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="49" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="M15" s="49"/>
       <c r="N15" s="49"/>
@@ -5106,7 +5149,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="33" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="D16" s="32">
         <v>0</v>
@@ -5129,7 +5172,7 @@
         <v>1</v>
       </c>
       <c r="L16" s="49" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="M16" s="49"/>
       <c r="N16" s="49"/>
@@ -5147,7 +5190,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="D17" s="32">
         <v>1</v>
@@ -5162,11 +5205,11 @@
         <v>0</v>
       </c>
       <c r="H17" s="49" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="I17" s="49"/>
       <c r="J17" s="49" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="K17" s="49"/>
       <c r="L17" s="32">
@@ -5194,13 +5237,13 @@
         <v>8</v>
       </c>
       <c r="U17" s="10" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="47"/>
       <c r="B18" s="33" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="D18" s="32">
         <v>1</v>
@@ -5215,11 +5258,11 @@
         <v>0</v>
       </c>
       <c r="H18" s="49" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="I18" s="49"/>
       <c r="J18" s="49" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="K18" s="49"/>
       <c r="L18" s="32">
@@ -5247,13 +5290,13 @@
         <v>8</v>
       </c>
       <c r="U18" s="10" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="47"/>
       <c r="B19" s="33" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="D19" s="32">
         <v>1</v>
@@ -5268,7 +5311,7 @@
         <v>0</v>
       </c>
       <c r="H19" s="50" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="I19" s="50"/>
       <c r="J19" s="50"/>
@@ -5298,7 +5341,7 @@
         <v>0</v>
       </c>
       <c r="U19" s="10" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
@@ -5530,7 +5573,7 @@
   <dimension ref="A1:Q48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5548,13 +5591,13 @@
   <sheetData>
     <row r="1" spans="1:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="35" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B1" s="36">
         <v>1</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -5603,10 +5646,10 @@
         <v>0</v>
       </c>
       <c r="I3" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>284</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>288</v>
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3" t="s">
@@ -5660,7 +5703,7 @@
         <v>14</v>
       </c>
       <c r="M4" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="N4" t="s">
         <v>155</v>
@@ -5754,7 +5797,7 @@
         <v>74</v>
       </c>
       <c r="M6" t="s">
-        <v>94</v>
+        <v>411</v>
       </c>
       <c r="N6" t="s">
         <v>155</v>
@@ -5801,7 +5844,7 @@
         <v>75</v>
       </c>
       <c r="M7" t="s">
-        <v>95</v>
+        <v>412</v>
       </c>
       <c r="N7" t="s">
         <v>155</v>
@@ -5936,12 +5979,12 @@
         <v>155</v>
       </c>
       <c r="P10" s="19" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6">
@@ -5971,10 +6014,10 @@
         <v>3Eh</v>
       </c>
       <c r="L11" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="M11" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="P11" s="19" t="s">
         <v>184</v>
@@ -6015,7 +6058,7 @@
         <v>77</v>
       </c>
       <c r="M12" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="P12" s="19" t="s">
         <v>185</v>
@@ -7511,7 +7554,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="35" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B1" s="36">
         <v>1</v>
@@ -7559,10 +7602,10 @@
         <v>0</v>
       </c>
       <c r="H3" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>284</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>288</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3" t="s">
@@ -7607,7 +7650,7 @@
         <v>14</v>
       </c>
       <c r="L4" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="M4" t="s">
         <v>155</v>
@@ -7729,7 +7772,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B8" s="29"/>
       <c r="C8" s="29">
@@ -7756,10 +7799,10 @@
         <v>1Eh</v>
       </c>
       <c r="K8" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="L8" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -7794,7 +7837,7 @@
         <v>77</v>
       </c>
       <c r="L9" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -8348,8 +8391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8364,13 +8407,13 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="35" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B1" s="36">
         <v>2</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -8409,13 +8452,13 @@
         <v>196</v>
       </c>
       <c r="C4" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D4" t="s">
         <v>213</v>
       </c>
       <c r="E4" t="s">
-        <v>220</v>
+        <v>414</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -8423,13 +8466,13 @@
         <v>198</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D5" t="s">
         <v>213</v>
       </c>
       <c r="E5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -8437,13 +8480,13 @@
         <v>199</v>
       </c>
       <c r="C6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D6" t="s">
         <v>213</v>
       </c>
       <c r="E6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -8451,13 +8494,13 @@
         <v>201</v>
       </c>
       <c r="C7" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D7" t="s">
         <v>214</v>
       </c>
       <c r="E7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -8465,13 +8508,13 @@
         <v>202</v>
       </c>
       <c r="C8" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D8" t="s">
         <v>215</v>
       </c>
       <c r="E8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -8479,13 +8522,13 @@
         <v>203</v>
       </c>
       <c r="C9" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D9" t="s">
         <v>216</v>
       </c>
       <c r="E9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F9" t="s">
         <v>218</v>
@@ -8496,16 +8539,16 @@
         <v>211</v>
       </c>
       <c r="C10" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D10" t="s">
         <v>219</v>
       </c>
       <c r="E10" t="s">
+        <v>225</v>
+      </c>
+      <c r="F10" t="s">
         <v>226</v>
-      </c>
-      <c r="F10" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -8541,13 +8584,13 @@
         <v>206</v>
       </c>
       <c r="C13" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D13" t="s">
         <v>213</v>
       </c>
       <c r="E13" t="s">
-        <v>228</v>
+        <v>413</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -8555,13 +8598,13 @@
         <v>207</v>
       </c>
       <c r="C14" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D14" t="s">
         <v>213</v>
       </c>
       <c r="E14" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -8569,13 +8612,13 @@
         <v>208</v>
       </c>
       <c r="C15" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D15" t="s">
         <v>213</v>
       </c>
       <c r="E15" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -8583,13 +8626,13 @@
         <v>209</v>
       </c>
       <c r="C16" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D16" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="E16" t="s">
-        <v>231</v>
+        <v>415</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -8597,13 +8640,13 @@
         <v>210</v>
       </c>
       <c r="C17" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D17" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E17" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -8611,27 +8654,27 @@
         <v>212</v>
       </c>
       <c r="C18" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D18" t="s">
         <v>219</v>
       </c>
       <c r="E18" t="s">
-        <v>233</v>
+        <v>416</v>
       </c>
       <c r="F18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="35" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B19" s="36">
         <v>3</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -8657,18 +8700,18 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="26" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C21" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D21" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="35" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B22" s="36">
         <v>4</v>
@@ -8700,63 +8743,63 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C24" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D24" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="E24" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C25" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D25" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="E25" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="26" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C26" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D26" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="E26" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="26" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C27" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D27" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="E27" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="35" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B28" s="36">
         <v>5</v>
@@ -8788,60 +8831,60 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D30" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="E30" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="D31" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="E31" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="F31" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="26" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="D32" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="E32" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="26" t="s">
+        <v>306</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>313</v>
+      </c>
+      <c r="E33" t="s">
         <v>310</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>317</v>
-      </c>
-      <c r="E33" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="35" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B34" s="36">
         <v>6</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -8867,126 +8910,126 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="26" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C36" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="D36" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="E36" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="F36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="26" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C37" t="s">
+        <v>317</v>
+      </c>
+      <c r="D37" t="s">
+        <v>312</v>
+      </c>
+      <c r="E37" t="s">
         <v>321</v>
       </c>
-      <c r="D37" t="s">
-        <v>316</v>
-      </c>
-      <c r="E37" t="s">
-        <v>325</v>
-      </c>
       <c r="F37" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="26" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C38" t="s">
+        <v>318</v>
+      </c>
+      <c r="D38" t="s">
+        <v>312</v>
+      </c>
+      <c r="E38" t="s">
         <v>322</v>
       </c>
-      <c r="D38" t="s">
-        <v>316</v>
-      </c>
-      <c r="E38" t="s">
-        <v>326</v>
-      </c>
       <c r="F38" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="26" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C39" t="s">
+        <v>319</v>
+      </c>
+      <c r="D39" t="s">
+        <v>312</v>
+      </c>
+      <c r="E39" t="s">
         <v>323</v>
       </c>
-      <c r="D39" t="s">
-        <v>316</v>
-      </c>
-      <c r="E39" t="s">
-        <v>327</v>
-      </c>
       <c r="F39" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="26" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C40" t="s">
+        <v>320</v>
+      </c>
+      <c r="D40" t="s">
+        <v>312</v>
+      </c>
+      <c r="E40" t="s">
         <v>324</v>
       </c>
-      <c r="D40" t="s">
-        <v>316</v>
-      </c>
-      <c r="E40" t="s">
-        <v>328</v>
-      </c>
       <c r="F40" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="26" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C41" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D41" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="E41" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="26" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C42" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="D42" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="E42" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="35" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B43" s="36">
         <v>7</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -9012,13 +9055,13 @@
     </row>
     <row r="46" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="35" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B46" s="36">
         <v>8</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -9044,13 +9087,13 @@
     </row>
     <row r="49" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="35" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B49" s="36">
         <v>9</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
@@ -9076,13 +9119,13 @@
     </row>
     <row r="52" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="35" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B52" s="36">
         <v>10</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
@@ -9108,13 +9151,13 @@
     </row>
     <row r="55" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="35" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B55" s="36">
         <v>11</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
@@ -9140,7 +9183,7 @@
     </row>
     <row r="58" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="35" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B58" s="36">
         <v>12</v>
@@ -9177,10 +9220,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ46"/>
+  <dimension ref="A1:AJ47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AJ11" sqref="AJ11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9194,7 +9237,7 @@
   <sheetData>
     <row r="1" spans="1:36" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -9232,7 +9275,7 @@
     </row>
     <row r="2" spans="1:36" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="4" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9339,7 +9382,7 @@
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="39" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="C5" s="41">
         <v>0</v>
@@ -9424,12 +9467,12 @@
       <c r="AG5" s="52"/>
       <c r="AH5" s="52"/>
       <c r="AJ5" s="10" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="46" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="C6" s="43">
         <v>0</v>
@@ -9511,17 +9554,17 @@
       <c r="AD6" s="53"/>
       <c r="AE6" s="53"/>
       <c r="AF6" s="52" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="AG6" s="52"/>
       <c r="AH6" s="52"/>
       <c r="AJ6" s="10" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="46" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="C7" s="43">
         <v>0</v>
@@ -9596,7 +9639,7 @@
         <v>132</v>
       </c>
       <c r="AA7" s="63" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="AB7" s="64"/>
       <c r="AC7" s="64"/>
@@ -9606,12 +9649,12 @@
       <c r="AG7" s="64"/>
       <c r="AH7" s="65"/>
       <c r="AJ7" s="10" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="39" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C8" s="41">
         <v>0</v>
@@ -9638,19 +9681,19 @@
         <v>1</v>
       </c>
       <c r="K8" s="52" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="L8" s="52"/>
       <c r="M8" s="52"/>
       <c r="N8" s="52"/>
       <c r="O8" s="52"/>
       <c r="P8" s="52" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="Q8" s="52"/>
       <c r="R8" s="52"/>
       <c r="S8" s="52" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="T8" s="52"/>
       <c r="U8" s="52"/>
@@ -9670,7 +9713,7 @@
       <c r="AG8" s="52"/>
       <c r="AH8" s="52"/>
       <c r="AJ8" s="10" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.25">
@@ -9701,149 +9744,173 @@
       <c r="J9" s="6">
         <v>0</v>
       </c>
-      <c r="K9" s="48" t="s">
-        <v>411</v>
-      </c>
-      <c r="L9" s="48"/>
-      <c r="M9" s="48"/>
-      <c r="N9" s="48"/>
-      <c r="O9" s="48"/>
-      <c r="P9" s="48"/>
-      <c r="Q9" s="48"/>
-      <c r="R9" s="48"/>
-      <c r="S9" s="48"/>
-      <c r="T9" s="48"/>
-      <c r="U9" s="48"/>
-      <c r="V9" s="48"/>
-      <c r="W9" s="48"/>
-      <c r="X9" s="48"/>
-      <c r="Y9" s="48"/>
-      <c r="Z9" s="48"/>
-      <c r="AA9" s="48"/>
-      <c r="AB9" s="48"/>
-      <c r="AC9" s="48"/>
-      <c r="AD9" s="48"/>
-      <c r="AE9" s="48"/>
-      <c r="AF9" s="48"/>
-      <c r="AG9" s="48"/>
-      <c r="AH9" s="48"/>
+      <c r="K9" s="79" t="s">
+        <v>150</v>
+      </c>
+      <c r="L9" s="80"/>
+      <c r="M9" s="69" t="s">
+        <v>407</v>
+      </c>
+      <c r="N9" s="70"/>
+      <c r="O9" s="70"/>
+      <c r="P9" s="70"/>
+      <c r="Q9" s="70"/>
+      <c r="R9" s="70"/>
+      <c r="S9" s="70"/>
+      <c r="T9" s="70"/>
+      <c r="U9" s="70"/>
+      <c r="V9" s="70"/>
+      <c r="W9" s="70"/>
+      <c r="X9" s="70"/>
+      <c r="Y9" s="70"/>
+      <c r="Z9" s="70"/>
+      <c r="AA9" s="70"/>
+      <c r="AB9" s="70"/>
+      <c r="AC9" s="70"/>
+      <c r="AD9" s="70"/>
+      <c r="AE9" s="70"/>
+      <c r="AF9" s="70"/>
+      <c r="AG9" s="70"/>
+      <c r="AH9" s="71"/>
       <c r="AJ9" s="10" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
-      <c r="U10" s="5"/>
-      <c r="V10" s="5"/>
-      <c r="W10" s="5"/>
-      <c r="X10" s="5"/>
-      <c r="Y10" s="5"/>
-      <c r="Z10" s="5"/>
-      <c r="AA10" s="5"/>
-      <c r="AB10" s="5"/>
-      <c r="AC10" s="5"/>
-      <c r="AD10" s="5"/>
-      <c r="AE10" s="5"/>
-      <c r="AF10" s="5"/>
-      <c r="AG10" s="5"/>
-      <c r="AH10" s="5"/>
-      <c r="AJ10" s="10"/>
+      <c r="A10" s="46" t="s">
+        <v>408</v>
+      </c>
+      <c r="C10" s="44">
+        <v>0</v>
+      </c>
+      <c r="D10" s="44">
+        <v>0</v>
+      </c>
+      <c r="E10" s="44">
+        <v>0</v>
+      </c>
+      <c r="F10" s="44">
+        <v>0</v>
+      </c>
+      <c r="G10" s="45">
+        <v>0</v>
+      </c>
+      <c r="H10" s="45">
+        <v>1</v>
+      </c>
+      <c r="I10" s="45">
+        <v>0</v>
+      </c>
+      <c r="J10" s="69" t="s">
+        <v>409</v>
+      </c>
+      <c r="K10" s="70"/>
+      <c r="L10" s="71"/>
+      <c r="M10" s="69" t="s">
+        <v>407</v>
+      </c>
+      <c r="N10" s="70"/>
+      <c r="O10" s="70"/>
+      <c r="P10" s="70"/>
+      <c r="Q10" s="70"/>
+      <c r="R10" s="70"/>
+      <c r="S10" s="70"/>
+      <c r="T10" s="70"/>
+      <c r="U10" s="70"/>
+      <c r="V10" s="70"/>
+      <c r="W10" s="70"/>
+      <c r="X10" s="70"/>
+      <c r="Y10" s="70"/>
+      <c r="Z10" s="70"/>
+      <c r="AA10" s="70"/>
+      <c r="AB10" s="70"/>
+      <c r="AC10" s="70"/>
+      <c r="AD10" s="70"/>
+      <c r="AE10" s="70"/>
+      <c r="AF10" s="70"/>
+      <c r="AG10" s="70"/>
+      <c r="AH10" s="71"/>
+      <c r="AJ10" s="10" t="s">
+        <v>410</v>
+      </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>397</v>
-      </c>
-      <c r="C11" s="6">
-        <v>1</v>
-      </c>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
-      <c r="N11" s="48"/>
-      <c r="O11" s="48"/>
-      <c r="P11" s="48"/>
-      <c r="Q11" s="48"/>
-      <c r="R11" s="48"/>
-      <c r="S11" s="48"/>
-      <c r="T11" s="48"/>
-      <c r="U11" s="48"/>
-      <c r="V11" s="48"/>
-      <c r="W11" s="48"/>
-      <c r="X11" s="48"/>
-      <c r="Y11" s="48"/>
-      <c r="Z11" s="48"/>
-      <c r="AA11" s="48"/>
-      <c r="AB11" s="48"/>
-      <c r="AC11" s="48"/>
-      <c r="AD11" s="48"/>
-      <c r="AE11" s="48"/>
-      <c r="AF11" s="48"/>
-      <c r="AG11" s="48"/>
-      <c r="AH11" s="48"/>
-      <c r="AJ11" s="10" t="s">
-        <v>398</v>
-      </c>
+      <c r="A11" s="7"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+      <c r="Z11" s="5"/>
+      <c r="AA11" s="5"/>
+      <c r="AB11" s="5"/>
+      <c r="AC11" s="5"/>
+      <c r="AD11" s="5"/>
+      <c r="AE11" s="5"/>
+      <c r="AF11" s="5"/>
+      <c r="AG11" s="5"/>
+      <c r="AH11" s="5"/>
+      <c r="AJ11" s="10"/>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="5"/>
-      <c r="U12" s="5"/>
-      <c r="V12" s="5"/>
-      <c r="W12" s="5"/>
-      <c r="X12" s="5"/>
-      <c r="Y12" s="5"/>
-      <c r="Z12" s="5"/>
-      <c r="AA12" s="5"/>
-      <c r="AB12" s="5"/>
-      <c r="AC12" s="5"/>
-      <c r="AD12" s="5"/>
-      <c r="AE12" s="5"/>
-      <c r="AF12" s="5"/>
-      <c r="AG12" s="5"/>
-      <c r="AH12" s="5"/>
-      <c r="AJ12" s="10"/>
+      <c r="A12" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="C12" s="6">
+        <v>1</v>
+      </c>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="48"/>
+      <c r="M12" s="48"/>
+      <c r="N12" s="48"/>
+      <c r="O12" s="48"/>
+      <c r="P12" s="48"/>
+      <c r="Q12" s="48"/>
+      <c r="R12" s="48"/>
+      <c r="S12" s="48"/>
+      <c r="T12" s="48"/>
+      <c r="U12" s="48"/>
+      <c r="V12" s="48"/>
+      <c r="W12" s="48"/>
+      <c r="X12" s="48"/>
+      <c r="Y12" s="48"/>
+      <c r="Z12" s="48"/>
+      <c r="AA12" s="48"/>
+      <c r="AB12" s="48"/>
+      <c r="AC12" s="48"/>
+      <c r="AD12" s="48"/>
+      <c r="AE12" s="48"/>
+      <c r="AF12" s="48"/>
+      <c r="AG12" s="48"/>
+      <c r="AH12" s="48"/>
+      <c r="AJ12" s="10" t="s">
+        <v>394</v>
+      </c>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
@@ -9857,12 +9924,12 @@
       <c r="J13" s="6"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="6"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
       <c r="S13" s="5"/>
       <c r="T13" s="5"/>
       <c r="U13" s="5"/>
@@ -9888,17 +9955,17 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="12"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
       <c r="J14" s="6"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
       <c r="S14" s="5"/>
       <c r="T14" s="5"/>
       <c r="U14" s="5"/>
@@ -9924,36 +9991,34 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
       <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="6"/>
-      <c r="S15" s="6"/>
-      <c r="T15" s="6"/>
-      <c r="U15" s="6"/>
-      <c r="V15" s="6"/>
-      <c r="W15" s="6"/>
-      <c r="X15" s="6"/>
-      <c r="Y15" s="6"/>
-      <c r="Z15" s="6"/>
-      <c r="AA15" s="6"/>
-      <c r="AB15" s="6"/>
-      <c r="AC15" s="6"/>
-      <c r="AD15" s="6"/>
-      <c r="AE15" s="6"/>
-      <c r="AF15" s="6"/>
-      <c r="AG15" s="6"/>
-      <c r="AH15" s="6"/>
-      <c r="AJ15" s="10" t="s">
-        <v>410</v>
-      </c>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="5"/>
+      <c r="V15" s="5"/>
+      <c r="W15" s="5"/>
+      <c r="X15" s="5"/>
+      <c r="Y15" s="5"/>
+      <c r="Z15" s="5"/>
+      <c r="AA15" s="5"/>
+      <c r="AB15" s="5"/>
+      <c r="AC15" s="5"/>
+      <c r="AD15" s="5"/>
+      <c r="AE15" s="5"/>
+      <c r="AF15" s="5"/>
+      <c r="AG15" s="5"/>
+      <c r="AH15" s="5"/>
+      <c r="AJ15" s="10"/>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
@@ -9989,7 +10054,9 @@
       <c r="AF16" s="6"/>
       <c r="AG16" s="6"/>
       <c r="AH16" s="6"/>
-      <c r="AJ16" s="10"/>
+      <c r="AJ16" s="10" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
@@ -9997,12 +10064,12 @@
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
       <c r="J17" s="6"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
       <c r="M17" s="6"/>
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
@@ -10017,14 +10084,14 @@
       <c r="X17" s="6"/>
       <c r="Y17" s="6"/>
       <c r="Z17" s="6"/>
-      <c r="AA17" s="5"/>
-      <c r="AB17" s="5"/>
-      <c r="AC17" s="5"/>
-      <c r="AD17" s="5"/>
-      <c r="AE17" s="5"/>
-      <c r="AF17" s="5"/>
-      <c r="AG17" s="5"/>
-      <c r="AH17" s="5"/>
+      <c r="AA17" s="6"/>
+      <c r="AB17" s="6"/>
+      <c r="AC17" s="6"/>
+      <c r="AD17" s="6"/>
+      <c r="AE17" s="6"/>
+      <c r="AF17" s="6"/>
+      <c r="AG17" s="6"/>
+      <c r="AH17" s="6"/>
       <c r="AJ17" s="10"/>
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.25">
@@ -10089,14 +10156,14 @@
       <c r="X19" s="6"/>
       <c r="Y19" s="6"/>
       <c r="Z19" s="6"/>
-      <c r="AA19" s="6"/>
-      <c r="AB19" s="6"/>
-      <c r="AC19" s="6"/>
-      <c r="AD19" s="6"/>
-      <c r="AE19" s="6"/>
-      <c r="AF19" s="6"/>
-      <c r="AG19" s="6"/>
-      <c r="AH19" s="6"/>
+      <c r="AA19" s="5"/>
+      <c r="AB19" s="5"/>
+      <c r="AC19" s="5"/>
+      <c r="AD19" s="5"/>
+      <c r="AE19" s="5"/>
+      <c r="AF19" s="5"/>
+      <c r="AG19" s="5"/>
+      <c r="AH19" s="5"/>
       <c r="AJ19" s="10"/>
     </row>
     <row r="20" spans="1:36" x14ac:dyDescent="0.25">
@@ -10109,8 +10176,8 @@
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
       <c r="M20" s="6"/>
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
@@ -10125,93 +10192,92 @@
       <c r="X20" s="6"/>
       <c r="Y20" s="6"/>
       <c r="Z20" s="6"/>
-      <c r="AA20" s="5"/>
-      <c r="AB20" s="5"/>
-      <c r="AC20" s="5"/>
-      <c r="AD20" s="5"/>
-      <c r="AE20" s="5"/>
-      <c r="AF20" s="5"/>
-      <c r="AG20" s="5"/>
-      <c r="AH20" s="5"/>
+      <c r="AA20" s="6"/>
+      <c r="AB20" s="6"/>
+      <c r="AC20" s="6"/>
+      <c r="AD20" s="6"/>
+      <c r="AE20" s="6"/>
+      <c r="AF20" s="6"/>
+      <c r="AG20" s="6"/>
+      <c r="AH20" s="6"/>
+      <c r="AJ20" s="10"/>
     </row>
     <row r="21" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
       <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="6"/>
+      <c r="U21" s="6"/>
+      <c r="V21" s="6"/>
+      <c r="W21" s="6"/>
+      <c r="X21" s="6"/>
+      <c r="Y21" s="6"/>
+      <c r="Z21" s="6"/>
+      <c r="AA21" s="5"/>
+      <c r="AB21" s="5"/>
+      <c r="AC21" s="5"/>
+      <c r="AD21" s="5"/>
+      <c r="AE21" s="5"/>
+      <c r="AF21" s="5"/>
+      <c r="AG21" s="5"/>
+      <c r="AH21" s="5"/>
     </row>
     <row r="22" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
       <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
-      <c r="P22" s="6"/>
-      <c r="Q22" s="6"/>
-      <c r="R22" s="6"/>
-      <c r="S22" s="6"/>
-      <c r="T22" s="6"/>
-      <c r="U22" s="6"/>
-      <c r="V22" s="6"/>
-      <c r="W22" s="6"/>
-      <c r="X22" s="6"/>
-      <c r="Y22" s="6"/>
-      <c r="Z22" s="6"/>
-      <c r="AA22" s="6"/>
-      <c r="AB22" s="6"/>
-      <c r="AC22" s="6"/>
-      <c r="AD22" s="6"/>
-      <c r="AE22" s="6"/>
-      <c r="AF22" s="6"/>
-      <c r="AG22" s="6"/>
-      <c r="AH22" s="6"/>
-      <c r="AJ22" s="10"/>
     </row>
     <row r="23" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
       <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
+      <c r="T23" s="6"/>
+      <c r="U23" s="6"/>
+      <c r="V23" s="6"/>
+      <c r="W23" s="6"/>
+      <c r="X23" s="6"/>
+      <c r="Y23" s="6"/>
+      <c r="Z23" s="6"/>
+      <c r="AA23" s="6"/>
+      <c r="AB23" s="6"/>
+      <c r="AC23" s="6"/>
+      <c r="AD23" s="6"/>
+      <c r="AE23" s="6"/>
+      <c r="AF23" s="6"/>
+      <c r="AG23" s="6"/>
+      <c r="AH23" s="6"/>
+      <c r="AJ23" s="10"/>
     </row>
     <row r="24" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
       <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
-      <c r="N24" s="6"/>
-      <c r="O24" s="6"/>
-      <c r="P24" s="6"/>
-      <c r="Q24" s="6"/>
-      <c r="R24" s="6"/>
-      <c r="S24" s="6"/>
-      <c r="T24" s="6"/>
-      <c r="U24" s="6"/>
-      <c r="V24" s="6"/>
-      <c r="W24" s="6"/>
-      <c r="X24" s="6"/>
-      <c r="Y24" s="6"/>
-      <c r="Z24" s="6"/>
-      <c r="AA24" s="6"/>
-      <c r="AB24" s="6"/>
-      <c r="AC24" s="6"/>
-      <c r="AD24" s="6"/>
-      <c r="AE24" s="6"/>
-      <c r="AF24" s="6"/>
-      <c r="AG24" s="6"/>
-      <c r="AH24" s="6"/>
-      <c r="AJ24" s="10"/>
     </row>
     <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
@@ -10324,26 +10390,14 @@
       <c r="AH27" s="6"/>
       <c r="AJ27" s="10"/>
     </row>
-    <row r="28" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="9" t="s">
-        <v>360</v>
-      </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4">
-        <v>4</v>
-      </c>
-      <c r="D28" s="4">
-        <v>3</v>
-      </c>
-      <c r="E28" s="4">
-        <v>2</v>
-      </c>
-      <c r="F28" s="4">
-        <v>1</v>
-      </c>
-      <c r="G28" s="4">
-        <v>0</v>
-      </c>
+    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
@@ -10373,60 +10427,58 @@
       <c r="AH28" s="6"/>
       <c r="AJ28" s="10"/>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
-        <v>355</v>
-      </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="45">
-        <v>0</v>
-      </c>
-      <c r="D29" s="6">
-        <v>0</v>
-      </c>
-      <c r="E29" s="6">
-        <v>0</v>
-      </c>
-      <c r="F29" s="6">
-        <v>0</v>
-      </c>
-      <c r="G29" s="6">
+    <row r="29" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="9" t="s">
+        <v>356</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4">
+        <v>4</v>
+      </c>
+      <c r="D29" s="4">
+        <v>3</v>
+      </c>
+      <c r="E29" s="4">
+        <v>2</v>
+      </c>
+      <c r="F29" s="4">
+        <v>1</v>
+      </c>
+      <c r="G29" s="4">
         <v>0</v>
       </c>
       <c r="H29" s="6"/>
-      <c r="I29" s="5" t="s">
-        <v>364</v>
-      </c>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
-      <c r="O29" s="5"/>
-      <c r="P29" s="5"/>
-      <c r="Q29" s="5"/>
-      <c r="R29" s="5"/>
-      <c r="S29" s="5"/>
-      <c r="T29" s="5"/>
-      <c r="U29" s="5"/>
-      <c r="V29" s="5"/>
-      <c r="W29" s="5"/>
-      <c r="X29" s="5"/>
-      <c r="Y29" s="5"/>
-      <c r="Z29" s="5"/>
-      <c r="AA29" s="5"/>
-      <c r="AB29" s="5"/>
-      <c r="AC29" s="5"/>
-      <c r="AD29" s="5"/>
-      <c r="AE29" s="5"/>
-      <c r="AF29" s="5"/>
-      <c r="AG29" s="5"/>
-      <c r="AH29" s="5"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="6"/>
+      <c r="T29" s="6"/>
+      <c r="U29" s="6"/>
+      <c r="V29" s="6"/>
+      <c r="W29" s="6"/>
+      <c r="X29" s="6"/>
+      <c r="Y29" s="6"/>
+      <c r="Z29" s="6"/>
+      <c r="AA29" s="6"/>
+      <c r="AB29" s="6"/>
+      <c r="AC29" s="6"/>
+      <c r="AD29" s="6"/>
+      <c r="AE29" s="6"/>
+      <c r="AF29" s="6"/>
+      <c r="AG29" s="6"/>
+      <c r="AH29" s="6"/>
       <c r="AJ29" s="10"/>
     </row>
     <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="45">
@@ -10442,43 +10494,44 @@
         <v>0</v>
       </c>
       <c r="G30" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
-      <c r="M30" s="6"/>
-      <c r="N30" s="6"/>
-      <c r="O30" s="6"/>
-      <c r="P30" s="6"/>
-      <c r="Q30" s="6"/>
-      <c r="R30" s="6"/>
-      <c r="S30" s="6"/>
-      <c r="T30" s="6"/>
-      <c r="U30" s="6"/>
-      <c r="V30" s="6"/>
-      <c r="W30" s="6"/>
-      <c r="X30" s="6"/>
-      <c r="Y30" s="6"/>
-      <c r="Z30" s="6"/>
-      <c r="AA30" s="6"/>
-      <c r="AB30" s="6"/>
-      <c r="AC30" s="6"/>
-      <c r="AD30" s="6"/>
-      <c r="AE30" s="6"/>
-      <c r="AF30" s="6"/>
-      <c r="AG30" s="6"/>
-      <c r="AH30" s="6"/>
-      <c r="AJ30" s="10" t="s">
-        <v>373</v>
-      </c>
+      <c r="I30" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="5"/>
+      <c r="R30" s="5"/>
+      <c r="S30" s="5"/>
+      <c r="T30" s="5"/>
+      <c r="U30" s="5"/>
+      <c r="V30" s="5"/>
+      <c r="W30" s="5"/>
+      <c r="X30" s="5"/>
+      <c r="Y30" s="5"/>
+      <c r="Z30" s="5"/>
+      <c r="AA30" s="5"/>
+      <c r="AB30" s="5"/>
+      <c r="AC30" s="5"/>
+      <c r="AD30" s="5"/>
+      <c r="AE30" s="5"/>
+      <c r="AF30" s="5"/>
+      <c r="AG30" s="5"/>
+      <c r="AH30" s="5"/>
+      <c r="AJ30" s="10"/>
     </row>
     <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>366</v>
-      </c>
+        <v>361</v>
+      </c>
+      <c r="B31" s="6"/>
       <c r="C31" s="45">
         <v>0</v>
       </c>
@@ -10489,15 +10542,13 @@
         <v>0</v>
       </c>
       <c r="F31" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G31" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31" s="6"/>
-      <c r="I31" s="10" t="s">
-        <v>367</v>
-      </c>
+      <c r="I31" s="6"/>
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
       <c r="L31" s="6"/>
@@ -10523,11 +10574,13 @@
       <c r="AF31" s="6"/>
       <c r="AG31" s="6"/>
       <c r="AH31" s="6"/>
-      <c r="AJ31" s="10"/>
+      <c r="AJ31" s="10" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="C32" s="45">
         <v>0</v>
@@ -10542,11 +10595,11 @@
         <v>1</v>
       </c>
       <c r="G32" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H32" s="6"/>
       <c r="I32" s="10" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="J32" s="6"/>
       <c r="K32" s="6"/>
@@ -10577,7 +10630,7 @@
     </row>
     <row r="33" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="C33" s="45">
         <v>0</v>
@@ -10586,17 +10639,17 @@
         <v>0</v>
       </c>
       <c r="E33" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F33" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="10" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="J33" s="6"/>
       <c r="K33" s="6"/>
@@ -10623,13 +10676,11 @@
       <c r="AF33" s="6"/>
       <c r="AG33" s="6"/>
       <c r="AH33" s="6"/>
-      <c r="AJ33" s="10" t="s">
-        <v>372</v>
-      </c>
+      <c r="AJ33" s="10"/>
     </row>
     <row r="34" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>394</v>
+        <v>365</v>
       </c>
       <c r="C34" s="45">
         <v>0</v>
@@ -10644,11 +10695,11 @@
         <v>0</v>
       </c>
       <c r="G34" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="10" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="J34" s="6"/>
       <c r="K34" s="6"/>
@@ -10675,130 +10726,132 @@
       <c r="AF34" s="6"/>
       <c r="AG34" s="6"/>
       <c r="AH34" s="6"/>
-      <c r="AJ34" s="10"/>
+      <c r="AJ34" s="10" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="35" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A35" s="46" t="s">
-        <v>377</v>
+      <c r="A35" s="7" t="s">
+        <v>390</v>
       </c>
       <c r="C35" s="45">
         <v>0</v>
       </c>
-      <c r="D35" s="44">
-        <v>0</v>
-      </c>
-      <c r="E35" s="44">
-        <v>1</v>
-      </c>
-      <c r="F35" s="44">
-        <v>1</v>
-      </c>
-      <c r="G35" s="44">
-        <v>0</v>
-      </c>
-      <c r="H35" s="44"/>
+      <c r="D35" s="6">
+        <v>0</v>
+      </c>
+      <c r="E35" s="6">
+        <v>1</v>
+      </c>
+      <c r="F35" s="6">
+        <v>0</v>
+      </c>
+      <c r="G35" s="6">
+        <v>1</v>
+      </c>
+      <c r="H35" s="6"/>
       <c r="I35" s="10" t="s">
-        <v>374</v>
-      </c>
-      <c r="J35" s="44"/>
-      <c r="K35" s="44"/>
-      <c r="L35" s="44"/>
-      <c r="M35" s="44"/>
-      <c r="N35" s="44"/>
-      <c r="O35" s="44"/>
-      <c r="P35" s="44"/>
-      <c r="Q35" s="44"/>
-      <c r="R35" s="44"/>
-      <c r="S35" s="44"/>
-      <c r="T35" s="44"/>
-      <c r="U35" s="44"/>
-      <c r="V35" s="44"/>
-      <c r="W35" s="44"/>
-      <c r="X35" s="44"/>
-      <c r="Y35" s="44"/>
-      <c r="Z35" s="44"/>
-      <c r="AA35" s="44"/>
-      <c r="AB35" s="44"/>
-      <c r="AC35" s="44"/>
-      <c r="AD35" s="44"/>
-      <c r="AE35" s="44"/>
-      <c r="AF35" s="44"/>
-      <c r="AG35" s="44"/>
-      <c r="AH35" s="44"/>
+        <v>370</v>
+      </c>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="6"/>
+      <c r="O35" s="6"/>
+      <c r="P35" s="6"/>
+      <c r="Q35" s="6"/>
+      <c r="R35" s="6"/>
+      <c r="S35" s="6"/>
+      <c r="T35" s="6"/>
+      <c r="U35" s="6"/>
+      <c r="V35" s="6"/>
+      <c r="W35" s="6"/>
+      <c r="X35" s="6"/>
+      <c r="Y35" s="6"/>
+      <c r="Z35" s="6"/>
+      <c r="AA35" s="6"/>
+      <c r="AB35" s="6"/>
+      <c r="AC35" s="6"/>
+      <c r="AD35" s="6"/>
+      <c r="AE35" s="6"/>
+      <c r="AF35" s="6"/>
+      <c r="AG35" s="6"/>
+      <c r="AH35" s="6"/>
       <c r="AJ35" s="10"/>
     </row>
     <row r="36" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
-        <v>375</v>
+      <c r="A36" s="46" t="s">
+        <v>373</v>
       </c>
       <c r="C36" s="45">
         <v>0</v>
       </c>
-      <c r="D36" s="6">
-        <v>0</v>
-      </c>
-      <c r="E36" s="6">
-        <v>1</v>
-      </c>
-      <c r="F36" s="6">
-        <v>1</v>
-      </c>
-      <c r="G36" s="6">
-        <v>1</v>
-      </c>
-      <c r="H36" s="6"/>
+      <c r="D36" s="44">
+        <v>0</v>
+      </c>
+      <c r="E36" s="44">
+        <v>1</v>
+      </c>
+      <c r="F36" s="44">
+        <v>1</v>
+      </c>
+      <c r="G36" s="44">
+        <v>0</v>
+      </c>
+      <c r="H36" s="44"/>
       <c r="I36" s="10" t="s">
-        <v>376</v>
-      </c>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
-      <c r="L36" s="6"/>
-      <c r="M36" s="6"/>
-      <c r="N36" s="6"/>
-      <c r="O36" s="6"/>
-      <c r="P36" s="6"/>
-      <c r="Q36" s="6"/>
-      <c r="R36" s="6"/>
-      <c r="S36" s="6"/>
-      <c r="T36" s="6"/>
-      <c r="U36" s="6"/>
-      <c r="V36" s="6"/>
-      <c r="W36" s="6"/>
-      <c r="X36" s="6"/>
-      <c r="Y36" s="6"/>
-      <c r="Z36" s="6"/>
-      <c r="AA36" s="6"/>
-      <c r="AB36" s="6"/>
-      <c r="AC36" s="6"/>
-      <c r="AD36" s="6"/>
-      <c r="AE36" s="6"/>
-      <c r="AF36" s="6"/>
-      <c r="AG36" s="6"/>
-      <c r="AH36" s="6"/>
+        <v>370</v>
+      </c>
+      <c r="J36" s="44"/>
+      <c r="K36" s="44"/>
+      <c r="L36" s="44"/>
+      <c r="M36" s="44"/>
+      <c r="N36" s="44"/>
+      <c r="O36" s="44"/>
+      <c r="P36" s="44"/>
+      <c r="Q36" s="44"/>
+      <c r="R36" s="44"/>
+      <c r="S36" s="44"/>
+      <c r="T36" s="44"/>
+      <c r="U36" s="44"/>
+      <c r="V36" s="44"/>
+      <c r="W36" s="44"/>
+      <c r="X36" s="44"/>
+      <c r="Y36" s="44"/>
+      <c r="Z36" s="44"/>
+      <c r="AA36" s="44"/>
+      <c r="AB36" s="44"/>
+      <c r="AC36" s="44"/>
+      <c r="AD36" s="44"/>
+      <c r="AE36" s="44"/>
+      <c r="AF36" s="44"/>
+      <c r="AG36" s="44"/>
+      <c r="AH36" s="44"/>
       <c r="AJ36" s="10"/>
     </row>
     <row r="37" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="C37" s="45">
         <v>0</v>
       </c>
       <c r="D37" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E37" s="6">
-        <v>0</v>
-      </c>
-      <c r="F37" s="44">
-        <v>0</v>
-      </c>
-      <c r="G37" s="44">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F37" s="6">
+        <v>1</v>
+      </c>
+      <c r="G37" s="6">
+        <v>1</v>
       </c>
       <c r="H37" s="6"/>
-      <c r="I37" s="5" t="s">
-        <v>364</v>
+      <c r="I37" s="10" t="s">
+        <v>372</v>
       </c>
       <c r="J37" s="6"/>
       <c r="K37" s="6"/>
@@ -10829,7 +10882,7 @@
     </row>
     <row r="38" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="C38" s="45">
         <v>0</v>
@@ -10840,15 +10893,15 @@
       <c r="E38" s="6">
         <v>0</v>
       </c>
-      <c r="F38" s="6">
-        <v>0</v>
-      </c>
-      <c r="G38" s="6">
-        <v>1</v>
+      <c r="F38" s="44">
+        <v>0</v>
+      </c>
+      <c r="G38" s="44">
+        <v>0</v>
       </c>
       <c r="H38" s="6"/>
-      <c r="I38" s="10" t="s">
-        <v>393</v>
+      <c r="I38" s="5" t="s">
+        <v>360</v>
       </c>
       <c r="J38" s="6"/>
       <c r="K38" s="6"/>
@@ -10879,7 +10932,7 @@
     </row>
     <row r="39" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="C39" s="45">
         <v>0</v>
@@ -10891,14 +10944,14 @@
         <v>0</v>
       </c>
       <c r="F39" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G39" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="10" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="J39" s="6"/>
       <c r="K39" s="6"/>
@@ -10929,7 +10982,7 @@
     </row>
     <row r="40" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="C40" s="45">
         <v>0</v>
@@ -10944,11 +10997,11 @@
         <v>1</v>
       </c>
       <c r="G40" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H40" s="6"/>
       <c r="I40" s="10" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="J40" s="6"/>
       <c r="K40" s="6"/>
@@ -10975,33 +11028,60 @@
       <c r="AF40" s="6"/>
       <c r="AG40" s="6"/>
       <c r="AH40" s="6"/>
+      <c r="AJ40" s="10"/>
     </row>
     <row r="41" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="C41" s="45">
         <v>0</v>
       </c>
-      <c r="D41" s="44">
-        <v>1</v>
-      </c>
-      <c r="E41" s="44">
-        <v>1</v>
+      <c r="D41" s="6">
+        <v>1</v>
+      </c>
+      <c r="E41" s="6">
+        <v>0</v>
       </c>
       <c r="F41" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G41" s="6">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H41" s="6"/>
       <c r="I41" s="10" t="s">
-        <v>387</v>
-      </c>
+        <v>381</v>
+      </c>
+      <c r="J41" s="6"/>
+      <c r="K41" s="6"/>
+      <c r="L41" s="6"/>
+      <c r="M41" s="6"/>
+      <c r="N41" s="6"/>
+      <c r="O41" s="6"/>
+      <c r="P41" s="6"/>
+      <c r="Q41" s="6"/>
+      <c r="R41" s="6"/>
+      <c r="S41" s="6"/>
+      <c r="T41" s="6"/>
+      <c r="U41" s="6"/>
+      <c r="V41" s="6"/>
+      <c r="W41" s="6"/>
+      <c r="X41" s="6"/>
+      <c r="Y41" s="6"/>
+      <c r="Z41" s="6"/>
+      <c r="AA41" s="6"/>
+      <c r="AB41" s="6"/>
+      <c r="AC41" s="6"/>
+      <c r="AD41" s="6"/>
+      <c r="AE41" s="6"/>
+      <c r="AF41" s="6"/>
+      <c r="AG41" s="6"/>
+      <c r="AH41" s="6"/>
     </row>
     <row r="42" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A42" s="46" t="s">
-        <v>395</v>
+      <c r="A42" s="7" t="s">
+        <v>382</v>
       </c>
       <c r="C42" s="45">
         <v>0</v>
@@ -11012,116 +11092,113 @@
       <c r="E42" s="44">
         <v>1</v>
       </c>
-      <c r="F42" s="44">
-        <v>0</v>
-      </c>
-      <c r="G42" s="44">
-        <v>1</v>
-      </c>
-      <c r="I42" s="10"/>
+      <c r="F42" s="6">
+        <v>0</v>
+      </c>
+      <c r="G42" s="6">
+        <v>0</v>
+      </c>
+      <c r="I42" s="10" t="s">
+        <v>383</v>
+      </c>
     </row>
     <row r="43" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A43" s="7" t="s">
-        <v>378</v>
+      <c r="A43" s="46" t="s">
+        <v>391</v>
       </c>
       <c r="C43" s="45">
         <v>0</v>
       </c>
-      <c r="D43" s="6">
-        <v>1</v>
-      </c>
-      <c r="E43" s="6">
+      <c r="D43" s="44">
+        <v>1</v>
+      </c>
+      <c r="E43" s="44">
         <v>1</v>
       </c>
       <c r="F43" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G43" s="44">
-        <v>0</v>
-      </c>
-      <c r="H43" s="6"/>
-      <c r="I43" s="10" t="s">
-        <v>381</v>
-      </c>
-      <c r="J43" s="6"/>
-      <c r="K43" s="6"/>
-      <c r="L43" s="6"/>
-      <c r="M43" s="6"/>
-      <c r="N43" s="6"/>
-      <c r="O43" s="6"/>
-      <c r="P43" s="6"/>
-      <c r="Q43" s="6"/>
-      <c r="R43" s="6"/>
-      <c r="S43" s="6"/>
-      <c r="T43" s="6"/>
-      <c r="U43" s="6"/>
-      <c r="V43" s="6"/>
-      <c r="W43" s="6"/>
-      <c r="X43" s="6"/>
-      <c r="Y43" s="6"/>
-      <c r="Z43" s="6"/>
-      <c r="AA43" s="6"/>
-      <c r="AB43" s="6"/>
-      <c r="AC43" s="6"/>
-      <c r="AD43" s="6"/>
-      <c r="AE43" s="6"/>
-      <c r="AF43" s="6"/>
-      <c r="AG43" s="6"/>
-      <c r="AH43" s="6"/>
-      <c r="AJ43" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="I43" s="10"/>
     </row>
     <row r="44" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A44" s="46" t="s">
-        <v>391</v>
+      <c r="A44" s="7" t="s">
+        <v>374</v>
       </c>
       <c r="C44" s="45">
         <v>0</v>
       </c>
-      <c r="D44" s="44">
-        <v>1</v>
-      </c>
-      <c r="E44" s="44">
+      <c r="D44" s="6">
+        <v>1</v>
+      </c>
+      <c r="E44" s="6">
         <v>1</v>
       </c>
       <c r="F44" s="44">
         <v>1</v>
       </c>
       <c r="G44" s="44">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H44" s="6"/>
       <c r="I44" s="10" t="s">
-        <v>392</v>
-      </c>
+        <v>377</v>
+      </c>
+      <c r="J44" s="6"/>
+      <c r="K44" s="6"/>
+      <c r="L44" s="6"/>
+      <c r="M44" s="6"/>
+      <c r="N44" s="6"/>
+      <c r="O44" s="6"/>
+      <c r="P44" s="6"/>
+      <c r="Q44" s="6"/>
+      <c r="R44" s="6"/>
+      <c r="S44" s="6"/>
+      <c r="T44" s="6"/>
+      <c r="U44" s="6"/>
+      <c r="V44" s="6"/>
+      <c r="W44" s="6"/>
+      <c r="X44" s="6"/>
+      <c r="Y44" s="6"/>
+      <c r="Z44" s="6"/>
+      <c r="AA44" s="6"/>
+      <c r="AB44" s="6"/>
+      <c r="AC44" s="6"/>
+      <c r="AD44" s="6"/>
+      <c r="AE44" s="6"/>
+      <c r="AF44" s="6"/>
+      <c r="AG44" s="6"/>
+      <c r="AH44" s="6"/>
+      <c r="AJ44" s="10"/>
     </row>
     <row r="45" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A45" s="46" t="s">
-        <v>399</v>
+        <v>387</v>
       </c>
       <c r="C45" s="45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D45" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E45" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F45" s="44">
         <v>1</v>
       </c>
       <c r="G45" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I45" s="10" t="s">
-        <v>402</v>
-      </c>
-      <c r="AJ45" t="s">
-        <v>401</v>
+        <v>388</v>
       </c>
     </row>
     <row r="46" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A46" s="46" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="C46" s="45">
         <v>1</v>
@@ -11136,23 +11213,52 @@
         <v>1</v>
       </c>
       <c r="G46" s="44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I46" s="10" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="AJ46" t="s">
-        <v>401</v>
+        <v>397</v>
+      </c>
+    </row>
+    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A47" s="46" t="s">
+        <v>396</v>
+      </c>
+      <c r="C47" s="45">
+        <v>1</v>
+      </c>
+      <c r="D47" s="44">
+        <v>0</v>
+      </c>
+      <c r="E47" s="44">
+        <v>0</v>
+      </c>
+      <c r="F47" s="44">
+        <v>1</v>
+      </c>
+      <c r="G47" s="44">
+        <v>1</v>
+      </c>
+      <c r="I47" s="10" t="s">
+        <v>398</v>
+      </c>
+      <c r="AJ47" t="s">
+        <v>397</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="D11:AH11"/>
+  <mergeCells count="13">
+    <mergeCell ref="D12:AH12"/>
     <mergeCell ref="K8:O8"/>
     <mergeCell ref="AA6:AE6"/>
     <mergeCell ref="AF6:AH6"/>
     <mergeCell ref="AA7:AH7"/>
-    <mergeCell ref="K9:AH9"/>
+    <mergeCell ref="M9:AH9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M10:AH10"/>
+    <mergeCell ref="J10:L10"/>
     <mergeCell ref="AA5:AH5"/>
     <mergeCell ref="AA8:AH8"/>
     <mergeCell ref="P8:R8"/>
@@ -11181,7 +11287,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="62" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B1" s="62"/>
       <c r="C1" s="62"/>
@@ -11226,15 +11332,15 @@
         <v>0</v>
       </c>
       <c r="K3" s="38" t="s">
+        <v>280</v>
+      </c>
+      <c r="L3" s="38" t="s">
         <v>284</v>
-      </c>
-      <c r="L3" s="38" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C4" s="25">
         <v>0</v>
@@ -11271,7 +11377,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C5" s="25">
         <v>0</v>
@@ -11308,7 +11414,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C6" s="25">
         <v>0</v>
@@ -11345,7 +11451,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C7" s="25">
         <v>0</v>
@@ -11565,7 +11671,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="39" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="C4" s="41">
         <v>0</v>
@@ -11613,7 +11719,7 @@
         <v>0</v>
       </c>
       <c r="R4" s="41" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="T4" s="10" t="s">
         <v>130</v>
@@ -11677,7 +11783,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="39" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C6" s="40">
         <v>0</v>
@@ -11731,7 +11837,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="39" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C7" s="40">
         <v>0</v>
@@ -11770,7 +11876,7 @@
         <v>1</v>
       </c>
       <c r="O7" s="48" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="P7" s="48"/>
       <c r="Q7" s="48"/>
@@ -11939,7 +12045,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C12" s="6">
         <v>0</v>
@@ -11966,7 +12072,7 @@
         <v>0</v>
       </c>
       <c r="K12" s="48" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="L12" s="48"/>
       <c r="M12" s="48"/>

</xml_diff>

<commit_message>
new asm: special register write; loader can execute bytes in buffer
</commit_message>
<xml_diff>
--- a/doc/RiscyInstSet32Bit.xlsx
+++ b/doc/RiscyInstSet32Bit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25410" windowHeight="12690" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25410" windowHeight="12690"/>
   </bookViews>
   <sheets>
     <sheet name="Summary - Terra" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="441">
   <si>
     <t>Description</t>
   </si>
@@ -1020,9 +1020,6 @@
     <t>Unconditionally decrement program counter</t>
   </si>
   <si>
-    <t>Special Register MOV (SMOV)</t>
-  </si>
-  <si>
     <t>SpReg</t>
   </si>
   <si>
@@ -1345,6 +1342,18 @@
   </si>
   <si>
     <t>(TBA, likely be unimplemented, DO NOT USE!!!)</t>
+  </si>
+  <si>
+    <t>expecting offset, not actual address</t>
+  </si>
+  <si>
+    <t>Special Register Read (SRR)</t>
+  </si>
+  <si>
+    <t>Special Register Read (SRW)</t>
+  </si>
+  <si>
+    <t>Reg: 0-pc, 1-sp, 2-lr; operation is write-only</t>
   </si>
 </sst>
 </file>
@@ -1445,7 +1454,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -1659,6 +1668,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9"/>
@@ -1670,7 +1690,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="6" applyFont="1"/>
@@ -1798,6 +1818,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1839,12 +1865,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1907,6 +1927,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Explanatory Text" xfId="7" builtinId="53" customBuiltin="1"/>
@@ -2194,10 +2223,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL52"/>
+  <dimension ref="A1:AL53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AG13" sqref="AG13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2253,7 +2282,7 @@
     <row r="2" spans="1:38" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.25">
@@ -2262,7 +2291,7 @@
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -2305,7 +2334,7 @@
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -2348,7 +2377,7 @@
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -2534,7 +2563,7 @@
       </c>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A10" s="63">
+      <c r="A10" s="86">
         <v>1</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -2603,7 +2632,7 @@
         <v>0</v>
       </c>
       <c r="AD10" s="66" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AE10" s="66"/>
       <c r="AF10" s="66"/>
@@ -2615,15 +2644,15 @@
       </c>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A11" s="64"/>
+      <c r="A11" s="87"/>
       <c r="B11" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="D11" s="50" t="s">
+      <c r="D11" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
       <c r="G11" s="18">
         <v>0</v>
       </c>
@@ -2702,15 +2731,15 @@
       </c>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A12" s="64"/>
+      <c r="A12" s="87"/>
       <c r="B12" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D12" s="50" t="s">
+      <c r="D12" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
       <c r="G12" s="18">
         <v>0</v>
       </c>
@@ -2723,16 +2752,16 @@
       <c r="J12" s="18">
         <v>0</v>
       </c>
-      <c r="K12" s="62" t="s">
+      <c r="K12" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="L12" s="62"/>
-      <c r="M12" s="62"/>
-      <c r="N12" s="62" t="s">
+      <c r="L12" s="64"/>
+      <c r="M12" s="64"/>
+      <c r="N12" s="64" t="s">
         <v>149</v>
       </c>
-      <c r="O12" s="62"/>
-      <c r="P12" s="62"/>
+      <c r="O12" s="64"/>
+      <c r="P12" s="64"/>
       <c r="Q12" s="65" t="s">
         <v>150</v>
       </c>
@@ -2791,37 +2820,37 @@
       </c>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A13" s="64"/>
+      <c r="A13" s="87"/>
       <c r="B13" s="33" t="s">
+        <v>438</v>
+      </c>
+      <c r="D13" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="31">
+        <v>0</v>
+      </c>
+      <c r="H13" s="31">
+        <v>0</v>
+      </c>
+      <c r="I13" s="31">
+        <v>0</v>
+      </c>
+      <c r="J13" s="31">
+        <v>0</v>
+      </c>
+      <c r="K13" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="L13" s="60"/>
+      <c r="M13" s="60"/>
+      <c r="N13" s="60" t="s">
         <v>329</v>
       </c>
-      <c r="D13" s="50" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="31">
-        <v>0</v>
-      </c>
-      <c r="H13" s="31">
-        <v>0</v>
-      </c>
-      <c r="I13" s="31">
-        <v>0</v>
-      </c>
-      <c r="J13" s="31">
-        <v>0</v>
-      </c>
-      <c r="K13" s="58" t="s">
-        <v>5</v>
-      </c>
-      <c r="L13" s="58"/>
-      <c r="M13" s="58"/>
-      <c r="N13" s="58" t="s">
-        <v>330</v>
-      </c>
-      <c r="O13" s="58"/>
-      <c r="P13" s="58"/>
+      <c r="O13" s="60"/>
+      <c r="P13" s="60"/>
       <c r="Q13" s="65" t="s">
         <v>150</v>
       </c>
@@ -2857,122 +2886,129 @@
       <c r="AC13" s="29">
         <v>0</v>
       </c>
-      <c r="AD13" s="62" t="s">
-        <v>333</v>
-      </c>
-      <c r="AE13" s="62"/>
-      <c r="AF13" s="62"/>
-      <c r="AG13" s="62"/>
-      <c r="AH13" s="62"/>
-      <c r="AI13" s="62"/>
+      <c r="AD13" s="50">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="50">
+        <v>0</v>
+      </c>
+      <c r="AF13" s="50">
+        <v>0</v>
+      </c>
+      <c r="AG13" s="50">
+        <v>0</v>
+      </c>
+      <c r="AH13" s="50">
+        <v>0</v>
+      </c>
+      <c r="AI13" s="50">
+        <v>0</v>
+      </c>
       <c r="AK13" s="10" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>2</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="D14" s="50" t="s">
+      <c r="A14" s="88"/>
+      <c r="B14" s="47" t="s">
+        <v>439</v>
+      </c>
+      <c r="D14" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="6">
-        <v>0</v>
-      </c>
-      <c r="H14" s="12">
-        <v>0</v>
-      </c>
-      <c r="I14" s="12">
-        <v>0</v>
-      </c>
-      <c r="J14" s="12">
-        <v>0</v>
-      </c>
-      <c r="K14" s="58" t="s">
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="50">
+        <v>0</v>
+      </c>
+      <c r="H14" s="50">
+        <v>0</v>
+      </c>
+      <c r="I14" s="50">
+        <v>0</v>
+      </c>
+      <c r="J14" s="50">
+        <v>0</v>
+      </c>
+      <c r="K14" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="L14" s="58"/>
-      <c r="M14" s="58"/>
-      <c r="N14" s="58" t="s">
-        <v>9</v>
-      </c>
-      <c r="O14" s="58"/>
-      <c r="P14" s="58"/>
-      <c r="Q14" s="58" t="s">
-        <v>86</v>
-      </c>
-      <c r="R14" s="58"/>
-      <c r="S14" s="58"/>
-      <c r="T14" s="6">
-        <v>0</v>
-      </c>
-      <c r="U14" s="6">
-        <v>0</v>
-      </c>
-      <c r="V14" s="6">
-        <v>0</v>
-      </c>
-      <c r="W14" s="6">
-        <v>0</v>
-      </c>
-      <c r="X14" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z14" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA14" s="6">
-        <v>0</v>
-      </c>
-      <c r="AB14" s="6">
-        <v>0</v>
-      </c>
-      <c r="AC14" s="6">
-        <v>1</v>
-      </c>
-      <c r="AD14" s="6">
-        <v>0</v>
-      </c>
-      <c r="AE14" s="6">
-        <v>0</v>
-      </c>
-      <c r="AF14" s="6">
-        <v>0</v>
-      </c>
-      <c r="AG14" s="50" t="s">
-        <v>163</v>
-      </c>
-      <c r="AH14" s="50"/>
-      <c r="AI14" s="22" t="s">
-        <v>84</v>
+      <c r="L14" s="60"/>
+      <c r="M14" s="60"/>
+      <c r="N14" s="60" t="s">
+        <v>329</v>
+      </c>
+      <c r="O14" s="60"/>
+      <c r="P14" s="60"/>
+      <c r="Q14" s="65" t="s">
+        <v>150</v>
+      </c>
+      <c r="R14" s="65"/>
+      <c r="S14" s="65"/>
+      <c r="T14" s="49">
+        <v>0</v>
+      </c>
+      <c r="U14" s="48">
+        <v>0</v>
+      </c>
+      <c r="V14" s="48">
+        <v>0</v>
+      </c>
+      <c r="W14" s="48">
+        <v>0</v>
+      </c>
+      <c r="X14" s="48">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="48">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="48">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="48">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="48">
+        <v>1</v>
+      </c>
+      <c r="AC14" s="48">
+        <v>1</v>
+      </c>
+      <c r="AD14" s="50">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="50">
+        <v>0</v>
+      </c>
+      <c r="AF14" s="50">
+        <v>0</v>
+      </c>
+      <c r="AG14" s="50">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="50">
+        <v>0</v>
+      </c>
+      <c r="AI14" s="50">
+        <v>0</v>
       </c>
       <c r="AK14" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="AL14" s="2" t="s">
-        <v>162</v>
+        <v>440</v>
       </c>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="D15" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D15" s="50" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
       <c r="G15" s="6">
         <v>0</v>
       </c>
@@ -2985,31 +3021,39 @@
       <c r="J15" s="12">
         <v>0</v>
       </c>
-      <c r="K15" s="58" t="s">
+      <c r="K15" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="L15" s="58"/>
-      <c r="M15" s="58"/>
-      <c r="N15" s="58" t="s">
+      <c r="L15" s="60"/>
+      <c r="M15" s="60"/>
+      <c r="N15" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="O15" s="58"/>
-      <c r="P15" s="58"/>
-      <c r="Q15" s="58" t="s">
-        <v>124</v>
-      </c>
-      <c r="R15" s="58"/>
-      <c r="S15" s="58"/>
-      <c r="T15" s="58" t="s">
-        <v>165</v>
-      </c>
-      <c r="U15" s="58"/>
-      <c r="V15" s="58"/>
-      <c r="W15" s="58" t="s">
-        <v>166</v>
-      </c>
-      <c r="X15" s="58"/>
-      <c r="Y15" s="58"/>
+      <c r="O15" s="60"/>
+      <c r="P15" s="60"/>
+      <c r="Q15" s="60" t="s">
+        <v>86</v>
+      </c>
+      <c r="R15" s="60"/>
+      <c r="S15" s="60"/>
+      <c r="T15" s="6">
+        <v>0</v>
+      </c>
+      <c r="U15" s="6">
+        <v>0</v>
+      </c>
+      <c r="V15" s="6">
+        <v>0</v>
+      </c>
+      <c r="W15" s="6">
+        <v>0</v>
+      </c>
+      <c r="X15" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="6">
+        <v>0</v>
+      </c>
       <c r="Z15" s="6">
         <v>0</v>
       </c>
@@ -3029,256 +3073,277 @@
         <v>0</v>
       </c>
       <c r="AF15" s="6">
-        <v>1</v>
-      </c>
-      <c r="AG15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AH15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI15" s="6">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="AG15" s="52" t="s">
+        <v>163</v>
+      </c>
+      <c r="AH15" s="52"/>
+      <c r="AI15" s="22" t="s">
+        <v>84</v>
       </c>
       <c r="AK15" s="10" t="s">
-        <v>164</v>
+        <v>171</v>
+      </c>
+      <c r="AL15" s="2" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="6">
+        <v>0</v>
+      </c>
+      <c r="H16" s="12">
+        <v>0</v>
+      </c>
+      <c r="I16" s="12">
+        <v>0</v>
+      </c>
+      <c r="J16" s="12">
+        <v>0</v>
+      </c>
+      <c r="K16" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="L16" s="60"/>
+      <c r="M16" s="60"/>
+      <c r="N16" s="60" t="s">
+        <v>9</v>
+      </c>
+      <c r="O16" s="60"/>
+      <c r="P16" s="60"/>
+      <c r="Q16" s="60" t="s">
+        <v>124</v>
+      </c>
+      <c r="R16" s="60"/>
+      <c r="S16" s="60"/>
+      <c r="T16" s="60" t="s">
+        <v>165</v>
+      </c>
+      <c r="U16" s="60"/>
+      <c r="V16" s="60"/>
+      <c r="W16" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="X16" s="60"/>
+      <c r="Y16" s="60"/>
+      <c r="Z16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="6">
+        <v>1</v>
+      </c>
+      <c r="AD16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF16" s="6">
+        <v>1</v>
+      </c>
+      <c r="AG16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AK16" s="10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>4</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B17" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="D16" s="50" t="s">
+      <c r="D17" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="6">
-        <v>0</v>
-      </c>
-      <c r="H16" s="12">
-        <v>0</v>
-      </c>
-      <c r="I16" s="12">
-        <v>0</v>
-      </c>
-      <c r="J16" s="12">
-        <v>1</v>
-      </c>
-      <c r="K16" s="58" t="s">
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="6">
+        <v>0</v>
+      </c>
+      <c r="H17" s="12">
+        <v>0</v>
+      </c>
+      <c r="I17" s="12">
+        <v>0</v>
+      </c>
+      <c r="J17" s="12">
+        <v>1</v>
+      </c>
+      <c r="K17" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="L16" s="58"/>
-      <c r="M16" s="58"/>
-      <c r="N16" s="58" t="s">
+      <c r="L17" s="60"/>
+      <c r="M17" s="60"/>
+      <c r="N17" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="O16" s="58"/>
-      <c r="P16" s="58"/>
-      <c r="Q16" s="6">
-        <v>0</v>
-      </c>
-      <c r="R16" s="6">
-        <v>0</v>
-      </c>
-      <c r="S16" s="6">
-        <v>0</v>
-      </c>
-      <c r="T16" s="6">
-        <v>0</v>
-      </c>
-      <c r="U16" s="6">
-        <v>0</v>
-      </c>
-      <c r="V16" s="6">
-        <v>0</v>
-      </c>
-      <c r="W16" s="6">
-        <v>0</v>
-      </c>
-      <c r="X16" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y16" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z16" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA16" s="6">
-        <v>0</v>
-      </c>
-      <c r="AB16" s="6">
-        <v>0</v>
-      </c>
-      <c r="AC16" s="6">
-        <v>0</v>
-      </c>
-      <c r="AD16" s="6">
-        <v>0</v>
-      </c>
-      <c r="AE16" s="6">
-        <v>0</v>
-      </c>
-      <c r="AF16" s="6">
-        <v>0</v>
-      </c>
-      <c r="AG16" s="6">
-        <v>0</v>
-      </c>
-      <c r="AH16" s="22" t="s">
+      <c r="O17" s="60"/>
+      <c r="P17" s="60"/>
+      <c r="Q17" s="6">
+        <v>0</v>
+      </c>
+      <c r="R17" s="6">
+        <v>0</v>
+      </c>
+      <c r="S17" s="6">
+        <v>0</v>
+      </c>
+      <c r="T17" s="6">
+        <v>0</v>
+      </c>
+      <c r="U17" s="6">
+        <v>0</v>
+      </c>
+      <c r="V17" s="6">
+        <v>0</v>
+      </c>
+      <c r="W17" s="6">
+        <v>0</v>
+      </c>
+      <c r="X17" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD17" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE17" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF17" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG17" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH17" s="22" t="s">
         <v>167</v>
       </c>
-      <c r="AI16" s="22" t="s">
+      <c r="AI17" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="AK16" s="10" t="s">
+      <c r="AK17" s="10" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A17" s="70">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A18" s="70">
         <v>2</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B18" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="D17" s="50" t="s">
+      <c r="D18" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="6">
-        <v>0</v>
-      </c>
-      <c r="H17" s="12">
-        <v>0</v>
-      </c>
-      <c r="I17" s="12">
-        <v>0</v>
-      </c>
-      <c r="J17" s="12">
-        <v>1</v>
-      </c>
-      <c r="K17" s="58" t="s">
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="6">
+        <v>0</v>
+      </c>
+      <c r="H18" s="12">
+        <v>0</v>
+      </c>
+      <c r="I18" s="12">
+        <v>0</v>
+      </c>
+      <c r="J18" s="12">
+        <v>1</v>
+      </c>
+      <c r="K18" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="L17" s="58"/>
-      <c r="M17" s="58"/>
-      <c r="N17" s="58" t="s">
+      <c r="L18" s="60"/>
+      <c r="M18" s="60"/>
+      <c r="N18" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="O17" s="58"/>
-      <c r="P17" s="58"/>
-      <c r="Q17" s="6">
-        <v>0</v>
-      </c>
-      <c r="R17" s="6">
-        <v>1</v>
-      </c>
-      <c r="S17" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="T17" s="6">
-        <v>0</v>
-      </c>
-      <c r="U17" s="6">
-        <v>0</v>
-      </c>
-      <c r="V17" s="6">
-        <v>0</v>
-      </c>
-      <c r="W17" s="6">
-        <v>0</v>
-      </c>
-      <c r="X17" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y17" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z17" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA17" s="6">
-        <v>0</v>
-      </c>
-      <c r="AB17" s="58" t="s">
-        <v>147</v>
-      </c>
-      <c r="AC17" s="58"/>
-      <c r="AD17" s="58"/>
-      <c r="AE17" s="58"/>
-      <c r="AF17" s="58"/>
-      <c r="AG17" s="58"/>
-      <c r="AH17" s="58"/>
-      <c r="AI17" s="58"/>
-      <c r="AK17" s="10" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A18" s="70"/>
-      <c r="B18" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="D18" s="50" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" s="50"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="6">
-        <v>0</v>
-      </c>
-      <c r="H18" s="12">
-        <v>0</v>
-      </c>
-      <c r="I18" s="12">
-        <v>0</v>
-      </c>
-      <c r="J18" s="12">
-        <v>1</v>
-      </c>
-      <c r="K18" s="58" t="s">
-        <v>5</v>
-      </c>
-      <c r="L18" s="58"/>
-      <c r="M18" s="58"/>
-      <c r="N18" s="58" t="s">
-        <v>86</v>
-      </c>
-      <c r="O18" s="58"/>
-      <c r="P18" s="58"/>
+      <c r="O18" s="60"/>
+      <c r="P18" s="60"/>
       <c r="Q18" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R18" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S18" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="T18" s="58" t="s">
-        <v>145</v>
-      </c>
-      <c r="U18" s="58"/>
-      <c r="V18" s="58"/>
-      <c r="W18" s="58"/>
-      <c r="X18" s="58"/>
-      <c r="Y18" s="58"/>
-      <c r="Z18" s="58"/>
-      <c r="AA18" s="58"/>
-      <c r="AB18" s="58"/>
-      <c r="AC18" s="58"/>
-      <c r="AD18" s="58"/>
-      <c r="AE18" s="58"/>
-      <c r="AF18" s="58"/>
-      <c r="AG18" s="58"/>
-      <c r="AH18" s="58"/>
-      <c r="AI18" s="58"/>
+      <c r="T18" s="6">
+        <v>0</v>
+      </c>
+      <c r="U18" s="6">
+        <v>0</v>
+      </c>
+      <c r="V18" s="6">
+        <v>0</v>
+      </c>
+      <c r="W18" s="6">
+        <v>0</v>
+      </c>
+      <c r="X18" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="60" t="s">
+        <v>147</v>
+      </c>
+      <c r="AC18" s="60"/>
+      <c r="AD18" s="60"/>
+      <c r="AE18" s="60"/>
+      <c r="AF18" s="60"/>
+      <c r="AG18" s="60"/>
+      <c r="AH18" s="60"/>
+      <c r="AI18" s="60"/>
       <c r="AK18" s="10" t="s">
         <v>140</v>
       </c>
@@ -3286,13 +3351,13 @@
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" s="70"/>
       <c r="B19" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="D19" s="50" t="s">
+        <v>141</v>
+      </c>
+      <c r="D19" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="52"/>
       <c r="G19" s="6">
         <v>0</v>
       </c>
@@ -3305,516 +3370,494 @@
       <c r="J19" s="12">
         <v>1</v>
       </c>
-      <c r="K19" s="58" t="s">
+      <c r="K19" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="L19" s="58"/>
-      <c r="M19" s="58"/>
-      <c r="N19" s="58" t="s">
+      <c r="L19" s="60"/>
+      <c r="M19" s="60"/>
+      <c r="N19" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="O19" s="58"/>
-      <c r="P19" s="58"/>
+      <c r="O19" s="60"/>
+      <c r="P19" s="60"/>
       <c r="Q19" s="6">
         <v>1</v>
       </c>
       <c r="R19" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S19" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="T19" s="58" t="s">
-        <v>146</v>
-      </c>
-      <c r="U19" s="58"/>
-      <c r="V19" s="58"/>
-      <c r="W19" s="58"/>
-      <c r="X19" s="58"/>
-      <c r="Y19" s="58"/>
-      <c r="Z19" s="58"/>
-      <c r="AA19" s="58"/>
-      <c r="AB19" s="58"/>
-      <c r="AC19" s="58"/>
-      <c r="AD19" s="58"/>
-      <c r="AE19" s="58"/>
-      <c r="AF19" s="58"/>
-      <c r="AG19" s="58"/>
-      <c r="AH19" s="58"/>
-      <c r="AI19" s="58"/>
+      <c r="T19" s="60" t="s">
+        <v>145</v>
+      </c>
+      <c r="U19" s="60"/>
+      <c r="V19" s="60"/>
+      <c r="W19" s="60"/>
+      <c r="X19" s="60"/>
+      <c r="Y19" s="60"/>
+      <c r="Z19" s="60"/>
+      <c r="AA19" s="60"/>
+      <c r="AB19" s="60"/>
+      <c r="AC19" s="60"/>
+      <c r="AD19" s="60"/>
+      <c r="AE19" s="60"/>
+      <c r="AF19" s="60"/>
+      <c r="AG19" s="60"/>
+      <c r="AH19" s="60"/>
+      <c r="AI19" s="60"/>
       <c r="AK19" s="10" t="s">
-        <v>172</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" s="70"/>
       <c r="B20" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D20" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="52"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="6">
+        <v>0</v>
+      </c>
+      <c r="H20" s="12">
+        <v>0</v>
+      </c>
+      <c r="I20" s="12">
+        <v>0</v>
+      </c>
+      <c r="J20" s="12">
+        <v>1</v>
+      </c>
+      <c r="K20" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="L20" s="60"/>
+      <c r="M20" s="60"/>
+      <c r="N20" s="60" t="s">
+        <v>86</v>
+      </c>
+      <c r="O20" s="60"/>
+      <c r="P20" s="60"/>
+      <c r="Q20" s="6">
+        <v>1</v>
+      </c>
+      <c r="R20" s="6">
+        <v>1</v>
+      </c>
+      <c r="S20" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="T20" s="60" t="s">
+        <v>146</v>
+      </c>
+      <c r="U20" s="60"/>
+      <c r="V20" s="60"/>
+      <c r="W20" s="60"/>
+      <c r="X20" s="60"/>
+      <c r="Y20" s="60"/>
+      <c r="Z20" s="60"/>
+      <c r="AA20" s="60"/>
+      <c r="AB20" s="60"/>
+      <c r="AC20" s="60"/>
+      <c r="AD20" s="60"/>
+      <c r="AE20" s="60"/>
+      <c r="AF20" s="60"/>
+      <c r="AG20" s="60"/>
+      <c r="AH20" s="60"/>
+      <c r="AI20" s="60"/>
+      <c r="AK20" s="10" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A21" s="70"/>
+      <c r="B21" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="D20" s="50" t="s">
+      <c r="D21" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="50"/>
-      <c r="F20" s="50"/>
-      <c r="G20" s="6">
-        <v>0</v>
-      </c>
-      <c r="H20" s="12">
-        <v>0</v>
-      </c>
-      <c r="I20" s="12">
-        <v>1</v>
-      </c>
-      <c r="J20" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="K20" s="58" t="s">
-        <v>5</v>
-      </c>
-      <c r="L20" s="58"/>
-      <c r="M20" s="58"/>
-      <c r="N20" s="58" t="s">
-        <v>4</v>
-      </c>
-      <c r="O20" s="58"/>
-      <c r="P20" s="58"/>
-      <c r="Q20" s="58"/>
-      <c r="R20" s="58"/>
-      <c r="S20" s="58"/>
-      <c r="T20" s="58"/>
-      <c r="U20" s="58"/>
-      <c r="V20" s="58"/>
-      <c r="W20" s="58"/>
-      <c r="X20" s="58"/>
-      <c r="Y20" s="58"/>
-      <c r="Z20" s="58"/>
-      <c r="AA20" s="58"/>
-      <c r="AB20" s="58"/>
-      <c r="AC20" s="58"/>
-      <c r="AD20" s="58"/>
-      <c r="AE20" s="58"/>
-      <c r="AF20" s="58"/>
-      <c r="AG20" s="58"/>
-      <c r="AH20" s="58"/>
-      <c r="AI20" s="58"/>
-      <c r="AK20" s="10" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>5</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="50" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="52"/>
       <c r="G21" s="6">
         <v>0</v>
       </c>
       <c r="H21" s="12">
-        <v>1</v>
-      </c>
-      <c r="I21" s="42" t="s">
-        <v>8</v>
+        <v>0</v>
+      </c>
+      <c r="I21" s="12">
+        <v>1</v>
       </c>
       <c r="J21" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="K21" s="58" t="s">
+      <c r="K21" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="L21" s="58"/>
-      <c r="M21" s="58"/>
-      <c r="N21" s="58" t="s">
+      <c r="L21" s="60"/>
+      <c r="M21" s="60"/>
+      <c r="N21" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="O21" s="60"/>
+      <c r="P21" s="60"/>
+      <c r="Q21" s="60"/>
+      <c r="R21" s="60"/>
+      <c r="S21" s="60"/>
+      <c r="T21" s="60"/>
+      <c r="U21" s="60"/>
+      <c r="V21" s="60"/>
+      <c r="W21" s="60"/>
+      <c r="X21" s="60"/>
+      <c r="Y21" s="60"/>
+      <c r="Z21" s="60"/>
+      <c r="AA21" s="60"/>
+      <c r="AB21" s="60"/>
+      <c r="AC21" s="60"/>
+      <c r="AD21" s="60"/>
+      <c r="AE21" s="60"/>
+      <c r="AF21" s="60"/>
+      <c r="AG21" s="60"/>
+      <c r="AH21" s="60"/>
+      <c r="AI21" s="60"/>
+      <c r="AK21" s="10" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>5</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="52"/>
+      <c r="F22" s="52"/>
+      <c r="G22" s="6">
+        <v>0</v>
+      </c>
+      <c r="H22" s="12">
+        <v>1</v>
+      </c>
+      <c r="I22" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="J22" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="K22" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="L22" s="60"/>
+      <c r="M22" s="60"/>
+      <c r="N22" s="60" t="s">
         <v>169</v>
       </c>
-      <c r="O21" s="58"/>
-      <c r="P21" s="58"/>
-      <c r="Q21" s="58"/>
-      <c r="R21" s="58"/>
-      <c r="S21" s="58"/>
-      <c r="T21" s="58"/>
-      <c r="U21" s="58"/>
-      <c r="V21" s="58"/>
-      <c r="W21" s="58"/>
-      <c r="X21" s="58"/>
-      <c r="Y21" s="58"/>
-      <c r="Z21" s="58"/>
-      <c r="AA21" s="58"/>
-      <c r="AB21" s="58"/>
-      <c r="AC21" s="58"/>
-      <c r="AD21" s="58"/>
-      <c r="AE21" s="58"/>
-      <c r="AF21" s="58"/>
-      <c r="AG21" s="58"/>
-      <c r="AH21" s="58"/>
-      <c r="AI21" s="58"/>
-      <c r="AK21" s="10" t="s">
+      <c r="O22" s="60"/>
+      <c r="P22" s="60"/>
+      <c r="Q22" s="60"/>
+      <c r="R22" s="60"/>
+      <c r="S22" s="60"/>
+      <c r="T22" s="60"/>
+      <c r="U22" s="60"/>
+      <c r="V22" s="60"/>
+      <c r="W22" s="60"/>
+      <c r="X22" s="60"/>
+      <c r="Y22" s="60"/>
+      <c r="Z22" s="60"/>
+      <c r="AA22" s="60"/>
+      <c r="AB22" s="60"/>
+      <c r="AC22" s="60"/>
+      <c r="AD22" s="60"/>
+      <c r="AE22" s="60"/>
+      <c r="AF22" s="60"/>
+      <c r="AG22" s="60"/>
+      <c r="AH22" s="60"/>
+      <c r="AI22" s="60"/>
+      <c r="AK22" s="10" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A22" s="71">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A23" s="71">
         <v>6</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B23" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="D22" s="50" t="s">
+      <c r="D23" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="50"/>
-      <c r="F22" s="50"/>
-      <c r="G22" s="6">
-        <v>1</v>
-      </c>
-      <c r="H22" s="12">
-        <v>0</v>
-      </c>
-      <c r="I22" s="12">
-        <v>0</v>
-      </c>
-      <c r="J22" s="12">
-        <v>0</v>
-      </c>
-      <c r="K22" s="68" t="s">
+      <c r="E23" s="52"/>
+      <c r="F23" s="52"/>
+      <c r="G23" s="6">
+        <v>1</v>
+      </c>
+      <c r="H23" s="12">
+        <v>0</v>
+      </c>
+      <c r="I23" s="12">
+        <v>0</v>
+      </c>
+      <c r="J23" s="12">
+        <v>0</v>
+      </c>
+      <c r="K23" s="68" t="s">
         <v>150</v>
       </c>
-      <c r="L22" s="68"/>
-      <c r="M22" s="68"/>
-      <c r="N22" s="58" t="s">
+      <c r="L23" s="68"/>
+      <c r="M23" s="68"/>
+      <c r="N23" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="O22" s="58"/>
-      <c r="P22" s="58"/>
-      <c r="Q22" s="58"/>
-      <c r="R22" s="58"/>
-      <c r="S22" s="58"/>
-      <c r="T22" s="58"/>
-      <c r="U22" s="58"/>
-      <c r="V22" s="58"/>
-      <c r="W22" s="58"/>
-      <c r="X22" s="58"/>
-      <c r="Y22" s="58"/>
-      <c r="Z22" s="58"/>
-      <c r="AA22" s="58"/>
-      <c r="AB22" s="58"/>
-      <c r="AC22" s="58"/>
-      <c r="AD22" s="58"/>
-      <c r="AE22" s="58"/>
-      <c r="AF22" s="58"/>
-      <c r="AG22" s="58"/>
-      <c r="AH22" s="58"/>
-      <c r="AI22" s="58"/>
-      <c r="AK22" s="10" t="s">
+      <c r="O23" s="60"/>
+      <c r="P23" s="60"/>
+      <c r="Q23" s="60"/>
+      <c r="R23" s="60"/>
+      <c r="S23" s="60"/>
+      <c r="T23" s="60"/>
+      <c r="U23" s="60"/>
+      <c r="V23" s="60"/>
+      <c r="W23" s="60"/>
+      <c r="X23" s="60"/>
+      <c r="Y23" s="60"/>
+      <c r="Z23" s="60"/>
+      <c r="AA23" s="60"/>
+      <c r="AB23" s="60"/>
+      <c r="AC23" s="60"/>
+      <c r="AD23" s="60"/>
+      <c r="AE23" s="60"/>
+      <c r="AF23" s="60"/>
+      <c r="AG23" s="60"/>
+      <c r="AH23" s="60"/>
+      <c r="AI23" s="60"/>
+      <c r="AK23" s="10" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A23" s="72"/>
-      <c r="B23" s="46" t="s">
-        <v>405</v>
-      </c>
-      <c r="D23" s="50" t="s">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A24" s="72"/>
+      <c r="B24" s="46" t="s">
+        <v>404</v>
+      </c>
+      <c r="D24" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="50"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="44">
-        <v>1</v>
-      </c>
-      <c r="H23" s="45">
-        <v>0</v>
-      </c>
-      <c r="I23" s="45">
-        <v>0</v>
-      </c>
-      <c r="J23" s="45">
-        <v>1</v>
-      </c>
-      <c r="K23" s="55" t="s">
+      <c r="E24" s="52"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="44">
+        <v>1</v>
+      </c>
+      <c r="H24" s="45">
+        <v>0</v>
+      </c>
+      <c r="I24" s="45">
+        <v>0</v>
+      </c>
+      <c r="J24" s="45">
+        <v>1</v>
+      </c>
+      <c r="K24" s="57" t="s">
         <v>150</v>
       </c>
-      <c r="L23" s="56"/>
-      <c r="M23" s="57"/>
-      <c r="N23" s="58" t="s">
+      <c r="L24" s="58"/>
+      <c r="M24" s="59"/>
+      <c r="N24" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="O23" s="58"/>
-      <c r="P23" s="58"/>
-      <c r="Q23" s="58"/>
-      <c r="R23" s="58"/>
-      <c r="S23" s="58"/>
-      <c r="T23" s="58"/>
-      <c r="U23" s="58"/>
-      <c r="V23" s="58"/>
-      <c r="W23" s="58"/>
-      <c r="X23" s="58"/>
-      <c r="Y23" s="58"/>
-      <c r="Z23" s="58"/>
-      <c r="AA23" s="58"/>
-      <c r="AB23" s="58"/>
-      <c r="AC23" s="58"/>
-      <c r="AD23" s="58"/>
-      <c r="AE23" s="58"/>
-      <c r="AF23" s="58"/>
-      <c r="AG23" s="58"/>
-      <c r="AH23" s="58"/>
-      <c r="AI23" s="58"/>
-      <c r="AK23" s="10"/>
-    </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>7</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="D24" s="50" t="s">
-        <v>3</v>
-      </c>
-      <c r="E24" s="50"/>
-      <c r="F24" s="50"/>
-      <c r="G24" s="24">
-        <v>1</v>
-      </c>
-      <c r="H24" s="25">
-        <v>0</v>
-      </c>
-      <c r="I24" s="25">
-        <v>1</v>
-      </c>
-      <c r="J24" s="25">
-        <v>0</v>
-      </c>
-      <c r="K24" s="68" t="s">
-        <v>150</v>
-      </c>
-      <c r="L24" s="68"/>
-      <c r="M24" s="68"/>
-      <c r="N24" s="25">
-        <v>0</v>
-      </c>
-      <c r="O24" s="25">
-        <v>0</v>
-      </c>
-      <c r="P24" s="25">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="67" t="s">
-        <v>241</v>
-      </c>
-      <c r="R24" s="67"/>
-      <c r="S24" s="67"/>
-      <c r="T24" s="67"/>
-      <c r="U24" s="67"/>
-      <c r="V24" s="67"/>
-      <c r="W24" s="58" t="s">
-        <v>240</v>
-      </c>
-      <c r="X24" s="58"/>
-      <c r="Y24" s="58"/>
-      <c r="Z24" s="58"/>
-      <c r="AA24" s="58"/>
-      <c r="AB24" s="58"/>
-      <c r="AC24" s="58"/>
-      <c r="AD24" s="58"/>
-      <c r="AE24" s="58"/>
-      <c r="AF24" s="58"/>
-      <c r="AG24" s="58"/>
-      <c r="AH24" s="58"/>
-      <c r="AI24" s="58"/>
-      <c r="AK24" s="10" t="s">
-        <v>244</v>
-      </c>
+      <c r="O24" s="60"/>
+      <c r="P24" s="60"/>
+      <c r="Q24" s="60"/>
+      <c r="R24" s="60"/>
+      <c r="S24" s="60"/>
+      <c r="T24" s="60"/>
+      <c r="U24" s="60"/>
+      <c r="V24" s="60"/>
+      <c r="W24" s="60"/>
+      <c r="X24" s="60"/>
+      <c r="Y24" s="60"/>
+      <c r="Z24" s="60"/>
+      <c r="AA24" s="60"/>
+      <c r="AB24" s="60"/>
+      <c r="AC24" s="60"/>
+      <c r="AD24" s="60"/>
+      <c r="AE24" s="60"/>
+      <c r="AF24" s="60"/>
+      <c r="AG24" s="60"/>
+      <c r="AH24" s="60"/>
+      <c r="AI24" s="60"/>
+      <c r="AK24" s="10"/>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>8</v>
-      </c>
-      <c r="B25" s="46" t="s">
-        <v>246</v>
-      </c>
-      <c r="D25" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="D25" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="50"/>
-      <c r="F25" s="51"/>
-      <c r="G25" s="44">
-        <v>1</v>
-      </c>
-      <c r="H25" s="45">
-        <v>0</v>
-      </c>
-      <c r="I25" s="45">
-        <v>1</v>
-      </c>
-      <c r="J25" s="45">
-        <v>0</v>
-      </c>
-      <c r="K25" s="52" t="s">
-        <v>5</v>
-      </c>
-      <c r="L25" s="53"/>
-      <c r="M25" s="54"/>
-      <c r="N25" s="45">
-        <v>0</v>
-      </c>
-      <c r="O25" s="45">
-        <v>0</v>
-      </c>
-      <c r="P25" s="45">
-        <v>1</v>
-      </c>
-      <c r="Q25" s="45">
-        <v>0</v>
-      </c>
-      <c r="R25" s="45">
-        <v>0</v>
-      </c>
-      <c r="S25" s="44">
-        <v>0</v>
-      </c>
-      <c r="T25" s="44">
-        <v>0</v>
-      </c>
-      <c r="U25" s="44">
-        <v>0</v>
-      </c>
-      <c r="V25" s="44">
-        <v>0</v>
-      </c>
-      <c r="W25" s="44">
-        <v>0</v>
-      </c>
-      <c r="X25" s="44">
-        <v>0</v>
-      </c>
-      <c r="Y25" s="44">
-        <v>0</v>
-      </c>
-      <c r="Z25" s="44">
-        <v>0</v>
-      </c>
-      <c r="AA25" s="44">
-        <v>0</v>
-      </c>
-      <c r="AB25" s="59" t="s">
-        <v>243</v>
-      </c>
+      <c r="E25" s="52"/>
+      <c r="F25" s="52"/>
+      <c r="G25" s="24">
+        <v>1</v>
+      </c>
+      <c r="H25" s="25">
+        <v>0</v>
+      </c>
+      <c r="I25" s="25">
+        <v>1</v>
+      </c>
+      <c r="J25" s="25">
+        <v>0</v>
+      </c>
+      <c r="K25" s="68" t="s">
+        <v>150</v>
+      </c>
+      <c r="L25" s="68"/>
+      <c r="M25" s="68"/>
+      <c r="N25" s="25">
+        <v>0</v>
+      </c>
+      <c r="O25" s="25">
+        <v>0</v>
+      </c>
+      <c r="P25" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="67" t="s">
+        <v>241</v>
+      </c>
+      <c r="R25" s="67"/>
+      <c r="S25" s="67"/>
+      <c r="T25" s="67"/>
+      <c r="U25" s="67"/>
+      <c r="V25" s="67"/>
+      <c r="W25" s="60" t="s">
+        <v>240</v>
+      </c>
+      <c r="X25" s="60"/>
+      <c r="Y25" s="60"/>
+      <c r="Z25" s="60"/>
+      <c r="AA25" s="60"/>
+      <c r="AB25" s="60"/>
       <c r="AC25" s="60"/>
       <c r="AD25" s="60"/>
       <c r="AE25" s="60"/>
       <c r="AF25" s="60"/>
       <c r="AG25" s="60"/>
       <c r="AH25" s="60"/>
-      <c r="AI25" s="61"/>
+      <c r="AI25" s="60"/>
       <c r="AK25" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>9</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D26" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="46" t="s">
+        <v>246</v>
+      </c>
+      <c r="D26" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="E26" s="50"/>
-      <c r="F26" s="50"/>
-      <c r="G26" s="6">
-        <v>1</v>
-      </c>
-      <c r="H26" s="6">
-        <v>1</v>
-      </c>
-      <c r="I26" s="6">
-        <v>1</v>
-      </c>
-      <c r="J26" s="6">
-        <v>1</v>
-      </c>
-      <c r="K26" s="58" t="s">
+      <c r="E26" s="52"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="44">
+        <v>1</v>
+      </c>
+      <c r="H26" s="45">
+        <v>0</v>
+      </c>
+      <c r="I26" s="45">
+        <v>1</v>
+      </c>
+      <c r="J26" s="45">
+        <v>0</v>
+      </c>
+      <c r="K26" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="L26" s="58"/>
-      <c r="M26" s="58"/>
-      <c r="N26" s="6">
-        <v>0</v>
-      </c>
-      <c r="O26" s="6">
-        <v>0</v>
-      </c>
-      <c r="P26" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="6">
-        <v>0</v>
-      </c>
-      <c r="R26" s="6">
-        <v>0</v>
-      </c>
-      <c r="S26" s="6">
-        <v>0</v>
-      </c>
-      <c r="T26" s="6">
-        <v>0</v>
-      </c>
-      <c r="U26" s="6">
-        <v>0</v>
-      </c>
-      <c r="V26" s="6">
-        <v>0</v>
-      </c>
-      <c r="W26" s="6">
-        <v>0</v>
-      </c>
-      <c r="X26" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y26" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z26" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA26" s="6">
-        <v>0</v>
-      </c>
-      <c r="AB26" s="58" t="s">
-        <v>81</v>
-      </c>
-      <c r="AC26" s="58"/>
-      <c r="AD26" s="58"/>
-      <c r="AE26" s="58"/>
-      <c r="AF26" s="58"/>
-      <c r="AG26" s="58"/>
-      <c r="AH26" s="58"/>
-      <c r="AI26" s="58"/>
+      <c r="L26" s="55"/>
+      <c r="M26" s="56"/>
+      <c r="N26" s="45">
+        <v>0</v>
+      </c>
+      <c r="O26" s="45">
+        <v>0</v>
+      </c>
+      <c r="P26" s="45">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="45">
+        <v>0</v>
+      </c>
+      <c r="R26" s="45">
+        <v>0</v>
+      </c>
+      <c r="S26" s="44">
+        <v>0</v>
+      </c>
+      <c r="T26" s="44">
+        <v>0</v>
+      </c>
+      <c r="U26" s="44">
+        <v>0</v>
+      </c>
+      <c r="V26" s="44">
+        <v>0</v>
+      </c>
+      <c r="W26" s="44">
+        <v>0</v>
+      </c>
+      <c r="X26" s="44">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="44">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="44">
+        <v>0</v>
+      </c>
+      <c r="AA26" s="44">
+        <v>0</v>
+      </c>
+      <c r="AB26" s="61" t="s">
+        <v>243</v>
+      </c>
+      <c r="AC26" s="62"/>
+      <c r="AD26" s="62"/>
+      <c r="AE26" s="62"/>
+      <c r="AF26" s="62"/>
+      <c r="AG26" s="62"/>
+      <c r="AH26" s="62"/>
+      <c r="AI26" s="63"/>
       <c r="AK26" s="10" t="s">
-        <v>83</v>
+        <v>245</v>
       </c>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D27" s="50" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50"/>
+      <c r="E27" s="52"/>
+      <c r="F27" s="52"/>
       <c r="G27" s="6">
         <v>1</v>
       </c>
@@ -3827,11 +3870,11 @@
       <c r="J27" s="6">
         <v>1</v>
       </c>
-      <c r="K27" s="58" t="s">
+      <c r="K27" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="L27" s="58"/>
-      <c r="M27" s="58"/>
+      <c r="L27" s="60"/>
+      <c r="M27" s="60"/>
       <c r="N27" s="6">
         <v>0</v>
       </c>
@@ -3872,34 +3915,34 @@
         <v>0</v>
       </c>
       <c r="AA27" s="6">
-        <v>1</v>
-      </c>
-      <c r="AB27" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="AC27" s="58"/>
-      <c r="AD27" s="58"/>
-      <c r="AE27" s="58"/>
-      <c r="AF27" s="58"/>
-      <c r="AG27" s="58"/>
-      <c r="AH27" s="58"/>
-      <c r="AI27" s="58"/>
+      <c r="AC27" s="60"/>
+      <c r="AD27" s="60"/>
+      <c r="AE27" s="60"/>
+      <c r="AF27" s="60"/>
+      <c r="AG27" s="60"/>
+      <c r="AH27" s="60"/>
+      <c r="AI27" s="60"/>
       <c r="AK27" s="10" t="s">
-        <v>170</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D28" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
+      <c r="E28" s="52"/>
+      <c r="F28" s="52"/>
       <c r="G28" s="6">
         <v>1</v>
       </c>
@@ -3912,11 +3955,11 @@
       <c r="J28" s="6">
         <v>1</v>
       </c>
-      <c r="K28" s="58" t="s">
+      <c r="K28" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="L28" s="58"/>
-      <c r="M28" s="58"/>
+      <c r="L28" s="60"/>
+      <c r="M28" s="60"/>
       <c r="N28" s="6">
         <v>0</v>
       </c>
@@ -3959,154 +4002,202 @@
       <c r="AA28" s="6">
         <v>1</v>
       </c>
-      <c r="AB28" s="6">
-        <v>1</v>
-      </c>
-      <c r="AC28" s="6">
-        <v>1</v>
-      </c>
-      <c r="AD28" s="6">
-        <v>1</v>
-      </c>
-      <c r="AE28" s="6">
-        <v>1</v>
-      </c>
-      <c r="AF28" s="6">
-        <v>1</v>
-      </c>
-      <c r="AG28" s="6">
-        <v>1</v>
-      </c>
-      <c r="AH28" s="6">
-        <v>1</v>
-      </c>
-      <c r="AI28" s="6">
-        <v>1</v>
-      </c>
-      <c r="AK28" s="10"/>
+      <c r="AB28" s="60" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC28" s="60"/>
+      <c r="AD28" s="60"/>
+      <c r="AE28" s="60"/>
+      <c r="AF28" s="60"/>
+      <c r="AG28" s="60"/>
+      <c r="AH28" s="60"/>
+      <c r="AI28" s="60"/>
+      <c r="AK28" s="10" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29">
+        <v>11</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="52"/>
+      <c r="F29" s="52"/>
+      <c r="G29" s="6">
+        <v>1</v>
+      </c>
+      <c r="H29" s="6">
+        <v>1</v>
+      </c>
+      <c r="I29" s="6">
+        <v>1</v>
+      </c>
+      <c r="J29" s="6">
+        <v>1</v>
+      </c>
+      <c r="K29" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="L29" s="60"/>
+      <c r="M29" s="60"/>
+      <c r="N29" s="6">
+        <v>0</v>
+      </c>
+      <c r="O29" s="6">
+        <v>0</v>
+      </c>
+      <c r="P29" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="6">
+        <v>0</v>
+      </c>
+      <c r="R29" s="6">
+        <v>0</v>
+      </c>
+      <c r="S29" s="6">
+        <v>0</v>
+      </c>
+      <c r="T29" s="6">
+        <v>0</v>
+      </c>
+      <c r="U29" s="6">
+        <v>0</v>
+      </c>
+      <c r="V29" s="6">
+        <v>0</v>
+      </c>
+      <c r="W29" s="6">
+        <v>0</v>
+      </c>
+      <c r="X29" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z29" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA29" s="6">
+        <v>1</v>
+      </c>
+      <c r="AB29" s="6">
+        <v>1</v>
+      </c>
+      <c r="AC29" s="6">
+        <v>1</v>
+      </c>
+      <c r="AD29" s="6">
+        <v>1</v>
+      </c>
+      <c r="AE29" s="6">
+        <v>1</v>
+      </c>
+      <c r="AF29" s="6">
+        <v>1</v>
+      </c>
+      <c r="AG29" s="6">
+        <v>1</v>
+      </c>
+      <c r="AH29" s="6">
+        <v>1</v>
+      </c>
+      <c r="AI29" s="6">
+        <v>1</v>
+      </c>
+      <c r="AK29" s="10"/>
+    </row>
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>12</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B30" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D29" s="50" t="s">
+      <c r="D30" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="E29" s="50"/>
-      <c r="F29" s="50"/>
-      <c r="G29" s="6">
-        <v>1</v>
-      </c>
-      <c r="H29" s="6">
-        <v>1</v>
-      </c>
-      <c r="I29" s="6">
-        <v>1</v>
-      </c>
-      <c r="J29" s="6">
-        <v>1</v>
-      </c>
-      <c r="K29" s="6">
-        <v>1</v>
-      </c>
-      <c r="L29" s="6">
-        <v>1</v>
-      </c>
-      <c r="M29" s="6">
-        <v>1</v>
-      </c>
-      <c r="N29" s="6">
-        <v>1</v>
-      </c>
-      <c r="O29" s="6">
-        <v>1</v>
-      </c>
-      <c r="P29" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q29" s="6">
-        <v>1</v>
-      </c>
-      <c r="R29" s="6">
-        <v>1</v>
-      </c>
-      <c r="S29" s="6">
-        <v>1</v>
-      </c>
-      <c r="T29" s="6">
-        <v>1</v>
-      </c>
-      <c r="U29" s="6">
-        <v>1</v>
-      </c>
-      <c r="V29" s="6">
-        <v>1</v>
-      </c>
-      <c r="W29" s="6">
-        <v>1</v>
-      </c>
-      <c r="X29" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y29" s="6">
-        <v>1</v>
-      </c>
-      <c r="Z29" s="6">
-        <v>1</v>
-      </c>
-      <c r="AA29" s="6">
-        <v>1</v>
-      </c>
-      <c r="AB29" s="58" t="s">
+      <c r="E30" s="52"/>
+      <c r="F30" s="52"/>
+      <c r="G30" s="6">
+        <v>1</v>
+      </c>
+      <c r="H30" s="6">
+        <v>1</v>
+      </c>
+      <c r="I30" s="6">
+        <v>1</v>
+      </c>
+      <c r="J30" s="6">
+        <v>1</v>
+      </c>
+      <c r="K30" s="6">
+        <v>1</v>
+      </c>
+      <c r="L30" s="6">
+        <v>1</v>
+      </c>
+      <c r="M30" s="6">
+        <v>1</v>
+      </c>
+      <c r="N30" s="6">
+        <v>1</v>
+      </c>
+      <c r="O30" s="6">
+        <v>1</v>
+      </c>
+      <c r="P30" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="6">
+        <v>1</v>
+      </c>
+      <c r="R30" s="6">
+        <v>1</v>
+      </c>
+      <c r="S30" s="6">
+        <v>1</v>
+      </c>
+      <c r="T30" s="6">
+        <v>1</v>
+      </c>
+      <c r="U30" s="6">
+        <v>1</v>
+      </c>
+      <c r="V30" s="6">
+        <v>1</v>
+      </c>
+      <c r="W30" s="6">
+        <v>1</v>
+      </c>
+      <c r="X30" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y30" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z30" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA30" s="6">
+        <v>1</v>
+      </c>
+      <c r="AB30" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="AC29" s="58"/>
-      <c r="AD29" s="58"/>
-      <c r="AE29" s="58"/>
-      <c r="AF29" s="58"/>
-      <c r="AG29" s="58"/>
-      <c r="AH29" s="58"/>
-      <c r="AI29" s="58"/>
-    </row>
-    <row r="36" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B36" s="7"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
-      <c r="L36" s="6"/>
-      <c r="M36" s="6"/>
-      <c r="N36" s="6"/>
-      <c r="O36" s="6"/>
-      <c r="P36" s="6"/>
-      <c r="Q36" s="6"/>
-      <c r="R36" s="6"/>
-      <c r="S36" s="6"/>
-      <c r="T36" s="6"/>
-      <c r="U36" s="6"/>
-      <c r="V36" s="6"/>
-      <c r="W36" s="6"/>
-      <c r="X36" s="6"/>
-      <c r="Y36" s="6"/>
-      <c r="Z36" s="6"/>
-      <c r="AA36" s="6"/>
-      <c r="AB36" s="6"/>
-      <c r="AC36" s="6"/>
-      <c r="AD36" s="6"/>
-      <c r="AE36" s="6"/>
-      <c r="AF36" s="6"/>
-      <c r="AG36" s="6"/>
-      <c r="AH36" s="6"/>
-      <c r="AI36" s="6"/>
-      <c r="AK36" s="10"/>
+      <c r="AC30" s="60"/>
+      <c r="AD30" s="60"/>
+      <c r="AE30" s="60"/>
+      <c r="AF30" s="60"/>
+      <c r="AG30" s="60"/>
+      <c r="AH30" s="60"/>
+      <c r="AI30" s="60"/>
     </row>
     <row r="37" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B37" s="7"/>
@@ -4221,6 +4312,7 @@
     </row>
     <row r="40" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B40" s="7"/>
+      <c r="C40" s="6"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
@@ -4649,68 +4741,107 @@
       <c r="AG51" s="6"/>
       <c r="AH51" s="6"/>
       <c r="AI51" s="6"/>
+      <c r="AK51" s="10"/>
     </row>
     <row r="52" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B52" s="7"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="6"/>
+      <c r="K52" s="6"/>
+      <c r="L52" s="6"/>
+      <c r="M52" s="6"/>
+      <c r="N52" s="6"/>
+      <c r="O52" s="6"/>
+      <c r="P52" s="6"/>
+      <c r="Q52" s="6"/>
+      <c r="R52" s="6"/>
+      <c r="S52" s="6"/>
+      <c r="T52" s="6"/>
+      <c r="U52" s="6"/>
+      <c r="V52" s="6"/>
+      <c r="W52" s="6"/>
+      <c r="X52" s="6"/>
+      <c r="Y52" s="6"/>
+      <c r="Z52" s="6"/>
+      <c r="AA52" s="6"/>
+      <c r="AB52" s="6"/>
+      <c r="AC52" s="6"/>
+      <c r="AD52" s="6"/>
+      <c r="AE52" s="6"/>
+      <c r="AF52" s="6"/>
+      <c r="AG52" s="6"/>
+      <c r="AH52" s="6"/>
+      <c r="AI52" s="6"/>
+    </row>
+    <row r="53" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B53" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="75">
-    <mergeCell ref="A17:A20"/>
+  <mergeCells count="78">
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="Q14:S14"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="W25:AI25"/>
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="Q25:V25"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="AG15:AH15"/>
+    <mergeCell ref="W16:Y16"/>
+    <mergeCell ref="N18:P18"/>
     <mergeCell ref="N19:P19"/>
-    <mergeCell ref="W24:AI24"/>
-    <mergeCell ref="K24:M24"/>
-    <mergeCell ref="Q24:V24"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="AG14:AH14"/>
-    <mergeCell ref="W15:Y15"/>
-    <mergeCell ref="N17:P17"/>
-    <mergeCell ref="N18:P18"/>
     <mergeCell ref="K12:M12"/>
     <mergeCell ref="N12:P12"/>
     <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="AB17:AI17"/>
+    <mergeCell ref="AB18:AI18"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="N16:P16"/>
+    <mergeCell ref="Q16:S16"/>
+    <mergeCell ref="T16:V16"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="T19:AI19"/>
+    <mergeCell ref="AB30:AI30"/>
+    <mergeCell ref="N21:AI21"/>
+    <mergeCell ref="K21:M21"/>
     <mergeCell ref="K15:M15"/>
     <mergeCell ref="N15:P15"/>
     <mergeCell ref="Q15:S15"/>
-    <mergeCell ref="T15:V15"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="T18:AI18"/>
-    <mergeCell ref="AB29:AI29"/>
-    <mergeCell ref="N20:AI20"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="N14:P14"/>
-    <mergeCell ref="Q14:S14"/>
+    <mergeCell ref="N23:AI23"/>
     <mergeCell ref="N22:AI22"/>
-    <mergeCell ref="N21:AI21"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="K26:M26"/>
-    <mergeCell ref="T19:AI19"/>
     <mergeCell ref="K22:M22"/>
     <mergeCell ref="K27:M27"/>
-    <mergeCell ref="AB27:AI27"/>
+    <mergeCell ref="T20:AI20"/>
+    <mergeCell ref="K23:M23"/>
     <mergeCell ref="K28:M28"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="AB28:AI28"/>
+    <mergeCell ref="K29:M29"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D23:F23"/>
     <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D21:F21"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F15"/>
     <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D15:F15"/>
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D22:F22"/>
     <mergeCell ref="D27:F27"/>
     <mergeCell ref="D28:F28"/>
-    <mergeCell ref="AD13:AI13"/>
-    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="A10:A14"/>
     <mergeCell ref="D13:F13"/>
     <mergeCell ref="K13:M13"/>
     <mergeCell ref="N13:P13"/>
@@ -4719,17 +4850,17 @@
     <mergeCell ref="K10:M10"/>
     <mergeCell ref="N10:P10"/>
     <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="AB26:AI26"/>
+    <mergeCell ref="AB27:AI27"/>
     <mergeCell ref="K11:M11"/>
     <mergeCell ref="N11:S11"/>
-    <mergeCell ref="N16:P16"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="K25:M25"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="N23:AI23"/>
-    <mergeCell ref="AB25:AI25"/>
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="K26:M26"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="N24:AI24"/>
+    <mergeCell ref="AB26:AI26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4781,7 +4912,7 @@
     <row r="2" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -4790,7 +4921,7 @@
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -4817,7 +4948,7 @@
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -4844,7 +4975,7 @@
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -4868,7 +4999,7 @@
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -4886,7 +5017,7 @@
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
       <c r="U7" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4962,25 +5093,25 @@
       <c r="F10" s="29">
         <v>0</v>
       </c>
-      <c r="G10" s="58" t="s">
-        <v>334</v>
-      </c>
-      <c r="H10" s="58"/>
-      <c r="I10" s="58"/>
-      <c r="J10" s="58"/>
-      <c r="K10" s="58"/>
-      <c r="L10" s="58" t="s">
+      <c r="G10" s="60" t="s">
+        <v>333</v>
+      </c>
+      <c r="H10" s="60"/>
+      <c r="I10" s="60"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="60"/>
+      <c r="L10" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="M10" s="58"/>
-      <c r="N10" s="58" t="s">
+      <c r="M10" s="60"/>
+      <c r="N10" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="O10" s="58"/>
-      <c r="P10" s="58" t="s">
+      <c r="O10" s="60"/>
+      <c r="P10" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="Q10" s="58"/>
+      <c r="Q10" s="60"/>
       <c r="R10" s="29">
         <v>0</v>
       </c>
@@ -4993,7 +5124,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D11" s="32">
         <v>0</v>
@@ -5019,14 +5150,14 @@
       <c r="K11" s="32">
         <v>0</v>
       </c>
-      <c r="L11" s="58" t="s">
+      <c r="L11" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="M11" s="58"/>
-      <c r="N11" s="58" t="s">
+      <c r="M11" s="60"/>
+      <c r="N11" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="O11" s="58"/>
+      <c r="O11" s="60"/>
       <c r="P11" s="29">
         <v>0</v>
       </c>
@@ -5072,14 +5203,14 @@
       <c r="K12" s="32">
         <v>0</v>
       </c>
-      <c r="L12" s="58" t="s">
+      <c r="L12" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="M12" s="58"/>
-      <c r="N12" s="58" t="s">
+      <c r="M12" s="60"/>
+      <c r="N12" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="O12" s="58"/>
+      <c r="O12" s="60"/>
       <c r="P12" s="32">
         <v>1</v>
       </c>
@@ -5266,7 +5397,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D17" s="32">
         <v>1</v>
@@ -5281,11 +5412,11 @@
         <v>0</v>
       </c>
       <c r="H17" s="67" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="I17" s="67"/>
       <c r="J17" s="67" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="K17" s="67"/>
       <c r="L17" s="32">
@@ -5313,13 +5444,13 @@
         <v>8</v>
       </c>
       <c r="U17" s="10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="70"/>
       <c r="B18" s="33" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D18" s="32">
         <v>1</v>
@@ -5334,11 +5465,11 @@
         <v>0</v>
       </c>
       <c r="H18" s="67" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="I18" s="67"/>
       <c r="J18" s="67" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="K18" s="67"/>
       <c r="L18" s="32">
@@ -5366,13 +5497,13 @@
         <v>8</v>
       </c>
       <c r="U18" s="10" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="70"/>
       <c r="B19" s="33" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D19" s="32">
         <v>1</v>
@@ -5387,7 +5518,7 @@
         <v>0</v>
       </c>
       <c r="H19" s="68" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="I19" s="68"/>
       <c r="J19" s="68"/>
@@ -5417,7 +5548,7 @@
         <v>0</v>
       </c>
       <c r="U19" s="10" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
@@ -5648,8 +5779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5660,7 +5791,7 @@
     <col min="9" max="10" width="6" customWidth="1"/>
     <col min="11" max="11" width="2.5703125" customWidth="1"/>
     <col min="13" max="13" width="45.7109375" customWidth="1"/>
-    <col min="15" max="15" width="3.42578125" customWidth="1"/>
+    <col min="15" max="15" width="39.28515625" customWidth="1"/>
     <col min="16" max="16" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -5873,7 +6004,7 @@
         <v>74</v>
       </c>
       <c r="M6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="N6" t="s">
         <v>155</v>
@@ -5920,7 +6051,7 @@
         <v>75</v>
       </c>
       <c r="M7" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="N7" t="s">
         <v>155</v>
@@ -5972,7 +6103,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="83" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B9" s="84"/>
       <c r="C9" s="84">
@@ -6003,10 +6134,10 @@
       </c>
       <c r="K9" s="85"/>
       <c r="L9" s="85" t="s">
+        <v>435</v>
+      </c>
+      <c r="M9" s="85" t="s">
         <v>436</v>
-      </c>
-      <c r="M9" s="85" t="s">
-        <v>437</v>
       </c>
       <c r="N9" s="85"/>
     </row>
@@ -6100,7 +6231,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="47" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B12" s="48"/>
       <c r="C12" s="48">
@@ -6130,21 +6261,24 @@
         <v>38h</v>
       </c>
       <c r="L12" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="M12" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="N12" t="s">
         <v>155</v>
       </c>
+      <c r="O12" t="s">
+        <v>437</v>
+      </c>
       <c r="P12" s="19" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="47" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B13" s="48"/>
       <c r="C13" s="48">
@@ -6174,10 +6308,13 @@
         <v>39h</v>
       </c>
       <c r="L13" t="s">
+        <v>419</v>
+      </c>
+      <c r="M13" t="s">
         <v>420</v>
       </c>
-      <c r="M13" t="s">
-        <v>421</v>
+      <c r="O13" t="s">
+        <v>437</v>
       </c>
       <c r="P13" s="19" t="s">
         <v>185</v>
@@ -6185,7 +6322,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="47" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B14" s="48"/>
       <c r="C14" s="48">
@@ -6215,18 +6352,21 @@
         <v>3Ah</v>
       </c>
       <c r="L14" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="M14" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="N14" t="s">
         <v>156</v>
       </c>
+      <c r="O14" t="s">
+        <v>437</v>
+      </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="47" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B15" s="48"/>
       <c r="C15" s="48">
@@ -6256,15 +6396,18 @@
         <v>3Bh</v>
       </c>
       <c r="L15" t="s">
+        <v>424</v>
+      </c>
+      <c r="M15" t="s">
         <v>425</v>
       </c>
-      <c r="M15" t="s">
-        <v>426</v>
+      <c r="O15" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="47" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B16" s="48"/>
       <c r="C16" s="48">
@@ -6294,18 +6437,21 @@
         <v>3Ch</v>
       </c>
       <c r="L16" t="s">
+        <v>429</v>
+      </c>
+      <c r="M16" t="s">
         <v>430</v>
-      </c>
-      <c r="M16" t="s">
-        <v>431</v>
       </c>
       <c r="N16" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O16" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="47" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B17" s="48"/>
       <c r="C17" s="48">
@@ -6335,13 +6481,16 @@
         <v>3Dh</v>
       </c>
       <c r="L17" t="s">
+        <v>432</v>
+      </c>
+      <c r="M17" t="s">
         <v>433</v>
       </c>
-      <c r="M17" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O17" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>289</v>
       </c>
@@ -6379,7 +6528,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>76</v>
       </c>
@@ -6417,7 +6566,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>17</v>
       </c>
@@ -6458,7 +6607,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>18</v>
       </c>
@@ -6499,7 +6648,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>19</v>
       </c>
@@ -6540,7 +6689,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>20</v>
       </c>
@@ -6581,7 +6730,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>21</v>
       </c>
@@ -6622,7 +6771,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>22</v>
       </c>
@@ -6663,7 +6812,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="33" t="str">
         <f>A20&amp;" integer"</f>
         <v>Add integer</v>
@@ -6707,7 +6856,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="str">
         <f t="shared" ref="A27:A31" si="4">A21&amp;" integer"</f>
         <v>Subtract integer</v>
@@ -6751,7 +6900,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="33" t="str">
         <f t="shared" si="4"/>
         <v>Multiply integer</v>
@@ -6795,7 +6944,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="33" t="str">
         <f t="shared" si="4"/>
         <v>Divide integer</v>
@@ -6839,7 +6988,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="33" t="str">
         <f t="shared" si="4"/>
         <v>Powerof integer</v>
@@ -6883,7 +7032,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="33" t="str">
         <f t="shared" si="4"/>
         <v>Modulo integer</v>
@@ -6927,7 +7076,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>23</v>
       </c>
@@ -8811,7 +8960,7 @@
         <v>213</v>
       </c>
       <c r="E4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -8943,7 +9092,7 @@
         <v>213</v>
       </c>
       <c r="E13" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -8985,7 +9134,7 @@
         <v>233</v>
       </c>
       <c r="E16" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -9013,7 +9162,7 @@
         <v>219</v>
       </c>
       <c r="E18" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F18" t="s">
         <v>226</v>
@@ -9576,7 +9725,7 @@
   <dimension ref="A1:AJ47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AJ11" sqref="AJ11"/>
+      <selection activeCell="G9" sqref="G9:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9590,7 +9739,7 @@
   <sheetData>
     <row r="1" spans="1:36" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -9628,7 +9777,7 @@
     </row>
     <row r="2" spans="1:36" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="4" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9735,7 +9884,7 @@
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="39" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C5" s="41">
         <v>0</v>
@@ -9809,23 +9958,23 @@
       <c r="Z5" s="41">
         <v>0</v>
       </c>
-      <c r="AA5" s="62" t="s">
+      <c r="AA5" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="AB5" s="62"/>
-      <c r="AC5" s="62"/>
-      <c r="AD5" s="62"/>
-      <c r="AE5" s="62"/>
-      <c r="AF5" s="62"/>
-      <c r="AG5" s="62"/>
-      <c r="AH5" s="62"/>
+      <c r="AB5" s="64"/>
+      <c r="AC5" s="64"/>
+      <c r="AD5" s="64"/>
+      <c r="AE5" s="64"/>
+      <c r="AF5" s="64"/>
+      <c r="AG5" s="64"/>
+      <c r="AH5" s="64"/>
       <c r="AJ5" s="10" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="46" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C6" s="43">
         <v>0</v>
@@ -9906,18 +10055,18 @@
       <c r="AC6" s="65"/>
       <c r="AD6" s="65"/>
       <c r="AE6" s="65"/>
-      <c r="AF6" s="62" t="s">
-        <v>358</v>
-      </c>
-      <c r="AG6" s="62"/>
-      <c r="AH6" s="62"/>
+      <c r="AF6" s="64" t="s">
+        <v>357</v>
+      </c>
+      <c r="AG6" s="64"/>
+      <c r="AH6" s="64"/>
       <c r="AJ6" s="10" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="46" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C7" s="43">
         <v>0</v>
@@ -9992,7 +10141,7 @@
         <v>132</v>
       </c>
       <c r="AA7" s="77" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AB7" s="78"/>
       <c r="AC7" s="78"/>
@@ -10002,12 +10151,12 @@
       <c r="AG7" s="78"/>
       <c r="AH7" s="79"/>
       <c r="AJ7" s="10" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="39" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C8" s="41">
         <v>0</v>
@@ -10033,40 +10182,40 @@
       <c r="J8" s="41">
         <v>1</v>
       </c>
-      <c r="K8" s="62" t="s">
+      <c r="K8" s="64" t="s">
+        <v>356</v>
+      </c>
+      <c r="L8" s="64"/>
+      <c r="M8" s="64"/>
+      <c r="N8" s="64"/>
+      <c r="O8" s="64"/>
+      <c r="P8" s="64" t="s">
         <v>357</v>
       </c>
-      <c r="L8" s="62"/>
-      <c r="M8" s="62"/>
-      <c r="N8" s="62"/>
-      <c r="O8" s="62"/>
-      <c r="P8" s="62" t="s">
+      <c r="Q8" s="64"/>
+      <c r="R8" s="64"/>
+      <c r="S8" s="64" t="s">
         <v>358</v>
       </c>
-      <c r="Q8" s="62"/>
-      <c r="R8" s="62"/>
-      <c r="S8" s="62" t="s">
-        <v>359</v>
-      </c>
-      <c r="T8" s="62"/>
-      <c r="U8" s="62"/>
-      <c r="V8" s="62"/>
-      <c r="W8" s="62"/>
-      <c r="X8" s="62"/>
-      <c r="Y8" s="62"/>
-      <c r="Z8" s="62"/>
-      <c r="AA8" s="62" t="s">
+      <c r="T8" s="64"/>
+      <c r="U8" s="64"/>
+      <c r="V8" s="64"/>
+      <c r="W8" s="64"/>
+      <c r="X8" s="64"/>
+      <c r="Y8" s="64"/>
+      <c r="Z8" s="64"/>
+      <c r="AA8" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="AB8" s="62"/>
-      <c r="AC8" s="62"/>
-      <c r="AD8" s="62"/>
-      <c r="AE8" s="62"/>
-      <c r="AF8" s="62"/>
-      <c r="AG8" s="62"/>
-      <c r="AH8" s="62"/>
+      <c r="AB8" s="64"/>
+      <c r="AC8" s="64"/>
+      <c r="AD8" s="64"/>
+      <c r="AE8" s="64"/>
+      <c r="AF8" s="64"/>
+      <c r="AG8" s="64"/>
+      <c r="AH8" s="64"/>
       <c r="AJ8" s="10" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.25">
@@ -10101,90 +10250,90 @@
         <v>150</v>
       </c>
       <c r="L9" s="81"/>
-      <c r="M9" s="59" t="s">
-        <v>407</v>
-      </c>
-      <c r="N9" s="60"/>
-      <c r="O9" s="60"/>
-      <c r="P9" s="60"/>
-      <c r="Q9" s="60"/>
-      <c r="R9" s="60"/>
-      <c r="S9" s="60"/>
-      <c r="T9" s="60"/>
-      <c r="U9" s="60"/>
-      <c r="V9" s="60"/>
-      <c r="W9" s="60"/>
-      <c r="X9" s="60"/>
-      <c r="Y9" s="60"/>
-      <c r="Z9" s="60"/>
-      <c r="AA9" s="60"/>
-      <c r="AB9" s="60"/>
-      <c r="AC9" s="60"/>
-      <c r="AD9" s="60"/>
-      <c r="AE9" s="60"/>
-      <c r="AF9" s="60"/>
-      <c r="AG9" s="60"/>
-      <c r="AH9" s="61"/>
+      <c r="M9" s="61" t="s">
+        <v>406</v>
+      </c>
+      <c r="N9" s="62"/>
+      <c r="O9" s="62"/>
+      <c r="P9" s="62"/>
+      <c r="Q9" s="62"/>
+      <c r="R9" s="62"/>
+      <c r="S9" s="62"/>
+      <c r="T9" s="62"/>
+      <c r="U9" s="62"/>
+      <c r="V9" s="62"/>
+      <c r="W9" s="62"/>
+      <c r="X9" s="62"/>
+      <c r="Y9" s="62"/>
+      <c r="Z9" s="62"/>
+      <c r="AA9" s="62"/>
+      <c r="AB9" s="62"/>
+      <c r="AC9" s="62"/>
+      <c r="AD9" s="62"/>
+      <c r="AE9" s="62"/>
+      <c r="AF9" s="62"/>
+      <c r="AG9" s="62"/>
+      <c r="AH9" s="63"/>
       <c r="AJ9" s="10" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="46" t="s">
+        <v>407</v>
+      </c>
+      <c r="C10" s="44">
+        <v>0</v>
+      </c>
+      <c r="D10" s="44">
+        <v>0</v>
+      </c>
+      <c r="E10" s="44">
+        <v>0</v>
+      </c>
+      <c r="F10" s="44">
+        <v>0</v>
+      </c>
+      <c r="G10" s="45">
+        <v>0</v>
+      </c>
+      <c r="H10" s="45">
+        <v>1</v>
+      </c>
+      <c r="I10" s="45">
+        <v>0</v>
+      </c>
+      <c r="J10" s="61" t="s">
         <v>408</v>
       </c>
-      <c r="C10" s="44">
-        <v>0</v>
-      </c>
-      <c r="D10" s="44">
-        <v>0</v>
-      </c>
-      <c r="E10" s="44">
-        <v>0</v>
-      </c>
-      <c r="F10" s="44">
-        <v>0</v>
-      </c>
-      <c r="G10" s="45">
-        <v>0</v>
-      </c>
-      <c r="H10" s="45">
-        <v>1</v>
-      </c>
-      <c r="I10" s="45">
-        <v>0</v>
-      </c>
-      <c r="J10" s="59" t="s">
+      <c r="K10" s="62"/>
+      <c r="L10" s="63"/>
+      <c r="M10" s="61" t="s">
+        <v>406</v>
+      </c>
+      <c r="N10" s="62"/>
+      <c r="O10" s="62"/>
+      <c r="P10" s="62"/>
+      <c r="Q10" s="62"/>
+      <c r="R10" s="62"/>
+      <c r="S10" s="62"/>
+      <c r="T10" s="62"/>
+      <c r="U10" s="62"/>
+      <c r="V10" s="62"/>
+      <c r="W10" s="62"/>
+      <c r="X10" s="62"/>
+      <c r="Y10" s="62"/>
+      <c r="Z10" s="62"/>
+      <c r="AA10" s="62"/>
+      <c r="AB10" s="62"/>
+      <c r="AC10" s="62"/>
+      <c r="AD10" s="62"/>
+      <c r="AE10" s="62"/>
+      <c r="AF10" s="62"/>
+      <c r="AG10" s="62"/>
+      <c r="AH10" s="63"/>
+      <c r="AJ10" s="10" t="s">
         <v>409</v>
-      </c>
-      <c r="K10" s="60"/>
-      <c r="L10" s="61"/>
-      <c r="M10" s="59" t="s">
-        <v>407</v>
-      </c>
-      <c r="N10" s="60"/>
-      <c r="O10" s="60"/>
-      <c r="P10" s="60"/>
-      <c r="Q10" s="60"/>
-      <c r="R10" s="60"/>
-      <c r="S10" s="60"/>
-      <c r="T10" s="60"/>
-      <c r="U10" s="60"/>
-      <c r="V10" s="60"/>
-      <c r="W10" s="60"/>
-      <c r="X10" s="60"/>
-      <c r="Y10" s="60"/>
-      <c r="Z10" s="60"/>
-      <c r="AA10" s="60"/>
-      <c r="AB10" s="60"/>
-      <c r="AC10" s="60"/>
-      <c r="AD10" s="60"/>
-      <c r="AE10" s="60"/>
-      <c r="AF10" s="60"/>
-      <c r="AG10" s="60"/>
-      <c r="AH10" s="61"/>
-      <c r="AJ10" s="10" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
@@ -10225,44 +10374,44 @@
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="C12" s="6">
+        <v>1</v>
+      </c>
+      <c r="D12" s="60"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="60"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="60"/>
+      <c r="M12" s="60"/>
+      <c r="N12" s="60"/>
+      <c r="O12" s="60"/>
+      <c r="P12" s="60"/>
+      <c r="Q12" s="60"/>
+      <c r="R12" s="60"/>
+      <c r="S12" s="60"/>
+      <c r="T12" s="60"/>
+      <c r="U12" s="60"/>
+      <c r="V12" s="60"/>
+      <c r="W12" s="60"/>
+      <c r="X12" s="60"/>
+      <c r="Y12" s="60"/>
+      <c r="Z12" s="60"/>
+      <c r="AA12" s="60"/>
+      <c r="AB12" s="60"/>
+      <c r="AC12" s="60"/>
+      <c r="AD12" s="60"/>
+      <c r="AE12" s="60"/>
+      <c r="AF12" s="60"/>
+      <c r="AG12" s="60"/>
+      <c r="AH12" s="60"/>
+      <c r="AJ12" s="10" t="s">
         <v>393</v>
-      </c>
-      <c r="C12" s="6">
-        <v>1</v>
-      </c>
-      <c r="D12" s="58"/>
-      <c r="E12" s="58"/>
-      <c r="F12" s="58"/>
-      <c r="G12" s="58"/>
-      <c r="H12" s="58"/>
-      <c r="I12" s="58"/>
-      <c r="J12" s="58"/>
-      <c r="K12" s="58"/>
-      <c r="L12" s="58"/>
-      <c r="M12" s="58"/>
-      <c r="N12" s="58"/>
-      <c r="O12" s="58"/>
-      <c r="P12" s="58"/>
-      <c r="Q12" s="58"/>
-      <c r="R12" s="58"/>
-      <c r="S12" s="58"/>
-      <c r="T12" s="58"/>
-      <c r="U12" s="58"/>
-      <c r="V12" s="58"/>
-      <c r="W12" s="58"/>
-      <c r="X12" s="58"/>
-      <c r="Y12" s="58"/>
-      <c r="Z12" s="58"/>
-      <c r="AA12" s="58"/>
-      <c r="AB12" s="58"/>
-      <c r="AC12" s="58"/>
-      <c r="AD12" s="58"/>
-      <c r="AE12" s="58"/>
-      <c r="AF12" s="58"/>
-      <c r="AG12" s="58"/>
-      <c r="AH12" s="58"/>
-      <c r="AJ12" s="10" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.25">
@@ -10408,7 +10557,7 @@
       <c r="AG16" s="6"/>
       <c r="AH16" s="6"/>
       <c r="AJ16" s="10" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.25">
@@ -10782,7 +10931,7 @@
     </row>
     <row r="29" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4">
@@ -10831,7 +10980,7 @@
     </row>
     <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="45">
@@ -10851,7 +11000,7 @@
       </c>
       <c r="H30" s="6"/>
       <c r="I30" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
@@ -10882,7 +11031,7 @@
     </row>
     <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="45">
@@ -10928,12 +11077,12 @@
       <c r="AG31" s="6"/>
       <c r="AH31" s="6"/>
       <c r="AJ31" s="10" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C32" s="45">
         <v>0</v>
@@ -10952,7 +11101,7 @@
       </c>
       <c r="H32" s="6"/>
       <c r="I32" s="10" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="J32" s="6"/>
       <c r="K32" s="6"/>
@@ -10983,7 +11132,7 @@
     </row>
     <row r="33" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C33" s="45">
         <v>0</v>
@@ -11002,7 +11151,7 @@
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="10" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="J33" s="6"/>
       <c r="K33" s="6"/>
@@ -11033,7 +11182,7 @@
     </row>
     <row r="34" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C34" s="45">
         <v>0</v>
@@ -11052,7 +11201,7 @@
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="10" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="J34" s="6"/>
       <c r="K34" s="6"/>
@@ -11080,12 +11229,12 @@
       <c r="AG34" s="6"/>
       <c r="AH34" s="6"/>
       <c r="AJ34" s="10" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="35" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C35" s="45">
         <v>0</v>
@@ -11104,7 +11253,7 @@
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="10" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="J35" s="6"/>
       <c r="K35" s="6"/>
@@ -11135,7 +11284,7 @@
     </row>
     <row r="36" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A36" s="46" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C36" s="45">
         <v>0</v>
@@ -11154,7 +11303,7 @@
       </c>
       <c r="H36" s="44"/>
       <c r="I36" s="10" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="J36" s="44"/>
       <c r="K36" s="44"/>
@@ -11185,7 +11334,7 @@
     </row>
     <row r="37" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C37" s="45">
         <v>0</v>
@@ -11204,7 +11353,7 @@
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="10" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="J37" s="6"/>
       <c r="K37" s="6"/>
@@ -11235,7 +11384,7 @@
     </row>
     <row r="38" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C38" s="45">
         <v>0</v>
@@ -11254,7 +11403,7 @@
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="J38" s="6"/>
       <c r="K38" s="6"/>
@@ -11285,7 +11434,7 @@
     </row>
     <row r="39" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C39" s="45">
         <v>0</v>
@@ -11304,7 +11453,7 @@
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="10" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="J39" s="6"/>
       <c r="K39" s="6"/>
@@ -11335,7 +11484,7 @@
     </row>
     <row r="40" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C40" s="45">
         <v>0</v>
@@ -11354,7 +11503,7 @@
       </c>
       <c r="H40" s="6"/>
       <c r="I40" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J40" s="6"/>
       <c r="K40" s="6"/>
@@ -11385,7 +11534,7 @@
     </row>
     <row r="41" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C41" s="45">
         <v>0</v>
@@ -11404,7 +11553,7 @@
       </c>
       <c r="H41" s="6"/>
       <c r="I41" s="10" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="J41" s="6"/>
       <c r="K41" s="6"/>
@@ -11434,30 +11583,30 @@
     </row>
     <row r="42" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="C42" s="45">
+        <v>0</v>
+      </c>
+      <c r="D42" s="44">
+        <v>1</v>
+      </c>
+      <c r="E42" s="44">
+        <v>1</v>
+      </c>
+      <c r="F42" s="6">
+        <v>0</v>
+      </c>
+      <c r="G42" s="6">
+        <v>0</v>
+      </c>
+      <c r="I42" s="10" t="s">
         <v>382</v>
-      </c>
-      <c r="C42" s="45">
-        <v>0</v>
-      </c>
-      <c r="D42" s="44">
-        <v>1</v>
-      </c>
-      <c r="E42" s="44">
-        <v>1</v>
-      </c>
-      <c r="F42" s="6">
-        <v>0</v>
-      </c>
-      <c r="G42" s="6">
-        <v>0</v>
-      </c>
-      <c r="I42" s="10" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="43" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A43" s="46" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C43" s="45">
         <v>0</v>
@@ -11478,7 +11627,7 @@
     </row>
     <row r="44" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C44" s="45">
         <v>0</v>
@@ -11497,7 +11646,7 @@
       </c>
       <c r="H44" s="6"/>
       <c r="I44" s="10" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="J44" s="6"/>
       <c r="K44" s="6"/>
@@ -11528,30 +11677,30 @@
     </row>
     <row r="45" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A45" s="46" t="s">
+        <v>386</v>
+      </c>
+      <c r="C45" s="45">
+        <v>0</v>
+      </c>
+      <c r="D45" s="44">
+        <v>1</v>
+      </c>
+      <c r="E45" s="44">
+        <v>1</v>
+      </c>
+      <c r="F45" s="44">
+        <v>1</v>
+      </c>
+      <c r="G45" s="44">
+        <v>1</v>
+      </c>
+      <c r="I45" s="10" t="s">
         <v>387</v>
-      </c>
-      <c r="C45" s="45">
-        <v>0</v>
-      </c>
-      <c r="D45" s="44">
-        <v>1</v>
-      </c>
-      <c r="E45" s="44">
-        <v>1</v>
-      </c>
-      <c r="F45" s="44">
-        <v>1</v>
-      </c>
-      <c r="G45" s="44">
-        <v>1</v>
-      </c>
-      <c r="I45" s="10" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="46" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A46" s="46" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C46" s="45">
         <v>1</v>
@@ -11569,36 +11718,36 @@
         <v>0</v>
       </c>
       <c r="I46" s="10" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="AJ46" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="47" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A47" s="46" t="s">
+        <v>395</v>
+      </c>
+      <c r="C47" s="45">
+        <v>1</v>
+      </c>
+      <c r="D47" s="44">
+        <v>0</v>
+      </c>
+      <c r="E47" s="44">
+        <v>0</v>
+      </c>
+      <c r="F47" s="44">
+        <v>1</v>
+      </c>
+      <c r="G47" s="44">
+        <v>1</v>
+      </c>
+      <c r="I47" s="10" t="s">
+        <v>397</v>
+      </c>
+      <c r="AJ47" t="s">
         <v>396</v>
-      </c>
-      <c r="C47" s="45">
-        <v>1</v>
-      </c>
-      <c r="D47" s="44">
-        <v>0</v>
-      </c>
-      <c r="E47" s="44">
-        <v>0</v>
-      </c>
-      <c r="F47" s="44">
-        <v>1</v>
-      </c>
-      <c r="G47" s="44">
-        <v>1</v>
-      </c>
-      <c r="I47" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="AJ47" t="s">
-        <v>397</v>
       </c>
     </row>
   </sheetData>
@@ -12228,12 +12377,12 @@
       <c r="N7" s="40">
         <v>1</v>
       </c>
-      <c r="O7" s="58" t="s">
+      <c r="O7" s="60" t="s">
         <v>302</v>
       </c>
-      <c r="P7" s="58"/>
-      <c r="Q7" s="58"/>
-      <c r="R7" s="58"/>
+      <c r="P7" s="60"/>
+      <c r="Q7" s="60"/>
+      <c r="R7" s="60"/>
       <c r="T7" s="10"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -12264,16 +12413,16 @@
       <c r="J8" s="40">
         <v>1</v>
       </c>
-      <c r="K8" s="58" t="s">
+      <c r="K8" s="60" t="s">
         <v>131</v>
       </c>
-      <c r="L8" s="58"/>
-      <c r="M8" s="58"/>
-      <c r="N8" s="58"/>
-      <c r="O8" s="58"/>
-      <c r="P8" s="58"/>
-      <c r="Q8" s="58"/>
-      <c r="R8" s="58"/>
+      <c r="L8" s="60"/>
+      <c r="M8" s="60"/>
+      <c r="N8" s="60"/>
+      <c r="O8" s="60"/>
+      <c r="P8" s="60"/>
+      <c r="Q8" s="60"/>
+      <c r="R8" s="60"/>
       <c r="T8" s="10"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -12304,16 +12453,16 @@
       <c r="J9" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="K9" s="58" t="s">
+      <c r="K9" s="60" t="s">
         <v>131</v>
       </c>
-      <c r="L9" s="58"/>
-      <c r="M9" s="58"/>
-      <c r="N9" s="58"/>
-      <c r="O9" s="58"/>
-      <c r="P9" s="58"/>
-      <c r="Q9" s="58"/>
-      <c r="R9" s="58"/>
+      <c r="L9" s="60"/>
+      <c r="M9" s="60"/>
+      <c r="N9" s="60"/>
+      <c r="O9" s="60"/>
+      <c r="P9" s="60"/>
+      <c r="Q9" s="60"/>
+      <c r="R9" s="60"/>
       <c r="T9" s="10"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -12344,16 +12493,16 @@
       <c r="J10" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="K10" s="58" t="s">
+      <c r="K10" s="60" t="s">
         <v>131</v>
       </c>
-      <c r="L10" s="58"/>
-      <c r="M10" s="58"/>
-      <c r="N10" s="58"/>
-      <c r="O10" s="58"/>
-      <c r="P10" s="58"/>
-      <c r="Q10" s="58"/>
-      <c r="R10" s="58"/>
+      <c r="L10" s="60"/>
+      <c r="M10" s="60"/>
+      <c r="N10" s="60"/>
+      <c r="O10" s="60"/>
+      <c r="P10" s="60"/>
+      <c r="Q10" s="60"/>
+      <c r="R10" s="60"/>
       <c r="T10" s="10"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -12384,16 +12533,16 @@
       <c r="J11" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="K11" s="58" t="s">
+      <c r="K11" s="60" t="s">
         <v>131</v>
       </c>
-      <c r="L11" s="58"/>
-      <c r="M11" s="58"/>
-      <c r="N11" s="58"/>
-      <c r="O11" s="58"/>
-      <c r="P11" s="58"/>
-      <c r="Q11" s="58"/>
-      <c r="R11" s="58"/>
+      <c r="L11" s="60"/>
+      <c r="M11" s="60"/>
+      <c r="N11" s="60"/>
+      <c r="O11" s="60"/>
+      <c r="P11" s="60"/>
+      <c r="Q11" s="60"/>
+      <c r="R11" s="60"/>
       <c r="T11" s="10"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -12424,16 +12573,16 @@
       <c r="J12" s="6">
         <v>0</v>
       </c>
-      <c r="K12" s="58" t="s">
+      <c r="K12" s="60" t="s">
         <v>300</v>
       </c>
-      <c r="L12" s="58"/>
-      <c r="M12" s="58"/>
-      <c r="N12" s="58"/>
-      <c r="O12" s="58"/>
-      <c r="P12" s="58"/>
-      <c r="Q12" s="58"/>
-      <c r="R12" s="58"/>
+      <c r="L12" s="60"/>
+      <c r="M12" s="60"/>
+      <c r="N12" s="60"/>
+      <c r="O12" s="60"/>
+      <c r="P12" s="60"/>
+      <c r="Q12" s="60"/>
+      <c r="R12" s="60"/>
       <c r="T12" s="10"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
smart watch test: displaying arb numbers
</commit_message>
<xml_diff>
--- a/doc/RiscyInstSet32Bit.xlsx
+++ b/doc/RiscyInstSet32Bit.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="447">
   <si>
     <t>Description</t>
   </si>
@@ -525,9 +525,6 @@
     <t>Mode</t>
   </si>
   <si>
-    <t>Rs/Rd: device (see Rperi); Rlen: length</t>
-  </si>
-  <si>
     <t>RfromAddr</t>
   </si>
   <si>
@@ -747,9 +744,6 @@
     <t>rDest = mem[offset]</t>
   </si>
   <si>
-    <t>Fill screen with fore/back</t>
-  </si>
-  <si>
     <t>Set memory bank</t>
   </si>
   <si>
@@ -1357,6 +1351,39 @@
   </si>
   <si>
     <t>No Operation (alternative)</t>
+  </si>
+  <si>
+    <t>Bitmapped card only</t>
+  </si>
+  <si>
+    <t>Fill screen with colour</t>
+  </si>
+  <si>
+    <t>Colour</t>
+  </si>
+  <si>
+    <t>Canvas can also be "pages" (one that contains texts only)</t>
+  </si>
+  <si>
+    <t>Alternatively you can manipulate graphics memory directly</t>
+  </si>
+  <si>
+    <t>Used to wipe out the screen before draw</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rs/Rd: device (see Rperi); Rlen: length </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WARNING: this expects actual address, NOT an offset</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1848,8 +1875,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="7" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1857,22 +1884,13 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
@@ -1887,13 +1905,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1952,9 +1982,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -2245,8 +2272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AK11" sqref="AK11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2262,7 +2289,7 @@
   <sheetData>
     <row r="1" spans="1:38" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2302,7 +2329,7 @@
     <row r="2" spans="1:38" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.25">
@@ -2311,7 +2338,7 @@
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -2350,11 +2377,11 @@
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B5" s="33" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -2397,7 +2424,7 @@
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="10" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -2436,7 +2463,7 @@
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
@@ -2474,12 +2501,12 @@
       <c r="AH7" s="5"/>
       <c r="AI7" s="5"/>
       <c r="AK7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>0</v>
@@ -2583,17 +2610,17 @@
       </c>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A10" s="65">
+      <c r="A10" s="62">
         <v>1</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="64" t="s">
+      <c r="D10" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
       <c r="G10" s="11">
         <v>0</v>
       </c>
@@ -2606,21 +2633,21 @@
       <c r="J10" s="11">
         <v>0</v>
       </c>
-      <c r="K10" s="68" t="s">
+      <c r="K10" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="L10" s="68"/>
-      <c r="M10" s="68"/>
-      <c r="N10" s="68" t="s">
+      <c r="L10" s="71"/>
+      <c r="M10" s="71"/>
+      <c r="N10" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="O10" s="68"/>
-      <c r="P10" s="68"/>
-      <c r="Q10" s="68" t="s">
+      <c r="O10" s="71"/>
+      <c r="P10" s="71"/>
+      <c r="Q10" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="R10" s="68"/>
-      <c r="S10" s="68"/>
+      <c r="R10" s="71"/>
+      <c r="S10" s="71"/>
       <c r="T10" s="12">
         <v>0</v>
       </c>
@@ -2651,28 +2678,28 @@
       <c r="AC10" s="6">
         <v>0</v>
       </c>
-      <c r="AD10" s="68" t="s">
-        <v>332</v>
-      </c>
-      <c r="AE10" s="68"/>
-      <c r="AF10" s="68"/>
-      <c r="AG10" s="68"/>
-      <c r="AH10" s="68"/>
-      <c r="AI10" s="68"/>
+      <c r="AD10" s="71" t="s">
+        <v>330</v>
+      </c>
+      <c r="AE10" s="71"/>
+      <c r="AF10" s="71"/>
+      <c r="AG10" s="71"/>
+      <c r="AH10" s="71"/>
+      <c r="AI10" s="71"/>
       <c r="AK10" s="10" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A11" s="66"/>
+      <c r="A11" s="63"/>
       <c r="B11" s="7" t="s">
-        <v>292</v>
-      </c>
-      <c r="D11" s="55" t="s">
+        <v>290</v>
+      </c>
+      <c r="D11" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
       <c r="G11" s="18">
         <v>0</v>
       </c>
@@ -2685,19 +2712,19 @@
       <c r="J11" s="18">
         <v>0</v>
       </c>
-      <c r="K11" s="60" t="s">
+      <c r="K11" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="L11" s="60"/>
-      <c r="M11" s="60"/>
-      <c r="N11" s="59" t="s">
+      <c r="L11" s="59"/>
+      <c r="M11" s="59"/>
+      <c r="N11" s="58" t="s">
         <v>150</v>
       </c>
-      <c r="O11" s="59"/>
-      <c r="P11" s="59"/>
-      <c r="Q11" s="59"/>
-      <c r="R11" s="59"/>
-      <c r="S11" s="59"/>
+      <c r="O11" s="58"/>
+      <c r="P11" s="58"/>
+      <c r="Q11" s="58"/>
+      <c r="R11" s="58"/>
+      <c r="S11" s="58"/>
       <c r="T11" s="12">
         <v>0</v>
       </c>
@@ -2747,19 +2774,19 @@
         <v>8</v>
       </c>
       <c r="AK11" s="10" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A12" s="66"/>
+      <c r="A12" s="63"/>
       <c r="B12" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D12" s="55" t="s">
+      <c r="D12" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="55"/>
-      <c r="F12" s="55"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
       <c r="G12" s="18">
         <v>0</v>
       </c>
@@ -2772,16 +2799,16 @@
       <c r="J12" s="18">
         <v>0</v>
       </c>
-      <c r="K12" s="63" t="s">
+      <c r="K12" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="L12" s="63"/>
-      <c r="M12" s="63"/>
-      <c r="N12" s="63" t="s">
+      <c r="L12" s="67"/>
+      <c r="M12" s="67"/>
+      <c r="N12" s="67" t="s">
         <v>149</v>
       </c>
-      <c r="O12" s="63"/>
-      <c r="P12" s="63"/>
+      <c r="O12" s="67"/>
+      <c r="P12" s="67"/>
       <c r="Q12" s="57" t="s">
         <v>150</v>
       </c>
@@ -2836,19 +2863,19 @@
         <v>0</v>
       </c>
       <c r="AK12" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A13" s="66"/>
+      <c r="A13" s="63"/>
       <c r="B13" s="33" t="s">
-        <v>438</v>
-      </c>
-      <c r="D13" s="55" t="s">
+        <v>436</v>
+      </c>
+      <c r="D13" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="55"/>
-      <c r="F13" s="55"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="60"/>
       <c r="G13" s="31">
         <v>0</v>
       </c>
@@ -2867,7 +2894,7 @@
       <c r="L13" s="56"/>
       <c r="M13" s="56"/>
       <c r="N13" s="56" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="O13" s="56"/>
       <c r="P13" s="56"/>
@@ -2925,19 +2952,19 @@
         <v>0</v>
       </c>
       <c r="AK13" s="10" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A14" s="67"/>
+      <c r="A14" s="64"/>
       <c r="B14" s="47" t="s">
-        <v>439</v>
-      </c>
-      <c r="D14" s="55" t="s">
+        <v>437</v>
+      </c>
+      <c r="D14" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="55"/>
-      <c r="F14" s="55"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
       <c r="G14" s="50">
         <v>0</v>
       </c>
@@ -2956,7 +2983,7 @@
       <c r="L14" s="56"/>
       <c r="M14" s="56"/>
       <c r="N14" s="56" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="O14" s="56"/>
       <c r="P14" s="56"/>
@@ -3014,7 +3041,7 @@
         <v>0</v>
       </c>
       <c r="AK14" s="10" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
@@ -3024,11 +3051,11 @@
       <c r="B15" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="D15" s="55" t="s">
+      <c r="D15" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="55"/>
-      <c r="F15" s="55"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="60"/>
       <c r="G15" s="6">
         <v>0</v>
       </c>
@@ -3095,15 +3122,15 @@
       <c r="AF15" s="6">
         <v>0</v>
       </c>
-      <c r="AG15" s="55" t="s">
+      <c r="AG15" s="60" t="s">
         <v>163</v>
       </c>
-      <c r="AH15" s="55"/>
+      <c r="AH15" s="60"/>
       <c r="AI15" s="22" t="s">
         <v>84</v>
       </c>
       <c r="AK15" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AL15" s="2" t="s">
         <v>162</v>
@@ -3116,11 +3143,11 @@
       <c r="B16" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D16" s="55" t="s">
+      <c r="D16" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
       <c r="G16" s="6">
         <v>0</v>
       </c>
@@ -3149,12 +3176,12 @@
       <c r="R16" s="56"/>
       <c r="S16" s="56"/>
       <c r="T16" s="56" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="U16" s="56"/>
       <c r="V16" s="56"/>
       <c r="W16" s="56" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X16" s="56"/>
       <c r="Y16" s="56"/>
@@ -3189,7 +3216,7 @@
         <v>0</v>
       </c>
       <c r="AK16" s="10" t="s">
-        <v>164</v>
+        <v>446</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
@@ -3199,11 +3226,11 @@
       <c r="B17" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="D17" s="55" t="s">
+      <c r="D17" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="55"/>
-      <c r="F17" s="55"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
       <c r="G17" s="6">
         <v>0</v>
       </c>
@@ -3278,27 +3305,27 @@
         <v>0</v>
       </c>
       <c r="AH17" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AI17" s="22" t="s">
         <v>96</v>
       </c>
       <c r="AK17" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A18" s="58">
+      <c r="A18" s="70">
         <v>2</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="D18" s="55" t="s">
+      <c r="D18" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="55"/>
-      <c r="F18" s="55"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
       <c r="G18" s="6">
         <v>0</v>
       </c>
@@ -3369,15 +3396,15 @@
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A19" s="58"/>
+      <c r="A19" s="70"/>
       <c r="B19" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D19" s="55" t="s">
+      <c r="D19" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="55"/>
-      <c r="F19" s="55"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="60"/>
       <c r="G19" s="6">
         <v>0</v>
       </c>
@@ -3432,15 +3459,15 @@
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A20" s="58"/>
+      <c r="A20" s="70"/>
       <c r="B20" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="D20" s="55" t="s">
+      <c r="D20" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="55"/>
-      <c r="F20" s="55"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="60"/>
       <c r="G20" s="6">
         <v>0</v>
       </c>
@@ -3491,19 +3518,19 @@
       <c r="AH20" s="56"/>
       <c r="AI20" s="56"/>
       <c r="AK20" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A21" s="58"/>
+      <c r="A21" s="70"/>
       <c r="B21" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="D21" s="55" t="s">
+      <c r="D21" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="E21" s="55"/>
-      <c r="F21" s="55"/>
+      <c r="E21" s="60"/>
+      <c r="F21" s="60"/>
       <c r="G21" s="6">
         <v>0</v>
       </c>
@@ -3546,7 +3573,7 @@
       <c r="AH21" s="56"/>
       <c r="AI21" s="56"/>
       <c r="AK21" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.25">
@@ -3556,11 +3583,11 @@
       <c r="B22" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="55" t="s">
+      <c r="D22" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="55"/>
-      <c r="F22" s="55"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="60"/>
       <c r="G22" s="6">
         <v>0</v>
       </c>
@@ -3579,7 +3606,7 @@
       <c r="L22" s="56"/>
       <c r="M22" s="56"/>
       <c r="N22" s="56" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O22" s="56"/>
       <c r="P22" s="56"/>
@@ -3603,21 +3630,21 @@
       <c r="AH22" s="56"/>
       <c r="AI22" s="56"/>
       <c r="AK22" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A23" s="61">
+      <c r="A23" s="68">
         <v>6</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="D23" s="55" t="s">
+        <v>276</v>
+      </c>
+      <c r="D23" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="55"/>
-      <c r="F23" s="55"/>
+      <c r="E23" s="60"/>
+      <c r="F23" s="60"/>
       <c r="G23" s="6">
         <v>1</v>
       </c>
@@ -3630,11 +3657,11 @@
       <c r="J23" s="12">
         <v>0</v>
       </c>
-      <c r="K23" s="59" t="s">
+      <c r="K23" s="58" t="s">
         <v>150</v>
       </c>
-      <c r="L23" s="59"/>
-      <c r="M23" s="59"/>
+      <c r="L23" s="58"/>
+      <c r="M23" s="58"/>
       <c r="N23" s="56" t="s">
         <v>4</v>
       </c>
@@ -3660,19 +3687,19 @@
       <c r="AH23" s="56"/>
       <c r="AI23" s="56"/>
       <c r="AK23" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A24" s="62"/>
+      <c r="A24" s="69"/>
       <c r="B24" s="46" t="s">
-        <v>404</v>
-      </c>
-      <c r="D24" s="55" t="s">
+        <v>402</v>
+      </c>
+      <c r="D24" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="55"/>
-      <c r="F24" s="55"/>
+      <c r="E24" s="60"/>
+      <c r="F24" s="60"/>
       <c r="G24" s="44">
         <v>1</v>
       </c>
@@ -3685,11 +3712,11 @@
       <c r="J24" s="45">
         <v>1</v>
       </c>
-      <c r="K24" s="74" t="s">
+      <c r="K24" s="75" t="s">
         <v>150</v>
       </c>
-      <c r="L24" s="75"/>
-      <c r="M24" s="76"/>
+      <c r="L24" s="76"/>
+      <c r="M24" s="77"/>
       <c r="N24" s="56" t="s">
         <v>4</v>
       </c>
@@ -3721,49 +3748,49 @@
         <v>7</v>
       </c>
       <c r="B25" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="D25" s="60" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="60"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="24">
+        <v>1</v>
+      </c>
+      <c r="H25" s="25">
+        <v>0</v>
+      </c>
+      <c r="I25" s="25">
+        <v>1</v>
+      </c>
+      <c r="J25" s="25">
+        <v>0</v>
+      </c>
+      <c r="K25" s="58" t="s">
+        <v>150</v>
+      </c>
+      <c r="L25" s="58"/>
+      <c r="M25" s="58"/>
+      <c r="N25" s="25">
+        <v>0</v>
+      </c>
+      <c r="O25" s="25">
+        <v>0</v>
+      </c>
+      <c r="P25" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="59" t="s">
         <v>239</v>
       </c>
-      <c r="D25" s="55" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" s="55"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="24">
-        <v>1</v>
-      </c>
-      <c r="H25" s="25">
-        <v>0</v>
-      </c>
-      <c r="I25" s="25">
-        <v>1</v>
-      </c>
-      <c r="J25" s="25">
-        <v>0</v>
-      </c>
-      <c r="K25" s="59" t="s">
-        <v>150</v>
-      </c>
-      <c r="L25" s="59"/>
-      <c r="M25" s="59"/>
-      <c r="N25" s="25">
-        <v>0</v>
-      </c>
-      <c r="O25" s="25">
-        <v>0</v>
-      </c>
-      <c r="P25" s="25">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="60" t="s">
-        <v>241</v>
-      </c>
-      <c r="R25" s="60"/>
-      <c r="S25" s="60"/>
-      <c r="T25" s="60"/>
-      <c r="U25" s="60"/>
-      <c r="V25" s="60"/>
+      <c r="R25" s="59"/>
+      <c r="S25" s="59"/>
+      <c r="T25" s="59"/>
+      <c r="U25" s="59"/>
+      <c r="V25" s="59"/>
       <c r="W25" s="56" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="X25" s="56"/>
       <c r="Y25" s="56"/>
@@ -3778,7 +3805,7 @@
       <c r="AH25" s="56"/>
       <c r="AI25" s="56"/>
       <c r="AK25" s="10" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
@@ -3786,13 +3813,13 @@
         <v>8</v>
       </c>
       <c r="B26" s="46" t="s">
-        <v>246</v>
-      </c>
-      <c r="D26" s="69" t="s">
+        <v>244</v>
+      </c>
+      <c r="D26" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="E26" s="55"/>
-      <c r="F26" s="70"/>
+      <c r="E26" s="60"/>
+      <c r="F26" s="66"/>
       <c r="G26" s="44">
         <v>1</v>
       </c>
@@ -3805,11 +3832,11 @@
       <c r="J26" s="45">
         <v>0</v>
       </c>
-      <c r="K26" s="71" t="s">
+      <c r="K26" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="L26" s="72"/>
-      <c r="M26" s="73"/>
+      <c r="L26" s="73"/>
+      <c r="M26" s="74"/>
       <c r="N26" s="45">
         <v>0</v>
       </c>
@@ -3852,18 +3879,18 @@
       <c r="AA26" s="44">
         <v>0</v>
       </c>
-      <c r="AB26" s="77" t="s">
+      <c r="AB26" s="78" t="s">
+        <v>241</v>
+      </c>
+      <c r="AC26" s="79"/>
+      <c r="AD26" s="79"/>
+      <c r="AE26" s="79"/>
+      <c r="AF26" s="79"/>
+      <c r="AG26" s="79"/>
+      <c r="AH26" s="79"/>
+      <c r="AI26" s="80"/>
+      <c r="AK26" s="10" t="s">
         <v>243</v>
-      </c>
-      <c r="AC26" s="78"/>
-      <c r="AD26" s="78"/>
-      <c r="AE26" s="78"/>
-      <c r="AF26" s="78"/>
-      <c r="AG26" s="78"/>
-      <c r="AH26" s="78"/>
-      <c r="AI26" s="79"/>
-      <c r="AK26" s="10" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.25">
@@ -3873,11 +3900,11 @@
       <c r="B27" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D27" s="55" t="s">
+      <c r="D27" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="E27" s="55"/>
-      <c r="F27" s="55"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="60"/>
       <c r="G27" s="6">
         <v>1</v>
       </c>
@@ -3958,11 +3985,11 @@
       <c r="B28" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D28" s="55" t="s">
+      <c r="D28" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="E28" s="55"/>
-      <c r="F28" s="55"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="60"/>
       <c r="G28" s="6">
         <v>1</v>
       </c>
@@ -4033,7 +4060,7 @@
       <c r="AH28" s="56"/>
       <c r="AI28" s="56"/>
       <c r="AK28" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.25">
@@ -4043,11 +4070,11 @@
       <c r="B29" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D29" s="55" t="s">
+      <c r="D29" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="E29" s="55"/>
-      <c r="F29" s="55"/>
+      <c r="E29" s="60"/>
+      <c r="F29" s="60"/>
       <c r="G29" s="6">
         <v>1</v>
       </c>
@@ -4140,11 +4167,11 @@
       <c r="B30" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D30" s="55" t="s">
+      <c r="D30" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="E30" s="55"/>
-      <c r="F30" s="55"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
       <c r="G30" s="6">
         <v>1</v>
       </c>
@@ -4220,8 +4247,8 @@
       <c r="AI30" s="56"/>
     </row>
     <row r="31" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B31" s="90" t="s">
-        <v>441</v>
+      <c r="B31" s="55" t="s">
+        <v>439</v>
       </c>
       <c r="D31" s="51">
         <v>1</v>
@@ -4917,6 +4944,9 @@
     <mergeCell ref="K24:M24"/>
     <mergeCell ref="N24:AI24"/>
     <mergeCell ref="AB26:AI26"/>
+    <mergeCell ref="AG15:AH15"/>
+    <mergeCell ref="W16:Y16"/>
+    <mergeCell ref="Q12:S12"/>
     <mergeCell ref="D29:F29"/>
     <mergeCell ref="A10:A14"/>
     <mergeCell ref="D13:F13"/>
@@ -4924,6 +4954,14 @@
     <mergeCell ref="N13:P13"/>
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="D24:F24"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="N12:P12"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="A18:A21"/>
     <mergeCell ref="D30:F30"/>
     <mergeCell ref="D23:F23"/>
     <mergeCell ref="D20:F20"/>
@@ -4956,32 +4994,21 @@
     <mergeCell ref="AB28:AI28"/>
     <mergeCell ref="K29:M29"/>
     <mergeCell ref="K17:M17"/>
-    <mergeCell ref="AG15:AH15"/>
-    <mergeCell ref="W16:Y16"/>
-    <mergeCell ref="N18:P18"/>
-    <mergeCell ref="N19:P19"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="N12:P12"/>
-    <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="AB18:AI18"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="N16:P16"/>
-    <mergeCell ref="Q16:S16"/>
-    <mergeCell ref="T16:V16"/>
-    <mergeCell ref="K19:M19"/>
     <mergeCell ref="T19:AI19"/>
     <mergeCell ref="Q13:S13"/>
     <mergeCell ref="W25:AI25"/>
     <mergeCell ref="K25:M25"/>
     <mergeCell ref="Q25:V25"/>
     <mergeCell ref="K20:M20"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="D14:F14"/>
     <mergeCell ref="K14:M14"/>
     <mergeCell ref="N14:P14"/>
     <mergeCell ref="Q14:S14"/>
-    <mergeCell ref="A18:A21"/>
     <mergeCell ref="N20:P20"/>
+    <mergeCell ref="AB18:AI18"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="N16:P16"/>
+    <mergeCell ref="Q16:S16"/>
+    <mergeCell ref="T16:V16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5009,7 +5036,7 @@
   <sheetData>
     <row r="1" spans="1:21" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -5033,7 +5060,7 @@
     <row r="2" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -5042,7 +5069,7 @@
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -5065,11 +5092,11 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B5" s="33" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -5096,7 +5123,7 @@
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -5116,11 +5143,11 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B7" s="33" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -5138,12 +5165,12 @@
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
       <c r="U7" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>0</v>
@@ -5215,7 +5242,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="56" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="H10" s="56"/>
       <c r="I10" s="56"/>
@@ -5245,7 +5272,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D11" s="32">
         <v>0</v>
@@ -5366,26 +5393,26 @@
       <c r="G13" s="32">
         <v>0</v>
       </c>
-      <c r="H13" s="60" t="s">
+      <c r="H13" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="I13" s="60"/>
+      <c r="I13" s="59"/>
       <c r="J13" s="32">
         <v>0</v>
       </c>
       <c r="K13" s="32">
         <v>1</v>
       </c>
-      <c r="L13" s="60" t="s">
+      <c r="L13" s="59" t="s">
         <v>147</v>
       </c>
-      <c r="M13" s="60"/>
-      <c r="N13" s="60"/>
-      <c r="O13" s="60"/>
-      <c r="P13" s="60"/>
-      <c r="Q13" s="60"/>
-      <c r="R13" s="60"/>
-      <c r="S13" s="60"/>
+      <c r="M13" s="59"/>
+      <c r="N13" s="59"/>
+      <c r="O13" s="59"/>
+      <c r="P13" s="59"/>
+      <c r="Q13" s="59"/>
+      <c r="R13" s="59"/>
+      <c r="S13" s="59"/>
       <c r="U13" s="10"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -5408,26 +5435,26 @@
       <c r="G14" s="32">
         <v>0</v>
       </c>
-      <c r="H14" s="60" t="s">
+      <c r="H14" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="I14" s="60"/>
+      <c r="I14" s="59"/>
       <c r="J14" s="32">
         <v>1</v>
       </c>
       <c r="K14" s="32">
         <v>0</v>
       </c>
-      <c r="L14" s="60" t="s">
-        <v>298</v>
-      </c>
-      <c r="M14" s="60"/>
-      <c r="N14" s="60"/>
-      <c r="O14" s="60"/>
-      <c r="P14" s="60"/>
-      <c r="Q14" s="60"/>
-      <c r="R14" s="60"/>
-      <c r="S14" s="60"/>
+      <c r="L14" s="59" t="s">
+        <v>296</v>
+      </c>
+      <c r="M14" s="59"/>
+      <c r="N14" s="59"/>
+      <c r="O14" s="59"/>
+      <c r="P14" s="59"/>
+      <c r="Q14" s="59"/>
+      <c r="R14" s="59"/>
+      <c r="S14" s="59"/>
       <c r="U14" s="10"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -5450,26 +5477,26 @@
       <c r="G15" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="H15" s="60" t="s">
+      <c r="H15" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="I15" s="60"/>
+      <c r="I15" s="59"/>
       <c r="J15" s="32">
         <v>0</v>
       </c>
       <c r="K15" s="32">
         <v>0</v>
       </c>
-      <c r="L15" s="60" t="s">
-        <v>298</v>
-      </c>
-      <c r="M15" s="60"/>
-      <c r="N15" s="60"/>
-      <c r="O15" s="60"/>
-      <c r="P15" s="60"/>
-      <c r="Q15" s="60"/>
-      <c r="R15" s="60"/>
-      <c r="S15" s="60"/>
+      <c r="L15" s="59" t="s">
+        <v>296</v>
+      </c>
+      <c r="M15" s="59"/>
+      <c r="N15" s="59"/>
+      <c r="O15" s="59"/>
+      <c r="P15" s="59"/>
+      <c r="Q15" s="59"/>
+      <c r="R15" s="59"/>
+      <c r="S15" s="59"/>
       <c r="U15" s="10"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -5477,7 +5504,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="33" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D16" s="32">
         <v>0</v>
@@ -5491,34 +5518,34 @@
       <c r="G16" s="32">
         <v>1</v>
       </c>
-      <c r="H16" s="80" t="s">
+      <c r="H16" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="I16" s="80"/>
-      <c r="J16" s="80"/>
+      <c r="I16" s="81"/>
+      <c r="J16" s="81"/>
       <c r="K16" s="32">
         <v>1</v>
       </c>
-      <c r="L16" s="60" t="s">
-        <v>298</v>
-      </c>
-      <c r="M16" s="60"/>
-      <c r="N16" s="60"/>
-      <c r="O16" s="60"/>
-      <c r="P16" s="60"/>
-      <c r="Q16" s="60"/>
-      <c r="R16" s="60"/>
-      <c r="S16" s="60"/>
+      <c r="L16" s="59" t="s">
+        <v>296</v>
+      </c>
+      <c r="M16" s="59"/>
+      <c r="N16" s="59"/>
+      <c r="O16" s="59"/>
+      <c r="P16" s="59"/>
+      <c r="Q16" s="59"/>
+      <c r="R16" s="59"/>
+      <c r="S16" s="59"/>
       <c r="U16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="58">
+      <c r="A17" s="70">
         <v>13</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D17" s="32">
         <v>1</v>
@@ -5532,14 +5559,14 @@
       <c r="G17" s="32">
         <v>0</v>
       </c>
-      <c r="H17" s="60" t="s">
-        <v>336</v>
-      </c>
-      <c r="I17" s="60"/>
-      <c r="J17" s="60" t="s">
-        <v>339</v>
-      </c>
-      <c r="K17" s="60"/>
+      <c r="H17" s="59" t="s">
+        <v>334</v>
+      </c>
+      <c r="I17" s="59"/>
+      <c r="J17" s="59" t="s">
+        <v>337</v>
+      </c>
+      <c r="K17" s="59"/>
       <c r="L17" s="32">
         <v>0</v>
       </c>
@@ -5565,34 +5592,34 @@
         <v>8</v>
       </c>
       <c r="U17" s="10" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="70"/>
+      <c r="B18" s="33" t="s">
+        <v>340</v>
+      </c>
+      <c r="D18" s="32">
+        <v>1</v>
+      </c>
+      <c r="E18" s="32">
+        <v>0</v>
+      </c>
+      <c r="F18" s="32">
+        <v>0</v>
+      </c>
+      <c r="G18" s="32">
+        <v>0</v>
+      </c>
+      <c r="H18" s="59" t="s">
+        <v>334</v>
+      </c>
+      <c r="I18" s="59"/>
+      <c r="J18" s="59" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="58"/>
-      <c r="B18" s="33" t="s">
-        <v>342</v>
-      </c>
-      <c r="D18" s="32">
-        <v>1</v>
-      </c>
-      <c r="E18" s="32">
-        <v>0</v>
-      </c>
-      <c r="F18" s="32">
-        <v>0</v>
-      </c>
-      <c r="G18" s="32">
-        <v>0</v>
-      </c>
-      <c r="H18" s="60" t="s">
-        <v>336</v>
-      </c>
-      <c r="I18" s="60"/>
-      <c r="J18" s="60" t="s">
-        <v>339</v>
-      </c>
-      <c r="K18" s="60"/>
+      <c r="K18" s="59"/>
       <c r="L18" s="32">
         <v>0</v>
       </c>
@@ -5618,58 +5645,58 @@
         <v>8</v>
       </c>
       <c r="U18" s="10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="58"/>
+      <c r="A19" s="70"/>
       <c r="B19" s="33" t="s">
+        <v>336</v>
+      </c>
+      <c r="D19" s="32">
+        <v>1</v>
+      </c>
+      <c r="E19" s="32">
+        <v>0</v>
+      </c>
+      <c r="F19" s="32">
+        <v>0</v>
+      </c>
+      <c r="G19" s="32">
+        <v>0</v>
+      </c>
+      <c r="H19" s="58" t="s">
+        <v>329</v>
+      </c>
+      <c r="I19" s="58"/>
+      <c r="J19" s="58"/>
+      <c r="K19" s="58"/>
+      <c r="L19" s="32">
+        <v>0</v>
+      </c>
+      <c r="M19" s="32">
+        <v>0</v>
+      </c>
+      <c r="N19" s="32">
+        <v>0</v>
+      </c>
+      <c r="O19" s="32">
+        <v>0</v>
+      </c>
+      <c r="P19" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="32">
+        <v>1</v>
+      </c>
+      <c r="R19" s="32">
+        <v>0</v>
+      </c>
+      <c r="S19" s="32">
+        <v>0</v>
+      </c>
+      <c r="U19" s="10" t="s">
         <v>338</v>
-      </c>
-      <c r="D19" s="32">
-        <v>1</v>
-      </c>
-      <c r="E19" s="32">
-        <v>0</v>
-      </c>
-      <c r="F19" s="32">
-        <v>0</v>
-      </c>
-      <c r="G19" s="32">
-        <v>0</v>
-      </c>
-      <c r="H19" s="59" t="s">
-        <v>331</v>
-      </c>
-      <c r="I19" s="59"/>
-      <c r="J19" s="59"/>
-      <c r="K19" s="59"/>
-      <c r="L19" s="32">
-        <v>0</v>
-      </c>
-      <c r="M19" s="32">
-        <v>0</v>
-      </c>
-      <c r="N19" s="32">
-        <v>0</v>
-      </c>
-      <c r="O19" s="32">
-        <v>0</v>
-      </c>
-      <c r="P19" s="32">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="32">
-        <v>1</v>
-      </c>
-      <c r="R19" s="32">
-        <v>0</v>
-      </c>
-      <c r="S19" s="32">
-        <v>0</v>
-      </c>
-      <c r="U19" s="10" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
@@ -5919,33 +5946,33 @@
   <sheetData>
     <row r="1" spans="1:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="35" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B1" s="36">
         <v>1</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="82" t="s">
         <v>153</v>
       </c>
-      <c r="B2" s="82"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
-      <c r="J2" s="82"/>
-      <c r="K2" s="82"/>
-      <c r="L2" s="83"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="84"/>
       <c r="M2" s="20" t="s">
         <v>152</v>
       </c>
@@ -5974,10 +6001,10 @@
         <v>0</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3" t="s">
@@ -5990,10 +6017,10 @@
         <v>154</v>
       </c>
       <c r="P3" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q3" s="23" t="s">
         <v>174</v>
-      </c>
-      <c r="Q3" s="23" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -6031,16 +6058,16 @@
         <v>14</v>
       </c>
       <c r="M4" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="N4" t="s">
         <v>155</v>
       </c>
       <c r="P4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Q4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -6084,10 +6111,10 @@
         <v>155</v>
       </c>
       <c r="P5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="Q5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -6125,16 +6152,16 @@
         <v>74</v>
       </c>
       <c r="M6" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="N6" t="s">
         <v>155</v>
       </c>
       <c r="P6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="Q6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -6172,16 +6199,16 @@
         <v>75</v>
       </c>
       <c r="M7" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="N7" t="s">
         <v>155</v>
       </c>
       <c r="P7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Q7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -6224,7 +6251,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="52" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B9" s="53"/>
       <c r="C9" s="53">
@@ -6255,10 +6282,10 @@
       </c>
       <c r="K9" s="54"/>
       <c r="L9" s="54" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="M9" s="54" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="N9" s="54"/>
     </row>
@@ -6297,13 +6324,13 @@
         <v>158</v>
       </c>
       <c r="M10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N10" t="s">
         <v>156</v>
       </c>
       <c r="P10" s="19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -6341,18 +6368,18 @@
         <v>159</v>
       </c>
       <c r="M11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="N11" t="s">
         <v>155</v>
       </c>
       <c r="P11" s="19" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="47" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B12" s="48"/>
       <c r="C12" s="48">
@@ -6382,24 +6409,24 @@
         <v>38h</v>
       </c>
       <c r="L12" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="M12" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="N12" t="s">
         <v>155</v>
       </c>
       <c r="O12" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="P12" s="19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="47" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B13" s="48"/>
       <c r="C13" s="48">
@@ -6429,21 +6456,21 @@
         <v>39h</v>
       </c>
       <c r="L13" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="M13" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="O13" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="P13" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="47" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B14" s="48"/>
       <c r="C14" s="48">
@@ -6473,21 +6500,21 @@
         <v>3Ah</v>
       </c>
       <c r="L14" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="M14" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="N14" t="s">
         <v>156</v>
       </c>
       <c r="O14" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="47" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B15" s="48"/>
       <c r="C15" s="48">
@@ -6517,18 +6544,18 @@
         <v>3Bh</v>
       </c>
       <c r="L15" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="M15" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="O15" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="47" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B16" s="48"/>
       <c r="C16" s="48">
@@ -6558,21 +6585,21 @@
         <v>3Ch</v>
       </c>
       <c r="L16" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="M16" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="N16" t="s">
         <v>155</v>
       </c>
       <c r="O16" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="47" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B17" s="48"/>
       <c r="C17" s="48">
@@ -6602,18 +6629,18 @@
         <v>3Dh</v>
       </c>
       <c r="L17" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="M17" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="O17" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6">
@@ -6643,10 +6670,10 @@
         <v>3Eh</v>
       </c>
       <c r="L18" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="M18" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -6684,7 +6711,7 @@
         <v>77</v>
       </c>
       <c r="M19" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -7773,7 +7800,7 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B46" s="6"/>
       <c r="C46" s="6">
@@ -7803,10 +7830,10 @@
         <v>18h</v>
       </c>
       <c r="L46" t="s">
+        <v>190</v>
+      </c>
+      <c r="M46" t="s">
         <v>191</v>
-      </c>
-      <c r="M46" t="s">
-        <v>192</v>
       </c>
       <c r="N46" t="s">
         <v>156</v>
@@ -8177,7 +8204,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="35" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B1" s="36">
         <v>1</v>
@@ -8187,19 +8214,19 @@
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="82" t="s">
         <v>153</v>
       </c>
-      <c r="B2" s="82"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
-      <c r="J2" s="82"/>
-      <c r="K2" s="83"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="84"/>
       <c r="L2" s="20" t="s">
         <v>152</v>
       </c>
@@ -8225,10 +8252,10 @@
         <v>0</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3" t="s">
@@ -8273,7 +8300,7 @@
         <v>14</v>
       </c>
       <c r="L4" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="M4" t="s">
         <v>155</v>
@@ -8395,7 +8422,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B8" s="29"/>
       <c r="C8" s="29">
@@ -8422,10 +8449,10 @@
         <v>1Eh</v>
       </c>
       <c r="K8" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="L8" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -8460,7 +8487,7 @@
         <v>77</v>
       </c>
       <c r="L9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -9030,13 +9057,13 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="35" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B1" s="36">
         <v>2</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -9044,7 +9071,7 @@
     </row>
     <row r="2" spans="1:6" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="28" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B2" s="37"/>
       <c r="C2" s="28"/>
@@ -9054,129 +9081,129 @@
     </row>
     <row r="3" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B3" s="38"/>
       <c r="C3" s="3" t="s">
         <v>92</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E4" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E10" t="s">
+        <v>224</v>
+      </c>
+      <c r="F10" t="s">
         <v>225</v>
-      </c>
-      <c r="F10" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="28" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B11" s="37"/>
       <c r="C11" s="28"/>
@@ -9186,118 +9213,118 @@
     </row>
     <row r="12" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B12" s="38"/>
       <c r="C12" s="3" t="s">
         <v>92</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E13" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D15" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E16" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E18" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="F18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="35" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B19" s="36">
         <v>3</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -9305,36 +9332,36 @@
     </row>
     <row r="20" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B20" s="38"/>
       <c r="C20" s="3" t="s">
         <v>92</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F20" s="23" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="26" t="s">
+        <v>248</v>
+      </c>
+      <c r="C21" t="s">
         <v>250</v>
       </c>
-      <c r="C21" t="s">
-        <v>252</v>
-      </c>
       <c r="D21" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="35" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B22" s="36">
         <v>4</v>
@@ -9348,81 +9375,81 @@
     </row>
     <row r="23" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B23" s="38"/>
       <c r="C23" s="3" t="s">
         <v>92</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F23" s="23" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="C24" t="s">
+        <v>252</v>
+      </c>
+      <c r="D24" t="s">
+        <v>283</v>
+      </c>
+      <c r="E24" t="s">
         <v>253</v>
-      </c>
-      <c r="C24" t="s">
-        <v>254</v>
-      </c>
-      <c r="D24" t="s">
-        <v>285</v>
-      </c>
-      <c r="E24" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C25" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D25" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E25" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="26" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C26" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D26" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E26" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="26" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C27" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D27" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E27" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="35" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B28" s="36">
         <v>5</v>
@@ -9436,78 +9463,78 @@
     </row>
     <row r="29" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B29" s="38"/>
       <c r="C29" s="3" t="s">
         <v>92</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F29" s="23" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D30" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E30" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D31" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E31" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F31" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="26" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D32" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E32" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="26" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E33" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="35" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B34" s="36">
         <v>6</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -9515,144 +9542,144 @@
     </row>
     <row r="35" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B35" s="38"/>
       <c r="C35" s="3" t="s">
         <v>92</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F35" s="23" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="26" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C36" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D36" t="s">
+        <v>310</v>
+      </c>
+      <c r="E36" t="s">
         <v>312</v>
       </c>
-      <c r="E36" t="s">
-        <v>314</v>
-      </c>
       <c r="F36" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="26" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C37" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D37" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E37" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F37" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="26" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C38" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D38" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E38" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="F38" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="26" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C39" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D39" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E39" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F39" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="26" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C40" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D40" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E40" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="F40" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="26" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C41" t="s">
+        <v>323</v>
+      </c>
+      <c r="D41" t="s">
+        <v>314</v>
+      </c>
+      <c r="E41" t="s">
         <v>325</v>
-      </c>
-      <c r="D41" t="s">
-        <v>316</v>
-      </c>
-      <c r="E41" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="26" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C42" t="s">
+        <v>324</v>
+      </c>
+      <c r="D42" t="s">
+        <v>314</v>
+      </c>
+      <c r="E42" t="s">
         <v>326</v>
-      </c>
-      <c r="D42" t="s">
-        <v>316</v>
-      </c>
-      <c r="E42" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="35" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B43" s="36">
         <v>7</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -9660,31 +9687,31 @@
     </row>
     <row r="44" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B44" s="38"/>
       <c r="C44" s="3" t="s">
         <v>92</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F44" s="23" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="35" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B46" s="36">
         <v>8</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -9692,31 +9719,31 @@
     </row>
     <row r="47" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B47" s="38"/>
       <c r="C47" s="3" t="s">
         <v>92</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F47" s="23" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="35" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B49" s="36">
         <v>9</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
@@ -9724,31 +9751,31 @@
     </row>
     <row r="50" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B50" s="38"/>
       <c r="C50" s="3" t="s">
         <v>92</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F50" s="23" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="35" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B52" s="36">
         <v>10</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
@@ -9756,31 +9783,31 @@
     </row>
     <row r="53" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B53" s="38"/>
       <c r="C53" s="3" t="s">
         <v>92</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F53" s="23" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="35" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B55" s="36">
         <v>11</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
@@ -9788,25 +9815,25 @@
     </row>
     <row r="56" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B56" s="38"/>
       <c r="C56" s="3" t="s">
         <v>92</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F56" s="23" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="35" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B58" s="36">
         <v>12</v>
@@ -9820,20 +9847,20 @@
     </row>
     <row r="59" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B59" s="38"/>
       <c r="C59" s="3" t="s">
         <v>92</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F59" s="23" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -9845,7 +9872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="G9" sqref="G9:J9"/>
     </sheetView>
   </sheetViews>
@@ -9860,7 +9887,7 @@
   <sheetData>
     <row r="1" spans="1:36" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -9898,7 +9925,7 @@
     </row>
     <row r="2" spans="1:36" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="4" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10005,7 +10032,7 @@
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="39" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C5" s="41">
         <v>0</v>
@@ -10079,23 +10106,23 @@
       <c r="Z5" s="41">
         <v>0</v>
       </c>
-      <c r="AA5" s="63" t="s">
+      <c r="AA5" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="AB5" s="63"/>
-      <c r="AC5" s="63"/>
-      <c r="AD5" s="63"/>
-      <c r="AE5" s="63"/>
-      <c r="AF5" s="63"/>
-      <c r="AG5" s="63"/>
-      <c r="AH5" s="63"/>
+      <c r="AB5" s="67"/>
+      <c r="AC5" s="67"/>
+      <c r="AD5" s="67"/>
+      <c r="AE5" s="67"/>
+      <c r="AF5" s="67"/>
+      <c r="AG5" s="67"/>
+      <c r="AH5" s="67"/>
       <c r="AJ5" s="10" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="46" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C6" s="43">
         <v>0</v>
@@ -10176,18 +10203,18 @@
       <c r="AC6" s="57"/>
       <c r="AD6" s="57"/>
       <c r="AE6" s="57"/>
-      <c r="AF6" s="63" t="s">
-        <v>357</v>
-      </c>
-      <c r="AG6" s="63"/>
-      <c r="AH6" s="63"/>
+      <c r="AF6" s="67" t="s">
+        <v>355</v>
+      </c>
+      <c r="AG6" s="67"/>
+      <c r="AH6" s="67"/>
       <c r="AJ6" s="10" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="46" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C7" s="43">
         <v>0</v>
@@ -10261,82 +10288,82 @@
       <c r="Z7" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="AA7" s="84" t="s">
-        <v>401</v>
-      </c>
-      <c r="AB7" s="85"/>
-      <c r="AC7" s="85"/>
-      <c r="AD7" s="85"/>
-      <c r="AE7" s="85"/>
-      <c r="AF7" s="85"/>
-      <c r="AG7" s="85"/>
-      <c r="AH7" s="86"/>
+      <c r="AA7" s="85" t="s">
+        <v>399</v>
+      </c>
+      <c r="AB7" s="86"/>
+      <c r="AC7" s="86"/>
+      <c r="AD7" s="86"/>
+      <c r="AE7" s="86"/>
+      <c r="AF7" s="86"/>
+      <c r="AG7" s="86"/>
+      <c r="AH7" s="87"/>
       <c r="AJ7" s="10" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="39" t="s">
+        <v>352</v>
+      </c>
+      <c r="C8" s="41">
+        <v>0</v>
+      </c>
+      <c r="D8" s="41">
+        <v>0</v>
+      </c>
+      <c r="E8" s="41">
+        <v>0</v>
+      </c>
+      <c r="F8" s="41">
+        <v>0</v>
+      </c>
+      <c r="G8" s="41">
+        <v>0</v>
+      </c>
+      <c r="H8" s="41">
+        <v>0</v>
+      </c>
+      <c r="I8" s="41">
+        <v>0</v>
+      </c>
+      <c r="J8" s="41">
+        <v>1</v>
+      </c>
+      <c r="K8" s="67" t="s">
         <v>354</v>
       </c>
-      <c r="C8" s="41">
-        <v>0</v>
-      </c>
-      <c r="D8" s="41">
-        <v>0</v>
-      </c>
-      <c r="E8" s="41">
-        <v>0</v>
-      </c>
-      <c r="F8" s="41">
-        <v>0</v>
-      </c>
-      <c r="G8" s="41">
-        <v>0</v>
-      </c>
-      <c r="H8" s="41">
-        <v>0</v>
-      </c>
-      <c r="I8" s="41">
-        <v>0</v>
-      </c>
-      <c r="J8" s="41">
-        <v>1</v>
-      </c>
-      <c r="K8" s="63" t="s">
+      <c r="L8" s="67"/>
+      <c r="M8" s="67"/>
+      <c r="N8" s="67"/>
+      <c r="O8" s="67"/>
+      <c r="P8" s="67" t="s">
+        <v>355</v>
+      </c>
+      <c r="Q8" s="67"/>
+      <c r="R8" s="67"/>
+      <c r="S8" s="67" t="s">
         <v>356</v>
       </c>
-      <c r="L8" s="63"/>
-      <c r="M8" s="63"/>
-      <c r="N8" s="63"/>
-      <c r="O8" s="63"/>
-      <c r="P8" s="63" t="s">
-        <v>357</v>
-      </c>
-      <c r="Q8" s="63"/>
-      <c r="R8" s="63"/>
-      <c r="S8" s="63" t="s">
-        <v>358</v>
-      </c>
-      <c r="T8" s="63"/>
-      <c r="U8" s="63"/>
-      <c r="V8" s="63"/>
-      <c r="W8" s="63"/>
-      <c r="X8" s="63"/>
-      <c r="Y8" s="63"/>
-      <c r="Z8" s="63"/>
-      <c r="AA8" s="63" t="s">
+      <c r="T8" s="67"/>
+      <c r="U8" s="67"/>
+      <c r="V8" s="67"/>
+      <c r="W8" s="67"/>
+      <c r="X8" s="67"/>
+      <c r="Y8" s="67"/>
+      <c r="Z8" s="67"/>
+      <c r="AA8" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="AB8" s="63"/>
-      <c r="AC8" s="63"/>
-      <c r="AD8" s="63"/>
-      <c r="AE8" s="63"/>
-      <c r="AF8" s="63"/>
-      <c r="AG8" s="63"/>
-      <c r="AH8" s="63"/>
+      <c r="AB8" s="67"/>
+      <c r="AC8" s="67"/>
+      <c r="AD8" s="67"/>
+      <c r="AE8" s="67"/>
+      <c r="AF8" s="67"/>
+      <c r="AG8" s="67"/>
+      <c r="AH8" s="67"/>
       <c r="AJ8" s="10" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.25">
@@ -10367,94 +10394,94 @@
       <c r="J9" s="6">
         <v>0</v>
       </c>
-      <c r="K9" s="87" t="s">
+      <c r="K9" s="88" t="s">
         <v>150</v>
       </c>
-      <c r="L9" s="88"/>
-      <c r="M9" s="77" t="s">
-        <v>406</v>
-      </c>
-      <c r="N9" s="78"/>
-      <c r="O9" s="78"/>
-      <c r="P9" s="78"/>
-      <c r="Q9" s="78"/>
-      <c r="R9" s="78"/>
-      <c r="S9" s="78"/>
-      <c r="T9" s="78"/>
-      <c r="U9" s="78"/>
-      <c r="V9" s="78"/>
-      <c r="W9" s="78"/>
-      <c r="X9" s="78"/>
-      <c r="Y9" s="78"/>
-      <c r="Z9" s="78"/>
-      <c r="AA9" s="78"/>
-      <c r="AB9" s="78"/>
-      <c r="AC9" s="78"/>
-      <c r="AD9" s="78"/>
-      <c r="AE9" s="78"/>
-      <c r="AF9" s="78"/>
-      <c r="AG9" s="78"/>
-      <c r="AH9" s="79"/>
+      <c r="L9" s="89"/>
+      <c r="M9" s="78" t="s">
+        <v>404</v>
+      </c>
+      <c r="N9" s="79"/>
+      <c r="O9" s="79"/>
+      <c r="P9" s="79"/>
+      <c r="Q9" s="79"/>
+      <c r="R9" s="79"/>
+      <c r="S9" s="79"/>
+      <c r="T9" s="79"/>
+      <c r="U9" s="79"/>
+      <c r="V9" s="79"/>
+      <c r="W9" s="79"/>
+      <c r="X9" s="79"/>
+      <c r="Y9" s="79"/>
+      <c r="Z9" s="79"/>
+      <c r="AA9" s="79"/>
+      <c r="AB9" s="79"/>
+      <c r="AC9" s="79"/>
+      <c r="AD9" s="79"/>
+      <c r="AE9" s="79"/>
+      <c r="AF9" s="79"/>
+      <c r="AG9" s="79"/>
+      <c r="AH9" s="80"/>
       <c r="AJ9" s="10" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="46" t="s">
+        <v>405</v>
+      </c>
+      <c r="C10" s="44">
+        <v>0</v>
+      </c>
+      <c r="D10" s="44">
+        <v>0</v>
+      </c>
+      <c r="E10" s="44">
+        <v>0</v>
+      </c>
+      <c r="F10" s="44">
+        <v>0</v>
+      </c>
+      <c r="G10" s="45">
+        <v>0</v>
+      </c>
+      <c r="H10" s="45">
+        <v>1</v>
+      </c>
+      <c r="I10" s="45">
+        <v>0</v>
+      </c>
+      <c r="J10" s="78" t="s">
+        <v>406</v>
+      </c>
+      <c r="K10" s="79"/>
+      <c r="L10" s="80"/>
+      <c r="M10" s="78" t="s">
+        <v>404</v>
+      </c>
+      <c r="N10" s="79"/>
+      <c r="O10" s="79"/>
+      <c r="P10" s="79"/>
+      <c r="Q10" s="79"/>
+      <c r="R10" s="79"/>
+      <c r="S10" s="79"/>
+      <c r="T10" s="79"/>
+      <c r="U10" s="79"/>
+      <c r="V10" s="79"/>
+      <c r="W10" s="79"/>
+      <c r="X10" s="79"/>
+      <c r="Y10" s="79"/>
+      <c r="Z10" s="79"/>
+      <c r="AA10" s="79"/>
+      <c r="AB10" s="79"/>
+      <c r="AC10" s="79"/>
+      <c r="AD10" s="79"/>
+      <c r="AE10" s="79"/>
+      <c r="AF10" s="79"/>
+      <c r="AG10" s="79"/>
+      <c r="AH10" s="80"/>
+      <c r="AJ10" s="10" t="s">
         <v>407</v>
-      </c>
-      <c r="C10" s="44">
-        <v>0</v>
-      </c>
-      <c r="D10" s="44">
-        <v>0</v>
-      </c>
-      <c r="E10" s="44">
-        <v>0</v>
-      </c>
-      <c r="F10" s="44">
-        <v>0</v>
-      </c>
-      <c r="G10" s="45">
-        <v>0</v>
-      </c>
-      <c r="H10" s="45">
-        <v>1</v>
-      </c>
-      <c r="I10" s="45">
-        <v>0</v>
-      </c>
-      <c r="J10" s="77" t="s">
-        <v>408</v>
-      </c>
-      <c r="K10" s="78"/>
-      <c r="L10" s="79"/>
-      <c r="M10" s="77" t="s">
-        <v>406</v>
-      </c>
-      <c r="N10" s="78"/>
-      <c r="O10" s="78"/>
-      <c r="P10" s="78"/>
-      <c r="Q10" s="78"/>
-      <c r="R10" s="78"/>
-      <c r="S10" s="78"/>
-      <c r="T10" s="78"/>
-      <c r="U10" s="78"/>
-      <c r="V10" s="78"/>
-      <c r="W10" s="78"/>
-      <c r="X10" s="78"/>
-      <c r="Y10" s="78"/>
-      <c r="Z10" s="78"/>
-      <c r="AA10" s="78"/>
-      <c r="AB10" s="78"/>
-      <c r="AC10" s="78"/>
-      <c r="AD10" s="78"/>
-      <c r="AE10" s="78"/>
-      <c r="AF10" s="78"/>
-      <c r="AG10" s="78"/>
-      <c r="AH10" s="79"/>
-      <c r="AJ10" s="10" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
@@ -10495,7 +10522,7 @@
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C12" s="6">
         <v>1</v>
@@ -10532,7 +10559,7 @@
       <c r="AG12" s="56"/>
       <c r="AH12" s="56"/>
       <c r="AJ12" s="10" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.25">
@@ -10678,7 +10705,7 @@
       <c r="AG16" s="6"/>
       <c r="AH16" s="6"/>
       <c r="AJ16" s="10" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.25">
@@ -11052,7 +11079,7 @@
     </row>
     <row r="29" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4">
@@ -11101,7 +11128,7 @@
     </row>
     <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="45">
@@ -11121,7 +11148,7 @@
       </c>
       <c r="H30" s="6"/>
       <c r="I30" s="5" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
@@ -11152,7 +11179,7 @@
     </row>
     <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="45">
@@ -11198,12 +11225,12 @@
       <c r="AG31" s="6"/>
       <c r="AH31" s="6"/>
       <c r="AJ31" s="10" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C32" s="45">
         <v>0</v>
@@ -11222,7 +11249,7 @@
       </c>
       <c r="H32" s="6"/>
       <c r="I32" s="10" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="J32" s="6"/>
       <c r="K32" s="6"/>
@@ -11253,7 +11280,7 @@
     </row>
     <row r="33" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C33" s="45">
         <v>0</v>
@@ -11272,7 +11299,7 @@
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="10" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="J33" s="6"/>
       <c r="K33" s="6"/>
@@ -11303,7 +11330,7 @@
     </row>
     <row r="34" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C34" s="45">
         <v>0</v>
@@ -11322,7 +11349,7 @@
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="10" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="J34" s="6"/>
       <c r="K34" s="6"/>
@@ -11350,12 +11377,12 @@
       <c r="AG34" s="6"/>
       <c r="AH34" s="6"/>
       <c r="AJ34" s="10" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="35" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C35" s="45">
         <v>0</v>
@@ -11374,7 +11401,7 @@
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="10" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="J35" s="6"/>
       <c r="K35" s="6"/>
@@ -11405,7 +11432,7 @@
     </row>
     <row r="36" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A36" s="46" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C36" s="45">
         <v>0</v>
@@ -11424,7 +11451,7 @@
       </c>
       <c r="H36" s="44"/>
       <c r="I36" s="10" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="J36" s="44"/>
       <c r="K36" s="44"/>
@@ -11455,7 +11482,7 @@
     </row>
     <row r="37" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C37" s="45">
         <v>0</v>
@@ -11474,7 +11501,7 @@
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="10" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="J37" s="6"/>
       <c r="K37" s="6"/>
@@ -11505,7 +11532,7 @@
     </row>
     <row r="38" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C38" s="45">
         <v>0</v>
@@ -11524,7 +11551,7 @@
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="5" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="J38" s="6"/>
       <c r="K38" s="6"/>
@@ -11555,7 +11582,7 @@
     </row>
     <row r="39" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C39" s="45">
         <v>0</v>
@@ -11574,7 +11601,7 @@
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="10" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="J39" s="6"/>
       <c r="K39" s="6"/>
@@ -11605,7 +11632,7 @@
     </row>
     <row r="40" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C40" s="45">
         <v>0</v>
@@ -11624,7 +11651,7 @@
       </c>
       <c r="H40" s="6"/>
       <c r="I40" s="10" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="J40" s="6"/>
       <c r="K40" s="6"/>
@@ -11655,7 +11682,7 @@
     </row>
     <row r="41" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C41" s="45">
         <v>0</v>
@@ -11674,7 +11701,7 @@
       </c>
       <c r="H41" s="6"/>
       <c r="I41" s="10" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="J41" s="6"/>
       <c r="K41" s="6"/>
@@ -11704,7 +11731,7 @@
     </row>
     <row r="42" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C42" s="45">
         <v>0</v>
@@ -11722,12 +11749,12 @@
         <v>0</v>
       </c>
       <c r="I42" s="10" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="43" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A43" s="46" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C43" s="45">
         <v>0</v>
@@ -11748,7 +11775,7 @@
     </row>
     <row r="44" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C44" s="45">
         <v>0</v>
@@ -11767,7 +11794,7 @@
       </c>
       <c r="H44" s="6"/>
       <c r="I44" s="10" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="J44" s="6"/>
       <c r="K44" s="6"/>
@@ -11798,7 +11825,7 @@
     </row>
     <row r="45" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A45" s="46" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C45" s="45">
         <v>0</v>
@@ -11816,59 +11843,59 @@
         <v>1</v>
       </c>
       <c r="I45" s="10" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="46" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A46" s="46" t="s">
+        <v>392</v>
+      </c>
+      <c r="C46" s="45">
+        <v>1</v>
+      </c>
+      <c r="D46" s="44">
+        <v>0</v>
+      </c>
+      <c r="E46" s="44">
+        <v>0</v>
+      </c>
+      <c r="F46" s="44">
+        <v>1</v>
+      </c>
+      <c r="G46" s="44">
+        <v>0</v>
+      </c>
+      <c r="I46" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="AJ46" t="s">
         <v>394</v>
-      </c>
-      <c r="C46" s="45">
-        <v>1</v>
-      </c>
-      <c r="D46" s="44">
-        <v>0</v>
-      </c>
-      <c r="E46" s="44">
-        <v>0</v>
-      </c>
-      <c r="F46" s="44">
-        <v>1</v>
-      </c>
-      <c r="G46" s="44">
-        <v>0</v>
-      </c>
-      <c r="I46" s="10" t="s">
-        <v>397</v>
-      </c>
-      <c r="AJ46" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="47" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A47" s="46" t="s">
+        <v>393</v>
+      </c>
+      <c r="C47" s="45">
+        <v>1</v>
+      </c>
+      <c r="D47" s="44">
+        <v>0</v>
+      </c>
+      <c r="E47" s="44">
+        <v>0</v>
+      </c>
+      <c r="F47" s="44">
+        <v>1</v>
+      </c>
+      <c r="G47" s="44">
+        <v>1</v>
+      </c>
+      <c r="I47" s="10" t="s">
         <v>395</v>
       </c>
-      <c r="C47" s="45">
-        <v>1</v>
-      </c>
-      <c r="D47" s="44">
-        <v>0</v>
-      </c>
-      <c r="E47" s="44">
-        <v>0</v>
-      </c>
-      <c r="F47" s="44">
-        <v>1</v>
-      </c>
-      <c r="G47" s="44">
-        <v>1</v>
-      </c>
-      <c r="I47" s="10" t="s">
-        <v>397</v>
-      </c>
       <c r="AJ47" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
   </sheetData>
@@ -11909,20 +11936,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="89" t="s">
-        <v>279</v>
-      </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
-      <c r="K1" s="89"/>
-      <c r="L1" s="89"/>
+      <c r="A1" s="90" t="s">
+        <v>277</v>
+      </c>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="90"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11955,15 +11982,15 @@
         <v>0</v>
       </c>
       <c r="K3" s="38" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="L3" s="38" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C4" s="25">
         <v>0</v>
@@ -12000,7 +12027,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C5" s="25">
         <v>0</v>
@@ -12037,7 +12064,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C6" s="25">
         <v>0</v>
@@ -12074,7 +12101,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C7" s="25">
         <v>0</v>
@@ -12197,10 +12224,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T43"/>
+  <dimension ref="A1:T42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12294,7 +12321,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="39" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C4" s="41">
         <v>0</v>
@@ -12342,7 +12369,7 @@
         <v>0</v>
       </c>
       <c r="R4" s="41" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="T4" s="10" t="s">
         <v>130</v>
@@ -12406,7 +12433,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="39" t="s">
-        <v>238</v>
+        <v>299</v>
       </c>
       <c r="C6" s="40">
         <v>0</v>
@@ -12442,25 +12469,21 @@
         <v>0</v>
       </c>
       <c r="N6" s="40">
-        <v>0</v>
-      </c>
-      <c r="O6" s="40">
-        <v>0</v>
-      </c>
-      <c r="P6" s="40">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="40">
-        <v>0</v>
-      </c>
-      <c r="R6" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="T6" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="O6" s="56" t="s">
+        <v>300</v>
+      </c>
+      <c r="P6" s="56"/>
+      <c r="Q6" s="56"/>
+      <c r="R6" s="56"/>
+      <c r="T6" s="10" t="s">
+        <v>443</v>
+      </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="39" t="s">
-        <v>301</v>
+        <v>134</v>
       </c>
       <c r="C7" s="40">
         <v>0</v>
@@ -12484,23 +12507,15 @@
         <v>0</v>
       </c>
       <c r="J7" s="40">
-        <v>0</v>
-      </c>
-      <c r="K7" s="40">
-        <v>0</v>
-      </c>
-      <c r="L7" s="40">
-        <v>0</v>
-      </c>
-      <c r="M7" s="40">
-        <v>0</v>
-      </c>
-      <c r="N7" s="40">
-        <v>1</v>
-      </c>
-      <c r="O7" s="56" t="s">
-        <v>302</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K7" s="56" t="s">
+        <v>131</v>
+      </c>
+      <c r="L7" s="56"/>
+      <c r="M7" s="56"/>
+      <c r="N7" s="56"/>
+      <c r="O7" s="56"/>
       <c r="P7" s="56"/>
       <c r="Q7" s="56"/>
       <c r="R7" s="56"/>
@@ -12508,7 +12523,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="39" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C8" s="40">
         <v>0</v>
@@ -12529,10 +12544,10 @@
         <v>0</v>
       </c>
       <c r="I8" s="40">
-        <v>0</v>
-      </c>
-      <c r="J8" s="40">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="J8" s="40" t="s">
+        <v>132</v>
       </c>
       <c r="K8" s="56" t="s">
         <v>131</v>
@@ -12548,7 +12563,7 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="39" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C9" s="40">
         <v>0</v>
@@ -12566,10 +12581,10 @@
         <v>0</v>
       </c>
       <c r="H9" s="40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" s="40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" s="40" t="s">
         <v>132</v>
@@ -12588,7 +12603,7 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="39" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C10" s="40">
         <v>0</v>
@@ -12609,7 +12624,7 @@
         <v>1</v>
       </c>
       <c r="I10" s="40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="40" t="s">
         <v>132</v>
@@ -12627,35 +12642,35 @@
       <c r="T10" s="10"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="39" t="s">
-        <v>136</v>
-      </c>
-      <c r="C11" s="40">
-        <v>0</v>
-      </c>
-      <c r="D11" s="40">
-        <v>0</v>
-      </c>
-      <c r="E11" s="40">
-        <v>0</v>
-      </c>
-      <c r="F11" s="40">
-        <v>0</v>
-      </c>
-      <c r="G11" s="40">
-        <v>0</v>
-      </c>
-      <c r="H11" s="40">
-        <v>1</v>
-      </c>
-      <c r="I11" s="40">
-        <v>1</v>
-      </c>
-      <c r="J11" s="40" t="s">
-        <v>132</v>
+      <c r="A11" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0</v>
+      </c>
+      <c r="G11" s="6">
+        <v>1</v>
+      </c>
+      <c r="H11" s="6">
+        <v>0</v>
+      </c>
+      <c r="I11" s="6">
+        <v>0</v>
+      </c>
+      <c r="J11" s="6">
+        <v>0</v>
       </c>
       <c r="K11" s="56" t="s">
-        <v>131</v>
+        <v>298</v>
       </c>
       <c r="L11" s="56"/>
       <c r="M11" s="56"/>
@@ -12664,50 +12679,34 @@
       <c r="P11" s="56"/>
       <c r="Q11" s="56"/>
       <c r="R11" s="56"/>
-      <c r="T11" s="10"/>
+      <c r="T11" s="10" t="s">
+        <v>444</v>
+      </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="C12" s="6">
-        <v>0</v>
-      </c>
-      <c r="D12" s="6">
-        <v>0</v>
-      </c>
-      <c r="E12" s="6">
-        <v>0</v>
-      </c>
-      <c r="F12" s="6">
-        <v>0</v>
-      </c>
-      <c r="G12" s="6">
-        <v>1</v>
-      </c>
-      <c r="H12" s="6">
-        <v>0</v>
-      </c>
-      <c r="I12" s="6">
-        <v>0</v>
-      </c>
-      <c r="J12" s="6">
-        <v>0</v>
-      </c>
-      <c r="K12" s="56" t="s">
-        <v>300</v>
-      </c>
-      <c r="L12" s="56"/>
-      <c r="M12" s="56"/>
-      <c r="N12" s="56"/>
-      <c r="O12" s="56"/>
-      <c r="P12" s="56"/>
-      <c r="Q12" s="56"/>
-      <c r="R12" s="56"/>
+      <c r="A12" s="7"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
       <c r="T12" s="10"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
+    <row r="13" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>440</v>
+      </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
@@ -12727,24 +12726,46 @@
       <c r="T13" s="10"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-      <c r="T14" s="10"/>
+      <c r="A14" s="7" t="s">
+        <v>441</v>
+      </c>
+      <c r="C14" s="6">
+        <v>1</v>
+      </c>
+      <c r="D14" s="6">
+        <v>0</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0</v>
+      </c>
+      <c r="H14" s="6">
+        <v>0</v>
+      </c>
+      <c r="I14" s="6">
+        <v>0</v>
+      </c>
+      <c r="J14" s="6">
+        <v>0</v>
+      </c>
+      <c r="K14" s="78" t="s">
+        <v>442</v>
+      </c>
+      <c r="L14" s="79"/>
+      <c r="M14" s="79"/>
+      <c r="N14" s="79"/>
+      <c r="O14" s="79"/>
+      <c r="P14" s="79"/>
+      <c r="Q14" s="79"/>
+      <c r="R14" s="80"/>
+      <c r="T14" s="10" t="s">
+        <v>445</v>
+      </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
@@ -12844,82 +12865,83 @@
       <c r="P19" s="6"/>
       <c r="Q19" s="6"/>
       <c r="R19" s="6"/>
-      <c r="T19" s="10"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="6"/>
-      <c r="R20" s="6"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="12"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="12"/>
-      <c r="O21" s="12"/>
-      <c r="P21" s="12"/>
-      <c r="Q21" s="12"/>
-      <c r="R21" s="12"/>
+      <c r="A21" s="7"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="T21" s="10"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
-      <c r="P22" s="6"/>
-      <c r="Q22" s="6"/>
-      <c r="R22" s="6"/>
-      <c r="T22" s="10"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="12"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="12"/>
-      <c r="O23" s="12"/>
-      <c r="P23" s="12"/>
-      <c r="Q23" s="12"/>
-      <c r="R23" s="12"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="T23" s="10"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
@@ -13049,7 +13071,6 @@
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
-      <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
@@ -13286,38 +13307,19 @@
       <c r="P41" s="6"/>
       <c r="Q41" s="6"/>
       <c r="R41" s="6"/>
-      <c r="T41" s="10"/>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
-      <c r="J42" s="6"/>
-      <c r="K42" s="6"/>
-      <c r="L42" s="6"/>
-      <c r="M42" s="6"/>
-      <c r="N42" s="6"/>
-      <c r="O42" s="6"/>
-      <c r="P42" s="6"/>
-      <c r="Q42" s="6"/>
-      <c r="R42" s="6"/>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="K12:R12"/>
-    <mergeCell ref="O7:R7"/>
+  <mergeCells count="7">
+    <mergeCell ref="K14:R14"/>
+    <mergeCell ref="K11:R11"/>
+    <mergeCell ref="O6:R6"/>
+    <mergeCell ref="K8:R8"/>
     <mergeCell ref="K9:R9"/>
+    <mergeCell ref="K7:R7"/>
     <mergeCell ref="K10:R10"/>
-    <mergeCell ref="K8:R8"/>
-    <mergeCell ref="K11:R11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
new commands: YIELD and PAUSE
</commit_message>
<xml_diff>
--- a/doc/RiscyInstSet32Bit.xlsx
+++ b/doc/RiscyInstSet32Bit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25410" windowHeight="12690"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25410" windowHeight="12690" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Summary - Terra" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="454">
   <si>
     <t>Description</t>
   </si>
@@ -1384,6 +1384,27 @@
       </rPr>
       <t>WARNING: this expects actual address, NOT an offset</t>
     </r>
+  </si>
+  <si>
+    <t>Yield</t>
+  </si>
+  <si>
+    <t>YIELD</t>
+  </si>
+  <si>
+    <t>Execution will immediately terminate. Manual reset of VM is required.</t>
+  </si>
+  <si>
+    <t>Virtual machine will pause execution at this point when yielding is requested from the host</t>
+  </si>
+  <si>
+    <t>Pause</t>
+  </si>
+  <si>
+    <t>PAUSE</t>
+  </si>
+  <si>
+    <t>Virtual machine will pause itself no matter what</t>
   </si>
 </sst>
 </file>
@@ -1731,7 +1752,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="6" applyFont="1"/>
@@ -1881,19 +1902,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="7" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1923,34 +1974,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="4" applyAlignment="1">
@@ -1982,6 +2006,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -2272,7 +2308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="AK11" sqref="AK11"/>
     </sheetView>
   </sheetViews>
@@ -2610,17 +2646,17 @@
       </c>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A10" s="62">
+      <c r="A10" s="72">
         <v>1</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="61" t="s">
+      <c r="D10" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
+      <c r="E10" s="81"/>
+      <c r="F10" s="81"/>
       <c r="G10" s="11">
         <v>0</v>
       </c>
@@ -2633,21 +2669,21 @@
       <c r="J10" s="11">
         <v>0</v>
       </c>
-      <c r="K10" s="71" t="s">
+      <c r="K10" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="L10" s="71"/>
-      <c r="M10" s="71"/>
-      <c r="N10" s="71" t="s">
+      <c r="L10" s="57"/>
+      <c r="M10" s="57"/>
+      <c r="N10" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="O10" s="71"/>
-      <c r="P10" s="71"/>
-      <c r="Q10" s="71" t="s">
+      <c r="O10" s="57"/>
+      <c r="P10" s="57"/>
+      <c r="Q10" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="R10" s="71"/>
-      <c r="S10" s="71"/>
+      <c r="R10" s="57"/>
+      <c r="S10" s="57"/>
       <c r="T10" s="12">
         <v>0</v>
       </c>
@@ -2678,28 +2714,28 @@
       <c r="AC10" s="6">
         <v>0</v>
       </c>
-      <c r="AD10" s="71" t="s">
+      <c r="AD10" s="57" t="s">
         <v>330</v>
       </c>
-      <c r="AE10" s="71"/>
-      <c r="AF10" s="71"/>
-      <c r="AG10" s="71"/>
-      <c r="AH10" s="71"/>
-      <c r="AI10" s="71"/>
+      <c r="AE10" s="57"/>
+      <c r="AF10" s="57"/>
+      <c r="AG10" s="57"/>
+      <c r="AH10" s="57"/>
+      <c r="AI10" s="57"/>
       <c r="AK10" s="10" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A11" s="63"/>
+      <c r="A11" s="73"/>
       <c r="B11" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="D11" s="60" t="s">
+      <c r="D11" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
       <c r="G11" s="18">
         <v>0</v>
       </c>
@@ -2717,14 +2753,14 @@
       </c>
       <c r="L11" s="59"/>
       <c r="M11" s="59"/>
-      <c r="N11" s="58" t="s">
+      <c r="N11" s="60" t="s">
         <v>150</v>
       </c>
-      <c r="O11" s="58"/>
-      <c r="P11" s="58"/>
-      <c r="Q11" s="58"/>
-      <c r="R11" s="58"/>
-      <c r="S11" s="58"/>
+      <c r="O11" s="60"/>
+      <c r="P11" s="60"/>
+      <c r="Q11" s="60"/>
+      <c r="R11" s="60"/>
+      <c r="S11" s="60"/>
       <c r="T11" s="12">
         <v>0</v>
       </c>
@@ -2778,15 +2814,15 @@
       </c>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A12" s="63"/>
+      <c r="A12" s="73"/>
       <c r="B12" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D12" s="60" t="s">
+      <c r="D12" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="60"/>
-      <c r="F12" s="60"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="70"/>
       <c r="G12" s="18">
         <v>0</v>
       </c>
@@ -2799,21 +2835,21 @@
       <c r="J12" s="18">
         <v>0</v>
       </c>
-      <c r="K12" s="67" t="s">
+      <c r="K12" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="L12" s="67"/>
-      <c r="M12" s="67"/>
-      <c r="N12" s="67" t="s">
+      <c r="L12" s="77"/>
+      <c r="M12" s="77"/>
+      <c r="N12" s="77" t="s">
         <v>149</v>
       </c>
-      <c r="O12" s="67"/>
-      <c r="P12" s="67"/>
-      <c r="Q12" s="57" t="s">
+      <c r="O12" s="77"/>
+      <c r="P12" s="77"/>
+      <c r="Q12" s="71" t="s">
         <v>150</v>
       </c>
-      <c r="R12" s="57"/>
-      <c r="S12" s="57"/>
+      <c r="R12" s="71"/>
+      <c r="S12" s="71"/>
       <c r="T12" s="12">
         <v>0</v>
       </c>
@@ -2867,15 +2903,15 @@
       </c>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A13" s="63"/>
+      <c r="A13" s="73"/>
       <c r="B13" s="33" t="s">
         <v>436</v>
       </c>
-      <c r="D13" s="60" t="s">
+      <c r="D13" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="60"/>
-      <c r="F13" s="60"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="70"/>
       <c r="G13" s="31">
         <v>0</v>
       </c>
@@ -2888,21 +2924,21 @@
       <c r="J13" s="31">
         <v>0</v>
       </c>
-      <c r="K13" s="56" t="s">
+      <c r="K13" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="L13" s="56"/>
-      <c r="M13" s="56"/>
-      <c r="N13" s="56" t="s">
+      <c r="L13" s="58"/>
+      <c r="M13" s="58"/>
+      <c r="N13" s="58" t="s">
         <v>327</v>
       </c>
-      <c r="O13" s="56"/>
-      <c r="P13" s="56"/>
-      <c r="Q13" s="57" t="s">
+      <c r="O13" s="58"/>
+      <c r="P13" s="58"/>
+      <c r="Q13" s="71" t="s">
         <v>150</v>
       </c>
-      <c r="R13" s="57"/>
-      <c r="S13" s="57"/>
+      <c r="R13" s="71"/>
+      <c r="S13" s="71"/>
       <c r="T13" s="32">
         <v>0</v>
       </c>
@@ -2956,15 +2992,15 @@
       </c>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A14" s="64"/>
+      <c r="A14" s="74"/>
       <c r="B14" s="47" t="s">
         <v>437</v>
       </c>
-      <c r="D14" s="60" t="s">
+      <c r="D14" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="60"/>
-      <c r="F14" s="60"/>
+      <c r="E14" s="70"/>
+      <c r="F14" s="70"/>
       <c r="G14" s="50">
         <v>0</v>
       </c>
@@ -2977,21 +3013,21 @@
       <c r="J14" s="50">
         <v>0</v>
       </c>
-      <c r="K14" s="56" t="s">
+      <c r="K14" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="L14" s="56"/>
-      <c r="M14" s="56"/>
-      <c r="N14" s="56" t="s">
+      <c r="L14" s="58"/>
+      <c r="M14" s="58"/>
+      <c r="N14" s="58" t="s">
         <v>327</v>
       </c>
-      <c r="O14" s="56"/>
-      <c r="P14" s="56"/>
-      <c r="Q14" s="57" t="s">
+      <c r="O14" s="58"/>
+      <c r="P14" s="58"/>
+      <c r="Q14" s="71" t="s">
         <v>150</v>
       </c>
-      <c r="R14" s="57"/>
-      <c r="S14" s="57"/>
+      <c r="R14" s="71"/>
+      <c r="S14" s="71"/>
       <c r="T14" s="49">
         <v>0</v>
       </c>
@@ -3051,11 +3087,11 @@
       <c r="B15" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="D15" s="60" t="s">
+      <c r="D15" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="60"/>
-      <c r="F15" s="60"/>
+      <c r="E15" s="70"/>
+      <c r="F15" s="70"/>
       <c r="G15" s="6">
         <v>0</v>
       </c>
@@ -3068,21 +3104,21 @@
       <c r="J15" s="12">
         <v>0</v>
       </c>
-      <c r="K15" s="56" t="s">
+      <c r="K15" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="L15" s="56"/>
-      <c r="M15" s="56"/>
-      <c r="N15" s="56" t="s">
+      <c r="L15" s="58"/>
+      <c r="M15" s="58"/>
+      <c r="N15" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="O15" s="56"/>
-      <c r="P15" s="56"/>
-      <c r="Q15" s="56" t="s">
+      <c r="O15" s="58"/>
+      <c r="P15" s="58"/>
+      <c r="Q15" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="R15" s="56"/>
-      <c r="S15" s="56"/>
+      <c r="R15" s="58"/>
+      <c r="S15" s="58"/>
       <c r="T15" s="6">
         <v>0</v>
       </c>
@@ -3122,10 +3158,10 @@
       <c r="AF15" s="6">
         <v>0</v>
       </c>
-      <c r="AG15" s="60" t="s">
+      <c r="AG15" s="70" t="s">
         <v>163</v>
       </c>
-      <c r="AH15" s="60"/>
+      <c r="AH15" s="70"/>
       <c r="AI15" s="22" t="s">
         <v>84</v>
       </c>
@@ -3143,11 +3179,11 @@
       <c r="B16" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D16" s="60" t="s">
+      <c r="D16" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="60"/>
-      <c r="F16" s="60"/>
+      <c r="E16" s="70"/>
+      <c r="F16" s="70"/>
       <c r="G16" s="6">
         <v>0</v>
       </c>
@@ -3160,31 +3196,31 @@
       <c r="J16" s="12">
         <v>0</v>
       </c>
-      <c r="K16" s="56" t="s">
+      <c r="K16" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="L16" s="56"/>
-      <c r="M16" s="56"/>
-      <c r="N16" s="56" t="s">
+      <c r="L16" s="58"/>
+      <c r="M16" s="58"/>
+      <c r="N16" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="O16" s="56"/>
-      <c r="P16" s="56"/>
-      <c r="Q16" s="56" t="s">
+      <c r="O16" s="58"/>
+      <c r="P16" s="58"/>
+      <c r="Q16" s="58" t="s">
         <v>124</v>
       </c>
-      <c r="R16" s="56"/>
-      <c r="S16" s="56"/>
-      <c r="T16" s="56" t="s">
+      <c r="R16" s="58"/>
+      <c r="S16" s="58"/>
+      <c r="T16" s="58" t="s">
         <v>164</v>
       </c>
-      <c r="U16" s="56"/>
-      <c r="V16" s="56"/>
-      <c r="W16" s="56" t="s">
+      <c r="U16" s="58"/>
+      <c r="V16" s="58"/>
+      <c r="W16" s="58" t="s">
         <v>165</v>
       </c>
-      <c r="X16" s="56"/>
-      <c r="Y16" s="56"/>
+      <c r="X16" s="58"/>
+      <c r="Y16" s="58"/>
       <c r="Z16" s="6">
         <v>0</v>
       </c>
@@ -3226,11 +3262,11 @@
       <c r="B17" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="D17" s="60" t="s">
+      <c r="D17" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="60"/>
-      <c r="F17" s="60"/>
+      <c r="E17" s="70"/>
+      <c r="F17" s="70"/>
       <c r="G17" s="6">
         <v>0</v>
       </c>
@@ -3243,16 +3279,16 @@
       <c r="J17" s="12">
         <v>1</v>
       </c>
-      <c r="K17" s="56" t="s">
+      <c r="K17" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="L17" s="56"/>
-      <c r="M17" s="56"/>
-      <c r="N17" s="56" t="s">
+      <c r="L17" s="58"/>
+      <c r="M17" s="58"/>
+      <c r="N17" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="O17" s="56"/>
-      <c r="P17" s="56"/>
+      <c r="O17" s="58"/>
+      <c r="P17" s="58"/>
       <c r="Q17" s="6">
         <v>0</v>
       </c>
@@ -3315,17 +3351,17 @@
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A18" s="70">
+      <c r="A18" s="80">
         <v>2</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="D18" s="60" t="s">
+      <c r="D18" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="60"/>
-      <c r="F18" s="60"/>
+      <c r="E18" s="70"/>
+      <c r="F18" s="70"/>
       <c r="G18" s="6">
         <v>0</v>
       </c>
@@ -3338,16 +3374,16 @@
       <c r="J18" s="12">
         <v>1</v>
       </c>
-      <c r="K18" s="56" t="s">
+      <c r="K18" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="L18" s="56"/>
-      <c r="M18" s="56"/>
-      <c r="N18" s="56" t="s">
+      <c r="L18" s="58"/>
+      <c r="M18" s="58"/>
+      <c r="N18" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="O18" s="56"/>
-      <c r="P18" s="56"/>
+      <c r="O18" s="58"/>
+      <c r="P18" s="58"/>
       <c r="Q18" s="6">
         <v>0</v>
       </c>
@@ -3381,30 +3417,30 @@
       <c r="AA18" s="6">
         <v>0</v>
       </c>
-      <c r="AB18" s="56" t="s">
+      <c r="AB18" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="AC18" s="56"/>
-      <c r="AD18" s="56"/>
-      <c r="AE18" s="56"/>
-      <c r="AF18" s="56"/>
-      <c r="AG18" s="56"/>
-      <c r="AH18" s="56"/>
-      <c r="AI18" s="56"/>
+      <c r="AC18" s="58"/>
+      <c r="AD18" s="58"/>
+      <c r="AE18" s="58"/>
+      <c r="AF18" s="58"/>
+      <c r="AG18" s="58"/>
+      <c r="AH18" s="58"/>
+      <c r="AI18" s="58"/>
       <c r="AK18" s="10" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A19" s="70"/>
+      <c r="A19" s="80"/>
       <c r="B19" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D19" s="60" t="s">
+      <c r="D19" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="60"/>
-      <c r="F19" s="60"/>
+      <c r="E19" s="70"/>
+      <c r="F19" s="70"/>
       <c r="G19" s="6">
         <v>0</v>
       </c>
@@ -3417,16 +3453,16 @@
       <c r="J19" s="12">
         <v>1</v>
       </c>
-      <c r="K19" s="56" t="s">
+      <c r="K19" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="L19" s="56"/>
-      <c r="M19" s="56"/>
-      <c r="N19" s="56" t="s">
+      <c r="L19" s="58"/>
+      <c r="M19" s="58"/>
+      <c r="N19" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="O19" s="56"/>
-      <c r="P19" s="56"/>
+      <c r="O19" s="58"/>
+      <c r="P19" s="58"/>
       <c r="Q19" s="6">
         <v>1</v>
       </c>
@@ -3436,38 +3472,38 @@
       <c r="S19" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="T19" s="56" t="s">
+      <c r="T19" s="58" t="s">
         <v>145</v>
       </c>
-      <c r="U19" s="56"/>
-      <c r="V19" s="56"/>
-      <c r="W19" s="56"/>
-      <c r="X19" s="56"/>
-      <c r="Y19" s="56"/>
-      <c r="Z19" s="56"/>
-      <c r="AA19" s="56"/>
-      <c r="AB19" s="56"/>
-      <c r="AC19" s="56"/>
-      <c r="AD19" s="56"/>
-      <c r="AE19" s="56"/>
-      <c r="AF19" s="56"/>
-      <c r="AG19" s="56"/>
-      <c r="AH19" s="56"/>
-      <c r="AI19" s="56"/>
+      <c r="U19" s="58"/>
+      <c r="V19" s="58"/>
+      <c r="W19" s="58"/>
+      <c r="X19" s="58"/>
+      <c r="Y19" s="58"/>
+      <c r="Z19" s="58"/>
+      <c r="AA19" s="58"/>
+      <c r="AB19" s="58"/>
+      <c r="AC19" s="58"/>
+      <c r="AD19" s="58"/>
+      <c r="AE19" s="58"/>
+      <c r="AF19" s="58"/>
+      <c r="AG19" s="58"/>
+      <c r="AH19" s="58"/>
+      <c r="AI19" s="58"/>
       <c r="AK19" s="10" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A20" s="70"/>
+      <c r="A20" s="80"/>
       <c r="B20" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="D20" s="60" t="s">
+      <c r="D20" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="60"/>
-      <c r="F20" s="60"/>
+      <c r="E20" s="70"/>
+      <c r="F20" s="70"/>
       <c r="G20" s="6">
         <v>0</v>
       </c>
@@ -3480,16 +3516,16 @@
       <c r="J20" s="12">
         <v>1</v>
       </c>
-      <c r="K20" s="56" t="s">
+      <c r="K20" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="L20" s="56"/>
-      <c r="M20" s="56"/>
-      <c r="N20" s="56" t="s">
+      <c r="L20" s="58"/>
+      <c r="M20" s="58"/>
+      <c r="N20" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="O20" s="56"/>
-      <c r="P20" s="56"/>
+      <c r="O20" s="58"/>
+      <c r="P20" s="58"/>
       <c r="Q20" s="6">
         <v>1</v>
       </c>
@@ -3499,38 +3535,38 @@
       <c r="S20" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="T20" s="56" t="s">
+      <c r="T20" s="58" t="s">
         <v>146</v>
       </c>
-      <c r="U20" s="56"/>
-      <c r="V20" s="56"/>
-      <c r="W20" s="56"/>
-      <c r="X20" s="56"/>
-      <c r="Y20" s="56"/>
-      <c r="Z20" s="56"/>
-      <c r="AA20" s="56"/>
-      <c r="AB20" s="56"/>
-      <c r="AC20" s="56"/>
-      <c r="AD20" s="56"/>
-      <c r="AE20" s="56"/>
-      <c r="AF20" s="56"/>
-      <c r="AG20" s="56"/>
-      <c r="AH20" s="56"/>
-      <c r="AI20" s="56"/>
+      <c r="U20" s="58"/>
+      <c r="V20" s="58"/>
+      <c r="W20" s="58"/>
+      <c r="X20" s="58"/>
+      <c r="Y20" s="58"/>
+      <c r="Z20" s="58"/>
+      <c r="AA20" s="58"/>
+      <c r="AB20" s="58"/>
+      <c r="AC20" s="58"/>
+      <c r="AD20" s="58"/>
+      <c r="AE20" s="58"/>
+      <c r="AF20" s="58"/>
+      <c r="AG20" s="58"/>
+      <c r="AH20" s="58"/>
+      <c r="AI20" s="58"/>
       <c r="AK20" s="10" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A21" s="70"/>
+      <c r="A21" s="80"/>
       <c r="B21" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="D21" s="60" t="s">
+      <c r="D21" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="E21" s="60"/>
-      <c r="F21" s="60"/>
+      <c r="E21" s="70"/>
+      <c r="F21" s="70"/>
       <c r="G21" s="6">
         <v>0</v>
       </c>
@@ -3543,35 +3579,35 @@
       <c r="J21" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="K21" s="56" t="s">
+      <c r="K21" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="L21" s="56"/>
-      <c r="M21" s="56"/>
-      <c r="N21" s="56" t="s">
+      <c r="L21" s="58"/>
+      <c r="M21" s="58"/>
+      <c r="N21" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="O21" s="56"/>
-      <c r="P21" s="56"/>
-      <c r="Q21" s="56"/>
-      <c r="R21" s="56"/>
-      <c r="S21" s="56"/>
-      <c r="T21" s="56"/>
-      <c r="U21" s="56"/>
-      <c r="V21" s="56"/>
-      <c r="W21" s="56"/>
-      <c r="X21" s="56"/>
-      <c r="Y21" s="56"/>
-      <c r="Z21" s="56"/>
-      <c r="AA21" s="56"/>
-      <c r="AB21" s="56"/>
-      <c r="AC21" s="56"/>
-      <c r="AD21" s="56"/>
-      <c r="AE21" s="56"/>
-      <c r="AF21" s="56"/>
-      <c r="AG21" s="56"/>
-      <c r="AH21" s="56"/>
-      <c r="AI21" s="56"/>
+      <c r="O21" s="58"/>
+      <c r="P21" s="58"/>
+      <c r="Q21" s="58"/>
+      <c r="R21" s="58"/>
+      <c r="S21" s="58"/>
+      <c r="T21" s="58"/>
+      <c r="U21" s="58"/>
+      <c r="V21" s="58"/>
+      <c r="W21" s="58"/>
+      <c r="X21" s="58"/>
+      <c r="Y21" s="58"/>
+      <c r="Z21" s="58"/>
+      <c r="AA21" s="58"/>
+      <c r="AB21" s="58"/>
+      <c r="AC21" s="58"/>
+      <c r="AD21" s="58"/>
+      <c r="AE21" s="58"/>
+      <c r="AF21" s="58"/>
+      <c r="AG21" s="58"/>
+      <c r="AH21" s="58"/>
+      <c r="AI21" s="58"/>
       <c r="AK21" s="10" t="s">
         <v>172</v>
       </c>
@@ -3583,11 +3619,11 @@
       <c r="B22" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="60" t="s">
+      <c r="D22" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="60"/>
-      <c r="F22" s="60"/>
+      <c r="E22" s="70"/>
+      <c r="F22" s="70"/>
       <c r="G22" s="6">
         <v>0</v>
       </c>
@@ -3600,51 +3636,51 @@
       <c r="J22" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="K22" s="56" t="s">
+      <c r="K22" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="L22" s="56"/>
-      <c r="M22" s="56"/>
-      <c r="N22" s="56" t="s">
+      <c r="L22" s="58"/>
+      <c r="M22" s="58"/>
+      <c r="N22" s="58" t="s">
         <v>168</v>
       </c>
-      <c r="O22" s="56"/>
-      <c r="P22" s="56"/>
-      <c r="Q22" s="56"/>
-      <c r="R22" s="56"/>
-      <c r="S22" s="56"/>
-      <c r="T22" s="56"/>
-      <c r="U22" s="56"/>
-      <c r="V22" s="56"/>
-      <c r="W22" s="56"/>
-      <c r="X22" s="56"/>
-      <c r="Y22" s="56"/>
-      <c r="Z22" s="56"/>
-      <c r="AA22" s="56"/>
-      <c r="AB22" s="56"/>
-      <c r="AC22" s="56"/>
-      <c r="AD22" s="56"/>
-      <c r="AE22" s="56"/>
-      <c r="AF22" s="56"/>
-      <c r="AG22" s="56"/>
-      <c r="AH22" s="56"/>
-      <c r="AI22" s="56"/>
+      <c r="O22" s="58"/>
+      <c r="P22" s="58"/>
+      <c r="Q22" s="58"/>
+      <c r="R22" s="58"/>
+      <c r="S22" s="58"/>
+      <c r="T22" s="58"/>
+      <c r="U22" s="58"/>
+      <c r="V22" s="58"/>
+      <c r="W22" s="58"/>
+      <c r="X22" s="58"/>
+      <c r="Y22" s="58"/>
+      <c r="Z22" s="58"/>
+      <c r="AA22" s="58"/>
+      <c r="AB22" s="58"/>
+      <c r="AC22" s="58"/>
+      <c r="AD22" s="58"/>
+      <c r="AE22" s="58"/>
+      <c r="AF22" s="58"/>
+      <c r="AG22" s="58"/>
+      <c r="AH22" s="58"/>
+      <c r="AI22" s="58"/>
       <c r="AK22" s="10" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A23" s="68">
+      <c r="A23" s="78">
         <v>6</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>276</v>
       </c>
-      <c r="D23" s="60" t="s">
+      <c r="D23" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="60"/>
-      <c r="F23" s="60"/>
+      <c r="E23" s="70"/>
+      <c r="F23" s="70"/>
       <c r="G23" s="6">
         <v>1</v>
       </c>
@@ -3657,49 +3693,49 @@
       <c r="J23" s="12">
         <v>0</v>
       </c>
-      <c r="K23" s="58" t="s">
+      <c r="K23" s="60" t="s">
         <v>150</v>
       </c>
-      <c r="L23" s="58"/>
-      <c r="M23" s="58"/>
-      <c r="N23" s="56" t="s">
+      <c r="L23" s="60"/>
+      <c r="M23" s="60"/>
+      <c r="N23" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="O23" s="56"/>
-      <c r="P23" s="56"/>
-      <c r="Q23" s="56"/>
-      <c r="R23" s="56"/>
-      <c r="S23" s="56"/>
-      <c r="T23" s="56"/>
-      <c r="U23" s="56"/>
-      <c r="V23" s="56"/>
-      <c r="W23" s="56"/>
-      <c r="X23" s="56"/>
-      <c r="Y23" s="56"/>
-      <c r="Z23" s="56"/>
-      <c r="AA23" s="56"/>
-      <c r="AB23" s="56"/>
-      <c r="AC23" s="56"/>
-      <c r="AD23" s="56"/>
-      <c r="AE23" s="56"/>
-      <c r="AF23" s="56"/>
-      <c r="AG23" s="56"/>
-      <c r="AH23" s="56"/>
-      <c r="AI23" s="56"/>
+      <c r="O23" s="58"/>
+      <c r="P23" s="58"/>
+      <c r="Q23" s="58"/>
+      <c r="R23" s="58"/>
+      <c r="S23" s="58"/>
+      <c r="T23" s="58"/>
+      <c r="U23" s="58"/>
+      <c r="V23" s="58"/>
+      <c r="W23" s="58"/>
+      <c r="X23" s="58"/>
+      <c r="Y23" s="58"/>
+      <c r="Z23" s="58"/>
+      <c r="AA23" s="58"/>
+      <c r="AB23" s="58"/>
+      <c r="AC23" s="58"/>
+      <c r="AD23" s="58"/>
+      <c r="AE23" s="58"/>
+      <c r="AF23" s="58"/>
+      <c r="AG23" s="58"/>
+      <c r="AH23" s="58"/>
+      <c r="AI23" s="58"/>
       <c r="AK23" s="10" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A24" s="69"/>
+      <c r="A24" s="79"/>
       <c r="B24" s="46" t="s">
         <v>402</v>
       </c>
-      <c r="D24" s="60" t="s">
+      <c r="D24" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="60"/>
-      <c r="F24" s="60"/>
+      <c r="E24" s="70"/>
+      <c r="F24" s="70"/>
       <c r="G24" s="44">
         <v>1</v>
       </c>
@@ -3712,35 +3748,35 @@
       <c r="J24" s="45">
         <v>1</v>
       </c>
-      <c r="K24" s="75" t="s">
+      <c r="K24" s="64" t="s">
         <v>150</v>
       </c>
-      <c r="L24" s="76"/>
-      <c r="M24" s="77"/>
-      <c r="N24" s="56" t="s">
+      <c r="L24" s="65"/>
+      <c r="M24" s="66"/>
+      <c r="N24" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="O24" s="56"/>
-      <c r="P24" s="56"/>
-      <c r="Q24" s="56"/>
-      <c r="R24" s="56"/>
-      <c r="S24" s="56"/>
-      <c r="T24" s="56"/>
-      <c r="U24" s="56"/>
-      <c r="V24" s="56"/>
-      <c r="W24" s="56"/>
-      <c r="X24" s="56"/>
-      <c r="Y24" s="56"/>
-      <c r="Z24" s="56"/>
-      <c r="AA24" s="56"/>
-      <c r="AB24" s="56"/>
-      <c r="AC24" s="56"/>
-      <c r="AD24" s="56"/>
-      <c r="AE24" s="56"/>
-      <c r="AF24" s="56"/>
-      <c r="AG24" s="56"/>
-      <c r="AH24" s="56"/>
-      <c r="AI24" s="56"/>
+      <c r="O24" s="58"/>
+      <c r="P24" s="58"/>
+      <c r="Q24" s="58"/>
+      <c r="R24" s="58"/>
+      <c r="S24" s="58"/>
+      <c r="T24" s="58"/>
+      <c r="U24" s="58"/>
+      <c r="V24" s="58"/>
+      <c r="W24" s="58"/>
+      <c r="X24" s="58"/>
+      <c r="Y24" s="58"/>
+      <c r="Z24" s="58"/>
+      <c r="AA24" s="58"/>
+      <c r="AB24" s="58"/>
+      <c r="AC24" s="58"/>
+      <c r="AD24" s="58"/>
+      <c r="AE24" s="58"/>
+      <c r="AF24" s="58"/>
+      <c r="AG24" s="58"/>
+      <c r="AH24" s="58"/>
+      <c r="AI24" s="58"/>
       <c r="AK24" s="10"/>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
@@ -3750,11 +3786,11 @@
       <c r="B25" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="D25" s="60" t="s">
+      <c r="D25" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="60"/>
-      <c r="F25" s="60"/>
+      <c r="E25" s="70"/>
+      <c r="F25" s="70"/>
       <c r="G25" s="24">
         <v>1</v>
       </c>
@@ -3767,11 +3803,11 @@
       <c r="J25" s="25">
         <v>0</v>
       </c>
-      <c r="K25" s="58" t="s">
+      <c r="K25" s="60" t="s">
         <v>150</v>
       </c>
-      <c r="L25" s="58"/>
-      <c r="M25" s="58"/>
+      <c r="L25" s="60"/>
+      <c r="M25" s="60"/>
       <c r="N25" s="25">
         <v>0</v>
       </c>
@@ -3789,21 +3825,21 @@
       <c r="T25" s="59"/>
       <c r="U25" s="59"/>
       <c r="V25" s="59"/>
-      <c r="W25" s="56" t="s">
+      <c r="W25" s="58" t="s">
         <v>238</v>
       </c>
-      <c r="X25" s="56"/>
-      <c r="Y25" s="56"/>
-      <c r="Z25" s="56"/>
-      <c r="AA25" s="56"/>
-      <c r="AB25" s="56"/>
-      <c r="AC25" s="56"/>
-      <c r="AD25" s="56"/>
-      <c r="AE25" s="56"/>
-      <c r="AF25" s="56"/>
-      <c r="AG25" s="56"/>
-      <c r="AH25" s="56"/>
-      <c r="AI25" s="56"/>
+      <c r="X25" s="58"/>
+      <c r="Y25" s="58"/>
+      <c r="Z25" s="58"/>
+      <c r="AA25" s="58"/>
+      <c r="AB25" s="58"/>
+      <c r="AC25" s="58"/>
+      <c r="AD25" s="58"/>
+      <c r="AE25" s="58"/>
+      <c r="AF25" s="58"/>
+      <c r="AG25" s="58"/>
+      <c r="AH25" s="58"/>
+      <c r="AI25" s="58"/>
       <c r="AK25" s="10" t="s">
         <v>242</v>
       </c>
@@ -3815,11 +3851,11 @@
       <c r="B26" s="46" t="s">
         <v>244</v>
       </c>
-      <c r="D26" s="65" t="s">
+      <c r="D26" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="E26" s="60"/>
-      <c r="F26" s="66"/>
+      <c r="E26" s="70"/>
+      <c r="F26" s="76"/>
       <c r="G26" s="44">
         <v>1</v>
       </c>
@@ -3832,11 +3868,11 @@
       <c r="J26" s="45">
         <v>0</v>
       </c>
-      <c r="K26" s="72" t="s">
+      <c r="K26" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="L26" s="73"/>
-      <c r="M26" s="74"/>
+      <c r="L26" s="62"/>
+      <c r="M26" s="63"/>
       <c r="N26" s="45">
         <v>0</v>
       </c>
@@ -3879,16 +3915,16 @@
       <c r="AA26" s="44">
         <v>0</v>
       </c>
-      <c r="AB26" s="78" t="s">
+      <c r="AB26" s="67" t="s">
         <v>241</v>
       </c>
-      <c r="AC26" s="79"/>
-      <c r="AD26" s="79"/>
-      <c r="AE26" s="79"/>
-      <c r="AF26" s="79"/>
-      <c r="AG26" s="79"/>
-      <c r="AH26" s="79"/>
-      <c r="AI26" s="80"/>
+      <c r="AC26" s="68"/>
+      <c r="AD26" s="68"/>
+      <c r="AE26" s="68"/>
+      <c r="AF26" s="68"/>
+      <c r="AG26" s="68"/>
+      <c r="AH26" s="68"/>
+      <c r="AI26" s="69"/>
       <c r="AK26" s="10" t="s">
         <v>243</v>
       </c>
@@ -3900,11 +3936,11 @@
       <c r="B27" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D27" s="60" t="s">
+      <c r="D27" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="E27" s="60"/>
-      <c r="F27" s="60"/>
+      <c r="E27" s="70"/>
+      <c r="F27" s="70"/>
       <c r="G27" s="6">
         <v>1</v>
       </c>
@@ -3917,11 +3953,11 @@
       <c r="J27" s="6">
         <v>1</v>
       </c>
-      <c r="K27" s="56" t="s">
+      <c r="K27" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="L27" s="56"/>
-      <c r="M27" s="56"/>
+      <c r="L27" s="58"/>
+      <c r="M27" s="58"/>
       <c r="N27" s="6">
         <v>0</v>
       </c>
@@ -3964,16 +4000,16 @@
       <c r="AA27" s="6">
         <v>0</v>
       </c>
-      <c r="AB27" s="56" t="s">
+      <c r="AB27" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="AC27" s="56"/>
-      <c r="AD27" s="56"/>
-      <c r="AE27" s="56"/>
-      <c r="AF27" s="56"/>
-      <c r="AG27" s="56"/>
-      <c r="AH27" s="56"/>
-      <c r="AI27" s="56"/>
+      <c r="AC27" s="58"/>
+      <c r="AD27" s="58"/>
+      <c r="AE27" s="58"/>
+      <c r="AF27" s="58"/>
+      <c r="AG27" s="58"/>
+      <c r="AH27" s="58"/>
+      <c r="AI27" s="58"/>
       <c r="AK27" s="10" t="s">
         <v>83</v>
       </c>
@@ -3985,11 +4021,11 @@
       <c r="B28" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D28" s="60" t="s">
+      <c r="D28" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="E28" s="60"/>
-      <c r="F28" s="60"/>
+      <c r="E28" s="70"/>
+      <c r="F28" s="70"/>
       <c r="G28" s="6">
         <v>1</v>
       </c>
@@ -4002,11 +4038,11 @@
       <c r="J28" s="6">
         <v>1</v>
       </c>
-      <c r="K28" s="56" t="s">
+      <c r="K28" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="L28" s="56"/>
-      <c r="M28" s="56"/>
+      <c r="L28" s="58"/>
+      <c r="M28" s="58"/>
       <c r="N28" s="6">
         <v>0</v>
       </c>
@@ -4049,16 +4085,16 @@
       <c r="AA28" s="6">
         <v>1</v>
       </c>
-      <c r="AB28" s="56" t="s">
+      <c r="AB28" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="AC28" s="56"/>
-      <c r="AD28" s="56"/>
-      <c r="AE28" s="56"/>
-      <c r="AF28" s="56"/>
-      <c r="AG28" s="56"/>
-      <c r="AH28" s="56"/>
-      <c r="AI28" s="56"/>
+      <c r="AC28" s="58"/>
+      <c r="AD28" s="58"/>
+      <c r="AE28" s="58"/>
+      <c r="AF28" s="58"/>
+      <c r="AG28" s="58"/>
+      <c r="AH28" s="58"/>
+      <c r="AI28" s="58"/>
       <c r="AK28" s="10" t="s">
         <v>169</v>
       </c>
@@ -4070,11 +4106,11 @@
       <c r="B29" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D29" s="60" t="s">
+      <c r="D29" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="E29" s="60"/>
-      <c r="F29" s="60"/>
+      <c r="E29" s="70"/>
+      <c r="F29" s="70"/>
       <c r="G29" s="6">
         <v>1</v>
       </c>
@@ -4087,11 +4123,11 @@
       <c r="J29" s="6">
         <v>1</v>
       </c>
-      <c r="K29" s="56" t="s">
+      <c r="K29" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="L29" s="56"/>
-      <c r="M29" s="56"/>
+      <c r="L29" s="58"/>
+      <c r="M29" s="58"/>
       <c r="N29" s="6">
         <v>0</v>
       </c>
@@ -4167,11 +4203,11 @@
       <c r="B30" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D30" s="60" t="s">
+      <c r="D30" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
+      <c r="E30" s="70"/>
+      <c r="F30" s="70"/>
       <c r="G30" s="6">
         <v>1</v>
       </c>
@@ -4235,16 +4271,16 @@
       <c r="AA30" s="6">
         <v>1</v>
       </c>
-      <c r="AB30" s="56" t="s">
+      <c r="AB30" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="AC30" s="56"/>
-      <c r="AD30" s="56"/>
-      <c r="AE30" s="56"/>
-      <c r="AF30" s="56"/>
-      <c r="AG30" s="56"/>
-      <c r="AH30" s="56"/>
-      <c r="AI30" s="56"/>
+      <c r="AC30" s="58"/>
+      <c r="AD30" s="58"/>
+      <c r="AE30" s="58"/>
+      <c r="AF30" s="58"/>
+      <c r="AG30" s="58"/>
+      <c r="AH30" s="58"/>
+      <c r="AI30" s="58"/>
     </row>
     <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B31" s="55" t="s">
@@ -4931,6 +4967,68 @@
     </row>
   </sheetData>
   <mergeCells count="78">
+    <mergeCell ref="T19:AI19"/>
+    <mergeCell ref="Q13:S13"/>
+    <mergeCell ref="W25:AI25"/>
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="Q25:V25"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="Q14:S14"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="AB18:AI18"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="N16:P16"/>
+    <mergeCell ref="Q16:S16"/>
+    <mergeCell ref="T16:V16"/>
+    <mergeCell ref="AB30:AI30"/>
+    <mergeCell ref="N21:AI21"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="N15:P15"/>
+    <mergeCell ref="Q15:S15"/>
+    <mergeCell ref="N23:AI23"/>
+    <mergeCell ref="N22:AI22"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="K27:M27"/>
+    <mergeCell ref="T20:AI20"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="K28:M28"/>
+    <mergeCell ref="AB28:AI28"/>
+    <mergeCell ref="K29:M29"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="N12:P12"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="A18:A21"/>
     <mergeCell ref="AD10:AI10"/>
     <mergeCell ref="K10:M10"/>
     <mergeCell ref="N10:P10"/>
@@ -4947,68 +5045,6 @@
     <mergeCell ref="AG15:AH15"/>
     <mergeCell ref="W16:Y16"/>
     <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="N13:P13"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="N18:P18"/>
-    <mergeCell ref="N19:P19"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="N12:P12"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="AB30:AI30"/>
-    <mergeCell ref="N21:AI21"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="K15:M15"/>
-    <mergeCell ref="N15:P15"/>
-    <mergeCell ref="Q15:S15"/>
-    <mergeCell ref="N23:AI23"/>
-    <mergeCell ref="N22:AI22"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="K27:M27"/>
-    <mergeCell ref="T20:AI20"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="K28:M28"/>
-    <mergeCell ref="AB28:AI28"/>
-    <mergeCell ref="K29:M29"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="T19:AI19"/>
-    <mergeCell ref="Q13:S13"/>
-    <mergeCell ref="W25:AI25"/>
-    <mergeCell ref="K25:M25"/>
-    <mergeCell ref="Q25:V25"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="N14:P14"/>
-    <mergeCell ref="Q14:S14"/>
-    <mergeCell ref="N20:P20"/>
-    <mergeCell ref="AB18:AI18"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="N16:P16"/>
-    <mergeCell ref="Q16:S16"/>
-    <mergeCell ref="T16:V16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5241,25 +5277,25 @@
       <c r="F10" s="29">
         <v>0</v>
       </c>
-      <c r="G10" s="56" t="s">
+      <c r="G10" s="58" t="s">
         <v>331</v>
       </c>
-      <c r="H10" s="56"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="56"/>
-      <c r="L10" s="56" t="s">
+      <c r="H10" s="58"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="58"/>
+      <c r="L10" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="M10" s="56"/>
-      <c r="N10" s="56" t="s">
+      <c r="M10" s="58"/>
+      <c r="N10" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="O10" s="56"/>
-      <c r="P10" s="56" t="s">
+      <c r="O10" s="58"/>
+      <c r="P10" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="Q10" s="56"/>
+      <c r="Q10" s="58"/>
       <c r="R10" s="29">
         <v>0</v>
       </c>
@@ -5298,14 +5334,14 @@
       <c r="K11" s="32">
         <v>0</v>
       </c>
-      <c r="L11" s="56" t="s">
+      <c r="L11" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="M11" s="56"/>
-      <c r="N11" s="56" t="s">
+      <c r="M11" s="58"/>
+      <c r="N11" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="O11" s="56"/>
+      <c r="O11" s="58"/>
       <c r="P11" s="29">
         <v>0</v>
       </c>
@@ -5351,14 +5387,14 @@
       <c r="K12" s="32">
         <v>0</v>
       </c>
-      <c r="L12" s="56" t="s">
+      <c r="L12" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="M12" s="56"/>
-      <c r="N12" s="56" t="s">
+      <c r="M12" s="58"/>
+      <c r="N12" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="O12" s="56"/>
+      <c r="O12" s="58"/>
       <c r="P12" s="32">
         <v>1</v>
       </c>
@@ -5518,11 +5554,11 @@
       <c r="G16" s="32">
         <v>1</v>
       </c>
-      <c r="H16" s="81" t="s">
+      <c r="H16" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="I16" s="81"/>
-      <c r="J16" s="81"/>
+      <c r="I16" s="82"/>
+      <c r="J16" s="82"/>
       <c r="K16" s="32">
         <v>1</v>
       </c>
@@ -5541,7 +5577,7 @@
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="70">
+      <c r="A17" s="80">
         <v>13</v>
       </c>
       <c r="B17" s="33" t="s">
@@ -5596,7 +5632,7 @@
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="70"/>
+      <c r="A18" s="80"/>
       <c r="B18" s="33" t="s">
         <v>340</v>
       </c>
@@ -5649,7 +5685,7 @@
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="70"/>
+      <c r="A19" s="80"/>
       <c r="B19" s="33" t="s">
         <v>336</v>
       </c>
@@ -5665,12 +5701,12 @@
       <c r="G19" s="32">
         <v>0</v>
       </c>
-      <c r="H19" s="58" t="s">
+      <c r="H19" s="60" t="s">
         <v>329</v>
       </c>
-      <c r="I19" s="58"/>
-      <c r="J19" s="58"/>
-      <c r="K19" s="58"/>
+      <c r="I19" s="60"/>
+      <c r="J19" s="60"/>
+      <c r="K19" s="60"/>
       <c r="L19" s="32">
         <v>0</v>
       </c>
@@ -5895,6 +5931,18 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="L13:S13"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="L14:S14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="N11:O11"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="J18:K18"/>
@@ -5905,18 +5953,6 @@
     <mergeCell ref="J17:K17"/>
     <mergeCell ref="H16:J16"/>
     <mergeCell ref="H15:I15"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="L13:S13"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="L14:S14"/>
-    <mergeCell ref="H14:I14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5925,10 +5961,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q55"/>
+  <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="L57" sqref="L57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5959,20 +5995,20 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="82" t="s">
+      <c r="A2" s="83" t="s">
         <v>153</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83"/>
-      <c r="J2" s="83"/>
-      <c r="K2" s="83"/>
-      <c r="L2" s="84"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="85"/>
       <c r="M2" s="20" t="s">
         <v>152</v>
       </c>
@@ -7921,7 +7957,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>39</v>
       </c>
@@ -7962,7 +7998,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>40</v>
       </c>
@@ -8003,7 +8039,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>41</v>
       </c>
@@ -8044,7 +8080,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>42</v>
       </c>
@@ -8085,7 +8121,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>43</v>
       </c>
@@ -8126,7 +8162,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="16" t="s">
         <v>78</v>
       </c>
@@ -8161,18 +8197,84 @@
       <c r="L54" s="17" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" s="7"/>
+      <c r="O54" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
+        <v>447</v>
+      </c>
       <c r="B55" s="6"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
-      <c r="E55" s="6"/>
-      <c r="F55" s="6"/>
-      <c r="G55" s="6"/>
-      <c r="H55" s="6"/>
-      <c r="I55" s="24"/>
-      <c r="J55" s="24"/>
+      <c r="C55" s="6">
+        <v>1</v>
+      </c>
+      <c r="D55" s="6">
+        <v>0</v>
+      </c>
+      <c r="E55" s="6">
+        <v>0</v>
+      </c>
+      <c r="F55" s="6">
+        <v>0</v>
+      </c>
+      <c r="G55" s="6">
+        <v>0</v>
+      </c>
+      <c r="H55" s="6">
+        <v>0</v>
+      </c>
+      <c r="I55" s="56">
+        <f t="shared" ref="I55:I56" si="7">_xlfn.DECIMAL(CONCATENATE(C55,D55,E55,F55,G55,H55),2)</f>
+        <v>32</v>
+      </c>
+      <c r="J55" s="56" t="str">
+        <f t="shared" ref="J55:J56" si="8">DEC2HEX(I55,2)&amp;"h"</f>
+        <v>20h</v>
+      </c>
+      <c r="L55" t="s">
+        <v>448</v>
+      </c>
+      <c r="O55" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A56" s="92" t="s">
+        <v>451</v>
+      </c>
+      <c r="C56" s="93">
+        <v>1</v>
+      </c>
+      <c r="D56" s="93">
+        <v>0</v>
+      </c>
+      <c r="E56" s="93">
+        <v>1</v>
+      </c>
+      <c r="F56" s="93">
+        <v>0</v>
+      </c>
+      <c r="G56" s="93">
+        <v>1</v>
+      </c>
+      <c r="H56" s="94">
+        <v>0</v>
+      </c>
+      <c r="I56" s="95">
+        <f t="shared" si="7"/>
+        <v>42</v>
+      </c>
+      <c r="J56" s="95" t="str">
+        <f t="shared" si="8"/>
+        <v>2Ah</v>
+      </c>
+      <c r="L56" t="s">
+        <v>452</v>
+      </c>
+      <c r="O56" t="s">
+        <v>453</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8214,19 +8316,19 @@
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="82" t="s">
+      <c r="A2" s="83" t="s">
         <v>153</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83"/>
-      <c r="J2" s="83"/>
-      <c r="K2" s="84"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="85"/>
       <c r="L2" s="20" t="s">
         <v>152</v>
       </c>
@@ -9042,7 +9144,7 @@
   <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10106,16 +10208,16 @@
       <c r="Z5" s="41">
         <v>0</v>
       </c>
-      <c r="AA5" s="67" t="s">
+      <c r="AA5" s="77" t="s">
         <v>81</v>
       </c>
-      <c r="AB5" s="67"/>
-      <c r="AC5" s="67"/>
-      <c r="AD5" s="67"/>
-      <c r="AE5" s="67"/>
-      <c r="AF5" s="67"/>
-      <c r="AG5" s="67"/>
-      <c r="AH5" s="67"/>
+      <c r="AB5" s="77"/>
+      <c r="AC5" s="77"/>
+      <c r="AD5" s="77"/>
+      <c r="AE5" s="77"/>
+      <c r="AF5" s="77"/>
+      <c r="AG5" s="77"/>
+      <c r="AH5" s="77"/>
       <c r="AJ5" s="10" t="s">
         <v>401</v>
       </c>
@@ -10196,18 +10298,18 @@
       <c r="Z6" s="43">
         <v>1</v>
       </c>
-      <c r="AA6" s="57" t="s">
+      <c r="AA6" s="71" t="s">
         <v>150</v>
       </c>
-      <c r="AB6" s="57"/>
-      <c r="AC6" s="57"/>
-      <c r="AD6" s="57"/>
-      <c r="AE6" s="57"/>
-      <c r="AF6" s="67" t="s">
+      <c r="AB6" s="71"/>
+      <c r="AC6" s="71"/>
+      <c r="AD6" s="71"/>
+      <c r="AE6" s="71"/>
+      <c r="AF6" s="77" t="s">
         <v>355</v>
       </c>
-      <c r="AG6" s="67"/>
-      <c r="AH6" s="67"/>
+      <c r="AG6" s="77"/>
+      <c r="AH6" s="77"/>
       <c r="AJ6" s="10" t="s">
         <v>397</v>
       </c>
@@ -10288,16 +10390,16 @@
       <c r="Z7" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="AA7" s="85" t="s">
+      <c r="AA7" s="86" t="s">
         <v>399</v>
       </c>
-      <c r="AB7" s="86"/>
-      <c r="AC7" s="86"/>
-      <c r="AD7" s="86"/>
-      <c r="AE7" s="86"/>
-      <c r="AF7" s="86"/>
-      <c r="AG7" s="86"/>
-      <c r="AH7" s="87"/>
+      <c r="AB7" s="87"/>
+      <c r="AC7" s="87"/>
+      <c r="AD7" s="87"/>
+      <c r="AE7" s="87"/>
+      <c r="AF7" s="87"/>
+      <c r="AG7" s="87"/>
+      <c r="AH7" s="88"/>
       <c r="AJ7" s="10" t="s">
         <v>400</v>
       </c>
@@ -10330,38 +10432,38 @@
       <c r="J8" s="41">
         <v>1</v>
       </c>
-      <c r="K8" s="67" t="s">
+      <c r="K8" s="77" t="s">
         <v>354</v>
       </c>
-      <c r="L8" s="67"/>
-      <c r="M8" s="67"/>
-      <c r="N8" s="67"/>
-      <c r="O8" s="67"/>
-      <c r="P8" s="67" t="s">
+      <c r="L8" s="77"/>
+      <c r="M8" s="77"/>
+      <c r="N8" s="77"/>
+      <c r="O8" s="77"/>
+      <c r="P8" s="77" t="s">
         <v>355</v>
       </c>
-      <c r="Q8" s="67"/>
-      <c r="R8" s="67"/>
-      <c r="S8" s="67" t="s">
+      <c r="Q8" s="77"/>
+      <c r="R8" s="77"/>
+      <c r="S8" s="77" t="s">
         <v>356</v>
       </c>
-      <c r="T8" s="67"/>
-      <c r="U8" s="67"/>
-      <c r="V8" s="67"/>
-      <c r="W8" s="67"/>
-      <c r="X8" s="67"/>
-      <c r="Y8" s="67"/>
-      <c r="Z8" s="67"/>
-      <c r="AA8" s="67" t="s">
+      <c r="T8" s="77"/>
+      <c r="U8" s="77"/>
+      <c r="V8" s="77"/>
+      <c r="W8" s="77"/>
+      <c r="X8" s="77"/>
+      <c r="Y8" s="77"/>
+      <c r="Z8" s="77"/>
+      <c r="AA8" s="77" t="s">
         <v>81</v>
       </c>
-      <c r="AB8" s="67"/>
-      <c r="AC8" s="67"/>
-      <c r="AD8" s="67"/>
-      <c r="AE8" s="67"/>
-      <c r="AF8" s="67"/>
-      <c r="AG8" s="67"/>
-      <c r="AH8" s="67"/>
+      <c r="AB8" s="77"/>
+      <c r="AC8" s="77"/>
+      <c r="AD8" s="77"/>
+      <c r="AE8" s="77"/>
+      <c r="AF8" s="77"/>
+      <c r="AG8" s="77"/>
+      <c r="AH8" s="77"/>
       <c r="AJ8" s="10" t="s">
         <v>382</v>
       </c>
@@ -10394,34 +10496,34 @@
       <c r="J9" s="6">
         <v>0</v>
       </c>
-      <c r="K9" s="88" t="s">
+      <c r="K9" s="89" t="s">
         <v>150</v>
       </c>
-      <c r="L9" s="89"/>
-      <c r="M9" s="78" t="s">
+      <c r="L9" s="90"/>
+      <c r="M9" s="67" t="s">
         <v>404</v>
       </c>
-      <c r="N9" s="79"/>
-      <c r="O9" s="79"/>
-      <c r="P9" s="79"/>
-      <c r="Q9" s="79"/>
-      <c r="R9" s="79"/>
-      <c r="S9" s="79"/>
-      <c r="T9" s="79"/>
-      <c r="U9" s="79"/>
-      <c r="V9" s="79"/>
-      <c r="W9" s="79"/>
-      <c r="X9" s="79"/>
-      <c r="Y9" s="79"/>
-      <c r="Z9" s="79"/>
-      <c r="AA9" s="79"/>
-      <c r="AB9" s="79"/>
-      <c r="AC9" s="79"/>
-      <c r="AD9" s="79"/>
-      <c r="AE9" s="79"/>
-      <c r="AF9" s="79"/>
-      <c r="AG9" s="79"/>
-      <c r="AH9" s="80"/>
+      <c r="N9" s="68"/>
+      <c r="O9" s="68"/>
+      <c r="P9" s="68"/>
+      <c r="Q9" s="68"/>
+      <c r="R9" s="68"/>
+      <c r="S9" s="68"/>
+      <c r="T9" s="68"/>
+      <c r="U9" s="68"/>
+      <c r="V9" s="68"/>
+      <c r="W9" s="68"/>
+      <c r="X9" s="68"/>
+      <c r="Y9" s="68"/>
+      <c r="Z9" s="68"/>
+      <c r="AA9" s="68"/>
+      <c r="AB9" s="68"/>
+      <c r="AC9" s="68"/>
+      <c r="AD9" s="68"/>
+      <c r="AE9" s="68"/>
+      <c r="AF9" s="68"/>
+      <c r="AG9" s="68"/>
+      <c r="AH9" s="69"/>
       <c r="AJ9" s="10" t="s">
         <v>381</v>
       </c>
@@ -10451,35 +10553,35 @@
       <c r="I10" s="45">
         <v>0</v>
       </c>
-      <c r="J10" s="78" t="s">
+      <c r="J10" s="67" t="s">
         <v>406</v>
       </c>
-      <c r="K10" s="79"/>
-      <c r="L10" s="80"/>
-      <c r="M10" s="78" t="s">
+      <c r="K10" s="68"/>
+      <c r="L10" s="69"/>
+      <c r="M10" s="67" t="s">
         <v>404</v>
       </c>
-      <c r="N10" s="79"/>
-      <c r="O10" s="79"/>
-      <c r="P10" s="79"/>
-      <c r="Q10" s="79"/>
-      <c r="R10" s="79"/>
-      <c r="S10" s="79"/>
-      <c r="T10" s="79"/>
-      <c r="U10" s="79"/>
-      <c r="V10" s="79"/>
-      <c r="W10" s="79"/>
-      <c r="X10" s="79"/>
-      <c r="Y10" s="79"/>
-      <c r="Z10" s="79"/>
-      <c r="AA10" s="79"/>
-      <c r="AB10" s="79"/>
-      <c r="AC10" s="79"/>
-      <c r="AD10" s="79"/>
-      <c r="AE10" s="79"/>
-      <c r="AF10" s="79"/>
-      <c r="AG10" s="79"/>
-      <c r="AH10" s="80"/>
+      <c r="N10" s="68"/>
+      <c r="O10" s="68"/>
+      <c r="P10" s="68"/>
+      <c r="Q10" s="68"/>
+      <c r="R10" s="68"/>
+      <c r="S10" s="68"/>
+      <c r="T10" s="68"/>
+      <c r="U10" s="68"/>
+      <c r="V10" s="68"/>
+      <c r="W10" s="68"/>
+      <c r="X10" s="68"/>
+      <c r="Y10" s="68"/>
+      <c r="Z10" s="68"/>
+      <c r="AA10" s="68"/>
+      <c r="AB10" s="68"/>
+      <c r="AC10" s="68"/>
+      <c r="AD10" s="68"/>
+      <c r="AE10" s="68"/>
+      <c r="AF10" s="68"/>
+      <c r="AG10" s="68"/>
+      <c r="AH10" s="69"/>
       <c r="AJ10" s="10" t="s">
         <v>407</v>
       </c>
@@ -10527,37 +10629,37 @@
       <c r="C12" s="6">
         <v>1</v>
       </c>
-      <c r="D12" s="56"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="56"/>
-      <c r="J12" s="56"/>
-      <c r="K12" s="56"/>
-      <c r="L12" s="56"/>
-      <c r="M12" s="56"/>
-      <c r="N12" s="56"/>
-      <c r="O12" s="56"/>
-      <c r="P12" s="56"/>
-      <c r="Q12" s="56"/>
-      <c r="R12" s="56"/>
-      <c r="S12" s="56"/>
-      <c r="T12" s="56"/>
-      <c r="U12" s="56"/>
-      <c r="V12" s="56"/>
-      <c r="W12" s="56"/>
-      <c r="X12" s="56"/>
-      <c r="Y12" s="56"/>
-      <c r="Z12" s="56"/>
-      <c r="AA12" s="56"/>
-      <c r="AB12" s="56"/>
-      <c r="AC12" s="56"/>
-      <c r="AD12" s="56"/>
-      <c r="AE12" s="56"/>
-      <c r="AF12" s="56"/>
-      <c r="AG12" s="56"/>
-      <c r="AH12" s="56"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="58"/>
+      <c r="H12" s="58"/>
+      <c r="I12" s="58"/>
+      <c r="J12" s="58"/>
+      <c r="K12" s="58"/>
+      <c r="L12" s="58"/>
+      <c r="M12" s="58"/>
+      <c r="N12" s="58"/>
+      <c r="O12" s="58"/>
+      <c r="P12" s="58"/>
+      <c r="Q12" s="58"/>
+      <c r="R12" s="58"/>
+      <c r="S12" s="58"/>
+      <c r="T12" s="58"/>
+      <c r="U12" s="58"/>
+      <c r="V12" s="58"/>
+      <c r="W12" s="58"/>
+      <c r="X12" s="58"/>
+      <c r="Y12" s="58"/>
+      <c r="Z12" s="58"/>
+      <c r="AA12" s="58"/>
+      <c r="AB12" s="58"/>
+      <c r="AC12" s="58"/>
+      <c r="AD12" s="58"/>
+      <c r="AE12" s="58"/>
+      <c r="AF12" s="58"/>
+      <c r="AG12" s="58"/>
+      <c r="AH12" s="58"/>
       <c r="AJ12" s="10" t="s">
         <v>391</v>
       </c>
@@ -11936,20 +12038,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="91" t="s">
         <v>277</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="90"/>
-      <c r="K1" s="90"/>
-      <c r="L1" s="90"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91"/>
+      <c r="L1" s="91"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12471,12 +12573,12 @@
       <c r="N6" s="40">
         <v>1</v>
       </c>
-      <c r="O6" s="56" t="s">
+      <c r="O6" s="58" t="s">
         <v>300</v>
       </c>
-      <c r="P6" s="56"/>
-      <c r="Q6" s="56"/>
-      <c r="R6" s="56"/>
+      <c r="P6" s="58"/>
+      <c r="Q6" s="58"/>
+      <c r="R6" s="58"/>
       <c r="T6" s="10" t="s">
         <v>443</v>
       </c>
@@ -12509,16 +12611,16 @@
       <c r="J7" s="40">
         <v>1</v>
       </c>
-      <c r="K7" s="56" t="s">
+      <c r="K7" s="58" t="s">
         <v>131</v>
       </c>
-      <c r="L7" s="56"/>
-      <c r="M7" s="56"/>
-      <c r="N7" s="56"/>
-      <c r="O7" s="56"/>
-      <c r="P7" s="56"/>
-      <c r="Q7" s="56"/>
-      <c r="R7" s="56"/>
+      <c r="L7" s="58"/>
+      <c r="M7" s="58"/>
+      <c r="N7" s="58"/>
+      <c r="O7" s="58"/>
+      <c r="P7" s="58"/>
+      <c r="Q7" s="58"/>
+      <c r="R7" s="58"/>
       <c r="T7" s="10"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -12549,16 +12651,16 @@
       <c r="J8" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="K8" s="56" t="s">
+      <c r="K8" s="58" t="s">
         <v>131</v>
       </c>
-      <c r="L8" s="56"/>
-      <c r="M8" s="56"/>
-      <c r="N8" s="56"/>
-      <c r="O8" s="56"/>
-      <c r="P8" s="56"/>
-      <c r="Q8" s="56"/>
-      <c r="R8" s="56"/>
+      <c r="L8" s="58"/>
+      <c r="M8" s="58"/>
+      <c r="N8" s="58"/>
+      <c r="O8" s="58"/>
+      <c r="P8" s="58"/>
+      <c r="Q8" s="58"/>
+      <c r="R8" s="58"/>
       <c r="T8" s="10"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -12589,16 +12691,16 @@
       <c r="J9" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="K9" s="56" t="s">
+      <c r="K9" s="58" t="s">
         <v>131</v>
       </c>
-      <c r="L9" s="56"/>
-      <c r="M9" s="56"/>
-      <c r="N9" s="56"/>
-      <c r="O9" s="56"/>
-      <c r="P9" s="56"/>
-      <c r="Q9" s="56"/>
-      <c r="R9" s="56"/>
+      <c r="L9" s="58"/>
+      <c r="M9" s="58"/>
+      <c r="N9" s="58"/>
+      <c r="O9" s="58"/>
+      <c r="P9" s="58"/>
+      <c r="Q9" s="58"/>
+      <c r="R9" s="58"/>
       <c r="T9" s="10"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -12629,16 +12731,16 @@
       <c r="J10" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="K10" s="56" t="s">
+      <c r="K10" s="58" t="s">
         <v>131</v>
       </c>
-      <c r="L10" s="56"/>
-      <c r="M10" s="56"/>
-      <c r="N10" s="56"/>
-      <c r="O10" s="56"/>
-      <c r="P10" s="56"/>
-      <c r="Q10" s="56"/>
-      <c r="R10" s="56"/>
+      <c r="L10" s="58"/>
+      <c r="M10" s="58"/>
+      <c r="N10" s="58"/>
+      <c r="O10" s="58"/>
+      <c r="P10" s="58"/>
+      <c r="Q10" s="58"/>
+      <c r="R10" s="58"/>
       <c r="T10" s="10"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -12669,16 +12771,16 @@
       <c r="J11" s="6">
         <v>0</v>
       </c>
-      <c r="K11" s="56" t="s">
+      <c r="K11" s="58" t="s">
         <v>298</v>
       </c>
-      <c r="L11" s="56"/>
-      <c r="M11" s="56"/>
-      <c r="N11" s="56"/>
-      <c r="O11" s="56"/>
-      <c r="P11" s="56"/>
-      <c r="Q11" s="56"/>
-      <c r="R11" s="56"/>
+      <c r="L11" s="58"/>
+      <c r="M11" s="58"/>
+      <c r="N11" s="58"/>
+      <c r="O11" s="58"/>
+      <c r="P11" s="58"/>
+      <c r="Q11" s="58"/>
+      <c r="R11" s="58"/>
       <c r="T11" s="10" t="s">
         <v>444</v>
       </c>
@@ -12753,16 +12855,16 @@
       <c r="J14" s="6">
         <v>0</v>
       </c>
-      <c r="K14" s="78" t="s">
+      <c r="K14" s="67" t="s">
         <v>442</v>
       </c>
-      <c r="L14" s="79"/>
-      <c r="M14" s="79"/>
-      <c r="N14" s="79"/>
-      <c r="O14" s="79"/>
-      <c r="P14" s="79"/>
-      <c r="Q14" s="79"/>
-      <c r="R14" s="80"/>
+      <c r="L14" s="68"/>
+      <c r="M14" s="68"/>
+      <c r="N14" s="68"/>
+      <c r="O14" s="68"/>
+      <c r="P14" s="68"/>
+      <c r="Q14" s="68"/>
+      <c r="R14" s="69"/>
       <c r="T14" s="10" t="s">
         <v>445</v>
       </c>

</xml_diff>

<commit_message>
removed some (unused) complications
</commit_message>
<xml_diff>
--- a/doc/RiscyInstSet32Bit.xlsx
+++ b/doc/RiscyInstSet32Bit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25410" windowHeight="12690"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25410" windowHeight="12690" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Summary - Terra" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="507">
   <si>
     <t>Description</t>
   </si>
@@ -469,9 +469,6 @@
     <t>MathOpcode 0 for Halt</t>
   </si>
   <si>
-    <t>Unused registers are ignored</t>
-  </si>
-  <si>
     <t>NOP = MOV r1, r1; XCHG r4, r4; etc.</t>
   </si>
   <si>
@@ -1547,13 +1544,22 @@
   </si>
   <si>
     <t>Rperi: register to peripheral # (Store 0 at Rperi for main mem); C: 0-Load, 1-Store; Mode: 0-Byte, 1-Halfword, 2-Word</t>
+  </si>
+  <si>
+    <t>Notes: in Assembler, labels return offset, but LOAD(STORE)BYTE/(H)WORD takes actual memory address stored in the register</t>
+  </si>
+  <si>
+    <t>NOTE: this shit is outdated</t>
+  </si>
+  <si>
+    <t>Unused registers are simply ignored</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1636,6 +1642,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1671,7 +1685,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -2030,6 +2044,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9"/>
@@ -2043,7 +2094,7 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="6" applyFont="1"/>
@@ -2482,6 +2533,18 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -2774,8 +2837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="AK14" sqref="AK14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2791,7 +2854,7 @@
   <sheetData>
     <row r="1" spans="1:38" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="123" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B1" s="123"/>
       <c r="C1" s="123"/>
@@ -2831,7 +2894,7 @@
     <row r="2" spans="1:38" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.25">
@@ -2840,7 +2903,7 @@
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -2879,11 +2942,11 @@
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B5" s="30" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -2926,7 +2989,7 @@
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="10" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -2965,7 +3028,7 @@
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
@@ -3003,7 +3066,7 @@
       <c r="AH7" s="5"/>
       <c r="AI7" s="5"/>
       <c r="AK7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3113,7 +3176,7 @@
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="90" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>11</v>
@@ -3175,7 +3238,7 @@
         <v>0</v>
       </c>
       <c r="AD10" s="96" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AE10" s="97"/>
       <c r="AF10" s="97"/>
@@ -3188,10 +3251,10 @@
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="91" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D11" s="103" t="s">
         <v>3</v>
@@ -3214,7 +3277,7 @@
       <c r="L11" s="105"/>
       <c r="M11" s="106"/>
       <c r="N11" s="116" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="O11" s="117"/>
       <c r="P11" s="117"/>
@@ -3268,15 +3331,15 @@
         <v>0</v>
       </c>
       <c r="AK11" s="10" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" s="92" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B12" s="43" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D12" s="103" t="s">
         <v>3</v>
@@ -3299,7 +3362,7 @@
       <c r="L12" s="105"/>
       <c r="M12" s="106"/>
       <c r="N12" s="116" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="O12" s="117"/>
       <c r="P12" s="117"/>
@@ -3353,12 +3416,12 @@
         <v>0</v>
       </c>
       <c r="AK12" s="10" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>123</v>
@@ -3429,22 +3492,22 @@
         <v>0</v>
       </c>
       <c r="AG13" s="102" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AH13" s="103"/>
       <c r="AI13" s="19" t="s">
         <v>84</v>
       </c>
       <c r="AK13" s="10" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="AL13" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>137</v>
@@ -3524,18 +3587,18 @@
         <v>0</v>
       </c>
       <c r="AH14" s="65" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AI14" s="19" t="s">
         <v>95</v>
       </c>
       <c r="AK14" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B15" s="67" t="s">
         <v>7</v>
@@ -3555,7 +3618,7 @@
         <v>0</v>
       </c>
       <c r="J15" s="104" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="K15" s="105"/>
       <c r="L15" s="105"/>
@@ -3621,15 +3684,15 @@
         <v>0</v>
       </c>
       <c r="AK15" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="73" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D16" s="102" t="s">
         <v>3</v>
@@ -3682,15 +3745,15 @@
       <c r="AH16" s="105"/>
       <c r="AI16" s="106"/>
       <c r="AK16" s="10" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" s="73" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B17" s="73" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D17" s="102" t="s">
         <v>3</v>
@@ -3725,7 +3788,7 @@
         <v>0</v>
       </c>
       <c r="T17" s="104" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="U17" s="105"/>
       <c r="V17" s="105"/>
@@ -3746,7 +3809,7 @@
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" s="73" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B18" s="67" t="s">
         <v>142</v>
@@ -3796,15 +3859,15 @@
       <c r="AH18" s="105"/>
       <c r="AI18" s="106"/>
       <c r="AK18" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" s="93" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B19" s="67" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D19" s="102" t="s">
         <v>3</v>
@@ -3851,15 +3914,15 @@
       <c r="AH19" s="105"/>
       <c r="AI19" s="106"/>
       <c r="AK19" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" s="94" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B20" s="67" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D20" s="102" t="s">
         <v>3</v>
@@ -3909,10 +3972,10 @@
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B21" s="67" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D21" s="102" t="s">
         <v>3</v>
@@ -3941,7 +4004,7 @@
         <v>0</v>
       </c>
       <c r="P21" s="125" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="Q21" s="126"/>
       <c r="R21" s="126"/>
@@ -3951,7 +4014,7 @@
       <c r="V21" s="126"/>
       <c r="W21" s="127"/>
       <c r="X21" s="104" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Y21" s="105"/>
       <c r="Z21" s="105"/>
@@ -3965,15 +4028,15 @@
       <c r="AH21" s="105"/>
       <c r="AI21" s="106"/>
       <c r="AK21" s="10" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" s="23" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B22" s="67" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D22" s="102" t="s">
         <v>3</v>
@@ -4038,7 +4101,7 @@
         <v>0</v>
       </c>
       <c r="AB22" s="104" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AC22" s="105"/>
       <c r="AD22" s="105"/>
@@ -4048,12 +4111,12 @@
       <c r="AH22" s="105"/>
       <c r="AI22" s="106"/>
       <c r="AK22" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B23" s="67" t="s">
         <v>82</v>
@@ -4136,7 +4199,7 @@
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B24" s="67" t="s">
         <v>88</v>
@@ -4214,12 +4277,12 @@
       <c r="AH24" s="105"/>
       <c r="AI24" s="106"/>
       <c r="AK24" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" s="23" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B25" s="67" t="s">
         <v>89</v>
@@ -4314,7 +4377,7 @@
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" s="23" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B26" s="67" t="s">
         <v>80</v>
@@ -4400,10 +4463,10 @@
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B27" s="49" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D27" s="99" t="s">
         <v>3</v>
@@ -4498,8 +4561,46 @@
         <v>1</v>
       </c>
       <c r="AK27" s="84" t="s">
-        <v>459</v>
-      </c>
+        <v>458</v>
+      </c>
+    </row>
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B29" s="153" t="s">
+        <v>504</v>
+      </c>
+      <c r="C29" s="154"/>
+      <c r="D29" s="154"/>
+      <c r="E29" s="154"/>
+      <c r="F29" s="154"/>
+      <c r="G29" s="154"/>
+      <c r="H29" s="154"/>
+      <c r="I29" s="154"/>
+      <c r="J29" s="154"/>
+      <c r="K29" s="154"/>
+      <c r="L29" s="154"/>
+      <c r="M29" s="154"/>
+      <c r="N29" s="154"/>
+      <c r="O29" s="154"/>
+      <c r="P29" s="154"/>
+      <c r="Q29" s="154"/>
+      <c r="R29" s="154"/>
+      <c r="S29" s="154"/>
+      <c r="T29" s="154"/>
+      <c r="U29" s="154"/>
+      <c r="V29" s="154"/>
+      <c r="W29" s="154"/>
+      <c r="X29" s="154"/>
+      <c r="Y29" s="154"/>
+      <c r="Z29" s="154"/>
+      <c r="AA29" s="154"/>
+      <c r="AB29" s="154"/>
+      <c r="AC29" s="154"/>
+      <c r="AD29" s="154"/>
+      <c r="AE29" s="154"/>
+      <c r="AF29" s="154"/>
+      <c r="AG29" s="154"/>
+      <c r="AH29" s="154"/>
+      <c r="AI29" s="155"/>
     </row>
     <row r="33" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B33" s="7"/>
@@ -5084,7 +5185,8 @@
       <c r="B49" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="60">
+  <mergeCells count="61">
+    <mergeCell ref="B29:AI29"/>
     <mergeCell ref="A1:AI1"/>
     <mergeCell ref="X21:AI21"/>
     <mergeCell ref="P21:W21"/>
@@ -5172,7 +5274,7 @@
   <sheetData>
     <row r="1" spans="1:21" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -5196,7 +5298,7 @@
     <row r="2" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -5205,7 +5307,7 @@
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -5228,11 +5330,11 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B5" s="30" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -5259,7 +5361,7 @@
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -5279,11 +5381,11 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B7" s="30" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -5301,12 +5403,12 @@
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
       <c r="U7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="24" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>0</v>
@@ -5378,7 +5480,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="118" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H10" s="118"/>
       <c r="I10" s="118"/>
@@ -5408,7 +5510,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D11" s="29">
         <v>0</v>
@@ -5582,7 +5684,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="129" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="M14" s="129"/>
       <c r="N14" s="129"/>
@@ -5624,7 +5726,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="129" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="M15" s="129"/>
       <c r="N15" s="129"/>
@@ -5640,7 +5742,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D16" s="29">
         <v>0</v>
@@ -5663,7 +5765,7 @@
         <v>1</v>
       </c>
       <c r="L16" s="129" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="M16" s="129"/>
       <c r="N16" s="129"/>
@@ -5673,7 +5775,7 @@
       <c r="R16" s="129"/>
       <c r="S16" s="129"/>
       <c r="U16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
@@ -5681,7 +5783,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D17" s="29">
         <v>1</v>
@@ -5696,11 +5798,11 @@
         <v>0</v>
       </c>
       <c r="H17" s="129" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I17" s="129"/>
       <c r="J17" s="129" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="K17" s="129"/>
       <c r="L17" s="29">
@@ -5728,13 +5830,13 @@
         <v>8</v>
       </c>
       <c r="U17" s="10" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="130"/>
       <c r="B18" s="30" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D18" s="29">
         <v>1</v>
@@ -5749,11 +5851,11 @@
         <v>0</v>
       </c>
       <c r="H18" s="129" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I18" s="129"/>
       <c r="J18" s="129" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="K18" s="129"/>
       <c r="L18" s="29">
@@ -5781,13 +5883,13 @@
         <v>8</v>
       </c>
       <c r="U18" s="10" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="130"/>
       <c r="B19" s="30" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D19" s="29">
         <v>1</v>
@@ -5802,7 +5904,7 @@
         <v>0</v>
       </c>
       <c r="H19" s="131" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I19" s="131"/>
       <c r="J19" s="131"/>
@@ -5832,7 +5934,7 @@
         <v>0</v>
       </c>
       <c r="U19" s="10" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
@@ -6063,8 +6165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q58"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L57" sqref="L57"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6082,13 +6184,13 @@
   <sheetData>
     <row r="1" spans="1:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="32" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B1" s="33">
         <v>1</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -6096,7 +6198,7 @@
     </row>
     <row r="2" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="133" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B2" s="134"/>
       <c r="C2" s="134"/>
@@ -6110,7 +6212,7 @@
       <c r="K2" s="134"/>
       <c r="L2" s="135"/>
       <c r="M2" s="17" t="s">
-        <v>145</v>
+        <v>506</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6137,10 +6239,10 @@
         <v>0</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3" t="s">
@@ -6150,13 +6252,13 @@
         <v>91</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P3" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q3" s="20" t="s">
         <v>161</v>
-      </c>
-      <c r="Q3" s="20" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -6194,16 +6296,16 @@
         <v>14</v>
       </c>
       <c r="M4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="N4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -6244,13 +6346,13 @@
         <v>92</v>
       </c>
       <c r="N5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Q5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -6288,16 +6390,16 @@
         <v>74</v>
       </c>
       <c r="M6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="N6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="Q6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -6335,16 +6437,16 @@
         <v>75</v>
       </c>
       <c r="M7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="N7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Q7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -6387,7 +6489,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="46" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B9" s="47"/>
       <c r="C9" s="47">
@@ -6418,16 +6520,16 @@
       </c>
       <c r="K9" s="48"/>
       <c r="L9" s="48" t="s">
+        <v>405</v>
+      </c>
+      <c r="M9" s="48" t="s">
         <v>406</v>
-      </c>
-      <c r="M9" s="48" t="s">
-        <v>407</v>
       </c>
       <c r="N9" s="48"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6">
@@ -6457,21 +6559,21 @@
         <v>36h</v>
       </c>
       <c r="L10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="N10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="P10" s="16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6">
@@ -6501,21 +6603,21 @@
         <v>37h</v>
       </c>
       <c r="L11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P11" s="16" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="43" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B12" s="44"/>
       <c r="C12" s="44">
@@ -6545,24 +6647,24 @@
         <v>38h</v>
       </c>
       <c r="L12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="M12" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="N12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O12" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="P12" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="43" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B13" s="44"/>
       <c r="C13" s="44">
@@ -6592,21 +6694,21 @@
         <v>39h</v>
       </c>
       <c r="L13" t="s">
+        <v>389</v>
+      </c>
+      <c r="M13" t="s">
         <v>390</v>
       </c>
-      <c r="M13" t="s">
-        <v>391</v>
-      </c>
       <c r="O13" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="P13" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="43" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B14" s="44"/>
       <c r="C14" s="44">
@@ -6636,21 +6738,21 @@
         <v>3Ah</v>
       </c>
       <c r="L14" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="M14" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="N14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O14" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="43" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B15" s="44"/>
       <c r="C15" s="44">
@@ -6680,18 +6782,18 @@
         <v>3Bh</v>
       </c>
       <c r="L15" t="s">
+        <v>394</v>
+      </c>
+      <c r="M15" t="s">
         <v>395</v>
       </c>
-      <c r="M15" t="s">
-        <v>396</v>
-      </c>
       <c r="O15" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="43" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B16" s="44"/>
       <c r="C16" s="44">
@@ -6721,21 +6823,21 @@
         <v>3Ch</v>
       </c>
       <c r="L16" t="s">
+        <v>399</v>
+      </c>
+      <c r="M16" t="s">
         <v>400</v>
       </c>
-      <c r="M16" t="s">
-        <v>401</v>
-      </c>
       <c r="N16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O16" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="43" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B17" s="44"/>
       <c r="C17" s="44">
@@ -6765,18 +6867,18 @@
         <v>3Dh</v>
       </c>
       <c r="L17" t="s">
+        <v>402</v>
+      </c>
+      <c r="M17" t="s">
         <v>403</v>
       </c>
-      <c r="M17" t="s">
-        <v>404</v>
-      </c>
       <c r="O17" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6">
@@ -6806,10 +6908,10 @@
         <v>3Eh</v>
       </c>
       <c r="L18" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="M18" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -6847,7 +6949,7 @@
         <v>77</v>
       </c>
       <c r="M19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -6888,7 +6990,7 @@
         <v>97</v>
       </c>
       <c r="N20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -6929,7 +7031,7 @@
         <v>98</v>
       </c>
       <c r="N21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -6970,7 +7072,7 @@
         <v>99</v>
       </c>
       <c r="N22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -7011,7 +7113,7 @@
         <v>100</v>
       </c>
       <c r="N23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -7052,7 +7154,7 @@
         <v>101</v>
       </c>
       <c r="N24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -7093,7 +7195,7 @@
         <v>102</v>
       </c>
       <c r="N25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -7137,7 +7239,7 @@
         <v>Rd = Rs + Rm</v>
       </c>
       <c r="N26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -7181,7 +7283,7 @@
         <v>Rd = Rs - Rm</v>
       </c>
       <c r="N27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -7225,7 +7327,7 @@
         <v>Rd = Rs * Rm</v>
       </c>
       <c r="N28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -7269,7 +7371,7 @@
         <v>Rd = Rs / Rm</v>
       </c>
       <c r="N29" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -7313,7 +7415,7 @@
         <v>Rd = Rs ^ Rm</v>
       </c>
       <c r="N30" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -7357,7 +7459,7 @@
         <v>Rd = Rs % Rm</v>
       </c>
       <c r="N31" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -7398,7 +7500,7 @@
         <v>103</v>
       </c>
       <c r="N32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -7439,7 +7541,7 @@
         <v>104</v>
       </c>
       <c r="N33" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -7480,7 +7582,7 @@
         <v>105</v>
       </c>
       <c r="N34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
@@ -7521,7 +7623,7 @@
         <v>106</v>
       </c>
       <c r="N35" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
@@ -7562,7 +7664,7 @@
         <v>107</v>
       </c>
       <c r="N36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
@@ -7603,7 +7705,7 @@
         <v>108</v>
       </c>
       <c r="N37" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -7644,7 +7746,7 @@
         <v>119</v>
       </c>
       <c r="N38" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
@@ -7685,7 +7787,7 @@
         <v>120</v>
       </c>
       <c r="N39" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
@@ -7726,7 +7828,7 @@
         <v>109</v>
       </c>
       <c r="N40" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
@@ -7767,7 +7869,7 @@
         <v>110</v>
       </c>
       <c r="N41" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
@@ -7808,7 +7910,7 @@
         <v>111</v>
       </c>
       <c r="N42" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
@@ -7849,7 +7951,7 @@
         <v>112</v>
       </c>
       <c r="N43" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
@@ -7890,7 +7992,7 @@
         <v>113</v>
       </c>
       <c r="N44" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
@@ -7931,12 +8033,12 @@
         <v>114</v>
       </c>
       <c r="N45" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B46" s="6"/>
       <c r="C46" s="6">
@@ -7966,13 +8068,13 @@
         <v>18h</v>
       </c>
       <c r="L46" t="s">
+        <v>177</v>
+      </c>
+      <c r="M46" t="s">
         <v>178</v>
       </c>
-      <c r="M46" t="s">
-        <v>179</v>
-      </c>
       <c r="N46" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
@@ -8010,10 +8112,10 @@
         <v>65</v>
       </c>
       <c r="M47" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="N47" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
@@ -8054,7 +8156,7 @@
         <v>115</v>
       </c>
       <c r="N48" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
@@ -8095,7 +8197,7 @@
         <v>116</v>
       </c>
       <c r="N49" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
@@ -8136,7 +8238,7 @@
         <v>117</v>
       </c>
       <c r="N50" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
@@ -8177,7 +8279,7 @@
         <v>122</v>
       </c>
       <c r="N51" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
@@ -8218,7 +8320,7 @@
         <v>118</v>
       </c>
       <c r="N52" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
@@ -8259,7 +8361,7 @@
         <v>121</v>
       </c>
       <c r="N53" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
@@ -8298,12 +8400,12 @@
         <v>79</v>
       </c>
       <c r="O54" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B55" s="6"/>
       <c r="C55" s="6">
@@ -8333,15 +8435,15 @@
         <v>20h</v>
       </c>
       <c r="L55" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="O55" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="52" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C56" s="53">
         <v>1</v>
@@ -8370,15 +8472,15 @@
         <v>2Ah</v>
       </c>
       <c r="L56" t="s">
+        <v>421</v>
+      </c>
+      <c r="O56" t="s">
         <v>422</v>
-      </c>
-      <c r="O56" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="52" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C57" s="53">
         <v>1</v>
@@ -8407,15 +8509,15 @@
         <v>2Ch</v>
       </c>
       <c r="L57" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="M57" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="52" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C58" s="53">
         <v>1</v>
@@ -8444,10 +8546,10 @@
         <v>2Dh</v>
       </c>
       <c r="L58" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="M58" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
   </sheetData>
@@ -8464,7 +8566,7 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8480,7 +8582,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="32" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B1" s="33">
         <v>1</v>
@@ -8491,7 +8593,7 @@
     </row>
     <row r="2" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="133" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B2" s="134"/>
       <c r="C2" s="134"/>
@@ -8504,7 +8606,7 @@
       <c r="J2" s="134"/>
       <c r="K2" s="135"/>
       <c r="L2" s="17" t="s">
-        <v>145</v>
+        <v>506</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8528,10 +8630,10 @@
         <v>0</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3" t="s">
@@ -8541,7 +8643,7 @@
         <v>91</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -8576,10 +8678,10 @@
         <v>14</v>
       </c>
       <c r="L4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="M4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -8617,7 +8719,7 @@
         <v>92</v>
       </c>
       <c r="M5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -8655,7 +8757,7 @@
         <v>93</v>
       </c>
       <c r="M6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -8693,12 +8795,12 @@
         <v>94</v>
       </c>
       <c r="M7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B8" s="26"/>
       <c r="C8" s="26">
@@ -8725,10 +8827,10 @@
         <v>1Eh</v>
       </c>
       <c r="K8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="L8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -8763,7 +8865,7 @@
         <v>77</v>
       </c>
       <c r="L9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -8801,7 +8903,7 @@
         <v>97</v>
       </c>
       <c r="M10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -8839,7 +8941,7 @@
         <v>98</v>
       </c>
       <c r="M11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -8877,7 +8979,7 @@
         <v>99</v>
       </c>
       <c r="M12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -8915,7 +9017,7 @@
         <v>100</v>
       </c>
       <c r="M13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -8953,7 +9055,7 @@
         <v>101</v>
       </c>
       <c r="M14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -8991,7 +9093,7 @@
         <v>102</v>
       </c>
       <c r="M15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -9029,7 +9131,7 @@
         <v>103</v>
       </c>
       <c r="M16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -9067,7 +9169,7 @@
         <v>104</v>
       </c>
       <c r="M17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -9105,7 +9207,7 @@
         <v>105</v>
       </c>
       <c r="M18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -9143,7 +9245,7 @@
         <v>106</v>
       </c>
       <c r="M19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -9181,7 +9283,7 @@
         <v>107</v>
       </c>
       <c r="M20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -9219,7 +9321,7 @@
         <v>108</v>
       </c>
       <c r="M21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -9257,7 +9359,7 @@
         <v>121</v>
       </c>
       <c r="M22" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -9315,10 +9417,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9331,797 +9433,810 @@
     <col min="6" max="6" width="108.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="156" t="s">
+        <v>505</v>
+      </c>
+      <c r="B1" s="156"/>
+      <c r="C1" s="156"/>
+      <c r="D1" s="156"/>
+      <c r="E1" s="156"/>
+    </row>
+    <row r="2" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="B2" s="33">
+        <v>2</v>
+      </c>
+      <c r="C2" s="31" t="s">
         <v>230</v>
       </c>
-      <c r="B1" s="33">
-        <v>2</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>231</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="25" t="s">
-        <v>189</v>
-      </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="3" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
-        <v>182</v>
-      </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="3" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="B3" s="34"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="B4" s="35"/>
+      <c r="C4" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
-        <v>181</v>
-      </c>
-      <c r="C4" t="s">
-        <v>215</v>
-      </c>
-      <c r="D4" t="s">
-        <v>198</v>
-      </c>
-      <c r="E4" t="s">
-        <v>384</v>
+      <c r="D4" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E5" t="s">
-        <v>205</v>
+        <v>383</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D8" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E9" t="s">
-        <v>209</v>
-      </c>
-      <c r="F9" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="C10" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="D10" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E10" t="s">
+        <v>208</v>
+      </c>
+      <c r="F10" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="C11" t="s">
+        <v>221</v>
+      </c>
+      <c r="D11" t="s">
+        <v>203</v>
+      </c>
+      <c r="E11" t="s">
+        <v>209</v>
+      </c>
+      <c r="F11" t="s">
         <v>210</v>
       </c>
-      <c r="F10" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="25" t="s">
-        <v>190</v>
-      </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="8"/>
-    </row>
-    <row r="12" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="24" t="s">
-        <v>182</v>
-      </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="3" t="s">
+    </row>
+    <row r="12" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="25" t="s">
+        <v>189</v>
+      </c>
+      <c r="B12" s="34"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="B13" s="35"/>
+      <c r="C13" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="23" t="s">
-        <v>191</v>
-      </c>
-      <c r="C13" t="s">
-        <v>217</v>
-      </c>
-      <c r="D13" t="s">
-        <v>198</v>
-      </c>
-      <c r="E13" t="s">
-        <v>383</v>
+      <c r="D13" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E14" t="s">
-        <v>212</v>
+        <v>382</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C16" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D16" t="s">
-        <v>218</v>
+        <v>197</v>
       </c>
       <c r="E16" t="s">
-        <v>385</v>
+        <v>212</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D17" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E17" t="s">
-        <v>214</v>
+        <v>384</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C18" t="s">
         <v>220</v>
       </c>
       <c r="D18" t="s">
-        <v>204</v>
+        <v>218</v>
       </c>
       <c r="E18" t="s">
-        <v>386</v>
-      </c>
-      <c r="F18" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="32" t="s">
-        <v>230</v>
-      </c>
-      <c r="B19" s="33" t="s">
-        <v>464</v>
-      </c>
-      <c r="C19" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="C19" t="s">
+        <v>219</v>
+      </c>
+      <c r="D19" t="s">
+        <v>203</v>
+      </c>
+      <c r="E19" t="s">
+        <v>385</v>
+      </c>
+      <c r="F19" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="B20" s="33" t="s">
+        <v>463</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="B21" s="35"/>
+      <c r="C21" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="23" t="s">
         <v>232</v>
       </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="24" t="s">
-        <v>182</v>
-      </c>
-      <c r="B20" s="35"/>
-      <c r="C20" s="3" t="s">
+      <c r="C22" t="s">
+        <v>234</v>
+      </c>
+      <c r="D22" t="s">
+        <v>233</v>
+      </c>
+      <c r="F22" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="B23" s="33">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="B24" s="35"/>
+      <c r="C24" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F20" s="20" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="23" t="s">
-        <v>233</v>
-      </c>
-      <c r="C21" t="s">
-        <v>235</v>
-      </c>
-      <c r="D21" t="s">
-        <v>234</v>
-      </c>
-      <c r="F21" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="32" t="s">
-        <v>230</v>
-      </c>
-      <c r="B22" s="33">
-        <v>4</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="24" t="s">
-        <v>182</v>
-      </c>
-      <c r="B23" s="35"/>
-      <c r="C23" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F23" s="20" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="23" t="s">
-        <v>236</v>
-      </c>
-      <c r="C24" t="s">
-        <v>237</v>
-      </c>
-      <c r="D24" t="s">
-        <v>268</v>
-      </c>
-      <c r="E24" t="s">
-        <v>238</v>
+      <c r="D24" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F24" s="20" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="23" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C25" t="s">
+        <v>236</v>
+      </c>
+      <c r="D25" t="s">
+        <v>267</v>
+      </c>
+      <c r="E25" t="s">
         <v>237</v>
-      </c>
-      <c r="D25" t="s">
-        <v>268</v>
-      </c>
-      <c r="E25" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="23" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C26" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D26" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E26" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C27" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D27" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E27" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="32" t="s">
-        <v>230</v>
-      </c>
-      <c r="B28" s="33">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="23" t="s">
+        <v>240</v>
+      </c>
+      <c r="C28" t="s">
+        <v>236</v>
+      </c>
+      <c r="D28" t="s">
+        <v>267</v>
+      </c>
+      <c r="E28" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="B29" s="33">
         <v>5</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="24" t="s">
-        <v>182</v>
-      </c>
-      <c r="B29" s="35"/>
-      <c r="C29" s="3" t="s">
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="B30" s="35"/>
+      <c r="C30" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F29" s="20" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="23" t="s">
-        <v>245</v>
-      </c>
-      <c r="C30" t="s">
-        <v>460</v>
-      </c>
-      <c r="D30" t="s">
-        <v>461</v>
-      </c>
-      <c r="E30" t="s">
-        <v>286</v>
+      <c r="D30" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F30" s="20" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="23" t="s">
+        <v>244</v>
+      </c>
+      <c r="C31" t="s">
+        <v>459</v>
+      </c>
+      <c r="D31" t="s">
+        <v>460</v>
+      </c>
+      <c r="E31" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="23" t="s">
+        <v>245</v>
+      </c>
+      <c r="C32" t="s">
+        <v>461</v>
+      </c>
+      <c r="E32" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="B33" s="33">
+        <v>6</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="C31" t="s">
-        <v>462</v>
-      </c>
-      <c r="E31" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="32" t="s">
-        <v>230</v>
-      </c>
-      <c r="B32" s="33">
-        <v>6</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="24" t="s">
-        <v>182</v>
-      </c>
-      <c r="B33" s="35"/>
-      <c r="C33" s="3" t="s">
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+    </row>
+    <row r="34" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="B34" s="35"/>
+      <c r="C34" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F33" s="20" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="23" t="s">
-        <v>248</v>
-      </c>
-      <c r="C34" t="s">
-        <v>290</v>
-      </c>
-      <c r="D34" t="s">
-        <v>288</v>
-      </c>
-      <c r="E34" t="s">
-        <v>289</v>
-      </c>
-      <c r="F34" t="s">
-        <v>211</v>
+      <c r="D34" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F34" s="20" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C35" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D35" t="s">
+        <v>287</v>
+      </c>
+      <c r="E35" t="s">
         <v>288</v>
       </c>
-      <c r="E35" t="s">
-        <v>296</v>
-      </c>
       <c r="F35" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="23" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C36" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D36" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E36" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F36" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="23" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C37" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D37" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E37" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F37" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="23" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C38" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D38" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E38" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F38" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C39" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="D39" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="E39" t="s">
-        <v>302</v>
+        <v>298</v>
+      </c>
+      <c r="F39" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="C40" t="s">
+        <v>299</v>
+      </c>
+      <c r="D40" t="s">
+        <v>290</v>
+      </c>
+      <c r="E40" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="23" t="s">
+        <v>253</v>
+      </c>
+      <c r="C41" t="s">
+        <v>300</v>
+      </c>
+      <c r="D41" t="s">
+        <v>290</v>
+      </c>
+      <c r="E41" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="B42" s="33">
+        <v>7</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="C40" t="s">
-        <v>301</v>
-      </c>
-      <c r="D40" t="s">
-        <v>291</v>
-      </c>
-      <c r="E40" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="32" t="s">
-        <v>230</v>
-      </c>
-      <c r="B41" s="33">
-        <v>7</v>
-      </c>
-      <c r="C41" s="1" t="s">
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+    </row>
+    <row r="43" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="B43" s="35"/>
+      <c r="C43" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F43" s="20" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="B45" s="33">
+        <v>8</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-    </row>
-    <row r="42" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="24" t="s">
-        <v>182</v>
-      </c>
-      <c r="B42" s="35"/>
-      <c r="C42" s="3" t="s">
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+    </row>
+    <row r="46" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="B46" s="35"/>
+      <c r="C46" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F42" s="20" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="32" t="s">
-        <v>230</v>
-      </c>
-      <c r="B44" s="33">
-        <v>8</v>
-      </c>
-      <c r="C44" s="1" t="s">
+      <c r="D46" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F46" s="20" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="B48" s="33">
+        <v>9</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-    </row>
-    <row r="45" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="24" t="s">
-        <v>182</v>
-      </c>
-      <c r="B45" s="35"/>
-      <c r="C45" s="3" t="s">
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+    </row>
+    <row r="49" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="B49" s="35"/>
+      <c r="C49" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F45" s="20" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="32" t="s">
-        <v>230</v>
-      </c>
-      <c r="B47" s="33">
-        <v>9</v>
-      </c>
-      <c r="C47" s="1" t="s">
+      <c r="D49" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F49" s="20" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="B51" s="33">
+        <v>10</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-    </row>
-    <row r="48" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="24" t="s">
-        <v>182</v>
-      </c>
-      <c r="B48" s="35"/>
-      <c r="C48" s="3" t="s">
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+    </row>
+    <row r="52" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="B52" s="35"/>
+      <c r="C52" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F48" s="20" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="32" t="s">
-        <v>230</v>
-      </c>
-      <c r="B50" s="33">
-        <v>10</v>
-      </c>
-      <c r="C50" s="1" t="s">
+      <c r="D52" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F52" s="20" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="B54" s="33">
+        <v>11</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-    </row>
-    <row r="51" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="24" t="s">
-        <v>182</v>
-      </c>
-      <c r="B51" s="35"/>
-      <c r="C51" s="3" t="s">
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+    </row>
+    <row r="55" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="B55" s="35"/>
+      <c r="C55" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D51" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F51" s="20" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="32" t="s">
-        <v>230</v>
-      </c>
-      <c r="B53" s="33">
-        <v>11</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-    </row>
-    <row r="54" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="24" t="s">
-        <v>182</v>
-      </c>
-      <c r="B54" s="35"/>
-      <c r="C54" s="3" t="s">
+      <c r="D55" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F55" s="20" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="B57" s="33">
+        <v>12</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+    </row>
+    <row r="58" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="B58" s="35"/>
+      <c r="C58" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D54" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F54" s="20" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="32" t="s">
-        <v>230</v>
-      </c>
-      <c r="B56" s="33">
-        <v>12</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-    </row>
-    <row r="57" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="24" t="s">
-        <v>182</v>
-      </c>
-      <c r="B57" s="35"/>
-      <c r="C57" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F57" s="20" t="s">
-        <v>202</v>
+      <c r="D58" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F58" s="20" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -10129,8 +10244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AA10" sqref="AA10:AH10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10144,7 +10259,7 @@
   <sheetData>
     <row r="1" spans="1:36" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="61" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -10182,12 +10297,12 @@
     </row>
     <row r="2" spans="1:36" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="AJ3" s="10" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="4" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10294,7 +10409,7 @@
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="51" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C5" s="38">
         <v>0</v>
@@ -10379,12 +10494,12 @@
       <c r="AG5" s="117"/>
       <c r="AH5" s="117"/>
       <c r="AJ5" s="10" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="51" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C6" s="40">
         <v>0</v>
@@ -10465,18 +10580,18 @@
       <c r="AC6" s="144"/>
       <c r="AD6" s="145"/>
       <c r="AE6" s="116" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="AF6" s="117"/>
       <c r="AG6" s="117"/>
       <c r="AH6" s="136"/>
       <c r="AJ6" s="10" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="51" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C7" s="40">
         <v>0</v>
@@ -10551,7 +10666,7 @@
         <v>130</v>
       </c>
       <c r="AA7" s="140" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="AB7" s="141"/>
       <c r="AC7" s="141"/>
@@ -10561,12 +10676,12 @@
       <c r="AG7" s="141"/>
       <c r="AH7" s="142"/>
       <c r="AJ7" s="10" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="59" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C8" s="58">
         <v>0</v>
@@ -10626,13 +10741,13 @@
         <v>1</v>
       </c>
       <c r="V8" s="116" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="W8" s="117"/>
       <c r="X8" s="117"/>
       <c r="Y8" s="117"/>
       <c r="Z8" s="18" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="AA8" s="141" t="s">
         <v>141</v>
@@ -10645,12 +10760,12 @@
       <c r="AG8" s="141"/>
       <c r="AH8" s="142"/>
       <c r="AJ8" s="10" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="89" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C9" s="86">
         <v>0</v>
@@ -10710,33 +10825,33 @@
         <v>0</v>
       </c>
       <c r="V9" s="116" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="W9" s="117"/>
       <c r="X9" s="117"/>
       <c r="Y9" s="117"/>
       <c r="Z9" s="85" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="AA9" s="116" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="AB9" s="117"/>
       <c r="AC9" s="117"/>
       <c r="AD9" s="117"/>
       <c r="AE9" s="116" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="AF9" s="117"/>
       <c r="AG9" s="117"/>
       <c r="AH9" s="117"/>
       <c r="AJ9" s="10" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="51" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C10" s="38">
         <v>0</v>
@@ -10763,19 +10878,19 @@
         <v>1</v>
       </c>
       <c r="K10" s="117" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="L10" s="117"/>
       <c r="M10" s="117"/>
       <c r="N10" s="117"/>
       <c r="O10" s="117"/>
       <c r="P10" s="117" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="Q10" s="117"/>
       <c r="R10" s="117"/>
       <c r="S10" s="117" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="T10" s="117"/>
       <c r="U10" s="117"/>
@@ -10795,7 +10910,7 @@
       <c r="AG10" s="117"/>
       <c r="AH10" s="117"/>
       <c r="AJ10" s="10" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
@@ -10831,7 +10946,7 @@
       </c>
       <c r="L11" s="111"/>
       <c r="M11" s="104" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="N11" s="105"/>
       <c r="O11" s="105"/>
@@ -10855,41 +10970,41 @@
       <c r="AG11" s="105"/>
       <c r="AH11" s="106"/>
       <c r="AJ11" s="10" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="51" t="s">
+        <v>377</v>
+      </c>
+      <c r="C12" s="41">
+        <v>0</v>
+      </c>
+      <c r="D12" s="41">
+        <v>0</v>
+      </c>
+      <c r="E12" s="41">
+        <v>0</v>
+      </c>
+      <c r="F12" s="41">
+        <v>0</v>
+      </c>
+      <c r="G12" s="42">
+        <v>0</v>
+      </c>
+      <c r="H12" s="80">
+        <v>1</v>
+      </c>
+      <c r="I12" s="42">
+        <v>0</v>
+      </c>
+      <c r="J12" s="104" t="s">
         <v>378</v>
-      </c>
-      <c r="C12" s="41">
-        <v>0</v>
-      </c>
-      <c r="D12" s="41">
-        <v>0</v>
-      </c>
-      <c r="E12" s="41">
-        <v>0</v>
-      </c>
-      <c r="F12" s="41">
-        <v>0</v>
-      </c>
-      <c r="G12" s="42">
-        <v>0</v>
-      </c>
-      <c r="H12" s="80">
-        <v>1</v>
-      </c>
-      <c r="I12" s="42">
-        <v>0</v>
-      </c>
-      <c r="J12" s="104" t="s">
-        <v>379</v>
       </c>
       <c r="K12" s="105"/>
       <c r="L12" s="106"/>
       <c r="M12" s="104" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="N12" s="105"/>
       <c r="O12" s="105"/>
@@ -10913,7 +11028,7 @@
       <c r="AG12" s="105"/>
       <c r="AH12" s="106"/>
       <c r="AJ12" s="10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.25">
@@ -10954,7 +11069,7 @@
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="51" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C14" s="74">
         <v>1</v>
@@ -10991,7 +11106,7 @@
       <c r="AG14" s="118"/>
       <c r="AH14" s="118"/>
       <c r="AJ14" s="10" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.25">
@@ -11032,7 +11147,7 @@
     </row>
     <row r="16" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4">
@@ -11081,7 +11196,7 @@
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" s="51" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="42">
@@ -11101,7 +11216,7 @@
       </c>
       <c r="H17" s="6"/>
       <c r="I17" s="5" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
@@ -11132,7 +11247,7 @@
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18" s="59" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B18" s="56"/>
       <c r="C18" s="57">
@@ -11181,7 +11296,7 @@
     </row>
     <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" s="59" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B19" s="56"/>
       <c r="C19" s="57">
@@ -11201,7 +11316,7 @@
       </c>
       <c r="H19" s="56"/>
       <c r="I19" s="5" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
@@ -11232,7 +11347,7 @@
     </row>
     <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20" s="51" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="42">
@@ -11278,12 +11393,12 @@
       <c r="AG20" s="6"/>
       <c r="AH20" s="6"/>
       <c r="AJ20" s="10" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21" s="51" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C21" s="57">
         <v>0</v>
@@ -11302,7 +11417,7 @@
       </c>
       <c r="H21" s="6"/>
       <c r="I21" s="10" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
@@ -11333,7 +11448,7 @@
     </row>
     <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22" s="51" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C22" s="57">
         <v>0</v>
@@ -11352,7 +11467,7 @@
       </c>
       <c r="H22" s="6"/>
       <c r="I22" s="10" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
@@ -11383,7 +11498,7 @@
     </row>
     <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23" s="51" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C23" s="57">
         <v>0</v>
@@ -11402,7 +11517,7 @@
       </c>
       <c r="H23" s="6"/>
       <c r="I23" s="10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
@@ -11430,12 +11545,12 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AJ23" s="10" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24" s="51" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C24" s="57">
         <v>0</v>
@@ -11454,7 +11569,7 @@
       </c>
       <c r="H24" s="6"/>
       <c r="I24" s="10" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
@@ -11485,7 +11600,7 @@
     </row>
     <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25" s="51" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C25" s="57">
         <v>0</v>
@@ -11504,7 +11619,7 @@
       </c>
       <c r="H25" s="41"/>
       <c r="I25" s="10" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="J25" s="41"/>
       <c r="K25" s="41"/>
@@ -11535,7 +11650,7 @@
     </row>
     <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A26" s="51" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C26" s="57">
         <v>0</v>
@@ -11554,7 +11669,7 @@
       </c>
       <c r="H26" s="6"/>
       <c r="I26" s="10" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
@@ -11585,7 +11700,7 @@
     </row>
     <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A27" s="51" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C27" s="57">
         <v>0</v>
@@ -11604,7 +11719,7 @@
       </c>
       <c r="H27" s="6"/>
       <c r="I27" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
@@ -11635,7 +11750,7 @@
     </row>
     <row r="28" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A28" s="51" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C28" s="57">
         <v>0</v>
@@ -11654,7 +11769,7 @@
       </c>
       <c r="H28" s="6"/>
       <c r="I28" s="10" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
@@ -11685,7 +11800,7 @@
     </row>
     <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A29" s="51" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C29" s="57">
         <v>0</v>
@@ -11704,7 +11819,7 @@
       </c>
       <c r="H29" s="6"/>
       <c r="I29" s="10" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
@@ -11735,7 +11850,7 @@
     </row>
     <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30" s="51" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C30" s="57">
         <v>0</v>
@@ -11754,7 +11869,7 @@
       </c>
       <c r="H30" s="6"/>
       <c r="I30" s="10" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
@@ -11784,30 +11899,30 @@
     </row>
     <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31" s="51" t="s">
+        <v>353</v>
+      </c>
+      <c r="C31" s="57">
+        <v>0</v>
+      </c>
+      <c r="D31" s="56">
+        <v>1</v>
+      </c>
+      <c r="E31" s="56">
+        <v>1</v>
+      </c>
+      <c r="F31" s="56">
+        <v>1</v>
+      </c>
+      <c r="G31" s="56">
+        <v>0</v>
+      </c>
+      <c r="I31" s="10" t="s">
         <v>354</v>
-      </c>
-      <c r="C31" s="57">
-        <v>0</v>
-      </c>
-      <c r="D31" s="56">
-        <v>1</v>
-      </c>
-      <c r="E31" s="56">
-        <v>1</v>
-      </c>
-      <c r="F31" s="56">
-        <v>1</v>
-      </c>
-      <c r="G31" s="56">
-        <v>0</v>
-      </c>
-      <c r="I31" s="10" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32" s="51" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C32" s="57">
         <v>0</v>
@@ -11828,7 +11943,7 @@
     </row>
     <row r="33" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A33" s="51" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C33" s="57">
         <v>1</v>
@@ -11847,7 +11962,7 @@
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="10" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="J33" s="6"/>
       <c r="K33" s="6"/>
@@ -11878,30 +11993,30 @@
     </row>
     <row r="34" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A34" s="51" t="s">
+        <v>358</v>
+      </c>
+      <c r="C34" s="57">
+        <v>1</v>
+      </c>
+      <c r="D34" s="56">
+        <v>0</v>
+      </c>
+      <c r="E34" s="56">
+        <v>0</v>
+      </c>
+      <c r="F34" s="56">
+        <v>0</v>
+      </c>
+      <c r="G34" s="56">
+        <v>1</v>
+      </c>
+      <c r="I34" s="10" t="s">
         <v>359</v>
-      </c>
-      <c r="C34" s="57">
-        <v>1</v>
-      </c>
-      <c r="D34" s="56">
-        <v>0</v>
-      </c>
-      <c r="E34" s="56">
-        <v>0</v>
-      </c>
-      <c r="F34" s="56">
-        <v>0</v>
-      </c>
-      <c r="G34" s="56">
-        <v>1</v>
-      </c>
-      <c r="I34" s="10" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="35" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A35" s="51" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C35" s="42">
         <v>1</v>
@@ -11919,36 +12034,36 @@
         <v>0</v>
       </c>
       <c r="I35" s="10" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="AJ35" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="36" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A36" s="51" t="s">
+        <v>366</v>
+      </c>
+      <c r="C36" s="42">
+        <v>1</v>
+      </c>
+      <c r="D36" s="41">
+        <v>0</v>
+      </c>
+      <c r="E36" s="41">
+        <v>0</v>
+      </c>
+      <c r="F36" s="41">
+        <v>1</v>
+      </c>
+      <c r="G36" s="41">
+        <v>1</v>
+      </c>
+      <c r="I36" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="AJ36" t="s">
         <v>367</v>
-      </c>
-      <c r="C36" s="42">
-        <v>1</v>
-      </c>
-      <c r="D36" s="41">
-        <v>0</v>
-      </c>
-      <c r="E36" s="41">
-        <v>0</v>
-      </c>
-      <c r="F36" s="41">
-        <v>1</v>
-      </c>
-      <c r="G36" s="41">
-        <v>1</v>
-      </c>
-      <c r="I36" s="10" t="s">
-        <v>369</v>
-      </c>
-      <c r="AJ36" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="37" spans="1:36" x14ac:dyDescent="0.25">
@@ -11962,7 +12077,7 @@
     </row>
     <row r="38" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B38" s="4"/>
       <c r="C38" s="4">
@@ -12065,7 +12180,7 @@
     <row r="39" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A39" s="89"/>
       <c r="C39" s="137" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D39" s="138"/>
       <c r="E39" s="138"/>
@@ -12083,7 +12198,7 @@
       <c r="Q39" s="138"/>
       <c r="R39" s="139"/>
       <c r="S39" s="137" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="T39" s="138"/>
       <c r="U39" s="138"/>
@@ -12093,7 +12208,7 @@
       <c r="Y39" s="138"/>
       <c r="Z39" s="139"/>
       <c r="AA39" s="137" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="AB39" s="138"/>
       <c r="AC39" s="138"/>
@@ -12103,12 +12218,12 @@
       <c r="AG39" s="138"/>
       <c r="AH39" s="139"/>
       <c r="AJ39" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="41" spans="1:36" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="60" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
@@ -12146,7 +12261,7 @@
     </row>
     <row r="42" spans="1:36" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A42" s="23" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C42" s="146">
         <v>8192</v>
@@ -12185,7 +12300,7 @@
     </row>
     <row r="44" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C44" s="150" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D44" s="151"/>
       <c r="E44" s="151"/>
@@ -12195,7 +12310,7 @@
       <c r="I44" s="151"/>
       <c r="J44" s="151"/>
       <c r="K44" s="151" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L44" s="151"/>
       <c r="M44" s="151"/>
@@ -12205,7 +12320,7 @@
       <c r="Q44" s="151"/>
       <c r="R44" s="151"/>
       <c r="S44" s="151" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="T44" s="151"/>
       <c r="U44" s="151"/>
@@ -12215,7 +12330,7 @@
       <c r="Y44" s="151"/>
       <c r="Z44" s="151"/>
       <c r="AA44" s="152" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="AB44" s="152"/>
       <c r="AC44" s="152"/>
@@ -12227,11 +12342,11 @@
     </row>
     <row r="45" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="24" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B45" s="3"/>
       <c r="C45" s="149" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D45" s="149"/>
       <c r="E45" s="149"/>
@@ -12241,7 +12356,7 @@
       <c r="I45" s="149"/>
       <c r="J45" s="149"/>
       <c r="K45" s="149" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="L45" s="149"/>
       <c r="M45" s="149"/>
@@ -12251,7 +12366,7 @@
       <c r="Q45" s="149"/>
       <c r="R45" s="149"/>
       <c r="S45" s="149" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="T45" s="149"/>
       <c r="U45" s="149"/>
@@ -12261,7 +12376,7 @@
       <c r="Y45" s="149"/>
       <c r="Z45" s="149"/>
       <c r="AA45" s="149" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="AB45" s="149"/>
       <c r="AC45" s="149"/>
@@ -12273,7 +12388,7 @@
     </row>
     <row r="46" spans="1:36" x14ac:dyDescent="0.25">
       <c r="C46" s="137" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D46" s="138"/>
       <c r="E46" s="138"/>
@@ -12283,7 +12398,7 @@
       <c r="I46" s="138"/>
       <c r="J46" s="139"/>
       <c r="K46" s="137" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L46" s="138"/>
       <c r="M46" s="138"/>
@@ -12293,7 +12408,7 @@
       <c r="Q46" s="138"/>
       <c r="R46" s="139"/>
       <c r="S46" s="137" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="T46" s="138"/>
       <c r="U46" s="138"/>
@@ -12303,7 +12418,7 @@
       <c r="Y46" s="138"/>
       <c r="Z46" s="138"/>
       <c r="AA46" s="138" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="AB46" s="138"/>
       <c r="AC46" s="138"/>
@@ -12315,15 +12430,15 @@
     </row>
     <row r="48" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="24" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="23" t="s">
+        <v>432</v>
+      </c>
+      <c r="C49" t="s">
         <v>433</v>
-      </c>
-      <c r="C49" t="s">
-        <v>434</v>
       </c>
     </row>
   </sheetData>
@@ -12386,7 +12501,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="123" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B1" s="123"/>
       <c r="C1" s="123"/>
@@ -12431,15 +12546,15 @@
         <v>0</v>
       </c>
       <c r="K3" s="35" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="L3" s="35" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C4" s="22">
         <v>0</v>
@@ -12476,7 +12591,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C5" s="22">
         <v>0</v>
@@ -12513,7 +12628,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C6" s="22">
         <v>0</v>
@@ -12550,7 +12665,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C7" s="22">
         <v>0</v>
@@ -12770,55 +12885,55 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
+        <v>283</v>
+      </c>
+      <c r="C4" s="38">
+        <v>0</v>
+      </c>
+      <c r="D4" s="38">
+        <v>0</v>
+      </c>
+      <c r="E4" s="38">
+        <v>0</v>
+      </c>
+      <c r="F4" s="38">
+        <v>0</v>
+      </c>
+      <c r="G4" s="38">
+        <v>0</v>
+      </c>
+      <c r="H4" s="38">
+        <v>0</v>
+      </c>
+      <c r="I4" s="38">
+        <v>0</v>
+      </c>
+      <c r="J4" s="38">
+        <v>0</v>
+      </c>
+      <c r="K4" s="38">
+        <v>0</v>
+      </c>
+      <c r="L4" s="38">
+        <v>0</v>
+      </c>
+      <c r="M4" s="38">
+        <v>0</v>
+      </c>
+      <c r="N4" s="38">
+        <v>0</v>
+      </c>
+      <c r="O4" s="38">
+        <v>0</v>
+      </c>
+      <c r="P4" s="38">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="38">
+        <v>0</v>
+      </c>
+      <c r="R4" s="38" t="s">
         <v>284</v>
-      </c>
-      <c r="C4" s="38">
-        <v>0</v>
-      </c>
-      <c r="D4" s="38">
-        <v>0</v>
-      </c>
-      <c r="E4" s="38">
-        <v>0</v>
-      </c>
-      <c r="F4" s="38">
-        <v>0</v>
-      </c>
-      <c r="G4" s="38">
-        <v>0</v>
-      </c>
-      <c r="H4" s="38">
-        <v>0</v>
-      </c>
-      <c r="I4" s="38">
-        <v>0</v>
-      </c>
-      <c r="J4" s="38">
-        <v>0</v>
-      </c>
-      <c r="K4" s="38">
-        <v>0</v>
-      </c>
-      <c r="L4" s="38">
-        <v>0</v>
-      </c>
-      <c r="M4" s="38">
-        <v>0</v>
-      </c>
-      <c r="N4" s="38">
-        <v>0</v>
-      </c>
-      <c r="O4" s="38">
-        <v>0</v>
-      </c>
-      <c r="P4" s="38">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="38">
-        <v>0</v>
-      </c>
-      <c r="R4" s="38" t="s">
-        <v>285</v>
       </c>
       <c r="T4" s="10" t="s">
         <v>128</v>
@@ -12882,52 +12997,52 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
+        <v>281</v>
+      </c>
+      <c r="C6" s="37">
+        <v>0</v>
+      </c>
+      <c r="D6" s="37">
+        <v>0</v>
+      </c>
+      <c r="E6" s="37">
+        <v>0</v>
+      </c>
+      <c r="F6" s="37">
+        <v>0</v>
+      </c>
+      <c r="G6" s="37">
+        <v>0</v>
+      </c>
+      <c r="H6" s="37">
+        <v>0</v>
+      </c>
+      <c r="I6" s="37">
+        <v>0</v>
+      </c>
+      <c r="J6" s="37">
+        <v>0</v>
+      </c>
+      <c r="K6" s="37">
+        <v>0</v>
+      </c>
+      <c r="L6" s="37">
+        <v>0</v>
+      </c>
+      <c r="M6" s="37">
+        <v>0</v>
+      </c>
+      <c r="N6" s="37">
+        <v>1</v>
+      </c>
+      <c r="O6" s="118" t="s">
         <v>282</v>
-      </c>
-      <c r="C6" s="37">
-        <v>0</v>
-      </c>
-      <c r="D6" s="37">
-        <v>0</v>
-      </c>
-      <c r="E6" s="37">
-        <v>0</v>
-      </c>
-      <c r="F6" s="37">
-        <v>0</v>
-      </c>
-      <c r="G6" s="37">
-        <v>0</v>
-      </c>
-      <c r="H6" s="37">
-        <v>0</v>
-      </c>
-      <c r="I6" s="37">
-        <v>0</v>
-      </c>
-      <c r="J6" s="37">
-        <v>0</v>
-      </c>
-      <c r="K6" s="37">
-        <v>0</v>
-      </c>
-      <c r="L6" s="37">
-        <v>0</v>
-      </c>
-      <c r="M6" s="37">
-        <v>0</v>
-      </c>
-      <c r="N6" s="37">
-        <v>1</v>
-      </c>
-      <c r="O6" s="118" t="s">
-        <v>283</v>
       </c>
       <c r="P6" s="118"/>
       <c r="Q6" s="118"/>
       <c r="R6" s="118"/>
       <c r="T6" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -13092,34 +13207,34 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0</v>
+      </c>
+      <c r="G11" s="6">
+        <v>1</v>
+      </c>
+      <c r="H11" s="6">
+        <v>0</v>
+      </c>
+      <c r="I11" s="6">
+        <v>0</v>
+      </c>
+      <c r="J11" s="6">
+        <v>0</v>
+      </c>
+      <c r="K11" s="118" t="s">
         <v>280</v>
-      </c>
-      <c r="C11" s="6">
-        <v>0</v>
-      </c>
-      <c r="D11" s="6">
-        <v>0</v>
-      </c>
-      <c r="E11" s="6">
-        <v>0</v>
-      </c>
-      <c r="F11" s="6">
-        <v>0</v>
-      </c>
-      <c r="G11" s="6">
-        <v>1</v>
-      </c>
-      <c r="H11" s="6">
-        <v>0</v>
-      </c>
-      <c r="I11" s="6">
-        <v>0</v>
-      </c>
-      <c r="J11" s="6">
-        <v>0</v>
-      </c>
-      <c r="K11" s="118" t="s">
-        <v>281</v>
       </c>
       <c r="L11" s="118"/>
       <c r="M11" s="118"/>
@@ -13129,7 +13244,7 @@
       <c r="Q11" s="118"/>
       <c r="R11" s="118"/>
       <c r="T11" s="10" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -13154,7 +13269,7 @@
     </row>
     <row r="13" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -13176,34 +13291,34 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="C14" s="6">
+        <v>1</v>
+      </c>
+      <c r="D14" s="6">
+        <v>0</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0</v>
+      </c>
+      <c r="H14" s="6">
+        <v>0</v>
+      </c>
+      <c r="I14" s="6">
+        <v>0</v>
+      </c>
+      <c r="J14" s="6">
+        <v>0</v>
+      </c>
+      <c r="K14" s="104" t="s">
         <v>412</v>
-      </c>
-      <c r="C14" s="6">
-        <v>1</v>
-      </c>
-      <c r="D14" s="6">
-        <v>0</v>
-      </c>
-      <c r="E14" s="6">
-        <v>0</v>
-      </c>
-      <c r="F14" s="6">
-        <v>0</v>
-      </c>
-      <c r="G14" s="6">
-        <v>0</v>
-      </c>
-      <c r="H14" s="6">
-        <v>0</v>
-      </c>
-      <c r="I14" s="6">
-        <v>0</v>
-      </c>
-      <c r="J14" s="6">
-        <v>0</v>
-      </c>
-      <c r="K14" s="104" t="s">
-        <v>413</v>
       </c>
       <c r="L14" s="105"/>
       <c r="M14" s="105"/>
@@ -13213,7 +13328,7 @@
       <c r="Q14" s="105"/>
       <c r="R14" s="106"/>
       <c r="T14" s="10" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
@@ -13791,7 +13906,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="123" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B1" s="123"/>
     </row>
@@ -13801,7 +13916,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -13809,7 +13924,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -13817,7 +13932,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
colour display; memcpy is now DMA copy
DMA == Direct Memory Access
</commit_message>
<xml_diff>
--- a/doc/RiscyInstSet32Bit.xlsx
+++ b/doc/RiscyInstSet32Bit.xlsx
@@ -1516,9 +1516,6 @@
     <t>Memcpy Parametres</t>
   </si>
   <si>
-    <t>Following values must be stored in the register</t>
-  </si>
-  <si>
     <t>Length</t>
   </si>
   <si>
@@ -1553,6 +1550,9 @@
   </si>
   <si>
     <t>Unused registers are simply ignored</t>
+  </si>
+  <si>
+    <t>Following values must be stored in the register. Length of zero is interpreted as 65536</t>
   </si>
 </sst>
 </file>
@@ -2363,6 +2363,60 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2381,27 +2435,33 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="28" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="29" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="30" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2411,63 +2471,12 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="28" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="29" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="30" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2483,68 +2492,59 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -2853,43 +2853,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="99" t="s">
         <v>276</v>
       </c>
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
-      <c r="J1" s="123"/>
-      <c r="K1" s="123"/>
-      <c r="L1" s="123"/>
-      <c r="M1" s="123"/>
-      <c r="N1" s="123"/>
-      <c r="O1" s="123"/>
-      <c r="P1" s="123"/>
-      <c r="Q1" s="123"/>
-      <c r="R1" s="123"/>
-      <c r="S1" s="123"/>
-      <c r="T1" s="123"/>
-      <c r="U1" s="123"/>
-      <c r="V1" s="123"/>
-      <c r="W1" s="123"/>
-      <c r="X1" s="123"/>
-      <c r="Y1" s="123"/>
-      <c r="Z1" s="123"/>
-      <c r="AA1" s="123"/>
-      <c r="AB1" s="123"/>
-      <c r="AC1" s="123"/>
-      <c r="AD1" s="123"/>
-      <c r="AE1" s="123"/>
-      <c r="AF1" s="123"/>
-      <c r="AG1" s="123"/>
-      <c r="AH1" s="123"/>
-      <c r="AI1" s="124"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
+      <c r="L1" s="99"/>
+      <c r="M1" s="99"/>
+      <c r="N1" s="99"/>
+      <c r="O1" s="99"/>
+      <c r="P1" s="99"/>
+      <c r="Q1" s="99"/>
+      <c r="R1" s="99"/>
+      <c r="S1" s="99"/>
+      <c r="T1" s="99"/>
+      <c r="U1" s="99"/>
+      <c r="V1" s="99"/>
+      <c r="W1" s="99"/>
+      <c r="X1" s="99"/>
+      <c r="Y1" s="99"/>
+      <c r="Z1" s="99"/>
+      <c r="AA1" s="99"/>
+      <c r="AB1" s="99"/>
+      <c r="AC1" s="99"/>
+      <c r="AD1" s="99"/>
+      <c r="AE1" s="99"/>
+      <c r="AF1" s="99"/>
+      <c r="AG1" s="99"/>
+      <c r="AH1" s="99"/>
+      <c r="AI1" s="100"/>
     </row>
     <row r="2" spans="1:38" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
@@ -3181,11 +3181,11 @@
       <c r="B10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="128" t="s">
+      <c r="D10" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="128"/>
-      <c r="F10" s="128"/>
+      <c r="E10" s="112"/>
+      <c r="F10" s="112"/>
       <c r="G10" s="11">
         <v>0</v>
       </c>
@@ -3195,24 +3195,24 @@
       <c r="I10" s="11">
         <v>0</v>
       </c>
-      <c r="J10" s="119" t="s">
+      <c r="J10" s="122" t="s">
         <v>5</v>
       </c>
-      <c r="K10" s="119"/>
-      <c r="L10" s="119"/>
-      <c r="M10" s="120"/>
-      <c r="N10" s="96" t="s">
+      <c r="K10" s="122"/>
+      <c r="L10" s="122"/>
+      <c r="M10" s="123"/>
+      <c r="N10" s="114" t="s">
         <v>9</v>
       </c>
-      <c r="O10" s="97"/>
-      <c r="P10" s="97"/>
-      <c r="Q10" s="98"/>
-      <c r="R10" s="96" t="s">
+      <c r="O10" s="115"/>
+      <c r="P10" s="115"/>
+      <c r="Q10" s="116"/>
+      <c r="R10" s="114" t="s">
         <v>10</v>
       </c>
-      <c r="S10" s="97"/>
-      <c r="T10" s="97"/>
-      <c r="U10" s="98"/>
+      <c r="S10" s="115"/>
+      <c r="T10" s="115"/>
+      <c r="U10" s="116"/>
       <c r="V10" s="6">
         <v>0</v>
       </c>
@@ -3237,14 +3237,14 @@
       <c r="AC10" s="87">
         <v>0</v>
       </c>
-      <c r="AD10" s="96" t="s">
+      <c r="AD10" s="114" t="s">
         <v>306</v>
       </c>
-      <c r="AE10" s="97"/>
-      <c r="AF10" s="97"/>
-      <c r="AG10" s="97"/>
-      <c r="AH10" s="97"/>
-      <c r="AI10" s="98"/>
+      <c r="AE10" s="115"/>
+      <c r="AF10" s="115"/>
+      <c r="AG10" s="115"/>
+      <c r="AH10" s="115"/>
+      <c r="AI10" s="116"/>
       <c r="AK10" s="10" t="s">
         <v>144</v>
       </c>
@@ -3256,11 +3256,11 @@
       <c r="B11" s="30" t="s">
         <v>471</v>
       </c>
-      <c r="D11" s="103" t="s">
+      <c r="D11" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="103"/>
-      <c r="F11" s="103"/>
+      <c r="E11" s="108"/>
+      <c r="F11" s="108"/>
       <c r="G11" s="28">
         <v>0</v>
       </c>
@@ -3270,24 +3270,24 @@
       <c r="I11" s="28">
         <v>0</v>
       </c>
-      <c r="J11" s="104" t="s">
+      <c r="J11" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="K11" s="105"/>
-      <c r="L11" s="105"/>
-      <c r="M11" s="106"/>
-      <c r="N11" s="116" t="s">
+      <c r="K11" s="102"/>
+      <c r="L11" s="102"/>
+      <c r="M11" s="103"/>
+      <c r="N11" s="110" t="s">
         <v>303</v>
       </c>
-      <c r="O11" s="117"/>
-      <c r="P11" s="117"/>
-      <c r="Q11" s="117"/>
-      <c r="R11" s="107" t="s">
+      <c r="O11" s="111"/>
+      <c r="P11" s="111"/>
+      <c r="Q11" s="111"/>
+      <c r="R11" s="120" t="s">
         <v>143</v>
       </c>
-      <c r="S11" s="107"/>
-      <c r="T11" s="107"/>
-      <c r="U11" s="108"/>
+      <c r="S11" s="120"/>
+      <c r="T11" s="120"/>
+      <c r="U11" s="121"/>
       <c r="V11" s="64">
         <v>0</v>
       </c>
@@ -3341,11 +3341,11 @@
       <c r="B12" s="43" t="s">
         <v>472</v>
       </c>
-      <c r="D12" s="103" t="s">
+      <c r="D12" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="103"/>
-      <c r="F12" s="103"/>
+      <c r="E12" s="108"/>
+      <c r="F12" s="108"/>
       <c r="G12" s="45">
         <v>0</v>
       </c>
@@ -3355,24 +3355,24 @@
       <c r="I12" s="45">
         <v>0</v>
       </c>
-      <c r="J12" s="104" t="s">
+      <c r="J12" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="K12" s="105"/>
-      <c r="L12" s="105"/>
-      <c r="M12" s="106"/>
-      <c r="N12" s="116" t="s">
+      <c r="K12" s="102"/>
+      <c r="L12" s="102"/>
+      <c r="M12" s="103"/>
+      <c r="N12" s="110" t="s">
         <v>303</v>
       </c>
-      <c r="O12" s="117"/>
-      <c r="P12" s="117"/>
-      <c r="Q12" s="117"/>
-      <c r="R12" s="107" t="s">
+      <c r="O12" s="111"/>
+      <c r="P12" s="111"/>
+      <c r="Q12" s="111"/>
+      <c r="R12" s="120" t="s">
         <v>143</v>
       </c>
-      <c r="S12" s="107"/>
-      <c r="T12" s="107"/>
-      <c r="U12" s="108"/>
+      <c r="S12" s="120"/>
+      <c r="T12" s="120"/>
+      <c r="U12" s="121"/>
       <c r="V12" s="64">
         <v>0</v>
       </c>
@@ -3426,11 +3426,11 @@
       <c r="B13" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D13" s="103" t="s">
+      <c r="D13" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="103"/>
-      <c r="F13" s="103"/>
+      <c r="E13" s="108"/>
+      <c r="F13" s="108"/>
       <c r="G13" s="12">
         <v>0</v>
       </c>
@@ -3440,24 +3440,24 @@
       <c r="I13" s="12">
         <v>0</v>
       </c>
-      <c r="J13" s="104" t="s">
+      <c r="J13" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="K13" s="105"/>
-      <c r="L13" s="105"/>
-      <c r="M13" s="106"/>
-      <c r="N13" s="116" t="s">
+      <c r="K13" s="102"/>
+      <c r="L13" s="102"/>
+      <c r="M13" s="103"/>
+      <c r="N13" s="110" t="s">
         <v>9</v>
       </c>
-      <c r="O13" s="117"/>
-      <c r="P13" s="117"/>
-      <c r="Q13" s="117"/>
-      <c r="R13" s="118" t="s">
+      <c r="O13" s="111"/>
+      <c r="P13" s="111"/>
+      <c r="Q13" s="111"/>
+      <c r="R13" s="124" t="s">
         <v>85</v>
       </c>
-      <c r="S13" s="118"/>
-      <c r="T13" s="118"/>
-      <c r="U13" s="118"/>
+      <c r="S13" s="124"/>
+      <c r="T13" s="124"/>
+      <c r="U13" s="124"/>
       <c r="V13" s="64">
         <v>0</v>
       </c>
@@ -3491,15 +3491,15 @@
       <c r="AF13" s="63">
         <v>0</v>
       </c>
-      <c r="AG13" s="102" t="s">
+      <c r="AG13" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="AH13" s="103"/>
+      <c r="AH13" s="108"/>
       <c r="AI13" s="19" t="s">
         <v>84</v>
       </c>
       <c r="AK13" s="10" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="AL13" s="2" t="s">
         <v>154</v>
@@ -3512,11 +3512,11 @@
       <c r="B14" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D14" s="103" t="s">
+      <c r="D14" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="103"/>
-      <c r="F14" s="103"/>
+      <c r="E14" s="108"/>
+      <c r="F14" s="108"/>
       <c r="G14" s="12">
         <v>0</v>
       </c>
@@ -3526,18 +3526,18 @@
       <c r="I14" s="12">
         <v>0</v>
       </c>
-      <c r="J14" s="104" t="s">
+      <c r="J14" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="K14" s="105"/>
-      <c r="L14" s="105"/>
-      <c r="M14" s="106"/>
-      <c r="N14" s="116" t="s">
+      <c r="K14" s="102"/>
+      <c r="L14" s="102"/>
+      <c r="M14" s="103"/>
+      <c r="N14" s="110" t="s">
         <v>9</v>
       </c>
-      <c r="O14" s="117"/>
-      <c r="P14" s="117"/>
-      <c r="Q14" s="117"/>
+      <c r="O14" s="111"/>
+      <c r="P14" s="111"/>
+      <c r="Q14" s="111"/>
       <c r="R14" s="6">
         <v>0</v>
       </c>
@@ -3603,11 +3603,11 @@
       <c r="B15" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="102" t="s">
+      <c r="D15" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="121"/>
-      <c r="F15" s="122"/>
+      <c r="E15" s="113"/>
+      <c r="F15" s="109"/>
       <c r="G15" s="76">
         <v>0</v>
       </c>
@@ -3617,18 +3617,18 @@
       <c r="I15" s="77">
         <v>0</v>
       </c>
-      <c r="J15" s="104" t="s">
+      <c r="J15" s="101" t="s">
         <v>490</v>
       </c>
-      <c r="K15" s="105"/>
-      <c r="L15" s="105"/>
-      <c r="M15" s="106"/>
-      <c r="N15" s="107" t="s">
+      <c r="K15" s="102"/>
+      <c r="L15" s="102"/>
+      <c r="M15" s="103"/>
+      <c r="N15" s="120" t="s">
         <v>143</v>
       </c>
-      <c r="O15" s="107"/>
-      <c r="P15" s="107"/>
-      <c r="Q15" s="108"/>
+      <c r="O15" s="120"/>
+      <c r="P15" s="120"/>
+      <c r="Q15" s="121"/>
       <c r="R15" s="63">
         <v>0</v>
       </c>
@@ -3694,11 +3694,11 @@
       <c r="B16" s="7" t="s">
         <v>467</v>
       </c>
-      <c r="D16" s="102" t="s">
+      <c r="D16" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="103"/>
-      <c r="F16" s="122"/>
+      <c r="E16" s="108"/>
+      <c r="F16" s="109"/>
       <c r="G16" s="12">
         <v>0</v>
       </c>
@@ -3708,42 +3708,42 @@
       <c r="I16" s="12">
         <v>1</v>
       </c>
-      <c r="J16" s="104" t="s">
+      <c r="J16" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="K16" s="105"/>
-      <c r="L16" s="105"/>
-      <c r="M16" s="106"/>
-      <c r="N16" s="107" t="s">
+      <c r="K16" s="102"/>
+      <c r="L16" s="102"/>
+      <c r="M16" s="103"/>
+      <c r="N16" s="120" t="s">
         <v>143</v>
       </c>
-      <c r="O16" s="107"/>
-      <c r="P16" s="107"/>
-      <c r="Q16" s="108"/>
+      <c r="O16" s="120"/>
+      <c r="P16" s="120"/>
+      <c r="Q16" s="121"/>
       <c r="R16" s="71">
         <v>0</v>
       </c>
       <c r="S16" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="T16" s="104" t="s">
+      <c r="T16" s="101" t="s">
         <v>140</v>
       </c>
-      <c r="U16" s="105"/>
-      <c r="V16" s="105"/>
-      <c r="W16" s="105"/>
-      <c r="X16" s="105"/>
-      <c r="Y16" s="105"/>
-      <c r="Z16" s="105"/>
-      <c r="AA16" s="105"/>
-      <c r="AB16" s="105"/>
-      <c r="AC16" s="105"/>
-      <c r="AD16" s="105"/>
-      <c r="AE16" s="105"/>
-      <c r="AF16" s="105"/>
-      <c r="AG16" s="105"/>
-      <c r="AH16" s="105"/>
-      <c r="AI16" s="106"/>
+      <c r="U16" s="102"/>
+      <c r="V16" s="102"/>
+      <c r="W16" s="102"/>
+      <c r="X16" s="102"/>
+      <c r="Y16" s="102"/>
+      <c r="Z16" s="102"/>
+      <c r="AA16" s="102"/>
+      <c r="AB16" s="102"/>
+      <c r="AC16" s="102"/>
+      <c r="AD16" s="102"/>
+      <c r="AE16" s="102"/>
+      <c r="AF16" s="102"/>
+      <c r="AG16" s="102"/>
+      <c r="AH16" s="102"/>
+      <c r="AI16" s="103"/>
       <c r="AK16" s="10" t="s">
         <v>464</v>
       </c>
@@ -3755,11 +3755,11 @@
       <c r="B17" s="73" t="s">
         <v>466</v>
       </c>
-      <c r="D17" s="102" t="s">
+      <c r="D17" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="103"/>
-      <c r="F17" s="122"/>
+      <c r="E17" s="108"/>
+      <c r="F17" s="109"/>
       <c r="G17" s="72">
         <v>0</v>
       </c>
@@ -3769,42 +3769,42 @@
       <c r="I17" s="72">
         <v>1</v>
       </c>
-      <c r="J17" s="104" t="s">
+      <c r="J17" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="K17" s="105"/>
-      <c r="L17" s="105"/>
-      <c r="M17" s="106"/>
-      <c r="N17" s="116" t="s">
+      <c r="K17" s="102"/>
+      <c r="L17" s="102"/>
+      <c r="M17" s="103"/>
+      <c r="N17" s="110" t="s">
         <v>85</v>
       </c>
-      <c r="O17" s="117"/>
-      <c r="P17" s="117"/>
-      <c r="Q17" s="117"/>
+      <c r="O17" s="111"/>
+      <c r="P17" s="111"/>
+      <c r="Q17" s="111"/>
       <c r="R17" s="74">
         <v>1</v>
       </c>
       <c r="S17" s="72">
         <v>0</v>
       </c>
-      <c r="T17" s="104" t="s">
+      <c r="T17" s="101" t="s">
         <v>465</v>
       </c>
-      <c r="U17" s="105"/>
-      <c r="V17" s="105"/>
-      <c r="W17" s="105"/>
-      <c r="X17" s="105"/>
-      <c r="Y17" s="105"/>
-      <c r="Z17" s="105"/>
-      <c r="AA17" s="105"/>
-      <c r="AB17" s="105"/>
-      <c r="AC17" s="105"/>
-      <c r="AD17" s="105"/>
-      <c r="AE17" s="105"/>
-      <c r="AF17" s="105"/>
-      <c r="AG17" s="105"/>
-      <c r="AH17" s="105"/>
-      <c r="AI17" s="106"/>
+      <c r="U17" s="102"/>
+      <c r="V17" s="102"/>
+      <c r="W17" s="102"/>
+      <c r="X17" s="102"/>
+      <c r="Y17" s="102"/>
+      <c r="Z17" s="102"/>
+      <c r="AA17" s="102"/>
+      <c r="AB17" s="102"/>
+      <c r="AC17" s="102"/>
+      <c r="AD17" s="102"/>
+      <c r="AE17" s="102"/>
+      <c r="AF17" s="102"/>
+      <c r="AG17" s="102"/>
+      <c r="AH17" s="102"/>
+      <c r="AI17" s="103"/>
       <c r="AK17" s="10"/>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
@@ -3814,11 +3814,11 @@
       <c r="B18" s="67" t="s">
         <v>142</v>
       </c>
-      <c r="D18" s="102" t="s">
+      <c r="D18" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="121"/>
-      <c r="F18" s="122"/>
+      <c r="E18" s="113"/>
+      <c r="F18" s="109"/>
       <c r="G18" s="64">
         <v>0</v>
       </c>
@@ -3828,36 +3828,36 @@
       <c r="I18" s="70" t="s">
         <v>84</v>
       </c>
-      <c r="J18" s="104" t="s">
+      <c r="J18" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="K18" s="105"/>
-      <c r="L18" s="105"/>
-      <c r="M18" s="106"/>
-      <c r="N18" s="104" t="s">
+      <c r="K18" s="102"/>
+      <c r="L18" s="102"/>
+      <c r="M18" s="103"/>
+      <c r="N18" s="101" t="s">
         <v>4</v>
       </c>
-      <c r="O18" s="105"/>
-      <c r="P18" s="105"/>
-      <c r="Q18" s="105"/>
-      <c r="R18" s="105"/>
-      <c r="S18" s="105"/>
-      <c r="T18" s="105"/>
-      <c r="U18" s="105"/>
-      <c r="V18" s="105"/>
-      <c r="W18" s="105"/>
-      <c r="X18" s="105"/>
-      <c r="Y18" s="105"/>
-      <c r="Z18" s="105"/>
-      <c r="AA18" s="105"/>
-      <c r="AB18" s="105"/>
-      <c r="AC18" s="105"/>
-      <c r="AD18" s="105"/>
-      <c r="AE18" s="105"/>
-      <c r="AF18" s="105"/>
-      <c r="AG18" s="105"/>
-      <c r="AH18" s="105"/>
-      <c r="AI18" s="106"/>
+      <c r="O18" s="102"/>
+      <c r="P18" s="102"/>
+      <c r="Q18" s="102"/>
+      <c r="R18" s="102"/>
+      <c r="S18" s="102"/>
+      <c r="T18" s="102"/>
+      <c r="U18" s="102"/>
+      <c r="V18" s="102"/>
+      <c r="W18" s="102"/>
+      <c r="X18" s="102"/>
+      <c r="Y18" s="102"/>
+      <c r="Z18" s="102"/>
+      <c r="AA18" s="102"/>
+      <c r="AB18" s="102"/>
+      <c r="AC18" s="102"/>
+      <c r="AD18" s="102"/>
+      <c r="AE18" s="102"/>
+      <c r="AF18" s="102"/>
+      <c r="AG18" s="102"/>
+      <c r="AH18" s="102"/>
+      <c r="AI18" s="103"/>
       <c r="AK18" s="10" t="s">
         <v>159</v>
       </c>
@@ -3869,11 +3869,11 @@
       <c r="B19" s="67" t="s">
         <v>260</v>
       </c>
-      <c r="D19" s="102" t="s">
+      <c r="D19" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="121"/>
-      <c r="F19" s="122"/>
+      <c r="E19" s="113"/>
+      <c r="F19" s="109"/>
       <c r="G19" s="64">
         <v>1</v>
       </c>
@@ -3883,36 +3883,36 @@
       <c r="I19" s="64">
         <v>0</v>
       </c>
-      <c r="J19" s="112" t="s">
+      <c r="J19" s="125" t="s">
         <v>143</v>
       </c>
-      <c r="K19" s="113"/>
-      <c r="L19" s="113"/>
-      <c r="M19" s="114"/>
-      <c r="N19" s="104" t="s">
+      <c r="K19" s="126"/>
+      <c r="L19" s="126"/>
+      <c r="M19" s="127"/>
+      <c r="N19" s="101" t="s">
         <v>4</v>
       </c>
-      <c r="O19" s="105"/>
-      <c r="P19" s="105"/>
-      <c r="Q19" s="105"/>
-      <c r="R19" s="105"/>
-      <c r="S19" s="105"/>
-      <c r="T19" s="105"/>
-      <c r="U19" s="105"/>
-      <c r="V19" s="105"/>
-      <c r="W19" s="105"/>
-      <c r="X19" s="105"/>
-      <c r="Y19" s="105"/>
-      <c r="Z19" s="105"/>
-      <c r="AA19" s="105"/>
-      <c r="AB19" s="105"/>
-      <c r="AC19" s="105"/>
-      <c r="AD19" s="105"/>
-      <c r="AE19" s="105"/>
-      <c r="AF19" s="105"/>
-      <c r="AG19" s="105"/>
-      <c r="AH19" s="105"/>
-      <c r="AI19" s="106"/>
+      <c r="O19" s="102"/>
+      <c r="P19" s="102"/>
+      <c r="Q19" s="102"/>
+      <c r="R19" s="102"/>
+      <c r="S19" s="102"/>
+      <c r="T19" s="102"/>
+      <c r="U19" s="102"/>
+      <c r="V19" s="102"/>
+      <c r="W19" s="102"/>
+      <c r="X19" s="102"/>
+      <c r="Y19" s="102"/>
+      <c r="Z19" s="102"/>
+      <c r="AA19" s="102"/>
+      <c r="AB19" s="102"/>
+      <c r="AC19" s="102"/>
+      <c r="AD19" s="102"/>
+      <c r="AE19" s="102"/>
+      <c r="AF19" s="102"/>
+      <c r="AG19" s="102"/>
+      <c r="AH19" s="102"/>
+      <c r="AI19" s="103"/>
       <c r="AK19" s="10" t="s">
         <v>173</v>
       </c>
@@ -3924,11 +3924,11 @@
       <c r="B20" s="67" t="s">
         <v>374</v>
       </c>
-      <c r="D20" s="102" t="s">
+      <c r="D20" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="121"/>
-      <c r="F20" s="122"/>
+      <c r="E20" s="113"/>
+      <c r="F20" s="109"/>
       <c r="G20" s="64">
         <v>1</v>
       </c>
@@ -3938,36 +3938,36 @@
       <c r="I20" s="64">
         <v>1</v>
       </c>
-      <c r="J20" s="115" t="s">
+      <c r="J20" s="128" t="s">
         <v>143</v>
       </c>
-      <c r="K20" s="107"/>
-      <c r="L20" s="107"/>
-      <c r="M20" s="108"/>
-      <c r="N20" s="104" t="s">
+      <c r="K20" s="120"/>
+      <c r="L20" s="120"/>
+      <c r="M20" s="121"/>
+      <c r="N20" s="101" t="s">
         <v>4</v>
       </c>
-      <c r="O20" s="105"/>
-      <c r="P20" s="105"/>
-      <c r="Q20" s="105"/>
-      <c r="R20" s="105"/>
-      <c r="S20" s="105"/>
-      <c r="T20" s="105"/>
-      <c r="U20" s="105"/>
-      <c r="V20" s="105"/>
-      <c r="W20" s="105"/>
-      <c r="X20" s="105"/>
-      <c r="Y20" s="105"/>
-      <c r="Z20" s="105"/>
-      <c r="AA20" s="105"/>
-      <c r="AB20" s="105"/>
-      <c r="AC20" s="105"/>
-      <c r="AD20" s="105"/>
-      <c r="AE20" s="105"/>
-      <c r="AF20" s="105"/>
-      <c r="AG20" s="105"/>
-      <c r="AH20" s="105"/>
-      <c r="AI20" s="106"/>
+      <c r="O20" s="102"/>
+      <c r="P20" s="102"/>
+      <c r="Q20" s="102"/>
+      <c r="R20" s="102"/>
+      <c r="S20" s="102"/>
+      <c r="T20" s="102"/>
+      <c r="U20" s="102"/>
+      <c r="V20" s="102"/>
+      <c r="W20" s="102"/>
+      <c r="X20" s="102"/>
+      <c r="Y20" s="102"/>
+      <c r="Z20" s="102"/>
+      <c r="AA20" s="102"/>
+      <c r="AB20" s="102"/>
+      <c r="AC20" s="102"/>
+      <c r="AD20" s="102"/>
+      <c r="AE20" s="102"/>
+      <c r="AF20" s="102"/>
+      <c r="AG20" s="102"/>
+      <c r="AH20" s="102"/>
+      <c r="AI20" s="103"/>
       <c r="AK20" s="10"/>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
@@ -3977,11 +3977,11 @@
       <c r="B21" s="67" t="s">
         <v>222</v>
       </c>
-      <c r="D21" s="102" t="s">
+      <c r="D21" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="E21" s="121"/>
-      <c r="F21" s="122"/>
+      <c r="E21" s="113"/>
+      <c r="F21" s="109"/>
       <c r="G21" s="64">
         <v>1</v>
       </c>
@@ -3991,42 +3991,42 @@
       <c r="I21" s="64">
         <v>0</v>
       </c>
-      <c r="J21" s="109" t="s">
+      <c r="J21" s="129" t="s">
         <v>143</v>
       </c>
-      <c r="K21" s="110"/>
-      <c r="L21" s="110"/>
-      <c r="M21" s="111"/>
+      <c r="K21" s="130"/>
+      <c r="L21" s="130"/>
+      <c r="M21" s="131"/>
       <c r="N21" s="64">
         <v>0</v>
       </c>
       <c r="O21" s="64">
         <v>0</v>
       </c>
-      <c r="P21" s="125" t="s">
+      <c r="P21" s="104" t="s">
         <v>224</v>
       </c>
-      <c r="Q21" s="126"/>
-      <c r="R21" s="126"/>
-      <c r="S21" s="126"/>
-      <c r="T21" s="126"/>
-      <c r="U21" s="126"/>
-      <c r="V21" s="126"/>
-      <c r="W21" s="127"/>
-      <c r="X21" s="104" t="s">
+      <c r="Q21" s="105"/>
+      <c r="R21" s="105"/>
+      <c r="S21" s="105"/>
+      <c r="T21" s="105"/>
+      <c r="U21" s="105"/>
+      <c r="V21" s="105"/>
+      <c r="W21" s="106"/>
+      <c r="X21" s="101" t="s">
         <v>223</v>
       </c>
-      <c r="Y21" s="105"/>
-      <c r="Z21" s="105"/>
-      <c r="AA21" s="105"/>
-      <c r="AB21" s="105"/>
-      <c r="AC21" s="105"/>
-      <c r="AD21" s="105"/>
-      <c r="AE21" s="105"/>
-      <c r="AF21" s="105"/>
-      <c r="AG21" s="105"/>
-      <c r="AH21" s="105"/>
-      <c r="AI21" s="106"/>
+      <c r="Y21" s="102"/>
+      <c r="Z21" s="102"/>
+      <c r="AA21" s="102"/>
+      <c r="AB21" s="102"/>
+      <c r="AC21" s="102"/>
+      <c r="AD21" s="102"/>
+      <c r="AE21" s="102"/>
+      <c r="AF21" s="102"/>
+      <c r="AG21" s="102"/>
+      <c r="AH21" s="102"/>
+      <c r="AI21" s="103"/>
       <c r="AK21" s="10" t="s">
         <v>489</v>
       </c>
@@ -4038,11 +4038,11 @@
       <c r="B22" s="67" t="s">
         <v>228</v>
       </c>
-      <c r="D22" s="102" t="s">
+      <c r="D22" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="121"/>
-      <c r="F22" s="122"/>
+      <c r="E22" s="113"/>
+      <c r="F22" s="109"/>
       <c r="G22" s="64">
         <v>1</v>
       </c>
@@ -4052,12 +4052,12 @@
       <c r="I22" s="64">
         <v>0</v>
       </c>
-      <c r="J22" s="104" t="s">
+      <c r="J22" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="K22" s="105"/>
-      <c r="L22" s="105"/>
-      <c r="M22" s="106"/>
+      <c r="K22" s="102"/>
+      <c r="L22" s="102"/>
+      <c r="M22" s="103"/>
       <c r="N22" s="64">
         <v>0</v>
       </c>
@@ -4100,16 +4100,16 @@
       <c r="AA22" s="55">
         <v>0</v>
       </c>
-      <c r="AB22" s="104" t="s">
+      <c r="AB22" s="101" t="s">
         <v>226</v>
       </c>
-      <c r="AC22" s="105"/>
-      <c r="AD22" s="105"/>
-      <c r="AE22" s="105"/>
-      <c r="AF22" s="105"/>
-      <c r="AG22" s="105"/>
-      <c r="AH22" s="105"/>
-      <c r="AI22" s="106"/>
+      <c r="AC22" s="102"/>
+      <c r="AD22" s="102"/>
+      <c r="AE22" s="102"/>
+      <c r="AF22" s="102"/>
+      <c r="AG22" s="102"/>
+      <c r="AH22" s="102"/>
+      <c r="AI22" s="103"/>
       <c r="AK22" s="10" t="s">
         <v>227</v>
       </c>
@@ -4121,11 +4121,11 @@
       <c r="B23" s="67" t="s">
         <v>82</v>
       </c>
-      <c r="D23" s="102" t="s">
+      <c r="D23" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="121"/>
-      <c r="F23" s="122"/>
+      <c r="E23" s="113"/>
+      <c r="F23" s="109"/>
       <c r="G23" s="63">
         <v>1</v>
       </c>
@@ -4135,12 +4135,12 @@
       <c r="I23" s="63">
         <v>0</v>
       </c>
-      <c r="J23" s="104" t="s">
+      <c r="J23" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="K23" s="105"/>
-      <c r="L23" s="105"/>
-      <c r="M23" s="106"/>
+      <c r="K23" s="102"/>
+      <c r="L23" s="102"/>
+      <c r="M23" s="103"/>
       <c r="N23" s="64">
         <v>0</v>
       </c>
@@ -4183,16 +4183,16 @@
       <c r="AA23" s="81">
         <v>1</v>
       </c>
-      <c r="AB23" s="104" t="s">
+      <c r="AB23" s="101" t="s">
         <v>81</v>
       </c>
-      <c r="AC23" s="105"/>
-      <c r="AD23" s="105"/>
-      <c r="AE23" s="105"/>
-      <c r="AF23" s="105"/>
-      <c r="AG23" s="105"/>
-      <c r="AH23" s="105"/>
-      <c r="AI23" s="106"/>
+      <c r="AC23" s="102"/>
+      <c r="AD23" s="102"/>
+      <c r="AE23" s="102"/>
+      <c r="AF23" s="102"/>
+      <c r="AG23" s="102"/>
+      <c r="AH23" s="102"/>
+      <c r="AI23" s="103"/>
       <c r="AK23" s="10" t="s">
         <v>83</v>
       </c>
@@ -4204,11 +4204,11 @@
       <c r="B24" s="67" t="s">
         <v>88</v>
       </c>
-      <c r="D24" s="102" t="s">
+      <c r="D24" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="121"/>
-      <c r="F24" s="122"/>
+      <c r="E24" s="113"/>
+      <c r="F24" s="109"/>
       <c r="G24" s="63">
         <v>1</v>
       </c>
@@ -4218,12 +4218,12 @@
       <c r="I24" s="63">
         <v>0</v>
       </c>
-      <c r="J24" s="104" t="s">
+      <c r="J24" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="K24" s="105"/>
-      <c r="L24" s="105"/>
-      <c r="M24" s="106"/>
+      <c r="K24" s="102"/>
+      <c r="L24" s="102"/>
+      <c r="M24" s="103"/>
       <c r="N24" s="64">
         <v>0</v>
       </c>
@@ -4266,16 +4266,16 @@
       <c r="AA24" s="55">
         <v>0</v>
       </c>
-      <c r="AB24" s="104" t="s">
+      <c r="AB24" s="101" t="s">
         <v>81</v>
       </c>
-      <c r="AC24" s="105"/>
-      <c r="AD24" s="105"/>
-      <c r="AE24" s="105"/>
-      <c r="AF24" s="105"/>
-      <c r="AG24" s="105"/>
-      <c r="AH24" s="105"/>
-      <c r="AI24" s="106"/>
+      <c r="AC24" s="102"/>
+      <c r="AD24" s="102"/>
+      <c r="AE24" s="102"/>
+      <c r="AF24" s="102"/>
+      <c r="AG24" s="102"/>
+      <c r="AH24" s="102"/>
+      <c r="AI24" s="103"/>
       <c r="AK24" s="10" t="s">
         <v>158</v>
       </c>
@@ -4287,11 +4287,11 @@
       <c r="B25" s="67" t="s">
         <v>89</v>
       </c>
-      <c r="D25" s="102" t="s">
+      <c r="D25" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="121"/>
-      <c r="F25" s="122"/>
+      <c r="E25" s="113"/>
+      <c r="F25" s="109"/>
       <c r="G25" s="63">
         <v>1</v>
       </c>
@@ -4301,12 +4301,12 @@
       <c r="I25" s="63">
         <v>0</v>
       </c>
-      <c r="J25" s="104" t="s">
+      <c r="J25" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="K25" s="105"/>
-      <c r="L25" s="105"/>
-      <c r="M25" s="106"/>
+      <c r="K25" s="102"/>
+      <c r="L25" s="102"/>
+      <c r="M25" s="103"/>
       <c r="N25" s="64">
         <v>0</v>
       </c>
@@ -4382,11 +4382,11 @@
       <c r="B26" s="67" t="s">
         <v>80</v>
       </c>
-      <c r="D26" s="99" t="s">
+      <c r="D26" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="E26" s="100"/>
-      <c r="F26" s="101"/>
+      <c r="E26" s="118"/>
+      <c r="F26" s="119"/>
       <c r="G26" s="63">
         <v>1</v>
       </c>
@@ -4450,16 +4450,16 @@
       <c r="AA26" s="83">
         <v>0</v>
       </c>
-      <c r="AB26" s="104" t="s">
+      <c r="AB26" s="101" t="s">
         <v>80</v>
       </c>
-      <c r="AC26" s="105"/>
-      <c r="AD26" s="105"/>
-      <c r="AE26" s="105"/>
-      <c r="AF26" s="105"/>
-      <c r="AG26" s="105"/>
-      <c r="AH26" s="105"/>
-      <c r="AI26" s="106"/>
+      <c r="AC26" s="102"/>
+      <c r="AD26" s="102"/>
+      <c r="AE26" s="102"/>
+      <c r="AF26" s="102"/>
+      <c r="AG26" s="102"/>
+      <c r="AH26" s="102"/>
+      <c r="AI26" s="103"/>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
@@ -4468,11 +4468,11 @@
       <c r="B27" s="49" t="s">
         <v>409</v>
       </c>
-      <c r="D27" s="99" t="s">
+      <c r="D27" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="E27" s="100"/>
-      <c r="F27" s="101"/>
+      <c r="E27" s="118"/>
+      <c r="F27" s="119"/>
       <c r="G27" s="63">
         <v>1</v>
       </c>
@@ -4565,42 +4565,42 @@
       </c>
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B29" s="153" t="s">
-        <v>504</v>
-      </c>
-      <c r="C29" s="154"/>
-      <c r="D29" s="154"/>
-      <c r="E29" s="154"/>
-      <c r="F29" s="154"/>
-      <c r="G29" s="154"/>
-      <c r="H29" s="154"/>
-      <c r="I29" s="154"/>
-      <c r="J29" s="154"/>
-      <c r="K29" s="154"/>
-      <c r="L29" s="154"/>
-      <c r="M29" s="154"/>
-      <c r="N29" s="154"/>
-      <c r="O29" s="154"/>
-      <c r="P29" s="154"/>
-      <c r="Q29" s="154"/>
-      <c r="R29" s="154"/>
-      <c r="S29" s="154"/>
-      <c r="T29" s="154"/>
-      <c r="U29" s="154"/>
-      <c r="V29" s="154"/>
-      <c r="W29" s="154"/>
-      <c r="X29" s="154"/>
-      <c r="Y29" s="154"/>
-      <c r="Z29" s="154"/>
-      <c r="AA29" s="154"/>
-      <c r="AB29" s="154"/>
-      <c r="AC29" s="154"/>
-      <c r="AD29" s="154"/>
-      <c r="AE29" s="154"/>
-      <c r="AF29" s="154"/>
-      <c r="AG29" s="154"/>
-      <c r="AH29" s="154"/>
-      <c r="AI29" s="155"/>
+      <c r="B29" s="96" t="s">
+        <v>503</v>
+      </c>
+      <c r="C29" s="97"/>
+      <c r="D29" s="97"/>
+      <c r="E29" s="97"/>
+      <c r="F29" s="97"/>
+      <c r="G29" s="97"/>
+      <c r="H29" s="97"/>
+      <c r="I29" s="97"/>
+      <c r="J29" s="97"/>
+      <c r="K29" s="97"/>
+      <c r="L29" s="97"/>
+      <c r="M29" s="97"/>
+      <c r="N29" s="97"/>
+      <c r="O29" s="97"/>
+      <c r="P29" s="97"/>
+      <c r="Q29" s="97"/>
+      <c r="R29" s="97"/>
+      <c r="S29" s="97"/>
+      <c r="T29" s="97"/>
+      <c r="U29" s="97"/>
+      <c r="V29" s="97"/>
+      <c r="W29" s="97"/>
+      <c r="X29" s="97"/>
+      <c r="Y29" s="97"/>
+      <c r="Z29" s="97"/>
+      <c r="AA29" s="97"/>
+      <c r="AB29" s="97"/>
+      <c r="AC29" s="97"/>
+      <c r="AD29" s="97"/>
+      <c r="AE29" s="97"/>
+      <c r="AF29" s="97"/>
+      <c r="AG29" s="97"/>
+      <c r="AH29" s="97"/>
+      <c r="AI29" s="98"/>
     </row>
     <row r="33" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B33" s="7"/>
@@ -5186,6 +5186,51 @@
     </row>
   </sheetData>
   <mergeCells count="61">
+    <mergeCell ref="AD10:AI10"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="AG13:AH13"/>
+    <mergeCell ref="AB22:AI22"/>
+    <mergeCell ref="AB23:AI23"/>
+    <mergeCell ref="AB24:AI24"/>
+    <mergeCell ref="T16:AI16"/>
+    <mergeCell ref="J15:M15"/>
+    <mergeCell ref="N15:Q15"/>
+    <mergeCell ref="J21:M21"/>
+    <mergeCell ref="J22:M22"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="J24:M24"/>
+    <mergeCell ref="J25:M25"/>
+    <mergeCell ref="N18:AI18"/>
+    <mergeCell ref="N20:AI20"/>
+    <mergeCell ref="J18:M18"/>
+    <mergeCell ref="J19:M19"/>
+    <mergeCell ref="J20:M20"/>
+    <mergeCell ref="AB26:AI26"/>
+    <mergeCell ref="J14:M14"/>
+    <mergeCell ref="N14:Q14"/>
+    <mergeCell ref="J16:M16"/>
+    <mergeCell ref="N16:Q16"/>
+    <mergeCell ref="N19:AI19"/>
+    <mergeCell ref="N12:Q12"/>
+    <mergeCell ref="R12:U12"/>
+    <mergeCell ref="J13:M13"/>
+    <mergeCell ref="N13:Q13"/>
+    <mergeCell ref="R13:U13"/>
+    <mergeCell ref="R10:U10"/>
+    <mergeCell ref="J11:M11"/>
+    <mergeCell ref="N11:Q11"/>
+    <mergeCell ref="R11:U11"/>
+    <mergeCell ref="J10:M10"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D20:F20"/>
     <mergeCell ref="B29:AI29"/>
     <mergeCell ref="A1:AI1"/>
     <mergeCell ref="X21:AI21"/>
@@ -5202,51 +5247,6 @@
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="J12:M12"/>
     <mergeCell ref="N10:Q10"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="R10:U10"/>
-    <mergeCell ref="J11:M11"/>
-    <mergeCell ref="N11:Q11"/>
-    <mergeCell ref="R11:U11"/>
-    <mergeCell ref="J10:M10"/>
-    <mergeCell ref="N12:Q12"/>
-    <mergeCell ref="R12:U12"/>
-    <mergeCell ref="J13:M13"/>
-    <mergeCell ref="N13:Q13"/>
-    <mergeCell ref="R13:U13"/>
-    <mergeCell ref="J18:M18"/>
-    <mergeCell ref="J19:M19"/>
-    <mergeCell ref="J20:M20"/>
-    <mergeCell ref="AB26:AI26"/>
-    <mergeCell ref="J14:M14"/>
-    <mergeCell ref="N14:Q14"/>
-    <mergeCell ref="J16:M16"/>
-    <mergeCell ref="N16:Q16"/>
-    <mergeCell ref="N19:AI19"/>
-    <mergeCell ref="AD10:AI10"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="AG13:AH13"/>
-    <mergeCell ref="AB22:AI22"/>
-    <mergeCell ref="AB23:AI23"/>
-    <mergeCell ref="AB24:AI24"/>
-    <mergeCell ref="T16:AI16"/>
-    <mergeCell ref="J15:M15"/>
-    <mergeCell ref="N15:Q15"/>
-    <mergeCell ref="J21:M21"/>
-    <mergeCell ref="J22:M22"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="J24:M24"/>
-    <mergeCell ref="J25:M25"/>
-    <mergeCell ref="N18:AI18"/>
-    <mergeCell ref="N20:AI20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5479,25 +5479,25 @@
       <c r="F10" s="26">
         <v>0</v>
       </c>
-      <c r="G10" s="118" t="s">
+      <c r="G10" s="124" t="s">
         <v>307</v>
       </c>
-      <c r="H10" s="118"/>
-      <c r="I10" s="118"/>
-      <c r="J10" s="118"/>
-      <c r="K10" s="118"/>
-      <c r="L10" s="118" t="s">
+      <c r="H10" s="124"/>
+      <c r="I10" s="124"/>
+      <c r="J10" s="124"/>
+      <c r="K10" s="124"/>
+      <c r="L10" s="124" t="s">
         <v>5</v>
       </c>
-      <c r="M10" s="118"/>
-      <c r="N10" s="118" t="s">
+      <c r="M10" s="124"/>
+      <c r="N10" s="124" t="s">
         <v>9</v>
       </c>
-      <c r="O10" s="118"/>
-      <c r="P10" s="118" t="s">
+      <c r="O10" s="124"/>
+      <c r="P10" s="124" t="s">
         <v>10</v>
       </c>
-      <c r="Q10" s="118"/>
+      <c r="Q10" s="124"/>
       <c r="R10" s="26">
         <v>0</v>
       </c>
@@ -5536,14 +5536,14 @@
       <c r="K11" s="29">
         <v>0</v>
       </c>
-      <c r="L11" s="118" t="s">
+      <c r="L11" s="124" t="s">
         <v>5</v>
       </c>
-      <c r="M11" s="118"/>
-      <c r="N11" s="118" t="s">
+      <c r="M11" s="124"/>
+      <c r="N11" s="124" t="s">
         <v>9</v>
       </c>
-      <c r="O11" s="118"/>
+      <c r="O11" s="124"/>
       <c r="P11" s="26">
         <v>0</v>
       </c>
@@ -5589,14 +5589,14 @@
       <c r="K12" s="29">
         <v>0</v>
       </c>
-      <c r="L12" s="118" t="s">
+      <c r="L12" s="124" t="s">
         <v>5</v>
       </c>
-      <c r="M12" s="118"/>
-      <c r="N12" s="118" t="s">
+      <c r="M12" s="124"/>
+      <c r="N12" s="124" t="s">
         <v>9</v>
       </c>
-      <c r="O12" s="118"/>
+      <c r="O12" s="124"/>
       <c r="P12" s="29">
         <v>1</v>
       </c>
@@ -5631,26 +5631,26 @@
       <c r="G13" s="29">
         <v>0</v>
       </c>
-      <c r="H13" s="129" t="s">
+      <c r="H13" s="133" t="s">
         <v>5</v>
       </c>
-      <c r="I13" s="129"/>
+      <c r="I13" s="133"/>
       <c r="J13" s="29">
         <v>0</v>
       </c>
       <c r="K13" s="29">
         <v>1</v>
       </c>
-      <c r="L13" s="129" t="s">
+      <c r="L13" s="133" t="s">
         <v>141</v>
       </c>
-      <c r="M13" s="129"/>
-      <c r="N13" s="129"/>
-      <c r="O13" s="129"/>
-      <c r="P13" s="129"/>
-      <c r="Q13" s="129"/>
-      <c r="R13" s="129"/>
-      <c r="S13" s="129"/>
+      <c r="M13" s="133"/>
+      <c r="N13" s="133"/>
+      <c r="O13" s="133"/>
+      <c r="P13" s="133"/>
+      <c r="Q13" s="133"/>
+      <c r="R13" s="133"/>
+      <c r="S13" s="133"/>
       <c r="U13" s="10"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -5673,26 +5673,26 @@
       <c r="G14" s="29">
         <v>0</v>
       </c>
-      <c r="H14" s="129" t="s">
+      <c r="H14" s="133" t="s">
         <v>5</v>
       </c>
-      <c r="I14" s="129"/>
+      <c r="I14" s="133"/>
       <c r="J14" s="29">
         <v>1</v>
       </c>
       <c r="K14" s="29">
         <v>0</v>
       </c>
-      <c r="L14" s="129" t="s">
+      <c r="L14" s="133" t="s">
         <v>278</v>
       </c>
-      <c r="M14" s="129"/>
-      <c r="N14" s="129"/>
-      <c r="O14" s="129"/>
-      <c r="P14" s="129"/>
-      <c r="Q14" s="129"/>
-      <c r="R14" s="129"/>
-      <c r="S14" s="129"/>
+      <c r="M14" s="133"/>
+      <c r="N14" s="133"/>
+      <c r="O14" s="133"/>
+      <c r="P14" s="133"/>
+      <c r="Q14" s="133"/>
+      <c r="R14" s="133"/>
+      <c r="S14" s="133"/>
       <c r="U14" s="10"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -5715,26 +5715,26 @@
       <c r="G15" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="H15" s="129" t="s">
+      <c r="H15" s="133" t="s">
         <v>5</v>
       </c>
-      <c r="I15" s="129"/>
+      <c r="I15" s="133"/>
       <c r="J15" s="29">
         <v>0</v>
       </c>
       <c r="K15" s="29">
         <v>0</v>
       </c>
-      <c r="L15" s="129" t="s">
+      <c r="L15" s="133" t="s">
         <v>278</v>
       </c>
-      <c r="M15" s="129"/>
-      <c r="N15" s="129"/>
-      <c r="O15" s="129"/>
-      <c r="P15" s="129"/>
-      <c r="Q15" s="129"/>
-      <c r="R15" s="129"/>
-      <c r="S15" s="129"/>
+      <c r="M15" s="133"/>
+      <c r="N15" s="133"/>
+      <c r="O15" s="133"/>
+      <c r="P15" s="133"/>
+      <c r="Q15" s="133"/>
+      <c r="R15" s="133"/>
+      <c r="S15" s="133"/>
       <c r="U15" s="10"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -5756,30 +5756,30 @@
       <c r="G16" s="29">
         <v>1</v>
       </c>
-      <c r="H16" s="132" t="s">
+      <c r="H16" s="135" t="s">
         <v>3</v>
       </c>
-      <c r="I16" s="132"/>
-      <c r="J16" s="132"/>
+      <c r="I16" s="135"/>
+      <c r="J16" s="135"/>
       <c r="K16" s="29">
         <v>1</v>
       </c>
-      <c r="L16" s="129" t="s">
+      <c r="L16" s="133" t="s">
         <v>278</v>
       </c>
-      <c r="M16" s="129"/>
-      <c r="N16" s="129"/>
-      <c r="O16" s="129"/>
-      <c r="P16" s="129"/>
-      <c r="Q16" s="129"/>
-      <c r="R16" s="129"/>
-      <c r="S16" s="129"/>
+      <c r="M16" s="133"/>
+      <c r="N16" s="133"/>
+      <c r="O16" s="133"/>
+      <c r="P16" s="133"/>
+      <c r="Q16" s="133"/>
+      <c r="R16" s="133"/>
+      <c r="S16" s="133"/>
       <c r="U16" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="130">
+      <c r="A17" s="132">
         <v>13</v>
       </c>
       <c r="B17" s="30" t="s">
@@ -5797,14 +5797,14 @@
       <c r="G17" s="29">
         <v>0</v>
       </c>
-      <c r="H17" s="129" t="s">
+      <c r="H17" s="133" t="s">
         <v>310</v>
       </c>
-      <c r="I17" s="129"/>
-      <c r="J17" s="129" t="s">
+      <c r="I17" s="133"/>
+      <c r="J17" s="133" t="s">
         <v>313</v>
       </c>
-      <c r="K17" s="129"/>
+      <c r="K17" s="133"/>
       <c r="L17" s="29">
         <v>0</v>
       </c>
@@ -5834,7 +5834,7 @@
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="130"/>
+      <c r="A18" s="132"/>
       <c r="B18" s="30" t="s">
         <v>316</v>
       </c>
@@ -5850,14 +5850,14 @@
       <c r="G18" s="29">
         <v>0</v>
       </c>
-      <c r="H18" s="129" t="s">
+      <c r="H18" s="133" t="s">
         <v>310</v>
       </c>
-      <c r="I18" s="129"/>
-      <c r="J18" s="129" t="s">
+      <c r="I18" s="133"/>
+      <c r="J18" s="133" t="s">
         <v>313</v>
       </c>
-      <c r="K18" s="129"/>
+      <c r="K18" s="133"/>
       <c r="L18" s="29">
         <v>0</v>
       </c>
@@ -5887,7 +5887,7 @@
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="130"/>
+      <c r="A19" s="132"/>
       <c r="B19" s="30" t="s">
         <v>312</v>
       </c>
@@ -5903,12 +5903,12 @@
       <c r="G19" s="29">
         <v>0</v>
       </c>
-      <c r="H19" s="131" t="s">
+      <c r="H19" s="134" t="s">
         <v>305</v>
       </c>
-      <c r="I19" s="131"/>
-      <c r="J19" s="131"/>
-      <c r="K19" s="131"/>
+      <c r="I19" s="134"/>
+      <c r="J19" s="134"/>
+      <c r="K19" s="134"/>
       <c r="L19" s="29">
         <v>0</v>
       </c>
@@ -6133,6 +6133,18 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="L13:S13"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="L14:S14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="N11:O11"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="J18:K18"/>
@@ -6143,18 +6155,6 @@
     <mergeCell ref="J17:K17"/>
     <mergeCell ref="H16:J16"/>
     <mergeCell ref="H15:I15"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="L13:S13"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="L14:S14"/>
-    <mergeCell ref="H14:I14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6197,22 +6197,22 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="133" t="s">
+      <c r="A2" s="136" t="s">
         <v>145</v>
       </c>
-      <c r="B2" s="134"/>
-      <c r="C2" s="134"/>
-      <c r="D2" s="134"/>
-      <c r="E2" s="134"/>
-      <c r="F2" s="134"/>
-      <c r="G2" s="134"/>
-      <c r="H2" s="134"/>
-      <c r="I2" s="134"/>
-      <c r="J2" s="134"/>
-      <c r="K2" s="134"/>
-      <c r="L2" s="135"/>
+      <c r="B2" s="137"/>
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+      <c r="E2" s="137"/>
+      <c r="F2" s="137"/>
+      <c r="G2" s="137"/>
+      <c r="H2" s="137"/>
+      <c r="I2" s="137"/>
+      <c r="J2" s="137"/>
+      <c r="K2" s="137"/>
+      <c r="L2" s="138"/>
       <c r="M2" s="17" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8592,21 +8592,21 @@
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="133" t="s">
+      <c r="A2" s="136" t="s">
         <v>145</v>
       </c>
-      <c r="B2" s="134"/>
-      <c r="C2" s="134"/>
-      <c r="D2" s="134"/>
-      <c r="E2" s="134"/>
-      <c r="F2" s="134"/>
-      <c r="G2" s="134"/>
-      <c r="H2" s="134"/>
-      <c r="I2" s="134"/>
-      <c r="J2" s="134"/>
-      <c r="K2" s="135"/>
+      <c r="B2" s="137"/>
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+      <c r="E2" s="137"/>
+      <c r="F2" s="137"/>
+      <c r="G2" s="137"/>
+      <c r="H2" s="137"/>
+      <c r="I2" s="137"/>
+      <c r="J2" s="137"/>
+      <c r="K2" s="138"/>
       <c r="L2" s="17" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9434,13 +9434,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="156" t="s">
-        <v>505</v>
-      </c>
-      <c r="B1" s="156"/>
-      <c r="C1" s="156"/>
-      <c r="D1" s="156"/>
-      <c r="E1" s="156"/>
+      <c r="A1" s="139" t="s">
+        <v>504</v>
+      </c>
+      <c r="B1" s="139"/>
+      <c r="C1" s="139"/>
+      <c r="D1" s="139"/>
+      <c r="E1" s="139"/>
     </row>
     <row r="2" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="32" t="s">
@@ -10244,8 +10244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K45" sqref="K45:R45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10483,16 +10483,16 @@
       <c r="Z5" s="38">
         <v>0</v>
       </c>
-      <c r="AA5" s="117" t="s">
+      <c r="AA5" s="111" t="s">
         <v>81</v>
       </c>
-      <c r="AB5" s="117"/>
-      <c r="AC5" s="117"/>
-      <c r="AD5" s="117"/>
-      <c r="AE5" s="117"/>
-      <c r="AF5" s="117"/>
-      <c r="AG5" s="117"/>
-      <c r="AH5" s="117"/>
+      <c r="AB5" s="111"/>
+      <c r="AC5" s="111"/>
+      <c r="AD5" s="111"/>
+      <c r="AE5" s="111"/>
+      <c r="AF5" s="111"/>
+      <c r="AG5" s="111"/>
+      <c r="AH5" s="111"/>
       <c r="AJ5" s="10" t="s">
         <v>434</v>
       </c>
@@ -10573,18 +10573,18 @@
       <c r="Z6" s="95">
         <v>1</v>
       </c>
-      <c r="AA6" s="143" t="s">
+      <c r="AA6" s="153" t="s">
         <v>143</v>
       </c>
-      <c r="AB6" s="144"/>
-      <c r="AC6" s="144"/>
-      <c r="AD6" s="145"/>
-      <c r="AE6" s="116" t="s">
+      <c r="AB6" s="154"/>
+      <c r="AC6" s="154"/>
+      <c r="AD6" s="155"/>
+      <c r="AE6" s="110" t="s">
         <v>329</v>
       </c>
-      <c r="AF6" s="117"/>
-      <c r="AG6" s="117"/>
-      <c r="AH6" s="136"/>
+      <c r="AF6" s="111"/>
+      <c r="AG6" s="111"/>
+      <c r="AH6" s="156"/>
       <c r="AJ6" s="10" t="s">
         <v>370</v>
       </c>
@@ -10665,16 +10665,16 @@
       <c r="Z7" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="AA7" s="140" t="s">
+      <c r="AA7" s="150" t="s">
         <v>372</v>
       </c>
-      <c r="AB7" s="141"/>
-      <c r="AC7" s="141"/>
-      <c r="AD7" s="141"/>
-      <c r="AE7" s="141"/>
-      <c r="AF7" s="141"/>
-      <c r="AG7" s="141"/>
-      <c r="AH7" s="142"/>
+      <c r="AB7" s="151"/>
+      <c r="AC7" s="151"/>
+      <c r="AD7" s="151"/>
+      <c r="AE7" s="151"/>
+      <c r="AF7" s="151"/>
+      <c r="AG7" s="151"/>
+      <c r="AH7" s="152"/>
       <c r="AJ7" s="10" t="s">
         <v>373</v>
       </c>
@@ -10740,25 +10740,25 @@
       <c r="U8" s="95">
         <v>1</v>
       </c>
-      <c r="V8" s="116" t="s">
+      <c r="V8" s="110" t="s">
         <v>329</v>
       </c>
-      <c r="W8" s="117"/>
-      <c r="X8" s="117"/>
-      <c r="Y8" s="117"/>
+      <c r="W8" s="111"/>
+      <c r="X8" s="111"/>
+      <c r="Y8" s="111"/>
       <c r="Z8" s="18" t="s">
         <v>436</v>
       </c>
-      <c r="AA8" s="141" t="s">
+      <c r="AA8" s="151" t="s">
         <v>141</v>
       </c>
-      <c r="AB8" s="141"/>
-      <c r="AC8" s="141"/>
-      <c r="AD8" s="141"/>
-      <c r="AE8" s="141"/>
-      <c r="AF8" s="141"/>
-      <c r="AG8" s="141"/>
-      <c r="AH8" s="142"/>
+      <c r="AB8" s="151"/>
+      <c r="AC8" s="151"/>
+      <c r="AD8" s="151"/>
+      <c r="AE8" s="151"/>
+      <c r="AF8" s="151"/>
+      <c r="AG8" s="151"/>
+      <c r="AH8" s="152"/>
       <c r="AJ8" s="10" t="s">
         <v>437</v>
       </c>
@@ -10824,29 +10824,29 @@
       <c r="U9" s="86">
         <v>0</v>
       </c>
-      <c r="V9" s="116" t="s">
+      <c r="V9" s="110" t="s">
+        <v>498</v>
+      </c>
+      <c r="W9" s="111"/>
+      <c r="X9" s="111"/>
+      <c r="Y9" s="111"/>
+      <c r="Z9" s="85" t="s">
+        <v>497</v>
+      </c>
+      <c r="AA9" s="110" t="s">
+        <v>500</v>
+      </c>
+      <c r="AB9" s="111"/>
+      <c r="AC9" s="111"/>
+      <c r="AD9" s="111"/>
+      <c r="AE9" s="110" t="s">
+        <v>501</v>
+      </c>
+      <c r="AF9" s="111"/>
+      <c r="AG9" s="111"/>
+      <c r="AH9" s="111"/>
+      <c r="AJ9" s="10" t="s">
         <v>499</v>
-      </c>
-      <c r="W9" s="117"/>
-      <c r="X9" s="117"/>
-      <c r="Y9" s="117"/>
-      <c r="Z9" s="85" t="s">
-        <v>498</v>
-      </c>
-      <c r="AA9" s="116" t="s">
-        <v>501</v>
-      </c>
-      <c r="AB9" s="117"/>
-      <c r="AC9" s="117"/>
-      <c r="AD9" s="117"/>
-      <c r="AE9" s="116" t="s">
-        <v>502</v>
-      </c>
-      <c r="AF9" s="117"/>
-      <c r="AG9" s="117"/>
-      <c r="AH9" s="117"/>
-      <c r="AJ9" s="10" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
@@ -10877,38 +10877,38 @@
       <c r="J10" s="95">
         <v>1</v>
       </c>
-      <c r="K10" s="117" t="s">
+      <c r="K10" s="111" t="s">
         <v>328</v>
       </c>
-      <c r="L10" s="117"/>
-      <c r="M10" s="117"/>
-      <c r="N10" s="117"/>
-      <c r="O10" s="117"/>
-      <c r="P10" s="117" t="s">
+      <c r="L10" s="111"/>
+      <c r="M10" s="111"/>
+      <c r="N10" s="111"/>
+      <c r="O10" s="111"/>
+      <c r="P10" s="111" t="s">
         <v>329</v>
       </c>
-      <c r="Q10" s="117"/>
-      <c r="R10" s="117"/>
-      <c r="S10" s="117" t="s">
+      <c r="Q10" s="111"/>
+      <c r="R10" s="111"/>
+      <c r="S10" s="111" t="s">
         <v>330</v>
       </c>
-      <c r="T10" s="117"/>
-      <c r="U10" s="117"/>
-      <c r="V10" s="117"/>
-      <c r="W10" s="117"/>
-      <c r="X10" s="117"/>
-      <c r="Y10" s="117"/>
-      <c r="Z10" s="117"/>
-      <c r="AA10" s="117" t="s">
+      <c r="T10" s="111"/>
+      <c r="U10" s="111"/>
+      <c r="V10" s="111"/>
+      <c r="W10" s="111"/>
+      <c r="X10" s="111"/>
+      <c r="Y10" s="111"/>
+      <c r="Z10" s="111"/>
+      <c r="AA10" s="111" t="s">
         <v>81</v>
       </c>
-      <c r="AB10" s="117"/>
-      <c r="AC10" s="117"/>
-      <c r="AD10" s="117"/>
-      <c r="AE10" s="117"/>
-      <c r="AF10" s="117"/>
-      <c r="AG10" s="117"/>
-      <c r="AH10" s="117"/>
+      <c r="AB10" s="111"/>
+      <c r="AC10" s="111"/>
+      <c r="AD10" s="111"/>
+      <c r="AE10" s="111"/>
+      <c r="AF10" s="111"/>
+      <c r="AG10" s="111"/>
+      <c r="AH10" s="111"/>
       <c r="AJ10" s="10" t="s">
         <v>356</v>
       </c>
@@ -10941,34 +10941,34 @@
       <c r="J11" s="6">
         <v>0</v>
       </c>
-      <c r="K11" s="109" t="s">
+      <c r="K11" s="129" t="s">
         <v>143</v>
       </c>
-      <c r="L11" s="111"/>
-      <c r="M11" s="104" t="s">
+      <c r="L11" s="131"/>
+      <c r="M11" s="101" t="s">
         <v>376</v>
       </c>
-      <c r="N11" s="105"/>
-      <c r="O11" s="105"/>
-      <c r="P11" s="105"/>
-      <c r="Q11" s="105"/>
-      <c r="R11" s="105"/>
-      <c r="S11" s="105"/>
-      <c r="T11" s="105"/>
-      <c r="U11" s="105"/>
-      <c r="V11" s="105"/>
-      <c r="W11" s="105"/>
-      <c r="X11" s="105"/>
-      <c r="Y11" s="105"/>
-      <c r="Z11" s="105"/>
-      <c r="AA11" s="105"/>
-      <c r="AB11" s="105"/>
-      <c r="AC11" s="105"/>
-      <c r="AD11" s="105"/>
-      <c r="AE11" s="105"/>
-      <c r="AF11" s="105"/>
-      <c r="AG11" s="105"/>
-      <c r="AH11" s="106"/>
+      <c r="N11" s="102"/>
+      <c r="O11" s="102"/>
+      <c r="P11" s="102"/>
+      <c r="Q11" s="102"/>
+      <c r="R11" s="102"/>
+      <c r="S11" s="102"/>
+      <c r="T11" s="102"/>
+      <c r="U11" s="102"/>
+      <c r="V11" s="102"/>
+      <c r="W11" s="102"/>
+      <c r="X11" s="102"/>
+      <c r="Y11" s="102"/>
+      <c r="Z11" s="102"/>
+      <c r="AA11" s="102"/>
+      <c r="AB11" s="102"/>
+      <c r="AC11" s="102"/>
+      <c r="AD11" s="102"/>
+      <c r="AE11" s="102"/>
+      <c r="AF11" s="102"/>
+      <c r="AG11" s="102"/>
+      <c r="AH11" s="103"/>
       <c r="AJ11" s="10" t="s">
         <v>355</v>
       </c>
@@ -10998,35 +10998,35 @@
       <c r="I12" s="42">
         <v>0</v>
       </c>
-      <c r="J12" s="104" t="s">
+      <c r="J12" s="101" t="s">
         <v>378</v>
       </c>
-      <c r="K12" s="105"/>
-      <c r="L12" s="106"/>
-      <c r="M12" s="104" t="s">
+      <c r="K12" s="102"/>
+      <c r="L12" s="103"/>
+      <c r="M12" s="101" t="s">
         <v>376</v>
       </c>
-      <c r="N12" s="105"/>
-      <c r="O12" s="105"/>
-      <c r="P12" s="105"/>
-      <c r="Q12" s="105"/>
-      <c r="R12" s="105"/>
-      <c r="S12" s="105"/>
-      <c r="T12" s="105"/>
-      <c r="U12" s="105"/>
-      <c r="V12" s="105"/>
-      <c r="W12" s="105"/>
-      <c r="X12" s="105"/>
-      <c r="Y12" s="105"/>
-      <c r="Z12" s="105"/>
-      <c r="AA12" s="105"/>
-      <c r="AB12" s="105"/>
-      <c r="AC12" s="105"/>
-      <c r="AD12" s="105"/>
-      <c r="AE12" s="105"/>
-      <c r="AF12" s="105"/>
-      <c r="AG12" s="105"/>
-      <c r="AH12" s="106"/>
+      <c r="N12" s="102"/>
+      <c r="O12" s="102"/>
+      <c r="P12" s="102"/>
+      <c r="Q12" s="102"/>
+      <c r="R12" s="102"/>
+      <c r="S12" s="102"/>
+      <c r="T12" s="102"/>
+      <c r="U12" s="102"/>
+      <c r="V12" s="102"/>
+      <c r="W12" s="102"/>
+      <c r="X12" s="102"/>
+      <c r="Y12" s="102"/>
+      <c r="Z12" s="102"/>
+      <c r="AA12" s="102"/>
+      <c r="AB12" s="102"/>
+      <c r="AC12" s="102"/>
+      <c r="AD12" s="102"/>
+      <c r="AE12" s="102"/>
+      <c r="AF12" s="102"/>
+      <c r="AG12" s="102"/>
+      <c r="AH12" s="103"/>
       <c r="AJ12" s="10" t="s">
         <v>379</v>
       </c>
@@ -11074,37 +11074,37 @@
       <c r="C14" s="74">
         <v>1</v>
       </c>
-      <c r="D14" s="118"/>
-      <c r="E14" s="118"/>
-      <c r="F14" s="118"/>
-      <c r="G14" s="118"/>
-      <c r="H14" s="118"/>
-      <c r="I14" s="118"/>
-      <c r="J14" s="118"/>
-      <c r="K14" s="118"/>
-      <c r="L14" s="118"/>
-      <c r="M14" s="118"/>
-      <c r="N14" s="118"/>
-      <c r="O14" s="118"/>
-      <c r="P14" s="118"/>
-      <c r="Q14" s="118"/>
-      <c r="R14" s="118"/>
-      <c r="S14" s="118"/>
-      <c r="T14" s="118"/>
-      <c r="U14" s="118"/>
-      <c r="V14" s="118"/>
-      <c r="W14" s="118"/>
-      <c r="X14" s="118"/>
-      <c r="Y14" s="118"/>
-      <c r="Z14" s="118"/>
-      <c r="AA14" s="118"/>
-      <c r="AB14" s="118"/>
-      <c r="AC14" s="118"/>
-      <c r="AD14" s="118"/>
-      <c r="AE14" s="118"/>
-      <c r="AF14" s="118"/>
-      <c r="AG14" s="118"/>
-      <c r="AH14" s="118"/>
+      <c r="D14" s="124"/>
+      <c r="E14" s="124"/>
+      <c r="F14" s="124"/>
+      <c r="G14" s="124"/>
+      <c r="H14" s="124"/>
+      <c r="I14" s="124"/>
+      <c r="J14" s="124"/>
+      <c r="K14" s="124"/>
+      <c r="L14" s="124"/>
+      <c r="M14" s="124"/>
+      <c r="N14" s="124"/>
+      <c r="O14" s="124"/>
+      <c r="P14" s="124"/>
+      <c r="Q14" s="124"/>
+      <c r="R14" s="124"/>
+      <c r="S14" s="124"/>
+      <c r="T14" s="124"/>
+      <c r="U14" s="124"/>
+      <c r="V14" s="124"/>
+      <c r="W14" s="124"/>
+      <c r="X14" s="124"/>
+      <c r="Y14" s="124"/>
+      <c r="Z14" s="124"/>
+      <c r="AA14" s="124"/>
+      <c r="AB14" s="124"/>
+      <c r="AC14" s="124"/>
+      <c r="AD14" s="124"/>
+      <c r="AE14" s="124"/>
+      <c r="AF14" s="124"/>
+      <c r="AG14" s="124"/>
+      <c r="AH14" s="124"/>
       <c r="AJ14" s="10" t="s">
         <v>364</v>
       </c>
@@ -12179,46 +12179,46 @@
     </row>
     <row r="39" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A39" s="89"/>
-      <c r="C39" s="137" t="s">
+      <c r="C39" s="140" t="s">
+        <v>494</v>
+      </c>
+      <c r="D39" s="141"/>
+      <c r="E39" s="141"/>
+      <c r="F39" s="141"/>
+      <c r="G39" s="141"/>
+      <c r="H39" s="141"/>
+      <c r="I39" s="141"/>
+      <c r="J39" s="141"/>
+      <c r="K39" s="141"/>
+      <c r="L39" s="141"/>
+      <c r="M39" s="141"/>
+      <c r="N39" s="141"/>
+      <c r="O39" s="141"/>
+      <c r="P39" s="141"/>
+      <c r="Q39" s="141"/>
+      <c r="R39" s="142"/>
+      <c r="S39" s="140" t="s">
+        <v>496</v>
+      </c>
+      <c r="T39" s="141"/>
+      <c r="U39" s="141"/>
+      <c r="V39" s="141"/>
+      <c r="W39" s="141"/>
+      <c r="X39" s="141"/>
+      <c r="Y39" s="141"/>
+      <c r="Z39" s="142"/>
+      <c r="AA39" s="140" t="s">
         <v>495</v>
       </c>
-      <c r="D39" s="138"/>
-      <c r="E39" s="138"/>
-      <c r="F39" s="138"/>
-      <c r="G39" s="138"/>
-      <c r="H39" s="138"/>
-      <c r="I39" s="138"/>
-      <c r="J39" s="138"/>
-      <c r="K39" s="138"/>
-      <c r="L39" s="138"/>
-      <c r="M39" s="138"/>
-      <c r="N39" s="138"/>
-      <c r="O39" s="138"/>
-      <c r="P39" s="138"/>
-      <c r="Q39" s="138"/>
-      <c r="R39" s="139"/>
-      <c r="S39" s="137" t="s">
-        <v>497</v>
-      </c>
-      <c r="T39" s="138"/>
-      <c r="U39" s="138"/>
-      <c r="V39" s="138"/>
-      <c r="W39" s="138"/>
-      <c r="X39" s="138"/>
-      <c r="Y39" s="138"/>
-      <c r="Z39" s="139"/>
-      <c r="AA39" s="137" t="s">
-        <v>496</v>
-      </c>
-      <c r="AB39" s="138"/>
-      <c r="AC39" s="138"/>
-      <c r="AD39" s="138"/>
-      <c r="AE39" s="138"/>
-      <c r="AF39" s="138"/>
-      <c r="AG39" s="138"/>
-      <c r="AH39" s="139"/>
+      <c r="AB39" s="141"/>
+      <c r="AC39" s="141"/>
+      <c r="AD39" s="141"/>
+      <c r="AE39" s="141"/>
+      <c r="AF39" s="141"/>
+      <c r="AG39" s="141"/>
+      <c r="AH39" s="142"/>
       <c r="AJ39" t="s">
-        <v>494</v>
+        <v>506</v>
       </c>
     </row>
     <row r="41" spans="1:36" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -12263,170 +12263,170 @@
       <c r="A42" s="23" t="s">
         <v>424</v>
       </c>
-      <c r="C42" s="146">
+      <c r="C42" s="143">
         <v>8192</v>
       </c>
-      <c r="D42" s="147"/>
-      <c r="E42" s="147"/>
-      <c r="F42" s="147"/>
-      <c r="G42" s="147"/>
-      <c r="H42" s="147"/>
-      <c r="I42" s="147"/>
-      <c r="J42" s="147"/>
-      <c r="K42" s="147"/>
-      <c r="L42" s="147"/>
-      <c r="M42" s="147"/>
-      <c r="N42" s="147"/>
-      <c r="O42" s="147"/>
-      <c r="P42" s="147"/>
-      <c r="Q42" s="147"/>
-      <c r="R42" s="147"/>
-      <c r="S42" s="147"/>
-      <c r="T42" s="147"/>
-      <c r="U42" s="147"/>
-      <c r="V42" s="147"/>
-      <c r="W42" s="147"/>
-      <c r="X42" s="147"/>
-      <c r="Y42" s="147"/>
-      <c r="Z42" s="147"/>
-      <c r="AA42" s="147"/>
-      <c r="AB42" s="147"/>
-      <c r="AC42" s="147"/>
-      <c r="AD42" s="147"/>
-      <c r="AE42" s="147"/>
-      <c r="AF42" s="147"/>
-      <c r="AG42" s="147"/>
-      <c r="AH42" s="148"/>
+      <c r="D42" s="144"/>
+      <c r="E42" s="144"/>
+      <c r="F42" s="144"/>
+      <c r="G42" s="144"/>
+      <c r="H42" s="144"/>
+      <c r="I42" s="144"/>
+      <c r="J42" s="144"/>
+      <c r="K42" s="144"/>
+      <c r="L42" s="144"/>
+      <c r="M42" s="144"/>
+      <c r="N42" s="144"/>
+      <c r="O42" s="144"/>
+      <c r="P42" s="144"/>
+      <c r="Q42" s="144"/>
+      <c r="R42" s="144"/>
+      <c r="S42" s="144"/>
+      <c r="T42" s="144"/>
+      <c r="U42" s="144"/>
+      <c r="V42" s="144"/>
+      <c r="W42" s="144"/>
+      <c r="X42" s="144"/>
+      <c r="Y42" s="144"/>
+      <c r="Z42" s="144"/>
+      <c r="AA42" s="144"/>
+      <c r="AB42" s="144"/>
+      <c r="AC42" s="144"/>
+      <c r="AD42" s="144"/>
+      <c r="AE42" s="144"/>
+      <c r="AF42" s="144"/>
+      <c r="AG42" s="144"/>
+      <c r="AH42" s="145"/>
     </row>
     <row r="44" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C44" s="150" t="s">
+      <c r="C44" s="147" t="s">
         <v>439</v>
       </c>
-      <c r="D44" s="151"/>
-      <c r="E44" s="151"/>
-      <c r="F44" s="151"/>
-      <c r="G44" s="151"/>
-      <c r="H44" s="151"/>
-      <c r="I44" s="151"/>
-      <c r="J44" s="151"/>
-      <c r="K44" s="151" t="s">
+      <c r="D44" s="148"/>
+      <c r="E44" s="148"/>
+      <c r="F44" s="148"/>
+      <c r="G44" s="148"/>
+      <c r="H44" s="148"/>
+      <c r="I44" s="148"/>
+      <c r="J44" s="148"/>
+      <c r="K44" s="148" t="s">
         <v>440</v>
       </c>
-      <c r="L44" s="151"/>
-      <c r="M44" s="151"/>
-      <c r="N44" s="151"/>
-      <c r="O44" s="151"/>
-      <c r="P44" s="151"/>
-      <c r="Q44" s="151"/>
-      <c r="R44" s="151"/>
-      <c r="S44" s="151" t="s">
+      <c r="L44" s="148"/>
+      <c r="M44" s="148"/>
+      <c r="N44" s="148"/>
+      <c r="O44" s="148"/>
+      <c r="P44" s="148"/>
+      <c r="Q44" s="148"/>
+      <c r="R44" s="148"/>
+      <c r="S44" s="148" t="s">
         <v>441</v>
       </c>
-      <c r="T44" s="151"/>
-      <c r="U44" s="151"/>
-      <c r="V44" s="151"/>
-      <c r="W44" s="151"/>
-      <c r="X44" s="151"/>
-      <c r="Y44" s="151"/>
-      <c r="Z44" s="151"/>
-      <c r="AA44" s="152" t="s">
+      <c r="T44" s="148"/>
+      <c r="U44" s="148"/>
+      <c r="V44" s="148"/>
+      <c r="W44" s="148"/>
+      <c r="X44" s="148"/>
+      <c r="Y44" s="148"/>
+      <c r="Z44" s="148"/>
+      <c r="AA44" s="149" t="s">
         <v>442</v>
       </c>
-      <c r="AB44" s="152"/>
-      <c r="AC44" s="152"/>
-      <c r="AD44" s="152"/>
-      <c r="AE44" s="152"/>
-      <c r="AF44" s="152"/>
-      <c r="AG44" s="152"/>
-      <c r="AH44" s="152"/>
+      <c r="AB44" s="149"/>
+      <c r="AC44" s="149"/>
+      <c r="AD44" s="149"/>
+      <c r="AE44" s="149"/>
+      <c r="AF44" s="149"/>
+      <c r="AG44" s="149"/>
+      <c r="AH44" s="149"/>
     </row>
     <row r="45" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="24" t="s">
         <v>425</v>
       </c>
       <c r="B45" s="3"/>
-      <c r="C45" s="149" t="s">
+      <c r="C45" s="146" t="s">
         <v>426</v>
       </c>
-      <c r="D45" s="149"/>
-      <c r="E45" s="149"/>
-      <c r="F45" s="149"/>
-      <c r="G45" s="149"/>
-      <c r="H45" s="149"/>
-      <c r="I45" s="149"/>
-      <c r="J45" s="149"/>
-      <c r="K45" s="149" t="s">
+      <c r="D45" s="146"/>
+      <c r="E45" s="146"/>
+      <c r="F45" s="146"/>
+      <c r="G45" s="146"/>
+      <c r="H45" s="146"/>
+      <c r="I45" s="146"/>
+      <c r="J45" s="146"/>
+      <c r="K45" s="146" t="s">
         <v>427</v>
       </c>
-      <c r="L45" s="149"/>
-      <c r="M45" s="149"/>
-      <c r="N45" s="149"/>
-      <c r="O45" s="149"/>
-      <c r="P45" s="149"/>
-      <c r="Q45" s="149"/>
-      <c r="R45" s="149"/>
-      <c r="S45" s="149" t="s">
+      <c r="L45" s="146"/>
+      <c r="M45" s="146"/>
+      <c r="N45" s="146"/>
+      <c r="O45" s="146"/>
+      <c r="P45" s="146"/>
+      <c r="Q45" s="146"/>
+      <c r="R45" s="146"/>
+      <c r="S45" s="146" t="s">
         <v>428</v>
       </c>
-      <c r="T45" s="149"/>
-      <c r="U45" s="149"/>
-      <c r="V45" s="149"/>
-      <c r="W45" s="149"/>
-      <c r="X45" s="149"/>
-      <c r="Y45" s="149"/>
-      <c r="Z45" s="149"/>
-      <c r="AA45" s="149" t="s">
+      <c r="T45" s="146"/>
+      <c r="U45" s="146"/>
+      <c r="V45" s="146"/>
+      <c r="W45" s="146"/>
+      <c r="X45" s="146"/>
+      <c r="Y45" s="146"/>
+      <c r="Z45" s="146"/>
+      <c r="AA45" s="146" t="s">
         <v>429</v>
       </c>
-      <c r="AB45" s="149"/>
-      <c r="AC45" s="149"/>
-      <c r="AD45" s="149"/>
-      <c r="AE45" s="149"/>
-      <c r="AF45" s="149"/>
-      <c r="AG45" s="149"/>
-      <c r="AH45" s="149"/>
+      <c r="AB45" s="146"/>
+      <c r="AC45" s="146"/>
+      <c r="AD45" s="146"/>
+      <c r="AE45" s="146"/>
+      <c r="AF45" s="146"/>
+      <c r="AG45" s="146"/>
+      <c r="AH45" s="146"/>
     </row>
     <row r="46" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="C46" s="137" t="s">
+      <c r="C46" s="140" t="s">
         <v>443</v>
       </c>
-      <c r="D46" s="138"/>
-      <c r="E46" s="138"/>
-      <c r="F46" s="138"/>
-      <c r="G46" s="138"/>
-      <c r="H46" s="138"/>
-      <c r="I46" s="138"/>
-      <c r="J46" s="139"/>
-      <c r="K46" s="137" t="s">
+      <c r="D46" s="141"/>
+      <c r="E46" s="141"/>
+      <c r="F46" s="141"/>
+      <c r="G46" s="141"/>
+      <c r="H46" s="141"/>
+      <c r="I46" s="141"/>
+      <c r="J46" s="142"/>
+      <c r="K46" s="140" t="s">
         <v>430</v>
       </c>
-      <c r="L46" s="138"/>
-      <c r="M46" s="138"/>
-      <c r="N46" s="138"/>
-      <c r="O46" s="138"/>
-      <c r="P46" s="138"/>
-      <c r="Q46" s="138"/>
-      <c r="R46" s="139"/>
-      <c r="S46" s="137" t="s">
+      <c r="L46" s="141"/>
+      <c r="M46" s="141"/>
+      <c r="N46" s="141"/>
+      <c r="O46" s="141"/>
+      <c r="P46" s="141"/>
+      <c r="Q46" s="141"/>
+      <c r="R46" s="142"/>
+      <c r="S46" s="140" t="s">
         <v>431</v>
       </c>
-      <c r="T46" s="138"/>
-      <c r="U46" s="138"/>
-      <c r="V46" s="138"/>
-      <c r="W46" s="138"/>
-      <c r="X46" s="138"/>
-      <c r="Y46" s="138"/>
-      <c r="Z46" s="138"/>
-      <c r="AA46" s="138" t="s">
+      <c r="T46" s="141"/>
+      <c r="U46" s="141"/>
+      <c r="V46" s="141"/>
+      <c r="W46" s="141"/>
+      <c r="X46" s="141"/>
+      <c r="Y46" s="141"/>
+      <c r="Z46" s="141"/>
+      <c r="AA46" s="141" t="s">
         <v>431</v>
       </c>
-      <c r="AB46" s="138"/>
-      <c r="AC46" s="138"/>
-      <c r="AD46" s="138"/>
-      <c r="AE46" s="138"/>
-      <c r="AF46" s="138"/>
-      <c r="AG46" s="138"/>
-      <c r="AH46" s="139"/>
+      <c r="AB46" s="141"/>
+      <c r="AC46" s="141"/>
+      <c r="AD46" s="141"/>
+      <c r="AE46" s="141"/>
+      <c r="AF46" s="141"/>
+      <c r="AG46" s="141"/>
+      <c r="AH46" s="142"/>
     </row>
     <row r="48" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="24" t="s">
@@ -12443,19 +12443,13 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="C46:J46"/>
-    <mergeCell ref="K46:R46"/>
-    <mergeCell ref="S46:Z46"/>
-    <mergeCell ref="AA46:AH46"/>
-    <mergeCell ref="C42:AH42"/>
-    <mergeCell ref="C45:J45"/>
-    <mergeCell ref="K45:R45"/>
-    <mergeCell ref="S45:Z45"/>
-    <mergeCell ref="AA45:AH45"/>
-    <mergeCell ref="C44:J44"/>
-    <mergeCell ref="K44:R44"/>
-    <mergeCell ref="S44:Z44"/>
-    <mergeCell ref="AA44:AH44"/>
+    <mergeCell ref="C39:R39"/>
+    <mergeCell ref="AA39:AH39"/>
+    <mergeCell ref="S39:Z39"/>
+    <mergeCell ref="V8:Y8"/>
+    <mergeCell ref="V9:Y9"/>
+    <mergeCell ref="AA9:AD9"/>
+    <mergeCell ref="AE9:AH9"/>
     <mergeCell ref="AA5:AH5"/>
     <mergeCell ref="AA10:AH10"/>
     <mergeCell ref="P10:R10"/>
@@ -12470,13 +12464,19 @@
     <mergeCell ref="AA8:AH8"/>
     <mergeCell ref="AA6:AD6"/>
     <mergeCell ref="AE6:AH6"/>
-    <mergeCell ref="C39:R39"/>
-    <mergeCell ref="AA39:AH39"/>
-    <mergeCell ref="S39:Z39"/>
-    <mergeCell ref="V8:Y8"/>
-    <mergeCell ref="V9:Y9"/>
-    <mergeCell ref="AA9:AD9"/>
-    <mergeCell ref="AE9:AH9"/>
+    <mergeCell ref="C46:J46"/>
+    <mergeCell ref="K46:R46"/>
+    <mergeCell ref="S46:Z46"/>
+    <mergeCell ref="AA46:AH46"/>
+    <mergeCell ref="C42:AH42"/>
+    <mergeCell ref="C45:J45"/>
+    <mergeCell ref="K45:R45"/>
+    <mergeCell ref="S45:Z45"/>
+    <mergeCell ref="AA45:AH45"/>
+    <mergeCell ref="C44:J44"/>
+    <mergeCell ref="K44:R44"/>
+    <mergeCell ref="S44:Z44"/>
+    <mergeCell ref="AA44:AH44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -12500,20 +12500,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="99" t="s">
         <v>261</v>
       </c>
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
-      <c r="J1" s="123"/>
-      <c r="K1" s="123"/>
-      <c r="L1" s="123"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
+      <c r="L1" s="99"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13035,12 +13035,12 @@
       <c r="N6" s="37">
         <v>1</v>
       </c>
-      <c r="O6" s="118" t="s">
+      <c r="O6" s="124" t="s">
         <v>282</v>
       </c>
-      <c r="P6" s="118"/>
-      <c r="Q6" s="118"/>
-      <c r="R6" s="118"/>
+      <c r="P6" s="124"/>
+      <c r="Q6" s="124"/>
+      <c r="R6" s="124"/>
       <c r="T6" s="10" t="s">
         <v>413</v>
       </c>
@@ -13073,16 +13073,16 @@
       <c r="J7" s="37">
         <v>1</v>
       </c>
-      <c r="K7" s="118" t="s">
+      <c r="K7" s="124" t="s">
         <v>129</v>
       </c>
-      <c r="L7" s="118"/>
-      <c r="M7" s="118"/>
-      <c r="N7" s="118"/>
-      <c r="O7" s="118"/>
-      <c r="P7" s="118"/>
-      <c r="Q7" s="118"/>
-      <c r="R7" s="118"/>
+      <c r="L7" s="124"/>
+      <c r="M7" s="124"/>
+      <c r="N7" s="124"/>
+      <c r="O7" s="124"/>
+      <c r="P7" s="124"/>
+      <c r="Q7" s="124"/>
+      <c r="R7" s="124"/>
       <c r="T7" s="10"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -13113,16 +13113,16 @@
       <c r="J8" s="37" t="s">
         <v>130</v>
       </c>
-      <c r="K8" s="118" t="s">
+      <c r="K8" s="124" t="s">
         <v>129</v>
       </c>
-      <c r="L8" s="118"/>
-      <c r="M8" s="118"/>
-      <c r="N8" s="118"/>
-      <c r="O8" s="118"/>
-      <c r="P8" s="118"/>
-      <c r="Q8" s="118"/>
-      <c r="R8" s="118"/>
+      <c r="L8" s="124"/>
+      <c r="M8" s="124"/>
+      <c r="N8" s="124"/>
+      <c r="O8" s="124"/>
+      <c r="P8" s="124"/>
+      <c r="Q8" s="124"/>
+      <c r="R8" s="124"/>
       <c r="T8" s="10"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -13153,16 +13153,16 @@
       <c r="J9" s="37" t="s">
         <v>130</v>
       </c>
-      <c r="K9" s="118" t="s">
+      <c r="K9" s="124" t="s">
         <v>129</v>
       </c>
-      <c r="L9" s="118"/>
-      <c r="M9" s="118"/>
-      <c r="N9" s="118"/>
-      <c r="O9" s="118"/>
-      <c r="P9" s="118"/>
-      <c r="Q9" s="118"/>
-      <c r="R9" s="118"/>
+      <c r="L9" s="124"/>
+      <c r="M9" s="124"/>
+      <c r="N9" s="124"/>
+      <c r="O9" s="124"/>
+      <c r="P9" s="124"/>
+      <c r="Q9" s="124"/>
+      <c r="R9" s="124"/>
       <c r="T9" s="10"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -13193,16 +13193,16 @@
       <c r="J10" s="37" t="s">
         <v>130</v>
       </c>
-      <c r="K10" s="118" t="s">
+      <c r="K10" s="124" t="s">
         <v>129</v>
       </c>
-      <c r="L10" s="118"/>
-      <c r="M10" s="118"/>
-      <c r="N10" s="118"/>
-      <c r="O10" s="118"/>
-      <c r="P10" s="118"/>
-      <c r="Q10" s="118"/>
-      <c r="R10" s="118"/>
+      <c r="L10" s="124"/>
+      <c r="M10" s="124"/>
+      <c r="N10" s="124"/>
+      <c r="O10" s="124"/>
+      <c r="P10" s="124"/>
+      <c r="Q10" s="124"/>
+      <c r="R10" s="124"/>
       <c r="T10" s="10"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -13233,16 +13233,16 @@
       <c r="J11" s="6">
         <v>0</v>
       </c>
-      <c r="K11" s="118" t="s">
+      <c r="K11" s="124" t="s">
         <v>280</v>
       </c>
-      <c r="L11" s="118"/>
-      <c r="M11" s="118"/>
-      <c r="N11" s="118"/>
-      <c r="O11" s="118"/>
-      <c r="P11" s="118"/>
-      <c r="Q11" s="118"/>
-      <c r="R11" s="118"/>
+      <c r="L11" s="124"/>
+      <c r="M11" s="124"/>
+      <c r="N11" s="124"/>
+      <c r="O11" s="124"/>
+      <c r="P11" s="124"/>
+      <c r="Q11" s="124"/>
+      <c r="R11" s="124"/>
       <c r="T11" s="10" t="s">
         <v>414</v>
       </c>
@@ -13317,16 +13317,16 @@
       <c r="J14" s="6">
         <v>0</v>
       </c>
-      <c r="K14" s="104" t="s">
+      <c r="K14" s="101" t="s">
         <v>412</v>
       </c>
-      <c r="L14" s="105"/>
-      <c r="M14" s="105"/>
-      <c r="N14" s="105"/>
-      <c r="O14" s="105"/>
-      <c r="P14" s="105"/>
-      <c r="Q14" s="105"/>
-      <c r="R14" s="106"/>
+      <c r="L14" s="102"/>
+      <c r="M14" s="102"/>
+      <c r="N14" s="102"/>
+      <c r="O14" s="102"/>
+      <c r="P14" s="102"/>
+      <c r="Q14" s="102"/>
+      <c r="R14" s="103"/>
       <c r="T14" s="10" t="s">
         <v>415</v>
       </c>
@@ -13905,10 +13905,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="99" t="s">
         <v>449</v>
       </c>
-      <c r="B1" s="123"/>
+      <c r="B1" s="99"/>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
ghetto NewToASM (not working yet)
Address is kept as virtual one, need to be resolved to the real address
</commit_message>
<xml_diff>
--- a/doc/RiscyInstSet32Bit.xlsx
+++ b/doc/RiscyInstSet32Bit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25410" windowHeight="12690" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25410" windowHeight="12690" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Summary - Terra" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="620">
   <si>
     <t>Description</t>
   </si>
@@ -1884,6 +1884,15 @@
   </si>
   <si>
     <t>-1 if the host is in fact virtual machine; 0 if not.</t>
+  </si>
+  <si>
+    <t>Zero to the zeroth power must be evaluated to 1.0</t>
+  </si>
+  <si>
+    <t>Zero to the zeroth power must be evaluated to 1</t>
+  </si>
+  <si>
+    <t>Rs should contain memory address, NOT an offset.</t>
   </si>
 </sst>
 </file>
@@ -2792,42 +2801,91 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="14" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="27" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="28" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="29" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="30" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2855,57 +2913,12 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="28" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="29" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="30" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="27" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2924,18 +2937,45 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2957,37 +2997,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="14" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Bad" xfId="9" builtinId="27"/>
@@ -3297,43 +3306,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="141" t="s">
         <v>223</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
-      <c r="D1" s="124"/>
-      <c r="E1" s="124"/>
-      <c r="F1" s="124"/>
-      <c r="G1" s="124"/>
-      <c r="H1" s="124"/>
-      <c r="I1" s="124"/>
-      <c r="J1" s="124"/>
-      <c r="K1" s="124"/>
-      <c r="L1" s="124"/>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="124"/>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="124"/>
-      <c r="V1" s="124"/>
-      <c r="W1" s="124"/>
-      <c r="X1" s="124"/>
-      <c r="Y1" s="124"/>
-      <c r="Z1" s="124"/>
-      <c r="AA1" s="124"/>
-      <c r="AB1" s="124"/>
-      <c r="AC1" s="124"/>
-      <c r="AD1" s="124"/>
-      <c r="AE1" s="124"/>
-      <c r="AF1" s="124"/>
-      <c r="AG1" s="124"/>
-      <c r="AH1" s="124"/>
-      <c r="AI1" s="125"/>
+      <c r="B1" s="141"/>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
+      <c r="H1" s="141"/>
+      <c r="I1" s="141"/>
+      <c r="J1" s="141"/>
+      <c r="K1" s="141"/>
+      <c r="L1" s="141"/>
+      <c r="M1" s="141"/>
+      <c r="N1" s="141"/>
+      <c r="O1" s="141"/>
+      <c r="P1" s="141"/>
+      <c r="Q1" s="141"/>
+      <c r="R1" s="141"/>
+      <c r="S1" s="141"/>
+      <c r="T1" s="141"/>
+      <c r="U1" s="141"/>
+      <c r="V1" s="141"/>
+      <c r="W1" s="141"/>
+      <c r="X1" s="141"/>
+      <c r="Y1" s="141"/>
+      <c r="Z1" s="141"/>
+      <c r="AA1" s="141"/>
+      <c r="AB1" s="141"/>
+      <c r="AC1" s="141"/>
+      <c r="AD1" s="141"/>
+      <c r="AE1" s="141"/>
+      <c r="AF1" s="141"/>
+      <c r="AG1" s="141"/>
+      <c r="AH1" s="141"/>
+      <c r="AI1" s="142"/>
     </row>
     <row r="2" spans="1:38" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
@@ -3625,11 +3634,11 @@
       <c r="B10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="129" t="s">
+      <c r="D10" s="146" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="129"/>
-      <c r="F10" s="129"/>
+      <c r="E10" s="146"/>
+      <c r="F10" s="146"/>
       <c r="G10" s="11">
         <v>0</v>
       </c>
@@ -3639,24 +3648,24 @@
       <c r="I10" s="11">
         <v>0</v>
       </c>
-      <c r="J10" s="136" t="s">
+      <c r="J10" s="132" t="s">
         <v>5</v>
       </c>
-      <c r="K10" s="136"/>
-      <c r="L10" s="136"/>
-      <c r="M10" s="137"/>
-      <c r="N10" s="130" t="s">
+      <c r="K10" s="132"/>
+      <c r="L10" s="132"/>
+      <c r="M10" s="133"/>
+      <c r="N10" s="111" t="s">
         <v>9</v>
       </c>
-      <c r="O10" s="131"/>
-      <c r="P10" s="131"/>
-      <c r="Q10" s="132"/>
-      <c r="R10" s="130" t="s">
+      <c r="O10" s="112"/>
+      <c r="P10" s="112"/>
+      <c r="Q10" s="113"/>
+      <c r="R10" s="111" t="s">
         <v>10</v>
       </c>
-      <c r="S10" s="131"/>
-      <c r="T10" s="131"/>
-      <c r="U10" s="132"/>
+      <c r="S10" s="112"/>
+      <c r="T10" s="112"/>
+      <c r="U10" s="113"/>
       <c r="V10" s="6">
         <v>0</v>
       </c>
@@ -3681,14 +3690,14 @@
       <c r="AC10" s="80">
         <v>0</v>
       </c>
-      <c r="AD10" s="130" t="s">
+      <c r="AD10" s="111" t="s">
         <v>244</v>
       </c>
-      <c r="AE10" s="131"/>
-      <c r="AF10" s="131"/>
-      <c r="AG10" s="131"/>
-      <c r="AH10" s="131"/>
-      <c r="AI10" s="132"/>
+      <c r="AE10" s="112"/>
+      <c r="AF10" s="112"/>
+      <c r="AG10" s="112"/>
+      <c r="AH10" s="112"/>
+      <c r="AI10" s="113"/>
       <c r="AK10" s="10" t="s">
         <v>138</v>
       </c>
@@ -3714,24 +3723,24 @@
       <c r="I11" s="26">
         <v>0</v>
       </c>
-      <c r="J11" s="112" t="s">
+      <c r="J11" s="119" t="s">
         <v>5</v>
       </c>
-      <c r="K11" s="113"/>
-      <c r="L11" s="113"/>
-      <c r="M11" s="114"/>
-      <c r="N11" s="119" t="s">
+      <c r="K11" s="120"/>
+      <c r="L11" s="120"/>
+      <c r="M11" s="121"/>
+      <c r="N11" s="129" t="s">
         <v>241</v>
       </c>
-      <c r="O11" s="120"/>
-      <c r="P11" s="120"/>
-      <c r="Q11" s="120"/>
-      <c r="R11" s="116" t="s">
+      <c r="O11" s="130"/>
+      <c r="P11" s="130"/>
+      <c r="Q11" s="130"/>
+      <c r="R11" s="122" t="s">
         <v>137</v>
       </c>
-      <c r="S11" s="116"/>
-      <c r="T11" s="116"/>
-      <c r="U11" s="117"/>
+      <c r="S11" s="122"/>
+      <c r="T11" s="122"/>
+      <c r="U11" s="123"/>
       <c r="V11" s="61">
         <v>0</v>
       </c>
@@ -3799,24 +3808,24 @@
       <c r="I12" s="42">
         <v>0</v>
       </c>
-      <c r="J12" s="112" t="s">
+      <c r="J12" s="119" t="s">
         <v>5</v>
       </c>
-      <c r="K12" s="113"/>
-      <c r="L12" s="113"/>
-      <c r="M12" s="114"/>
-      <c r="N12" s="119" t="s">
+      <c r="K12" s="120"/>
+      <c r="L12" s="120"/>
+      <c r="M12" s="121"/>
+      <c r="N12" s="129" t="s">
         <v>241</v>
       </c>
-      <c r="O12" s="120"/>
-      <c r="P12" s="120"/>
-      <c r="Q12" s="120"/>
-      <c r="R12" s="116" t="s">
+      <c r="O12" s="130"/>
+      <c r="P12" s="130"/>
+      <c r="Q12" s="130"/>
+      <c r="R12" s="122" t="s">
         <v>137</v>
       </c>
-      <c r="S12" s="116"/>
-      <c r="T12" s="116"/>
-      <c r="U12" s="117"/>
+      <c r="S12" s="122"/>
+      <c r="T12" s="122"/>
+      <c r="U12" s="123"/>
       <c r="V12" s="61">
         <v>0</v>
       </c>
@@ -3884,24 +3893,24 @@
       <c r="I13" s="12">
         <v>0</v>
       </c>
-      <c r="J13" s="112" t="s">
+      <c r="J13" s="119" t="s">
         <v>5</v>
       </c>
-      <c r="K13" s="113"/>
-      <c r="L13" s="113"/>
-      <c r="M13" s="114"/>
-      <c r="N13" s="119" t="s">
+      <c r="K13" s="120"/>
+      <c r="L13" s="120"/>
+      <c r="M13" s="121"/>
+      <c r="N13" s="129" t="s">
         <v>9</v>
       </c>
-      <c r="O13" s="120"/>
-      <c r="P13" s="120"/>
-      <c r="Q13" s="120"/>
-      <c r="R13" s="138" t="s">
+      <c r="O13" s="130"/>
+      <c r="P13" s="130"/>
+      <c r="Q13" s="130"/>
+      <c r="R13" s="131" t="s">
         <v>83</v>
       </c>
-      <c r="S13" s="138"/>
-      <c r="T13" s="138"/>
-      <c r="U13" s="138"/>
+      <c r="S13" s="131"/>
+      <c r="T13" s="131"/>
+      <c r="U13" s="131"/>
       <c r="V13" s="61">
         <v>0</v>
       </c>
@@ -3935,7 +3944,7 @@
       <c r="AF13" s="60">
         <v>0</v>
       </c>
-      <c r="AG13" s="109" t="s">
+      <c r="AG13" s="117" t="s">
         <v>146</v>
       </c>
       <c r="AH13" s="118"/>
@@ -3956,11 +3965,11 @@
       <c r="B14" s="96" t="s">
         <v>381</v>
       </c>
-      <c r="D14" s="109" t="s">
+      <c r="D14" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="110"/>
-      <c r="F14" s="111"/>
+      <c r="E14" s="127"/>
+      <c r="F14" s="128"/>
       <c r="G14" s="97">
         <v>0</v>
       </c>
@@ -3970,42 +3979,42 @@
       <c r="I14" s="97">
         <v>1</v>
       </c>
-      <c r="J14" s="112" t="s">
+      <c r="J14" s="119" t="s">
         <v>5</v>
       </c>
-      <c r="K14" s="113"/>
-      <c r="L14" s="113"/>
-      <c r="M14" s="114"/>
-      <c r="N14" s="115" t="s">
+      <c r="K14" s="120"/>
+      <c r="L14" s="120"/>
+      <c r="M14" s="121"/>
+      <c r="N14" s="137" t="s">
         <v>137</v>
       </c>
-      <c r="O14" s="116"/>
-      <c r="P14" s="116"/>
-      <c r="Q14" s="117"/>
+      <c r="O14" s="122"/>
+      <c r="P14" s="122"/>
+      <c r="Q14" s="123"/>
       <c r="R14" s="95">
         <v>0</v>
       </c>
       <c r="S14" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="T14" s="112" t="s">
+      <c r="T14" s="119" t="s">
         <v>134</v>
       </c>
-      <c r="U14" s="113"/>
-      <c r="V14" s="113"/>
-      <c r="W14" s="113"/>
-      <c r="X14" s="113"/>
-      <c r="Y14" s="113"/>
-      <c r="Z14" s="113"/>
-      <c r="AA14" s="113"/>
-      <c r="AB14" s="113"/>
-      <c r="AC14" s="113"/>
-      <c r="AD14" s="113"/>
-      <c r="AE14" s="113"/>
-      <c r="AF14" s="113"/>
-      <c r="AG14" s="113"/>
-      <c r="AH14" s="113"/>
-      <c r="AI14" s="114"/>
+      <c r="U14" s="120"/>
+      <c r="V14" s="120"/>
+      <c r="W14" s="120"/>
+      <c r="X14" s="120"/>
+      <c r="Y14" s="120"/>
+      <c r="Z14" s="120"/>
+      <c r="AA14" s="120"/>
+      <c r="AB14" s="120"/>
+      <c r="AC14" s="120"/>
+      <c r="AD14" s="120"/>
+      <c r="AE14" s="120"/>
+      <c r="AF14" s="120"/>
+      <c r="AG14" s="120"/>
+      <c r="AH14" s="120"/>
+      <c r="AI14" s="121"/>
       <c r="AK14" s="10" t="s">
         <v>378</v>
       </c>
@@ -4017,11 +4026,11 @@
       <c r="B15" s="96" t="s">
         <v>380</v>
       </c>
-      <c r="D15" s="109" t="s">
+      <c r="D15" s="117" t="s">
         <v>3</v>
       </c>
       <c r="E15" s="118"/>
-      <c r="F15" s="111"/>
+      <c r="F15" s="128"/>
       <c r="G15" s="97">
         <v>0</v>
       </c>
@@ -4031,42 +4040,42 @@
       <c r="I15" s="97">
         <v>1</v>
       </c>
-      <c r="J15" s="112" t="s">
+      <c r="J15" s="119" t="s">
         <v>5</v>
       </c>
-      <c r="K15" s="113"/>
-      <c r="L15" s="113"/>
-      <c r="M15" s="114"/>
-      <c r="N15" s="119" t="s">
+      <c r="K15" s="120"/>
+      <c r="L15" s="120"/>
+      <c r="M15" s="121"/>
+      <c r="N15" s="129" t="s">
         <v>83</v>
       </c>
-      <c r="O15" s="120"/>
-      <c r="P15" s="120"/>
-      <c r="Q15" s="120"/>
+      <c r="O15" s="130"/>
+      <c r="P15" s="130"/>
+      <c r="Q15" s="130"/>
       <c r="R15" s="68">
         <v>1</v>
       </c>
       <c r="S15" s="97">
         <v>0</v>
       </c>
-      <c r="T15" s="112" t="s">
+      <c r="T15" s="119" t="s">
         <v>379</v>
       </c>
-      <c r="U15" s="113"/>
-      <c r="V15" s="113"/>
-      <c r="W15" s="113"/>
-      <c r="X15" s="113"/>
-      <c r="Y15" s="113"/>
-      <c r="Z15" s="113"/>
-      <c r="AA15" s="113"/>
-      <c r="AB15" s="113"/>
-      <c r="AC15" s="113"/>
-      <c r="AD15" s="113"/>
-      <c r="AE15" s="113"/>
-      <c r="AF15" s="113"/>
-      <c r="AG15" s="113"/>
-      <c r="AH15" s="113"/>
-      <c r="AI15" s="114"/>
+      <c r="U15" s="120"/>
+      <c r="V15" s="120"/>
+      <c r="W15" s="120"/>
+      <c r="X15" s="120"/>
+      <c r="Y15" s="120"/>
+      <c r="Z15" s="120"/>
+      <c r="AA15" s="120"/>
+      <c r="AB15" s="120"/>
+      <c r="AC15" s="120"/>
+      <c r="AD15" s="120"/>
+      <c r="AE15" s="120"/>
+      <c r="AF15" s="120"/>
+      <c r="AG15" s="120"/>
+      <c r="AH15" s="120"/>
+      <c r="AI15" s="121"/>
       <c r="AK15" s="10"/>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
@@ -4076,11 +4085,11 @@
       <c r="B16" s="96" t="s">
         <v>136</v>
       </c>
-      <c r="D16" s="109" t="s">
+      <c r="D16" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="110"/>
-      <c r="F16" s="111"/>
+      <c r="E16" s="127"/>
+      <c r="F16" s="128"/>
       <c r="G16" s="97">
         <v>0</v>
       </c>
@@ -4090,36 +4099,36 @@
       <c r="I16" s="98" t="s">
         <v>82</v>
       </c>
-      <c r="J16" s="112" t="s">
+      <c r="J16" s="119" t="s">
         <v>5</v>
       </c>
-      <c r="K16" s="113"/>
-      <c r="L16" s="113"/>
-      <c r="M16" s="114"/>
-      <c r="N16" s="112" t="s">
+      <c r="K16" s="120"/>
+      <c r="L16" s="120"/>
+      <c r="M16" s="121"/>
+      <c r="N16" s="119" t="s">
         <v>4</v>
       </c>
-      <c r="O16" s="113"/>
-      <c r="P16" s="113"/>
-      <c r="Q16" s="113"/>
-      <c r="R16" s="113"/>
-      <c r="S16" s="113"/>
-      <c r="T16" s="113"/>
-      <c r="U16" s="113"/>
-      <c r="V16" s="113"/>
-      <c r="W16" s="113"/>
-      <c r="X16" s="113"/>
-      <c r="Y16" s="113"/>
-      <c r="Z16" s="113"/>
-      <c r="AA16" s="113"/>
-      <c r="AB16" s="113"/>
-      <c r="AC16" s="113"/>
-      <c r="AD16" s="113"/>
-      <c r="AE16" s="113"/>
-      <c r="AF16" s="113"/>
-      <c r="AG16" s="113"/>
-      <c r="AH16" s="113"/>
-      <c r="AI16" s="114"/>
+      <c r="O16" s="120"/>
+      <c r="P16" s="120"/>
+      <c r="Q16" s="120"/>
+      <c r="R16" s="120"/>
+      <c r="S16" s="120"/>
+      <c r="T16" s="120"/>
+      <c r="U16" s="120"/>
+      <c r="V16" s="120"/>
+      <c r="W16" s="120"/>
+      <c r="X16" s="120"/>
+      <c r="Y16" s="120"/>
+      <c r="Z16" s="120"/>
+      <c r="AA16" s="120"/>
+      <c r="AB16" s="120"/>
+      <c r="AC16" s="120"/>
+      <c r="AD16" s="120"/>
+      <c r="AE16" s="120"/>
+      <c r="AF16" s="120"/>
+      <c r="AG16" s="120"/>
+      <c r="AH16" s="120"/>
+      <c r="AI16" s="121"/>
       <c r="AK16" s="10" t="s">
         <v>150</v>
       </c>
@@ -4131,11 +4140,11 @@
       <c r="B17" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="109" t="s">
+      <c r="D17" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="110"/>
-      <c r="F17" s="111"/>
+      <c r="E17" s="127"/>
+      <c r="F17" s="128"/>
       <c r="G17" s="70">
         <v>0</v>
       </c>
@@ -4145,18 +4154,18 @@
       <c r="I17" s="71">
         <v>0</v>
       </c>
-      <c r="J17" s="112" t="s">
+      <c r="J17" s="119" t="s">
         <v>404</v>
       </c>
-      <c r="K17" s="113"/>
-      <c r="L17" s="113"/>
-      <c r="M17" s="114"/>
-      <c r="N17" s="116" t="s">
+      <c r="K17" s="120"/>
+      <c r="L17" s="120"/>
+      <c r="M17" s="121"/>
+      <c r="N17" s="122" t="s">
         <v>137</v>
       </c>
-      <c r="O17" s="116"/>
-      <c r="P17" s="116"/>
-      <c r="Q17" s="117"/>
+      <c r="O17" s="122"/>
+      <c r="P17" s="122"/>
+      <c r="Q17" s="123"/>
       <c r="R17" s="60">
         <v>0</v>
       </c>
@@ -4236,18 +4245,18 @@
       <c r="I18" s="12">
         <v>0</v>
       </c>
-      <c r="J18" s="112" t="s">
+      <c r="J18" s="119" t="s">
         <v>5</v>
       </c>
-      <c r="K18" s="113"/>
-      <c r="L18" s="113"/>
-      <c r="M18" s="114"/>
-      <c r="N18" s="119" t="s">
+      <c r="K18" s="120"/>
+      <c r="L18" s="120"/>
+      <c r="M18" s="121"/>
+      <c r="N18" s="129" t="s">
         <v>9</v>
       </c>
-      <c r="O18" s="120"/>
-      <c r="P18" s="120"/>
-      <c r="Q18" s="120"/>
+      <c r="O18" s="130"/>
+      <c r="P18" s="130"/>
+      <c r="Q18" s="130"/>
       <c r="R18" s="6">
         <v>0</v>
       </c>
@@ -4313,11 +4322,11 @@
       <c r="B19" s="64" t="s">
         <v>207</v>
       </c>
-      <c r="D19" s="109" t="s">
+      <c r="D19" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="110"/>
-      <c r="F19" s="111"/>
+      <c r="E19" s="127"/>
+      <c r="F19" s="128"/>
       <c r="G19" s="61">
         <v>1</v>
       </c>
@@ -4327,36 +4336,36 @@
       <c r="I19" s="61">
         <v>0</v>
       </c>
-      <c r="J19" s="139" t="s">
+      <c r="J19" s="134" t="s">
         <v>137</v>
       </c>
-      <c r="K19" s="140"/>
-      <c r="L19" s="140"/>
-      <c r="M19" s="141"/>
-      <c r="N19" s="112" t="s">
+      <c r="K19" s="135"/>
+      <c r="L19" s="135"/>
+      <c r="M19" s="136"/>
+      <c r="N19" s="119" t="s">
         <v>4</v>
       </c>
-      <c r="O19" s="113"/>
-      <c r="P19" s="113"/>
-      <c r="Q19" s="113"/>
-      <c r="R19" s="113"/>
-      <c r="S19" s="113"/>
-      <c r="T19" s="113"/>
-      <c r="U19" s="113"/>
-      <c r="V19" s="113"/>
-      <c r="W19" s="113"/>
-      <c r="X19" s="113"/>
-      <c r="Y19" s="113"/>
-      <c r="Z19" s="113"/>
-      <c r="AA19" s="113"/>
-      <c r="AB19" s="113"/>
-      <c r="AC19" s="113"/>
-      <c r="AD19" s="113"/>
-      <c r="AE19" s="113"/>
-      <c r="AF19" s="113"/>
-      <c r="AG19" s="113"/>
-      <c r="AH19" s="113"/>
-      <c r="AI19" s="114"/>
+      <c r="O19" s="120"/>
+      <c r="P19" s="120"/>
+      <c r="Q19" s="120"/>
+      <c r="R19" s="120"/>
+      <c r="S19" s="120"/>
+      <c r="T19" s="120"/>
+      <c r="U19" s="120"/>
+      <c r="V19" s="120"/>
+      <c r="W19" s="120"/>
+      <c r="X19" s="120"/>
+      <c r="Y19" s="120"/>
+      <c r="Z19" s="120"/>
+      <c r="AA19" s="120"/>
+      <c r="AB19" s="120"/>
+      <c r="AC19" s="120"/>
+      <c r="AD19" s="120"/>
+      <c r="AE19" s="120"/>
+      <c r="AF19" s="120"/>
+      <c r="AG19" s="120"/>
+      <c r="AH19" s="120"/>
+      <c r="AI19" s="121"/>
       <c r="AK19" s="10" t="s">
         <v>164</v>
       </c>
@@ -4368,11 +4377,11 @@
       <c r="B20" s="64" t="s">
         <v>312</v>
       </c>
-      <c r="D20" s="109" t="s">
+      <c r="D20" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="110"/>
-      <c r="F20" s="111"/>
+      <c r="E20" s="127"/>
+      <c r="F20" s="128"/>
       <c r="G20" s="61">
         <v>1</v>
       </c>
@@ -4382,36 +4391,36 @@
       <c r="I20" s="61">
         <v>1</v>
       </c>
-      <c r="J20" s="115" t="s">
+      <c r="J20" s="137" t="s">
         <v>137</v>
       </c>
-      <c r="K20" s="116"/>
-      <c r="L20" s="116"/>
-      <c r="M20" s="117"/>
-      <c r="N20" s="112" t="s">
+      <c r="K20" s="122"/>
+      <c r="L20" s="122"/>
+      <c r="M20" s="123"/>
+      <c r="N20" s="119" t="s">
         <v>4</v>
       </c>
-      <c r="O20" s="113"/>
-      <c r="P20" s="113"/>
-      <c r="Q20" s="113"/>
-      <c r="R20" s="113"/>
-      <c r="S20" s="113"/>
-      <c r="T20" s="113"/>
-      <c r="U20" s="113"/>
-      <c r="V20" s="113"/>
-      <c r="W20" s="113"/>
-      <c r="X20" s="113"/>
-      <c r="Y20" s="113"/>
-      <c r="Z20" s="113"/>
-      <c r="AA20" s="113"/>
-      <c r="AB20" s="113"/>
-      <c r="AC20" s="113"/>
-      <c r="AD20" s="113"/>
-      <c r="AE20" s="113"/>
-      <c r="AF20" s="113"/>
-      <c r="AG20" s="113"/>
-      <c r="AH20" s="113"/>
-      <c r="AI20" s="114"/>
+      <c r="O20" s="120"/>
+      <c r="P20" s="120"/>
+      <c r="Q20" s="120"/>
+      <c r="R20" s="120"/>
+      <c r="S20" s="120"/>
+      <c r="T20" s="120"/>
+      <c r="U20" s="120"/>
+      <c r="V20" s="120"/>
+      <c r="W20" s="120"/>
+      <c r="X20" s="120"/>
+      <c r="Y20" s="120"/>
+      <c r="Z20" s="120"/>
+      <c r="AA20" s="120"/>
+      <c r="AB20" s="120"/>
+      <c r="AC20" s="120"/>
+      <c r="AD20" s="120"/>
+      <c r="AE20" s="120"/>
+      <c r="AF20" s="120"/>
+      <c r="AG20" s="120"/>
+      <c r="AH20" s="120"/>
+      <c r="AI20" s="121"/>
       <c r="AK20" s="10"/>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
@@ -4421,11 +4430,11 @@
       <c r="B21" s="64" t="s">
         <v>185</v>
       </c>
-      <c r="D21" s="109" t="s">
+      <c r="D21" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="E21" s="110"/>
-      <c r="F21" s="111"/>
+      <c r="E21" s="127"/>
+      <c r="F21" s="128"/>
       <c r="G21" s="61">
         <v>1</v>
       </c>
@@ -4435,42 +4444,42 @@
       <c r="I21" s="61">
         <v>0</v>
       </c>
-      <c r="J21" s="142" t="s">
+      <c r="J21" s="124" t="s">
         <v>137</v>
       </c>
-      <c r="K21" s="143"/>
-      <c r="L21" s="143"/>
-      <c r="M21" s="144"/>
+      <c r="K21" s="125"/>
+      <c r="L21" s="125"/>
+      <c r="M21" s="126"/>
       <c r="N21" s="61">
         <v>0</v>
       </c>
       <c r="O21" s="61">
         <v>0</v>
       </c>
-      <c r="P21" s="126" t="s">
+      <c r="P21" s="143" t="s">
         <v>187</v>
       </c>
-      <c r="Q21" s="127"/>
-      <c r="R21" s="127"/>
-      <c r="S21" s="127"/>
-      <c r="T21" s="127"/>
-      <c r="U21" s="127"/>
-      <c r="V21" s="127"/>
-      <c r="W21" s="128"/>
-      <c r="X21" s="112" t="s">
+      <c r="Q21" s="144"/>
+      <c r="R21" s="144"/>
+      <c r="S21" s="144"/>
+      <c r="T21" s="144"/>
+      <c r="U21" s="144"/>
+      <c r="V21" s="144"/>
+      <c r="W21" s="145"/>
+      <c r="X21" s="119" t="s">
         <v>186</v>
       </c>
-      <c r="Y21" s="113"/>
-      <c r="Z21" s="113"/>
-      <c r="AA21" s="113"/>
-      <c r="AB21" s="113"/>
-      <c r="AC21" s="113"/>
-      <c r="AD21" s="113"/>
-      <c r="AE21" s="113"/>
-      <c r="AF21" s="113"/>
-      <c r="AG21" s="113"/>
-      <c r="AH21" s="113"/>
-      <c r="AI21" s="114"/>
+      <c r="Y21" s="120"/>
+      <c r="Z21" s="120"/>
+      <c r="AA21" s="120"/>
+      <c r="AB21" s="120"/>
+      <c r="AC21" s="120"/>
+      <c r="AD21" s="120"/>
+      <c r="AE21" s="120"/>
+      <c r="AF21" s="120"/>
+      <c r="AG21" s="120"/>
+      <c r="AH21" s="120"/>
+      <c r="AI21" s="121"/>
       <c r="AK21" s="10" t="s">
         <v>403</v>
       </c>
@@ -4482,11 +4491,11 @@
       <c r="B22" s="64" t="s">
         <v>191</v>
       </c>
-      <c r="D22" s="109" t="s">
+      <c r="D22" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="110"/>
-      <c r="F22" s="111"/>
+      <c r="E22" s="127"/>
+      <c r="F22" s="128"/>
       <c r="G22" s="61">
         <v>1</v>
       </c>
@@ -4496,12 +4505,12 @@
       <c r="I22" s="61">
         <v>0</v>
       </c>
-      <c r="J22" s="112" t="s">
+      <c r="J22" s="119" t="s">
         <v>5</v>
       </c>
-      <c r="K22" s="113"/>
-      <c r="L22" s="113"/>
-      <c r="M22" s="114"/>
+      <c r="K22" s="120"/>
+      <c r="L22" s="120"/>
+      <c r="M22" s="121"/>
       <c r="N22" s="61">
         <v>0</v>
       </c>
@@ -4544,16 +4553,16 @@
       <c r="AA22" s="52">
         <v>0</v>
       </c>
-      <c r="AB22" s="112" t="s">
+      <c r="AB22" s="119" t="s">
         <v>189</v>
       </c>
-      <c r="AC22" s="113"/>
-      <c r="AD22" s="113"/>
-      <c r="AE22" s="113"/>
-      <c r="AF22" s="113"/>
-      <c r="AG22" s="113"/>
-      <c r="AH22" s="113"/>
-      <c r="AI22" s="114"/>
+      <c r="AC22" s="120"/>
+      <c r="AD22" s="120"/>
+      <c r="AE22" s="120"/>
+      <c r="AF22" s="120"/>
+      <c r="AG22" s="120"/>
+      <c r="AH22" s="120"/>
+      <c r="AI22" s="121"/>
       <c r="AK22" s="10" t="s">
         <v>190</v>
       </c>
@@ -4565,11 +4574,11 @@
       <c r="B23" s="64" t="s">
         <v>80</v>
       </c>
-      <c r="D23" s="109" t="s">
+      <c r="D23" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="110"/>
-      <c r="F23" s="111"/>
+      <c r="E23" s="127"/>
+      <c r="F23" s="128"/>
       <c r="G23" s="60">
         <v>1</v>
       </c>
@@ -4579,12 +4588,12 @@
       <c r="I23" s="60">
         <v>0</v>
       </c>
-      <c r="J23" s="112" t="s">
+      <c r="J23" s="119" t="s">
         <v>5</v>
       </c>
-      <c r="K23" s="113"/>
-      <c r="L23" s="113"/>
-      <c r="M23" s="114"/>
+      <c r="K23" s="120"/>
+      <c r="L23" s="120"/>
+      <c r="M23" s="121"/>
       <c r="N23" s="61">
         <v>0</v>
       </c>
@@ -4627,16 +4636,16 @@
       <c r="AA23" s="75">
         <v>1</v>
       </c>
-      <c r="AB23" s="112" t="s">
+      <c r="AB23" s="119" t="s">
         <v>79</v>
       </c>
-      <c r="AC23" s="113"/>
-      <c r="AD23" s="113"/>
-      <c r="AE23" s="113"/>
-      <c r="AF23" s="113"/>
-      <c r="AG23" s="113"/>
-      <c r="AH23" s="113"/>
-      <c r="AI23" s="114"/>
+      <c r="AC23" s="120"/>
+      <c r="AD23" s="120"/>
+      <c r="AE23" s="120"/>
+      <c r="AF23" s="120"/>
+      <c r="AG23" s="120"/>
+      <c r="AH23" s="120"/>
+      <c r="AI23" s="121"/>
       <c r="AK23" s="10" t="s">
         <v>81</v>
       </c>
@@ -4648,11 +4657,11 @@
       <c r="B24" s="64" t="s">
         <v>86</v>
       </c>
-      <c r="D24" s="109" t="s">
+      <c r="D24" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="110"/>
-      <c r="F24" s="111"/>
+      <c r="E24" s="127"/>
+      <c r="F24" s="128"/>
       <c r="G24" s="60">
         <v>1</v>
       </c>
@@ -4662,12 +4671,12 @@
       <c r="I24" s="60">
         <v>0</v>
       </c>
-      <c r="J24" s="112" t="s">
+      <c r="J24" s="119" t="s">
         <v>5</v>
       </c>
-      <c r="K24" s="113"/>
-      <c r="L24" s="113"/>
-      <c r="M24" s="114"/>
+      <c r="K24" s="120"/>
+      <c r="L24" s="120"/>
+      <c r="M24" s="121"/>
       <c r="N24" s="61">
         <v>0</v>
       </c>
@@ -4710,16 +4719,16 @@
       <c r="AA24" s="52">
         <v>0</v>
       </c>
-      <c r="AB24" s="112" t="s">
+      <c r="AB24" s="119" t="s">
         <v>79</v>
       </c>
-      <c r="AC24" s="113"/>
-      <c r="AD24" s="113"/>
-      <c r="AE24" s="113"/>
-      <c r="AF24" s="113"/>
-      <c r="AG24" s="113"/>
-      <c r="AH24" s="113"/>
-      <c r="AI24" s="114"/>
+      <c r="AC24" s="120"/>
+      <c r="AD24" s="120"/>
+      <c r="AE24" s="120"/>
+      <c r="AF24" s="120"/>
+      <c r="AG24" s="120"/>
+      <c r="AH24" s="120"/>
+      <c r="AI24" s="121"/>
       <c r="AK24" s="10" t="s">
         <v>149</v>
       </c>
@@ -4731,11 +4740,11 @@
       <c r="B25" s="64" t="s">
         <v>87</v>
       </c>
-      <c r="D25" s="109" t="s">
+      <c r="D25" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="110"/>
-      <c r="F25" s="111"/>
+      <c r="E25" s="127"/>
+      <c r="F25" s="128"/>
       <c r="G25" s="60">
         <v>1</v>
       </c>
@@ -4745,12 +4754,12 @@
       <c r="I25" s="60">
         <v>0</v>
       </c>
-      <c r="J25" s="112" t="s">
+      <c r="J25" s="119" t="s">
         <v>5</v>
       </c>
-      <c r="K25" s="113"/>
-      <c r="L25" s="113"/>
-      <c r="M25" s="114"/>
+      <c r="K25" s="120"/>
+      <c r="L25" s="120"/>
+      <c r="M25" s="121"/>
       <c r="N25" s="61">
         <v>0</v>
       </c>
@@ -4826,11 +4835,11 @@
       <c r="B26" s="102" t="s">
         <v>605</v>
       </c>
-      <c r="D26" s="109" t="s">
+      <c r="D26" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="E26" s="110"/>
-      <c r="F26" s="111"/>
+      <c r="E26" s="127"/>
+      <c r="F26" s="128"/>
       <c r="G26" s="99">
         <v>1</v>
       </c>
@@ -4840,12 +4849,12 @@
       <c r="I26" s="99">
         <v>1</v>
       </c>
-      <c r="J26" s="112" t="s">
+      <c r="J26" s="119" t="s">
         <v>5</v>
       </c>
-      <c r="K26" s="113"/>
-      <c r="L26" s="113"/>
-      <c r="M26" s="114"/>
+      <c r="K26" s="120"/>
+      <c r="L26" s="120"/>
+      <c r="M26" s="121"/>
       <c r="N26" s="74">
         <v>1</v>
       </c>
@@ -4867,7 +4876,7 @@
       <c r="T26" s="69">
         <v>1</v>
       </c>
-      <c r="U26" s="173">
+      <c r="U26" s="109">
         <v>1</v>
       </c>
       <c r="V26" s="74">
@@ -4888,16 +4897,16 @@
       <c r="AA26" s="76">
         <v>0</v>
       </c>
-      <c r="AB26" s="138" t="s">
+      <c r="AB26" s="131" t="s">
         <v>604</v>
       </c>
-      <c r="AC26" s="138"/>
-      <c r="AD26" s="138"/>
-      <c r="AE26" s="138"/>
-      <c r="AF26" s="138"/>
-      <c r="AG26" s="138"/>
-      <c r="AH26" s="138"/>
-      <c r="AI26" s="138"/>
+      <c r="AC26" s="131"/>
+      <c r="AD26" s="131"/>
+      <c r="AE26" s="131"/>
+      <c r="AF26" s="131"/>
+      <c r="AG26" s="131"/>
+      <c r="AH26" s="131"/>
+      <c r="AI26" s="131"/>
       <c r="AK26" s="10" t="s">
         <v>606</v>
       </c>
@@ -4909,11 +4918,11 @@
       <c r="B27" s="64" t="s">
         <v>78</v>
       </c>
-      <c r="D27" s="133" t="s">
+      <c r="D27" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="E27" s="134"/>
-      <c r="F27" s="135"/>
+      <c r="E27" s="115"/>
+      <c r="F27" s="116"/>
       <c r="G27" s="60">
         <v>1</v>
       </c>
@@ -4977,16 +4986,16 @@
       <c r="AA27" s="77">
         <v>0</v>
       </c>
-      <c r="AB27" s="112" t="s">
+      <c r="AB27" s="119" t="s">
         <v>78</v>
       </c>
-      <c r="AC27" s="113"/>
-      <c r="AD27" s="113"/>
-      <c r="AE27" s="113"/>
-      <c r="AF27" s="113"/>
-      <c r="AG27" s="113"/>
-      <c r="AH27" s="113"/>
-      <c r="AI27" s="114"/>
+      <c r="AC27" s="120"/>
+      <c r="AD27" s="120"/>
+      <c r="AE27" s="120"/>
+      <c r="AF27" s="120"/>
+      <c r="AG27" s="120"/>
+      <c r="AH27" s="120"/>
+      <c r="AI27" s="121"/>
     </row>
     <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
@@ -4995,11 +5004,11 @@
       <c r="B28" s="46" t="s">
         <v>334</v>
       </c>
-      <c r="D28" s="133" t="s">
+      <c r="D28" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="E28" s="134"/>
-      <c r="F28" s="135"/>
+      <c r="E28" s="115"/>
+      <c r="F28" s="116"/>
       <c r="G28" s="60">
         <v>1</v>
       </c>
@@ -5092,42 +5101,42 @@
       </c>
     </row>
     <row r="36" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B36" s="121" t="s">
+      <c r="B36" s="138" t="s">
         <v>414</v>
       </c>
-      <c r="C36" s="122"/>
-      <c r="D36" s="122"/>
-      <c r="E36" s="122"/>
-      <c r="F36" s="122"/>
-      <c r="G36" s="122"/>
-      <c r="H36" s="122"/>
-      <c r="I36" s="122"/>
-      <c r="J36" s="122"/>
-      <c r="K36" s="122"/>
-      <c r="L36" s="122"/>
-      <c r="M36" s="122"/>
-      <c r="N36" s="122"/>
-      <c r="O36" s="122"/>
-      <c r="P36" s="122"/>
-      <c r="Q36" s="122"/>
-      <c r="R36" s="122"/>
-      <c r="S36" s="122"/>
-      <c r="T36" s="122"/>
-      <c r="U36" s="122"/>
-      <c r="V36" s="122"/>
-      <c r="W36" s="122"/>
-      <c r="X36" s="122"/>
-      <c r="Y36" s="122"/>
-      <c r="Z36" s="122"/>
-      <c r="AA36" s="122"/>
-      <c r="AB36" s="122"/>
-      <c r="AC36" s="122"/>
-      <c r="AD36" s="122"/>
-      <c r="AE36" s="122"/>
-      <c r="AF36" s="122"/>
-      <c r="AG36" s="122"/>
-      <c r="AH36" s="122"/>
-      <c r="AI36" s="123"/>
+      <c r="C36" s="139"/>
+      <c r="D36" s="139"/>
+      <c r="E36" s="139"/>
+      <c r="F36" s="139"/>
+      <c r="G36" s="139"/>
+      <c r="H36" s="139"/>
+      <c r="I36" s="139"/>
+      <c r="J36" s="139"/>
+      <c r="K36" s="139"/>
+      <c r="L36" s="139"/>
+      <c r="M36" s="139"/>
+      <c r="N36" s="139"/>
+      <c r="O36" s="139"/>
+      <c r="P36" s="139"/>
+      <c r="Q36" s="139"/>
+      <c r="R36" s="139"/>
+      <c r="S36" s="139"/>
+      <c r="T36" s="139"/>
+      <c r="U36" s="139"/>
+      <c r="V36" s="139"/>
+      <c r="W36" s="139"/>
+      <c r="X36" s="139"/>
+      <c r="Y36" s="139"/>
+      <c r="Z36" s="139"/>
+      <c r="AA36" s="139"/>
+      <c r="AB36" s="139"/>
+      <c r="AC36" s="139"/>
+      <c r="AD36" s="139"/>
+      <c r="AE36" s="139"/>
+      <c r="AF36" s="139"/>
+      <c r="AG36" s="139"/>
+      <c r="AH36" s="139"/>
+      <c r="AI36" s="140"/>
     </row>
     <row r="40" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B40" s="7"/>
@@ -5713,6 +5722,54 @@
     </row>
   </sheetData>
   <mergeCells count="64">
+    <mergeCell ref="T14:AI14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="J15:M15"/>
+    <mergeCell ref="N15:Q15"/>
+    <mergeCell ref="T15:AI15"/>
+    <mergeCell ref="B36:AI36"/>
+    <mergeCell ref="A1:AI1"/>
+    <mergeCell ref="X21:AI21"/>
+    <mergeCell ref="P21:W21"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="J12:M12"/>
+    <mergeCell ref="N10:Q10"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="R10:U10"/>
+    <mergeCell ref="J11:M11"/>
+    <mergeCell ref="N11:Q11"/>
+    <mergeCell ref="R11:U11"/>
+    <mergeCell ref="J10:M10"/>
+    <mergeCell ref="N12:Q12"/>
+    <mergeCell ref="R12:U12"/>
+    <mergeCell ref="J13:M13"/>
+    <mergeCell ref="N13:Q13"/>
+    <mergeCell ref="R13:U13"/>
+    <mergeCell ref="J19:M19"/>
+    <mergeCell ref="J20:M20"/>
+    <mergeCell ref="N16:AI16"/>
+    <mergeCell ref="J14:M14"/>
+    <mergeCell ref="N14:Q14"/>
+    <mergeCell ref="J18:M18"/>
+    <mergeCell ref="N18:Q18"/>
+    <mergeCell ref="J16:M16"/>
+    <mergeCell ref="N19:AI19"/>
+    <mergeCell ref="J26:M26"/>
+    <mergeCell ref="AB26:AI26"/>
     <mergeCell ref="AD10:AI10"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="AG13:AH13"/>
@@ -5729,54 +5786,6 @@
     <mergeCell ref="N20:AI20"/>
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="AB27:AI27"/>
-    <mergeCell ref="J18:M18"/>
-    <mergeCell ref="N18:Q18"/>
-    <mergeCell ref="J16:M16"/>
-    <mergeCell ref="N19:AI19"/>
-    <mergeCell ref="J26:M26"/>
-    <mergeCell ref="AB26:AI26"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="R10:U10"/>
-    <mergeCell ref="J11:M11"/>
-    <mergeCell ref="N11:Q11"/>
-    <mergeCell ref="R11:U11"/>
-    <mergeCell ref="J10:M10"/>
-    <mergeCell ref="N12:Q12"/>
-    <mergeCell ref="R12:U12"/>
-    <mergeCell ref="J13:M13"/>
-    <mergeCell ref="N13:Q13"/>
-    <mergeCell ref="R13:U13"/>
-    <mergeCell ref="J19:M19"/>
-    <mergeCell ref="J20:M20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="N16:AI16"/>
-    <mergeCell ref="B36:AI36"/>
-    <mergeCell ref="A1:AI1"/>
-    <mergeCell ref="X21:AI21"/>
-    <mergeCell ref="P21:W21"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="J12:M12"/>
-    <mergeCell ref="N10:Q10"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="J14:M14"/>
-    <mergeCell ref="N14:Q14"/>
-    <mergeCell ref="T14:AI14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="J15:M15"/>
-    <mergeCell ref="N15:Q15"/>
-    <mergeCell ref="T15:AI15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5788,7 +5797,7 @@
   <dimension ref="A1:I97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5886,7 +5895,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="106" t="str">
         <f>$B$2&amp;'Terra-Math'!L8&amp;$C$2&amp;$D$2&amp;'Terra-Math'!N8&amp;$E$2&amp;"\n"&amp;$F$2&amp;'Terra-Math'!A8&amp;$G$2&amp;"\n"&amp;'Terra-Math'!O8&amp;"\n"&amp;$H$2&amp;'Terra-Math'!M8&amp;$I$2&amp;"\n"&amp;'Terra-Math'!P8</f>
-        <v>## POW(Rd, Rs, Rm : Float)\n### *Powerof*\nRaises to power of numbers in registers and stores the result in the register.\n```Rd = Rs ^ Rm```\n</v>
+        <v>## POW(Rd, Rs, Rm : Float)\n### *Powerof*\nRaises to power of numbers in registers and stores the result in the register.\n```Rd = Rs ^ Rm```\nZero to the zeroth power must be evaluated to 1.0</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -5922,7 +5931,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="106" t="str">
         <f>$B$2&amp;'Terra-Math'!L14&amp;$C$2&amp;$D$2&amp;'Terra-Math'!N14&amp;$E$2&amp;"\n"&amp;$F$2&amp;'Terra-Math'!A14&amp;$G$2&amp;"\n"&amp;'Terra-Math'!O14&amp;"\n"&amp;$H$2&amp;'Terra-Math'!M14&amp;$I$2&amp;"\n"&amp;'Terra-Math'!P14</f>
-        <v>## POWINT(Rd, Rs, Rm : Int32)\n### *Powerof Integer*\nRaises to power of two integers in registers and stores the result in the register.\n```Rd = Rs ^ Rm```\n</v>
+        <v>## POWINT(Rd, Rs, Rm : Int32)\n### *Powerof Integer*\nRaises to power of two integers in registers and stores the result in the register.\n```Rd = Rs ^ Rm```\nZero to the zeroth power must be evaluated to 1</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -6198,19 +6207,19 @@
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
         <f>$B$2&amp;'Terra&amp;FlowerPot-Instructions'!A3&amp;$C$2&amp;$D$2&amp;'Terra&amp;FlowerPot-Instructions'!D3&amp;$E$2&amp;"\n"&amp;'Terra&amp;FlowerPot-Instructions'!E3&amp;"\n"&amp;$H$2&amp;'Terra&amp;FlowerPot-Instructions'!C3&amp;$I$2&amp;"\n"&amp;'Terra&amp;FlowerPot-Instructions'!F3</f>
-        <v>## LOADBYTE(destination, source, peripheral)\nLoads destination register with a byte from address (NOT at offset) stored in source register, in the device (IRQ) stored in peripheral register.\n```Rd = dev[Rperi].mem[Rs]```\n</v>
+        <v>## LOADBYTE(destination, source, peripheral)\nLoads destination register with a byte from address (NOT at offset) stored in source register, in the device (IRQ) stored in peripheral register.\n```Rd = dev[Rperi].mem[Rs]```\nRs should contain memory address, NOT an offset.</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
         <f>$B$2&amp;'Terra&amp;FlowerPot-Instructions'!A4&amp;$C$2&amp;$D$2&amp;'Terra&amp;FlowerPot-Instructions'!D4&amp;$E$2&amp;"\n"&amp;'Terra&amp;FlowerPot-Instructions'!E4&amp;"\n"&amp;$H$2&amp;'Terra&amp;FlowerPot-Instructions'!C4&amp;$I$2&amp;"\n"&amp;'Terra&amp;FlowerPot-Instructions'!F4</f>
-        <v>## LOADHWORD(destination, source, peripheral)\nLoads destination register with a halfword (two consecutive bytes) from address stored in source register, in the device (IRQ) stored in peripheral register.\n```Rd = dev[Rperi].mem[Rs]```\n</v>
+        <v>## LOADHWORD(destination, source, peripheral)\nLoads destination register with a halfword (two consecutive bytes) from address stored in source register, in the device (IRQ) stored in peripheral register.\n```Rd = dev[Rperi].mem[Rs]```\nRs should contain memory address, NOT an offset.</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
         <f>$B$2&amp;'Terra&amp;FlowerPot-Instructions'!A5&amp;$C$2&amp;$D$2&amp;'Terra&amp;FlowerPot-Instructions'!D5&amp;$E$2&amp;"\n"&amp;'Terra&amp;FlowerPot-Instructions'!E5&amp;"\n"&amp;$H$2&amp;'Terra&amp;FlowerPot-Instructions'!C5&amp;$I$2&amp;"\n"&amp;'Terra&amp;FlowerPot-Instructions'!F5</f>
-        <v>## LOADWORD(destination, source, peripheral)\nLoads destination register with a full word (four consecutive bytes) from address stored in source register, in the device (IRQ) stored in peripheral register.\n```Rd = dev[Rperi].mem[Rs]```\n</v>
+        <v>## LOADWORD(destination, source, peripheral)\nLoads destination register with a full word (four consecutive bytes) from address stored in source register, in the device (IRQ) stored in peripheral register.\n```Rd = dev[Rperi].mem[Rs]```\nRs should contain memory address, NOT an offset.</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
@@ -6636,25 +6645,25 @@
       <c r="F10" s="24">
         <v>0</v>
       </c>
-      <c r="G10" s="138" t="s">
+      <c r="G10" s="131" t="s">
         <v>245</v>
       </c>
-      <c r="H10" s="138"/>
-      <c r="I10" s="138"/>
-      <c r="J10" s="138"/>
-      <c r="K10" s="138"/>
-      <c r="L10" s="138" t="s">
+      <c r="H10" s="131"/>
+      <c r="I10" s="131"/>
+      <c r="J10" s="131"/>
+      <c r="K10" s="131"/>
+      <c r="L10" s="131" t="s">
         <v>5</v>
       </c>
-      <c r="M10" s="138"/>
-      <c r="N10" s="138" t="s">
+      <c r="M10" s="131"/>
+      <c r="N10" s="131" t="s">
         <v>9</v>
       </c>
-      <c r="O10" s="138"/>
-      <c r="P10" s="138" t="s">
+      <c r="O10" s="131"/>
+      <c r="P10" s="131" t="s">
         <v>10</v>
       </c>
-      <c r="Q10" s="138"/>
+      <c r="Q10" s="131"/>
       <c r="R10" s="24">
         <v>0</v>
       </c>
@@ -6693,14 +6702,14 @@
       <c r="K11" s="27">
         <v>0</v>
       </c>
-      <c r="L11" s="138" t="s">
+      <c r="L11" s="131" t="s">
         <v>5</v>
       </c>
-      <c r="M11" s="138"/>
-      <c r="N11" s="138" t="s">
+      <c r="M11" s="131"/>
+      <c r="N11" s="131" t="s">
         <v>9</v>
       </c>
-      <c r="O11" s="138"/>
+      <c r="O11" s="131"/>
       <c r="P11" s="24">
         <v>0</v>
       </c>
@@ -6746,14 +6755,14 @@
       <c r="K12" s="27">
         <v>0</v>
       </c>
-      <c r="L12" s="138" t="s">
+      <c r="L12" s="131" t="s">
         <v>5</v>
       </c>
-      <c r="M12" s="138"/>
-      <c r="N12" s="138" t="s">
+      <c r="M12" s="131"/>
+      <c r="N12" s="131" t="s">
         <v>9</v>
       </c>
-      <c r="O12" s="138"/>
+      <c r="O12" s="131"/>
       <c r="P12" s="27">
         <v>1</v>
       </c>
@@ -6788,26 +6797,26 @@
       <c r="G13" s="27">
         <v>0</v>
       </c>
-      <c r="H13" s="146" t="s">
+      <c r="H13" s="147" t="s">
         <v>5</v>
       </c>
-      <c r="I13" s="146"/>
+      <c r="I13" s="147"/>
       <c r="J13" s="27">
         <v>0</v>
       </c>
       <c r="K13" s="27">
         <v>1</v>
       </c>
-      <c r="L13" s="146" t="s">
+      <c r="L13" s="147" t="s">
         <v>135</v>
       </c>
-      <c r="M13" s="146"/>
-      <c r="N13" s="146"/>
-      <c r="O13" s="146"/>
-      <c r="P13" s="146"/>
-      <c r="Q13" s="146"/>
-      <c r="R13" s="146"/>
-      <c r="S13" s="146"/>
+      <c r="M13" s="147"/>
+      <c r="N13" s="147"/>
+      <c r="O13" s="147"/>
+      <c r="P13" s="147"/>
+      <c r="Q13" s="147"/>
+      <c r="R13" s="147"/>
+      <c r="S13" s="147"/>
       <c r="U13" s="10"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -6830,26 +6839,26 @@
       <c r="G14" s="27">
         <v>0</v>
       </c>
-      <c r="H14" s="146" t="s">
+      <c r="H14" s="147" t="s">
         <v>5</v>
       </c>
-      <c r="I14" s="146"/>
+      <c r="I14" s="147"/>
       <c r="J14" s="27">
         <v>1</v>
       </c>
       <c r="K14" s="27">
         <v>0</v>
       </c>
-      <c r="L14" s="146" t="s">
+      <c r="L14" s="147" t="s">
         <v>225</v>
       </c>
-      <c r="M14" s="146"/>
-      <c r="N14" s="146"/>
-      <c r="O14" s="146"/>
-      <c r="P14" s="146"/>
-      <c r="Q14" s="146"/>
-      <c r="R14" s="146"/>
-      <c r="S14" s="146"/>
+      <c r="M14" s="147"/>
+      <c r="N14" s="147"/>
+      <c r="O14" s="147"/>
+      <c r="P14" s="147"/>
+      <c r="Q14" s="147"/>
+      <c r="R14" s="147"/>
+      <c r="S14" s="147"/>
       <c r="U14" s="10"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -6872,26 +6881,26 @@
       <c r="G15" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="H15" s="146" t="s">
+      <c r="H15" s="147" t="s">
         <v>5</v>
       </c>
-      <c r="I15" s="146"/>
+      <c r="I15" s="147"/>
       <c r="J15" s="27">
         <v>0</v>
       </c>
       <c r="K15" s="27">
         <v>0</v>
       </c>
-      <c r="L15" s="146" t="s">
+      <c r="L15" s="147" t="s">
         <v>225</v>
       </c>
-      <c r="M15" s="146"/>
-      <c r="N15" s="146"/>
-      <c r="O15" s="146"/>
-      <c r="P15" s="146"/>
-      <c r="Q15" s="146"/>
-      <c r="R15" s="146"/>
-      <c r="S15" s="146"/>
+      <c r="M15" s="147"/>
+      <c r="N15" s="147"/>
+      <c r="O15" s="147"/>
+      <c r="P15" s="147"/>
+      <c r="Q15" s="147"/>
+      <c r="R15" s="147"/>
+      <c r="S15" s="147"/>
       <c r="U15" s="10"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -6913,30 +6922,30 @@
       <c r="G16" s="27">
         <v>1</v>
       </c>
-      <c r="H16" s="148" t="s">
+      <c r="H16" s="150" t="s">
         <v>3</v>
       </c>
-      <c r="I16" s="148"/>
-      <c r="J16" s="148"/>
+      <c r="I16" s="150"/>
+      <c r="J16" s="150"/>
       <c r="K16" s="27">
         <v>1</v>
       </c>
-      <c r="L16" s="146" t="s">
+      <c r="L16" s="147" t="s">
         <v>225</v>
       </c>
-      <c r="M16" s="146"/>
-      <c r="N16" s="146"/>
-      <c r="O16" s="146"/>
-      <c r="P16" s="146"/>
-      <c r="Q16" s="146"/>
-      <c r="R16" s="146"/>
-      <c r="S16" s="146"/>
+      <c r="M16" s="147"/>
+      <c r="N16" s="147"/>
+      <c r="O16" s="147"/>
+      <c r="P16" s="147"/>
+      <c r="Q16" s="147"/>
+      <c r="R16" s="147"/>
+      <c r="S16" s="147"/>
       <c r="U16" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="145">
+      <c r="A17" s="148">
         <v>13</v>
       </c>
       <c r="B17" s="28" t="s">
@@ -6954,14 +6963,14 @@
       <c r="G17" s="27">
         <v>0</v>
       </c>
-      <c r="H17" s="146" t="s">
+      <c r="H17" s="147" t="s">
         <v>248</v>
       </c>
-      <c r="I17" s="146"/>
-      <c r="J17" s="146" t="s">
+      <c r="I17" s="147"/>
+      <c r="J17" s="147" t="s">
         <v>251</v>
       </c>
-      <c r="K17" s="146"/>
+      <c r="K17" s="147"/>
       <c r="L17" s="27">
         <v>0</v>
       </c>
@@ -6991,7 +7000,7 @@
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="145"/>
+      <c r="A18" s="148"/>
       <c r="B18" s="28" t="s">
         <v>254</v>
       </c>
@@ -7007,14 +7016,14 @@
       <c r="G18" s="27">
         <v>0</v>
       </c>
-      <c r="H18" s="146" t="s">
+      <c r="H18" s="147" t="s">
         <v>248</v>
       </c>
-      <c r="I18" s="146"/>
-      <c r="J18" s="146" t="s">
+      <c r="I18" s="147"/>
+      <c r="J18" s="147" t="s">
         <v>251</v>
       </c>
-      <c r="K18" s="146"/>
+      <c r="K18" s="147"/>
       <c r="L18" s="27">
         <v>0</v>
       </c>
@@ -7044,7 +7053,7 @@
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="145"/>
+      <c r="A19" s="148"/>
       <c r="B19" s="28" t="s">
         <v>250</v>
       </c>
@@ -7060,12 +7069,12 @@
       <c r="G19" s="27">
         <v>0</v>
       </c>
-      <c r="H19" s="147" t="s">
+      <c r="H19" s="149" t="s">
         <v>243</v>
       </c>
-      <c r="I19" s="147"/>
-      <c r="J19" s="147"/>
-      <c r="K19" s="147"/>
+      <c r="I19" s="149"/>
+      <c r="J19" s="149"/>
+      <c r="K19" s="149"/>
       <c r="L19" s="27">
         <v>0</v>
       </c>
@@ -7290,18 +7299,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="L13:S13"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="L14:S14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="N11:O11"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="J18:K18"/>
@@ -7312,6 +7309,18 @@
     <mergeCell ref="J17:K17"/>
     <mergeCell ref="H16:J16"/>
     <mergeCell ref="H15:I15"/>
+    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="L13:S13"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="L14:S14"/>
+    <mergeCell ref="H14:I14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7322,8 +7331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:L2"/>
+    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7356,20 +7365,20 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="149" t="s">
+      <c r="A2" s="151" t="s">
         <v>139</v>
       </c>
-      <c r="B2" s="150"/>
-      <c r="C2" s="150"/>
-      <c r="D2" s="150"/>
-      <c r="E2" s="150"/>
-      <c r="F2" s="150"/>
-      <c r="G2" s="150"/>
-      <c r="H2" s="150"/>
-      <c r="I2" s="150"/>
-      <c r="J2" s="150"/>
-      <c r="K2" s="150"/>
-      <c r="L2" s="151"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="153"/>
       <c r="M2" s="17" t="s">
         <v>415</v>
       </c>
@@ -7645,6 +7654,9 @@
       <c r="O8" t="s">
         <v>449</v>
       </c>
+      <c r="P8" t="s">
+        <v>617</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="96" t="s">
@@ -7918,6 +7930,9 @@
       </c>
       <c r="O14" t="s">
         <v>457</v>
+      </c>
+      <c r="P14" t="s">
+        <v>618</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -10175,19 +10190,19 @@
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="149" t="s">
+      <c r="A2" s="151" t="s">
         <v>139</v>
       </c>
-      <c r="B2" s="150"/>
-      <c r="C2" s="150"/>
-      <c r="D2" s="150"/>
-      <c r="E2" s="150"/>
-      <c r="F2" s="150"/>
-      <c r="G2" s="150"/>
-      <c r="H2" s="150"/>
-      <c r="I2" s="150"/>
-      <c r="J2" s="150"/>
-      <c r="K2" s="151"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="153"/>
       <c r="L2" s="17" t="s">
         <v>415</v>
       </c>
@@ -11002,8 +11017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11017,11 +11032,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="152"/>
-      <c r="B1" s="152"/>
-      <c r="C1" s="152"/>
-      <c r="D1" s="152"/>
-      <c r="E1" s="152"/>
+      <c r="A1" s="154"/>
+      <c r="B1" s="154"/>
+      <c r="C1" s="154"/>
+      <c r="D1" s="154"/>
+      <c r="E1" s="154"/>
     </row>
     <row r="2" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="108" t="s">
@@ -11054,6 +11069,9 @@
       <c r="E3" t="s">
         <v>561</v>
       </c>
+      <c r="F3" t="s">
+        <v>619</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
@@ -11068,6 +11086,9 @@
       <c r="E4" t="s">
         <v>560</v>
       </c>
+      <c r="F4" t="s">
+        <v>619</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
@@ -11081,6 +11102,9 @@
       </c>
       <c r="E5" t="s">
         <v>559</v>
+      </c>
+      <c r="F5" t="s">
+        <v>619</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -11718,16 +11742,16 @@
       <c r="Z5" s="35">
         <v>0</v>
       </c>
-      <c r="AA5" s="120" t="s">
+      <c r="AA5" s="130" t="s">
         <v>79</v>
       </c>
-      <c r="AB5" s="120"/>
-      <c r="AC5" s="120"/>
-      <c r="AD5" s="120"/>
-      <c r="AE5" s="120"/>
-      <c r="AF5" s="120"/>
-      <c r="AG5" s="120"/>
-      <c r="AH5" s="120"/>
+      <c r="AB5" s="130"/>
+      <c r="AC5" s="130"/>
+      <c r="AD5" s="130"/>
+      <c r="AE5" s="130"/>
+      <c r="AF5" s="130"/>
+      <c r="AG5" s="130"/>
+      <c r="AH5" s="130"/>
       <c r="AJ5" s="10" t="s">
         <v>356</v>
       </c>
@@ -11808,18 +11832,18 @@
       <c r="Z6" s="88">
         <v>1</v>
       </c>
-      <c r="AA6" s="160" t="s">
+      <c r="AA6" s="171" t="s">
         <v>137</v>
       </c>
-      <c r="AB6" s="161"/>
-      <c r="AC6" s="161"/>
-      <c r="AD6" s="162"/>
-      <c r="AE6" s="119" t="s">
+      <c r="AB6" s="172"/>
+      <c r="AC6" s="172"/>
+      <c r="AD6" s="173"/>
+      <c r="AE6" s="129" t="s">
         <v>267</v>
       </c>
-      <c r="AF6" s="120"/>
-      <c r="AG6" s="120"/>
-      <c r="AH6" s="163"/>
+      <c r="AF6" s="130"/>
+      <c r="AG6" s="130"/>
+      <c r="AH6" s="174"/>
       <c r="AJ6" s="10" t="s">
         <v>308</v>
       </c>
@@ -11900,16 +11924,16 @@
       <c r="Z7" s="92" t="s">
         <v>124</v>
       </c>
-      <c r="AA7" s="157" t="s">
+      <c r="AA7" s="168" t="s">
         <v>310</v>
       </c>
-      <c r="AB7" s="158"/>
-      <c r="AC7" s="158"/>
-      <c r="AD7" s="158"/>
-      <c r="AE7" s="158"/>
-      <c r="AF7" s="158"/>
-      <c r="AG7" s="158"/>
-      <c r="AH7" s="159"/>
+      <c r="AB7" s="169"/>
+      <c r="AC7" s="169"/>
+      <c r="AD7" s="169"/>
+      <c r="AE7" s="169"/>
+      <c r="AF7" s="169"/>
+      <c r="AG7" s="169"/>
+      <c r="AH7" s="170"/>
       <c r="AJ7" s="10" t="s">
         <v>311</v>
       </c>
@@ -11975,25 +11999,25 @@
       <c r="U8" s="88">
         <v>1</v>
       </c>
-      <c r="V8" s="119" t="s">
+      <c r="V8" s="129" t="s">
         <v>267</v>
       </c>
-      <c r="W8" s="120"/>
-      <c r="X8" s="120"/>
-      <c r="Y8" s="120"/>
+      <c r="W8" s="130"/>
+      <c r="X8" s="130"/>
+      <c r="Y8" s="130"/>
       <c r="Z8" s="92" t="s">
         <v>358</v>
       </c>
-      <c r="AA8" s="158" t="s">
+      <c r="AA8" s="169" t="s">
         <v>135</v>
       </c>
-      <c r="AB8" s="158"/>
-      <c r="AC8" s="158"/>
-      <c r="AD8" s="158"/>
-      <c r="AE8" s="158"/>
-      <c r="AF8" s="158"/>
-      <c r="AG8" s="158"/>
-      <c r="AH8" s="159"/>
+      <c r="AB8" s="169"/>
+      <c r="AC8" s="169"/>
+      <c r="AD8" s="169"/>
+      <c r="AE8" s="169"/>
+      <c r="AF8" s="169"/>
+      <c r="AG8" s="169"/>
+      <c r="AH8" s="170"/>
       <c r="AJ8" s="10" t="s">
         <v>359</v>
       </c>
@@ -12059,27 +12083,27 @@
       <c r="U9" s="79">
         <v>0</v>
       </c>
-      <c r="V9" s="119" t="s">
+      <c r="V9" s="129" t="s">
         <v>410</v>
       </c>
-      <c r="W9" s="120"/>
-      <c r="X9" s="120"/>
-      <c r="Y9" s="120"/>
+      <c r="W9" s="130"/>
+      <c r="X9" s="130"/>
+      <c r="Y9" s="130"/>
       <c r="Z9" s="89" t="s">
         <v>409</v>
       </c>
-      <c r="AA9" s="119" t="s">
+      <c r="AA9" s="129" t="s">
         <v>411</v>
       </c>
-      <c r="AB9" s="120"/>
-      <c r="AC9" s="120"/>
-      <c r="AD9" s="120"/>
-      <c r="AE9" s="119" t="s">
+      <c r="AB9" s="130"/>
+      <c r="AC9" s="130"/>
+      <c r="AD9" s="130"/>
+      <c r="AE9" s="129" t="s">
         <v>412</v>
       </c>
-      <c r="AF9" s="120"/>
-      <c r="AG9" s="120"/>
-      <c r="AH9" s="120"/>
+      <c r="AF9" s="130"/>
+      <c r="AG9" s="130"/>
+      <c r="AH9" s="130"/>
       <c r="AJ9" s="10" t="s">
         <v>420</v>
       </c>
@@ -12109,39 +12133,39 @@
       <c r="I10" s="88">
         <v>1</v>
       </c>
-      <c r="J10" s="120" t="s">
+      <c r="J10" s="130" t="s">
         <v>266</v>
       </c>
-      <c r="K10" s="120"/>
-      <c r="L10" s="120"/>
-      <c r="M10" s="120"/>
-      <c r="N10" s="120"/>
-      <c r="O10" s="155" t="s">
+      <c r="K10" s="130"/>
+      <c r="L10" s="130"/>
+      <c r="M10" s="130"/>
+      <c r="N10" s="130"/>
+      <c r="O10" s="165" t="s">
         <v>267</v>
       </c>
-      <c r="P10" s="155"/>
-      <c r="Q10" s="155"/>
-      <c r="R10" s="156"/>
-      <c r="S10" s="120" t="s">
+      <c r="P10" s="165"/>
+      <c r="Q10" s="165"/>
+      <c r="R10" s="166"/>
+      <c r="S10" s="130" t="s">
         <v>268</v>
       </c>
-      <c r="T10" s="120"/>
-      <c r="U10" s="120"/>
-      <c r="V10" s="120"/>
-      <c r="W10" s="120"/>
-      <c r="X10" s="120"/>
-      <c r="Y10" s="120"/>
-      <c r="Z10" s="120"/>
-      <c r="AA10" s="120" t="s">
+      <c r="T10" s="130"/>
+      <c r="U10" s="130"/>
+      <c r="V10" s="130"/>
+      <c r="W10" s="130"/>
+      <c r="X10" s="130"/>
+      <c r="Y10" s="130"/>
+      <c r="Z10" s="130"/>
+      <c r="AA10" s="130" t="s">
         <v>79</v>
       </c>
-      <c r="AB10" s="120"/>
-      <c r="AC10" s="120"/>
-      <c r="AD10" s="120"/>
-      <c r="AE10" s="120"/>
-      <c r="AF10" s="120"/>
-      <c r="AG10" s="120"/>
-      <c r="AH10" s="120"/>
+      <c r="AB10" s="130"/>
+      <c r="AC10" s="130"/>
+      <c r="AD10" s="130"/>
+      <c r="AE10" s="130"/>
+      <c r="AF10" s="130"/>
+      <c r="AG10" s="130"/>
+      <c r="AH10" s="130"/>
       <c r="AJ10" s="10" t="s">
         <v>294</v>
       </c>
@@ -12180,30 +12204,30 @@
       <c r="L11" s="91">
         <v>0</v>
       </c>
-      <c r="M11" s="112" t="s">
+      <c r="M11" s="119" t="s">
         <v>313</v>
       </c>
-      <c r="N11" s="113"/>
-      <c r="O11" s="113"/>
-      <c r="P11" s="113"/>
-      <c r="Q11" s="113"/>
-      <c r="R11" s="113"/>
-      <c r="S11" s="113"/>
-      <c r="T11" s="113"/>
-      <c r="U11" s="113"/>
-      <c r="V11" s="113"/>
-      <c r="W11" s="113"/>
-      <c r="X11" s="113"/>
-      <c r="Y11" s="113"/>
-      <c r="Z11" s="113"/>
-      <c r="AA11" s="113"/>
-      <c r="AB11" s="113"/>
-      <c r="AC11" s="113"/>
-      <c r="AD11" s="113"/>
-      <c r="AE11" s="113"/>
-      <c r="AF11" s="113"/>
-      <c r="AG11" s="113"/>
-      <c r="AH11" s="114"/>
+      <c r="N11" s="120"/>
+      <c r="O11" s="120"/>
+      <c r="P11" s="120"/>
+      <c r="Q11" s="120"/>
+      <c r="R11" s="120"/>
+      <c r="S11" s="120"/>
+      <c r="T11" s="120"/>
+      <c r="U11" s="120"/>
+      <c r="V11" s="120"/>
+      <c r="W11" s="120"/>
+      <c r="X11" s="120"/>
+      <c r="Y11" s="120"/>
+      <c r="Z11" s="120"/>
+      <c r="AA11" s="120"/>
+      <c r="AB11" s="120"/>
+      <c r="AC11" s="120"/>
+      <c r="AD11" s="120"/>
+      <c r="AE11" s="120"/>
+      <c r="AF11" s="120"/>
+      <c r="AG11" s="120"/>
+      <c r="AH11" s="121"/>
       <c r="AJ11" s="10" t="s">
         <v>293</v>
       </c>
@@ -12230,36 +12254,36 @@
       <c r="H12" s="74">
         <v>1</v>
       </c>
-      <c r="I12" s="154" t="s">
+      <c r="I12" s="167" t="s">
         <v>421</v>
       </c>
-      <c r="J12" s="155"/>
-      <c r="K12" s="155"/>
-      <c r="L12" s="156"/>
-      <c r="M12" s="112" t="s">
+      <c r="J12" s="165"/>
+      <c r="K12" s="165"/>
+      <c r="L12" s="166"/>
+      <c r="M12" s="119" t="s">
         <v>313</v>
       </c>
-      <c r="N12" s="113"/>
-      <c r="O12" s="113"/>
-      <c r="P12" s="113"/>
-      <c r="Q12" s="113"/>
-      <c r="R12" s="113"/>
-      <c r="S12" s="113"/>
-      <c r="T12" s="113"/>
-      <c r="U12" s="113"/>
-      <c r="V12" s="113"/>
-      <c r="W12" s="113"/>
-      <c r="X12" s="113"/>
-      <c r="Y12" s="113"/>
-      <c r="Z12" s="113"/>
-      <c r="AA12" s="113"/>
-      <c r="AB12" s="113"/>
-      <c r="AC12" s="113"/>
-      <c r="AD12" s="113"/>
-      <c r="AE12" s="113"/>
-      <c r="AF12" s="113"/>
-      <c r="AG12" s="113"/>
-      <c r="AH12" s="114"/>
+      <c r="N12" s="120"/>
+      <c r="O12" s="120"/>
+      <c r="P12" s="120"/>
+      <c r="Q12" s="120"/>
+      <c r="R12" s="120"/>
+      <c r="S12" s="120"/>
+      <c r="T12" s="120"/>
+      <c r="U12" s="120"/>
+      <c r="V12" s="120"/>
+      <c r="W12" s="120"/>
+      <c r="X12" s="120"/>
+      <c r="Y12" s="120"/>
+      <c r="Z12" s="120"/>
+      <c r="AA12" s="120"/>
+      <c r="AB12" s="120"/>
+      <c r="AC12" s="120"/>
+      <c r="AD12" s="120"/>
+      <c r="AE12" s="120"/>
+      <c r="AF12" s="120"/>
+      <c r="AG12" s="120"/>
+      <c r="AH12" s="121"/>
       <c r="AJ12" s="10" t="s">
         <v>315</v>
       </c>
@@ -12307,37 +12331,37 @@
       <c r="C14" s="68">
         <v>1</v>
       </c>
-      <c r="D14" s="138"/>
-      <c r="E14" s="138"/>
-      <c r="F14" s="138"/>
-      <c r="G14" s="138"/>
-      <c r="H14" s="138"/>
-      <c r="I14" s="138"/>
-      <c r="J14" s="138"/>
-      <c r="K14" s="138"/>
-      <c r="L14" s="138"/>
-      <c r="M14" s="138"/>
-      <c r="N14" s="138"/>
-      <c r="O14" s="138"/>
-      <c r="P14" s="138"/>
-      <c r="Q14" s="138"/>
-      <c r="R14" s="138"/>
-      <c r="S14" s="138"/>
-      <c r="T14" s="138"/>
-      <c r="U14" s="138"/>
-      <c r="V14" s="138"/>
-      <c r="W14" s="138"/>
-      <c r="X14" s="138"/>
-      <c r="Y14" s="138"/>
-      <c r="Z14" s="138"/>
-      <c r="AA14" s="138"/>
-      <c r="AB14" s="138"/>
-      <c r="AC14" s="138"/>
-      <c r="AD14" s="138"/>
-      <c r="AE14" s="138"/>
-      <c r="AF14" s="138"/>
-      <c r="AG14" s="138"/>
-      <c r="AH14" s="138"/>
+      <c r="D14" s="131"/>
+      <c r="E14" s="131"/>
+      <c r="F14" s="131"/>
+      <c r="G14" s="131"/>
+      <c r="H14" s="131"/>
+      <c r="I14" s="131"/>
+      <c r="J14" s="131"/>
+      <c r="K14" s="131"/>
+      <c r="L14" s="131"/>
+      <c r="M14" s="131"/>
+      <c r="N14" s="131"/>
+      <c r="O14" s="131"/>
+      <c r="P14" s="131"/>
+      <c r="Q14" s="131"/>
+      <c r="R14" s="131"/>
+      <c r="S14" s="131"/>
+      <c r="T14" s="131"/>
+      <c r="U14" s="131"/>
+      <c r="V14" s="131"/>
+      <c r="W14" s="131"/>
+      <c r="X14" s="131"/>
+      <c r="Y14" s="131"/>
+      <c r="Z14" s="131"/>
+      <c r="AA14" s="131"/>
+      <c r="AB14" s="131"/>
+      <c r="AC14" s="131"/>
+      <c r="AD14" s="131"/>
+      <c r="AE14" s="131"/>
+      <c r="AF14" s="131"/>
+      <c r="AG14" s="131"/>
+      <c r="AH14" s="131"/>
       <c r="AJ14" s="10" t="s">
         <v>302</v>
       </c>
@@ -13412,44 +13436,44 @@
     </row>
     <row r="39" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A39" s="82"/>
-      <c r="C39" s="164" t="s">
+      <c r="C39" s="155" t="s">
         <v>406</v>
       </c>
-      <c r="D39" s="165"/>
-      <c r="E39" s="165"/>
-      <c r="F39" s="165"/>
-      <c r="G39" s="165"/>
-      <c r="H39" s="165"/>
-      <c r="I39" s="165"/>
-      <c r="J39" s="165"/>
-      <c r="K39" s="165"/>
-      <c r="L39" s="165"/>
-      <c r="M39" s="165"/>
-      <c r="N39" s="165"/>
-      <c r="O39" s="165"/>
-      <c r="P39" s="165"/>
-      <c r="Q39" s="165"/>
-      <c r="R39" s="166"/>
-      <c r="S39" s="164" t="s">
+      <c r="D39" s="156"/>
+      <c r="E39" s="156"/>
+      <c r="F39" s="156"/>
+      <c r="G39" s="156"/>
+      <c r="H39" s="156"/>
+      <c r="I39" s="156"/>
+      <c r="J39" s="156"/>
+      <c r="K39" s="156"/>
+      <c r="L39" s="156"/>
+      <c r="M39" s="156"/>
+      <c r="N39" s="156"/>
+      <c r="O39" s="156"/>
+      <c r="P39" s="156"/>
+      <c r="Q39" s="156"/>
+      <c r="R39" s="157"/>
+      <c r="S39" s="155" t="s">
         <v>408</v>
       </c>
-      <c r="T39" s="165"/>
-      <c r="U39" s="165"/>
-      <c r="V39" s="165"/>
-      <c r="W39" s="165"/>
-      <c r="X39" s="165"/>
-      <c r="Y39" s="165"/>
-      <c r="Z39" s="166"/>
-      <c r="AA39" s="164" t="s">
+      <c r="T39" s="156"/>
+      <c r="U39" s="156"/>
+      <c r="V39" s="156"/>
+      <c r="W39" s="156"/>
+      <c r="X39" s="156"/>
+      <c r="Y39" s="156"/>
+      <c r="Z39" s="157"/>
+      <c r="AA39" s="155" t="s">
         <v>407</v>
       </c>
-      <c r="AB39" s="165"/>
-      <c r="AC39" s="165"/>
-      <c r="AD39" s="165"/>
-      <c r="AE39" s="165"/>
-      <c r="AF39" s="165"/>
-      <c r="AG39" s="165"/>
-      <c r="AH39" s="166"/>
+      <c r="AB39" s="156"/>
+      <c r="AC39" s="156"/>
+      <c r="AD39" s="156"/>
+      <c r="AE39" s="156"/>
+      <c r="AF39" s="156"/>
+      <c r="AG39" s="156"/>
+      <c r="AH39" s="157"/>
       <c r="AJ39" t="s">
         <v>416</v>
       </c>
@@ -13496,172 +13520,172 @@
       <c r="A42" s="22" t="s">
         <v>346</v>
       </c>
-      <c r="C42" s="167">
+      <c r="C42" s="158">
         <v>16384</v>
       </c>
-      <c r="D42" s="168"/>
-      <c r="E42" s="168"/>
-      <c r="F42" s="168"/>
-      <c r="G42" s="168"/>
-      <c r="H42" s="168"/>
-      <c r="I42" s="168"/>
-      <c r="J42" s="168"/>
-      <c r="K42" s="168"/>
-      <c r="L42" s="168"/>
-      <c r="M42" s="168"/>
-      <c r="N42" s="168"/>
-      <c r="O42" s="168"/>
-      <c r="P42" s="168"/>
-      <c r="Q42" s="168"/>
-      <c r="R42" s="168"/>
-      <c r="S42" s="168"/>
-      <c r="T42" s="168"/>
-      <c r="U42" s="168"/>
-      <c r="V42" s="168"/>
-      <c r="W42" s="168"/>
-      <c r="X42" s="168"/>
-      <c r="Y42" s="168"/>
-      <c r="Z42" s="168"/>
-      <c r="AA42" s="168"/>
-      <c r="AB42" s="168"/>
-      <c r="AC42" s="168"/>
-      <c r="AD42" s="168"/>
-      <c r="AE42" s="168"/>
-      <c r="AF42" s="168"/>
-      <c r="AG42" s="168"/>
-      <c r="AH42" s="169"/>
+      <c r="D42" s="159"/>
+      <c r="E42" s="159"/>
+      <c r="F42" s="159"/>
+      <c r="G42" s="159"/>
+      <c r="H42" s="159"/>
+      <c r="I42" s="159"/>
+      <c r="J42" s="159"/>
+      <c r="K42" s="159"/>
+      <c r="L42" s="159"/>
+      <c r="M42" s="159"/>
+      <c r="N42" s="159"/>
+      <c r="O42" s="159"/>
+      <c r="P42" s="159"/>
+      <c r="Q42" s="159"/>
+      <c r="R42" s="159"/>
+      <c r="S42" s="159"/>
+      <c r="T42" s="159"/>
+      <c r="U42" s="159"/>
+      <c r="V42" s="159"/>
+      <c r="W42" s="159"/>
+      <c r="X42" s="159"/>
+      <c r="Y42" s="159"/>
+      <c r="Z42" s="159"/>
+      <c r="AA42" s="159"/>
+      <c r="AB42" s="159"/>
+      <c r="AC42" s="159"/>
+      <c r="AD42" s="159"/>
+      <c r="AE42" s="159"/>
+      <c r="AF42" s="159"/>
+      <c r="AG42" s="159"/>
+      <c r="AH42" s="160"/>
     </row>
     <row r="44" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C44" s="172" t="s">
+      <c r="C44" s="164" t="s">
         <v>361</v>
       </c>
-      <c r="D44" s="153"/>
-      <c r="E44" s="153"/>
-      <c r="F44" s="153"/>
-      <c r="G44" s="153" t="s">
+      <c r="D44" s="162"/>
+      <c r="E44" s="162"/>
+      <c r="F44" s="162"/>
+      <c r="G44" s="162" t="s">
         <v>362</v>
       </c>
-      <c r="H44" s="153"/>
-      <c r="I44" s="153"/>
-      <c r="J44" s="153"/>
-      <c r="K44" s="153" t="s">
+      <c r="H44" s="162"/>
+      <c r="I44" s="162"/>
+      <c r="J44" s="162"/>
+      <c r="K44" s="162" t="s">
         <v>363</v>
       </c>
-      <c r="L44" s="153"/>
-      <c r="M44" s="153"/>
-      <c r="N44" s="153"/>
-      <c r="O44" s="153"/>
-      <c r="P44" s="153"/>
-      <c r="Q44" s="153"/>
-      <c r="R44" s="153"/>
-      <c r="S44" s="153" t="s">
+      <c r="L44" s="162"/>
+      <c r="M44" s="162"/>
+      <c r="N44" s="162"/>
+      <c r="O44" s="162"/>
+      <c r="P44" s="162"/>
+      <c r="Q44" s="162"/>
+      <c r="R44" s="162"/>
+      <c r="S44" s="162" t="s">
         <v>422</v>
       </c>
-      <c r="T44" s="153"/>
-      <c r="U44" s="153"/>
-      <c r="V44" s="153"/>
-      <c r="W44" s="153"/>
-      <c r="X44" s="153"/>
-      <c r="Y44" s="153"/>
-      <c r="Z44" s="153"/>
-      <c r="AA44" s="171" t="s">
+      <c r="T44" s="162"/>
+      <c r="U44" s="162"/>
+      <c r="V44" s="162"/>
+      <c r="W44" s="162"/>
+      <c r="X44" s="162"/>
+      <c r="Y44" s="162"/>
+      <c r="Z44" s="162"/>
+      <c r="AA44" s="163" t="s">
         <v>423</v>
       </c>
-      <c r="AB44" s="171"/>
-      <c r="AC44" s="171"/>
-      <c r="AD44" s="171"/>
-      <c r="AE44" s="171"/>
-      <c r="AF44" s="171"/>
-      <c r="AG44" s="171"/>
-      <c r="AH44" s="171"/>
+      <c r="AB44" s="163"/>
+      <c r="AC44" s="163"/>
+      <c r="AD44" s="163"/>
+      <c r="AE44" s="163"/>
+      <c r="AF44" s="163"/>
+      <c r="AG44" s="163"/>
+      <c r="AH44" s="163"/>
     </row>
     <row r="45" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="23" t="s">
         <v>347</v>
       </c>
       <c r="B45" s="3"/>
-      <c r="C45" s="170" t="s">
+      <c r="C45" s="161" t="s">
         <v>348</v>
       </c>
-      <c r="D45" s="170"/>
-      <c r="E45" s="170"/>
-      <c r="F45" s="170"/>
-      <c r="G45" s="170"/>
-      <c r="H45" s="170"/>
-      <c r="I45" s="170"/>
-      <c r="J45" s="170"/>
-      <c r="K45" s="170" t="s">
+      <c r="D45" s="161"/>
+      <c r="E45" s="161"/>
+      <c r="F45" s="161"/>
+      <c r="G45" s="161"/>
+      <c r="H45" s="161"/>
+      <c r="I45" s="161"/>
+      <c r="J45" s="161"/>
+      <c r="K45" s="161" t="s">
         <v>349</v>
       </c>
-      <c r="L45" s="170"/>
-      <c r="M45" s="170"/>
-      <c r="N45" s="170"/>
-      <c r="O45" s="170"/>
-      <c r="P45" s="170"/>
-      <c r="Q45" s="170"/>
-      <c r="R45" s="170"/>
-      <c r="S45" s="170" t="s">
+      <c r="L45" s="161"/>
+      <c r="M45" s="161"/>
+      <c r="N45" s="161"/>
+      <c r="O45" s="161"/>
+      <c r="P45" s="161"/>
+      <c r="Q45" s="161"/>
+      <c r="R45" s="161"/>
+      <c r="S45" s="161" t="s">
         <v>350</v>
       </c>
-      <c r="T45" s="170"/>
-      <c r="U45" s="170"/>
-      <c r="V45" s="170"/>
-      <c r="W45" s="170"/>
-      <c r="X45" s="170"/>
-      <c r="Y45" s="170"/>
-      <c r="Z45" s="170"/>
-      <c r="AA45" s="170" t="s">
+      <c r="T45" s="161"/>
+      <c r="U45" s="161"/>
+      <c r="V45" s="161"/>
+      <c r="W45" s="161"/>
+      <c r="X45" s="161"/>
+      <c r="Y45" s="161"/>
+      <c r="Z45" s="161"/>
+      <c r="AA45" s="161" t="s">
         <v>351</v>
       </c>
-      <c r="AB45" s="170"/>
-      <c r="AC45" s="170"/>
-      <c r="AD45" s="170"/>
-      <c r="AE45" s="170"/>
-      <c r="AF45" s="170"/>
-      <c r="AG45" s="170"/>
-      <c r="AH45" s="170"/>
+      <c r="AB45" s="161"/>
+      <c r="AC45" s="161"/>
+      <c r="AD45" s="161"/>
+      <c r="AE45" s="161"/>
+      <c r="AF45" s="161"/>
+      <c r="AG45" s="161"/>
+      <c r="AH45" s="161"/>
     </row>
     <row r="46" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="C46" s="164" t="s">
+      <c r="C46" s="155" t="s">
         <v>364</v>
       </c>
-      <c r="D46" s="165"/>
-      <c r="E46" s="165"/>
-      <c r="F46" s="165"/>
-      <c r="G46" s="165" t="s">
+      <c r="D46" s="156"/>
+      <c r="E46" s="156"/>
+      <c r="F46" s="156"/>
+      <c r="G46" s="156" t="s">
         <v>424</v>
       </c>
-      <c r="H46" s="165"/>
-      <c r="I46" s="165"/>
-      <c r="J46" s="166"/>
-      <c r="K46" s="164" t="s">
+      <c r="H46" s="156"/>
+      <c r="I46" s="156"/>
+      <c r="J46" s="157"/>
+      <c r="K46" s="155" t="s">
         <v>352</v>
       </c>
-      <c r="L46" s="165"/>
-      <c r="M46" s="165"/>
-      <c r="N46" s="165"/>
-      <c r="O46" s="165"/>
-      <c r="P46" s="165"/>
-      <c r="Q46" s="165"/>
-      <c r="R46" s="166"/>
-      <c r="S46" s="164" t="s">
+      <c r="L46" s="156"/>
+      <c r="M46" s="156"/>
+      <c r="N46" s="156"/>
+      <c r="O46" s="156"/>
+      <c r="P46" s="156"/>
+      <c r="Q46" s="156"/>
+      <c r="R46" s="157"/>
+      <c r="S46" s="155" t="s">
         <v>353</v>
       </c>
-      <c r="T46" s="165"/>
-      <c r="U46" s="165"/>
-      <c r="V46" s="165"/>
-      <c r="W46" s="165"/>
-      <c r="X46" s="165"/>
-      <c r="Y46" s="165"/>
-      <c r="Z46" s="165"/>
-      <c r="AA46" s="165"/>
-      <c r="AB46" s="165"/>
-      <c r="AC46" s="165"/>
-      <c r="AD46" s="165"/>
-      <c r="AE46" s="165"/>
-      <c r="AF46" s="165"/>
-      <c r="AG46" s="165"/>
-      <c r="AH46" s="166"/>
+      <c r="T46" s="156"/>
+      <c r="U46" s="156"/>
+      <c r="V46" s="156"/>
+      <c r="W46" s="156"/>
+      <c r="X46" s="156"/>
+      <c r="Y46" s="156"/>
+      <c r="Z46" s="156"/>
+      <c r="AA46" s="156"/>
+      <c r="AB46" s="156"/>
+      <c r="AC46" s="156"/>
+      <c r="AD46" s="156"/>
+      <c r="AE46" s="156"/>
+      <c r="AF46" s="156"/>
+      <c r="AG46" s="156"/>
+      <c r="AH46" s="157"/>
     </row>
     <row r="48" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="23" t="s">
@@ -13678,26 +13702,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="AA39:AH39"/>
-    <mergeCell ref="S39:Z39"/>
-    <mergeCell ref="K46:R46"/>
-    <mergeCell ref="C42:AH42"/>
-    <mergeCell ref="C45:J45"/>
-    <mergeCell ref="K45:R45"/>
-    <mergeCell ref="S45:Z45"/>
-    <mergeCell ref="AA45:AH45"/>
-    <mergeCell ref="K44:R44"/>
-    <mergeCell ref="S44:Z44"/>
-    <mergeCell ref="AA44:AH44"/>
-    <mergeCell ref="S46:AH46"/>
-    <mergeCell ref="C44:F44"/>
-    <mergeCell ref="J10:N10"/>
-    <mergeCell ref="O10:R10"/>
-    <mergeCell ref="C46:F46"/>
-    <mergeCell ref="G46:J46"/>
-    <mergeCell ref="C39:R39"/>
-    <mergeCell ref="G44:J44"/>
-    <mergeCell ref="I12:L12"/>
     <mergeCell ref="AA5:AH5"/>
     <mergeCell ref="AA10:AH10"/>
     <mergeCell ref="S10:Z10"/>
@@ -13712,6 +13716,26 @@
     <mergeCell ref="V9:Y9"/>
     <mergeCell ref="AA9:AD9"/>
     <mergeCell ref="AE9:AH9"/>
+    <mergeCell ref="J10:N10"/>
+    <mergeCell ref="O10:R10"/>
+    <mergeCell ref="C46:F46"/>
+    <mergeCell ref="G46:J46"/>
+    <mergeCell ref="C39:R39"/>
+    <mergeCell ref="G44:J44"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="AA39:AH39"/>
+    <mergeCell ref="S39:Z39"/>
+    <mergeCell ref="K46:R46"/>
+    <mergeCell ref="C42:AH42"/>
+    <mergeCell ref="C45:J45"/>
+    <mergeCell ref="K45:R45"/>
+    <mergeCell ref="S45:Z45"/>
+    <mergeCell ref="AA45:AH45"/>
+    <mergeCell ref="K44:R44"/>
+    <mergeCell ref="S44:Z44"/>
+    <mergeCell ref="AA44:AH44"/>
+    <mergeCell ref="S46:AH46"/>
+    <mergeCell ref="C44:F44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13722,7 +13746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
@@ -13736,20 +13760,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="141" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
-      <c r="D1" s="124"/>
-      <c r="E1" s="124"/>
-      <c r="F1" s="124"/>
-      <c r="G1" s="124"/>
-      <c r="H1" s="124"/>
-      <c r="I1" s="124"/>
-      <c r="J1" s="124"/>
-      <c r="K1" s="124"/>
-      <c r="L1" s="124"/>
+      <c r="B1" s="141"/>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
+      <c r="H1" s="141"/>
+      <c r="I1" s="141"/>
+      <c r="J1" s="141"/>
+      <c r="K1" s="141"/>
+      <c r="L1" s="141"/>
       <c r="M1" s="1"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -14241,7 +14265,7 @@
         <f t="shared" si="3"/>
         <v>05h</v>
       </c>
-      <c r="M18" s="174" t="s">
+      <c r="M18" s="110" t="s">
         <v>616</v>
       </c>
     </row>
@@ -14547,12 +14571,12 @@
       <c r="N6" s="34">
         <v>1</v>
       </c>
-      <c r="O6" s="138" t="s">
+      <c r="O6" s="131" t="s">
         <v>229</v>
       </c>
-      <c r="P6" s="138"/>
-      <c r="Q6" s="138"/>
-      <c r="R6" s="138"/>
+      <c r="P6" s="131"/>
+      <c r="Q6" s="131"/>
+      <c r="R6" s="131"/>
       <c r="T6" s="10" t="s">
         <v>338</v>
       </c>
@@ -14585,16 +14609,16 @@
       <c r="J7" s="34">
         <v>1</v>
       </c>
-      <c r="K7" s="138" t="s">
+      <c r="K7" s="131" t="s">
         <v>123</v>
       </c>
-      <c r="L7" s="138"/>
-      <c r="M7" s="138"/>
-      <c r="N7" s="138"/>
-      <c r="O7" s="138"/>
-      <c r="P7" s="138"/>
-      <c r="Q7" s="138"/>
-      <c r="R7" s="138"/>
+      <c r="L7" s="131"/>
+      <c r="M7" s="131"/>
+      <c r="N7" s="131"/>
+      <c r="O7" s="131"/>
+      <c r="P7" s="131"/>
+      <c r="Q7" s="131"/>
+      <c r="R7" s="131"/>
       <c r="T7" s="10"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -14625,16 +14649,16 @@
       <c r="J8" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="K8" s="138" t="s">
+      <c r="K8" s="131" t="s">
         <v>123</v>
       </c>
-      <c r="L8" s="138"/>
-      <c r="M8" s="138"/>
-      <c r="N8" s="138"/>
-      <c r="O8" s="138"/>
-      <c r="P8" s="138"/>
-      <c r="Q8" s="138"/>
-      <c r="R8" s="138"/>
+      <c r="L8" s="131"/>
+      <c r="M8" s="131"/>
+      <c r="N8" s="131"/>
+      <c r="O8" s="131"/>
+      <c r="P8" s="131"/>
+      <c r="Q8" s="131"/>
+      <c r="R8" s="131"/>
       <c r="T8" s="10"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -14665,16 +14689,16 @@
       <c r="J9" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="K9" s="138" t="s">
+      <c r="K9" s="131" t="s">
         <v>123</v>
       </c>
-      <c r="L9" s="138"/>
-      <c r="M9" s="138"/>
-      <c r="N9" s="138"/>
-      <c r="O9" s="138"/>
-      <c r="P9" s="138"/>
-      <c r="Q9" s="138"/>
-      <c r="R9" s="138"/>
+      <c r="L9" s="131"/>
+      <c r="M9" s="131"/>
+      <c r="N9" s="131"/>
+      <c r="O9" s="131"/>
+      <c r="P9" s="131"/>
+      <c r="Q9" s="131"/>
+      <c r="R9" s="131"/>
       <c r="T9" s="10"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -14705,16 +14729,16 @@
       <c r="J10" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="K10" s="138" t="s">
+      <c r="K10" s="131" t="s">
         <v>123</v>
       </c>
-      <c r="L10" s="138"/>
-      <c r="M10" s="138"/>
-      <c r="N10" s="138"/>
-      <c r="O10" s="138"/>
-      <c r="P10" s="138"/>
-      <c r="Q10" s="138"/>
-      <c r="R10" s="138"/>
+      <c r="L10" s="131"/>
+      <c r="M10" s="131"/>
+      <c r="N10" s="131"/>
+      <c r="O10" s="131"/>
+      <c r="P10" s="131"/>
+      <c r="Q10" s="131"/>
+      <c r="R10" s="131"/>
       <c r="T10" s="10"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -14745,16 +14769,16 @@
       <c r="J11" s="6">
         <v>0</v>
       </c>
-      <c r="K11" s="138" t="s">
+      <c r="K11" s="131" t="s">
         <v>227</v>
       </c>
-      <c r="L11" s="138"/>
-      <c r="M11" s="138"/>
-      <c r="N11" s="138"/>
-      <c r="O11" s="138"/>
-      <c r="P11" s="138"/>
-      <c r="Q11" s="138"/>
-      <c r="R11" s="138"/>
+      <c r="L11" s="131"/>
+      <c r="M11" s="131"/>
+      <c r="N11" s="131"/>
+      <c r="O11" s="131"/>
+      <c r="P11" s="131"/>
+      <c r="Q11" s="131"/>
+      <c r="R11" s="131"/>
       <c r="T11" s="10" t="s">
         <v>339</v>
       </c>
@@ -14829,16 +14853,16 @@
       <c r="J14" s="6">
         <v>0</v>
       </c>
-      <c r="K14" s="112" t="s">
+      <c r="K14" s="119" t="s">
         <v>337</v>
       </c>
-      <c r="L14" s="113"/>
-      <c r="M14" s="113"/>
-      <c r="N14" s="113"/>
-      <c r="O14" s="113"/>
-      <c r="P14" s="113"/>
-      <c r="Q14" s="113"/>
-      <c r="R14" s="114"/>
+      <c r="L14" s="120"/>
+      <c r="M14" s="120"/>
+      <c r="N14" s="120"/>
+      <c r="O14" s="120"/>
+      <c r="P14" s="120"/>
+      <c r="Q14" s="120"/>
+      <c r="R14" s="121"/>
       <c r="T14" s="10" t="s">
         <v>340</v>
       </c>
@@ -15417,10 +15441,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="141" t="s">
         <v>370</v>
       </c>
-      <c r="B1" s="124"/>
+      <c r="B1" s="141"/>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>